<commit_message>
updated rubric and copyright
updated the rubric and the copyright date.
</commit_message>
<xml_diff>
--- a/GameDocuments/gam352_papercut_rubric.xlsx
+++ b/GameDocuments/gam352_papercut_rubric.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Game Data" sheetId="1" r:id="rId1"/>
@@ -5716,6 +5716,90 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -5749,18 +5833,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -5818,99 +5890,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="4" borderId="16" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="4" borderId="18" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="26" fillId="3" borderId="21" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5921,6 +5900,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="26" fillId="3" borderId="26" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5989,55 +5974,37 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="4" borderId="16" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="4" borderId="18" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6049,28 +6016,28 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6097,19 +6064,52 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -38646,54 +38646,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="178"/>
+      <c r="B1" s="145"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="146"/>
       <c r="E1" s="103"/>
-      <c r="F1" s="176" t="s">
+      <c r="F1" s="144" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="177"/>
-      <c r="H1" s="177"/>
-      <c r="I1" s="177"/>
-      <c r="J1" s="178"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
+      <c r="J1" s="146"/>
       <c r="K1" s="104"/>
       <c r="L1" s="104"/>
       <c r="M1" s="105"/>
     </row>
     <row r="2" spans="1:13" ht="14.1" customHeight="1">
-      <c r="A2" s="182" t="s">
+      <c r="A2" s="147" t="s">
         <v>951</v>
       </c>
-      <c r="B2" s="183"/>
-      <c r="C2" s="183"/>
-      <c r="D2" s="184"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="149"/>
       <c r="E2" s="103"/>
-      <c r="F2" s="182" t="s">
+      <c r="F2" s="147" t="s">
         <v>954</v>
       </c>
-      <c r="G2" s="183"/>
-      <c r="H2" s="183"/>
-      <c r="I2" s="183"/>
-      <c r="J2" s="184"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="149"/>
       <c r="K2" s="104"/>
       <c r="L2" s="104"/>
       <c r="M2" s="105"/>
     </row>
     <row r="3" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A3" s="185"/>
-      <c r="B3" s="186"/>
-      <c r="C3" s="186"/>
-      <c r="D3" s="187"/>
+      <c r="A3" s="150"/>
+      <c r="B3" s="151"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="103"/>
-      <c r="F3" s="185"/>
-      <c r="G3" s="186"/>
-      <c r="H3" s="186"/>
-      <c r="I3" s="186"/>
-      <c r="J3" s="187"/>
+      <c r="F3" s="150"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="151"/>
+      <c r="J3" s="152"/>
       <c r="K3" s="104"/>
       <c r="L3" s="104"/>
       <c r="M3" s="105"/>
@@ -38714,41 +38714,41 @@
       <c r="M4" s="105"/>
     </row>
     <row r="5" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="144" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="177"/>
-      <c r="C5" s="177"/>
-      <c r="D5" s="178"/>
+      <c r="B5" s="145"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="146"/>
       <c r="E5" s="103"/>
-      <c r="F5" s="176" t="s">
+      <c r="F5" s="144" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="177"/>
-      <c r="H5" s="177"/>
-      <c r="I5" s="177"/>
-      <c r="J5" s="178"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="145"/>
+      <c r="I5" s="145"/>
+      <c r="J5" s="146"/>
       <c r="K5" s="104"/>
       <c r="L5" s="107"/>
       <c r="M5" s="105"/>
     </row>
     <row r="6" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="156" t="s">
         <v>952</v>
       </c>
-      <c r="B6" s="174"/>
-      <c r="C6" s="174"/>
-      <c r="D6" s="175"/>
+      <c r="B6" s="157"/>
+      <c r="C6" s="157"/>
+      <c r="D6" s="158"/>
       <c r="E6" s="103"/>
-      <c r="F6" s="173" t="s">
+      <c r="F6" s="156" t="s">
         <v>955</v>
       </c>
-      <c r="G6" s="174"/>
-      <c r="H6" s="174"/>
-      <c r="I6" s="174"/>
-      <c r="J6" s="175"/>
+      <c r="G6" s="157"/>
+      <c r="H6" s="157"/>
+      <c r="I6" s="157"/>
+      <c r="J6" s="158"/>
       <c r="K6" s="104"/>
-      <c r="L6" s="170" t="s">
+      <c r="L6" s="153" t="s">
         <v>24</v>
       </c>
       <c r="M6" s="105"/>
@@ -38759,47 +38759,47 @@
       <c r="C7" s="108"/>
       <c r="D7" s="109"/>
       <c r="E7" s="103"/>
-      <c r="F7" s="173"/>
-      <c r="G7" s="174"/>
-      <c r="H7" s="174"/>
-      <c r="I7" s="174"/>
-      <c r="J7" s="175"/>
+      <c r="F7" s="156"/>
+      <c r="G7" s="157"/>
+      <c r="H7" s="157"/>
+      <c r="I7" s="157"/>
+      <c r="J7" s="158"/>
       <c r="K7" s="104"/>
-      <c r="L7" s="171"/>
+      <c r="L7" s="154"/>
       <c r="M7" s="105"/>
     </row>
     <row r="8" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="144" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="177"/>
-      <c r="C8" s="177"/>
-      <c r="D8" s="178"/>
+      <c r="B8" s="145"/>
+      <c r="C8" s="145"/>
+      <c r="D8" s="146"/>
       <c r="E8" s="103"/>
-      <c r="F8" s="173"/>
-      <c r="G8" s="174"/>
-      <c r="H8" s="174"/>
-      <c r="I8" s="174"/>
-      <c r="J8" s="175"/>
+      <c r="F8" s="156"/>
+      <c r="G8" s="157"/>
+      <c r="H8" s="157"/>
+      <c r="I8" s="157"/>
+      <c r="J8" s="158"/>
       <c r="K8" s="104"/>
-      <c r="L8" s="171"/>
+      <c r="L8" s="154"/>
       <c r="M8" s="105"/>
     </row>
     <row r="9" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="156" t="s">
         <v>953</v>
       </c>
-      <c r="B9" s="174"/>
-      <c r="C9" s="174"/>
-      <c r="D9" s="175"/>
+      <c r="B9" s="157"/>
+      <c r="C9" s="157"/>
+      <c r="D9" s="158"/>
       <c r="E9" s="103"/>
-      <c r="F9" s="173"/>
-      <c r="G9" s="174"/>
-      <c r="H9" s="174"/>
-      <c r="I9" s="174"/>
-      <c r="J9" s="175"/>
+      <c r="F9" s="156"/>
+      <c r="G9" s="157"/>
+      <c r="H9" s="157"/>
+      <c r="I9" s="157"/>
+      <c r="J9" s="158"/>
       <c r="K9" s="104"/>
-      <c r="L9" s="172"/>
+      <c r="L9" s="155"/>
       <c r="M9" s="105"/>
     </row>
     <row r="10" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -38818,18 +38818,18 @@
       <c r="M10" s="105"/>
     </row>
     <row r="11" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="144" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="177"/>
-      <c r="C11" s="177"/>
-      <c r="D11" s="178"/>
+      <c r="B11" s="145"/>
+      <c r="C11" s="145"/>
+      <c r="D11" s="146"/>
       <c r="E11" s="103"/>
-      <c r="F11" s="176" t="s">
+      <c r="F11" s="144" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="177"/>
-      <c r="H11" s="178"/>
+      <c r="G11" s="145"/>
+      <c r="H11" s="146"/>
       <c r="I11" s="134" t="s">
         <v>7</v>
       </c>
@@ -38869,7 +38869,7 @@
         <v>-0.12</v>
       </c>
       <c r="K12" s="104"/>
-      <c r="L12" s="170" t="s">
+      <c r="L12" s="153" t="s">
         <v>8</v>
       </c>
       <c r="M12" s="105"/>
@@ -38902,7 +38902,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="120"/>
-      <c r="L13" s="171"/>
+      <c r="L13" s="154"/>
       <c r="M13" s="121"/>
     </row>
     <row r="14" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -38932,7 +38932,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="124"/>
-      <c r="L14" s="172"/>
+      <c r="L14" s="155"/>
       <c r="M14" s="125"/>
     </row>
     <row r="15" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39000,11 +39000,11 @@
         <v>939</v>
       </c>
       <c r="E17" s="104"/>
-      <c r="F17" s="176" t="s">
+      <c r="F17" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="177"/>
-      <c r="H17" s="178"/>
+      <c r="G17" s="145"/>
+      <c r="H17" s="146"/>
       <c r="I17" s="111"/>
       <c r="J17" s="135">
         <v>0.75</v>
@@ -39030,17 +39030,17 @@
       <c r="F18" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="179" t="s">
+      <c r="G18" s="159" t="s">
         <v>956</v>
       </c>
-      <c r="H18" s="180"/>
-      <c r="I18" s="181"/>
+      <c r="H18" s="160"/>
+      <c r="I18" s="161"/>
       <c r="J18" s="137">
         <f>IF(LEFT(G18,6)="Entire",0,IF(LEFT(G18,6)="Custom",-0.05,-0.1))</f>
         <v>-0.1</v>
       </c>
       <c r="K18" s="128"/>
-      <c r="L18" s="170" t="s">
+      <c r="L18" s="153" t="s">
         <v>18</v>
       </c>
       <c r="M18" s="105"/>
@@ -39060,17 +39060,17 @@
       <c r="F19" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="153" t="s">
+      <c r="G19" s="162" t="s">
         <v>957</v>
       </c>
-      <c r="H19" s="154"/>
-      <c r="I19" s="155"/>
+      <c r="H19" s="163"/>
+      <c r="I19" s="164"/>
       <c r="J19" s="139">
         <f>IF(G19="2D Graphics and 2D Gameplay",IF(J11=0.15,-0.05,0),IF(G19="3D Graphics but 2D Gameplay",IF(J11=0.15,-0.02,-0.3),IF(J11=0.15,0,-0.3)))</f>
         <v>0</v>
       </c>
       <c r="K19" s="104"/>
-      <c r="L19" s="172"/>
+      <c r="L19" s="155"/>
       <c r="M19" s="105"/>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39120,22 +39120,22 @@
       <c r="C22" s="118"/>
       <c r="D22" s="119"/>
       <c r="E22" s="104"/>
-      <c r="F22" s="168" t="s">
+      <c r="F22" s="186" t="s">
         <v>713</v>
       </c>
-      <c r="G22" s="166" t="s">
+      <c r="G22" s="184" t="s">
         <v>714</v>
       </c>
-      <c r="H22" s="165"/>
+      <c r="H22" s="183"/>
       <c r="I22" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="163">
+      <c r="J22" s="181">
         <f>J20+J15</f>
         <v>0.68</v>
       </c>
       <c r="K22" s="104"/>
-      <c r="L22" s="144" t="s">
+      <c r="L22" s="165" t="s">
         <v>725</v>
       </c>
       <c r="M22" s="105"/>
@@ -39146,15 +39146,15 @@
       <c r="C23" s="118"/>
       <c r="D23" s="119"/>
       <c r="E23" s="104"/>
-      <c r="F23" s="169"/>
-      <c r="G23" s="167"/>
-      <c r="H23" s="165"/>
+      <c r="F23" s="187"/>
+      <c r="G23" s="185"/>
+      <c r="H23" s="183"/>
       <c r="I23" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="164"/>
+      <c r="J23" s="182"/>
       <c r="K23" s="104"/>
-      <c r="L23" s="145"/>
+      <c r="L23" s="166"/>
       <c r="M23" s="105"/>
     </row>
     <row r="24" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39178,13 +39178,13 @@
       <c r="C25" s="118"/>
       <c r="D25" s="119"/>
       <c r="E25" s="104"/>
-      <c r="F25" s="157" t="s">
+      <c r="F25" s="175" t="s">
         <v>932</v>
       </c>
-      <c r="G25" s="158"/>
-      <c r="H25" s="158"/>
-      <c r="I25" s="158"/>
-      <c r="J25" s="159"/>
+      <c r="G25" s="176"/>
+      <c r="H25" s="176"/>
+      <c r="I25" s="176"/>
+      <c r="J25" s="177"/>
       <c r="K25" s="104"/>
       <c r="L25" s="104"/>
       <c r="M25" s="105"/>
@@ -39195,11 +39195,11 @@
       <c r="C26" s="118"/>
       <c r="D26" s="119"/>
       <c r="E26" s="103"/>
-      <c r="F26" s="160"/>
-      <c r="G26" s="161"/>
-      <c r="H26" s="161"/>
-      <c r="I26" s="161"/>
-      <c r="J26" s="162"/>
+      <c r="F26" s="178"/>
+      <c r="G26" s="179"/>
+      <c r="H26" s="179"/>
+      <c r="I26" s="179"/>
+      <c r="J26" s="180"/>
       <c r="K26" s="104"/>
       <c r="L26" s="104"/>
       <c r="M26" s="105"/>
@@ -39225,13 +39225,13 @@
       <c r="C28" s="118"/>
       <c r="D28" s="119"/>
       <c r="E28" s="103"/>
-      <c r="F28" s="156" t="s">
+      <c r="F28" s="174" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="156"/>
-      <c r="H28" s="156"/>
-      <c r="I28" s="156"/>
-      <c r="J28" s="156"/>
+      <c r="G28" s="174"/>
+      <c r="H28" s="174"/>
+      <c r="I28" s="174"/>
+      <c r="J28" s="174"/>
       <c r="K28" s="104"/>
       <c r="L28" s="104"/>
       <c r="M28" s="105"/>
@@ -39242,13 +39242,13 @@
       <c r="C29" s="118"/>
       <c r="D29" s="119"/>
       <c r="E29" s="103"/>
-      <c r="F29" s="150" t="s">
+      <c r="F29" s="171" t="s">
         <v>933</v>
       </c>
-      <c r="G29" s="151"/>
-      <c r="H29" s="151"/>
-      <c r="I29" s="151"/>
-      <c r="J29" s="152"/>
+      <c r="G29" s="172"/>
+      <c r="H29" s="172"/>
+      <c r="I29" s="172"/>
+      <c r="J29" s="173"/>
       <c r="K29" s="104"/>
       <c r="L29" s="104"/>
       <c r="M29" s="105"/>
@@ -39259,30 +39259,30 @@
       <c r="C30" s="118"/>
       <c r="D30" s="119"/>
       <c r="E30" s="103"/>
-      <c r="F30" s="150"/>
-      <c r="G30" s="151"/>
-      <c r="H30" s="151"/>
-      <c r="I30" s="151"/>
-      <c r="J30" s="152"/>
+      <c r="F30" s="171"/>
+      <c r="G30" s="172"/>
+      <c r="H30" s="172"/>
+      <c r="I30" s="172"/>
+      <c r="J30" s="173"/>
       <c r="K30" s="104"/>
       <c r="L30" s="104"/>
       <c r="M30" s="105"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A31" s="146" t="s">
+      <c r="A31" s="167" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="147"/>
-      <c r="C31" s="148" t="s">
+      <c r="B31" s="168"/>
+      <c r="C31" s="169" t="s">
         <v>950</v>
       </c>
-      <c r="D31" s="149"/>
+      <c r="D31" s="170"/>
       <c r="E31" s="104"/>
-      <c r="F31" s="153"/>
-      <c r="G31" s="154"/>
-      <c r="H31" s="154"/>
-      <c r="I31" s="154"/>
-      <c r="J31" s="155"/>
+      <c r="F31" s="162"/>
+      <c r="G31" s="163"/>
+      <c r="H31" s="163"/>
+      <c r="I31" s="163"/>
+      <c r="J31" s="164"/>
       <c r="K31" s="104"/>
       <c r="L31" s="104"/>
       <c r="M31" s="105"/>
@@ -39305,12 +39305,16 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0"/>
   <mergeCells count="31">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="A2:D3"/>
-    <mergeCell ref="F2:J3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F29:J31"/>
+    <mergeCell ref="F28:J28"/>
+    <mergeCell ref="F25:J26"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F22:F23"/>
     <mergeCell ref="L12:L14"/>
     <mergeCell ref="L18:L19"/>
     <mergeCell ref="A6:D6"/>
@@ -39326,16 +39330,12 @@
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="G18:I18"/>
     <mergeCell ref="G19:I19"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F29:J31"/>
-    <mergeCell ref="F28:J28"/>
-    <mergeCell ref="F25:J26"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A2:D3"/>
+    <mergeCell ref="F2:J3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:J5"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6:D6">
@@ -39403,57 +39403,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="194" t="s">
         <v>556</v>
       </c>
-      <c r="B1" s="200"/>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
-      <c r="E1" s="200"/>
-      <c r="F1" s="200"/>
-      <c r="G1" s="200"/>
-      <c r="H1" s="200"/>
-      <c r="J1" s="210" t="s">
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
+      <c r="F1" s="195"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="195"/>
+      <c r="J1" s="205" t="s">
         <v>482</v>
       </c>
-      <c r="K1" s="211"/>
-      <c r="L1" s="212"/>
+      <c r="K1" s="206"/>
+      <c r="L1" s="207"/>
       <c r="M1" s="79"/>
       <c r="N1" s="24" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A2" s="199"/>
-      <c r="B2" s="200"/>
-      <c r="C2" s="200"/>
-      <c r="D2" s="200"/>
-      <c r="E2" s="200"/>
-      <c r="F2" s="200"/>
-      <c r="G2" s="200"/>
-      <c r="H2" s="200"/>
-      <c r="J2" s="213" t="s">
+      <c r="A2" s="194"/>
+      <c r="B2" s="195"/>
+      <c r="C2" s="195"/>
+      <c r="D2" s="195"/>
+      <c r="E2" s="195"/>
+      <c r="F2" s="195"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="195"/>
+      <c r="J2" s="208" t="s">
         <v>706</v>
       </c>
-      <c r="K2" s="214"/>
-      <c r="L2" s="215"/>
+      <c r="K2" s="209"/>
+      <c r="L2" s="210"/>
       <c r="M2" s="23"/>
       <c r="N2" s="26" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A3" s="199"/>
-      <c r="B3" s="200"/>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200"/>
-      <c r="E3" s="200"/>
-      <c r="F3" s="200"/>
-      <c r="G3" s="200"/>
-      <c r="H3" s="200"/>
-      <c r="J3" s="213"/>
-      <c r="K3" s="214"/>
-      <c r="L3" s="215"/>
+      <c r="A3" s="194"/>
+      <c r="B3" s="195"/>
+      <c r="C3" s="195"/>
+      <c r="D3" s="195"/>
+      <c r="E3" s="195"/>
+      <c r="F3" s="195"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="195"/>
+      <c r="J3" s="208"/>
+      <c r="K3" s="209"/>
+      <c r="L3" s="210"/>
       <c r="M3" s="23"/>
       <c r="N3" s="26" t="s">
         <v>431</v>
@@ -39463,14 +39463,14 @@
       <c r="A4" s="2"/>
       <c r="B4" s="5"/>
       <c r="C4" s="8"/>
-      <c r="D4" s="192"/>
-      <c r="E4" s="192"/>
+      <c r="D4" s="193"/>
+      <c r="E4" s="193"/>
       <c r="F4" s="43"/>
-      <c r="G4" s="192"/>
-      <c r="H4" s="192"/>
-      <c r="J4" s="213"/>
-      <c r="K4" s="214"/>
-      <c r="L4" s="215"/>
+      <c r="G4" s="193"/>
+      <c r="H4" s="193"/>
+      <c r="J4" s="208"/>
+      <c r="K4" s="209"/>
+      <c r="L4" s="210"/>
       <c r="M4" s="34"/>
       <c r="N4" s="26" t="s">
         <v>432</v>
@@ -39478,24 +39478,24 @@
       <c r="O4" s="81"/>
     </row>
     <row r="5" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A5" s="201" t="s">
+      <c r="A5" s="196" t="s">
         <v>425</v>
       </c>
-      <c r="B5" s="202"/>
+      <c r="B5" s="197"/>
       <c r="C5" s="8"/>
-      <c r="D5" s="205" t="s">
+      <c r="D5" s="200" t="s">
         <v>717</v>
       </c>
-      <c r="E5" s="206"/>
-      <c r="F5" s="207"/>
-      <c r="G5" s="208">
+      <c r="E5" s="201"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="203">
         <f>Submission!$E$17</f>
         <v>0</v>
       </c>
-      <c r="H5" s="209"/>
-      <c r="J5" s="213"/>
-      <c r="K5" s="214"/>
-      <c r="L5" s="215"/>
+      <c r="H5" s="204"/>
+      <c r="J5" s="208"/>
+      <c r="K5" s="209"/>
+      <c r="L5" s="210"/>
       <c r="M5" s="34"/>
       <c r="N5" s="26" t="s">
         <v>433</v>
@@ -39503,21 +39503,21 @@
       <c r="O5" s="81"/>
     </row>
     <row r="6" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A6" s="203"/>
-      <c r="B6" s="204"/>
+      <c r="A6" s="198"/>
+      <c r="B6" s="199"/>
       <c r="C6" s="43"/>
-      <c r="D6" s="192" t="s">
+      <c r="D6" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="192"/>
+      <c r="E6" s="193"/>
       <c r="F6" s="43"/>
-      <c r="G6" s="192" t="s">
+      <c r="G6" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="192"/>
-      <c r="J6" s="213"/>
-      <c r="K6" s="214"/>
-      <c r="L6" s="215"/>
+      <c r="H6" s="193"/>
+      <c r="J6" s="208"/>
+      <c r="K6" s="209"/>
+      <c r="L6" s="210"/>
       <c r="M6" s="34"/>
       <c r="N6" s="26" t="s">
         <v>434</v>
@@ -39525,24 +39525,24 @@
       <c r="O6" s="81"/>
     </row>
     <row r="7" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A7" s="195">
+      <c r="A7" s="188">
         <f>'Game Data'!$J$22</f>
         <v>0.68</v>
       </c>
-      <c r="B7" s="196"/>
+      <c r="B7" s="189"/>
       <c r="C7" s="43"/>
-      <c r="D7" s="193" t="s">
+      <c r="D7" s="216" t="s">
         <v>724</v>
       </c>
-      <c r="E7" s="194"/>
+      <c r="E7" s="217"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="193" t="s">
+      <c r="G7" s="216" t="s">
         <v>724</v>
       </c>
-      <c r="H7" s="194"/>
-      <c r="J7" s="213"/>
-      <c r="K7" s="214"/>
-      <c r="L7" s="215"/>
+      <c r="H7" s="217"/>
+      <c r="J7" s="208"/>
+      <c r="K7" s="209"/>
+      <c r="L7" s="210"/>
       <c r="M7" s="33"/>
       <c r="N7" s="26" t="s">
         <v>435</v>
@@ -39550,23 +39550,23 @@
       <c r="O7" s="81"/>
     </row>
     <row r="8" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A8" s="197"/>
-      <c r="B8" s="198"/>
+      <c r="A8" s="190"/>
+      <c r="B8" s="191"/>
       <c r="C8" s="97"/>
-      <c r="D8" s="219">
+      <c r="D8" s="214">
         <f>E17+E26+E35+E44+E53</f>
         <v>-4.1250000000000002E-2</v>
       </c>
-      <c r="E8" s="220"/>
+      <c r="E8" s="215"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="219">
+      <c r="G8" s="214">
         <f>H17+H26+H35+H44+H53</f>
         <v>0</v>
       </c>
-      <c r="H8" s="220"/>
-      <c r="J8" s="216"/>
-      <c r="K8" s="217"/>
-      <c r="L8" s="218"/>
+      <c r="H8" s="215"/>
+      <c r="J8" s="211"/>
+      <c r="K8" s="212"/>
+      <c r="L8" s="213"/>
       <c r="M8" s="80"/>
       <c r="N8" s="25" t="s">
         <v>436</v>
@@ -39577,15 +39577,15 @@
       <c r="A9" s="2"/>
       <c r="B9" s="5"/>
       <c r="C9" s="43"/>
-      <c r="D9" s="192" t="s">
+      <c r="D9" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="192"/>
+      <c r="E9" s="193"/>
       <c r="F9" s="43"/>
-      <c r="G9" s="192" t="s">
+      <c r="G9" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="192"/>
+      <c r="H9" s="193"/>
       <c r="J9" s="82"/>
       <c r="K9" s="82"/>
       <c r="L9" s="82"/>
@@ -39612,11 +39612,11 @@
       <c r="H10" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="191" t="s">
+      <c r="J10" s="192" t="s">
         <v>707</v>
       </c>
-      <c r="K10" s="191"/>
-      <c r="L10" s="191"/>
+      <c r="K10" s="192"/>
+      <c r="L10" s="192"/>
       <c r="O10" s="84"/>
     </row>
     <row r="11" spans="1:15" ht="14.1" customHeight="1">
@@ -39645,11 +39645,11 @@
         <f t="shared" ref="H11:H16" si="1">$B11*G11</f>
         <v>0</v>
       </c>
-      <c r="J11" s="190" t="s">
+      <c r="J11" s="220" t="s">
         <v>792</v>
       </c>
-      <c r="K11" s="190"/>
-      <c r="L11" s="190"/>
+      <c r="K11" s="220"/>
+      <c r="L11" s="220"/>
       <c r="M11" s="82"/>
       <c r="O11" s="84"/>
     </row>
@@ -39679,9 +39679,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J12" s="190"/>
-      <c r="K12" s="190"/>
-      <c r="L12" s="190"/>
+      <c r="J12" s="220"/>
+      <c r="K12" s="220"/>
+      <c r="L12" s="220"/>
       <c r="M12" s="82"/>
       <c r="O12" s="84"/>
     </row>
@@ -39711,9 +39711,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="190"/>
-      <c r="K13" s="190"/>
-      <c r="L13" s="190"/>
+      <c r="J13" s="220"/>
+      <c r="K13" s="220"/>
+      <c r="L13" s="220"/>
       <c r="M13" s="82"/>
       <c r="O13" s="84"/>
     </row>
@@ -39779,11 +39779,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J15" s="188">
+      <c r="J15" s="218">
         <f>MAX(0,MIN(1,IF($J17 &lt;= 0.95, ROUND($J17,2), FLOOR((0.95+($J17-0.95)/5),0.01))))</f>
         <v>0.63</v>
       </c>
-      <c r="L15" s="188">
+      <c r="L15" s="218">
         <f>MAX(0,MIN(1,IF($L17 &lt;= 0.95, ROUND($L17,2), FLOOR((0.95+($L17-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -39816,8 +39816,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J16" s="189"/>
-      <c r="L16" s="189"/>
+      <c r="J16" s="219"/>
+      <c r="L16" s="219"/>
       <c r="M16" s="82"/>
       <c r="O16" s="84"/>
     </row>
@@ -39854,15 +39854,15 @@
       <c r="A18" s="2"/>
       <c r="B18" s="5"/>
       <c r="C18" s="43"/>
-      <c r="D18" s="192" t="s">
+      <c r="D18" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="192"/>
+      <c r="E18" s="193"/>
       <c r="F18" s="43"/>
-      <c r="G18" s="192" t="s">
+      <c r="G18" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="192"/>
+      <c r="H18" s="193"/>
       <c r="J18" s="88"/>
       <c r="M18" s="78"/>
     </row>
@@ -39887,11 +39887,11 @@
       <c r="H19" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="191" t="s">
+      <c r="J19" s="192" t="s">
         <v>715</v>
       </c>
-      <c r="K19" s="191"/>
-      <c r="L19" s="191"/>
+      <c r="K19" s="192"/>
+      <c r="L19" s="192"/>
       <c r="M19" s="83"/>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1">
@@ -39920,11 +39920,11 @@
         <f t="shared" ref="H20:H25" si="3">$B20*G20</f>
         <v>0</v>
       </c>
-      <c r="J20" s="190" t="s">
+      <c r="J20" s="220" t="s">
         <v>722</v>
       </c>
-      <c r="K20" s="190"/>
-      <c r="L20" s="190"/>
+      <c r="K20" s="220"/>
+      <c r="L20" s="220"/>
       <c r="M20" s="84"/>
     </row>
     <row r="21" spans="1:13" ht="14.1" customHeight="1">
@@ -39953,9 +39953,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J21" s="190"/>
-      <c r="K21" s="190"/>
-      <c r="L21" s="190"/>
+      <c r="J21" s="220"/>
+      <c r="K21" s="220"/>
+      <c r="L21" s="220"/>
       <c r="M21" s="84"/>
     </row>
     <row r="22" spans="1:13" ht="14.1" customHeight="1">
@@ -39984,9 +39984,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J22" s="190"/>
-      <c r="K22" s="190"/>
-      <c r="L22" s="190"/>
+      <c r="J22" s="220"/>
+      <c r="K22" s="220"/>
+      <c r="L22" s="220"/>
       <c r="M22" s="84"/>
     </row>
     <row r="23" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40050,11 +40050,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J24" s="188">
+      <c r="J24" s="218">
         <f>MAX(0,MIN(1,IF($J26 &lt;= 0.95, ROUND($J26,2), FLOOR((0.95+($J26-0.95)/5),0.01))))</f>
         <v>0.64</v>
       </c>
-      <c r="L24" s="188">
+      <c r="L24" s="218">
         <f>MAX(0,MIN(1,IF($L26 &lt;= 0.95, ROUND($L26,2), FLOOR((0.95+($L26-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40086,8 +40086,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J25" s="189"/>
-      <c r="L25" s="189"/>
+      <c r="J25" s="219"/>
+      <c r="L25" s="219"/>
       <c r="M25" s="84"/>
     </row>
     <row r="26" spans="1:13" ht="14.1" customHeight="1">
@@ -40123,15 +40123,15 @@
       <c r="A27" s="2"/>
       <c r="B27" s="5"/>
       <c r="C27" s="43"/>
-      <c r="D27" s="192" t="s">
+      <c r="D27" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="192"/>
+      <c r="E27" s="193"/>
       <c r="F27" s="43"/>
-      <c r="G27" s="192" t="s">
+      <c r="G27" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H27" s="192"/>
+      <c r="H27" s="193"/>
     </row>
     <row r="28" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
       <c r="A28" s="1" t="s">
@@ -40154,11 +40154,11 @@
       <c r="H28" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J28" s="191" t="s">
+      <c r="J28" s="192" t="s">
         <v>709</v>
       </c>
-      <c r="K28" s="191"/>
-      <c r="L28" s="191"/>
+      <c r="K28" s="192"/>
+      <c r="L28" s="192"/>
     </row>
     <row r="29" spans="1:13" ht="14.1" customHeight="1">
       <c r="A29" s="57" t="str">
@@ -40186,11 +40186,11 @@
         <f t="shared" ref="H29:H34" si="5">$B29*G29</f>
         <v>0</v>
       </c>
-      <c r="J29" s="190" t="s">
+      <c r="J29" s="220" t="s">
         <v>710</v>
       </c>
-      <c r="K29" s="190"/>
-      <c r="L29" s="190"/>
+      <c r="K29" s="220"/>
+      <c r="L29" s="220"/>
     </row>
     <row r="30" spans="1:13" ht="14.1" customHeight="1">
       <c r="A30" s="58" t="str">
@@ -40218,9 +40218,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J30" s="190"/>
-      <c r="K30" s="190"/>
-      <c r="L30" s="190"/>
+      <c r="J30" s="220"/>
+      <c r="K30" s="220"/>
+      <c r="L30" s="220"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1">
       <c r="A31" s="58" t="str">
@@ -40248,9 +40248,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J31" s="190"/>
-      <c r="K31" s="190"/>
-      <c r="L31" s="190"/>
+      <c r="J31" s="220"/>
+      <c r="K31" s="220"/>
+      <c r="L31" s="220"/>
     </row>
     <row r="32" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
       <c r="A32" s="58" t="str">
@@ -40312,11 +40312,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J33" s="188">
+      <c r="J33" s="218">
         <f>MAX(0,MIN(1,IF($J35 &lt;= 0.95, ROUND($J35,2), FLOOR((0.95+($J35-0.95)/5),0.01))))</f>
         <v>0.64</v>
       </c>
-      <c r="L33" s="188">
+      <c r="L33" s="218">
         <f>MAX(0,MIN(1,IF($L35 &lt;= 0.95, ROUND($L35,2), FLOOR((0.95+($L35-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40347,8 +40347,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J34" s="189"/>
-      <c r="L34" s="189"/>
+      <c r="J34" s="219"/>
+      <c r="L34" s="219"/>
     </row>
     <row r="35" spans="1:12" ht="14.1" customHeight="1">
       <c r="A35" s="2"/>
@@ -40382,15 +40382,15 @@
       <c r="A36" s="2"/>
       <c r="B36" s="5"/>
       <c r="C36" s="43"/>
-      <c r="D36" s="192" t="s">
+      <c r="D36" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="192"/>
+      <c r="E36" s="193"/>
       <c r="F36" s="43"/>
-      <c r="G36" s="192" t="s">
+      <c r="G36" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H36" s="192"/>
+      <c r="H36" s="193"/>
     </row>
     <row r="37" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A37" s="1" t="s">
@@ -40413,11 +40413,11 @@
       <c r="H37" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J37" s="191" t="s">
+      <c r="J37" s="192" t="s">
         <v>711</v>
       </c>
-      <c r="K37" s="191"/>
-      <c r="L37" s="191"/>
+      <c r="K37" s="192"/>
+      <c r="L37" s="192"/>
     </row>
     <row r="38" spans="1:12" ht="14.1" customHeight="1">
       <c r="A38" s="57" t="str">
@@ -40445,11 +40445,11 @@
         <f t="shared" ref="H38:H43" si="7">$B38*G38</f>
         <v>0</v>
       </c>
-      <c r="J38" s="190" t="s">
+      <c r="J38" s="220" t="s">
         <v>712</v>
       </c>
-      <c r="K38" s="190"/>
-      <c r="L38" s="190"/>
+      <c r="K38" s="220"/>
+      <c r="L38" s="220"/>
     </row>
     <row r="39" spans="1:12" ht="14.1" customHeight="1">
       <c r="A39" s="58" t="str">
@@ -40477,9 +40477,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J39" s="190"/>
-      <c r="K39" s="190"/>
-      <c r="L39" s="190"/>
+      <c r="J39" s="220"/>
+      <c r="K39" s="220"/>
+      <c r="L39" s="220"/>
     </row>
     <row r="40" spans="1:12" ht="14.1" customHeight="1">
       <c r="A40" s="58" t="str">
@@ -40507,9 +40507,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J40" s="190"/>
-      <c r="K40" s="190"/>
-      <c r="L40" s="190"/>
+      <c r="J40" s="220"/>
+      <c r="K40" s="220"/>
+      <c r="L40" s="220"/>
     </row>
     <row r="41" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A41" s="58" t="str">
@@ -40571,11 +40571,11 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J42" s="188">
+      <c r="J42" s="218">
         <f>MAX(0,MIN(1,IF($J44 &lt;= 0.95, ROUND($J44,2), FLOOR((0.95+($J44-0.95)/5),0.01))))</f>
         <v>0.63</v>
       </c>
-      <c r="L42" s="188">
+      <c r="L42" s="218">
         <f>MAX(0,MIN(1,IF($L44 &lt;= 0.95, ROUND($L44,2), FLOOR((0.95+($L44-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40606,8 +40606,8 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J43" s="189"/>
-      <c r="L43" s="189"/>
+      <c r="J43" s="219"/>
+      <c r="L43" s="219"/>
     </row>
     <row r="44" spans="1:12" ht="14.1" customHeight="1">
       <c r="A44" s="2"/>
@@ -40641,15 +40641,15 @@
       <c r="A45" s="2"/>
       <c r="B45" s="5"/>
       <c r="C45" s="43"/>
-      <c r="D45" s="192" t="s">
+      <c r="D45" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="192"/>
+      <c r="E45" s="193"/>
       <c r="F45" s="43"/>
-      <c r="G45" s="192" t="s">
+      <c r="G45" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="192"/>
+      <c r="H45" s="193"/>
     </row>
     <row r="46" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A46" s="1" t="s">
@@ -40857,6 +40857,34 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="J29:L31"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="L33:L34"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="J38:L40"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="J11:L13"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J20:L22"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G36:H36"/>
     <mergeCell ref="A7:B8"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="D6:E6"/>
@@ -40870,34 +40898,6 @@
     <mergeCell ref="J2:L8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="J11:L13"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J20:L22"/>
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="L42:L43"/>
-    <mergeCell ref="J29:L31"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="L33:L34"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="J38:L40"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -40925,59 +40925,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="235" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="233"/>
-      <c r="C1" s="233"/>
-      <c r="D1" s="233"/>
-      <c r="E1" s="233"/>
-      <c r="F1" s="233"/>
-      <c r="G1" s="234"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="237"/>
     </row>
     <row r="2" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A2" s="221" t="s">
+      <c r="A2" s="230" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="222"/>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
-      <c r="G2" s="223"/>
+      <c r="B2" s="231"/>
+      <c r="C2" s="231"/>
+      <c r="D2" s="231"/>
+      <c r="E2" s="231"/>
+      <c r="F2" s="231"/>
+      <c r="G2" s="232"/>
     </row>
     <row r="3" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A3" s="238" t="s">
+      <c r="A3" s="227" t="s">
         <v>930</v>
       </c>
-      <c r="B3" s="239"/>
-      <c r="C3" s="239"/>
-      <c r="D3" s="239"/>
-      <c r="E3" s="239"/>
-      <c r="F3" s="239"/>
-      <c r="G3" s="240"/>
+      <c r="B3" s="228"/>
+      <c r="C3" s="228"/>
+      <c r="D3" s="228"/>
+      <c r="E3" s="228"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="229"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A4" s="221" t="s">
+      <c r="A4" s="230" t="s">
         <v>438</v>
       </c>
-      <c r="B4" s="222"/>
-      <c r="C4" s="222"/>
-      <c r="D4" s="222"/>
-      <c r="E4" s="222"/>
-      <c r="F4" s="222"/>
-      <c r="G4" s="223"/>
+      <c r="B4" s="231"/>
+      <c r="C4" s="231"/>
+      <c r="D4" s="231"/>
+      <c r="E4" s="231"/>
+      <c r="F4" s="231"/>
+      <c r="G4" s="232"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A5" s="249" t="s">
+      <c r="A5" s="238" t="s">
         <v>580</v>
       </c>
-      <c r="B5" s="250"/>
-      <c r="C5" s="250"/>
-      <c r="D5" s="250"/>
-      <c r="E5" s="250"/>
-      <c r="F5" s="250"/>
-      <c r="G5" s="251"/>
+      <c r="B5" s="239"/>
+      <c r="C5" s="239"/>
+      <c r="D5" s="239"/>
+      <c r="E5" s="239"/>
+      <c r="F5" s="239"/>
+      <c r="G5" s="240"/>
     </row>
     <row r="6" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
       <c r="A6" s="2"/>
@@ -41010,10 +41010,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75">
-      <c r="A8" s="247" t="s">
+      <c r="A8" s="233" t="s">
         <v>718</v>
       </c>
-      <c r="B8" s="248"/>
+      <c r="B8" s="234"/>
       <c r="C8" s="65">
         <v>0</v>
       </c>
@@ -41030,10 +41030,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75">
-      <c r="A9" s="253" t="s">
+      <c r="A9" s="242" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="254"/>
+      <c r="B9" s="243"/>
       <c r="C9" s="92">
         <v>0</v>
       </c>
@@ -41050,10 +41050,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75">
-      <c r="A10" s="255" t="s">
+      <c r="A10" s="244" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="256"/>
+      <c r="B10" s="245"/>
       <c r="C10" s="69">
         <v>0</v>
       </c>
@@ -41070,10 +41070,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75">
-      <c r="A11" s="256" t="s">
+      <c r="A11" s="245" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="256"/>
+      <c r="B11" s="245"/>
       <c r="C11" s="69">
         <v>0</v>
       </c>
@@ -41090,10 +41090,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75">
-      <c r="A12" s="256" t="s">
+      <c r="A12" s="245" t="s">
         <v>716</v>
       </c>
-      <c r="B12" s="256"/>
+      <c r="B12" s="245"/>
       <c r="C12" s="69">
         <v>0</v>
       </c>
@@ -41110,10 +41110,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75">
-      <c r="A13" s="256" t="s">
+      <c r="A13" s="245" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="256"/>
+      <c r="B13" s="245"/>
       <c r="C13" s="69">
         <v>0</v>
       </c>
@@ -41130,10 +41130,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75">
-      <c r="A14" s="255" t="s">
+      <c r="A14" s="244" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="256"/>
+      <c r="B14" s="245"/>
       <c r="C14" s="69">
         <v>0</v>
       </c>
@@ -41150,10 +41150,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75">
-      <c r="A15" s="255" t="s">
+      <c r="A15" s="244" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="256"/>
+      <c r="B15" s="245"/>
       <c r="C15" s="69">
         <v>0</v>
       </c>
@@ -41170,10 +41170,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A16" s="230" t="s">
+      <c r="A16" s="246" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="231"/>
+      <c r="B16" s="247"/>
       <c r="C16" s="73">
         <v>0</v>
       </c>
@@ -41191,11 +41191,11 @@
     </row>
     <row r="17" spans="1:7" ht="14.1" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="252" t="s">
+      <c r="B17" s="241" t="s">
         <v>721</v>
       </c>
-      <c r="C17" s="252"/>
-      <c r="D17" s="252"/>
+      <c r="C17" s="241"/>
+      <c r="D17" s="241"/>
       <c r="E17" s="63">
         <f>SUM(E9:E16)</f>
         <v>0</v>
@@ -41216,527 +41216,559 @@
       <c r="A19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="232" t="s">
+      <c r="B19" s="235" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="233"/>
-      <c r="D19" s="233"/>
-      <c r="E19" s="233"/>
-      <c r="F19" s="233"/>
-      <c r="G19" s="234"/>
+      <c r="C19" s="236"/>
+      <c r="D19" s="236"/>
+      <c r="E19" s="236"/>
+      <c r="F19" s="236"/>
+      <c r="G19" s="237"/>
     </row>
     <row r="20" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="A20" s="10" t="s">
         <v>582</v>
       </c>
-      <c r="B20" s="221" t="s">
+      <c r="B20" s="230" t="s">
         <v>931</v>
       </c>
-      <c r="C20" s="222"/>
-      <c r="D20" s="222"/>
-      <c r="E20" s="222"/>
-      <c r="F20" s="222"/>
-      <c r="G20" s="223"/>
+      <c r="C20" s="231"/>
+      <c r="D20" s="231"/>
+      <c r="E20" s="231"/>
+      <c r="F20" s="231"/>
+      <c r="G20" s="232"/>
     </row>
     <row r="21" spans="1:7" ht="60" customHeight="1" thickBot="1">
       <c r="A21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="221" t="s">
+      <c r="B21" s="230" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="222"/>
-      <c r="D21" s="222"/>
-      <c r="E21" s="222"/>
-      <c r="F21" s="222"/>
-      <c r="G21" s="223"/>
+      <c r="C21" s="231"/>
+      <c r="D21" s="231"/>
+      <c r="E21" s="231"/>
+      <c r="F21" s="231"/>
+      <c r="G21" s="232"/>
     </row>
     <row r="22" spans="1:7" ht="45.95" customHeight="1" thickBot="1">
       <c r="A22" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="221" t="s">
+      <c r="B22" s="230" t="s">
         <v>917</v>
       </c>
-      <c r="C22" s="222"/>
-      <c r="D22" s="222"/>
-      <c r="E22" s="222"/>
-      <c r="F22" s="222"/>
-      <c r="G22" s="223"/>
+      <c r="C22" s="231"/>
+      <c r="D22" s="231"/>
+      <c r="E22" s="231"/>
+      <c r="F22" s="231"/>
+      <c r="G22" s="232"/>
     </row>
     <row r="23" spans="1:7" ht="32.1" customHeight="1">
       <c r="A23" s="98" t="s">
         <v>899</v>
       </c>
-      <c r="B23" s="238" t="s">
+      <c r="B23" s="227" t="s">
         <v>916</v>
       </c>
-      <c r="C23" s="239"/>
-      <c r="D23" s="239"/>
-      <c r="E23" s="239"/>
-      <c r="F23" s="239"/>
-      <c r="G23" s="240"/>
+      <c r="C23" s="228"/>
+      <c r="D23" s="228"/>
+      <c r="E23" s="228"/>
+      <c r="F23" s="228"/>
+      <c r="G23" s="229"/>
     </row>
     <row r="24" spans="1:7" ht="15.75">
       <c r="A24" s="99"/>
-      <c r="B24" s="257" t="s">
+      <c r="B24" s="221" t="s">
         <v>900</v>
       </c>
-      <c r="C24" s="258"/>
-      <c r="D24" s="260" t="s">
+      <c r="C24" s="222"/>
+      <c r="D24" s="223" t="s">
         <v>901</v>
       </c>
-      <c r="E24" s="260"/>
-      <c r="F24" s="260"/>
-      <c r="G24" s="261"/>
+      <c r="E24" s="223"/>
+      <c r="F24" s="223"/>
+      <c r="G24" s="224"/>
     </row>
     <row r="25" spans="1:7" ht="15.75">
       <c r="A25" s="99"/>
-      <c r="B25" s="257" t="s">
+      <c r="B25" s="221" t="s">
         <v>902</v>
       </c>
-      <c r="C25" s="258"/>
-      <c r="D25" s="260" t="s">
+      <c r="C25" s="222"/>
+      <c r="D25" s="223" t="s">
         <v>903</v>
       </c>
-      <c r="E25" s="260"/>
-      <c r="F25" s="260"/>
-      <c r="G25" s="261"/>
+      <c r="E25" s="223"/>
+      <c r="F25" s="223"/>
+      <c r="G25" s="224"/>
     </row>
     <row r="26" spans="1:7" ht="15.75">
       <c r="A26" s="99"/>
-      <c r="B26" s="257" t="s">
+      <c r="B26" s="221" t="s">
         <v>904</v>
       </c>
-      <c r="C26" s="258"/>
-      <c r="D26" s="260" t="s">
+      <c r="C26" s="222"/>
+      <c r="D26" s="223" t="s">
         <v>905</v>
       </c>
-      <c r="E26" s="260"/>
-      <c r="F26" s="260"/>
-      <c r="G26" s="261"/>
+      <c r="E26" s="223"/>
+      <c r="F26" s="223"/>
+      <c r="G26" s="224"/>
     </row>
     <row r="27" spans="1:7" ht="15.75">
       <c r="A27" s="99"/>
-      <c r="B27" s="257" t="s">
+      <c r="B27" s="221" t="s">
         <v>906</v>
       </c>
-      <c r="C27" s="258"/>
+      <c r="C27" s="222"/>
       <c r="D27" s="225" t="s">
         <v>907</v>
       </c>
       <c r="E27" s="225"/>
       <c r="F27" s="225"/>
-      <c r="G27" s="259"/>
+      <c r="G27" s="226"/>
     </row>
     <row r="28" spans="1:7" ht="15.75">
       <c r="A28" s="99"/>
-      <c r="B28" s="257" t="s">
+      <c r="B28" s="221" t="s">
         <v>908</v>
       </c>
-      <c r="C28" s="258"/>
-      <c r="D28" s="260" t="s">
+      <c r="C28" s="222"/>
+      <c r="D28" s="223" t="s">
         <v>909</v>
       </c>
-      <c r="E28" s="260"/>
-      <c r="F28" s="260"/>
-      <c r="G28" s="261"/>
+      <c r="E28" s="223"/>
+      <c r="F28" s="223"/>
+      <c r="G28" s="224"/>
     </row>
     <row r="29" spans="1:7" ht="15.75">
       <c r="A29" s="99"/>
-      <c r="B29" s="257" t="s">
+      <c r="B29" s="221" t="s">
         <v>910</v>
       </c>
-      <c r="C29" s="258"/>
+      <c r="C29" s="222"/>
       <c r="D29" s="225" t="s">
         <v>911</v>
       </c>
       <c r="E29" s="225"/>
       <c r="F29" s="225"/>
-      <c r="G29" s="259"/>
+      <c r="G29" s="226"/>
     </row>
     <row r="30" spans="1:7" ht="15.75">
       <c r="A30" s="99"/>
-      <c r="B30" s="257" t="s">
+      <c r="B30" s="221" t="s">
         <v>914</v>
       </c>
-      <c r="C30" s="258"/>
-      <c r="D30" s="260" t="s">
+      <c r="C30" s="222"/>
+      <c r="D30" s="223" t="s">
         <v>915</v>
       </c>
-      <c r="E30" s="260"/>
-      <c r="F30" s="260"/>
-      <c r="G30" s="261"/>
+      <c r="E30" s="223"/>
+      <c r="F30" s="223"/>
+      <c r="G30" s="224"/>
     </row>
     <row r="31" spans="1:7" ht="15.75">
       <c r="A31" s="99"/>
-      <c r="B31" s="257" t="s">
+      <c r="B31" s="221" t="s">
         <v>912</v>
       </c>
-      <c r="C31" s="258"/>
+      <c r="C31" s="222"/>
       <c r="D31" s="225" t="s">
         <v>913</v>
       </c>
       <c r="E31" s="225"/>
       <c r="F31" s="225"/>
-      <c r="G31" s="259"/>
+      <c r="G31" s="226"/>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickBot="1">
       <c r="A32" s="99"/>
-      <c r="B32" s="257" t="s">
+      <c r="B32" s="221" t="s">
         <v>928</v>
       </c>
-      <c r="C32" s="258"/>
+      <c r="C32" s="222"/>
       <c r="D32" s="225" t="s">
         <v>929</v>
       </c>
       <c r="E32" s="225"/>
       <c r="F32" s="225"/>
-      <c r="G32" s="259"/>
+      <c r="G32" s="226"/>
     </row>
     <row r="33" spans="1:7" ht="15.75">
       <c r="A33" s="98" t="s">
         <v>918</v>
       </c>
-      <c r="B33" s="238" t="s">
+      <c r="B33" s="227" t="s">
         <v>919</v>
       </c>
-      <c r="C33" s="239"/>
-      <c r="D33" s="239"/>
-      <c r="E33" s="239"/>
-      <c r="F33" s="239"/>
-      <c r="G33" s="240"/>
+      <c r="C33" s="228"/>
+      <c r="D33" s="228"/>
+      <c r="E33" s="228"/>
+      <c r="F33" s="228"/>
+      <c r="G33" s="229"/>
     </row>
     <row r="34" spans="1:7" ht="15.75">
       <c r="A34" s="99"/>
-      <c r="B34" s="257" t="s">
+      <c r="B34" s="221" t="s">
         <v>920</v>
       </c>
-      <c r="C34" s="258"/>
-      <c r="D34" s="260" t="s">
+      <c r="C34" s="222"/>
+      <c r="D34" s="223" t="s">
         <v>925</v>
       </c>
-      <c r="E34" s="260"/>
-      <c r="F34" s="260"/>
-      <c r="G34" s="261"/>
+      <c r="E34" s="223"/>
+      <c r="F34" s="223"/>
+      <c r="G34" s="224"/>
     </row>
     <row r="35" spans="1:7" ht="15.75">
       <c r="A35" s="99"/>
-      <c r="B35" s="257" t="s">
+      <c r="B35" s="221" t="s">
         <v>921</v>
       </c>
-      <c r="C35" s="258"/>
-      <c r="D35" s="260" t="s">
+      <c r="C35" s="222"/>
+      <c r="D35" s="223" t="s">
         <v>926</v>
       </c>
-      <c r="E35" s="260"/>
-      <c r="F35" s="260"/>
-      <c r="G35" s="261"/>
+      <c r="E35" s="223"/>
+      <c r="F35" s="223"/>
+      <c r="G35" s="224"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" thickBot="1">
       <c r="A36" s="99"/>
-      <c r="B36" s="257" t="s">
+      <c r="B36" s="221" t="s">
         <v>922</v>
       </c>
-      <c r="C36" s="258"/>
-      <c r="D36" s="260" t="s">
+      <c r="C36" s="222"/>
+      <c r="D36" s="223" t="s">
         <v>927</v>
       </c>
-      <c r="E36" s="260"/>
-      <c r="F36" s="260"/>
-      <c r="G36" s="261"/>
+      <c r="E36" s="223"/>
+      <c r="F36" s="223"/>
+      <c r="G36" s="224"/>
     </row>
     <row r="37" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="A37" s="98" t="s">
         <v>923</v>
       </c>
-      <c r="B37" s="238" t="s">
+      <c r="B37" s="227" t="s">
         <v>924</v>
       </c>
-      <c r="C37" s="239"/>
-      <c r="D37" s="239"/>
-      <c r="E37" s="239"/>
-      <c r="F37" s="239"/>
-      <c r="G37" s="240"/>
+      <c r="C37" s="228"/>
+      <c r="D37" s="228"/>
+      <c r="E37" s="228"/>
+      <c r="F37" s="228"/>
+      <c r="G37" s="229"/>
     </row>
     <row r="38" spans="1:7" ht="29.1" customHeight="1">
-      <c r="A38" s="235" t="s">
+      <c r="A38" s="248" t="s">
         <v>517</v>
       </c>
-      <c r="B38" s="238" t="s">
+      <c r="B38" s="227" t="s">
         <v>490</v>
       </c>
-      <c r="C38" s="239"/>
-      <c r="D38" s="239"/>
-      <c r="E38" s="239"/>
-      <c r="F38" s="239"/>
-      <c r="G38" s="240"/>
+      <c r="C38" s="228"/>
+      <c r="D38" s="228"/>
+      <c r="E38" s="228"/>
+      <c r="F38" s="228"/>
+      <c r="G38" s="229"/>
     </row>
     <row r="39" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A39" s="236"/>
-      <c r="B39" s="241"/>
-      <c r="C39" s="242"/>
-      <c r="D39" s="242"/>
-      <c r="E39" s="242"/>
-      <c r="F39" s="242"/>
-      <c r="G39" s="243"/>
+      <c r="A39" s="249"/>
+      <c r="B39" s="251"/>
+      <c r="C39" s="252"/>
+      <c r="D39" s="252"/>
+      <c r="E39" s="252"/>
+      <c r="F39" s="252"/>
+      <c r="G39" s="253"/>
     </row>
     <row r="40" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A40" s="236"/>
-      <c r="B40" s="244" t="s">
+      <c r="A40" s="249"/>
+      <c r="B40" s="254" t="s">
         <v>491</v>
       </c>
-      <c r="C40" s="245"/>
-      <c r="D40" s="245"/>
-      <c r="E40" s="245"/>
-      <c r="F40" s="245"/>
-      <c r="G40" s="246"/>
+      <c r="C40" s="255"/>
+      <c r="D40" s="255"/>
+      <c r="E40" s="255"/>
+      <c r="F40" s="255"/>
+      <c r="G40" s="256"/>
     </row>
     <row r="41" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A41" s="236"/>
-      <c r="B41" s="224" t="s">
+      <c r="A41" s="249"/>
+      <c r="B41" s="257" t="s">
         <v>492</v>
       </c>
       <c r="C41" s="225"/>
       <c r="D41" s="225"/>
       <c r="E41" s="225"/>
       <c r="F41" s="225"/>
-      <c r="G41" s="226"/>
+      <c r="G41" s="258"/>
     </row>
     <row r="42" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A42" s="236"/>
-      <c r="B42" s="241"/>
-      <c r="C42" s="242"/>
-      <c r="D42" s="242"/>
-      <c r="E42" s="242"/>
-      <c r="F42" s="242"/>
-      <c r="G42" s="243"/>
+      <c r="A42" s="249"/>
+      <c r="B42" s="251"/>
+      <c r="C42" s="252"/>
+      <c r="D42" s="252"/>
+      <c r="E42" s="252"/>
+      <c r="F42" s="252"/>
+      <c r="G42" s="253"/>
     </row>
     <row r="43" spans="1:7" ht="42.95" customHeight="1">
-      <c r="A43" s="236"/>
-      <c r="B43" s="224" t="s">
+      <c r="A43" s="249"/>
+      <c r="B43" s="257" t="s">
         <v>493</v>
       </c>
       <c r="C43" s="225"/>
       <c r="D43" s="225"/>
       <c r="E43" s="225"/>
       <c r="F43" s="225"/>
-      <c r="G43" s="226"/>
+      <c r="G43" s="258"/>
     </row>
     <row r="44" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A44" s="236"/>
-      <c r="B44" s="241"/>
-      <c r="C44" s="242"/>
-      <c r="D44" s="242"/>
-      <c r="E44" s="242"/>
-      <c r="F44" s="242"/>
-      <c r="G44" s="243"/>
+      <c r="A44" s="249"/>
+      <c r="B44" s="251"/>
+      <c r="C44" s="252"/>
+      <c r="D44" s="252"/>
+      <c r="E44" s="252"/>
+      <c r="F44" s="252"/>
+      <c r="G44" s="253"/>
     </row>
     <row r="45" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A45" s="236"/>
-      <c r="B45" s="224" t="s">
+      <c r="A45" s="249"/>
+      <c r="B45" s="257" t="s">
         <v>494</v>
       </c>
       <c r="C45" s="225"/>
       <c r="D45" s="225"/>
       <c r="E45" s="225"/>
       <c r="F45" s="225"/>
-      <c r="G45" s="226"/>
+      <c r="G45" s="258"/>
     </row>
     <row r="46" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A46" s="236"/>
-      <c r="B46" s="224" t="s">
+      <c r="A46" s="249"/>
+      <c r="B46" s="257" t="s">
         <v>495</v>
       </c>
       <c r="C46" s="225"/>
       <c r="D46" s="225"/>
       <c r="E46" s="225"/>
       <c r="F46" s="225"/>
-      <c r="G46" s="226"/>
+      <c r="G46" s="258"/>
     </row>
     <row r="47" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A47" s="236"/>
-      <c r="B47" s="224" t="s">
+      <c r="A47" s="249"/>
+      <c r="B47" s="257" t="s">
         <v>496</v>
       </c>
       <c r="C47" s="225"/>
       <c r="D47" s="225"/>
       <c r="E47" s="225"/>
       <c r="F47" s="225"/>
-      <c r="G47" s="226"/>
+      <c r="G47" s="258"/>
     </row>
     <row r="48" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A48" s="236"/>
-      <c r="B48" s="224" t="s">
+      <c r="A48" s="249"/>
+      <c r="B48" s="257" t="s">
         <v>497</v>
       </c>
       <c r="C48" s="225"/>
       <c r="D48" s="225"/>
       <c r="E48" s="225"/>
       <c r="F48" s="225"/>
-      <c r="G48" s="226"/>
+      <c r="G48" s="258"/>
     </row>
     <row r="49" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A49" s="236"/>
-      <c r="B49" s="224" t="s">
+      <c r="A49" s="249"/>
+      <c r="B49" s="257" t="s">
         <v>498</v>
       </c>
       <c r="C49" s="225"/>
       <c r="D49" s="225"/>
       <c r="E49" s="225"/>
       <c r="F49" s="225"/>
-      <c r="G49" s="226"/>
+      <c r="G49" s="258"/>
     </row>
     <row r="50" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A50" s="236"/>
-      <c r="B50" s="224" t="s">
+      <c r="A50" s="249"/>
+      <c r="B50" s="257" t="s">
         <v>499</v>
       </c>
       <c r="C50" s="225"/>
       <c r="D50" s="225"/>
       <c r="E50" s="225"/>
       <c r="F50" s="225"/>
-      <c r="G50" s="226"/>
+      <c r="G50" s="258"/>
     </row>
     <row r="51" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A51" s="236"/>
-      <c r="B51" s="224" t="s">
+      <c r="A51" s="249"/>
+      <c r="B51" s="257" t="s">
         <v>500</v>
       </c>
       <c r="C51" s="225"/>
       <c r="D51" s="225"/>
       <c r="E51" s="225"/>
       <c r="F51" s="225"/>
-      <c r="G51" s="226"/>
+      <c r="G51" s="258"/>
     </row>
     <row r="52" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A52" s="237"/>
-      <c r="B52" s="227" t="s">
+      <c r="A52" s="250"/>
+      <c r="B52" s="259" t="s">
         <v>501</v>
       </c>
-      <c r="C52" s="228"/>
-      <c r="D52" s="228"/>
-      <c r="E52" s="228"/>
-      <c r="F52" s="228"/>
-      <c r="G52" s="229"/>
+      <c r="C52" s="260"/>
+      <c r="D52" s="260"/>
+      <c r="E52" s="260"/>
+      <c r="F52" s="260"/>
+      <c r="G52" s="261"/>
     </row>
     <row r="53" spans="1:7" ht="57.95" customHeight="1" thickBot="1">
       <c r="A53" s="10" t="s">
         <v>516</v>
       </c>
-      <c r="B53" s="221" t="s">
+      <c r="B53" s="230" t="s">
         <v>581</v>
       </c>
-      <c r="C53" s="222"/>
-      <c r="D53" s="222"/>
-      <c r="E53" s="222"/>
-      <c r="F53" s="222"/>
-      <c r="G53" s="223"/>
+      <c r="C53" s="231"/>
+      <c r="D53" s="231"/>
+      <c r="E53" s="231"/>
+      <c r="F53" s="231"/>
+      <c r="G53" s="232"/>
     </row>
     <row r="54" spans="1:7" ht="57.95" customHeight="1" thickBot="1">
       <c r="A54" s="10" t="s">
         <v>515</v>
       </c>
-      <c r="B54" s="221" t="s">
+      <c r="B54" s="230" t="s">
         <v>502</v>
       </c>
-      <c r="C54" s="222"/>
-      <c r="D54" s="222"/>
-      <c r="E54" s="222"/>
-      <c r="F54" s="222"/>
-      <c r="G54" s="223"/>
+      <c r="C54" s="231"/>
+      <c r="D54" s="231"/>
+      <c r="E54" s="231"/>
+      <c r="F54" s="231"/>
+      <c r="G54" s="232"/>
     </row>
     <row r="55" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A55" s="10" t="s">
         <v>514</v>
       </c>
-      <c r="B55" s="221" t="s">
+      <c r="B55" s="230" t="s">
         <v>503</v>
       </c>
-      <c r="C55" s="222"/>
-      <c r="D55" s="222"/>
-      <c r="E55" s="222"/>
-      <c r="F55" s="222"/>
-      <c r="G55" s="223"/>
+      <c r="C55" s="231"/>
+      <c r="D55" s="231"/>
+      <c r="E55" s="231"/>
+      <c r="F55" s="231"/>
+      <c r="G55" s="232"/>
     </row>
     <row r="56" spans="1:7" ht="42.95" customHeight="1" thickBot="1">
       <c r="A56" s="11" t="s">
         <v>508</v>
       </c>
-      <c r="B56" s="221" t="s">
+      <c r="B56" s="230" t="s">
         <v>504</v>
       </c>
-      <c r="C56" s="222"/>
-      <c r="D56" s="222"/>
-      <c r="E56" s="222"/>
-      <c r="F56" s="222"/>
-      <c r="G56" s="223"/>
+      <c r="C56" s="231"/>
+      <c r="D56" s="231"/>
+      <c r="E56" s="231"/>
+      <c r="F56" s="231"/>
+      <c r="G56" s="232"/>
     </row>
     <row r="57" spans="1:7" ht="29.1" customHeight="1" thickBot="1">
       <c r="A57" s="10" t="s">
         <v>513</v>
       </c>
-      <c r="B57" s="221" t="s">
+      <c r="B57" s="230" t="s">
         <v>505</v>
       </c>
-      <c r="C57" s="222"/>
-      <c r="D57" s="222"/>
-      <c r="E57" s="222"/>
-      <c r="F57" s="222"/>
-      <c r="G57" s="223"/>
+      <c r="C57" s="231"/>
+      <c r="D57" s="231"/>
+      <c r="E57" s="231"/>
+      <c r="F57" s="231"/>
+      <c r="G57" s="232"/>
     </row>
     <row r="58" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A58" s="10" t="s">
         <v>512</v>
       </c>
-      <c r="B58" s="221" t="s">
+      <c r="B58" s="230" t="s">
         <v>506</v>
       </c>
-      <c r="C58" s="222"/>
-      <c r="D58" s="222"/>
-      <c r="E58" s="222"/>
-      <c r="F58" s="222"/>
-      <c r="G58" s="223"/>
+      <c r="C58" s="231"/>
+      <c r="D58" s="231"/>
+      <c r="E58" s="231"/>
+      <c r="F58" s="231"/>
+      <c r="G58" s="232"/>
     </row>
     <row r="59" spans="1:7" ht="42.95" customHeight="1" thickBot="1">
       <c r="A59" s="11" t="s">
         <v>509</v>
       </c>
-      <c r="B59" s="221" t="s">
+      <c r="B59" s="230" t="s">
         <v>510</v>
       </c>
-      <c r="C59" s="222"/>
-      <c r="D59" s="222"/>
-      <c r="E59" s="222"/>
-      <c r="F59" s="222"/>
-      <c r="G59" s="223"/>
+      <c r="C59" s="231"/>
+      <c r="D59" s="231"/>
+      <c r="E59" s="231"/>
+      <c r="F59" s="231"/>
+      <c r="G59" s="232"/>
     </row>
     <row r="60" spans="1:7" ht="29.1" customHeight="1" thickBot="1">
       <c r="A60" s="10" t="s">
         <v>511</v>
       </c>
-      <c r="B60" s="221" t="s">
+      <c r="B60" s="230" t="s">
         <v>507</v>
       </c>
-      <c r="C60" s="222"/>
-      <c r="D60" s="222"/>
-      <c r="E60" s="222"/>
-      <c r="F60" s="222"/>
-      <c r="G60" s="223"/>
+      <c r="C60" s="231"/>
+      <c r="D60" s="231"/>
+      <c r="E60" s="231"/>
+      <c r="F60" s="231"/>
+      <c r="G60" s="232"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="A38:A52"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="B37:G37"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="D29:G29"/>
@@ -41753,49 +41785,17 @@
     <mergeCell ref="D34:G34"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="D35:G35"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="A38:A52"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="B43:G43"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B53:G53"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:G28"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -41806,7 +41806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
@@ -42019,10 +42019,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>485</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -42268,10 +42268,10 @@
       <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A23" s="232" t="s">
+      <c r="A23" s="235" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="234"/>
+      <c r="B23" s="237"/>
       <c r="C23" s="4" t="s">
         <v>63</v>
       </c>
@@ -42574,10 +42574,10 @@
       <c r="G38" s="11"/>
     </row>
     <row r="39" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A39" s="232" t="s">
+      <c r="A39" s="235" t="s">
         <v>524</v>
       </c>
-      <c r="B39" s="234"/>
+      <c r="B39" s="237"/>
       <c r="C39" s="4" t="s">
         <v>63</v>
       </c>
@@ -42690,10 +42690,10 @@
       <c r="G44" s="11"/>
     </row>
     <row r="45" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A45" s="232" t="s">
+      <c r="A45" s="235" t="s">
         <v>529</v>
       </c>
-      <c r="B45" s="234"/>
+      <c r="B45" s="237"/>
       <c r="C45" s="4" t="s">
         <v>63</v>
       </c>
@@ -42825,10 +42825,10 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A52" s="232" t="s">
+      <c r="A52" s="235" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="234"/>
+      <c r="B52" s="237"/>
       <c r="C52" s="4" t="s">
         <v>63</v>
       </c>
@@ -42998,10 +42998,10 @@
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A61" s="232" t="s">
+      <c r="A61" s="235" t="s">
         <v>111</v>
       </c>
-      <c r="B61" s="234"/>
+      <c r="B61" s="237"/>
       <c r="C61" s="4" t="s">
         <v>63</v>
       </c>
@@ -43095,10 +43095,10 @@
       <c r="G65" s="11"/>
     </row>
     <row r="66" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A66" s="232" t="s">
+      <c r="A66" s="235" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="234"/>
+      <c r="B66" s="237"/>
       <c r="C66" s="4" t="s">
         <v>63</v>
       </c>
@@ -43384,10 +43384,10 @@
       <c r="G80" s="11"/>
     </row>
     <row r="81" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A81" s="232" t="s">
+      <c r="A81" s="235" t="s">
         <v>133</v>
       </c>
-      <c r="B81" s="234"/>
+      <c r="B81" s="237"/>
       <c r="C81" s="4" t="s">
         <v>63</v>
       </c>
@@ -43519,10 +43519,10 @@
       <c r="G87" s="11"/>
     </row>
     <row r="88" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A88" s="232" t="s">
+      <c r="A88" s="235" t="s">
         <v>558</v>
       </c>
-      <c r="B88" s="234"/>
+      <c r="B88" s="237"/>
       <c r="C88" s="4" t="s">
         <v>63</v>
       </c>
@@ -43637,10 +43637,10 @@
       <c r="G93" s="11"/>
     </row>
     <row r="94" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A94" s="232" t="s">
+      <c r="A94" s="235" t="s">
         <v>156</v>
       </c>
-      <c r="B94" s="234"/>
+      <c r="B94" s="237"/>
       <c r="C94" s="4" t="s">
         <v>63</v>
       </c>
@@ -43715,10 +43715,10 @@
       <c r="G97" s="11"/>
     </row>
     <row r="98" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A98" s="232" t="s">
+      <c r="A98" s="235" t="s">
         <v>150</v>
       </c>
-      <c r="B98" s="234"/>
+      <c r="B98" s="237"/>
       <c r="C98" s="4" t="s">
         <v>63</v>
       </c>
@@ -43793,10 +43793,10 @@
       <c r="G101" s="11"/>
     </row>
     <row r="102" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A102" s="232" t="s">
+      <c r="A102" s="235" t="s">
         <v>547</v>
       </c>
-      <c r="B102" s="234"/>
+      <c r="B102" s="237"/>
       <c r="C102" s="4" t="s">
         <v>63</v>
       </c>
@@ -43892,10 +43892,10 @@
       <c r="G106" s="11"/>
     </row>
     <row r="107" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A107" s="232" t="s">
+      <c r="A107" s="235" t="s">
         <v>140</v>
       </c>
-      <c r="B107" s="234"/>
+      <c r="B107" s="237"/>
       <c r="C107" s="4" t="s">
         <v>63</v>
       </c>
@@ -44046,10 +44046,10 @@
       <c r="G114" s="11"/>
     </row>
     <row r="115" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A115" s="232" t="s">
+      <c r="A115" s="235" t="s">
         <v>161</v>
       </c>
-      <c r="B115" s="234"/>
+      <c r="B115" s="237"/>
       <c r="C115" s="4" t="s">
         <v>453</v>
       </c>
@@ -44220,6 +44220,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A88:B88"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="C2:D9"/>
@@ -44229,14 +44237,6 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A88:B88"/>
   </mergeCells>
   <conditionalFormatting sqref="A11:A18 A107:A109 A81:A85 A115:A248 A52:A57 A40 A33:A37 A42:A43 A112 A94:A100 A61:A69 A59 A20:A29">
     <cfRule type="beginsWith" dxfId="2421" priority="1148" stopIfTrue="1" operator="beginsWith" text="Exceptional">
@@ -46685,10 +46685,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>701</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -46972,10 +46972,10 @@
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A25" s="232" t="s">
+      <c r="A25" s="235" t="s">
         <v>688</v>
       </c>
-      <c r="B25" s="234"/>
+      <c r="B25" s="237"/>
       <c r="C25" s="4" t="s">
         <v>63</v>
       </c>
@@ -47183,10 +47183,10 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A36" s="232" t="s">
+      <c r="A36" s="235" t="s">
         <v>612</v>
       </c>
-      <c r="B36" s="234"/>
+      <c r="B36" s="237"/>
       <c r="C36" s="4" t="s">
         <v>63</v>
       </c>
@@ -47605,10 +47605,10 @@
       <c r="G57" s="11"/>
     </row>
     <row r="58" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A58" s="232" t="s">
+      <c r="A58" s="235" t="s">
         <v>627</v>
       </c>
-      <c r="B58" s="234"/>
+      <c r="B58" s="237"/>
       <c r="C58" s="4" t="s">
         <v>63</v>
       </c>
@@ -47911,10 +47911,10 @@
       <c r="G73" s="11"/>
     </row>
     <row r="74" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A74" s="232" t="s">
+      <c r="A74" s="235" t="s">
         <v>651</v>
       </c>
-      <c r="B74" s="234"/>
+      <c r="B74" s="237"/>
       <c r="C74" s="4" t="s">
         <v>63</v>
       </c>
@@ -48103,10 +48103,10 @@
       <c r="G83" s="11"/>
     </row>
     <row r="84" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A84" s="232" t="s">
+      <c r="A84" s="235" t="s">
         <v>663</v>
       </c>
-      <c r="B84" s="234"/>
+      <c r="B84" s="237"/>
       <c r="C84" s="21" t="s">
         <v>456</v>
       </c>
@@ -48466,10 +48466,10 @@
       <c r="G102" s="11"/>
     </row>
     <row r="103" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A103" s="232" t="s">
+      <c r="A103" s="235" t="s">
         <v>677</v>
       </c>
-      <c r="B103" s="234"/>
+      <c r="B103" s="237"/>
       <c r="C103" s="4" t="s">
         <v>63</v>
       </c>
@@ -51637,10 +51637,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>291</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -52000,10 +52000,10 @@
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A29" s="232" t="s">
+      <c r="A29" s="235" t="s">
         <v>564</v>
       </c>
-      <c r="B29" s="234"/>
+      <c r="B29" s="237"/>
       <c r="C29" s="4" t="s">
         <v>451</v>
       </c>
@@ -52232,10 +52232,10 @@
       <c r="G40" s="11"/>
     </row>
     <row r="41" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A41" s="232" t="s">
+      <c r="A41" s="235" t="s">
         <v>334</v>
       </c>
-      <c r="B41" s="234"/>
+      <c r="B41" s="237"/>
       <c r="C41" s="4" t="s">
         <v>63</v>
       </c>
@@ -52447,10 +52447,10 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" s="7" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A52" s="232" t="s">
+      <c r="A52" s="235" t="s">
         <v>84</v>
       </c>
-      <c r="B52" s="234"/>
+      <c r="B52" s="237"/>
       <c r="C52" s="4" t="s">
         <v>63</v>
       </c>
@@ -52620,10 +52620,10 @@
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" s="7" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A61" s="232" t="s">
+      <c r="A61" s="235" t="s">
         <v>370</v>
       </c>
-      <c r="B61" s="234"/>
+      <c r="B61" s="237"/>
       <c r="C61" s="21" t="s">
         <v>452</v>
       </c>
@@ -53760,8 +53760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -53973,10 +53973,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>810</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -54279,10 +54279,10 @@
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A26" s="232" t="s">
+      <c r="A26" s="235" t="s">
         <v>390</v>
       </c>
-      <c r="B26" s="234"/>
+      <c r="B26" s="237"/>
       <c r="C26" s="4" t="s">
         <v>855</v>
       </c>
@@ -54547,10 +54547,10 @@
       <c r="G39" s="11"/>
     </row>
     <row r="40" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A40" s="232" t="s">
+      <c r="A40" s="235" t="s">
         <v>448</v>
       </c>
-      <c r="B40" s="234"/>
+      <c r="B40" s="237"/>
       <c r="C40" s="102" t="s">
         <v>856</v>
       </c>
@@ -54815,10 +54815,10 @@
       <c r="G53" s="11"/>
     </row>
     <row r="54" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A54" s="232" t="s">
+      <c r="A54" s="235" t="s">
         <v>412</v>
       </c>
-      <c r="B54" s="234"/>
+      <c r="B54" s="237"/>
       <c r="C54" s="4" t="s">
         <v>63</v>
       </c>
@@ -56677,10 +56677,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>239</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -56774,10 +56774,10 @@
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A15" s="232" t="s">
+      <c r="A15" s="235" t="s">
         <v>246</v>
       </c>
-      <c r="B15" s="234"/>
+      <c r="B15" s="237"/>
       <c r="C15" s="4" t="s">
         <v>874</v>
       </c>
@@ -56890,10 +56890,10 @@
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A21" s="232" t="s">
+      <c r="A21" s="235" t="s">
         <v>878</v>
       </c>
-      <c r="B21" s="234"/>
+      <c r="B21" s="237"/>
       <c r="C21" s="4" t="s">
         <v>63</v>
       </c>
@@ -57025,10 +57025,10 @@
       <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A28" s="232" t="s">
+      <c r="A28" s="235" t="s">
         <v>254</v>
       </c>
-      <c r="B28" s="234"/>
+      <c r="B28" s="237"/>
       <c r="C28" s="4" t="s">
         <v>875</v>
       </c>
@@ -57179,10 +57179,10 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A36" s="232" t="s">
+      <c r="A36" s="235" t="s">
         <v>891</v>
       </c>
-      <c r="B36" s="234"/>
+      <c r="B36" s="237"/>
       <c r="C36" s="4" t="s">
         <v>454</v>
       </c>
@@ -57314,10 +57314,10 @@
       <c r="G42" s="11"/>
     </row>
     <row r="43" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A43" s="232" t="s">
+      <c r="A43" s="235" t="s">
         <v>275</v>
       </c>
-      <c r="B43" s="234"/>
+      <c r="B43" s="237"/>
       <c r="C43" s="4" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Added the restart game option and updated the credits.
</commit_message>
<xml_diff>
--- a/GameDocuments/gam352_papercut_rubric.xlsx
+++ b/GameDocuments/gam352_papercut_rubric.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2303" uniqueCount="964">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2305" uniqueCount="966">
   <si>
     <t>GAME NAME</t>
   </si>
@@ -3667,13 +3667,22 @@
     <t>Pull tabs</t>
   </si>
   <si>
-    <t>Windows 7,8,10</t>
-  </si>
-  <si>
     <t xml:space="preserve">Unity </t>
   </si>
   <si>
     <t xml:space="preserve">Pressing 0-9 skips to different levels in the game </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tested on my laptop with integrated graphics card.  Runs at resonable framerate on normal quality </t>
+  </si>
+  <si>
+    <t>Windows 7,8,10 -
+ Windows 7 school computer
+Windows 8 laptop
+Windows 10 laptop</t>
+  </si>
+  <si>
+    <t>Unity Launcher</t>
   </si>
 </sst>
 </file>
@@ -5716,6 +5725,90 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -5749,18 +5842,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -5818,99 +5899,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="4" borderId="16" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="4" borderId="18" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="26" fillId="3" borderId="21" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5921,6 +5909,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="26" fillId="3" borderId="26" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5989,55 +5983,37 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="4" borderId="16" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="4" borderId="18" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6049,28 +6025,28 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6097,19 +6073,52 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -38646,54 +38655,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="178"/>
+      <c r="B1" s="145"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="146"/>
       <c r="E1" s="103"/>
-      <c r="F1" s="176" t="s">
+      <c r="F1" s="144" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="177"/>
-      <c r="H1" s="177"/>
-      <c r="I1" s="177"/>
-      <c r="J1" s="178"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
+      <c r="J1" s="146"/>
       <c r="K1" s="104"/>
       <c r="L1" s="104"/>
       <c r="M1" s="105"/>
     </row>
     <row r="2" spans="1:13" ht="14.1" customHeight="1">
-      <c r="A2" s="182" t="s">
+      <c r="A2" s="147" t="s">
         <v>951</v>
       </c>
-      <c r="B2" s="183"/>
-      <c r="C2" s="183"/>
-      <c r="D2" s="184"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="149"/>
       <c r="E2" s="103"/>
-      <c r="F2" s="182" t="s">
+      <c r="F2" s="147" t="s">
         <v>954</v>
       </c>
-      <c r="G2" s="183"/>
-      <c r="H2" s="183"/>
-      <c r="I2" s="183"/>
-      <c r="J2" s="184"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="149"/>
       <c r="K2" s="104"/>
       <c r="L2" s="104"/>
       <c r="M2" s="105"/>
     </row>
     <row r="3" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A3" s="185"/>
-      <c r="B3" s="186"/>
-      <c r="C3" s="186"/>
-      <c r="D3" s="187"/>
+      <c r="A3" s="150"/>
+      <c r="B3" s="151"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="103"/>
-      <c r="F3" s="185"/>
-      <c r="G3" s="186"/>
-      <c r="H3" s="186"/>
-      <c r="I3" s="186"/>
-      <c r="J3" s="187"/>
+      <c r="F3" s="150"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="151"/>
+      <c r="J3" s="152"/>
       <c r="K3" s="104"/>
       <c r="L3" s="104"/>
       <c r="M3" s="105"/>
@@ -38714,41 +38723,41 @@
       <c r="M4" s="105"/>
     </row>
     <row r="5" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="144" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="177"/>
-      <c r="C5" s="177"/>
-      <c r="D5" s="178"/>
+      <c r="B5" s="145"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="146"/>
       <c r="E5" s="103"/>
-      <c r="F5" s="176" t="s">
+      <c r="F5" s="144" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="177"/>
-      <c r="H5" s="177"/>
-      <c r="I5" s="177"/>
-      <c r="J5" s="178"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="145"/>
+      <c r="I5" s="145"/>
+      <c r="J5" s="146"/>
       <c r="K5" s="104"/>
       <c r="L5" s="107"/>
       <c r="M5" s="105"/>
     </row>
     <row r="6" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="156" t="s">
         <v>952</v>
       </c>
-      <c r="B6" s="174"/>
-      <c r="C6" s="174"/>
-      <c r="D6" s="175"/>
+      <c r="B6" s="157"/>
+      <c r="C6" s="157"/>
+      <c r="D6" s="158"/>
       <c r="E6" s="103"/>
-      <c r="F6" s="173" t="s">
+      <c r="F6" s="156" t="s">
         <v>955</v>
       </c>
-      <c r="G6" s="174"/>
-      <c r="H6" s="174"/>
-      <c r="I6" s="174"/>
-      <c r="J6" s="175"/>
+      <c r="G6" s="157"/>
+      <c r="H6" s="157"/>
+      <c r="I6" s="157"/>
+      <c r="J6" s="158"/>
       <c r="K6" s="104"/>
-      <c r="L6" s="170" t="s">
+      <c r="L6" s="153" t="s">
         <v>24</v>
       </c>
       <c r="M6" s="105"/>
@@ -38759,47 +38768,47 @@
       <c r="C7" s="108"/>
       <c r="D7" s="109"/>
       <c r="E7" s="103"/>
-      <c r="F7" s="173"/>
-      <c r="G7" s="174"/>
-      <c r="H7" s="174"/>
-      <c r="I7" s="174"/>
-      <c r="J7" s="175"/>
+      <c r="F7" s="156"/>
+      <c r="G7" s="157"/>
+      <c r="H7" s="157"/>
+      <c r="I7" s="157"/>
+      <c r="J7" s="158"/>
       <c r="K7" s="104"/>
-      <c r="L7" s="171"/>
+      <c r="L7" s="154"/>
       <c r="M7" s="105"/>
     </row>
     <row r="8" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="144" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="177"/>
-      <c r="C8" s="177"/>
-      <c r="D8" s="178"/>
+      <c r="B8" s="145"/>
+      <c r="C8" s="145"/>
+      <c r="D8" s="146"/>
       <c r="E8" s="103"/>
-      <c r="F8" s="173"/>
-      <c r="G8" s="174"/>
-      <c r="H8" s="174"/>
-      <c r="I8" s="174"/>
-      <c r="J8" s="175"/>
+      <c r="F8" s="156"/>
+      <c r="G8" s="157"/>
+      <c r="H8" s="157"/>
+      <c r="I8" s="157"/>
+      <c r="J8" s="158"/>
       <c r="K8" s="104"/>
-      <c r="L8" s="171"/>
+      <c r="L8" s="154"/>
       <c r="M8" s="105"/>
     </row>
     <row r="9" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="156" t="s">
         <v>953</v>
       </c>
-      <c r="B9" s="174"/>
-      <c r="C9" s="174"/>
-      <c r="D9" s="175"/>
+      <c r="B9" s="157"/>
+      <c r="C9" s="157"/>
+      <c r="D9" s="158"/>
       <c r="E9" s="103"/>
-      <c r="F9" s="173"/>
-      <c r="G9" s="174"/>
-      <c r="H9" s="174"/>
-      <c r="I9" s="174"/>
-      <c r="J9" s="175"/>
+      <c r="F9" s="156"/>
+      <c r="G9" s="157"/>
+      <c r="H9" s="157"/>
+      <c r="I9" s="157"/>
+      <c r="J9" s="158"/>
       <c r="K9" s="104"/>
-      <c r="L9" s="172"/>
+      <c r="L9" s="155"/>
       <c r="M9" s="105"/>
     </row>
     <row r="10" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -38818,18 +38827,18 @@
       <c r="M10" s="105"/>
     </row>
     <row r="11" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="144" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="177"/>
-      <c r="C11" s="177"/>
-      <c r="D11" s="178"/>
+      <c r="B11" s="145"/>
+      <c r="C11" s="145"/>
+      <c r="D11" s="146"/>
       <c r="E11" s="103"/>
-      <c r="F11" s="176" t="s">
+      <c r="F11" s="144" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="177"/>
-      <c r="H11" s="178"/>
+      <c r="G11" s="145"/>
+      <c r="H11" s="146"/>
       <c r="I11" s="134" t="s">
         <v>7</v>
       </c>
@@ -38869,7 +38878,7 @@
         <v>-0.12</v>
       </c>
       <c r="K12" s="104"/>
-      <c r="L12" s="170" t="s">
+      <c r="L12" s="153" t="s">
         <v>8</v>
       </c>
       <c r="M12" s="105"/>
@@ -38902,7 +38911,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="120"/>
-      <c r="L13" s="171"/>
+      <c r="L13" s="154"/>
       <c r="M13" s="121"/>
     </row>
     <row r="14" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -38932,7 +38941,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="124"/>
-      <c r="L14" s="172"/>
+      <c r="L14" s="155"/>
       <c r="M14" s="125"/>
     </row>
     <row r="15" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39000,11 +39009,11 @@
         <v>939</v>
       </c>
       <c r="E17" s="104"/>
-      <c r="F17" s="176" t="s">
+      <c r="F17" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="177"/>
-      <c r="H17" s="178"/>
+      <c r="G17" s="145"/>
+      <c r="H17" s="146"/>
       <c r="I17" s="111"/>
       <c r="J17" s="135">
         <v>0.75</v>
@@ -39030,17 +39039,17 @@
       <c r="F18" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="179" t="s">
+      <c r="G18" s="159" t="s">
         <v>956</v>
       </c>
-      <c r="H18" s="180"/>
-      <c r="I18" s="181"/>
+      <c r="H18" s="160"/>
+      <c r="I18" s="161"/>
       <c r="J18" s="137">
         <f>IF(LEFT(G18,6)="Entire",0,IF(LEFT(G18,6)="Custom",-0.05,-0.1))</f>
         <v>-0.1</v>
       </c>
       <c r="K18" s="128"/>
-      <c r="L18" s="170" t="s">
+      <c r="L18" s="153" t="s">
         <v>18</v>
       </c>
       <c r="M18" s="105"/>
@@ -39060,17 +39069,17 @@
       <c r="F19" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="153" t="s">
+      <c r="G19" s="162" t="s">
         <v>957</v>
       </c>
-      <c r="H19" s="154"/>
-      <c r="I19" s="155"/>
+      <c r="H19" s="163"/>
+      <c r="I19" s="164"/>
       <c r="J19" s="139">
         <f>IF(G19="2D Graphics and 2D Gameplay",IF(J11=0.15,-0.05,0),IF(G19="3D Graphics but 2D Gameplay",IF(J11=0.15,-0.02,-0.3),IF(J11=0.15,0,-0.3)))</f>
         <v>0</v>
       </c>
       <c r="K19" s="104"/>
-      <c r="L19" s="172"/>
+      <c r="L19" s="155"/>
       <c r="M19" s="105"/>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39120,22 +39129,22 @@
       <c r="C22" s="118"/>
       <c r="D22" s="119"/>
       <c r="E22" s="104"/>
-      <c r="F22" s="168" t="s">
+      <c r="F22" s="186" t="s">
         <v>713</v>
       </c>
-      <c r="G22" s="166" t="s">
+      <c r="G22" s="184" t="s">
         <v>714</v>
       </c>
-      <c r="H22" s="165"/>
+      <c r="H22" s="183"/>
       <c r="I22" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="163">
+      <c r="J22" s="181">
         <f>J20+J15</f>
         <v>0.68</v>
       </c>
       <c r="K22" s="104"/>
-      <c r="L22" s="144" t="s">
+      <c r="L22" s="165" t="s">
         <v>725</v>
       </c>
       <c r="M22" s="105"/>
@@ -39146,15 +39155,15 @@
       <c r="C23" s="118"/>
       <c r="D23" s="119"/>
       <c r="E23" s="104"/>
-      <c r="F23" s="169"/>
-      <c r="G23" s="167"/>
-      <c r="H23" s="165"/>
+      <c r="F23" s="187"/>
+      <c r="G23" s="185"/>
+      <c r="H23" s="183"/>
       <c r="I23" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="164"/>
+      <c r="J23" s="182"/>
       <c r="K23" s="104"/>
-      <c r="L23" s="145"/>
+      <c r="L23" s="166"/>
       <c r="M23" s="105"/>
     </row>
     <row r="24" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39178,13 +39187,13 @@
       <c r="C25" s="118"/>
       <c r="D25" s="119"/>
       <c r="E25" s="104"/>
-      <c r="F25" s="157" t="s">
+      <c r="F25" s="175" t="s">
         <v>932</v>
       </c>
-      <c r="G25" s="158"/>
-      <c r="H25" s="158"/>
-      <c r="I25" s="158"/>
-      <c r="J25" s="159"/>
+      <c r="G25" s="176"/>
+      <c r="H25" s="176"/>
+      <c r="I25" s="176"/>
+      <c r="J25" s="177"/>
       <c r="K25" s="104"/>
       <c r="L25" s="104"/>
       <c r="M25" s="105"/>
@@ -39195,11 +39204,11 @@
       <c r="C26" s="118"/>
       <c r="D26" s="119"/>
       <c r="E26" s="103"/>
-      <c r="F26" s="160"/>
-      <c r="G26" s="161"/>
-      <c r="H26" s="161"/>
-      <c r="I26" s="161"/>
-      <c r="J26" s="162"/>
+      <c r="F26" s="178"/>
+      <c r="G26" s="179"/>
+      <c r="H26" s="179"/>
+      <c r="I26" s="179"/>
+      <c r="J26" s="180"/>
       <c r="K26" s="104"/>
       <c r="L26" s="104"/>
       <c r="M26" s="105"/>
@@ -39225,13 +39234,13 @@
       <c r="C28" s="118"/>
       <c r="D28" s="119"/>
       <c r="E28" s="103"/>
-      <c r="F28" s="156" t="s">
+      <c r="F28" s="174" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="156"/>
-      <c r="H28" s="156"/>
-      <c r="I28" s="156"/>
-      <c r="J28" s="156"/>
+      <c r="G28" s="174"/>
+      <c r="H28" s="174"/>
+      <c r="I28" s="174"/>
+      <c r="J28" s="174"/>
       <c r="K28" s="104"/>
       <c r="L28" s="104"/>
       <c r="M28" s="105"/>
@@ -39242,13 +39251,13 @@
       <c r="C29" s="118"/>
       <c r="D29" s="119"/>
       <c r="E29" s="103"/>
-      <c r="F29" s="150" t="s">
+      <c r="F29" s="171" t="s">
         <v>933</v>
       </c>
-      <c r="G29" s="151"/>
-      <c r="H29" s="151"/>
-      <c r="I29" s="151"/>
-      <c r="J29" s="152"/>
+      <c r="G29" s="172"/>
+      <c r="H29" s="172"/>
+      <c r="I29" s="172"/>
+      <c r="J29" s="173"/>
       <c r="K29" s="104"/>
       <c r="L29" s="104"/>
       <c r="M29" s="105"/>
@@ -39259,30 +39268,30 @@
       <c r="C30" s="118"/>
       <c r="D30" s="119"/>
       <c r="E30" s="103"/>
-      <c r="F30" s="150"/>
-      <c r="G30" s="151"/>
-      <c r="H30" s="151"/>
-      <c r="I30" s="151"/>
-      <c r="J30" s="152"/>
+      <c r="F30" s="171"/>
+      <c r="G30" s="172"/>
+      <c r="H30" s="172"/>
+      <c r="I30" s="172"/>
+      <c r="J30" s="173"/>
       <c r="K30" s="104"/>
       <c r="L30" s="104"/>
       <c r="M30" s="105"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A31" s="146" t="s">
+      <c r="A31" s="167" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="147"/>
-      <c r="C31" s="148" t="s">
+      <c r="B31" s="168"/>
+      <c r="C31" s="169" t="s">
         <v>950</v>
       </c>
-      <c r="D31" s="149"/>
+      <c r="D31" s="170"/>
       <c r="E31" s="104"/>
-      <c r="F31" s="153"/>
-      <c r="G31" s="154"/>
-      <c r="H31" s="154"/>
-      <c r="I31" s="154"/>
-      <c r="J31" s="155"/>
+      <c r="F31" s="162"/>
+      <c r="G31" s="163"/>
+      <c r="H31" s="163"/>
+      <c r="I31" s="163"/>
+      <c r="J31" s="164"/>
       <c r="K31" s="104"/>
       <c r="L31" s="104"/>
       <c r="M31" s="105"/>
@@ -39305,12 +39314,16 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0"/>
   <mergeCells count="31">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="A2:D3"/>
-    <mergeCell ref="F2:J3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F29:J31"/>
+    <mergeCell ref="F28:J28"/>
+    <mergeCell ref="F25:J26"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F22:F23"/>
     <mergeCell ref="L12:L14"/>
     <mergeCell ref="L18:L19"/>
     <mergeCell ref="A6:D6"/>
@@ -39326,16 +39339,12 @@
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="G18:I18"/>
     <mergeCell ref="G19:I19"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F29:J31"/>
-    <mergeCell ref="F28:J28"/>
-    <mergeCell ref="F25:J26"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A2:D3"/>
+    <mergeCell ref="F2:J3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:J5"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6:D6">
@@ -39403,57 +39412,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="194" t="s">
         <v>556</v>
       </c>
-      <c r="B1" s="200"/>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
-      <c r="E1" s="200"/>
-      <c r="F1" s="200"/>
-      <c r="G1" s="200"/>
-      <c r="H1" s="200"/>
-      <c r="J1" s="210" t="s">
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
+      <c r="F1" s="195"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="195"/>
+      <c r="J1" s="205" t="s">
         <v>482</v>
       </c>
-      <c r="K1" s="211"/>
-      <c r="L1" s="212"/>
+      <c r="K1" s="206"/>
+      <c r="L1" s="207"/>
       <c r="M1" s="79"/>
       <c r="N1" s="24" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A2" s="199"/>
-      <c r="B2" s="200"/>
-      <c r="C2" s="200"/>
-      <c r="D2" s="200"/>
-      <c r="E2" s="200"/>
-      <c r="F2" s="200"/>
-      <c r="G2" s="200"/>
-      <c r="H2" s="200"/>
-      <c r="J2" s="213" t="s">
+      <c r="A2" s="194"/>
+      <c r="B2" s="195"/>
+      <c r="C2" s="195"/>
+      <c r="D2" s="195"/>
+      <c r="E2" s="195"/>
+      <c r="F2" s="195"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="195"/>
+      <c r="J2" s="208" t="s">
         <v>706</v>
       </c>
-      <c r="K2" s="214"/>
-      <c r="L2" s="215"/>
+      <c r="K2" s="209"/>
+      <c r="L2" s="210"/>
       <c r="M2" s="23"/>
       <c r="N2" s="26" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A3" s="199"/>
-      <c r="B3" s="200"/>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200"/>
-      <c r="E3" s="200"/>
-      <c r="F3" s="200"/>
-      <c r="G3" s="200"/>
-      <c r="H3" s="200"/>
-      <c r="J3" s="213"/>
-      <c r="K3" s="214"/>
-      <c r="L3" s="215"/>
+      <c r="A3" s="194"/>
+      <c r="B3" s="195"/>
+      <c r="C3" s="195"/>
+      <c r="D3" s="195"/>
+      <c r="E3" s="195"/>
+      <c r="F3" s="195"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="195"/>
+      <c r="J3" s="208"/>
+      <c r="K3" s="209"/>
+      <c r="L3" s="210"/>
       <c r="M3" s="23"/>
       <c r="N3" s="26" t="s">
         <v>431</v>
@@ -39463,14 +39472,14 @@
       <c r="A4" s="2"/>
       <c r="B4" s="5"/>
       <c r="C4" s="8"/>
-      <c r="D4" s="192"/>
-      <c r="E4" s="192"/>
+      <c r="D4" s="193"/>
+      <c r="E4" s="193"/>
       <c r="F4" s="43"/>
-      <c r="G4" s="192"/>
-      <c r="H4" s="192"/>
-      <c r="J4" s="213"/>
-      <c r="K4" s="214"/>
-      <c r="L4" s="215"/>
+      <c r="G4" s="193"/>
+      <c r="H4" s="193"/>
+      <c r="J4" s="208"/>
+      <c r="K4" s="209"/>
+      <c r="L4" s="210"/>
       <c r="M4" s="34"/>
       <c r="N4" s="26" t="s">
         <v>432</v>
@@ -39478,24 +39487,24 @@
       <c r="O4" s="81"/>
     </row>
     <row r="5" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A5" s="201" t="s">
+      <c r="A5" s="196" t="s">
         <v>425</v>
       </c>
-      <c r="B5" s="202"/>
+      <c r="B5" s="197"/>
       <c r="C5" s="8"/>
-      <c r="D5" s="205" t="s">
+      <c r="D5" s="200" t="s">
         <v>717</v>
       </c>
-      <c r="E5" s="206"/>
-      <c r="F5" s="207"/>
-      <c r="G5" s="208">
+      <c r="E5" s="201"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="203">
         <f>Submission!$E$17</f>
         <v>0</v>
       </c>
-      <c r="H5" s="209"/>
-      <c r="J5" s="213"/>
-      <c r="K5" s="214"/>
-      <c r="L5" s="215"/>
+      <c r="H5" s="204"/>
+      <c r="J5" s="208"/>
+      <c r="K5" s="209"/>
+      <c r="L5" s="210"/>
       <c r="M5" s="34"/>
       <c r="N5" s="26" t="s">
         <v>433</v>
@@ -39503,21 +39512,21 @@
       <c r="O5" s="81"/>
     </row>
     <row r="6" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A6" s="203"/>
-      <c r="B6" s="204"/>
+      <c r="A6" s="198"/>
+      <c r="B6" s="199"/>
       <c r="C6" s="43"/>
-      <c r="D6" s="192" t="s">
+      <c r="D6" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="192"/>
+      <c r="E6" s="193"/>
       <c r="F6" s="43"/>
-      <c r="G6" s="192" t="s">
+      <c r="G6" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="192"/>
-      <c r="J6" s="213"/>
-      <c r="K6" s="214"/>
-      <c r="L6" s="215"/>
+      <c r="H6" s="193"/>
+      <c r="J6" s="208"/>
+      <c r="K6" s="209"/>
+      <c r="L6" s="210"/>
       <c r="M6" s="34"/>
       <c r="N6" s="26" t="s">
         <v>434</v>
@@ -39525,24 +39534,24 @@
       <c r="O6" s="81"/>
     </row>
     <row r="7" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A7" s="195">
+      <c r="A7" s="188">
         <f>'Game Data'!$J$22</f>
         <v>0.68</v>
       </c>
-      <c r="B7" s="196"/>
+      <c r="B7" s="189"/>
       <c r="C7" s="43"/>
-      <c r="D7" s="193" t="s">
+      <c r="D7" s="216" t="s">
         <v>724</v>
       </c>
-      <c r="E7" s="194"/>
+      <c r="E7" s="217"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="193" t="s">
+      <c r="G7" s="216" t="s">
         <v>724</v>
       </c>
-      <c r="H7" s="194"/>
-      <c r="J7" s="213"/>
-      <c r="K7" s="214"/>
-      <c r="L7" s="215"/>
+      <c r="H7" s="217"/>
+      <c r="J7" s="208"/>
+      <c r="K7" s="209"/>
+      <c r="L7" s="210"/>
       <c r="M7" s="33"/>
       <c r="N7" s="26" t="s">
         <v>435</v>
@@ -39550,23 +39559,23 @@
       <c r="O7" s="81"/>
     </row>
     <row r="8" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A8" s="197"/>
-      <c r="B8" s="198"/>
+      <c r="A8" s="190"/>
+      <c r="B8" s="191"/>
       <c r="C8" s="97"/>
-      <c r="D8" s="219">
+      <c r="D8" s="214">
         <f>E17+E26+E35+E44+E53</f>
-        <v>-3.1249999999999986E-2</v>
-      </c>
-      <c r="E8" s="220"/>
+        <v>1.875000000000001E-2</v>
+      </c>
+      <c r="E8" s="215"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="219">
+      <c r="G8" s="214">
         <f>H17+H26+H35+H44+H53</f>
         <v>0</v>
       </c>
-      <c r="H8" s="220"/>
-      <c r="J8" s="216"/>
-      <c r="K8" s="217"/>
-      <c r="L8" s="218"/>
+      <c r="H8" s="215"/>
+      <c r="J8" s="211"/>
+      <c r="K8" s="212"/>
+      <c r="L8" s="213"/>
       <c r="M8" s="80"/>
       <c r="N8" s="25" t="s">
         <v>436</v>
@@ -39577,15 +39586,15 @@
       <c r="A9" s="2"/>
       <c r="B9" s="5"/>
       <c r="C9" s="43"/>
-      <c r="D9" s="192" t="s">
+      <c r="D9" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="192"/>
+      <c r="E9" s="193"/>
       <c r="F9" s="43"/>
-      <c r="G9" s="192" t="s">
+      <c r="G9" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="192"/>
+      <c r="H9" s="193"/>
       <c r="J9" s="82"/>
       <c r="K9" s="82"/>
       <c r="L9" s="82"/>
@@ -39612,11 +39621,11 @@
       <c r="H10" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="191" t="s">
+      <c r="J10" s="192" t="s">
         <v>707</v>
       </c>
-      <c r="K10" s="191"/>
-      <c r="L10" s="191"/>
+      <c r="K10" s="192"/>
+      <c r="L10" s="192"/>
       <c r="O10" s="84"/>
     </row>
     <row r="11" spans="1:15" ht="14.1" customHeight="1">
@@ -39645,11 +39654,11 @@
         <f t="shared" ref="H11:H16" si="1">$B11*G11</f>
         <v>0</v>
       </c>
-      <c r="J11" s="190" t="s">
+      <c r="J11" s="220" t="s">
         <v>792</v>
       </c>
-      <c r="K11" s="190"/>
-      <c r="L11" s="190"/>
+      <c r="K11" s="220"/>
+      <c r="L11" s="220"/>
       <c r="M11" s="82"/>
       <c r="O11" s="84"/>
     </row>
@@ -39664,11 +39673,11 @@
       <c r="C12" s="35"/>
       <c r="D12" s="39">
         <f>TECH!$E$3</f>
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="E12" s="47">
         <f t="shared" si="0"/>
-        <v>-0.03</v>
+        <v>0</v>
       </c>
       <c r="F12" s="43"/>
       <c r="G12" s="39">
@@ -39679,9 +39688,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J12" s="190"/>
-      <c r="K12" s="190"/>
-      <c r="L12" s="190"/>
+      <c r="J12" s="220"/>
+      <c r="K12" s="220"/>
+      <c r="L12" s="220"/>
       <c r="M12" s="82"/>
       <c r="O12" s="84"/>
     </row>
@@ -39696,11 +39705,11 @@
       <c r="C13" s="35"/>
       <c r="D13" s="39">
         <f>TECH!$E$4</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13" s="47">
         <f t="shared" si="0"/>
-        <v>-0.03</v>
+        <v>-0.02</v>
       </c>
       <c r="F13" s="43"/>
       <c r="G13" s="39">
@@ -39711,9 +39720,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="190"/>
-      <c r="K13" s="190"/>
-      <c r="L13" s="190"/>
+      <c r="J13" s="220"/>
+      <c r="K13" s="220"/>
+      <c r="L13" s="220"/>
       <c r="M13" s="82"/>
       <c r="O13" s="84"/>
     </row>
@@ -39728,11 +39737,11 @@
       <c r="C14" s="36"/>
       <c r="D14" s="39">
         <f>TECH!$E$7</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E14" s="47">
         <f t="shared" si="0"/>
-        <v>1.4999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="F14" s="43"/>
       <c r="G14" s="39">
@@ -39779,11 +39788,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J15" s="188">
+      <c r="J15" s="218">
         <f>MAX(0,MIN(1,IF($J17 &lt;= 0.95, ROUND($J17,2), FLOOR((0.95+($J17-0.95)/5),0.01))))</f>
-        <v>0.64</v>
-      </c>
-      <c r="L15" s="188">
+        <v>0.69</v>
+      </c>
+      <c r="L15" s="218">
         <f>MAX(0,MIN(1,IF($L17 &lt;= 0.95, ROUND($L17,2), FLOOR((0.95+($L17-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -39816,8 +39825,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J16" s="189"/>
-      <c r="L16" s="189"/>
+      <c r="J16" s="219"/>
+      <c r="L16" s="219"/>
       <c r="M16" s="82"/>
       <c r="O16" s="84"/>
     </row>
@@ -39830,7 +39839,7 @@
       </c>
       <c r="E17" s="41">
         <f>SUM(E11:E16)</f>
-        <v>-4.1249999999999995E-2</v>
+        <v>8.7500000000000008E-3</v>
       </c>
       <c r="F17" s="43"/>
       <c r="G17" s="22" t="s">
@@ -39842,7 +39851,7 @@
       </c>
       <c r="J17" s="87">
         <f>$A$7+$E17+IF($D$8-$E17 &gt; 0, ($D$8-$E17)/2, $D$8-$E17)+$G$5</f>
-        <v>0.64375000000000004</v>
+        <v>0.69375000000000009</v>
       </c>
       <c r="L17" s="87">
         <f>$A$7+$H17+IF($G$8 &gt; 0, ($G$8-$H17)/2, $G$8-$H17)+$G$5</f>
@@ -39854,15 +39863,15 @@
       <c r="A18" s="2"/>
       <c r="B18" s="5"/>
       <c r="C18" s="43"/>
-      <c r="D18" s="192" t="s">
+      <c r="D18" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="192"/>
+      <c r="E18" s="193"/>
       <c r="F18" s="43"/>
-      <c r="G18" s="192" t="s">
+      <c r="G18" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="192"/>
+      <c r="H18" s="193"/>
       <c r="J18" s="88"/>
       <c r="M18" s="78"/>
     </row>
@@ -39887,11 +39896,11 @@
       <c r="H19" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="191" t="s">
+      <c r="J19" s="192" t="s">
         <v>715</v>
       </c>
-      <c r="K19" s="191"/>
-      <c r="L19" s="191"/>
+      <c r="K19" s="192"/>
+      <c r="L19" s="192"/>
       <c r="M19" s="83"/>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1">
@@ -39920,11 +39929,11 @@
         <f t="shared" ref="H20:H25" si="3">$B20*G20</f>
         <v>0</v>
       </c>
-      <c r="J20" s="190" t="s">
+      <c r="J20" s="220" t="s">
         <v>722</v>
       </c>
-      <c r="K20" s="190"/>
-      <c r="L20" s="190"/>
+      <c r="K20" s="220"/>
+      <c r="L20" s="220"/>
       <c r="M20" s="84"/>
     </row>
     <row r="21" spans="1:13" ht="14.1" customHeight="1">
@@ -39953,9 +39962,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J21" s="190"/>
-      <c r="K21" s="190"/>
-      <c r="L21" s="190"/>
+      <c r="J21" s="220"/>
+      <c r="K21" s="220"/>
+      <c r="L21" s="220"/>
       <c r="M21" s="84"/>
     </row>
     <row r="22" spans="1:13" ht="14.1" customHeight="1">
@@ -39984,9 +39993,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J22" s="190"/>
-      <c r="K22" s="190"/>
-      <c r="L22" s="190"/>
+      <c r="J22" s="220"/>
+      <c r="K22" s="220"/>
+      <c r="L22" s="220"/>
       <c r="M22" s="84"/>
     </row>
     <row r="23" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40050,11 +40059,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J24" s="188">
+      <c r="J24" s="218">
         <f>MAX(0,MIN(1,IF($J26 &lt;= 0.95, ROUND($J26,2), FLOOR((0.95+($J26-0.95)/5),0.01))))</f>
         <v>0.65</v>
       </c>
-      <c r="L24" s="188">
+      <c r="L24" s="218">
         <f>MAX(0,MIN(1,IF($L26 &lt;= 0.95, ROUND($L26,2), FLOOR((0.95+($L26-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40086,8 +40095,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J25" s="189"/>
-      <c r="L25" s="189"/>
+      <c r="J25" s="219"/>
+      <c r="L25" s="219"/>
       <c r="M25" s="84"/>
     </row>
     <row r="26" spans="1:13" ht="14.1" customHeight="1">
@@ -40123,15 +40132,15 @@
       <c r="A27" s="2"/>
       <c r="B27" s="5"/>
       <c r="C27" s="43"/>
-      <c r="D27" s="192" t="s">
+      <c r="D27" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="192"/>
+      <c r="E27" s="193"/>
       <c r="F27" s="43"/>
-      <c r="G27" s="192" t="s">
+      <c r="G27" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H27" s="192"/>
+      <c r="H27" s="193"/>
     </row>
     <row r="28" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
       <c r="A28" s="1" t="s">
@@ -40154,11 +40163,11 @@
       <c r="H28" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J28" s="191" t="s">
+      <c r="J28" s="192" t="s">
         <v>709</v>
       </c>
-      <c r="K28" s="191"/>
-      <c r="L28" s="191"/>
+      <c r="K28" s="192"/>
+      <c r="L28" s="192"/>
     </row>
     <row r="29" spans="1:13" ht="14.1" customHeight="1">
       <c r="A29" s="57" t="str">
@@ -40186,11 +40195,11 @@
         <f t="shared" ref="H29:H34" si="5">$B29*G29</f>
         <v>0</v>
       </c>
-      <c r="J29" s="190" t="s">
+      <c r="J29" s="220" t="s">
         <v>710</v>
       </c>
-      <c r="K29" s="190"/>
-      <c r="L29" s="190"/>
+      <c r="K29" s="220"/>
+      <c r="L29" s="220"/>
     </row>
     <row r="30" spans="1:13" ht="14.1" customHeight="1">
       <c r="A30" s="58" t="str">
@@ -40218,9 +40227,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J30" s="190"/>
-      <c r="K30" s="190"/>
-      <c r="L30" s="190"/>
+      <c r="J30" s="220"/>
+      <c r="K30" s="220"/>
+      <c r="L30" s="220"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1">
       <c r="A31" s="58" t="str">
@@ -40248,9 +40257,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J31" s="190"/>
-      <c r="K31" s="190"/>
-      <c r="L31" s="190"/>
+      <c r="J31" s="220"/>
+      <c r="K31" s="220"/>
+      <c r="L31" s="220"/>
     </row>
     <row r="32" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
       <c r="A32" s="58" t="str">
@@ -40312,11 +40321,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J33" s="188">
+      <c r="J33" s="218">
         <f>MAX(0,MIN(1,IF($J35 &lt;= 0.95, ROUND($J35,2), FLOOR((0.95+($J35-0.95)/5),0.01))))</f>
-        <v>0.65</v>
-      </c>
-      <c r="L33" s="188">
+        <v>0.7</v>
+      </c>
+      <c r="L33" s="218">
         <f>MAX(0,MIN(1,IF($L35 &lt;= 0.95, ROUND($L35,2), FLOOR((0.95+($L35-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40347,8 +40356,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J34" s="189"/>
-      <c r="L34" s="189"/>
+      <c r="J34" s="219"/>
+      <c r="L34" s="219"/>
     </row>
     <row r="35" spans="1:12" ht="14.1" customHeight="1">
       <c r="A35" s="2"/>
@@ -40371,7 +40380,7 @@
       </c>
       <c r="J35" s="87">
         <f>$A$7+MIN(MAX($E35*2,$E35),$D$8)</f>
-        <v>0.64875000000000005</v>
+        <v>0.69875000000000009</v>
       </c>
       <c r="L35" s="87">
         <f>$A$7+MIN(MAX($H35*2,$H35),$G$8)+$G$5</f>
@@ -40382,15 +40391,15 @@
       <c r="A36" s="2"/>
       <c r="B36" s="5"/>
       <c r="C36" s="43"/>
-      <c r="D36" s="192" t="s">
+      <c r="D36" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="192"/>
+      <c r="E36" s="193"/>
       <c r="F36" s="43"/>
-      <c r="G36" s="192" t="s">
+      <c r="G36" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H36" s="192"/>
+      <c r="H36" s="193"/>
     </row>
     <row r="37" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A37" s="1" t="s">
@@ -40413,11 +40422,11 @@
       <c r="H37" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J37" s="191" t="s">
+      <c r="J37" s="192" t="s">
         <v>711</v>
       </c>
-      <c r="K37" s="191"/>
-      <c r="L37" s="191"/>
+      <c r="K37" s="192"/>
+      <c r="L37" s="192"/>
     </row>
     <row r="38" spans="1:12" ht="14.1" customHeight="1">
       <c r="A38" s="57" t="str">
@@ -40445,11 +40454,11 @@
         <f t="shared" ref="H38:H43" si="7">$B38*G38</f>
         <v>0</v>
       </c>
-      <c r="J38" s="190" t="s">
+      <c r="J38" s="220" t="s">
         <v>712</v>
       </c>
-      <c r="K38" s="190"/>
-      <c r="L38" s="190"/>
+      <c r="K38" s="220"/>
+      <c r="L38" s="220"/>
     </row>
     <row r="39" spans="1:12" ht="14.1" customHeight="1">
       <c r="A39" s="58" t="str">
@@ -40477,9 +40486,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J39" s="190"/>
-      <c r="K39" s="190"/>
-      <c r="L39" s="190"/>
+      <c r="J39" s="220"/>
+      <c r="K39" s="220"/>
+      <c r="L39" s="220"/>
     </row>
     <row r="40" spans="1:12" ht="14.1" customHeight="1">
       <c r="A40" s="58" t="str">
@@ -40507,9 +40516,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J40" s="190"/>
-      <c r="K40" s="190"/>
-      <c r="L40" s="190"/>
+      <c r="J40" s="220"/>
+      <c r="K40" s="220"/>
+      <c r="L40" s="220"/>
     </row>
     <row r="41" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A41" s="58" t="str">
@@ -40571,11 +40580,11 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J42" s="188">
+      <c r="J42" s="218">
         <f>MAX(0,MIN(1,IF($J44 &lt;= 0.95, ROUND($J44,2), FLOOR((0.95+($J44-0.95)/5),0.01))))</f>
         <v>0.63</v>
       </c>
-      <c r="L42" s="188">
+      <c r="L42" s="218">
         <f>MAX(0,MIN(1,IF($L44 &lt;= 0.95, ROUND($L44,2), FLOOR((0.95+($L44-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40606,8 +40615,8 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J43" s="189"/>
-      <c r="L43" s="189"/>
+      <c r="J43" s="219"/>
+      <c r="L43" s="219"/>
     </row>
     <row r="44" spans="1:12" ht="14.1" customHeight="1">
       <c r="A44" s="2"/>
@@ -40641,15 +40650,15 @@
       <c r="A45" s="2"/>
       <c r="B45" s="5"/>
       <c r="C45" s="43"/>
-      <c r="D45" s="192" t="s">
+      <c r="D45" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="192"/>
+      <c r="E45" s="193"/>
       <c r="F45" s="43"/>
-      <c r="G45" s="192" t="s">
+      <c r="G45" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="192"/>
+      <c r="H45" s="193"/>
     </row>
     <row r="46" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A46" s="1" t="s">
@@ -40857,6 +40866,34 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="J29:L31"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="L33:L34"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="J38:L40"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="J11:L13"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J20:L22"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G36:H36"/>
     <mergeCell ref="A7:B8"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="D6:E6"/>
@@ -40870,34 +40907,6 @@
     <mergeCell ref="J2:L8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="J11:L13"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J20:L22"/>
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="L42:L43"/>
-    <mergeCell ref="J29:L31"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="L33:L34"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="J38:L40"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -40925,59 +40934,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="235" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="233"/>
-      <c r="C1" s="233"/>
-      <c r="D1" s="233"/>
-      <c r="E1" s="233"/>
-      <c r="F1" s="233"/>
-      <c r="G1" s="234"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="237"/>
     </row>
     <row r="2" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A2" s="221" t="s">
+      <c r="A2" s="230" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="222"/>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
-      <c r="G2" s="223"/>
+      <c r="B2" s="231"/>
+      <c r="C2" s="231"/>
+      <c r="D2" s="231"/>
+      <c r="E2" s="231"/>
+      <c r="F2" s="231"/>
+      <c r="G2" s="232"/>
     </row>
     <row r="3" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A3" s="238" t="s">
+      <c r="A3" s="227" t="s">
         <v>930</v>
       </c>
-      <c r="B3" s="239"/>
-      <c r="C3" s="239"/>
-      <c r="D3" s="239"/>
-      <c r="E3" s="239"/>
-      <c r="F3" s="239"/>
-      <c r="G3" s="240"/>
+      <c r="B3" s="228"/>
+      <c r="C3" s="228"/>
+      <c r="D3" s="228"/>
+      <c r="E3" s="228"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="229"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A4" s="221" t="s">
+      <c r="A4" s="230" t="s">
         <v>438</v>
       </c>
-      <c r="B4" s="222"/>
-      <c r="C4" s="222"/>
-      <c r="D4" s="222"/>
-      <c r="E4" s="222"/>
-      <c r="F4" s="222"/>
-      <c r="G4" s="223"/>
+      <c r="B4" s="231"/>
+      <c r="C4" s="231"/>
+      <c r="D4" s="231"/>
+      <c r="E4" s="231"/>
+      <c r="F4" s="231"/>
+      <c r="G4" s="232"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A5" s="249" t="s">
+      <c r="A5" s="238" t="s">
         <v>580</v>
       </c>
-      <c r="B5" s="250"/>
-      <c r="C5" s="250"/>
-      <c r="D5" s="250"/>
-      <c r="E5" s="250"/>
-      <c r="F5" s="250"/>
-      <c r="G5" s="251"/>
+      <c r="B5" s="239"/>
+      <c r="C5" s="239"/>
+      <c r="D5" s="239"/>
+      <c r="E5" s="239"/>
+      <c r="F5" s="239"/>
+      <c r="G5" s="240"/>
     </row>
     <row r="6" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
       <c r="A6" s="2"/>
@@ -41010,10 +41019,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75">
-      <c r="A8" s="247" t="s">
+      <c r="A8" s="233" t="s">
         <v>718</v>
       </c>
-      <c r="B8" s="248"/>
+      <c r="B8" s="234"/>
       <c r="C8" s="65">
         <v>0</v>
       </c>
@@ -41030,10 +41039,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75">
-      <c r="A9" s="253" t="s">
+      <c r="A9" s="242" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="254"/>
+      <c r="B9" s="243"/>
       <c r="C9" s="92">
         <v>0</v>
       </c>
@@ -41050,10 +41059,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75">
-      <c r="A10" s="255" t="s">
+      <c r="A10" s="244" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="256"/>
+      <c r="B10" s="245"/>
       <c r="C10" s="69">
         <v>0</v>
       </c>
@@ -41070,10 +41079,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75">
-      <c r="A11" s="256" t="s">
+      <c r="A11" s="245" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="256"/>
+      <c r="B11" s="245"/>
       <c r="C11" s="69">
         <v>0</v>
       </c>
@@ -41090,10 +41099,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75">
-      <c r="A12" s="256" t="s">
+      <c r="A12" s="245" t="s">
         <v>716</v>
       </c>
-      <c r="B12" s="256"/>
+      <c r="B12" s="245"/>
       <c r="C12" s="69">
         <v>0</v>
       </c>
@@ -41110,10 +41119,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75">
-      <c r="A13" s="256" t="s">
+      <c r="A13" s="245" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="256"/>
+      <c r="B13" s="245"/>
       <c r="C13" s="69">
         <v>0</v>
       </c>
@@ -41130,10 +41139,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75">
-      <c r="A14" s="255" t="s">
+      <c r="A14" s="244" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="256"/>
+      <c r="B14" s="245"/>
       <c r="C14" s="69">
         <v>0</v>
       </c>
@@ -41150,10 +41159,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75">
-      <c r="A15" s="255" t="s">
+      <c r="A15" s="244" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="256"/>
+      <c r="B15" s="245"/>
       <c r="C15" s="69">
         <v>0</v>
       </c>
@@ -41170,10 +41179,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A16" s="230" t="s">
+      <c r="A16" s="246" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="231"/>
+      <c r="B16" s="247"/>
       <c r="C16" s="73">
         <v>0</v>
       </c>
@@ -41191,11 +41200,11 @@
     </row>
     <row r="17" spans="1:7" ht="14.1" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="252" t="s">
+      <c r="B17" s="241" t="s">
         <v>721</v>
       </c>
-      <c r="C17" s="252"/>
-      <c r="D17" s="252"/>
+      <c r="C17" s="241"/>
+      <c r="D17" s="241"/>
       <c r="E17" s="63">
         <f>SUM(E9:E16)</f>
         <v>0</v>
@@ -41216,527 +41225,559 @@
       <c r="A19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="232" t="s">
+      <c r="B19" s="235" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="233"/>
-      <c r="D19" s="233"/>
-      <c r="E19" s="233"/>
-      <c r="F19" s="233"/>
-      <c r="G19" s="234"/>
+      <c r="C19" s="236"/>
+      <c r="D19" s="236"/>
+      <c r="E19" s="236"/>
+      <c r="F19" s="236"/>
+      <c r="G19" s="237"/>
     </row>
     <row r="20" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="A20" s="10" t="s">
         <v>582</v>
       </c>
-      <c r="B20" s="221" t="s">
+      <c r="B20" s="230" t="s">
         <v>931</v>
       </c>
-      <c r="C20" s="222"/>
-      <c r="D20" s="222"/>
-      <c r="E20" s="222"/>
-      <c r="F20" s="222"/>
-      <c r="G20" s="223"/>
+      <c r="C20" s="231"/>
+      <c r="D20" s="231"/>
+      <c r="E20" s="231"/>
+      <c r="F20" s="231"/>
+      <c r="G20" s="232"/>
     </row>
     <row r="21" spans="1:7" ht="60" customHeight="1" thickBot="1">
       <c r="A21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="221" t="s">
+      <c r="B21" s="230" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="222"/>
-      <c r="D21" s="222"/>
-      <c r="E21" s="222"/>
-      <c r="F21" s="222"/>
-      <c r="G21" s="223"/>
+      <c r="C21" s="231"/>
+      <c r="D21" s="231"/>
+      <c r="E21" s="231"/>
+      <c r="F21" s="231"/>
+      <c r="G21" s="232"/>
     </row>
     <row r="22" spans="1:7" ht="45.95" customHeight="1" thickBot="1">
       <c r="A22" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="221" t="s">
+      <c r="B22" s="230" t="s">
         <v>917</v>
       </c>
-      <c r="C22" s="222"/>
-      <c r="D22" s="222"/>
-      <c r="E22" s="222"/>
-      <c r="F22" s="222"/>
-      <c r="G22" s="223"/>
+      <c r="C22" s="231"/>
+      <c r="D22" s="231"/>
+      <c r="E22" s="231"/>
+      <c r="F22" s="231"/>
+      <c r="G22" s="232"/>
     </row>
     <row r="23" spans="1:7" ht="32.1" customHeight="1">
       <c r="A23" s="98" t="s">
         <v>899</v>
       </c>
-      <c r="B23" s="238" t="s">
+      <c r="B23" s="227" t="s">
         <v>916</v>
       </c>
-      <c r="C23" s="239"/>
-      <c r="D23" s="239"/>
-      <c r="E23" s="239"/>
-      <c r="F23" s="239"/>
-      <c r="G23" s="240"/>
+      <c r="C23" s="228"/>
+      <c r="D23" s="228"/>
+      <c r="E23" s="228"/>
+      <c r="F23" s="228"/>
+      <c r="G23" s="229"/>
     </row>
     <row r="24" spans="1:7" ht="15.75">
       <c r="A24" s="99"/>
-      <c r="B24" s="257" t="s">
+      <c r="B24" s="221" t="s">
         <v>900</v>
       </c>
-      <c r="C24" s="258"/>
-      <c r="D24" s="260" t="s">
+      <c r="C24" s="222"/>
+      <c r="D24" s="223" t="s">
         <v>901</v>
       </c>
-      <c r="E24" s="260"/>
-      <c r="F24" s="260"/>
-      <c r="G24" s="261"/>
+      <c r="E24" s="223"/>
+      <c r="F24" s="223"/>
+      <c r="G24" s="224"/>
     </row>
     <row r="25" spans="1:7" ht="15.75">
       <c r="A25" s="99"/>
-      <c r="B25" s="257" t="s">
+      <c r="B25" s="221" t="s">
         <v>902</v>
       </c>
-      <c r="C25" s="258"/>
-      <c r="D25" s="260" t="s">
+      <c r="C25" s="222"/>
+      <c r="D25" s="223" t="s">
         <v>903</v>
       </c>
-      <c r="E25" s="260"/>
-      <c r="F25" s="260"/>
-      <c r="G25" s="261"/>
+      <c r="E25" s="223"/>
+      <c r="F25" s="223"/>
+      <c r="G25" s="224"/>
     </row>
     <row r="26" spans="1:7" ht="15.75">
       <c r="A26" s="99"/>
-      <c r="B26" s="257" t="s">
+      <c r="B26" s="221" t="s">
         <v>904</v>
       </c>
-      <c r="C26" s="258"/>
-      <c r="D26" s="260" t="s">
+      <c r="C26" s="222"/>
+      <c r="D26" s="223" t="s">
         <v>905</v>
       </c>
-      <c r="E26" s="260"/>
-      <c r="F26" s="260"/>
-      <c r="G26" s="261"/>
+      <c r="E26" s="223"/>
+      <c r="F26" s="223"/>
+      <c r="G26" s="224"/>
     </row>
     <row r="27" spans="1:7" ht="15.75">
       <c r="A27" s="99"/>
-      <c r="B27" s="257" t="s">
+      <c r="B27" s="221" t="s">
         <v>906</v>
       </c>
-      <c r="C27" s="258"/>
+      <c r="C27" s="222"/>
       <c r="D27" s="225" t="s">
         <v>907</v>
       </c>
       <c r="E27" s="225"/>
       <c r="F27" s="225"/>
-      <c r="G27" s="259"/>
+      <c r="G27" s="226"/>
     </row>
     <row r="28" spans="1:7" ht="15.75">
       <c r="A28" s="99"/>
-      <c r="B28" s="257" t="s">
+      <c r="B28" s="221" t="s">
         <v>908</v>
       </c>
-      <c r="C28" s="258"/>
-      <c r="D28" s="260" t="s">
+      <c r="C28" s="222"/>
+      <c r="D28" s="223" t="s">
         <v>909</v>
       </c>
-      <c r="E28" s="260"/>
-      <c r="F28" s="260"/>
-      <c r="G28" s="261"/>
+      <c r="E28" s="223"/>
+      <c r="F28" s="223"/>
+      <c r="G28" s="224"/>
     </row>
     <row r="29" spans="1:7" ht="15.75">
       <c r="A29" s="99"/>
-      <c r="B29" s="257" t="s">
+      <c r="B29" s="221" t="s">
         <v>910</v>
       </c>
-      <c r="C29" s="258"/>
+      <c r="C29" s="222"/>
       <c r="D29" s="225" t="s">
         <v>911</v>
       </c>
       <c r="E29" s="225"/>
       <c r="F29" s="225"/>
-      <c r="G29" s="259"/>
+      <c r="G29" s="226"/>
     </row>
     <row r="30" spans="1:7" ht="15.75">
       <c r="A30" s="99"/>
-      <c r="B30" s="257" t="s">
+      <c r="B30" s="221" t="s">
         <v>914</v>
       </c>
-      <c r="C30" s="258"/>
-      <c r="D30" s="260" t="s">
+      <c r="C30" s="222"/>
+      <c r="D30" s="223" t="s">
         <v>915</v>
       </c>
-      <c r="E30" s="260"/>
-      <c r="F30" s="260"/>
-      <c r="G30" s="261"/>
+      <c r="E30" s="223"/>
+      <c r="F30" s="223"/>
+      <c r="G30" s="224"/>
     </row>
     <row r="31" spans="1:7" ht="15.75">
       <c r="A31" s="99"/>
-      <c r="B31" s="257" t="s">
+      <c r="B31" s="221" t="s">
         <v>912</v>
       </c>
-      <c r="C31" s="258"/>
+      <c r="C31" s="222"/>
       <c r="D31" s="225" t="s">
         <v>913</v>
       </c>
       <c r="E31" s="225"/>
       <c r="F31" s="225"/>
-      <c r="G31" s="259"/>
+      <c r="G31" s="226"/>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickBot="1">
       <c r="A32" s="99"/>
-      <c r="B32" s="257" t="s">
+      <c r="B32" s="221" t="s">
         <v>928</v>
       </c>
-      <c r="C32" s="258"/>
+      <c r="C32" s="222"/>
       <c r="D32" s="225" t="s">
         <v>929</v>
       </c>
       <c r="E32" s="225"/>
       <c r="F32" s="225"/>
-      <c r="G32" s="259"/>
+      <c r="G32" s="226"/>
     </row>
     <row r="33" spans="1:7" ht="15.75">
       <c r="A33" s="98" t="s">
         <v>918</v>
       </c>
-      <c r="B33" s="238" t="s">
+      <c r="B33" s="227" t="s">
         <v>919</v>
       </c>
-      <c r="C33" s="239"/>
-      <c r="D33" s="239"/>
-      <c r="E33" s="239"/>
-      <c r="F33" s="239"/>
-      <c r="G33" s="240"/>
+      <c r="C33" s="228"/>
+      <c r="D33" s="228"/>
+      <c r="E33" s="228"/>
+      <c r="F33" s="228"/>
+      <c r="G33" s="229"/>
     </row>
     <row r="34" spans="1:7" ht="15.75">
       <c r="A34" s="99"/>
-      <c r="B34" s="257" t="s">
+      <c r="B34" s="221" t="s">
         <v>920</v>
       </c>
-      <c r="C34" s="258"/>
-      <c r="D34" s="260" t="s">
+      <c r="C34" s="222"/>
+      <c r="D34" s="223" t="s">
         <v>925</v>
       </c>
-      <c r="E34" s="260"/>
-      <c r="F34" s="260"/>
-      <c r="G34" s="261"/>
+      <c r="E34" s="223"/>
+      <c r="F34" s="223"/>
+      <c r="G34" s="224"/>
     </row>
     <row r="35" spans="1:7" ht="15.75">
       <c r="A35" s="99"/>
-      <c r="B35" s="257" t="s">
+      <c r="B35" s="221" t="s">
         <v>921</v>
       </c>
-      <c r="C35" s="258"/>
-      <c r="D35" s="260" t="s">
+      <c r="C35" s="222"/>
+      <c r="D35" s="223" t="s">
         <v>926</v>
       </c>
-      <c r="E35" s="260"/>
-      <c r="F35" s="260"/>
-      <c r="G35" s="261"/>
+      <c r="E35" s="223"/>
+      <c r="F35" s="223"/>
+      <c r="G35" s="224"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" thickBot="1">
       <c r="A36" s="99"/>
-      <c r="B36" s="257" t="s">
+      <c r="B36" s="221" t="s">
         <v>922</v>
       </c>
-      <c r="C36" s="258"/>
-      <c r="D36" s="260" t="s">
+      <c r="C36" s="222"/>
+      <c r="D36" s="223" t="s">
         <v>927</v>
       </c>
-      <c r="E36" s="260"/>
-      <c r="F36" s="260"/>
-      <c r="G36" s="261"/>
+      <c r="E36" s="223"/>
+      <c r="F36" s="223"/>
+      <c r="G36" s="224"/>
     </row>
     <row r="37" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="A37" s="98" t="s">
         <v>923</v>
       </c>
-      <c r="B37" s="238" t="s">
+      <c r="B37" s="227" t="s">
         <v>924</v>
       </c>
-      <c r="C37" s="239"/>
-      <c r="D37" s="239"/>
-      <c r="E37" s="239"/>
-      <c r="F37" s="239"/>
-      <c r="G37" s="240"/>
+      <c r="C37" s="228"/>
+      <c r="D37" s="228"/>
+      <c r="E37" s="228"/>
+      <c r="F37" s="228"/>
+      <c r="G37" s="229"/>
     </row>
     <row r="38" spans="1:7" ht="29.1" customHeight="1">
-      <c r="A38" s="235" t="s">
+      <c r="A38" s="248" t="s">
         <v>517</v>
       </c>
-      <c r="B38" s="238" t="s">
+      <c r="B38" s="227" t="s">
         <v>490</v>
       </c>
-      <c r="C38" s="239"/>
-      <c r="D38" s="239"/>
-      <c r="E38" s="239"/>
-      <c r="F38" s="239"/>
-      <c r="G38" s="240"/>
+      <c r="C38" s="228"/>
+      <c r="D38" s="228"/>
+      <c r="E38" s="228"/>
+      <c r="F38" s="228"/>
+      <c r="G38" s="229"/>
     </row>
     <row r="39" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A39" s="236"/>
-      <c r="B39" s="241"/>
-      <c r="C39" s="242"/>
-      <c r="D39" s="242"/>
-      <c r="E39" s="242"/>
-      <c r="F39" s="242"/>
-      <c r="G39" s="243"/>
+      <c r="A39" s="249"/>
+      <c r="B39" s="251"/>
+      <c r="C39" s="252"/>
+      <c r="D39" s="252"/>
+      <c r="E39" s="252"/>
+      <c r="F39" s="252"/>
+      <c r="G39" s="253"/>
     </row>
     <row r="40" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A40" s="236"/>
-      <c r="B40" s="244" t="s">
+      <c r="A40" s="249"/>
+      <c r="B40" s="254" t="s">
         <v>491</v>
       </c>
-      <c r="C40" s="245"/>
-      <c r="D40" s="245"/>
-      <c r="E40" s="245"/>
-      <c r="F40" s="245"/>
-      <c r="G40" s="246"/>
+      <c r="C40" s="255"/>
+      <c r="D40" s="255"/>
+      <c r="E40" s="255"/>
+      <c r="F40" s="255"/>
+      <c r="G40" s="256"/>
     </row>
     <row r="41" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A41" s="236"/>
-      <c r="B41" s="224" t="s">
+      <c r="A41" s="249"/>
+      <c r="B41" s="257" t="s">
         <v>492</v>
       </c>
       <c r="C41" s="225"/>
       <c r="D41" s="225"/>
       <c r="E41" s="225"/>
       <c r="F41" s="225"/>
-      <c r="G41" s="226"/>
+      <c r="G41" s="258"/>
     </row>
     <row r="42" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A42" s="236"/>
-      <c r="B42" s="241"/>
-      <c r="C42" s="242"/>
-      <c r="D42" s="242"/>
-      <c r="E42" s="242"/>
-      <c r="F42" s="242"/>
-      <c r="G42" s="243"/>
+      <c r="A42" s="249"/>
+      <c r="B42" s="251"/>
+      <c r="C42" s="252"/>
+      <c r="D42" s="252"/>
+      <c r="E42" s="252"/>
+      <c r="F42" s="252"/>
+      <c r="G42" s="253"/>
     </row>
     <row r="43" spans="1:7" ht="42.95" customHeight="1">
-      <c r="A43" s="236"/>
-      <c r="B43" s="224" t="s">
+      <c r="A43" s="249"/>
+      <c r="B43" s="257" t="s">
         <v>493</v>
       </c>
       <c r="C43" s="225"/>
       <c r="D43" s="225"/>
       <c r="E43" s="225"/>
       <c r="F43" s="225"/>
-      <c r="G43" s="226"/>
+      <c r="G43" s="258"/>
     </row>
     <row r="44" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A44" s="236"/>
-      <c r="B44" s="241"/>
-      <c r="C44" s="242"/>
-      <c r="D44" s="242"/>
-      <c r="E44" s="242"/>
-      <c r="F44" s="242"/>
-      <c r="G44" s="243"/>
+      <c r="A44" s="249"/>
+      <c r="B44" s="251"/>
+      <c r="C44" s="252"/>
+      <c r="D44" s="252"/>
+      <c r="E44" s="252"/>
+      <c r="F44" s="252"/>
+      <c r="G44" s="253"/>
     </row>
     <row r="45" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A45" s="236"/>
-      <c r="B45" s="224" t="s">
+      <c r="A45" s="249"/>
+      <c r="B45" s="257" t="s">
         <v>494</v>
       </c>
       <c r="C45" s="225"/>
       <c r="D45" s="225"/>
       <c r="E45" s="225"/>
       <c r="F45" s="225"/>
-      <c r="G45" s="226"/>
+      <c r="G45" s="258"/>
     </row>
     <row r="46" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A46" s="236"/>
-      <c r="B46" s="224" t="s">
+      <c r="A46" s="249"/>
+      <c r="B46" s="257" t="s">
         <v>495</v>
       </c>
       <c r="C46" s="225"/>
       <c r="D46" s="225"/>
       <c r="E46" s="225"/>
       <c r="F46" s="225"/>
-      <c r="G46" s="226"/>
+      <c r="G46" s="258"/>
     </row>
     <row r="47" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A47" s="236"/>
-      <c r="B47" s="224" t="s">
+      <c r="A47" s="249"/>
+      <c r="B47" s="257" t="s">
         <v>496</v>
       </c>
       <c r="C47" s="225"/>
       <c r="D47" s="225"/>
       <c r="E47" s="225"/>
       <c r="F47" s="225"/>
-      <c r="G47" s="226"/>
+      <c r="G47" s="258"/>
     </row>
     <row r="48" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A48" s="236"/>
-      <c r="B48" s="224" t="s">
+      <c r="A48" s="249"/>
+      <c r="B48" s="257" t="s">
         <v>497</v>
       </c>
       <c r="C48" s="225"/>
       <c r="D48" s="225"/>
       <c r="E48" s="225"/>
       <c r="F48" s="225"/>
-      <c r="G48" s="226"/>
+      <c r="G48" s="258"/>
     </row>
     <row r="49" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A49" s="236"/>
-      <c r="B49" s="224" t="s">
+      <c r="A49" s="249"/>
+      <c r="B49" s="257" t="s">
         <v>498</v>
       </c>
       <c r="C49" s="225"/>
       <c r="D49" s="225"/>
       <c r="E49" s="225"/>
       <c r="F49" s="225"/>
-      <c r="G49" s="226"/>
+      <c r="G49" s="258"/>
     </row>
     <row r="50" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A50" s="236"/>
-      <c r="B50" s="224" t="s">
+      <c r="A50" s="249"/>
+      <c r="B50" s="257" t="s">
         <v>499</v>
       </c>
       <c r="C50" s="225"/>
       <c r="D50" s="225"/>
       <c r="E50" s="225"/>
       <c r="F50" s="225"/>
-      <c r="G50" s="226"/>
+      <c r="G50" s="258"/>
     </row>
     <row r="51" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A51" s="236"/>
-      <c r="B51" s="224" t="s">
+      <c r="A51" s="249"/>
+      <c r="B51" s="257" t="s">
         <v>500</v>
       </c>
       <c r="C51" s="225"/>
       <c r="D51" s="225"/>
       <c r="E51" s="225"/>
       <c r="F51" s="225"/>
-      <c r="G51" s="226"/>
+      <c r="G51" s="258"/>
     </row>
     <row r="52" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A52" s="237"/>
-      <c r="B52" s="227" t="s">
+      <c r="A52" s="250"/>
+      <c r="B52" s="259" t="s">
         <v>501</v>
       </c>
-      <c r="C52" s="228"/>
-      <c r="D52" s="228"/>
-      <c r="E52" s="228"/>
-      <c r="F52" s="228"/>
-      <c r="G52" s="229"/>
+      <c r="C52" s="260"/>
+      <c r="D52" s="260"/>
+      <c r="E52" s="260"/>
+      <c r="F52" s="260"/>
+      <c r="G52" s="261"/>
     </row>
     <row r="53" spans="1:7" ht="57.95" customHeight="1" thickBot="1">
       <c r="A53" s="10" t="s">
         <v>516</v>
       </c>
-      <c r="B53" s="221" t="s">
+      <c r="B53" s="230" t="s">
         <v>581</v>
       </c>
-      <c r="C53" s="222"/>
-      <c r="D53" s="222"/>
-      <c r="E53" s="222"/>
-      <c r="F53" s="222"/>
-      <c r="G53" s="223"/>
+      <c r="C53" s="231"/>
+      <c r="D53" s="231"/>
+      <c r="E53" s="231"/>
+      <c r="F53" s="231"/>
+      <c r="G53" s="232"/>
     </row>
     <row r="54" spans="1:7" ht="57.95" customHeight="1" thickBot="1">
       <c r="A54" s="10" t="s">
         <v>515</v>
       </c>
-      <c r="B54" s="221" t="s">
+      <c r="B54" s="230" t="s">
         <v>502</v>
       </c>
-      <c r="C54" s="222"/>
-      <c r="D54" s="222"/>
-      <c r="E54" s="222"/>
-      <c r="F54" s="222"/>
-      <c r="G54" s="223"/>
+      <c r="C54" s="231"/>
+      <c r="D54" s="231"/>
+      <c r="E54" s="231"/>
+      <c r="F54" s="231"/>
+      <c r="G54" s="232"/>
     </row>
     <row r="55" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A55" s="10" t="s">
         <v>514</v>
       </c>
-      <c r="B55" s="221" t="s">
+      <c r="B55" s="230" t="s">
         <v>503</v>
       </c>
-      <c r="C55" s="222"/>
-      <c r="D55" s="222"/>
-      <c r="E55" s="222"/>
-      <c r="F55" s="222"/>
-      <c r="G55" s="223"/>
+      <c r="C55" s="231"/>
+      <c r="D55" s="231"/>
+      <c r="E55" s="231"/>
+      <c r="F55" s="231"/>
+      <c r="G55" s="232"/>
     </row>
     <row r="56" spans="1:7" ht="42.95" customHeight="1" thickBot="1">
       <c r="A56" s="11" t="s">
         <v>508</v>
       </c>
-      <c r="B56" s="221" t="s">
+      <c r="B56" s="230" t="s">
         <v>504</v>
       </c>
-      <c r="C56" s="222"/>
-      <c r="D56" s="222"/>
-      <c r="E56" s="222"/>
-      <c r="F56" s="222"/>
-      <c r="G56" s="223"/>
+      <c r="C56" s="231"/>
+      <c r="D56" s="231"/>
+      <c r="E56" s="231"/>
+      <c r="F56" s="231"/>
+      <c r="G56" s="232"/>
     </row>
     <row r="57" spans="1:7" ht="29.1" customHeight="1" thickBot="1">
       <c r="A57" s="10" t="s">
         <v>513</v>
       </c>
-      <c r="B57" s="221" t="s">
+      <c r="B57" s="230" t="s">
         <v>505</v>
       </c>
-      <c r="C57" s="222"/>
-      <c r="D57" s="222"/>
-      <c r="E57" s="222"/>
-      <c r="F57" s="222"/>
-      <c r="G57" s="223"/>
+      <c r="C57" s="231"/>
+      <c r="D57" s="231"/>
+      <c r="E57" s="231"/>
+      <c r="F57" s="231"/>
+      <c r="G57" s="232"/>
     </row>
     <row r="58" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A58" s="10" t="s">
         <v>512</v>
       </c>
-      <c r="B58" s="221" t="s">
+      <c r="B58" s="230" t="s">
         <v>506</v>
       </c>
-      <c r="C58" s="222"/>
-      <c r="D58" s="222"/>
-      <c r="E58" s="222"/>
-      <c r="F58" s="222"/>
-      <c r="G58" s="223"/>
+      <c r="C58" s="231"/>
+      <c r="D58" s="231"/>
+      <c r="E58" s="231"/>
+      <c r="F58" s="231"/>
+      <c r="G58" s="232"/>
     </row>
     <row r="59" spans="1:7" ht="42.95" customHeight="1" thickBot="1">
       <c r="A59" s="11" t="s">
         <v>509</v>
       </c>
-      <c r="B59" s="221" t="s">
+      <c r="B59" s="230" t="s">
         <v>510</v>
       </c>
-      <c r="C59" s="222"/>
-      <c r="D59" s="222"/>
-      <c r="E59" s="222"/>
-      <c r="F59" s="222"/>
-      <c r="G59" s="223"/>
+      <c r="C59" s="231"/>
+      <c r="D59" s="231"/>
+      <c r="E59" s="231"/>
+      <c r="F59" s="231"/>
+      <c r="G59" s="232"/>
     </row>
     <row r="60" spans="1:7" ht="29.1" customHeight="1" thickBot="1">
       <c r="A60" s="10" t="s">
         <v>511</v>
       </c>
-      <c r="B60" s="221" t="s">
+      <c r="B60" s="230" t="s">
         <v>507</v>
       </c>
-      <c r="C60" s="222"/>
-      <c r="D60" s="222"/>
-      <c r="E60" s="222"/>
-      <c r="F60" s="222"/>
-      <c r="G60" s="223"/>
+      <c r="C60" s="231"/>
+      <c r="D60" s="231"/>
+      <c r="E60" s="231"/>
+      <c r="F60" s="231"/>
+      <c r="G60" s="232"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="A38:A52"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="B37:G37"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="D29:G29"/>
@@ -41753,49 +41794,17 @@
     <mergeCell ref="D34:G34"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="D35:G35"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="A38:A52"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="B43:G43"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B53:G53"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:G28"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -41806,8 +41815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -41879,7 +41888,7 @@
       <c r="D3" s="265"/>
       <c r="E3" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Basic")*(E$10:E$247="Missing"))+0.5*SUMPRODUCT(($A$10:$A$247="Basic")*(E$10:E$247="Partial"))</f>
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="F3" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Basic")*(F$10:F$247="Missing"))+0.5*SUMPRODUCT(($A$10:$A$247="Basic")*(F$10:F$247="Partial"))</f>
@@ -41901,7 +41910,7 @@
       <c r="D4" s="265"/>
       <c r="E4" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Intermediate")*(E$10:E$247="Missing"))+0.5*SUMPRODUCT(($A$10:$A$247="Intermediate")*(E$10:E$247="Partial"))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Intermediate")*(F$10:F$247="Missing"))+0.5*SUMPRODUCT(($A$10:$A$247="Intermediate")*(F$10:F$247="Partial"))</f>
@@ -41923,7 +41932,7 @@
       <c r="D5" s="265"/>
       <c r="E5" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Intermediate")*(E$10:E$247="Completed"))+SUMPRODUCT(($A$10:$A$247="Intermediate")*(E$10:E$247="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$247="Intermediate")*(E$10:E$247="Partial"))</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F5" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Intermediate")*(F$10:F$247="Completed"))+SUMPRODUCT(($A$10:$A$247="Intermediate")*(F$10:F$247="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$247="Intermediate")*(F$10:F$247="Partial"))</f>
@@ -41945,7 +41954,7 @@
       <c r="D6" s="265"/>
       <c r="E6" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Advanced")*(E$10:E$247="Missing"))+0.5*SUMPRODUCT(($A$10:$A$247="Advanced")*(E$10:E$247="Partial"))</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F6" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Advanced")*(F$10:F$247="Missing"))+0.5*SUMPRODUCT(($A$10:$A$247="Advanced")*(F$10:F$247="Partial"))</f>
@@ -41967,7 +41976,7 @@
       <c r="D7" s="265"/>
       <c r="E7" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Advanced")*(E$10:E$247="Completed"))+SUMPRODUCT(($A$10:$A$247="Advanced")*(E$10:E$247="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$247="Advanced")*(E$10:E$247="Partial"))</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F7" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Advanced")*(F$10:F$247="Completed"))+SUMPRODUCT(($A$10:$A$247="Advanced")*(F$10:F$247="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$247="Advanced")*(F$10:F$247="Partial"))</f>
@@ -42019,10 +42028,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>485</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -42268,10 +42277,10 @@
       <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A23" s="232" t="s">
+      <c r="A23" s="235" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="234"/>
+      <c r="B23" s="237"/>
       <c r="C23" s="4" t="s">
         <v>63</v>
       </c>
@@ -42471,7 +42480,7 @@
       </c>
       <c r="D33" s="11"/>
       <c r="E33" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>52</v>
@@ -42566,7 +42575,7 @@
       </c>
       <c r="D38" s="11"/>
       <c r="E38" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>52</v>
@@ -42574,10 +42583,10 @@
       <c r="G38" s="11"/>
     </row>
     <row r="39" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A39" s="232" t="s">
+      <c r="A39" s="235" t="s">
         <v>524</v>
       </c>
-      <c r="B39" s="234"/>
+      <c r="B39" s="237"/>
       <c r="C39" s="4" t="s">
         <v>63</v>
       </c>
@@ -42690,10 +42699,10 @@
       <c r="G44" s="11"/>
     </row>
     <row r="45" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A45" s="232" t="s">
+      <c r="A45" s="235" t="s">
         <v>529</v>
       </c>
-      <c r="B45" s="234"/>
+      <c r="B45" s="237"/>
       <c r="C45" s="4" t="s">
         <v>63</v>
       </c>
@@ -42760,7 +42769,7 @@
       </c>
       <c r="D48" s="11"/>
       <c r="E48" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>52</v>
@@ -42825,10 +42834,10 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A52" s="232" t="s">
+      <c r="A52" s="235" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="234"/>
+      <c r="B52" s="237"/>
       <c r="C52" s="4" t="s">
         <v>63</v>
       </c>
@@ -42998,10 +43007,10 @@
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A61" s="232" t="s">
+      <c r="A61" s="235" t="s">
         <v>111</v>
       </c>
-      <c r="B61" s="234"/>
+      <c r="B61" s="237"/>
       <c r="C61" s="4" t="s">
         <v>63</v>
       </c>
@@ -43095,10 +43104,10 @@
       <c r="G65" s="11"/>
     </row>
     <row r="66" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A66" s="232" t="s">
+      <c r="A66" s="235" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="234"/>
+      <c r="B66" s="237"/>
       <c r="C66" s="4" t="s">
         <v>63</v>
       </c>
@@ -43316,7 +43325,7 @@
         <v>752</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>58</v>
@@ -43336,9 +43345,11 @@
       <c r="C78" s="11" t="s">
         <v>751</v>
       </c>
-      <c r="D78" s="11"/>
+      <c r="D78" s="11" t="s">
+        <v>965</v>
+      </c>
       <c r="E78" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F78" s="4" t="s">
         <v>52</v>
@@ -43384,10 +43395,10 @@
       <c r="G80" s="11"/>
     </row>
     <row r="81" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A81" s="232" t="s">
+      <c r="A81" s="235" t="s">
         <v>133</v>
       </c>
-      <c r="B81" s="234"/>
+      <c r="B81" s="237"/>
       <c r="C81" s="4" t="s">
         <v>63</v>
       </c>
@@ -43480,7 +43491,7 @@
       </c>
       <c r="G85" s="11"/>
     </row>
-    <row r="86" spans="1:7" ht="39" thickBot="1">
+    <row r="86" spans="1:7" ht="51.75" thickBot="1">
       <c r="A86" s="17" t="s">
         <v>70</v>
       </c>
@@ -43490,9 +43501,11 @@
       <c r="C86" s="11" t="s">
         <v>746</v>
       </c>
-      <c r="D86" s="11"/>
+      <c r="D86" s="11" t="s">
+        <v>963</v>
+      </c>
       <c r="E86" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F86" s="4" t="s">
         <v>52</v>
@@ -43519,10 +43532,10 @@
       <c r="G87" s="11"/>
     </row>
     <row r="88" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A88" s="232" t="s">
+      <c r="A88" s="235" t="s">
         <v>558</v>
       </c>
-      <c r="B88" s="234"/>
+      <c r="B88" s="237"/>
       <c r="C88" s="4" t="s">
         <v>63</v>
       </c>
@@ -43550,7 +43563,7 @@
         <v>743</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>58</v>
@@ -43637,10 +43650,10 @@
       <c r="G93" s="11"/>
     </row>
     <row r="94" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A94" s="232" t="s">
+      <c r="A94" s="235" t="s">
         <v>156</v>
       </c>
-      <c r="B94" s="234"/>
+      <c r="B94" s="237"/>
       <c r="C94" s="4" t="s">
         <v>63</v>
       </c>
@@ -43715,10 +43728,10 @@
       <c r="G97" s="11"/>
     </row>
     <row r="98" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A98" s="232" t="s">
+      <c r="A98" s="235" t="s">
         <v>150</v>
       </c>
-      <c r="B98" s="234"/>
+      <c r="B98" s="237"/>
       <c r="C98" s="4" t="s">
         <v>63</v>
       </c>
@@ -43793,10 +43806,10 @@
       <c r="G101" s="11"/>
     </row>
     <row r="102" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A102" s="232" t="s">
+      <c r="A102" s="235" t="s">
         <v>547</v>
       </c>
-      <c r="B102" s="234"/>
+      <c r="B102" s="237"/>
       <c r="C102" s="4" t="s">
         <v>63</v>
       </c>
@@ -43851,7 +43864,7 @@
       </c>
       <c r="G104" s="11"/>
     </row>
-    <row r="105" spans="1:7" ht="26.25" thickBot="1">
+    <row r="105" spans="1:7" ht="51.75" thickBot="1">
       <c r="A105" s="19" t="s">
         <v>101</v>
       </c>
@@ -43862,7 +43875,7 @@
         <v>737</v>
       </c>
       <c r="D105" s="11" t="s">
-        <v>961</v>
+        <v>964</v>
       </c>
       <c r="E105" s="4" t="s">
         <v>56</v>
@@ -43892,10 +43905,10 @@
       <c r="G106" s="11"/>
     </row>
     <row r="107" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A107" s="232" t="s">
+      <c r="A107" s="235" t="s">
         <v>140</v>
       </c>
-      <c r="B107" s="234"/>
+      <c r="B107" s="237"/>
       <c r="C107" s="4" t="s">
         <v>63</v>
       </c>
@@ -44046,10 +44059,10 @@
       <c r="G114" s="11"/>
     </row>
     <row r="115" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A115" s="232" t="s">
+      <c r="A115" s="235" t="s">
         <v>161</v>
       </c>
-      <c r="B115" s="234"/>
+      <c r="B115" s="237"/>
       <c r="C115" s="4" t="s">
         <v>453</v>
       </c>
@@ -44220,6 +44233,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A88:B88"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="C2:D9"/>
@@ -44229,14 +44250,6 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A88:B88"/>
   </mergeCells>
   <conditionalFormatting sqref="A11:A18 A107:A109 A81:A85 A115:A248 A52:A57 A40 A33:A37 A42:A43 A112 A94:A100 A61:A69 A59 A20:A29">
     <cfRule type="beginsWith" dxfId="2421" priority="1148" stopIfTrue="1" operator="beginsWith" text="Exceptional">
@@ -46685,10 +46698,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>701</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -46972,10 +46985,10 @@
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A25" s="232" t="s">
+      <c r="A25" s="235" t="s">
         <v>688</v>
       </c>
-      <c r="B25" s="234"/>
+      <c r="B25" s="237"/>
       <c r="C25" s="4" t="s">
         <v>63</v>
       </c>
@@ -47183,10 +47196,10 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A36" s="232" t="s">
+      <c r="A36" s="235" t="s">
         <v>612</v>
       </c>
-      <c r="B36" s="234"/>
+      <c r="B36" s="237"/>
       <c r="C36" s="4" t="s">
         <v>63</v>
       </c>
@@ -47605,10 +47618,10 @@
       <c r="G57" s="11"/>
     </row>
     <row r="58" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A58" s="232" t="s">
+      <c r="A58" s="235" t="s">
         <v>627</v>
       </c>
-      <c r="B58" s="234"/>
+      <c r="B58" s="237"/>
       <c r="C58" s="4" t="s">
         <v>63</v>
       </c>
@@ -47911,10 +47924,10 @@
       <c r="G73" s="11"/>
     </row>
     <row r="74" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A74" s="232" t="s">
+      <c r="A74" s="235" t="s">
         <v>651</v>
       </c>
-      <c r="B74" s="234"/>
+      <c r="B74" s="237"/>
       <c r="C74" s="4" t="s">
         <v>63</v>
       </c>
@@ -48103,10 +48116,10 @@
       <c r="G83" s="11"/>
     </row>
     <row r="84" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A84" s="232" t="s">
+      <c r="A84" s="235" t="s">
         <v>663</v>
       </c>
-      <c r="B84" s="234"/>
+      <c r="B84" s="237"/>
       <c r="C84" s="21" t="s">
         <v>456</v>
       </c>
@@ -48466,10 +48479,10 @@
       <c r="G102" s="11"/>
     </row>
     <row r="103" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A103" s="232" t="s">
+      <c r="A103" s="235" t="s">
         <v>677</v>
       </c>
-      <c r="B103" s="234"/>
+      <c r="B103" s="237"/>
       <c r="C103" s="4" t="s">
         <v>63</v>
       </c>
@@ -51637,10 +51650,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>291</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -52000,10 +52013,10 @@
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A29" s="232" t="s">
+      <c r="A29" s="235" t="s">
         <v>564</v>
       </c>
-      <c r="B29" s="234"/>
+      <c r="B29" s="237"/>
       <c r="C29" s="4" t="s">
         <v>451</v>
       </c>
@@ -52232,10 +52245,10 @@
       <c r="G40" s="11"/>
     </row>
     <row r="41" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A41" s="232" t="s">
+      <c r="A41" s="235" t="s">
         <v>334</v>
       </c>
-      <c r="B41" s="234"/>
+      <c r="B41" s="237"/>
       <c r="C41" s="4" t="s">
         <v>63</v>
       </c>
@@ -52447,10 +52460,10 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" s="7" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A52" s="232" t="s">
+      <c r="A52" s="235" t="s">
         <v>84</v>
       </c>
-      <c r="B52" s="234"/>
+      <c r="B52" s="237"/>
       <c r="C52" s="4" t="s">
         <v>63</v>
       </c>
@@ -52620,10 +52633,10 @@
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" s="7" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A61" s="232" t="s">
+      <c r="A61" s="235" t="s">
         <v>370</v>
       </c>
-      <c r="B61" s="234"/>
+      <c r="B61" s="237"/>
       <c r="C61" s="21" t="s">
         <v>452</v>
       </c>
@@ -53973,10 +53986,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>810</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -54279,10 +54292,10 @@
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A26" s="232" t="s">
+      <c r="A26" s="235" t="s">
         <v>390</v>
       </c>
-      <c r="B26" s="234"/>
+      <c r="B26" s="237"/>
       <c r="C26" s="4" t="s">
         <v>855</v>
       </c>
@@ -54547,10 +54560,10 @@
       <c r="G39" s="11"/>
     </row>
     <row r="40" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A40" s="232" t="s">
+      <c r="A40" s="235" t="s">
         <v>448</v>
       </c>
-      <c r="B40" s="234"/>
+      <c r="B40" s="237"/>
       <c r="C40" s="102" t="s">
         <v>856</v>
       </c>
@@ -54815,10 +54828,10 @@
       <c r="G53" s="11"/>
     </row>
     <row r="54" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A54" s="232" t="s">
+      <c r="A54" s="235" t="s">
         <v>412</v>
       </c>
-      <c r="B54" s="234"/>
+      <c r="B54" s="237"/>
       <c r="C54" s="4" t="s">
         <v>63</v>
       </c>
@@ -56677,10 +56690,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>239</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -56774,10 +56787,10 @@
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A15" s="232" t="s">
+      <c r="A15" s="235" t="s">
         <v>246</v>
       </c>
-      <c r="B15" s="234"/>
+      <c r="B15" s="237"/>
       <c r="C15" s="4" t="s">
         <v>874</v>
       </c>
@@ -56890,10 +56903,10 @@
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A21" s="232" t="s">
+      <c r="A21" s="235" t="s">
         <v>878</v>
       </c>
-      <c r="B21" s="234"/>
+      <c r="B21" s="237"/>
       <c r="C21" s="4" t="s">
         <v>63</v>
       </c>
@@ -57025,10 +57038,10 @@
       <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A28" s="232" t="s">
+      <c r="A28" s="235" t="s">
         <v>254</v>
       </c>
-      <c r="B28" s="234"/>
+      <c r="B28" s="237"/>
       <c r="C28" s="4" t="s">
         <v>875</v>
       </c>
@@ -57179,10 +57192,10 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A36" s="232" t="s">
+      <c r="A36" s="235" t="s">
         <v>891</v>
       </c>
-      <c r="B36" s="234"/>
+      <c r="B36" s="237"/>
       <c r="C36" s="4" t="s">
         <v>454</v>
       </c>
@@ -57314,10 +57327,10 @@
       <c r="G42" s="11"/>
     </row>
     <row r="43" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A43" s="232" t="s">
+      <c r="A43" s="235" t="s">
         <v>275</v>
       </c>
-      <c r="B43" s="234"/>
+      <c r="B43" s="237"/>
       <c r="C43" s="4" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Added dynamic teaching, fixed some issues with the restart option and splash screen skipping.
</commit_message>
<xml_diff>
--- a/GameDocuments/gam352_papercut_rubric.xlsx
+++ b/GameDocuments/gam352_papercut_rubric.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Game Data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2305" uniqueCount="966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2310" uniqueCount="971">
   <si>
     <t>GAME NAME</t>
   </si>
@@ -3683,6 +3683,21 @@
   </si>
   <si>
     <t>Unity Launcher</t>
+  </si>
+  <si>
+    <t>Machine explosion</t>
+  </si>
+  <si>
+    <t>No defeate state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No hud elements </t>
+  </si>
+  <si>
+    <t>Take your pick</t>
+  </si>
+  <si>
+    <t>Transformation sequence</t>
   </si>
 </sst>
 </file>
@@ -39387,8 +39402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -39564,7 +39579,7 @@
       <c r="C8" s="97"/>
       <c r="D8" s="214">
         <f>E17+E26+E35+E44+E53</f>
-        <v>1.875000000000001E-2</v>
+        <v>0.13874999999999998</v>
       </c>
       <c r="E8" s="215"/>
       <c r="F8" s="5"/>
@@ -39790,7 +39805,7 @@
       </c>
       <c r="J15" s="218">
         <f>MAX(0,MIN(1,IF($J17 &lt;= 0.95, ROUND($J17,2), FLOOR((0.95+($J17-0.95)/5),0.01))))</f>
-        <v>0.69</v>
+        <v>0.75</v>
       </c>
       <c r="L15" s="218">
         <f>MAX(0,MIN(1,IF($L17 &lt;= 0.95, ROUND($L17,2), FLOOR((0.95+($L17-0.95)/5),0.01))))</f>
@@ -39851,7 +39866,7 @@
       </c>
       <c r="J17" s="87">
         <f>$A$7+$E17+IF($D$8-$E17 &gt; 0, ($D$8-$E17)/2, $D$8-$E17)+$G$5</f>
-        <v>0.69375000000000009</v>
+        <v>0.75375000000000003</v>
       </c>
       <c r="L17" s="87">
         <f>$A$7+$H17+IF($G$8 &gt; 0, ($G$8-$H17)/2, $G$8-$H17)+$G$5</f>
@@ -39947,11 +39962,11 @@
       <c r="C21" s="35"/>
       <c r="D21" s="39">
         <f>DESIGN!$E$3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" s="47">
         <f t="shared" si="2"/>
-        <v>-0.02</v>
+        <v>0</v>
       </c>
       <c r="F21" s="43"/>
       <c r="G21" s="39">
@@ -39978,11 +39993,11 @@
       <c r="C22" s="35"/>
       <c r="D22" s="39">
         <f>DESIGN!$E$4</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E22" s="47">
         <f t="shared" si="2"/>
-        <v>-0.03</v>
+        <v>-0.01</v>
       </c>
       <c r="F22" s="43"/>
       <c r="G22" s="39">
@@ -40009,11 +40024,11 @@
       <c r="C23" s="36"/>
       <c r="D23" s="39">
         <f>DESIGN!$E$7</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="47">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F23" s="43"/>
       <c r="G23" s="39">
@@ -40044,11 +40059,11 @@
       <c r="C24" s="37"/>
       <c r="D24" s="39">
         <f>DESIGN!$E$8</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" s="47">
         <f t="shared" si="2"/>
-        <v>7.4999999999999997E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F24" s="43"/>
       <c r="G24" s="39">
@@ -40061,7 +40076,7 @@
       </c>
       <c r="J24" s="218">
         <f>MAX(0,MIN(1,IF($J26 &lt;= 0.95, ROUND($J26,2), FLOOR((0.95+($J26-0.95)/5),0.01))))</f>
-        <v>0.65</v>
+        <v>0.72</v>
       </c>
       <c r="L24" s="218">
         <f>MAX(0,MIN(1,IF($L26 &lt;= 0.95, ROUND($L26,2), FLOOR((0.95+($L26-0.95)/5),0.01))))</f>
@@ -40108,7 +40123,7 @@
       </c>
       <c r="E26" s="41">
         <f>SUM(E20:E25)</f>
-        <v>-3.2500000000000001E-2</v>
+        <v>1.9999999999999997E-2</v>
       </c>
       <c r="F26" s="43"/>
       <c r="G26" s="22" t="s">
@@ -40120,7 +40135,7 @@
       </c>
       <c r="J26" s="87">
         <f>$A$7+MIN(MAX($E26*2,$E26),$D$8)</f>
-        <v>0.64750000000000008</v>
+        <v>0.72000000000000008</v>
       </c>
       <c r="L26" s="87">
         <f>$A$7+MIN(MAX($H26*2,$H26),$G$8)+$G$5</f>
@@ -40323,7 +40338,7 @@
       </c>
       <c r="J33" s="218">
         <f>MAX(0,MIN(1,IF($J35 &lt;= 0.95, ROUND($J35,2), FLOOR((0.95+($J35-0.95)/5),0.01))))</f>
-        <v>0.7</v>
+        <v>0.82</v>
       </c>
       <c r="L33" s="218">
         <f>MAX(0,MIN(1,IF($L35 &lt;= 0.95, ROUND($L35,2), FLOOR((0.95+($L35-0.95)/5),0.01))))</f>
@@ -40380,7 +40395,7 @@
       </c>
       <c r="J35" s="87">
         <f>$A$7+MIN(MAX($E35*2,$E35),$D$8)</f>
-        <v>0.69875000000000009</v>
+        <v>0.81875000000000009</v>
       </c>
       <c r="L35" s="87">
         <f>$A$7+MIN(MAX($H35*2,$H35),$G$8)+$G$5</f>
@@ -40471,11 +40486,11 @@
       <c r="C39" s="35"/>
       <c r="D39" s="39">
         <f>AUDIO!$E$3</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" s="47">
         <f t="shared" si="6"/>
-        <v>-0.04</v>
+        <v>-0.02</v>
       </c>
       <c r="F39" s="43"/>
       <c r="G39" s="39">
@@ -40501,11 +40516,11 @@
       <c r="C40" s="35"/>
       <c r="D40" s="39">
         <f>AUDIO!$E$4</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E40" s="47">
         <f t="shared" si="6"/>
-        <v>-0.02</v>
+        <v>0</v>
       </c>
       <c r="F40" s="43"/>
       <c r="G40" s="39">
@@ -40565,11 +40580,11 @@
       <c r="C42" s="37"/>
       <c r="D42" s="39">
         <f>AUDIO!$E$8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" s="47">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="F42" s="43"/>
       <c r="G42" s="39">
@@ -40582,7 +40597,7 @@
       </c>
       <c r="J42" s="218">
         <f>MAX(0,MIN(1,IF($J44 &lt;= 0.95, ROUND($J44,2), FLOOR((0.95+($J44-0.95)/5),0.01))))</f>
-        <v>0.63</v>
+        <v>0.68</v>
       </c>
       <c r="L42" s="218">
         <f>MAX(0,MIN(1,IF($L44 &lt;= 0.95, ROUND($L44,2), FLOOR((0.95+($L44-0.95)/5),0.01))))</f>
@@ -40627,7 +40642,7 @@
       </c>
       <c r="E44" s="41">
         <f>SUM(E38:E43)</f>
-        <v>-4.9999999999999996E-2</v>
+        <v>-2.5000000000000005E-3</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="22" t="s">
@@ -40639,7 +40654,7 @@
       </c>
       <c r="J44" s="87">
         <f>$A$7+MIN(MAX($E44*2,$E44),$D$8)</f>
-        <v>0.63</v>
+        <v>0.6775000000000001</v>
       </c>
       <c r="L44" s="87">
         <f>$A$7+MIN(MAX($H44*2,$H44),$G$8)+$G$5</f>
@@ -40774,11 +40789,11 @@
       <c r="C50" s="36"/>
       <c r="D50" s="39">
         <f>NARRATIVE!$E$7</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E50" s="47">
         <f t="shared" si="8"/>
-        <v>5.0000000000000001E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F50" s="43"/>
       <c r="G50" s="39">
@@ -40828,11 +40843,11 @@
       <c r="C52" s="35"/>
       <c r="D52" s="40">
         <f>NARRATIVE!$E$9</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E52" s="48">
         <f t="shared" si="8"/>
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="F52" s="43"/>
       <c r="G52" s="40">
@@ -40853,7 +40868,7 @@
       </c>
       <c r="E53" s="41">
         <f>SUM(E47:E52)</f>
-        <v>2.2499999999999999E-2</v>
+        <v>4.2499999999999996E-2</v>
       </c>
       <c r="F53" s="5"/>
       <c r="G53" s="22" t="s">
@@ -41815,7 +41830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
@@ -46485,8 +46500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -46558,7 +46573,7 @@
       <c r="D3" s="265"/>
       <c r="E3" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Basic")*(E$10:E$209="Missing"))+0.5*SUMPRODUCT(($A$10:$A$209="Basic")*(E$10:E$209="Partial"))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Basic")*(F$10:F$209="Missing"))+0.5*SUMPRODUCT(($A$10:$A$209="Basic")*(F$10:F$209="Partial"))</f>
@@ -46580,7 +46595,7 @@
       <c r="D4" s="265"/>
       <c r="E4" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Intermediate")*(E$10:E$209="Missing"))+0.5*SUMPRODUCT(($A$10:$A$209="Intermediate")*(E$10:E$209="Partial"))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F4" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Intermediate")*(F$10:F$209="Missing"))+0.5*SUMPRODUCT(($A$10:$A$209="Intermediate")*(F$10:F$209="Partial"))</f>
@@ -46602,7 +46617,7 @@
       <c r="D5" s="265"/>
       <c r="E5" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Intermediate")*(E$10:E$209="Completed"))+SUMPRODUCT(($A$10:$A$209="Intermediate")*(E$10:E$209="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$209="Intermediate")*(E$10:E$209="Partial"))</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F5" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Intermediate")*(F$10:F$209="Completed"))+SUMPRODUCT(($A$10:$A$209="Intermediate")*(F$10:F$209="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$209="Intermediate")*(F$10:F$209="Partial"))</f>
@@ -46624,7 +46639,7 @@
       <c r="D6" s="265"/>
       <c r="E6" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Advanced")*(E$10:E$209="Missing"))+0.5*SUMPRODUCT(($A$10:$A$209="Advanced")*(E$10:E$209="Partial"))</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Advanced")*(F$10:F$209="Missing"))+0.5*SUMPRODUCT(($A$10:$A$209="Advanced")*(F$10:F$209="Partial"))</f>
@@ -46646,7 +46661,7 @@
       <c r="D7" s="265"/>
       <c r="E7" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Advanced")*(E$10:E$209="Completed"))+SUMPRODUCT(($A$10:$A$209="Advanced")*(E$10:E$209="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$209="Advanced")*(E$10:E$209="Partial"))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Advanced")*(F$10:F$209="Completed"))+SUMPRODUCT(($A$10:$A$209="Advanced")*(F$10:F$209="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$209="Advanced")*(F$10:F$209="Partial"))</f>
@@ -46666,7 +46681,7 @@
       <c r="D8" s="265"/>
       <c r="E8" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Professional")*(E$10:E$209="Completed"))+SUMPRODUCT(($A$10:$A$209="Professional")*(E$10:E$209="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$209="Professional")*(E$10:E$209="Partial"))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Professional")*(F$10:F$209="Completed"))+SUMPRODUCT(($A$10:$A$209="Professional")*(F$10:F$209="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$209="Professional")*(F$10:F$209="Partial"))</f>
@@ -46825,7 +46840,7 @@
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>52</v>
@@ -46844,7 +46859,7 @@
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>52</v>
@@ -46937,9 +46952,11 @@
       <c r="C22" s="11" t="s">
         <v>685</v>
       </c>
-      <c r="D22" s="11"/>
+      <c r="D22" s="11" t="s">
+        <v>970</v>
+      </c>
       <c r="E22" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>52</v>
@@ -47399,7 +47416,7 @@
       </c>
       <c r="D46" s="11"/>
       <c r="E46" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>52</v>
@@ -48224,7 +48241,7 @@
       </c>
       <c r="D89" s="11"/>
       <c r="E89" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F89" s="4" t="s">
         <v>52</v>
@@ -48756,7 +48773,9 @@
       <c r="C117" s="11" t="s">
         <v>459</v>
       </c>
-      <c r="D117" s="11"/>
+      <c r="D117" s="11" t="s">
+        <v>966</v>
+      </c>
       <c r="E117" s="4" t="s">
         <v>58</v>
       </c>
@@ -51437,8 +51456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -53773,8 +53792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -53846,7 +53865,7 @@
       <c r="D3" s="265"/>
       <c r="E3" s="14">
         <f>SUMPRODUCT(($A$10:$A$257="Basic")*(E$10:E$257="Missing"))+0.5*SUMPRODUCT(($A$10:$A$257="Basic")*(E$10:E$257="Partial"))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="14">
         <f>SUMPRODUCT(($A$10:$A$257="Basic")*(F$10:F$257="Missing"))+0.5*SUMPRODUCT(($A$10:$A$257="Basic")*(F$10:F$257="Partial"))</f>
@@ -53868,7 +53887,7 @@
       <c r="D4" s="265"/>
       <c r="E4" s="14">
         <f>SUMPRODUCT(($A$10:$A$257="Intermediate")*(E$10:E$257="Missing"))+0.5*SUMPRODUCT(($A$10:$A$257="Intermediate")*(E$10:E$257="Partial"))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F4" s="14">
         <f>SUMPRODUCT(($A$10:$A$257="Intermediate")*(F$10:F$257="Missing"))+0.5*SUMPRODUCT(($A$10:$A$257="Intermediate")*(F$10:F$257="Partial"))</f>
@@ -53890,7 +53909,7 @@
       <c r="D5" s="265"/>
       <c r="E5" s="14">
         <f>SUMPRODUCT(($A$10:$A$257="Intermediate")*(E$10:E$257="Completed"))+SUMPRODUCT(($A$10:$A$257="Intermediate")*(E$10:E$257="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$257="Intermediate")*(E$10:E$257="Partial"))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5" s="14">
         <f>SUMPRODUCT(($A$10:$A$257="Intermediate")*(F$10:F$257="Completed"))+SUMPRODUCT(($A$10:$A$257="Intermediate")*(F$10:F$257="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$257="Intermediate")*(F$10:F$257="Partial"))</f>
@@ -53954,7 +53973,7 @@
       <c r="D8" s="265"/>
       <c r="E8" s="14">
         <f>SUMPRODUCT(($A$10:$A$257="Professional")*(E$10:E$257="Completed"))+SUMPRODUCT(($A$10:$A$257="Professional")*(E$10:E$257="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$257="Professional")*(E$10:E$257="Partial"))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="14">
         <f>SUMPRODUCT(($A$10:$A$257="Professional")*(F$10:F$257="Completed"))+SUMPRODUCT(($A$10:$A$257="Professional")*(F$10:F$257="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$257="Professional")*(F$10:F$257="Partial"))</f>
@@ -54438,7 +54457,7 @@
       </c>
       <c r="D33" s="11"/>
       <c r="E33" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>52</v>
@@ -54455,9 +54474,11 @@
       <c r="C34" s="11" t="s">
         <v>401</v>
       </c>
-      <c r="D34" s="11"/>
+      <c r="D34" s="11" t="s">
+        <v>968</v>
+      </c>
       <c r="E34" s="4" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>52</v>
@@ -54514,7 +54535,7 @@
       </c>
       <c r="D37" s="11"/>
       <c r="E37" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>52</v>
@@ -54877,9 +54898,11 @@
       <c r="C56" s="11" t="s">
         <v>415</v>
       </c>
-      <c r="D56" s="11"/>
+      <c r="D56" s="11" t="s">
+        <v>967</v>
+      </c>
       <c r="E56" s="4" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="F56" s="4" t="s">
         <v>52</v>
@@ -56478,7 +56501,7 @@
   <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -56616,7 +56639,7 @@
       <c r="D6" s="265"/>
       <c r="E6" s="14">
         <f>SUMPRODUCT(($A$10:$A$245="Advanced")*(E$10:E$245="Missing"))+0.5*SUMPRODUCT(($A$10:$A$245="Advanced")*(E$10:E$245="Partial"))</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F6" s="14">
         <f>SUMPRODUCT(($A$10:$A$245="Advanced")*(F$10:F$245="Missing"))+0.5*SUMPRODUCT(($A$10:$A$245="Advanced")*(F$10:F$245="Partial"))</f>
@@ -56638,7 +56661,7 @@
       <c r="D7" s="265"/>
       <c r="E7" s="14">
         <f>SUMPRODUCT(($A$10:$A$245="Advanced")*(E$10:E$245="Completed"))+SUMPRODUCT(($A$10:$A$245="Advanced")*(E$10:E$245="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$245="Advanced")*(E$10:E$245="Partial"))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F7" s="14">
         <f>SUMPRODUCT(($A$10:$A$245="Advanced")*(F$10:F$245="Completed"))+SUMPRODUCT(($A$10:$A$245="Advanced")*(F$10:F$245="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$245="Advanced")*(F$10:F$245="Partial"))</f>
@@ -56678,7 +56701,7 @@
       <c r="D9" s="267"/>
       <c r="E9" s="14">
         <f>SUMPRODUCT(($A$10:$A$237="Exceptional")*(E$10:E$237="Completed"))+SUMPRODUCT(($A$10:$A$237="Exceptional")*(E$10:E$237="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$237="Exceptional")*(E$10:E$237="Partial"))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="14">
         <f>SUMPRODUCT(($A$10:$A$237="Exceptional")*(F$10:F$237="Completed"))+SUMPRODUCT(($A$10:$A$237="Exceptional")*(F$10:F$237="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$237="Exceptional")*(F$10:F$237="Partial"))</f>
@@ -57108,7 +57131,7 @@
       </c>
       <c r="D31" s="13"/>
       <c r="E31" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>52</v>
@@ -57144,9 +57167,11 @@
       <c r="C33" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="D33" s="11"/>
+      <c r="D33" s="11" t="s">
+        <v>969</v>
+      </c>
       <c r="E33" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>52</v>
@@ -57262,7 +57287,7 @@
       </c>
       <c r="D39" s="13"/>
       <c r="E39" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Added highlights to the pulltabs, updated the rubric
</commit_message>
<xml_diff>
--- a/GameDocuments/gam352_papercut_rubric.xlsx
+++ b/GameDocuments/gam352_papercut_rubric.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Game Data" sheetId="1" r:id="rId1"/>
@@ -5740,90 +5740,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -5857,6 +5773,18 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -5914,6 +5842,99 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="4" borderId="16" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="4" borderId="18" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="9" fontId="26" fillId="3" borderId="21" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5924,12 +5945,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="26" fillId="3" borderId="26" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5998,37 +6013,55 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="4" borderId="16" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="4" borderId="18" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6040,28 +6073,28 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6088,52 +6121,19 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -38670,54 +38670,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A1" s="144" t="s">
+      <c r="A1" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="146"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="178"/>
       <c r="E1" s="103"/>
-      <c r="F1" s="144" t="s">
+      <c r="F1" s="176" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
-      <c r="J1" s="146"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="178"/>
       <c r="K1" s="104"/>
       <c r="L1" s="104"/>
       <c r="M1" s="105"/>
     </row>
     <row r="2" spans="1:13" ht="14.1" customHeight="1">
-      <c r="A2" s="147" t="s">
+      <c r="A2" s="182" t="s">
         <v>951</v>
       </c>
-      <c r="B2" s="148"/>
-      <c r="C2" s="148"/>
-      <c r="D2" s="149"/>
+      <c r="B2" s="183"/>
+      <c r="C2" s="183"/>
+      <c r="D2" s="184"/>
       <c r="E2" s="103"/>
-      <c r="F2" s="147" t="s">
+      <c r="F2" s="182" t="s">
         <v>954</v>
       </c>
-      <c r="G2" s="148"/>
-      <c r="H2" s="148"/>
-      <c r="I2" s="148"/>
-      <c r="J2" s="149"/>
+      <c r="G2" s="183"/>
+      <c r="H2" s="183"/>
+      <c r="I2" s="183"/>
+      <c r="J2" s="184"/>
       <c r="K2" s="104"/>
       <c r="L2" s="104"/>
       <c r="M2" s="105"/>
     </row>
     <row r="3" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A3" s="150"/>
-      <c r="B3" s="151"/>
-      <c r="C3" s="151"/>
-      <c r="D3" s="152"/>
+      <c r="A3" s="185"/>
+      <c r="B3" s="186"/>
+      <c r="C3" s="186"/>
+      <c r="D3" s="187"/>
       <c r="E3" s="103"/>
-      <c r="F3" s="150"/>
-      <c r="G3" s="151"/>
-      <c r="H3" s="151"/>
-      <c r="I3" s="151"/>
-      <c r="J3" s="152"/>
+      <c r="F3" s="185"/>
+      <c r="G3" s="186"/>
+      <c r="H3" s="186"/>
+      <c r="I3" s="186"/>
+      <c r="J3" s="187"/>
       <c r="K3" s="104"/>
       <c r="L3" s="104"/>
       <c r="M3" s="105"/>
@@ -38738,41 +38738,41 @@
       <c r="M4" s="105"/>
     </row>
     <row r="5" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A5" s="144" t="s">
+      <c r="A5" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="145"/>
-      <c r="C5" s="145"/>
-      <c r="D5" s="146"/>
+      <c r="B5" s="177"/>
+      <c r="C5" s="177"/>
+      <c r="D5" s="178"/>
       <c r="E5" s="103"/>
-      <c r="F5" s="144" t="s">
+      <c r="F5" s="176" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="145"/>
-      <c r="H5" s="145"/>
-      <c r="I5" s="145"/>
-      <c r="J5" s="146"/>
+      <c r="G5" s="177"/>
+      <c r="H5" s="177"/>
+      <c r="I5" s="177"/>
+      <c r="J5" s="178"/>
       <c r="K5" s="104"/>
       <c r="L5" s="107"/>
       <c r="M5" s="105"/>
     </row>
     <row r="6" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A6" s="156" t="s">
+      <c r="A6" s="173" t="s">
         <v>952</v>
       </c>
-      <c r="B6" s="157"/>
-      <c r="C6" s="157"/>
-      <c r="D6" s="158"/>
+      <c r="B6" s="174"/>
+      <c r="C6" s="174"/>
+      <c r="D6" s="175"/>
       <c r="E6" s="103"/>
-      <c r="F6" s="156" t="s">
+      <c r="F6" s="173" t="s">
         <v>955</v>
       </c>
-      <c r="G6" s="157"/>
-      <c r="H6" s="157"/>
-      <c r="I6" s="157"/>
-      <c r="J6" s="158"/>
+      <c r="G6" s="174"/>
+      <c r="H6" s="174"/>
+      <c r="I6" s="174"/>
+      <c r="J6" s="175"/>
       <c r="K6" s="104"/>
-      <c r="L6" s="153" t="s">
+      <c r="L6" s="170" t="s">
         <v>24</v>
       </c>
       <c r="M6" s="105"/>
@@ -38783,47 +38783,47 @@
       <c r="C7" s="108"/>
       <c r="D7" s="109"/>
       <c r="E7" s="103"/>
-      <c r="F7" s="156"/>
-      <c r="G7" s="157"/>
-      <c r="H7" s="157"/>
-      <c r="I7" s="157"/>
-      <c r="J7" s="158"/>
+      <c r="F7" s="173"/>
+      <c r="G7" s="174"/>
+      <c r="H7" s="174"/>
+      <c r="I7" s="174"/>
+      <c r="J7" s="175"/>
       <c r="K7" s="104"/>
-      <c r="L7" s="154"/>
+      <c r="L7" s="171"/>
       <c r="M7" s="105"/>
     </row>
     <row r="8" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A8" s="144" t="s">
+      <c r="A8" s="176" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="145"/>
-      <c r="C8" s="145"/>
-      <c r="D8" s="146"/>
+      <c r="B8" s="177"/>
+      <c r="C8" s="177"/>
+      <c r="D8" s="178"/>
       <c r="E8" s="103"/>
-      <c r="F8" s="156"/>
-      <c r="G8" s="157"/>
-      <c r="H8" s="157"/>
-      <c r="I8" s="157"/>
-      <c r="J8" s="158"/>
+      <c r="F8" s="173"/>
+      <c r="G8" s="174"/>
+      <c r="H8" s="174"/>
+      <c r="I8" s="174"/>
+      <c r="J8" s="175"/>
       <c r="K8" s="104"/>
-      <c r="L8" s="154"/>
+      <c r="L8" s="171"/>
       <c r="M8" s="105"/>
     </row>
     <row r="9" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A9" s="156" t="s">
+      <c r="A9" s="173" t="s">
         <v>953</v>
       </c>
-      <c r="B9" s="157"/>
-      <c r="C9" s="157"/>
-      <c r="D9" s="158"/>
+      <c r="B9" s="174"/>
+      <c r="C9" s="174"/>
+      <c r="D9" s="175"/>
       <c r="E9" s="103"/>
-      <c r="F9" s="156"/>
-      <c r="G9" s="157"/>
-      <c r="H9" s="157"/>
-      <c r="I9" s="157"/>
-      <c r="J9" s="158"/>
+      <c r="F9" s="173"/>
+      <c r="G9" s="174"/>
+      <c r="H9" s="174"/>
+      <c r="I9" s="174"/>
+      <c r="J9" s="175"/>
       <c r="K9" s="104"/>
-      <c r="L9" s="155"/>
+      <c r="L9" s="172"/>
       <c r="M9" s="105"/>
     </row>
     <row r="10" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -38842,18 +38842,18 @@
       <c r="M10" s="105"/>
     </row>
     <row r="11" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A11" s="144" t="s">
+      <c r="A11" s="176" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="145"/>
-      <c r="C11" s="145"/>
-      <c r="D11" s="146"/>
+      <c r="B11" s="177"/>
+      <c r="C11" s="177"/>
+      <c r="D11" s="178"/>
       <c r="E11" s="103"/>
-      <c r="F11" s="144" t="s">
+      <c r="F11" s="176" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="145"/>
-      <c r="H11" s="146"/>
+      <c r="G11" s="177"/>
+      <c r="H11" s="178"/>
       <c r="I11" s="134" t="s">
         <v>7</v>
       </c>
@@ -38893,7 +38893,7 @@
         <v>-0.12</v>
       </c>
       <c r="K12" s="104"/>
-      <c r="L12" s="153" t="s">
+      <c r="L12" s="170" t="s">
         <v>8</v>
       </c>
       <c r="M12" s="105"/>
@@ -38926,7 +38926,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="120"/>
-      <c r="L13" s="154"/>
+      <c r="L13" s="171"/>
       <c r="M13" s="121"/>
     </row>
     <row r="14" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -38956,7 +38956,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="124"/>
-      <c r="L14" s="155"/>
+      <c r="L14" s="172"/>
       <c r="M14" s="125"/>
     </row>
     <row r="15" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39024,11 +39024,11 @@
         <v>939</v>
       </c>
       <c r="E17" s="104"/>
-      <c r="F17" s="144" t="s">
+      <c r="F17" s="176" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="145"/>
-      <c r="H17" s="146"/>
+      <c r="G17" s="177"/>
+      <c r="H17" s="178"/>
       <c r="I17" s="111"/>
       <c r="J17" s="135">
         <v>0.75</v>
@@ -39054,17 +39054,17 @@
       <c r="F18" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="159" t="s">
+      <c r="G18" s="179" t="s">
         <v>956</v>
       </c>
-      <c r="H18" s="160"/>
-      <c r="I18" s="161"/>
+      <c r="H18" s="180"/>
+      <c r="I18" s="181"/>
       <c r="J18" s="137">
         <f>IF(LEFT(G18,6)="Entire",0,IF(LEFT(G18,6)="Custom",-0.05,-0.1))</f>
         <v>-0.1</v>
       </c>
       <c r="K18" s="128"/>
-      <c r="L18" s="153" t="s">
+      <c r="L18" s="170" t="s">
         <v>18</v>
       </c>
       <c r="M18" s="105"/>
@@ -39084,17 +39084,17 @@
       <c r="F19" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="162" t="s">
+      <c r="G19" s="153" t="s">
         <v>957</v>
       </c>
-      <c r="H19" s="163"/>
-      <c r="I19" s="164"/>
+      <c r="H19" s="154"/>
+      <c r="I19" s="155"/>
       <c r="J19" s="139">
         <f>IF(G19="2D Graphics and 2D Gameplay",IF(J11=0.15,-0.05,0),IF(G19="3D Graphics but 2D Gameplay",IF(J11=0.15,-0.02,-0.3),IF(J11=0.15,0,-0.3)))</f>
         <v>0</v>
       </c>
       <c r="K19" s="104"/>
-      <c r="L19" s="155"/>
+      <c r="L19" s="172"/>
       <c r="M19" s="105"/>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39144,22 +39144,22 @@
       <c r="C22" s="118"/>
       <c r="D22" s="119"/>
       <c r="E22" s="104"/>
-      <c r="F22" s="186" t="s">
+      <c r="F22" s="168" t="s">
         <v>713</v>
       </c>
-      <c r="G22" s="184" t="s">
+      <c r="G22" s="166" t="s">
         <v>714</v>
       </c>
-      <c r="H22" s="183"/>
+      <c r="H22" s="165"/>
       <c r="I22" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="181">
+      <c r="J22" s="163">
         <f>J20+J15</f>
         <v>0.68</v>
       </c>
       <c r="K22" s="104"/>
-      <c r="L22" s="165" t="s">
+      <c r="L22" s="144" t="s">
         <v>725</v>
       </c>
       <c r="M22" s="105"/>
@@ -39170,15 +39170,15 @@
       <c r="C23" s="118"/>
       <c r="D23" s="119"/>
       <c r="E23" s="104"/>
-      <c r="F23" s="187"/>
-      <c r="G23" s="185"/>
-      <c r="H23" s="183"/>
+      <c r="F23" s="169"/>
+      <c r="G23" s="167"/>
+      <c r="H23" s="165"/>
       <c r="I23" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="182"/>
+      <c r="J23" s="164"/>
       <c r="K23" s="104"/>
-      <c r="L23" s="166"/>
+      <c r="L23" s="145"/>
       <c r="M23" s="105"/>
     </row>
     <row r="24" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39202,13 +39202,13 @@
       <c r="C25" s="118"/>
       <c r="D25" s="119"/>
       <c r="E25" s="104"/>
-      <c r="F25" s="175" t="s">
+      <c r="F25" s="157" t="s">
         <v>932</v>
       </c>
-      <c r="G25" s="176"/>
-      <c r="H25" s="176"/>
-      <c r="I25" s="176"/>
-      <c r="J25" s="177"/>
+      <c r="G25" s="158"/>
+      <c r="H25" s="158"/>
+      <c r="I25" s="158"/>
+      <c r="J25" s="159"/>
       <c r="K25" s="104"/>
       <c r="L25" s="104"/>
       <c r="M25" s="105"/>
@@ -39219,11 +39219,11 @@
       <c r="C26" s="118"/>
       <c r="D26" s="119"/>
       <c r="E26" s="103"/>
-      <c r="F26" s="178"/>
-      <c r="G26" s="179"/>
-      <c r="H26" s="179"/>
-      <c r="I26" s="179"/>
-      <c r="J26" s="180"/>
+      <c r="F26" s="160"/>
+      <c r="G26" s="161"/>
+      <c r="H26" s="161"/>
+      <c r="I26" s="161"/>
+      <c r="J26" s="162"/>
       <c r="K26" s="104"/>
       <c r="L26" s="104"/>
       <c r="M26" s="105"/>
@@ -39249,13 +39249,13 @@
       <c r="C28" s="118"/>
       <c r="D28" s="119"/>
       <c r="E28" s="103"/>
-      <c r="F28" s="174" t="s">
+      <c r="F28" s="156" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="174"/>
-      <c r="H28" s="174"/>
-      <c r="I28" s="174"/>
-      <c r="J28" s="174"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
       <c r="K28" s="104"/>
       <c r="L28" s="104"/>
       <c r="M28" s="105"/>
@@ -39266,13 +39266,13 @@
       <c r="C29" s="118"/>
       <c r="D29" s="119"/>
       <c r="E29" s="103"/>
-      <c r="F29" s="171" t="s">
+      <c r="F29" s="150" t="s">
         <v>933</v>
       </c>
-      <c r="G29" s="172"/>
-      <c r="H29" s="172"/>
-      <c r="I29" s="172"/>
-      <c r="J29" s="173"/>
+      <c r="G29" s="151"/>
+      <c r="H29" s="151"/>
+      <c r="I29" s="151"/>
+      <c r="J29" s="152"/>
       <c r="K29" s="104"/>
       <c r="L29" s="104"/>
       <c r="M29" s="105"/>
@@ -39283,30 +39283,30 @@
       <c r="C30" s="118"/>
       <c r="D30" s="119"/>
       <c r="E30" s="103"/>
-      <c r="F30" s="171"/>
-      <c r="G30" s="172"/>
-      <c r="H30" s="172"/>
-      <c r="I30" s="172"/>
-      <c r="J30" s="173"/>
+      <c r="F30" s="150"/>
+      <c r="G30" s="151"/>
+      <c r="H30" s="151"/>
+      <c r="I30" s="151"/>
+      <c r="J30" s="152"/>
       <c r="K30" s="104"/>
       <c r="L30" s="104"/>
       <c r="M30" s="105"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A31" s="167" t="s">
+      <c r="A31" s="146" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="168"/>
-      <c r="C31" s="169" t="s">
+      <c r="B31" s="147"/>
+      <c r="C31" s="148" t="s">
         <v>950</v>
       </c>
-      <c r="D31" s="170"/>
+      <c r="D31" s="149"/>
       <c r="E31" s="104"/>
-      <c r="F31" s="162"/>
-      <c r="G31" s="163"/>
-      <c r="H31" s="163"/>
-      <c r="I31" s="163"/>
-      <c r="J31" s="164"/>
+      <c r="F31" s="153"/>
+      <c r="G31" s="154"/>
+      <c r="H31" s="154"/>
+      <c r="I31" s="154"/>
+      <c r="J31" s="155"/>
       <c r="K31" s="104"/>
       <c r="L31" s="104"/>
       <c r="M31" s="105"/>
@@ -39329,16 +39329,12 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0"/>
   <mergeCells count="31">
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F29:J31"/>
-    <mergeCell ref="F28:J28"/>
-    <mergeCell ref="F25:J26"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A2:D3"/>
+    <mergeCell ref="F2:J3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:J5"/>
     <mergeCell ref="L12:L14"/>
     <mergeCell ref="L18:L19"/>
     <mergeCell ref="A6:D6"/>
@@ -39354,12 +39350,16 @@
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="G18:I18"/>
     <mergeCell ref="G19:I19"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="A2:D3"/>
-    <mergeCell ref="F2:J3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F29:J31"/>
+    <mergeCell ref="F28:J28"/>
+    <mergeCell ref="F25:J26"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F22:F23"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6:D6">
@@ -39427,57 +39427,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A1" s="194" t="s">
+      <c r="A1" s="199" t="s">
         <v>556</v>
       </c>
-      <c r="B1" s="195"/>
-      <c r="C1" s="195"/>
-      <c r="D1" s="195"/>
-      <c r="E1" s="195"/>
-      <c r="F1" s="195"/>
-      <c r="G1" s="195"/>
-      <c r="H1" s="195"/>
-      <c r="J1" s="205" t="s">
+      <c r="B1" s="200"/>
+      <c r="C1" s="200"/>
+      <c r="D1" s="200"/>
+      <c r="E1" s="200"/>
+      <c r="F1" s="200"/>
+      <c r="G1" s="200"/>
+      <c r="H1" s="200"/>
+      <c r="J1" s="210" t="s">
         <v>482</v>
       </c>
-      <c r="K1" s="206"/>
-      <c r="L1" s="207"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="212"/>
       <c r="M1" s="79"/>
       <c r="N1" s="24" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A2" s="194"/>
-      <c r="B2" s="195"/>
-      <c r="C2" s="195"/>
-      <c r="D2" s="195"/>
-      <c r="E2" s="195"/>
-      <c r="F2" s="195"/>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
-      <c r="J2" s="208" t="s">
+      <c r="A2" s="199"/>
+      <c r="B2" s="200"/>
+      <c r="C2" s="200"/>
+      <c r="D2" s="200"/>
+      <c r="E2" s="200"/>
+      <c r="F2" s="200"/>
+      <c r="G2" s="200"/>
+      <c r="H2" s="200"/>
+      <c r="J2" s="213" t="s">
         <v>706</v>
       </c>
-      <c r="K2" s="209"/>
-      <c r="L2" s="210"/>
+      <c r="K2" s="214"/>
+      <c r="L2" s="215"/>
       <c r="M2" s="23"/>
       <c r="N2" s="26" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A3" s="194"/>
-      <c r="B3" s="195"/>
-      <c r="C3" s="195"/>
-      <c r="D3" s="195"/>
-      <c r="E3" s="195"/>
-      <c r="F3" s="195"/>
-      <c r="G3" s="195"/>
-      <c r="H3" s="195"/>
-      <c r="J3" s="208"/>
-      <c r="K3" s="209"/>
-      <c r="L3" s="210"/>
+      <c r="A3" s="199"/>
+      <c r="B3" s="200"/>
+      <c r="C3" s="200"/>
+      <c r="D3" s="200"/>
+      <c r="E3" s="200"/>
+      <c r="F3" s="200"/>
+      <c r="G3" s="200"/>
+      <c r="H3" s="200"/>
+      <c r="J3" s="213"/>
+      <c r="K3" s="214"/>
+      <c r="L3" s="215"/>
       <c r="M3" s="23"/>
       <c r="N3" s="26" t="s">
         <v>431</v>
@@ -39487,14 +39487,14 @@
       <c r="A4" s="2"/>
       <c r="B4" s="5"/>
       <c r="C4" s="8"/>
-      <c r="D4" s="193"/>
-      <c r="E4" s="193"/>
+      <c r="D4" s="192"/>
+      <c r="E4" s="192"/>
       <c r="F4" s="43"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="193"/>
-      <c r="J4" s="208"/>
-      <c r="K4" s="209"/>
-      <c r="L4" s="210"/>
+      <c r="G4" s="192"/>
+      <c r="H4" s="192"/>
+      <c r="J4" s="213"/>
+      <c r="K4" s="214"/>
+      <c r="L4" s="215"/>
       <c r="M4" s="34"/>
       <c r="N4" s="26" t="s">
         <v>432</v>
@@ -39502,24 +39502,24 @@
       <c r="O4" s="81"/>
     </row>
     <row r="5" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A5" s="196" t="s">
+      <c r="A5" s="201" t="s">
         <v>425</v>
       </c>
-      <c r="B5" s="197"/>
+      <c r="B5" s="202"/>
       <c r="C5" s="8"/>
-      <c r="D5" s="200" t="s">
+      <c r="D5" s="205" t="s">
         <v>717</v>
       </c>
-      <c r="E5" s="201"/>
-      <c r="F5" s="202"/>
-      <c r="G5" s="203">
+      <c r="E5" s="206"/>
+      <c r="F5" s="207"/>
+      <c r="G5" s="208">
         <f>Submission!$E$17</f>
         <v>0</v>
       </c>
-      <c r="H5" s="204"/>
-      <c r="J5" s="208"/>
-      <c r="K5" s="209"/>
-      <c r="L5" s="210"/>
+      <c r="H5" s="209"/>
+      <c r="J5" s="213"/>
+      <c r="K5" s="214"/>
+      <c r="L5" s="215"/>
       <c r="M5" s="34"/>
       <c r="N5" s="26" t="s">
         <v>433</v>
@@ -39527,21 +39527,21 @@
       <c r="O5" s="81"/>
     </row>
     <row r="6" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A6" s="198"/>
-      <c r="B6" s="199"/>
+      <c r="A6" s="203"/>
+      <c r="B6" s="204"/>
       <c r="C6" s="43"/>
-      <c r="D6" s="193" t="s">
+      <c r="D6" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="193"/>
+      <c r="E6" s="192"/>
       <c r="F6" s="43"/>
-      <c r="G6" s="193" t="s">
+      <c r="G6" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="193"/>
-      <c r="J6" s="208"/>
-      <c r="K6" s="209"/>
-      <c r="L6" s="210"/>
+      <c r="H6" s="192"/>
+      <c r="J6" s="213"/>
+      <c r="K6" s="214"/>
+      <c r="L6" s="215"/>
       <c r="M6" s="34"/>
       <c r="N6" s="26" t="s">
         <v>434</v>
@@ -39549,24 +39549,24 @@
       <c r="O6" s="81"/>
     </row>
     <row r="7" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A7" s="188">
+      <c r="A7" s="195">
         <f>'Game Data'!$J$22</f>
         <v>0.68</v>
       </c>
-      <c r="B7" s="189"/>
+      <c r="B7" s="196"/>
       <c r="C7" s="43"/>
-      <c r="D7" s="216" t="s">
+      <c r="D7" s="193" t="s">
         <v>724</v>
       </c>
-      <c r="E7" s="217"/>
+      <c r="E7" s="194"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="216" t="s">
+      <c r="G7" s="193" t="s">
         <v>724</v>
       </c>
-      <c r="H7" s="217"/>
-      <c r="J7" s="208"/>
-      <c r="K7" s="209"/>
-      <c r="L7" s="210"/>
+      <c r="H7" s="194"/>
+      <c r="J7" s="213"/>
+      <c r="K7" s="214"/>
+      <c r="L7" s="215"/>
       <c r="M7" s="33"/>
       <c r="N7" s="26" t="s">
         <v>435</v>
@@ -39574,23 +39574,23 @@
       <c r="O7" s="81"/>
     </row>
     <row r="8" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A8" s="190"/>
-      <c r="B8" s="191"/>
+      <c r="A8" s="197"/>
+      <c r="B8" s="198"/>
       <c r="C8" s="97"/>
-      <c r="D8" s="214">
+      <c r="D8" s="219">
         <f>E17+E26+E35+E44+E53</f>
         <v>0.13874999999999998</v>
       </c>
-      <c r="E8" s="215"/>
+      <c r="E8" s="220"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="214">
+      <c r="G8" s="219">
         <f>H17+H26+H35+H44+H53</f>
         <v>0</v>
       </c>
-      <c r="H8" s="215"/>
-      <c r="J8" s="211"/>
-      <c r="K8" s="212"/>
-      <c r="L8" s="213"/>
+      <c r="H8" s="220"/>
+      <c r="J8" s="216"/>
+      <c r="K8" s="217"/>
+      <c r="L8" s="218"/>
       <c r="M8" s="80"/>
       <c r="N8" s="25" t="s">
         <v>436</v>
@@ -39601,15 +39601,15 @@
       <c r="A9" s="2"/>
       <c r="B9" s="5"/>
       <c r="C9" s="43"/>
-      <c r="D9" s="193" t="s">
+      <c r="D9" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="193"/>
+      <c r="E9" s="192"/>
       <c r="F9" s="43"/>
-      <c r="G9" s="193" t="s">
+      <c r="G9" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="193"/>
+      <c r="H9" s="192"/>
       <c r="J9" s="82"/>
       <c r="K9" s="82"/>
       <c r="L9" s="82"/>
@@ -39636,11 +39636,11 @@
       <c r="H10" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="192" t="s">
+      <c r="J10" s="191" t="s">
         <v>707</v>
       </c>
-      <c r="K10" s="192"/>
-      <c r="L10" s="192"/>
+      <c r="K10" s="191"/>
+      <c r="L10" s="191"/>
       <c r="O10" s="84"/>
     </row>
     <row r="11" spans="1:15" ht="14.1" customHeight="1">
@@ -39669,11 +39669,11 @@
         <f t="shared" ref="H11:H16" si="1">$B11*G11</f>
         <v>0</v>
       </c>
-      <c r="J11" s="220" t="s">
+      <c r="J11" s="190" t="s">
         <v>792</v>
       </c>
-      <c r="K11" s="220"/>
-      <c r="L11" s="220"/>
+      <c r="K11" s="190"/>
+      <c r="L11" s="190"/>
       <c r="M11" s="82"/>
       <c r="O11" s="84"/>
     </row>
@@ -39703,9 +39703,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J12" s="220"/>
-      <c r="K12" s="220"/>
-      <c r="L12" s="220"/>
+      <c r="J12" s="190"/>
+      <c r="K12" s="190"/>
+      <c r="L12" s="190"/>
       <c r="M12" s="82"/>
       <c r="O12" s="84"/>
     </row>
@@ -39735,9 +39735,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="220"/>
-      <c r="K13" s="220"/>
-      <c r="L13" s="220"/>
+      <c r="J13" s="190"/>
+      <c r="K13" s="190"/>
+      <c r="L13" s="190"/>
       <c r="M13" s="82"/>
       <c r="O13" s="84"/>
     </row>
@@ -39803,11 +39803,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J15" s="218">
+      <c r="J15" s="188">
         <f>MAX(0,MIN(1,IF($J17 &lt;= 0.95, ROUND($J17,2), FLOOR((0.95+($J17-0.95)/5),0.01))))</f>
         <v>0.75</v>
       </c>
-      <c r="L15" s="218">
+      <c r="L15" s="188">
         <f>MAX(0,MIN(1,IF($L17 &lt;= 0.95, ROUND($L17,2), FLOOR((0.95+($L17-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -39840,8 +39840,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J16" s="219"/>
-      <c r="L16" s="219"/>
+      <c r="J16" s="189"/>
+      <c r="L16" s="189"/>
       <c r="M16" s="82"/>
       <c r="O16" s="84"/>
     </row>
@@ -39878,15 +39878,15 @@
       <c r="A18" s="2"/>
       <c r="B18" s="5"/>
       <c r="C18" s="43"/>
-      <c r="D18" s="193" t="s">
+      <c r="D18" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="193"/>
+      <c r="E18" s="192"/>
       <c r="F18" s="43"/>
-      <c r="G18" s="193" t="s">
+      <c r="G18" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="193"/>
+      <c r="H18" s="192"/>
       <c r="J18" s="88"/>
       <c r="M18" s="78"/>
     </row>
@@ -39911,11 +39911,11 @@
       <c r="H19" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="192" t="s">
+      <c r="J19" s="191" t="s">
         <v>715</v>
       </c>
-      <c r="K19" s="192"/>
-      <c r="L19" s="192"/>
+      <c r="K19" s="191"/>
+      <c r="L19" s="191"/>
       <c r="M19" s="83"/>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1">
@@ -39944,11 +39944,11 @@
         <f t="shared" ref="H20:H25" si="3">$B20*G20</f>
         <v>0</v>
       </c>
-      <c r="J20" s="220" t="s">
+      <c r="J20" s="190" t="s">
         <v>722</v>
       </c>
-      <c r="K20" s="220"/>
-      <c r="L20" s="220"/>
+      <c r="K20" s="190"/>
+      <c r="L20" s="190"/>
       <c r="M20" s="84"/>
     </row>
     <row r="21" spans="1:13" ht="14.1" customHeight="1">
@@ -39977,9 +39977,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J21" s="220"/>
-      <c r="K21" s="220"/>
-      <c r="L21" s="220"/>
+      <c r="J21" s="190"/>
+      <c r="K21" s="190"/>
+      <c r="L21" s="190"/>
       <c r="M21" s="84"/>
     </row>
     <row r="22" spans="1:13" ht="14.1" customHeight="1">
@@ -40008,9 +40008,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J22" s="220"/>
-      <c r="K22" s="220"/>
-      <c r="L22" s="220"/>
+      <c r="J22" s="190"/>
+      <c r="K22" s="190"/>
+      <c r="L22" s="190"/>
       <c r="M22" s="84"/>
     </row>
     <row r="23" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40074,11 +40074,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J24" s="218">
+      <c r="J24" s="188">
         <f>MAX(0,MIN(1,IF($J26 &lt;= 0.95, ROUND($J26,2), FLOOR((0.95+($J26-0.95)/5),0.01))))</f>
         <v>0.72</v>
       </c>
-      <c r="L24" s="218">
+      <c r="L24" s="188">
         <f>MAX(0,MIN(1,IF($L26 &lt;= 0.95, ROUND($L26,2), FLOOR((0.95+($L26-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40110,8 +40110,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J25" s="219"/>
-      <c r="L25" s="219"/>
+      <c r="J25" s="189"/>
+      <c r="L25" s="189"/>
       <c r="M25" s="84"/>
     </row>
     <row r="26" spans="1:13" ht="14.1" customHeight="1">
@@ -40147,15 +40147,15 @@
       <c r="A27" s="2"/>
       <c r="B27" s="5"/>
       <c r="C27" s="43"/>
-      <c r="D27" s="193" t="s">
+      <c r="D27" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="193"/>
+      <c r="E27" s="192"/>
       <c r="F27" s="43"/>
-      <c r="G27" s="193" t="s">
+      <c r="G27" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H27" s="193"/>
+      <c r="H27" s="192"/>
     </row>
     <row r="28" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
       <c r="A28" s="1" t="s">
@@ -40178,11 +40178,11 @@
       <c r="H28" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J28" s="192" t="s">
+      <c r="J28" s="191" t="s">
         <v>709</v>
       </c>
-      <c r="K28" s="192"/>
-      <c r="L28" s="192"/>
+      <c r="K28" s="191"/>
+      <c r="L28" s="191"/>
     </row>
     <row r="29" spans="1:13" ht="14.1" customHeight="1">
       <c r="A29" s="57" t="str">
@@ -40210,11 +40210,11 @@
         <f t="shared" ref="H29:H34" si="5">$B29*G29</f>
         <v>0</v>
       </c>
-      <c r="J29" s="220" t="s">
+      <c r="J29" s="190" t="s">
         <v>710</v>
       </c>
-      <c r="K29" s="220"/>
-      <c r="L29" s="220"/>
+      <c r="K29" s="190"/>
+      <c r="L29" s="190"/>
     </row>
     <row r="30" spans="1:13" ht="14.1" customHeight="1">
       <c r="A30" s="58" t="str">
@@ -40242,9 +40242,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J30" s="220"/>
-      <c r="K30" s="220"/>
-      <c r="L30" s="220"/>
+      <c r="J30" s="190"/>
+      <c r="K30" s="190"/>
+      <c r="L30" s="190"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1">
       <c r="A31" s="58" t="str">
@@ -40272,9 +40272,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J31" s="220"/>
-      <c r="K31" s="220"/>
-      <c r="L31" s="220"/>
+      <c r="J31" s="190"/>
+      <c r="K31" s="190"/>
+      <c r="L31" s="190"/>
     </row>
     <row r="32" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
       <c r="A32" s="58" t="str">
@@ -40336,11 +40336,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J33" s="218">
+      <c r="J33" s="188">
         <f>MAX(0,MIN(1,IF($J35 &lt;= 0.95, ROUND($J35,2), FLOOR((0.95+($J35-0.95)/5),0.01))))</f>
         <v>0.82</v>
       </c>
-      <c r="L33" s="218">
+      <c r="L33" s="188">
         <f>MAX(0,MIN(1,IF($L35 &lt;= 0.95, ROUND($L35,2), FLOOR((0.95+($L35-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40371,8 +40371,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J34" s="219"/>
-      <c r="L34" s="219"/>
+      <c r="J34" s="189"/>
+      <c r="L34" s="189"/>
     </row>
     <row r="35" spans="1:12" ht="14.1" customHeight="1">
       <c r="A35" s="2"/>
@@ -40406,15 +40406,15 @@
       <c r="A36" s="2"/>
       <c r="B36" s="5"/>
       <c r="C36" s="43"/>
-      <c r="D36" s="193" t="s">
+      <c r="D36" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="193"/>
+      <c r="E36" s="192"/>
       <c r="F36" s="43"/>
-      <c r="G36" s="193" t="s">
+      <c r="G36" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H36" s="193"/>
+      <c r="H36" s="192"/>
     </row>
     <row r="37" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A37" s="1" t="s">
@@ -40437,11 +40437,11 @@
       <c r="H37" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J37" s="192" t="s">
+      <c r="J37" s="191" t="s">
         <v>711</v>
       </c>
-      <c r="K37" s="192"/>
-      <c r="L37" s="192"/>
+      <c r="K37" s="191"/>
+      <c r="L37" s="191"/>
     </row>
     <row r="38" spans="1:12" ht="14.1" customHeight="1">
       <c r="A38" s="57" t="str">
@@ -40469,11 +40469,11 @@
         <f t="shared" ref="H38:H43" si="7">$B38*G38</f>
         <v>0</v>
       </c>
-      <c r="J38" s="220" t="s">
+      <c r="J38" s="190" t="s">
         <v>712</v>
       </c>
-      <c r="K38" s="220"/>
-      <c r="L38" s="220"/>
+      <c r="K38" s="190"/>
+      <c r="L38" s="190"/>
     </row>
     <row r="39" spans="1:12" ht="14.1" customHeight="1">
       <c r="A39" s="58" t="str">
@@ -40501,9 +40501,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J39" s="220"/>
-      <c r="K39" s="220"/>
-      <c r="L39" s="220"/>
+      <c r="J39" s="190"/>
+      <c r="K39" s="190"/>
+      <c r="L39" s="190"/>
     </row>
     <row r="40" spans="1:12" ht="14.1" customHeight="1">
       <c r="A40" s="58" t="str">
@@ -40531,9 +40531,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J40" s="220"/>
-      <c r="K40" s="220"/>
-      <c r="L40" s="220"/>
+      <c r="J40" s="190"/>
+      <c r="K40" s="190"/>
+      <c r="L40" s="190"/>
     </row>
     <row r="41" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A41" s="58" t="str">
@@ -40595,11 +40595,11 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J42" s="218">
+      <c r="J42" s="188">
         <f>MAX(0,MIN(1,IF($J44 &lt;= 0.95, ROUND($J44,2), FLOOR((0.95+($J44-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
-      <c r="L42" s="218">
+      <c r="L42" s="188">
         <f>MAX(0,MIN(1,IF($L44 &lt;= 0.95, ROUND($L44,2), FLOOR((0.95+($L44-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40630,8 +40630,8 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J43" s="219"/>
-      <c r="L43" s="219"/>
+      <c r="J43" s="189"/>
+      <c r="L43" s="189"/>
     </row>
     <row r="44" spans="1:12" ht="14.1" customHeight="1">
       <c r="A44" s="2"/>
@@ -40665,15 +40665,15 @@
       <c r="A45" s="2"/>
       <c r="B45" s="5"/>
       <c r="C45" s="43"/>
-      <c r="D45" s="193" t="s">
+      <c r="D45" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="193"/>
+      <c r="E45" s="192"/>
       <c r="F45" s="43"/>
-      <c r="G45" s="193" t="s">
+      <c r="G45" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="193"/>
+      <c r="H45" s="192"/>
     </row>
     <row r="46" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A46" s="1" t="s">
@@ -40881,34 +40881,6 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="L42:L43"/>
-    <mergeCell ref="J29:L31"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="L33:L34"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="J38:L40"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="J11:L13"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J20:L22"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G36:H36"/>
     <mergeCell ref="A7:B8"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="D6:E6"/>
@@ -40922,6 +40894,34 @@
     <mergeCell ref="J2:L8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G8:H8"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="J11:L13"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J20:L22"/>
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="J29:L31"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="L33:L34"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="J38:L40"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -40949,59 +40949,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A1" s="235" t="s">
+      <c r="A1" s="232" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="237"/>
+      <c r="B1" s="233"/>
+      <c r="C1" s="233"/>
+      <c r="D1" s="233"/>
+      <c r="E1" s="233"/>
+      <c r="F1" s="233"/>
+      <c r="G1" s="234"/>
     </row>
     <row r="2" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A2" s="230" t="s">
+      <c r="A2" s="221" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="231"/>
-      <c r="C2" s="231"/>
-      <c r="D2" s="231"/>
-      <c r="E2" s="231"/>
-      <c r="F2" s="231"/>
-      <c r="G2" s="232"/>
+      <c r="B2" s="222"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="223"/>
     </row>
     <row r="3" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A3" s="227" t="s">
+      <c r="A3" s="238" t="s">
         <v>930</v>
       </c>
-      <c r="B3" s="228"/>
-      <c r="C3" s="228"/>
-      <c r="D3" s="228"/>
-      <c r="E3" s="228"/>
-      <c r="F3" s="228"/>
-      <c r="G3" s="229"/>
+      <c r="B3" s="239"/>
+      <c r="C3" s="239"/>
+      <c r="D3" s="239"/>
+      <c r="E3" s="239"/>
+      <c r="F3" s="239"/>
+      <c r="G3" s="240"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A4" s="230" t="s">
+      <c r="A4" s="221" t="s">
         <v>438</v>
       </c>
-      <c r="B4" s="231"/>
-      <c r="C4" s="231"/>
-      <c r="D4" s="231"/>
-      <c r="E4" s="231"/>
-      <c r="F4" s="231"/>
-      <c r="G4" s="232"/>
+      <c r="B4" s="222"/>
+      <c r="C4" s="222"/>
+      <c r="D4" s="222"/>
+      <c r="E4" s="222"/>
+      <c r="F4" s="222"/>
+      <c r="G4" s="223"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A5" s="238" t="s">
+      <c r="A5" s="249" t="s">
         <v>580</v>
       </c>
-      <c r="B5" s="239"/>
-      <c r="C5" s="239"/>
-      <c r="D5" s="239"/>
-      <c r="E5" s="239"/>
-      <c r="F5" s="239"/>
-      <c r="G5" s="240"/>
+      <c r="B5" s="250"/>
+      <c r="C5" s="250"/>
+      <c r="D5" s="250"/>
+      <c r="E5" s="250"/>
+      <c r="F5" s="250"/>
+      <c r="G5" s="251"/>
     </row>
     <row r="6" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
       <c r="A6" s="2"/>
@@ -41034,10 +41034,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75">
-      <c r="A8" s="233" t="s">
+      <c r="A8" s="247" t="s">
         <v>718</v>
       </c>
-      <c r="B8" s="234"/>
+      <c r="B8" s="248"/>
       <c r="C8" s="65">
         <v>0</v>
       </c>
@@ -41054,10 +41054,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75">
-      <c r="A9" s="242" t="s">
+      <c r="A9" s="253" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="243"/>
+      <c r="B9" s="254"/>
       <c r="C9" s="92">
         <v>0</v>
       </c>
@@ -41074,10 +41074,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75">
-      <c r="A10" s="244" t="s">
+      <c r="A10" s="255" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="245"/>
+      <c r="B10" s="256"/>
       <c r="C10" s="69">
         <v>0</v>
       </c>
@@ -41094,10 +41094,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75">
-      <c r="A11" s="245" t="s">
+      <c r="A11" s="256" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="245"/>
+      <c r="B11" s="256"/>
       <c r="C11" s="69">
         <v>0</v>
       </c>
@@ -41114,10 +41114,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75">
-      <c r="A12" s="245" t="s">
+      <c r="A12" s="256" t="s">
         <v>716</v>
       </c>
-      <c r="B12" s="245"/>
+      <c r="B12" s="256"/>
       <c r="C12" s="69">
         <v>0</v>
       </c>
@@ -41134,10 +41134,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75">
-      <c r="A13" s="245" t="s">
+      <c r="A13" s="256" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="245"/>
+      <c r="B13" s="256"/>
       <c r="C13" s="69">
         <v>0</v>
       </c>
@@ -41154,10 +41154,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75">
-      <c r="A14" s="244" t="s">
+      <c r="A14" s="255" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="245"/>
+      <c r="B14" s="256"/>
       <c r="C14" s="69">
         <v>0</v>
       </c>
@@ -41174,10 +41174,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75">
-      <c r="A15" s="244" t="s">
+      <c r="A15" s="255" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="245"/>
+      <c r="B15" s="256"/>
       <c r="C15" s="69">
         <v>0</v>
       </c>
@@ -41194,10 +41194,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A16" s="246" t="s">
+      <c r="A16" s="230" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="247"/>
+      <c r="B16" s="231"/>
       <c r="C16" s="73">
         <v>0</v>
       </c>
@@ -41215,11 +41215,11 @@
     </row>
     <row r="17" spans="1:7" ht="14.1" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="241" t="s">
+      <c r="B17" s="252" t="s">
         <v>721</v>
       </c>
-      <c r="C17" s="241"/>
-      <c r="D17" s="241"/>
+      <c r="C17" s="252"/>
+      <c r="D17" s="252"/>
       <c r="E17" s="63">
         <f>SUM(E9:E16)</f>
         <v>0</v>
@@ -41240,527 +41240,559 @@
       <c r="A19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="235" t="s">
+      <c r="B19" s="232" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="236"/>
-      <c r="D19" s="236"/>
-      <c r="E19" s="236"/>
-      <c r="F19" s="236"/>
-      <c r="G19" s="237"/>
+      <c r="C19" s="233"/>
+      <c r="D19" s="233"/>
+      <c r="E19" s="233"/>
+      <c r="F19" s="233"/>
+      <c r="G19" s="234"/>
     </row>
     <row r="20" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="A20" s="10" t="s">
         <v>582</v>
       </c>
-      <c r="B20" s="230" t="s">
+      <c r="B20" s="221" t="s">
         <v>931</v>
       </c>
-      <c r="C20" s="231"/>
-      <c r="D20" s="231"/>
-      <c r="E20" s="231"/>
-      <c r="F20" s="231"/>
-      <c r="G20" s="232"/>
+      <c r="C20" s="222"/>
+      <c r="D20" s="222"/>
+      <c r="E20" s="222"/>
+      <c r="F20" s="222"/>
+      <c r="G20" s="223"/>
     </row>
     <row r="21" spans="1:7" ht="60" customHeight="1" thickBot="1">
       <c r="A21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="230" t="s">
+      <c r="B21" s="221" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="231"/>
-      <c r="D21" s="231"/>
-      <c r="E21" s="231"/>
-      <c r="F21" s="231"/>
-      <c r="G21" s="232"/>
+      <c r="C21" s="222"/>
+      <c r="D21" s="222"/>
+      <c r="E21" s="222"/>
+      <c r="F21" s="222"/>
+      <c r="G21" s="223"/>
     </row>
     <row r="22" spans="1:7" ht="45.95" customHeight="1" thickBot="1">
       <c r="A22" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="230" t="s">
+      <c r="B22" s="221" t="s">
         <v>917</v>
       </c>
-      <c r="C22" s="231"/>
-      <c r="D22" s="231"/>
-      <c r="E22" s="231"/>
-      <c r="F22" s="231"/>
-      <c r="G22" s="232"/>
+      <c r="C22" s="222"/>
+      <c r="D22" s="222"/>
+      <c r="E22" s="222"/>
+      <c r="F22" s="222"/>
+      <c r="G22" s="223"/>
     </row>
     <row r="23" spans="1:7" ht="32.1" customHeight="1">
       <c r="A23" s="98" t="s">
         <v>899</v>
       </c>
-      <c r="B23" s="227" t="s">
+      <c r="B23" s="238" t="s">
         <v>916</v>
       </c>
-      <c r="C23" s="228"/>
-      <c r="D23" s="228"/>
-      <c r="E23" s="228"/>
-      <c r="F23" s="228"/>
-      <c r="G23" s="229"/>
+      <c r="C23" s="239"/>
+      <c r="D23" s="239"/>
+      <c r="E23" s="239"/>
+      <c r="F23" s="239"/>
+      <c r="G23" s="240"/>
     </row>
     <row r="24" spans="1:7" ht="15.75">
       <c r="A24" s="99"/>
-      <c r="B24" s="221" t="s">
+      <c r="B24" s="257" t="s">
         <v>900</v>
       </c>
-      <c r="C24" s="222"/>
-      <c r="D24" s="223" t="s">
+      <c r="C24" s="258"/>
+      <c r="D24" s="260" t="s">
         <v>901</v>
       </c>
-      <c r="E24" s="223"/>
-      <c r="F24" s="223"/>
-      <c r="G24" s="224"/>
+      <c r="E24" s="260"/>
+      <c r="F24" s="260"/>
+      <c r="G24" s="261"/>
     </row>
     <row r="25" spans="1:7" ht="15.75">
       <c r="A25" s="99"/>
-      <c r="B25" s="221" t="s">
+      <c r="B25" s="257" t="s">
         <v>902</v>
       </c>
-      <c r="C25" s="222"/>
-      <c r="D25" s="223" t="s">
+      <c r="C25" s="258"/>
+      <c r="D25" s="260" t="s">
         <v>903</v>
       </c>
-      <c r="E25" s="223"/>
-      <c r="F25" s="223"/>
-      <c r="G25" s="224"/>
+      <c r="E25" s="260"/>
+      <c r="F25" s="260"/>
+      <c r="G25" s="261"/>
     </row>
     <row r="26" spans="1:7" ht="15.75">
       <c r="A26" s="99"/>
-      <c r="B26" s="221" t="s">
+      <c r="B26" s="257" t="s">
         <v>904</v>
       </c>
-      <c r="C26" s="222"/>
-      <c r="D26" s="223" t="s">
+      <c r="C26" s="258"/>
+      <c r="D26" s="260" t="s">
         <v>905</v>
       </c>
-      <c r="E26" s="223"/>
-      <c r="F26" s="223"/>
-      <c r="G26" s="224"/>
+      <c r="E26" s="260"/>
+      <c r="F26" s="260"/>
+      <c r="G26" s="261"/>
     </row>
     <row r="27" spans="1:7" ht="15.75">
       <c r="A27" s="99"/>
-      <c r="B27" s="221" t="s">
+      <c r="B27" s="257" t="s">
         <v>906</v>
       </c>
-      <c r="C27" s="222"/>
+      <c r="C27" s="258"/>
       <c r="D27" s="225" t="s">
         <v>907</v>
       </c>
       <c r="E27" s="225"/>
       <c r="F27" s="225"/>
-      <c r="G27" s="226"/>
+      <c r="G27" s="259"/>
     </row>
     <row r="28" spans="1:7" ht="15.75">
       <c r="A28" s="99"/>
-      <c r="B28" s="221" t="s">
+      <c r="B28" s="257" t="s">
         <v>908</v>
       </c>
-      <c r="C28" s="222"/>
-      <c r="D28" s="223" t="s">
+      <c r="C28" s="258"/>
+      <c r="D28" s="260" t="s">
         <v>909</v>
       </c>
-      <c r="E28" s="223"/>
-      <c r="F28" s="223"/>
-      <c r="G28" s="224"/>
+      <c r="E28" s="260"/>
+      <c r="F28" s="260"/>
+      <c r="G28" s="261"/>
     </row>
     <row r="29" spans="1:7" ht="15.75">
       <c r="A29" s="99"/>
-      <c r="B29" s="221" t="s">
+      <c r="B29" s="257" t="s">
         <v>910</v>
       </c>
-      <c r="C29" s="222"/>
+      <c r="C29" s="258"/>
       <c r="D29" s="225" t="s">
         <v>911</v>
       </c>
       <c r="E29" s="225"/>
       <c r="F29" s="225"/>
-      <c r="G29" s="226"/>
+      <c r="G29" s="259"/>
     </row>
     <row r="30" spans="1:7" ht="15.75">
       <c r="A30" s="99"/>
-      <c r="B30" s="221" t="s">
+      <c r="B30" s="257" t="s">
         <v>914</v>
       </c>
-      <c r="C30" s="222"/>
-      <c r="D30" s="223" t="s">
+      <c r="C30" s="258"/>
+      <c r="D30" s="260" t="s">
         <v>915</v>
       </c>
-      <c r="E30" s="223"/>
-      <c r="F30" s="223"/>
-      <c r="G30" s="224"/>
+      <c r="E30" s="260"/>
+      <c r="F30" s="260"/>
+      <c r="G30" s="261"/>
     </row>
     <row r="31" spans="1:7" ht="15.75">
       <c r="A31" s="99"/>
-      <c r="B31" s="221" t="s">
+      <c r="B31" s="257" t="s">
         <v>912</v>
       </c>
-      <c r="C31" s="222"/>
+      <c r="C31" s="258"/>
       <c r="D31" s="225" t="s">
         <v>913</v>
       </c>
       <c r="E31" s="225"/>
       <c r="F31" s="225"/>
-      <c r="G31" s="226"/>
+      <c r="G31" s="259"/>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickBot="1">
       <c r="A32" s="99"/>
-      <c r="B32" s="221" t="s">
+      <c r="B32" s="257" t="s">
         <v>928</v>
       </c>
-      <c r="C32" s="222"/>
+      <c r="C32" s="258"/>
       <c r="D32" s="225" t="s">
         <v>929</v>
       </c>
       <c r="E32" s="225"/>
       <c r="F32" s="225"/>
-      <c r="G32" s="226"/>
+      <c r="G32" s="259"/>
     </row>
     <row r="33" spans="1:7" ht="15.75">
       <c r="A33" s="98" t="s">
         <v>918</v>
       </c>
-      <c r="B33" s="227" t="s">
+      <c r="B33" s="238" t="s">
         <v>919</v>
       </c>
-      <c r="C33" s="228"/>
-      <c r="D33" s="228"/>
-      <c r="E33" s="228"/>
-      <c r="F33" s="228"/>
-      <c r="G33" s="229"/>
+      <c r="C33" s="239"/>
+      <c r="D33" s="239"/>
+      <c r="E33" s="239"/>
+      <c r="F33" s="239"/>
+      <c r="G33" s="240"/>
     </row>
     <row r="34" spans="1:7" ht="15.75">
       <c r="A34" s="99"/>
-      <c r="B34" s="221" t="s">
+      <c r="B34" s="257" t="s">
         <v>920</v>
       </c>
-      <c r="C34" s="222"/>
-      <c r="D34" s="223" t="s">
+      <c r="C34" s="258"/>
+      <c r="D34" s="260" t="s">
         <v>925</v>
       </c>
-      <c r="E34" s="223"/>
-      <c r="F34" s="223"/>
-      <c r="G34" s="224"/>
+      <c r="E34" s="260"/>
+      <c r="F34" s="260"/>
+      <c r="G34" s="261"/>
     </row>
     <row r="35" spans="1:7" ht="15.75">
       <c r="A35" s="99"/>
-      <c r="B35" s="221" t="s">
+      <c r="B35" s="257" t="s">
         <v>921</v>
       </c>
-      <c r="C35" s="222"/>
-      <c r="D35" s="223" t="s">
+      <c r="C35" s="258"/>
+      <c r="D35" s="260" t="s">
         <v>926</v>
       </c>
-      <c r="E35" s="223"/>
-      <c r="F35" s="223"/>
-      <c r="G35" s="224"/>
+      <c r="E35" s="260"/>
+      <c r="F35" s="260"/>
+      <c r="G35" s="261"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" thickBot="1">
       <c r="A36" s="99"/>
-      <c r="B36" s="221" t="s">
+      <c r="B36" s="257" t="s">
         <v>922</v>
       </c>
-      <c r="C36" s="222"/>
-      <c r="D36" s="223" t="s">
+      <c r="C36" s="258"/>
+      <c r="D36" s="260" t="s">
         <v>927</v>
       </c>
-      <c r="E36" s="223"/>
-      <c r="F36" s="223"/>
-      <c r="G36" s="224"/>
+      <c r="E36" s="260"/>
+      <c r="F36" s="260"/>
+      <c r="G36" s="261"/>
     </row>
     <row r="37" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="A37" s="98" t="s">
         <v>923</v>
       </c>
-      <c r="B37" s="227" t="s">
+      <c r="B37" s="238" t="s">
         <v>924</v>
       </c>
-      <c r="C37" s="228"/>
-      <c r="D37" s="228"/>
-      <c r="E37" s="228"/>
-      <c r="F37" s="228"/>
-      <c r="G37" s="229"/>
+      <c r="C37" s="239"/>
+      <c r="D37" s="239"/>
+      <c r="E37" s="239"/>
+      <c r="F37" s="239"/>
+      <c r="G37" s="240"/>
     </row>
     <row r="38" spans="1:7" ht="29.1" customHeight="1">
-      <c r="A38" s="248" t="s">
+      <c r="A38" s="235" t="s">
         <v>517</v>
       </c>
-      <c r="B38" s="227" t="s">
+      <c r="B38" s="238" t="s">
         <v>490</v>
       </c>
-      <c r="C38" s="228"/>
-      <c r="D38" s="228"/>
-      <c r="E38" s="228"/>
-      <c r="F38" s="228"/>
-      <c r="G38" s="229"/>
+      <c r="C38" s="239"/>
+      <c r="D38" s="239"/>
+      <c r="E38" s="239"/>
+      <c r="F38" s="239"/>
+      <c r="G38" s="240"/>
     </row>
     <row r="39" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A39" s="249"/>
-      <c r="B39" s="251"/>
-      <c r="C39" s="252"/>
-      <c r="D39" s="252"/>
-      <c r="E39" s="252"/>
-      <c r="F39" s="252"/>
-      <c r="G39" s="253"/>
+      <c r="A39" s="236"/>
+      <c r="B39" s="241"/>
+      <c r="C39" s="242"/>
+      <c r="D39" s="242"/>
+      <c r="E39" s="242"/>
+      <c r="F39" s="242"/>
+      <c r="G39" s="243"/>
     </row>
     <row r="40" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A40" s="249"/>
-      <c r="B40" s="254" t="s">
+      <c r="A40" s="236"/>
+      <c r="B40" s="244" t="s">
         <v>491</v>
       </c>
-      <c r="C40" s="255"/>
-      <c r="D40" s="255"/>
-      <c r="E40" s="255"/>
-      <c r="F40" s="255"/>
-      <c r="G40" s="256"/>
+      <c r="C40" s="245"/>
+      <c r="D40" s="245"/>
+      <c r="E40" s="245"/>
+      <c r="F40" s="245"/>
+      <c r="G40" s="246"/>
     </row>
     <row r="41" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A41" s="249"/>
-      <c r="B41" s="257" t="s">
+      <c r="A41" s="236"/>
+      <c r="B41" s="224" t="s">
         <v>492</v>
       </c>
       <c r="C41" s="225"/>
       <c r="D41" s="225"/>
       <c r="E41" s="225"/>
       <c r="F41" s="225"/>
-      <c r="G41" s="258"/>
+      <c r="G41" s="226"/>
     </row>
     <row r="42" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A42" s="249"/>
-      <c r="B42" s="251"/>
-      <c r="C42" s="252"/>
-      <c r="D42" s="252"/>
-      <c r="E42" s="252"/>
-      <c r="F42" s="252"/>
-      <c r="G42" s="253"/>
+      <c r="A42" s="236"/>
+      <c r="B42" s="241"/>
+      <c r="C42" s="242"/>
+      <c r="D42" s="242"/>
+      <c r="E42" s="242"/>
+      <c r="F42" s="242"/>
+      <c r="G42" s="243"/>
     </row>
     <row r="43" spans="1:7" ht="42.95" customHeight="1">
-      <c r="A43" s="249"/>
-      <c r="B43" s="257" t="s">
+      <c r="A43" s="236"/>
+      <c r="B43" s="224" t="s">
         <v>493</v>
       </c>
       <c r="C43" s="225"/>
       <c r="D43" s="225"/>
       <c r="E43" s="225"/>
       <c r="F43" s="225"/>
-      <c r="G43" s="258"/>
+      <c r="G43" s="226"/>
     </row>
     <row r="44" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A44" s="249"/>
-      <c r="B44" s="251"/>
-      <c r="C44" s="252"/>
-      <c r="D44" s="252"/>
-      <c r="E44" s="252"/>
-      <c r="F44" s="252"/>
-      <c r="G44" s="253"/>
+      <c r="A44" s="236"/>
+      <c r="B44" s="241"/>
+      <c r="C44" s="242"/>
+      <c r="D44" s="242"/>
+      <c r="E44" s="242"/>
+      <c r="F44" s="242"/>
+      <c r="G44" s="243"/>
     </row>
     <row r="45" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A45" s="249"/>
-      <c r="B45" s="257" t="s">
+      <c r="A45" s="236"/>
+      <c r="B45" s="224" t="s">
         <v>494</v>
       </c>
       <c r="C45" s="225"/>
       <c r="D45" s="225"/>
       <c r="E45" s="225"/>
       <c r="F45" s="225"/>
-      <c r="G45" s="258"/>
+      <c r="G45" s="226"/>
     </row>
     <row r="46" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A46" s="249"/>
-      <c r="B46" s="257" t="s">
+      <c r="A46" s="236"/>
+      <c r="B46" s="224" t="s">
         <v>495</v>
       </c>
       <c r="C46" s="225"/>
       <c r="D46" s="225"/>
       <c r="E46" s="225"/>
       <c r="F46" s="225"/>
-      <c r="G46" s="258"/>
+      <c r="G46" s="226"/>
     </row>
     <row r="47" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A47" s="249"/>
-      <c r="B47" s="257" t="s">
+      <c r="A47" s="236"/>
+      <c r="B47" s="224" t="s">
         <v>496</v>
       </c>
       <c r="C47" s="225"/>
       <c r="D47" s="225"/>
       <c r="E47" s="225"/>
       <c r="F47" s="225"/>
-      <c r="G47" s="258"/>
+      <c r="G47" s="226"/>
     </row>
     <row r="48" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A48" s="249"/>
-      <c r="B48" s="257" t="s">
+      <c r="A48" s="236"/>
+      <c r="B48" s="224" t="s">
         <v>497</v>
       </c>
       <c r="C48" s="225"/>
       <c r="D48" s="225"/>
       <c r="E48" s="225"/>
       <c r="F48" s="225"/>
-      <c r="G48" s="258"/>
+      <c r="G48" s="226"/>
     </row>
     <row r="49" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A49" s="249"/>
-      <c r="B49" s="257" t="s">
+      <c r="A49" s="236"/>
+      <c r="B49" s="224" t="s">
         <v>498</v>
       </c>
       <c r="C49" s="225"/>
       <c r="D49" s="225"/>
       <c r="E49" s="225"/>
       <c r="F49" s="225"/>
-      <c r="G49" s="258"/>
+      <c r="G49" s="226"/>
     </row>
     <row r="50" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A50" s="249"/>
-      <c r="B50" s="257" t="s">
+      <c r="A50" s="236"/>
+      <c r="B50" s="224" t="s">
         <v>499</v>
       </c>
       <c r="C50" s="225"/>
       <c r="D50" s="225"/>
       <c r="E50" s="225"/>
       <c r="F50" s="225"/>
-      <c r="G50" s="258"/>
+      <c r="G50" s="226"/>
     </row>
     <row r="51" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A51" s="249"/>
-      <c r="B51" s="257" t="s">
+      <c r="A51" s="236"/>
+      <c r="B51" s="224" t="s">
         <v>500</v>
       </c>
       <c r="C51" s="225"/>
       <c r="D51" s="225"/>
       <c r="E51" s="225"/>
       <c r="F51" s="225"/>
-      <c r="G51" s="258"/>
+      <c r="G51" s="226"/>
     </row>
     <row r="52" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A52" s="250"/>
-      <c r="B52" s="259" t="s">
+      <c r="A52" s="237"/>
+      <c r="B52" s="227" t="s">
         <v>501</v>
       </c>
-      <c r="C52" s="260"/>
-      <c r="D52" s="260"/>
-      <c r="E52" s="260"/>
-      <c r="F52" s="260"/>
-      <c r="G52" s="261"/>
+      <c r="C52" s="228"/>
+      <c r="D52" s="228"/>
+      <c r="E52" s="228"/>
+      <c r="F52" s="228"/>
+      <c r="G52" s="229"/>
     </row>
     <row r="53" spans="1:7" ht="57.95" customHeight="1" thickBot="1">
       <c r="A53" s="10" t="s">
         <v>516</v>
       </c>
-      <c r="B53" s="230" t="s">
+      <c r="B53" s="221" t="s">
         <v>581</v>
       </c>
-      <c r="C53" s="231"/>
-      <c r="D53" s="231"/>
-      <c r="E53" s="231"/>
-      <c r="F53" s="231"/>
-      <c r="G53" s="232"/>
+      <c r="C53" s="222"/>
+      <c r="D53" s="222"/>
+      <c r="E53" s="222"/>
+      <c r="F53" s="222"/>
+      <c r="G53" s="223"/>
     </row>
     <row r="54" spans="1:7" ht="57.95" customHeight="1" thickBot="1">
       <c r="A54" s="10" t="s">
         <v>515</v>
       </c>
-      <c r="B54" s="230" t="s">
+      <c r="B54" s="221" t="s">
         <v>502</v>
       </c>
-      <c r="C54" s="231"/>
-      <c r="D54" s="231"/>
-      <c r="E54" s="231"/>
-      <c r="F54" s="231"/>
-      <c r="G54" s="232"/>
+      <c r="C54" s="222"/>
+      <c r="D54" s="222"/>
+      <c r="E54" s="222"/>
+      <c r="F54" s="222"/>
+      <c r="G54" s="223"/>
     </row>
     <row r="55" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A55" s="10" t="s">
         <v>514</v>
       </c>
-      <c r="B55" s="230" t="s">
+      <c r="B55" s="221" t="s">
         <v>503</v>
       </c>
-      <c r="C55" s="231"/>
-      <c r="D55" s="231"/>
-      <c r="E55" s="231"/>
-      <c r="F55" s="231"/>
-      <c r="G55" s="232"/>
+      <c r="C55" s="222"/>
+      <c r="D55" s="222"/>
+      <c r="E55" s="222"/>
+      <c r="F55" s="222"/>
+      <c r="G55" s="223"/>
     </row>
     <row r="56" spans="1:7" ht="42.95" customHeight="1" thickBot="1">
       <c r="A56" s="11" t="s">
         <v>508</v>
       </c>
-      <c r="B56" s="230" t="s">
+      <c r="B56" s="221" t="s">
         <v>504</v>
       </c>
-      <c r="C56" s="231"/>
-      <c r="D56" s="231"/>
-      <c r="E56" s="231"/>
-      <c r="F56" s="231"/>
-      <c r="G56" s="232"/>
+      <c r="C56" s="222"/>
+      <c r="D56" s="222"/>
+      <c r="E56" s="222"/>
+      <c r="F56" s="222"/>
+      <c r="G56" s="223"/>
     </row>
     <row r="57" spans="1:7" ht="29.1" customHeight="1" thickBot="1">
       <c r="A57" s="10" t="s">
         <v>513</v>
       </c>
-      <c r="B57" s="230" t="s">
+      <c r="B57" s="221" t="s">
         <v>505</v>
       </c>
-      <c r="C57" s="231"/>
-      <c r="D57" s="231"/>
-      <c r="E57" s="231"/>
-      <c r="F57" s="231"/>
-      <c r="G57" s="232"/>
+      <c r="C57" s="222"/>
+      <c r="D57" s="222"/>
+      <c r="E57" s="222"/>
+      <c r="F57" s="222"/>
+      <c r="G57" s="223"/>
     </row>
     <row r="58" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A58" s="10" t="s">
         <v>512</v>
       </c>
-      <c r="B58" s="230" t="s">
+      <c r="B58" s="221" t="s">
         <v>506</v>
       </c>
-      <c r="C58" s="231"/>
-      <c r="D58" s="231"/>
-      <c r="E58" s="231"/>
-      <c r="F58" s="231"/>
-      <c r="G58" s="232"/>
+      <c r="C58" s="222"/>
+      <c r="D58" s="222"/>
+      <c r="E58" s="222"/>
+      <c r="F58" s="222"/>
+      <c r="G58" s="223"/>
     </row>
     <row r="59" spans="1:7" ht="42.95" customHeight="1" thickBot="1">
       <c r="A59" s="11" t="s">
         <v>509</v>
       </c>
-      <c r="B59" s="230" t="s">
+      <c r="B59" s="221" t="s">
         <v>510</v>
       </c>
-      <c r="C59" s="231"/>
-      <c r="D59" s="231"/>
-      <c r="E59" s="231"/>
-      <c r="F59" s="231"/>
-      <c r="G59" s="232"/>
+      <c r="C59" s="222"/>
+      <c r="D59" s="222"/>
+      <c r="E59" s="222"/>
+      <c r="F59" s="222"/>
+      <c r="G59" s="223"/>
     </row>
     <row r="60" spans="1:7" ht="29.1" customHeight="1" thickBot="1">
       <c r="A60" s="10" t="s">
         <v>511</v>
       </c>
-      <c r="B60" s="230" t="s">
+      <c r="B60" s="221" t="s">
         <v>507</v>
       </c>
-      <c r="C60" s="231"/>
-      <c r="D60" s="231"/>
-      <c r="E60" s="231"/>
-      <c r="F60" s="231"/>
-      <c r="G60" s="232"/>
+      <c r="C60" s="222"/>
+      <c r="D60" s="222"/>
+      <c r="E60" s="222"/>
+      <c r="F60" s="222"/>
+      <c r="G60" s="223"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:G59"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B53:G53"/>
-    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B20:G20"/>
@@ -41777,49 +41809,17 @@
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="B48:G48"/>
     <mergeCell ref="B49:G49"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:G36"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:G35"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B59:G59"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -41830,8 +41830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -42043,10 +42043,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="232" t="s">
         <v>485</v>
       </c>
-      <c r="B10" s="237"/>
+      <c r="B10" s="234"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -42292,10 +42292,10 @@
       <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A23" s="235" t="s">
+      <c r="A23" s="232" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="237"/>
+      <c r="B23" s="234"/>
       <c r="C23" s="4" t="s">
         <v>63</v>
       </c>
@@ -42598,10 +42598,10 @@
       <c r="G38" s="11"/>
     </row>
     <row r="39" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A39" s="235" t="s">
+      <c r="A39" s="232" t="s">
         <v>524</v>
       </c>
-      <c r="B39" s="237"/>
+      <c r="B39" s="234"/>
       <c r="C39" s="4" t="s">
         <v>63</v>
       </c>
@@ -42714,10 +42714,10 @@
       <c r="G44" s="11"/>
     </row>
     <row r="45" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A45" s="235" t="s">
+      <c r="A45" s="232" t="s">
         <v>529</v>
       </c>
-      <c r="B45" s="237"/>
+      <c r="B45" s="234"/>
       <c r="C45" s="4" t="s">
         <v>63</v>
       </c>
@@ -42849,10 +42849,10 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A52" s="235" t="s">
+      <c r="A52" s="232" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="237"/>
+      <c r="B52" s="234"/>
       <c r="C52" s="4" t="s">
         <v>63</v>
       </c>
@@ -43022,10 +43022,10 @@
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A61" s="235" t="s">
+      <c r="A61" s="232" t="s">
         <v>111</v>
       </c>
-      <c r="B61" s="237"/>
+      <c r="B61" s="234"/>
       <c r="C61" s="4" t="s">
         <v>63</v>
       </c>
@@ -43119,10 +43119,10 @@
       <c r="G65" s="11"/>
     </row>
     <row r="66" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A66" s="235" t="s">
+      <c r="A66" s="232" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="237"/>
+      <c r="B66" s="234"/>
       <c r="C66" s="4" t="s">
         <v>63</v>
       </c>
@@ -43410,10 +43410,10 @@
       <c r="G80" s="11"/>
     </row>
     <row r="81" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A81" s="235" t="s">
+      <c r="A81" s="232" t="s">
         <v>133</v>
       </c>
-      <c r="B81" s="237"/>
+      <c r="B81" s="234"/>
       <c r="C81" s="4" t="s">
         <v>63</v>
       </c>
@@ -43547,10 +43547,10 @@
       <c r="G87" s="11"/>
     </row>
     <row r="88" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A88" s="235" t="s">
+      <c r="A88" s="232" t="s">
         <v>558</v>
       </c>
-      <c r="B88" s="237"/>
+      <c r="B88" s="234"/>
       <c r="C88" s="4" t="s">
         <v>63</v>
       </c>
@@ -43665,10 +43665,10 @@
       <c r="G93" s="11"/>
     </row>
     <row r="94" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A94" s="235" t="s">
+      <c r="A94" s="232" t="s">
         <v>156</v>
       </c>
-      <c r="B94" s="237"/>
+      <c r="B94" s="234"/>
       <c r="C94" s="4" t="s">
         <v>63</v>
       </c>
@@ -43743,10 +43743,10 @@
       <c r="G97" s="11"/>
     </row>
     <row r="98" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A98" s="235" t="s">
+      <c r="A98" s="232" t="s">
         <v>150</v>
       </c>
-      <c r="B98" s="237"/>
+      <c r="B98" s="234"/>
       <c r="C98" s="4" t="s">
         <v>63</v>
       </c>
@@ -43821,10 +43821,10 @@
       <c r="G101" s="11"/>
     </row>
     <row r="102" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A102" s="235" t="s">
+      <c r="A102" s="232" t="s">
         <v>547</v>
       </c>
-      <c r="B102" s="237"/>
+      <c r="B102" s="234"/>
       <c r="C102" s="4" t="s">
         <v>63</v>
       </c>
@@ -43920,10 +43920,10 @@
       <c r="G106" s="11"/>
     </row>
     <row r="107" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A107" s="235" t="s">
+      <c r="A107" s="232" t="s">
         <v>140</v>
       </c>
-      <c r="B107" s="237"/>
+      <c r="B107" s="234"/>
       <c r="C107" s="4" t="s">
         <v>63</v>
       </c>
@@ -44074,10 +44074,10 @@
       <c r="G114" s="11"/>
     </row>
     <row r="115" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A115" s="235" t="s">
+      <c r="A115" s="232" t="s">
         <v>161</v>
       </c>
-      <c r="B115" s="237"/>
+      <c r="B115" s="234"/>
       <c r="C115" s="4" t="s">
         <v>453</v>
       </c>
@@ -44248,14 +44248,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A88:B88"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="C2:D9"/>
@@ -44265,6 +44257,14 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A88:B88"/>
   </mergeCells>
   <conditionalFormatting sqref="A11:A18 A107:A109 A81:A85 A115:A248 A52:A57 A40 A33:A37 A42:A43 A112 A94:A100 A61:A69 A59 A20:A29">
     <cfRule type="beginsWith" dxfId="2421" priority="1148" stopIfTrue="1" operator="beginsWith" text="Exceptional">
@@ -46500,7 +46500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A91" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -46713,10 +46713,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="232" t="s">
         <v>701</v>
       </c>
-      <c r="B10" s="237"/>
+      <c r="B10" s="234"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -47002,10 +47002,10 @@
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A25" s="235" t="s">
+      <c r="A25" s="232" t="s">
         <v>688</v>
       </c>
-      <c r="B25" s="237"/>
+      <c r="B25" s="234"/>
       <c r="C25" s="4" t="s">
         <v>63</v>
       </c>
@@ -47213,10 +47213,10 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A36" s="235" t="s">
+      <c r="A36" s="232" t="s">
         <v>612</v>
       </c>
-      <c r="B36" s="237"/>
+      <c r="B36" s="234"/>
       <c r="C36" s="4" t="s">
         <v>63</v>
       </c>
@@ -47635,10 +47635,10 @@
       <c r="G57" s="11"/>
     </row>
     <row r="58" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A58" s="235" t="s">
+      <c r="A58" s="232" t="s">
         <v>627</v>
       </c>
-      <c r="B58" s="237"/>
+      <c r="B58" s="234"/>
       <c r="C58" s="4" t="s">
         <v>63</v>
       </c>
@@ -47941,10 +47941,10 @@
       <c r="G73" s="11"/>
     </row>
     <row r="74" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A74" s="235" t="s">
+      <c r="A74" s="232" t="s">
         <v>651</v>
       </c>
-      <c r="B74" s="237"/>
+      <c r="B74" s="234"/>
       <c r="C74" s="4" t="s">
         <v>63</v>
       </c>
@@ -48133,10 +48133,10 @@
       <c r="G83" s="11"/>
     </row>
     <row r="84" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A84" s="235" t="s">
+      <c r="A84" s="232" t="s">
         <v>663</v>
       </c>
-      <c r="B84" s="237"/>
+      <c r="B84" s="234"/>
       <c r="C84" s="21" t="s">
         <v>456</v>
       </c>
@@ -48496,10 +48496,10 @@
       <c r="G102" s="11"/>
     </row>
     <row r="103" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A103" s="235" t="s">
+      <c r="A103" s="232" t="s">
         <v>677</v>
       </c>
-      <c r="B103" s="237"/>
+      <c r="B103" s="234"/>
       <c r="C103" s="4" t="s">
         <v>63</v>
       </c>
@@ -51669,10 +51669,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="232" t="s">
         <v>291</v>
       </c>
-      <c r="B10" s="237"/>
+      <c r="B10" s="234"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -52032,10 +52032,10 @@
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A29" s="235" t="s">
+      <c r="A29" s="232" t="s">
         <v>564</v>
       </c>
-      <c r="B29" s="237"/>
+      <c r="B29" s="234"/>
       <c r="C29" s="4" t="s">
         <v>451</v>
       </c>
@@ -52264,10 +52264,10 @@
       <c r="G40" s="11"/>
     </row>
     <row r="41" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A41" s="235" t="s">
+      <c r="A41" s="232" t="s">
         <v>334</v>
       </c>
-      <c r="B41" s="237"/>
+      <c r="B41" s="234"/>
       <c r="C41" s="4" t="s">
         <v>63</v>
       </c>
@@ -52479,10 +52479,10 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" s="7" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A52" s="235" t="s">
+      <c r="A52" s="232" t="s">
         <v>84</v>
       </c>
-      <c r="B52" s="237"/>
+      <c r="B52" s="234"/>
       <c r="C52" s="4" t="s">
         <v>63</v>
       </c>
@@ -52652,10 +52652,10 @@
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" s="7" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A61" s="235" t="s">
+      <c r="A61" s="232" t="s">
         <v>370</v>
       </c>
-      <c r="B61" s="237"/>
+      <c r="B61" s="234"/>
       <c r="C61" s="21" t="s">
         <v>452</v>
       </c>
@@ -54005,10 +54005,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="232" t="s">
         <v>810</v>
       </c>
-      <c r="B10" s="237"/>
+      <c r="B10" s="234"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -54311,10 +54311,10 @@
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A26" s="235" t="s">
+      <c r="A26" s="232" t="s">
         <v>390</v>
       </c>
-      <c r="B26" s="237"/>
+      <c r="B26" s="234"/>
       <c r="C26" s="4" t="s">
         <v>855</v>
       </c>
@@ -54581,10 +54581,10 @@
       <c r="G39" s="11"/>
     </row>
     <row r="40" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A40" s="235" t="s">
+      <c r="A40" s="232" t="s">
         <v>448</v>
       </c>
-      <c r="B40" s="237"/>
+      <c r="B40" s="234"/>
       <c r="C40" s="102" t="s">
         <v>856</v>
       </c>
@@ -54849,10 +54849,10 @@
       <c r="G53" s="11"/>
     </row>
     <row r="54" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A54" s="235" t="s">
+      <c r="A54" s="232" t="s">
         <v>412</v>
       </c>
-      <c r="B54" s="237"/>
+      <c r="B54" s="234"/>
       <c r="C54" s="4" t="s">
         <v>63</v>
       </c>
@@ -56713,10 +56713,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="232" t="s">
         <v>239</v>
       </c>
-      <c r="B10" s="237"/>
+      <c r="B10" s="234"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -56810,10 +56810,10 @@
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A15" s="235" t="s">
+      <c r="A15" s="232" t="s">
         <v>246</v>
       </c>
-      <c r="B15" s="237"/>
+      <c r="B15" s="234"/>
       <c r="C15" s="4" t="s">
         <v>874</v>
       </c>
@@ -56926,10 +56926,10 @@
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A21" s="235" t="s">
+      <c r="A21" s="232" t="s">
         <v>878</v>
       </c>
-      <c r="B21" s="237"/>
+      <c r="B21" s="234"/>
       <c r="C21" s="4" t="s">
         <v>63</v>
       </c>
@@ -57061,10 +57061,10 @@
       <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A28" s="235" t="s">
+      <c r="A28" s="232" t="s">
         <v>254</v>
       </c>
-      <c r="B28" s="237"/>
+      <c r="B28" s="234"/>
       <c r="C28" s="4" t="s">
         <v>875</v>
       </c>
@@ -57217,10 +57217,10 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A36" s="235" t="s">
+      <c r="A36" s="232" t="s">
         <v>891</v>
       </c>
-      <c r="B36" s="237"/>
+      <c r="B36" s="234"/>
       <c r="C36" s="4" t="s">
         <v>454</v>
       </c>
@@ -57352,10 +57352,10 @@
       <c r="G42" s="11"/>
     </row>
     <row r="43" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A43" s="235" t="s">
+      <c r="A43" s="232" t="s">
         <v>275</v>
       </c>
-      <c r="B43" s="237"/>
+      <c r="B43" s="234"/>
       <c r="C43" s="4" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Added cheat codes for skipping levels and giving yourself items.
</commit_message>
<xml_diff>
--- a/GameDocuments/gam352_papercut_rubric.xlsx
+++ b/GameDocuments/gam352_papercut_rubric.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Game Data" sheetId="1" r:id="rId1"/>
@@ -46503,7 +46503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
       <selection activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
@@ -53797,7 +53797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added options menu to the main menu for a cleaner look.  Updated rubric.
</commit_message>
<xml_diff>
--- a/GameDocuments/gam352_papercut_rubric.xlsx
+++ b/GameDocuments/gam352_papercut_rubric.xlsx
@@ -21,7 +21,7 @@
     <sheet name="AUDIO" sheetId="8" r:id="rId7"/>
     <sheet name="NARRATIVE" sheetId="6" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2311" uniqueCount="972">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2318" uniqueCount="978">
   <si>
     <t>GAME NAME</t>
   </si>
@@ -3670,37 +3670,56 @@
     <t xml:space="preserve">Unity </t>
   </si>
   <si>
-    <t xml:space="preserve">Pressing 0-9 skips to different levels in the game </t>
-  </si>
-  <si>
     <t xml:space="preserve">Tested on my laptop with integrated graphics card.  Runs at resonable framerate on normal quality </t>
   </si>
   <si>
+    <t>Unity Launcher</t>
+  </si>
+  <si>
+    <t>Machine explosion</t>
+  </si>
+  <si>
+    <t>No defeate state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No hud elements </t>
+  </si>
+  <si>
+    <t>Take your pick</t>
+  </si>
+  <si>
+    <t>Transformation sequence</t>
+  </si>
+  <si>
+    <t>Dynamic teaching in player house.</t>
+  </si>
+  <si>
+    <t>Pressing 0-9 skips to different levels in the game.
+Pressing the enter key gives the player the two items they need to complete the game.</t>
+  </si>
+  <si>
+    <t>Pressing the ~ key activates autoplay</t>
+  </si>
+  <si>
     <t>Windows 7,8,10 -
- Windows 7 school computer
+Windows 7 Lab machine
 Windows 8 laptop
 Windows 10 laptop</t>
   </si>
   <si>
-    <t>Unity Launcher</t>
-  </si>
-  <si>
-    <t>Machine explosion</t>
-  </si>
-  <si>
-    <t>No defeate state</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No hud elements </t>
-  </si>
-  <si>
-    <t>Take your pick</t>
-  </si>
-  <si>
-    <t>Transformation sequence</t>
-  </si>
-  <si>
-    <t>Dynamic teaching in player house.</t>
+    <t>Ending</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discovery, Catharsis, Sensation </t>
+  </si>
+  <si>
+    <t>Rocket credits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End Credits theme </t>
+  </si>
+  <si>
+    <t>Presented in humerous way</t>
   </si>
 </sst>
 </file>
@@ -39405,7 +39424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -39582,7 +39601,7 @@
       <c r="C8" s="97"/>
       <c r="D8" s="219">
         <f>E17+E26+E35+E44+E53</f>
-        <v>0.18875000000000003</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E8" s="220"/>
       <c r="F8" s="5"/>
@@ -39755,11 +39774,11 @@
       <c r="C14" s="36"/>
       <c r="D14" s="39">
         <f>TECH!$E$7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E14" s="47">
         <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
+        <v>0.03</v>
       </c>
       <c r="F14" s="43"/>
       <c r="G14" s="39">
@@ -39808,7 +39827,7 @@
       </c>
       <c r="J15" s="188">
         <f>MAX(0,MIN(1,IF($J17 &lt;= 0.95, ROUND($J17,2), FLOOR((0.95+($J17-0.95)/5),0.01))))</f>
-        <v>0.78</v>
+        <v>0.83</v>
       </c>
       <c r="L15" s="188">
         <f>MAX(0,MIN(1,IF($L17 &lt;= 0.95, ROUND($L17,2), FLOOR((0.95+($L17-0.95)/5),0.01))))</f>
@@ -39857,7 +39876,7 @@
       </c>
       <c r="E17" s="41">
         <f>SUM(E11:E16)</f>
-        <v>1.8750000000000003E-2</v>
+        <v>2.3749999999999997E-2</v>
       </c>
       <c r="F17" s="43"/>
       <c r="G17" s="22" t="s">
@@ -39869,7 +39888,7 @@
       </c>
       <c r="J17" s="87">
         <f>$A$7+$E17+IF($D$8-$E17 &gt; 0, ($D$8-$E17)/2, $D$8-$E17)+$G$5</f>
-        <v>0.78375000000000017</v>
+        <v>0.83187500000000014</v>
       </c>
       <c r="L17" s="87">
         <f>$A$7+$H17+IF($G$8 &gt; 0, ($G$8-$H17)/2, $G$8-$H17)+$G$5</f>
@@ -39996,11 +40015,11 @@
       <c r="C22" s="35"/>
       <c r="D22" s="39">
         <f>DESIGN!$E$4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="47">
         <f t="shared" si="2"/>
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="F22" s="43"/>
       <c r="G22" s="39">
@@ -40027,11 +40046,11 @@
       <c r="C23" s="36"/>
       <c r="D23" s="39">
         <f>DESIGN!$E$7</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E23" s="47">
         <f t="shared" si="2"/>
-        <v>3.5000000000000003E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F23" s="43"/>
       <c r="G23" s="39">
@@ -40062,11 +40081,11 @@
       <c r="C24" s="37"/>
       <c r="D24" s="39">
         <f>DESIGN!$E$8</f>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E24" s="47">
         <f t="shared" si="2"/>
-        <v>1.4999999999999999E-2</v>
+        <v>1.8749999999999999E-2</v>
       </c>
       <c r="F24" s="43"/>
       <c r="G24" s="39">
@@ -40079,7 +40098,7 @@
       </c>
       <c r="J24" s="188">
         <f>MAX(0,MIN(1,IF($J26 &lt;= 0.95, ROUND($J26,2), FLOOR((0.95+($J26-0.95)/5),0.01))))</f>
-        <v>0.78</v>
+        <v>0.86</v>
       </c>
       <c r="L24" s="188">
         <f>MAX(0,MIN(1,IF($L26 &lt;= 0.95, ROUND($L26,2), FLOOR((0.95+($L26-0.95)/5),0.01))))</f>
@@ -40098,11 +40117,11 @@
       <c r="C25" s="35"/>
       <c r="D25" s="40">
         <f>DESIGN!$E$9</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25" s="48">
         <f t="shared" si="2"/>
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="F25" s="43"/>
       <c r="G25" s="40">
@@ -40126,7 +40145,7 @@
       </c>
       <c r="E26" s="41">
         <f>SUM(E20:E25)</f>
-        <v>0.05</v>
+        <v>8.8750000000000009E-2</v>
       </c>
       <c r="F26" s="43"/>
       <c r="G26" s="22" t="s">
@@ -40138,7 +40157,7 @@
       </c>
       <c r="J26" s="87">
         <f>$A$7+MIN(MAX($E26*2,$E26),$D$8)</f>
-        <v>0.78</v>
+        <v>0.85750000000000004</v>
       </c>
       <c r="L26" s="87">
         <f>$A$7+MIN(MAX($H26*2,$H26),$G$8)+$G$5</f>
@@ -40230,11 +40249,11 @@
       <c r="C30" s="35"/>
       <c r="D30" s="39">
         <f>ART!$E$3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" s="47">
         <f t="shared" si="4"/>
-        <v>-0.02</v>
+        <v>0</v>
       </c>
       <c r="F30" s="43"/>
       <c r="G30" s="39">
@@ -40290,11 +40309,11 @@
       <c r="C32" s="36"/>
       <c r="D32" s="39">
         <f>ART!$E$7</f>
-        <v>5</v>
+        <v>6.5</v>
       </c>
       <c r="E32" s="47">
         <f t="shared" si="4"/>
-        <v>2.5000000000000001E-2</v>
+        <v>3.2500000000000001E-2</v>
       </c>
       <c r="F32" s="43"/>
       <c r="G32" s="39">
@@ -40341,7 +40360,7 @@
       </c>
       <c r="J33" s="188">
         <f>MAX(0,MIN(1,IF($J35 &lt;= 0.95, ROUND($J35,2), FLOOR((0.95+($J35-0.95)/5),0.01))))</f>
-        <v>0.82</v>
+        <v>0.88</v>
       </c>
       <c r="L33" s="188">
         <f>MAX(0,MIN(1,IF($L35 &lt;= 0.95, ROUND($L35,2), FLOOR((0.95+($L35-0.95)/5),0.01))))</f>
@@ -40386,7 +40405,7 @@
       </c>
       <c r="E35" s="41">
         <f>SUM(E29:E34)</f>
-        <v>7.0000000000000007E-2</v>
+        <v>9.7500000000000003E-2</v>
       </c>
       <c r="F35" s="43"/>
       <c r="G35" s="22" t="s">
@@ -40398,7 +40417,7 @@
       </c>
       <c r="J35" s="87">
         <f>$A$7+MIN(MAX($E35*2,$E35),$D$8)</f>
-        <v>0.82000000000000006</v>
+        <v>0.875</v>
       </c>
       <c r="L35" s="87">
         <f>$A$7+MIN(MAX($H35*2,$H35),$G$8)+$G$5</f>
@@ -40489,11 +40508,11 @@
       <c r="C39" s="35"/>
       <c r="D39" s="39">
         <f>AUDIO!$E$3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39" s="47">
         <f t="shared" si="6"/>
-        <v>-0.02</v>
+        <v>0</v>
       </c>
       <c r="F39" s="43"/>
       <c r="G39" s="39">
@@ -40600,7 +40619,7 @@
       </c>
       <c r="J42" s="188">
         <f>MAX(0,MIN(1,IF($J44 &lt;= 0.95, ROUND($J44,2), FLOOR((0.95+($J44-0.95)/5),0.01))))</f>
-        <v>0.69</v>
+        <v>0.73</v>
       </c>
       <c r="L42" s="188">
         <f>MAX(0,MIN(1,IF($L44 &lt;= 0.95, ROUND($L44,2), FLOOR((0.95+($L44-0.95)/5),0.01))))</f>
@@ -40645,7 +40664,7 @@
       </c>
       <c r="E44" s="41">
         <f>SUM(E38:E43)</f>
-        <v>2.4999999999999988E-3</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="22" t="s">
@@ -40657,7 +40676,7 @@
       </c>
       <c r="J44" s="87">
         <f>$A$7+MIN(MAX($E44*2,$E44),$D$8)</f>
-        <v>0.68500000000000005</v>
+        <v>0.72500000000000009</v>
       </c>
       <c r="L44" s="87">
         <f>$A$7+MIN(MAX($H44*2,$H44),$G$8)+$G$5</f>
@@ -40935,7 +40954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -41833,8 +41852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -41972,7 +41991,7 @@
       <c r="D6" s="265"/>
       <c r="E6" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Advanced")*(E$10:E$247="Missing"))+0.5*SUMPRODUCT(($A$10:$A$247="Advanced")*(E$10:E$247="Partial"))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Advanced")*(F$10:F$247="Missing"))+0.5*SUMPRODUCT(($A$10:$A$247="Advanced")*(F$10:F$247="Partial"))</f>
@@ -41994,7 +42013,7 @@
       <c r="D7" s="265"/>
       <c r="E7" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Advanced")*(E$10:E$247="Completed"))+SUMPRODUCT(($A$10:$A$247="Advanced")*(E$10:E$247="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$247="Advanced")*(E$10:E$247="Partial"))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F7" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Advanced")*(F$10:F$247="Completed"))+SUMPRODUCT(($A$10:$A$247="Advanced")*(F$10:F$247="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$247="Advanced")*(F$10:F$247="Partial"))</f>
@@ -43364,7 +43383,7 @@
         <v>751</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>58</v>
@@ -43384,9 +43403,11 @@
       <c r="C79" s="11" t="s">
         <v>750</v>
       </c>
-      <c r="D79" s="11"/>
+      <c r="D79" s="11" t="s">
+        <v>956</v>
+      </c>
       <c r="E79" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F79" s="4" t="s">
         <v>52</v>
@@ -43520,7 +43541,7 @@
         <v>746</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="E86" s="4" t="s">
         <v>58</v>
@@ -43581,7 +43602,7 @@
         <v>743</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>962</v>
+        <v>970</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>58</v>
@@ -43601,7 +43622,9 @@
       <c r="C90" s="11" t="s">
         <v>741</v>
       </c>
-      <c r="D90" s="11"/>
+      <c r="D90" s="11" t="s">
+        <v>971</v>
+      </c>
       <c r="E90" s="4" t="s">
         <v>58</v>
       </c>
@@ -43893,7 +43916,7 @@
         <v>737</v>
       </c>
       <c r="D105" s="11" t="s">
-        <v>964</v>
+        <v>972</v>
       </c>
       <c r="E105" s="4" t="s">
         <v>56</v>
@@ -46503,8 +46526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="E110" sqref="E110"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -46598,7 +46621,7 @@
       <c r="D4" s="265"/>
       <c r="E4" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Intermediate")*(E$10:E$209="Missing"))+0.5*SUMPRODUCT(($A$10:$A$209="Intermediate")*(E$10:E$209="Partial"))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Intermediate")*(F$10:F$209="Missing"))+0.5*SUMPRODUCT(($A$10:$A$209="Intermediate")*(F$10:F$209="Partial"))</f>
@@ -46620,7 +46643,7 @@
       <c r="D5" s="265"/>
       <c r="E5" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Intermediate")*(E$10:E$209="Completed"))+SUMPRODUCT(($A$10:$A$209="Intermediate")*(E$10:E$209="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$209="Intermediate")*(E$10:E$209="Partial"))</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F5" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Intermediate")*(F$10:F$209="Completed"))+SUMPRODUCT(($A$10:$A$209="Intermediate")*(F$10:F$209="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$209="Intermediate")*(F$10:F$209="Partial"))</f>
@@ -46642,7 +46665,7 @@
       <c r="D6" s="265"/>
       <c r="E6" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Advanced")*(E$10:E$209="Missing"))+0.5*SUMPRODUCT(($A$10:$A$209="Advanced")*(E$10:E$209="Partial"))</f>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F6" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Advanced")*(F$10:F$209="Missing"))+0.5*SUMPRODUCT(($A$10:$A$209="Advanced")*(F$10:F$209="Partial"))</f>
@@ -46664,7 +46687,7 @@
       <c r="D7" s="265"/>
       <c r="E7" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Advanced")*(E$10:E$209="Completed"))+SUMPRODUCT(($A$10:$A$209="Advanced")*(E$10:E$209="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$209="Advanced")*(E$10:E$209="Partial"))</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F7" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Advanced")*(F$10:F$209="Completed"))+SUMPRODUCT(($A$10:$A$209="Advanced")*(F$10:F$209="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$209="Advanced")*(F$10:F$209="Partial"))</f>
@@ -46684,7 +46707,7 @@
       <c r="D8" s="265"/>
       <c r="E8" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Professional")*(E$10:E$209="Completed"))+SUMPRODUCT(($A$10:$A$209="Professional")*(E$10:E$209="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$209="Professional")*(E$10:E$209="Partial"))</f>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="F8" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Professional")*(F$10:F$209="Completed"))+SUMPRODUCT(($A$10:$A$209="Professional")*(F$10:F$209="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$209="Professional")*(F$10:F$209="Partial"))</f>
@@ -46704,7 +46727,7 @@
       <c r="D9" s="267"/>
       <c r="E9" s="14">
         <f>SUMPRODUCT(($A$10:$A$208="Exceptional")*(E$10:E$208="Completed"))+SUMPRODUCT(($A$10:$A$208="Exceptional")*(E$10:E$208="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$208="Exceptional")*(E$10:E$208="Partial"))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="14">
         <f>SUMPRODUCT(($A$10:$A$208="Exceptional")*(F$10:F$208="Completed"))+SUMPRODUCT(($A$10:$A$208="Exceptional")*(F$10:F$208="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$208="Exceptional")*(F$10:F$208="Partial"))</f>
@@ -46956,7 +46979,7 @@
         <v>685</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>58</v>
@@ -47150,7 +47173,7 @@
         <v>695</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>58</v>
@@ -47824,7 +47847,7 @@
       </c>
       <c r="D67" s="11"/>
       <c r="E67" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F67" s="4" t="s">
         <v>52</v>
@@ -47860,9 +47883,11 @@
       <c r="C69" s="11" t="s">
         <v>478</v>
       </c>
-      <c r="D69" s="11"/>
+      <c r="D69" s="11" t="s">
+        <v>977</v>
+      </c>
       <c r="E69" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F69" s="4" t="s">
         <v>52</v>
@@ -48092,7 +48117,7 @@
       </c>
       <c r="D81" s="11"/>
       <c r="E81" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F81" s="4" t="s">
         <v>52</v>
@@ -48284,7 +48309,7 @@
       </c>
       <c r="D91" s="11"/>
       <c r="E91" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F91" s="4" t="s">
         <v>52</v>
@@ -48702,9 +48727,11 @@
       <c r="C113" s="11" t="s">
         <v>675</v>
       </c>
-      <c r="D113" s="11"/>
+      <c r="D113" s="11" t="s">
+        <v>974</v>
+      </c>
       <c r="E113" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F113" s="4" t="s">
         <v>52</v>
@@ -48779,7 +48806,7 @@
         <v>459</v>
       </c>
       <c r="D117" s="11" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="E117" s="4" t="s">
         <v>58</v>
@@ -48799,9 +48826,11 @@
       <c r="C118" s="11" t="s">
         <v>460</v>
       </c>
-      <c r="D118" s="11"/>
+      <c r="D118" s="11" t="s">
+        <v>973</v>
+      </c>
       <c r="E118" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F118" s="4" t="s">
         <v>52</v>
@@ -51461,8 +51490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -51534,7 +51563,7 @@
       <c r="D3" s="265"/>
       <c r="E3" s="14">
         <f>SUMPRODUCT(($A$10:$A$238="Basic")*(E$10:E$238="Missing"))+0.5*SUMPRODUCT(($A$10:$A$238="Basic")*(E$10:E$238="Partial"))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="14">
         <f>SUMPRODUCT(($A$10:$A$238="Basic")*(F$10:F$238="Missing"))+0.5*SUMPRODUCT(($A$10:$A$238="Basic")*(F$10:F$238="Partial"))</f>
@@ -51600,7 +51629,7 @@
       <c r="D6" s="265"/>
       <c r="E6" s="14">
         <f>SUMPRODUCT(($A$10:$A$238="Advanced")*(E$10:E$238="Missing"))+0.5*SUMPRODUCT(($A$10:$A$238="Advanced")*(E$10:E$238="Partial"))</f>
-        <v>7</v>
+        <v>5.5</v>
       </c>
       <c r="F6" s="14">
         <f>SUMPRODUCT(($A$10:$A$238="Advanced")*(F$10:F$238="Missing"))+0.5*SUMPRODUCT(($A$10:$A$238="Advanced")*(F$10:F$238="Partial"))</f>
@@ -51622,7 +51651,7 @@
       <c r="D7" s="265"/>
       <c r="E7" s="14">
         <f>SUMPRODUCT(($A$10:$A$238="Advanced")*(E$10:E$238="Completed"))+SUMPRODUCT(($A$10:$A$238="Advanced")*(E$10:E$238="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$238="Advanced")*(E$10:E$238="Partial"))</f>
-        <v>5</v>
+        <v>6.5</v>
       </c>
       <c r="F7" s="14">
         <f>SUMPRODUCT(($A$10:$A$238="Advanced")*(F$10:F$238="Completed"))+SUMPRODUCT(($A$10:$A$238="Advanced")*(F$10:F$238="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$238="Advanced")*(F$10:F$238="Partial"))</f>
@@ -52377,9 +52406,11 @@
       <c r="C46" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="D46" s="11"/>
+      <c r="D46" s="11" t="s">
+        <v>975</v>
+      </c>
       <c r="E46" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>52</v>
@@ -52398,7 +52429,7 @@
       </c>
       <c r="D47" s="11"/>
       <c r="E47" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>52</v>
@@ -52417,7 +52448,7 @@
       </c>
       <c r="D48" s="11"/>
       <c r="E48" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>52</v>
@@ -53797,8 +53828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -53870,7 +53901,7 @@
       <c r="D3" s="265"/>
       <c r="E3" s="14">
         <f>SUMPRODUCT(($A$10:$A$257="Basic")*(E$10:E$257="Missing"))+0.5*SUMPRODUCT(($A$10:$A$257="Basic")*(E$10:E$257="Partial"))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="14">
         <f>SUMPRODUCT(($A$10:$A$257="Basic")*(F$10:F$257="Missing"))+0.5*SUMPRODUCT(($A$10:$A$257="Basic")*(F$10:F$257="Partial"))</f>
@@ -54480,7 +54511,7 @@
         <v>401</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>61</v>
@@ -54904,7 +54935,7 @@
         <v>415</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>61</v>
@@ -54924,9 +54955,11 @@
       <c r="C57" s="11" t="s">
         <v>417</v>
       </c>
-      <c r="D57" s="11"/>
+      <c r="D57" s="11" t="s">
+        <v>976</v>
+      </c>
       <c r="E57" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F57" s="4" t="s">
         <v>52</v>
@@ -57173,7 +57206,7 @@
         <v>264</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
Updated scrolling credits with special thanks and copyrights
</commit_message>
<xml_diff>
--- a/GameDocuments/gam352_papercut_rubric.xlsx
+++ b/GameDocuments/gam352_papercut_rubric.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Game Data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2318" uniqueCount="978">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2317" uniqueCount="977">
   <si>
     <t>GAME NAME</t>
   </si>
@@ -3683,9 +3683,6 @@
   </si>
   <si>
     <t xml:space="preserve">No hud elements </t>
-  </si>
-  <si>
-    <t>Take your pick</t>
   </si>
   <si>
     <t>Transformation sequence</t>
@@ -5762,6 +5759,90 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -5795,18 +5876,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -5864,99 +5933,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="4" borderId="16" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="4" borderId="18" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="26" fillId="3" borderId="21" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5967,6 +5943,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="26" fillId="3" borderId="26" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6035,55 +6017,37 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="4" borderId="16" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="4" borderId="18" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6095,28 +6059,28 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6143,19 +6107,52 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -38692,54 +38689,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="178"/>
+      <c r="B1" s="145"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="146"/>
       <c r="E1" s="103"/>
-      <c r="F1" s="176" t="s">
+      <c r="F1" s="144" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="177"/>
-      <c r="H1" s="177"/>
-      <c r="I1" s="177"/>
-      <c r="J1" s="178"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
+      <c r="J1" s="146"/>
       <c r="K1" s="104"/>
       <c r="L1" s="104"/>
       <c r="M1" s="105"/>
     </row>
     <row r="2" spans="1:13" ht="14.1" customHeight="1">
-      <c r="A2" s="182" t="s">
+      <c r="A2" s="147" t="s">
         <v>951</v>
       </c>
-      <c r="B2" s="183"/>
-      <c r="C2" s="183"/>
-      <c r="D2" s="184"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="149"/>
       <c r="E2" s="103"/>
-      <c r="F2" s="182" t="s">
+      <c r="F2" s="147" t="s">
         <v>954</v>
       </c>
-      <c r="G2" s="183"/>
-      <c r="H2" s="183"/>
-      <c r="I2" s="183"/>
-      <c r="J2" s="184"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="149"/>
       <c r="K2" s="104"/>
       <c r="L2" s="104"/>
       <c r="M2" s="105"/>
     </row>
     <row r="3" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A3" s="185"/>
-      <c r="B3" s="186"/>
-      <c r="C3" s="186"/>
-      <c r="D3" s="187"/>
+      <c r="A3" s="150"/>
+      <c r="B3" s="151"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="103"/>
-      <c r="F3" s="185"/>
-      <c r="G3" s="186"/>
-      <c r="H3" s="186"/>
-      <c r="I3" s="186"/>
-      <c r="J3" s="187"/>
+      <c r="F3" s="150"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="151"/>
+      <c r="J3" s="152"/>
       <c r="K3" s="104"/>
       <c r="L3" s="104"/>
       <c r="M3" s="105"/>
@@ -38760,41 +38757,41 @@
       <c r="M4" s="105"/>
     </row>
     <row r="5" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="144" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="177"/>
-      <c r="C5" s="177"/>
-      <c r="D5" s="178"/>
+      <c r="B5" s="145"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="146"/>
       <c r="E5" s="103"/>
-      <c r="F5" s="176" t="s">
+      <c r="F5" s="144" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="177"/>
-      <c r="H5" s="177"/>
-      <c r="I5" s="177"/>
-      <c r="J5" s="178"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="145"/>
+      <c r="I5" s="145"/>
+      <c r="J5" s="146"/>
       <c r="K5" s="104"/>
       <c r="L5" s="107"/>
       <c r="M5" s="105"/>
     </row>
     <row r="6" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="156" t="s">
         <v>952</v>
       </c>
-      <c r="B6" s="174"/>
-      <c r="C6" s="174"/>
-      <c r="D6" s="175"/>
+      <c r="B6" s="157"/>
+      <c r="C6" s="157"/>
+      <c r="D6" s="158"/>
       <c r="E6" s="103"/>
-      <c r="F6" s="173" t="s">
+      <c r="F6" s="156" t="s">
         <v>955</v>
       </c>
-      <c r="G6" s="174"/>
-      <c r="H6" s="174"/>
-      <c r="I6" s="174"/>
-      <c r="J6" s="175"/>
+      <c r="G6" s="157"/>
+      <c r="H6" s="157"/>
+      <c r="I6" s="157"/>
+      <c r="J6" s="158"/>
       <c r="K6" s="104"/>
-      <c r="L6" s="170" t="s">
+      <c r="L6" s="153" t="s">
         <v>24</v>
       </c>
       <c r="M6" s="105"/>
@@ -38805,47 +38802,47 @@
       <c r="C7" s="108"/>
       <c r="D7" s="109"/>
       <c r="E7" s="103"/>
-      <c r="F7" s="173"/>
-      <c r="G7" s="174"/>
-      <c r="H7" s="174"/>
-      <c r="I7" s="174"/>
-      <c r="J7" s="175"/>
+      <c r="F7" s="156"/>
+      <c r="G7" s="157"/>
+      <c r="H7" s="157"/>
+      <c r="I7" s="157"/>
+      <c r="J7" s="158"/>
       <c r="K7" s="104"/>
-      <c r="L7" s="171"/>
+      <c r="L7" s="154"/>
       <c r="M7" s="105"/>
     </row>
     <row r="8" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="144" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="177"/>
-      <c r="C8" s="177"/>
-      <c r="D8" s="178"/>
+      <c r="B8" s="145"/>
+      <c r="C8" s="145"/>
+      <c r="D8" s="146"/>
       <c r="E8" s="103"/>
-      <c r="F8" s="173"/>
-      <c r="G8" s="174"/>
-      <c r="H8" s="174"/>
-      <c r="I8" s="174"/>
-      <c r="J8" s="175"/>
+      <c r="F8" s="156"/>
+      <c r="G8" s="157"/>
+      <c r="H8" s="157"/>
+      <c r="I8" s="157"/>
+      <c r="J8" s="158"/>
       <c r="K8" s="104"/>
-      <c r="L8" s="171"/>
+      <c r="L8" s="154"/>
       <c r="M8" s="105"/>
     </row>
     <row r="9" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="156" t="s">
         <v>953</v>
       </c>
-      <c r="B9" s="174"/>
-      <c r="C9" s="174"/>
-      <c r="D9" s="175"/>
+      <c r="B9" s="157"/>
+      <c r="C9" s="157"/>
+      <c r="D9" s="158"/>
       <c r="E9" s="103"/>
-      <c r="F9" s="173"/>
-      <c r="G9" s="174"/>
-      <c r="H9" s="174"/>
-      <c r="I9" s="174"/>
-      <c r="J9" s="175"/>
+      <c r="F9" s="156"/>
+      <c r="G9" s="157"/>
+      <c r="H9" s="157"/>
+      <c r="I9" s="157"/>
+      <c r="J9" s="158"/>
       <c r="K9" s="104"/>
-      <c r="L9" s="172"/>
+      <c r="L9" s="155"/>
       <c r="M9" s="105"/>
     </row>
     <row r="10" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -38864,18 +38861,18 @@
       <c r="M10" s="105"/>
     </row>
     <row r="11" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="144" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="177"/>
-      <c r="C11" s="177"/>
-      <c r="D11" s="178"/>
+      <c r="B11" s="145"/>
+      <c r="C11" s="145"/>
+      <c r="D11" s="146"/>
       <c r="E11" s="103"/>
-      <c r="F11" s="176" t="s">
+      <c r="F11" s="144" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="177"/>
-      <c r="H11" s="178"/>
+      <c r="G11" s="145"/>
+      <c r="H11" s="146"/>
       <c r="I11" s="134" t="s">
         <v>7</v>
       </c>
@@ -38915,7 +38912,7 @@
         <v>-0.12</v>
       </c>
       <c r="K12" s="104"/>
-      <c r="L12" s="170" t="s">
+      <c r="L12" s="153" t="s">
         <v>8</v>
       </c>
       <c r="M12" s="105"/>
@@ -38948,7 +38945,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="120"/>
-      <c r="L13" s="171"/>
+      <c r="L13" s="154"/>
       <c r="M13" s="121"/>
     </row>
     <row r="14" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -38978,7 +38975,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="124"/>
-      <c r="L14" s="172"/>
+      <c r="L14" s="155"/>
       <c r="M14" s="125"/>
     </row>
     <row r="15" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39046,11 +39043,11 @@
         <v>939</v>
       </c>
       <c r="E17" s="104"/>
-      <c r="F17" s="176" t="s">
+      <c r="F17" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="177"/>
-      <c r="H17" s="178"/>
+      <c r="G17" s="145"/>
+      <c r="H17" s="146"/>
       <c r="I17" s="111"/>
       <c r="J17" s="135">
         <v>0.75</v>
@@ -39076,17 +39073,17 @@
       <c r="F18" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="179" t="s">
+      <c r="G18" s="159" t="s">
         <v>956</v>
       </c>
-      <c r="H18" s="180"/>
-      <c r="I18" s="181"/>
+      <c r="H18" s="160"/>
+      <c r="I18" s="161"/>
       <c r="J18" s="137">
         <f>IF(LEFT(G18,6)="Entire",0,IF(LEFT(G18,6)="Custom",-0.05,-0.1))</f>
         <v>-0.1</v>
       </c>
       <c r="K18" s="128"/>
-      <c r="L18" s="170" t="s">
+      <c r="L18" s="153" t="s">
         <v>18</v>
       </c>
       <c r="M18" s="105"/>
@@ -39106,17 +39103,17 @@
       <c r="F19" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="153" t="s">
+      <c r="G19" s="162" t="s">
         <v>957</v>
       </c>
-      <c r="H19" s="154"/>
-      <c r="I19" s="155"/>
+      <c r="H19" s="163"/>
+      <c r="I19" s="164"/>
       <c r="J19" s="139">
         <f>IF(G19="2D Graphics and 2D Gameplay",IF(J11=0.15,-0.05,0),IF(G19="3D Graphics but 2D Gameplay",IF(J11=0.15,-0.02,-0.3),IF(J11=0.15,0,-0.3)))</f>
         <v>0</v>
       </c>
       <c r="K19" s="104"/>
-      <c r="L19" s="172"/>
+      <c r="L19" s="155"/>
       <c r="M19" s="105"/>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39166,22 +39163,22 @@
       <c r="C22" s="118"/>
       <c r="D22" s="119"/>
       <c r="E22" s="104"/>
-      <c r="F22" s="168" t="s">
+      <c r="F22" s="186" t="s">
         <v>713</v>
       </c>
-      <c r="G22" s="166" t="s">
+      <c r="G22" s="184" t="s">
         <v>714</v>
       </c>
-      <c r="H22" s="165"/>
+      <c r="H22" s="183"/>
       <c r="I22" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="163">
+      <c r="J22" s="181">
         <f>J20+J15</f>
         <v>0.68</v>
       </c>
       <c r="K22" s="104"/>
-      <c r="L22" s="144" t="s">
+      <c r="L22" s="165" t="s">
         <v>725</v>
       </c>
       <c r="M22" s="105"/>
@@ -39192,15 +39189,15 @@
       <c r="C23" s="118"/>
       <c r="D23" s="119"/>
       <c r="E23" s="104"/>
-      <c r="F23" s="169"/>
-      <c r="G23" s="167"/>
-      <c r="H23" s="165"/>
+      <c r="F23" s="187"/>
+      <c r="G23" s="185"/>
+      <c r="H23" s="183"/>
       <c r="I23" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="164"/>
+      <c r="J23" s="182"/>
       <c r="K23" s="104"/>
-      <c r="L23" s="145"/>
+      <c r="L23" s="166"/>
       <c r="M23" s="105"/>
     </row>
     <row r="24" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39224,13 +39221,13 @@
       <c r="C25" s="118"/>
       <c r="D25" s="119"/>
       <c r="E25" s="104"/>
-      <c r="F25" s="157" t="s">
+      <c r="F25" s="175" t="s">
         <v>932</v>
       </c>
-      <c r="G25" s="158"/>
-      <c r="H25" s="158"/>
-      <c r="I25" s="158"/>
-      <c r="J25" s="159"/>
+      <c r="G25" s="176"/>
+      <c r="H25" s="176"/>
+      <c r="I25" s="176"/>
+      <c r="J25" s="177"/>
       <c r="K25" s="104"/>
       <c r="L25" s="104"/>
       <c r="M25" s="105"/>
@@ -39241,11 +39238,11 @@
       <c r="C26" s="118"/>
       <c r="D26" s="119"/>
       <c r="E26" s="103"/>
-      <c r="F26" s="160"/>
-      <c r="G26" s="161"/>
-      <c r="H26" s="161"/>
-      <c r="I26" s="161"/>
-      <c r="J26" s="162"/>
+      <c r="F26" s="178"/>
+      <c r="G26" s="179"/>
+      <c r="H26" s="179"/>
+      <c r="I26" s="179"/>
+      <c r="J26" s="180"/>
       <c r="K26" s="104"/>
       <c r="L26" s="104"/>
       <c r="M26" s="105"/>
@@ -39271,13 +39268,13 @@
       <c r="C28" s="118"/>
       <c r="D28" s="119"/>
       <c r="E28" s="103"/>
-      <c r="F28" s="156" t="s">
+      <c r="F28" s="174" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="156"/>
-      <c r="H28" s="156"/>
-      <c r="I28" s="156"/>
-      <c r="J28" s="156"/>
+      <c r="G28" s="174"/>
+      <c r="H28" s="174"/>
+      <c r="I28" s="174"/>
+      <c r="J28" s="174"/>
       <c r="K28" s="104"/>
       <c r="L28" s="104"/>
       <c r="M28" s="105"/>
@@ -39288,13 +39285,13 @@
       <c r="C29" s="118"/>
       <c r="D29" s="119"/>
       <c r="E29" s="103"/>
-      <c r="F29" s="150" t="s">
+      <c r="F29" s="171" t="s">
         <v>933</v>
       </c>
-      <c r="G29" s="151"/>
-      <c r="H29" s="151"/>
-      <c r="I29" s="151"/>
-      <c r="J29" s="152"/>
+      <c r="G29" s="172"/>
+      <c r="H29" s="172"/>
+      <c r="I29" s="172"/>
+      <c r="J29" s="173"/>
       <c r="K29" s="104"/>
       <c r="L29" s="104"/>
       <c r="M29" s="105"/>
@@ -39305,30 +39302,30 @@
       <c r="C30" s="118"/>
       <c r="D30" s="119"/>
       <c r="E30" s="103"/>
-      <c r="F30" s="150"/>
-      <c r="G30" s="151"/>
-      <c r="H30" s="151"/>
-      <c r="I30" s="151"/>
-      <c r="J30" s="152"/>
+      <c r="F30" s="171"/>
+      <c r="G30" s="172"/>
+      <c r="H30" s="172"/>
+      <c r="I30" s="172"/>
+      <c r="J30" s="173"/>
       <c r="K30" s="104"/>
       <c r="L30" s="104"/>
       <c r="M30" s="105"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A31" s="146" t="s">
+      <c r="A31" s="167" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="147"/>
-      <c r="C31" s="148" t="s">
+      <c r="B31" s="168"/>
+      <c r="C31" s="169" t="s">
         <v>950</v>
       </c>
-      <c r="D31" s="149"/>
+      <c r="D31" s="170"/>
       <c r="E31" s="104"/>
-      <c r="F31" s="153"/>
-      <c r="G31" s="154"/>
-      <c r="H31" s="154"/>
-      <c r="I31" s="154"/>
-      <c r="J31" s="155"/>
+      <c r="F31" s="162"/>
+      <c r="G31" s="163"/>
+      <c r="H31" s="163"/>
+      <c r="I31" s="163"/>
+      <c r="J31" s="164"/>
       <c r="K31" s="104"/>
       <c r="L31" s="104"/>
       <c r="M31" s="105"/>
@@ -39351,12 +39348,16 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0"/>
   <mergeCells count="31">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="A2:D3"/>
-    <mergeCell ref="F2:J3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F29:J31"/>
+    <mergeCell ref="F28:J28"/>
+    <mergeCell ref="F25:J26"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F22:F23"/>
     <mergeCell ref="L12:L14"/>
     <mergeCell ref="L18:L19"/>
     <mergeCell ref="A6:D6"/>
@@ -39372,16 +39373,12 @@
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="G18:I18"/>
     <mergeCell ref="G19:I19"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F29:J31"/>
-    <mergeCell ref="F28:J28"/>
-    <mergeCell ref="F25:J26"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A2:D3"/>
+    <mergeCell ref="F2:J3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:J5"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6:D6">
@@ -39449,57 +39446,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="194" t="s">
         <v>556</v>
       </c>
-      <c r="B1" s="200"/>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
-      <c r="E1" s="200"/>
-      <c r="F1" s="200"/>
-      <c r="G1" s="200"/>
-      <c r="H1" s="200"/>
-      <c r="J1" s="210" t="s">
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
+      <c r="F1" s="195"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="195"/>
+      <c r="J1" s="205" t="s">
         <v>482</v>
       </c>
-      <c r="K1" s="211"/>
-      <c r="L1" s="212"/>
+      <c r="K1" s="206"/>
+      <c r="L1" s="207"/>
       <c r="M1" s="79"/>
       <c r="N1" s="24" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A2" s="199"/>
-      <c r="B2" s="200"/>
-      <c r="C2" s="200"/>
-      <c r="D2" s="200"/>
-      <c r="E2" s="200"/>
-      <c r="F2" s="200"/>
-      <c r="G2" s="200"/>
-      <c r="H2" s="200"/>
-      <c r="J2" s="213" t="s">
+      <c r="A2" s="194"/>
+      <c r="B2" s="195"/>
+      <c r="C2" s="195"/>
+      <c r="D2" s="195"/>
+      <c r="E2" s="195"/>
+      <c r="F2" s="195"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="195"/>
+      <c r="J2" s="208" t="s">
         <v>706</v>
       </c>
-      <c r="K2" s="214"/>
-      <c r="L2" s="215"/>
+      <c r="K2" s="209"/>
+      <c r="L2" s="210"/>
       <c r="M2" s="23"/>
       <c r="N2" s="26" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A3" s="199"/>
-      <c r="B3" s="200"/>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200"/>
-      <c r="E3" s="200"/>
-      <c r="F3" s="200"/>
-      <c r="G3" s="200"/>
-      <c r="H3" s="200"/>
-      <c r="J3" s="213"/>
-      <c r="K3" s="214"/>
-      <c r="L3" s="215"/>
+      <c r="A3" s="194"/>
+      <c r="B3" s="195"/>
+      <c r="C3" s="195"/>
+      <c r="D3" s="195"/>
+      <c r="E3" s="195"/>
+      <c r="F3" s="195"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="195"/>
+      <c r="J3" s="208"/>
+      <c r="K3" s="209"/>
+      <c r="L3" s="210"/>
       <c r="M3" s="23"/>
       <c r="N3" s="26" t="s">
         <v>431</v>
@@ -39509,14 +39506,14 @@
       <c r="A4" s="2"/>
       <c r="B4" s="5"/>
       <c r="C4" s="8"/>
-      <c r="D4" s="192"/>
-      <c r="E4" s="192"/>
+      <c r="D4" s="193"/>
+      <c r="E4" s="193"/>
       <c r="F4" s="43"/>
-      <c r="G4" s="192"/>
-      <c r="H4" s="192"/>
-      <c r="J4" s="213"/>
-      <c r="K4" s="214"/>
-      <c r="L4" s="215"/>
+      <c r="G4" s="193"/>
+      <c r="H4" s="193"/>
+      <c r="J4" s="208"/>
+      <c r="K4" s="209"/>
+      <c r="L4" s="210"/>
       <c r="M4" s="34"/>
       <c r="N4" s="26" t="s">
         <v>432</v>
@@ -39524,24 +39521,24 @@
       <c r="O4" s="81"/>
     </row>
     <row r="5" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A5" s="201" t="s">
+      <c r="A5" s="196" t="s">
         <v>425</v>
       </c>
-      <c r="B5" s="202"/>
+      <c r="B5" s="197"/>
       <c r="C5" s="8"/>
-      <c r="D5" s="205" t="s">
+      <c r="D5" s="200" t="s">
         <v>717</v>
       </c>
-      <c r="E5" s="206"/>
-      <c r="F5" s="207"/>
-      <c r="G5" s="208">
+      <c r="E5" s="201"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="203">
         <f>Submission!$E$17</f>
         <v>0</v>
       </c>
-      <c r="H5" s="209"/>
-      <c r="J5" s="213"/>
-      <c r="K5" s="214"/>
-      <c r="L5" s="215"/>
+      <c r="H5" s="204"/>
+      <c r="J5" s="208"/>
+      <c r="K5" s="209"/>
+      <c r="L5" s="210"/>
       <c r="M5" s="34"/>
       <c r="N5" s="26" t="s">
         <v>433</v>
@@ -39549,21 +39546,21 @@
       <c r="O5" s="81"/>
     </row>
     <row r="6" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A6" s="203"/>
-      <c r="B6" s="204"/>
+      <c r="A6" s="198"/>
+      <c r="B6" s="199"/>
       <c r="C6" s="43"/>
-      <c r="D6" s="192" t="s">
+      <c r="D6" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="192"/>
+      <c r="E6" s="193"/>
       <c r="F6" s="43"/>
-      <c r="G6" s="192" t="s">
+      <c r="G6" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="192"/>
-      <c r="J6" s="213"/>
-      <c r="K6" s="214"/>
-      <c r="L6" s="215"/>
+      <c r="H6" s="193"/>
+      <c r="J6" s="208"/>
+      <c r="K6" s="209"/>
+      <c r="L6" s="210"/>
       <c r="M6" s="34"/>
       <c r="N6" s="26" t="s">
         <v>434</v>
@@ -39571,24 +39568,24 @@
       <c r="O6" s="81"/>
     </row>
     <row r="7" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A7" s="195">
+      <c r="A7" s="188">
         <f>'Game Data'!$J$22</f>
         <v>0.68</v>
       </c>
-      <c r="B7" s="196"/>
+      <c r="B7" s="189"/>
       <c r="C7" s="43"/>
-      <c r="D7" s="193" t="s">
+      <c r="D7" s="216" t="s">
         <v>724</v>
       </c>
-      <c r="E7" s="194"/>
+      <c r="E7" s="217"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="193" t="s">
+      <c r="G7" s="216" t="s">
         <v>724</v>
       </c>
-      <c r="H7" s="194"/>
-      <c r="J7" s="213"/>
-      <c r="K7" s="214"/>
-      <c r="L7" s="215"/>
+      <c r="H7" s="217"/>
+      <c r="J7" s="208"/>
+      <c r="K7" s="209"/>
+      <c r="L7" s="210"/>
       <c r="M7" s="33"/>
       <c r="N7" s="26" t="s">
         <v>435</v>
@@ -39596,23 +39593,23 @@
       <c r="O7" s="81"/>
     </row>
     <row r="8" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A8" s="197"/>
-      <c r="B8" s="198"/>
+      <c r="A8" s="190"/>
+      <c r="B8" s="191"/>
       <c r="C8" s="97"/>
-      <c r="D8" s="219">
+      <c r="D8" s="214">
         <f>E17+E26+E35+E44+E53</f>
         <v>0.28000000000000003</v>
       </c>
-      <c r="E8" s="220"/>
+      <c r="E8" s="215"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="219">
+      <c r="G8" s="214">
         <f>H17+H26+H35+H44+H53</f>
         <v>0</v>
       </c>
-      <c r="H8" s="220"/>
-      <c r="J8" s="216"/>
-      <c r="K8" s="217"/>
-      <c r="L8" s="218"/>
+      <c r="H8" s="215"/>
+      <c r="J8" s="211"/>
+      <c r="K8" s="212"/>
+      <c r="L8" s="213"/>
       <c r="M8" s="80"/>
       <c r="N8" s="25" t="s">
         <v>436</v>
@@ -39623,15 +39620,15 @@
       <c r="A9" s="2"/>
       <c r="B9" s="5"/>
       <c r="C9" s="43"/>
-      <c r="D9" s="192" t="s">
+      <c r="D9" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="192"/>
+      <c r="E9" s="193"/>
       <c r="F9" s="43"/>
-      <c r="G9" s="192" t="s">
+      <c r="G9" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="192"/>
+      <c r="H9" s="193"/>
       <c r="J9" s="82"/>
       <c r="K9" s="82"/>
       <c r="L9" s="82"/>
@@ -39658,11 +39655,11 @@
       <c r="H10" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="191" t="s">
+      <c r="J10" s="192" t="s">
         <v>707</v>
       </c>
-      <c r="K10" s="191"/>
-      <c r="L10" s="191"/>
+      <c r="K10" s="192"/>
+      <c r="L10" s="192"/>
       <c r="O10" s="84"/>
     </row>
     <row r="11" spans="1:15" ht="14.1" customHeight="1">
@@ -39691,11 +39688,11 @@
         <f t="shared" ref="H11:H16" si="1">$B11*G11</f>
         <v>0</v>
       </c>
-      <c r="J11" s="190" t="s">
+      <c r="J11" s="220" t="s">
         <v>792</v>
       </c>
-      <c r="K11" s="190"/>
-      <c r="L11" s="190"/>
+      <c r="K11" s="220"/>
+      <c r="L11" s="220"/>
       <c r="M11" s="82"/>
       <c r="O11" s="84"/>
     </row>
@@ -39725,9 +39722,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J12" s="190"/>
-      <c r="K12" s="190"/>
-      <c r="L12" s="190"/>
+      <c r="J12" s="220"/>
+      <c r="K12" s="220"/>
+      <c r="L12" s="220"/>
       <c r="M12" s="82"/>
       <c r="O12" s="84"/>
     </row>
@@ -39757,9 +39754,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="190"/>
-      <c r="K13" s="190"/>
-      <c r="L13" s="190"/>
+      <c r="J13" s="220"/>
+      <c r="K13" s="220"/>
+      <c r="L13" s="220"/>
       <c r="M13" s="82"/>
       <c r="O13" s="84"/>
     </row>
@@ -39825,11 +39822,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J15" s="188">
+      <c r="J15" s="218">
         <f>MAX(0,MIN(1,IF($J17 &lt;= 0.95, ROUND($J17,2), FLOOR((0.95+($J17-0.95)/5),0.01))))</f>
         <v>0.83</v>
       </c>
-      <c r="L15" s="188">
+      <c r="L15" s="218">
         <f>MAX(0,MIN(1,IF($L17 &lt;= 0.95, ROUND($L17,2), FLOOR((0.95+($L17-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -39862,8 +39859,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J16" s="189"/>
-      <c r="L16" s="189"/>
+      <c r="J16" s="219"/>
+      <c r="L16" s="219"/>
       <c r="M16" s="82"/>
       <c r="O16" s="84"/>
     </row>
@@ -39900,15 +39897,15 @@
       <c r="A18" s="2"/>
       <c r="B18" s="5"/>
       <c r="C18" s="43"/>
-      <c r="D18" s="192" t="s">
+      <c r="D18" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="192"/>
+      <c r="E18" s="193"/>
       <c r="F18" s="43"/>
-      <c r="G18" s="192" t="s">
+      <c r="G18" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="192"/>
+      <c r="H18" s="193"/>
       <c r="J18" s="88"/>
       <c r="M18" s="78"/>
     </row>
@@ -39933,11 +39930,11 @@
       <c r="H19" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="191" t="s">
+      <c r="J19" s="192" t="s">
         <v>715</v>
       </c>
-      <c r="K19" s="191"/>
-      <c r="L19" s="191"/>
+      <c r="K19" s="192"/>
+      <c r="L19" s="192"/>
       <c r="M19" s="83"/>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1">
@@ -39966,11 +39963,11 @@
         <f t="shared" ref="H20:H25" si="3">$B20*G20</f>
         <v>0</v>
       </c>
-      <c r="J20" s="190" t="s">
+      <c r="J20" s="220" t="s">
         <v>722</v>
       </c>
-      <c r="K20" s="190"/>
-      <c r="L20" s="190"/>
+      <c r="K20" s="220"/>
+      <c r="L20" s="220"/>
       <c r="M20" s="84"/>
     </row>
     <row r="21" spans="1:13" ht="14.1" customHeight="1">
@@ -39999,9 +39996,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J21" s="190"/>
-      <c r="K21" s="190"/>
-      <c r="L21" s="190"/>
+      <c r="J21" s="220"/>
+      <c r="K21" s="220"/>
+      <c r="L21" s="220"/>
       <c r="M21" s="84"/>
     </row>
     <row r="22" spans="1:13" ht="14.1" customHeight="1">
@@ -40030,9 +40027,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J22" s="190"/>
-      <c r="K22" s="190"/>
-      <c r="L22" s="190"/>
+      <c r="J22" s="220"/>
+      <c r="K22" s="220"/>
+      <c r="L22" s="220"/>
       <c r="M22" s="84"/>
     </row>
     <row r="23" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40096,11 +40093,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J24" s="188">
+      <c r="J24" s="218">
         <f>MAX(0,MIN(1,IF($J26 &lt;= 0.95, ROUND($J26,2), FLOOR((0.95+($J26-0.95)/5),0.01))))</f>
         <v>0.86</v>
       </c>
-      <c r="L24" s="188">
+      <c r="L24" s="218">
         <f>MAX(0,MIN(1,IF($L26 &lt;= 0.95, ROUND($L26,2), FLOOR((0.95+($L26-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40132,8 +40129,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J25" s="189"/>
-      <c r="L25" s="189"/>
+      <c r="J25" s="219"/>
+      <c r="L25" s="219"/>
       <c r="M25" s="84"/>
     </row>
     <row r="26" spans="1:13" ht="14.1" customHeight="1">
@@ -40169,15 +40166,15 @@
       <c r="A27" s="2"/>
       <c r="B27" s="5"/>
       <c r="C27" s="43"/>
-      <c r="D27" s="192" t="s">
+      <c r="D27" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="192"/>
+      <c r="E27" s="193"/>
       <c r="F27" s="43"/>
-      <c r="G27" s="192" t="s">
+      <c r="G27" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H27" s="192"/>
+      <c r="H27" s="193"/>
     </row>
     <row r="28" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
       <c r="A28" s="1" t="s">
@@ -40200,11 +40197,11 @@
       <c r="H28" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J28" s="191" t="s">
+      <c r="J28" s="192" t="s">
         <v>709</v>
       </c>
-      <c r="K28" s="191"/>
-      <c r="L28" s="191"/>
+      <c r="K28" s="192"/>
+      <c r="L28" s="192"/>
     </row>
     <row r="29" spans="1:13" ht="14.1" customHeight="1">
       <c r="A29" s="57" t="str">
@@ -40232,11 +40229,11 @@
         <f t="shared" ref="H29:H34" si="5">$B29*G29</f>
         <v>0</v>
       </c>
-      <c r="J29" s="190" t="s">
+      <c r="J29" s="220" t="s">
         <v>710</v>
       </c>
-      <c r="K29" s="190"/>
-      <c r="L29" s="190"/>
+      <c r="K29" s="220"/>
+      <c r="L29" s="220"/>
     </row>
     <row r="30" spans="1:13" ht="14.1" customHeight="1">
       <c r="A30" s="58" t="str">
@@ -40264,9 +40261,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J30" s="190"/>
-      <c r="K30" s="190"/>
-      <c r="L30" s="190"/>
+      <c r="J30" s="220"/>
+      <c r="K30" s="220"/>
+      <c r="L30" s="220"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1">
       <c r="A31" s="58" t="str">
@@ -40294,9 +40291,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J31" s="190"/>
-      <c r="K31" s="190"/>
-      <c r="L31" s="190"/>
+      <c r="J31" s="220"/>
+      <c r="K31" s="220"/>
+      <c r="L31" s="220"/>
     </row>
     <row r="32" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
       <c r="A32" s="58" t="str">
@@ -40358,11 +40355,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J33" s="188">
+      <c r="J33" s="218">
         <f>MAX(0,MIN(1,IF($J35 &lt;= 0.95, ROUND($J35,2), FLOOR((0.95+($J35-0.95)/5),0.01))))</f>
         <v>0.88</v>
       </c>
-      <c r="L33" s="188">
+      <c r="L33" s="218">
         <f>MAX(0,MIN(1,IF($L35 &lt;= 0.95, ROUND($L35,2), FLOOR((0.95+($L35-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40393,8 +40390,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J34" s="189"/>
-      <c r="L34" s="189"/>
+      <c r="J34" s="219"/>
+      <c r="L34" s="219"/>
     </row>
     <row r="35" spans="1:12" ht="14.1" customHeight="1">
       <c r="A35" s="2"/>
@@ -40428,15 +40425,15 @@
       <c r="A36" s="2"/>
       <c r="B36" s="5"/>
       <c r="C36" s="43"/>
-      <c r="D36" s="192" t="s">
+      <c r="D36" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="192"/>
+      <c r="E36" s="193"/>
       <c r="F36" s="43"/>
-      <c r="G36" s="192" t="s">
+      <c r="G36" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H36" s="192"/>
+      <c r="H36" s="193"/>
     </row>
     <row r="37" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A37" s="1" t="s">
@@ -40459,11 +40456,11 @@
       <c r="H37" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J37" s="191" t="s">
+      <c r="J37" s="192" t="s">
         <v>711</v>
       </c>
-      <c r="K37" s="191"/>
-      <c r="L37" s="191"/>
+      <c r="K37" s="192"/>
+      <c r="L37" s="192"/>
     </row>
     <row r="38" spans="1:12" ht="14.1" customHeight="1">
       <c r="A38" s="57" t="str">
@@ -40491,11 +40488,11 @@
         <f t="shared" ref="H38:H43" si="7">$B38*G38</f>
         <v>0</v>
       </c>
-      <c r="J38" s="190" t="s">
+      <c r="J38" s="220" t="s">
         <v>712</v>
       </c>
-      <c r="K38" s="190"/>
-      <c r="L38" s="190"/>
+      <c r="K38" s="220"/>
+      <c r="L38" s="220"/>
     </row>
     <row r="39" spans="1:12" ht="14.1" customHeight="1">
       <c r="A39" s="58" t="str">
@@ -40523,9 +40520,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J39" s="190"/>
-      <c r="K39" s="190"/>
-      <c r="L39" s="190"/>
+      <c r="J39" s="220"/>
+      <c r="K39" s="220"/>
+      <c r="L39" s="220"/>
     </row>
     <row r="40" spans="1:12" ht="14.1" customHeight="1">
       <c r="A40" s="58" t="str">
@@ -40553,9 +40550,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J40" s="190"/>
-      <c r="K40" s="190"/>
-      <c r="L40" s="190"/>
+      <c r="J40" s="220"/>
+      <c r="K40" s="220"/>
+      <c r="L40" s="220"/>
     </row>
     <row r="41" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A41" s="58" t="str">
@@ -40617,11 +40614,11 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J42" s="188">
+      <c r="J42" s="218">
         <f>MAX(0,MIN(1,IF($J44 &lt;= 0.95, ROUND($J44,2), FLOOR((0.95+($J44-0.95)/5),0.01))))</f>
         <v>0.73</v>
       </c>
-      <c r="L42" s="188">
+      <c r="L42" s="218">
         <f>MAX(0,MIN(1,IF($L44 &lt;= 0.95, ROUND($L44,2), FLOOR((0.95+($L44-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40652,8 +40649,8 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J43" s="189"/>
-      <c r="L43" s="189"/>
+      <c r="J43" s="219"/>
+      <c r="L43" s="219"/>
     </row>
     <row r="44" spans="1:12" ht="14.1" customHeight="1">
       <c r="A44" s="2"/>
@@ -40687,15 +40684,15 @@
       <c r="A45" s="2"/>
       <c r="B45" s="5"/>
       <c r="C45" s="43"/>
-      <c r="D45" s="192" t="s">
+      <c r="D45" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="192"/>
+      <c r="E45" s="193"/>
       <c r="F45" s="43"/>
-      <c r="G45" s="192" t="s">
+      <c r="G45" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="192"/>
+      <c r="H45" s="193"/>
     </row>
     <row r="46" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A46" s="1" t="s">
@@ -40903,6 +40900,34 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="J29:L31"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="L33:L34"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="J38:L40"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="J11:L13"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J20:L22"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G36:H36"/>
     <mergeCell ref="A7:B8"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="D6:E6"/>
@@ -40916,34 +40941,6 @@
     <mergeCell ref="J2:L8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="J11:L13"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J20:L22"/>
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="L42:L43"/>
-    <mergeCell ref="J29:L31"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="L33:L34"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="J38:L40"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -40971,59 +40968,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="235" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="233"/>
-      <c r="C1" s="233"/>
-      <c r="D1" s="233"/>
-      <c r="E1" s="233"/>
-      <c r="F1" s="233"/>
-      <c r="G1" s="234"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="237"/>
     </row>
     <row r="2" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A2" s="221" t="s">
+      <c r="A2" s="230" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="222"/>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
-      <c r="G2" s="223"/>
+      <c r="B2" s="231"/>
+      <c r="C2" s="231"/>
+      <c r="D2" s="231"/>
+      <c r="E2" s="231"/>
+      <c r="F2" s="231"/>
+      <c r="G2" s="232"/>
     </row>
     <row r="3" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A3" s="238" t="s">
+      <c r="A3" s="227" t="s">
         <v>930</v>
       </c>
-      <c r="B3" s="239"/>
-      <c r="C3" s="239"/>
-      <c r="D3" s="239"/>
-      <c r="E3" s="239"/>
-      <c r="F3" s="239"/>
-      <c r="G3" s="240"/>
+      <c r="B3" s="228"/>
+      <c r="C3" s="228"/>
+      <c r="D3" s="228"/>
+      <c r="E3" s="228"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="229"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A4" s="221" t="s">
+      <c r="A4" s="230" t="s">
         <v>438</v>
       </c>
-      <c r="B4" s="222"/>
-      <c r="C4" s="222"/>
-      <c r="D4" s="222"/>
-      <c r="E4" s="222"/>
-      <c r="F4" s="222"/>
-      <c r="G4" s="223"/>
+      <c r="B4" s="231"/>
+      <c r="C4" s="231"/>
+      <c r="D4" s="231"/>
+      <c r="E4" s="231"/>
+      <c r="F4" s="231"/>
+      <c r="G4" s="232"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A5" s="249" t="s">
+      <c r="A5" s="238" t="s">
         <v>580</v>
       </c>
-      <c r="B5" s="250"/>
-      <c r="C5" s="250"/>
-      <c r="D5" s="250"/>
-      <c r="E5" s="250"/>
-      <c r="F5" s="250"/>
-      <c r="G5" s="251"/>
+      <c r="B5" s="239"/>
+      <c r="C5" s="239"/>
+      <c r="D5" s="239"/>
+      <c r="E5" s="239"/>
+      <c r="F5" s="239"/>
+      <c r="G5" s="240"/>
     </row>
     <row r="6" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
       <c r="A6" s="2"/>
@@ -41056,10 +41053,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75">
-      <c r="A8" s="247" t="s">
+      <c r="A8" s="233" t="s">
         <v>718</v>
       </c>
-      <c r="B8" s="248"/>
+      <c r="B8" s="234"/>
       <c r="C8" s="65">
         <v>0</v>
       </c>
@@ -41076,10 +41073,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75">
-      <c r="A9" s="253" t="s">
+      <c r="A9" s="242" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="254"/>
+      <c r="B9" s="243"/>
       <c r="C9" s="92">
         <v>0</v>
       </c>
@@ -41096,10 +41093,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75">
-      <c r="A10" s="255" t="s">
+      <c r="A10" s="244" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="256"/>
+      <c r="B10" s="245"/>
       <c r="C10" s="69">
         <v>0</v>
       </c>
@@ -41116,10 +41113,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75">
-      <c r="A11" s="256" t="s">
+      <c r="A11" s="245" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="256"/>
+      <c r="B11" s="245"/>
       <c r="C11" s="69">
         <v>0</v>
       </c>
@@ -41136,10 +41133,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75">
-      <c r="A12" s="256" t="s">
+      <c r="A12" s="245" t="s">
         <v>716</v>
       </c>
-      <c r="B12" s="256"/>
+      <c r="B12" s="245"/>
       <c r="C12" s="69">
         <v>0</v>
       </c>
@@ -41156,10 +41153,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75">
-      <c r="A13" s="256" t="s">
+      <c r="A13" s="245" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="256"/>
+      <c r="B13" s="245"/>
       <c r="C13" s="69">
         <v>0</v>
       </c>
@@ -41176,10 +41173,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75">
-      <c r="A14" s="255" t="s">
+      <c r="A14" s="244" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="256"/>
+      <c r="B14" s="245"/>
       <c r="C14" s="69">
         <v>0</v>
       </c>
@@ -41196,10 +41193,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75">
-      <c r="A15" s="255" t="s">
+      <c r="A15" s="244" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="256"/>
+      <c r="B15" s="245"/>
       <c r="C15" s="69">
         <v>0</v>
       </c>
@@ -41216,10 +41213,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A16" s="230" t="s">
+      <c r="A16" s="246" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="231"/>
+      <c r="B16" s="247"/>
       <c r="C16" s="73">
         <v>0</v>
       </c>
@@ -41237,11 +41234,11 @@
     </row>
     <row r="17" spans="1:7" ht="14.1" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="252" t="s">
+      <c r="B17" s="241" t="s">
         <v>721</v>
       </c>
-      <c r="C17" s="252"/>
-      <c r="D17" s="252"/>
+      <c r="C17" s="241"/>
+      <c r="D17" s="241"/>
       <c r="E17" s="63">
         <f>SUM(E9:E16)</f>
         <v>0</v>
@@ -41262,527 +41259,559 @@
       <c r="A19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="232" t="s">
+      <c r="B19" s="235" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="233"/>
-      <c r="D19" s="233"/>
-      <c r="E19" s="233"/>
-      <c r="F19" s="233"/>
-      <c r="G19" s="234"/>
+      <c r="C19" s="236"/>
+      <c r="D19" s="236"/>
+      <c r="E19" s="236"/>
+      <c r="F19" s="236"/>
+      <c r="G19" s="237"/>
     </row>
     <row r="20" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="A20" s="10" t="s">
         <v>582</v>
       </c>
-      <c r="B20" s="221" t="s">
+      <c r="B20" s="230" t="s">
         <v>931</v>
       </c>
-      <c r="C20" s="222"/>
-      <c r="D20" s="222"/>
-      <c r="E20" s="222"/>
-      <c r="F20" s="222"/>
-      <c r="G20" s="223"/>
+      <c r="C20" s="231"/>
+      <c r="D20" s="231"/>
+      <c r="E20" s="231"/>
+      <c r="F20" s="231"/>
+      <c r="G20" s="232"/>
     </row>
     <row r="21" spans="1:7" ht="60" customHeight="1" thickBot="1">
       <c r="A21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="221" t="s">
+      <c r="B21" s="230" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="222"/>
-      <c r="D21" s="222"/>
-      <c r="E21" s="222"/>
-      <c r="F21" s="222"/>
-      <c r="G21" s="223"/>
+      <c r="C21" s="231"/>
+      <c r="D21" s="231"/>
+      <c r="E21" s="231"/>
+      <c r="F21" s="231"/>
+      <c r="G21" s="232"/>
     </row>
     <row r="22" spans="1:7" ht="45.95" customHeight="1" thickBot="1">
       <c r="A22" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="221" t="s">
+      <c r="B22" s="230" t="s">
         <v>917</v>
       </c>
-      <c r="C22" s="222"/>
-      <c r="D22" s="222"/>
-      <c r="E22" s="222"/>
-      <c r="F22" s="222"/>
-      <c r="G22" s="223"/>
+      <c r="C22" s="231"/>
+      <c r="D22" s="231"/>
+      <c r="E22" s="231"/>
+      <c r="F22" s="231"/>
+      <c r="G22" s="232"/>
     </row>
     <row r="23" spans="1:7" ht="32.1" customHeight="1">
       <c r="A23" s="98" t="s">
         <v>899</v>
       </c>
-      <c r="B23" s="238" t="s">
+      <c r="B23" s="227" t="s">
         <v>916</v>
       </c>
-      <c r="C23" s="239"/>
-      <c r="D23" s="239"/>
-      <c r="E23" s="239"/>
-      <c r="F23" s="239"/>
-      <c r="G23" s="240"/>
+      <c r="C23" s="228"/>
+      <c r="D23" s="228"/>
+      <c r="E23" s="228"/>
+      <c r="F23" s="228"/>
+      <c r="G23" s="229"/>
     </row>
     <row r="24" spans="1:7" ht="15.75">
       <c r="A24" s="99"/>
-      <c r="B24" s="257" t="s">
+      <c r="B24" s="221" t="s">
         <v>900</v>
       </c>
-      <c r="C24" s="258"/>
-      <c r="D24" s="260" t="s">
+      <c r="C24" s="222"/>
+      <c r="D24" s="223" t="s">
         <v>901</v>
       </c>
-      <c r="E24" s="260"/>
-      <c r="F24" s="260"/>
-      <c r="G24" s="261"/>
+      <c r="E24" s="223"/>
+      <c r="F24" s="223"/>
+      <c r="G24" s="224"/>
     </row>
     <row r="25" spans="1:7" ht="15.75">
       <c r="A25" s="99"/>
-      <c r="B25" s="257" t="s">
+      <c r="B25" s="221" t="s">
         <v>902</v>
       </c>
-      <c r="C25" s="258"/>
-      <c r="D25" s="260" t="s">
+      <c r="C25" s="222"/>
+      <c r="D25" s="223" t="s">
         <v>903</v>
       </c>
-      <c r="E25" s="260"/>
-      <c r="F25" s="260"/>
-      <c r="G25" s="261"/>
+      <c r="E25" s="223"/>
+      <c r="F25" s="223"/>
+      <c r="G25" s="224"/>
     </row>
     <row r="26" spans="1:7" ht="15.75">
       <c r="A26" s="99"/>
-      <c r="B26" s="257" t="s">
+      <c r="B26" s="221" t="s">
         <v>904</v>
       </c>
-      <c r="C26" s="258"/>
-      <c r="D26" s="260" t="s">
+      <c r="C26" s="222"/>
+      <c r="D26" s="223" t="s">
         <v>905</v>
       </c>
-      <c r="E26" s="260"/>
-      <c r="F26" s="260"/>
-      <c r="G26" s="261"/>
+      <c r="E26" s="223"/>
+      <c r="F26" s="223"/>
+      <c r="G26" s="224"/>
     </row>
     <row r="27" spans="1:7" ht="15.75">
       <c r="A27" s="99"/>
-      <c r="B27" s="257" t="s">
+      <c r="B27" s="221" t="s">
         <v>906</v>
       </c>
-      <c r="C27" s="258"/>
+      <c r="C27" s="222"/>
       <c r="D27" s="225" t="s">
         <v>907</v>
       </c>
       <c r="E27" s="225"/>
       <c r="F27" s="225"/>
-      <c r="G27" s="259"/>
+      <c r="G27" s="226"/>
     </row>
     <row r="28" spans="1:7" ht="15.75">
       <c r="A28" s="99"/>
-      <c r="B28" s="257" t="s">
+      <c r="B28" s="221" t="s">
         <v>908</v>
       </c>
-      <c r="C28" s="258"/>
-      <c r="D28" s="260" t="s">
+      <c r="C28" s="222"/>
+      <c r="D28" s="223" t="s">
         <v>909</v>
       </c>
-      <c r="E28" s="260"/>
-      <c r="F28" s="260"/>
-      <c r="G28" s="261"/>
+      <c r="E28" s="223"/>
+      <c r="F28" s="223"/>
+      <c r="G28" s="224"/>
     </row>
     <row r="29" spans="1:7" ht="15.75">
       <c r="A29" s="99"/>
-      <c r="B29" s="257" t="s">
+      <c r="B29" s="221" t="s">
         <v>910</v>
       </c>
-      <c r="C29" s="258"/>
+      <c r="C29" s="222"/>
       <c r="D29" s="225" t="s">
         <v>911</v>
       </c>
       <c r="E29" s="225"/>
       <c r="F29" s="225"/>
-      <c r="G29" s="259"/>
+      <c r="G29" s="226"/>
     </row>
     <row r="30" spans="1:7" ht="15.75">
       <c r="A30" s="99"/>
-      <c r="B30" s="257" t="s">
+      <c r="B30" s="221" t="s">
         <v>914</v>
       </c>
-      <c r="C30" s="258"/>
-      <c r="D30" s="260" t="s">
+      <c r="C30" s="222"/>
+      <c r="D30" s="223" t="s">
         <v>915</v>
       </c>
-      <c r="E30" s="260"/>
-      <c r="F30" s="260"/>
-      <c r="G30" s="261"/>
+      <c r="E30" s="223"/>
+      <c r="F30" s="223"/>
+      <c r="G30" s="224"/>
     </row>
     <row r="31" spans="1:7" ht="15.75">
       <c r="A31" s="99"/>
-      <c r="B31" s="257" t="s">
+      <c r="B31" s="221" t="s">
         <v>912</v>
       </c>
-      <c r="C31" s="258"/>
+      <c r="C31" s="222"/>
       <c r="D31" s="225" t="s">
         <v>913</v>
       </c>
       <c r="E31" s="225"/>
       <c r="F31" s="225"/>
-      <c r="G31" s="259"/>
+      <c r="G31" s="226"/>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickBot="1">
       <c r="A32" s="99"/>
-      <c r="B32" s="257" t="s">
+      <c r="B32" s="221" t="s">
         <v>928</v>
       </c>
-      <c r="C32" s="258"/>
+      <c r="C32" s="222"/>
       <c r="D32" s="225" t="s">
         <v>929</v>
       </c>
       <c r="E32" s="225"/>
       <c r="F32" s="225"/>
-      <c r="G32" s="259"/>
+      <c r="G32" s="226"/>
     </row>
     <row r="33" spans="1:7" ht="15.75">
       <c r="A33" s="98" t="s">
         <v>918</v>
       </c>
-      <c r="B33" s="238" t="s">
+      <c r="B33" s="227" t="s">
         <v>919</v>
       </c>
-      <c r="C33" s="239"/>
-      <c r="D33" s="239"/>
-      <c r="E33" s="239"/>
-      <c r="F33" s="239"/>
-      <c r="G33" s="240"/>
+      <c r="C33" s="228"/>
+      <c r="D33" s="228"/>
+      <c r="E33" s="228"/>
+      <c r="F33" s="228"/>
+      <c r="G33" s="229"/>
     </row>
     <row r="34" spans="1:7" ht="15.75">
       <c r="A34" s="99"/>
-      <c r="B34" s="257" t="s">
+      <c r="B34" s="221" t="s">
         <v>920</v>
       </c>
-      <c r="C34" s="258"/>
-      <c r="D34" s="260" t="s">
+      <c r="C34" s="222"/>
+      <c r="D34" s="223" t="s">
         <v>925</v>
       </c>
-      <c r="E34" s="260"/>
-      <c r="F34" s="260"/>
-      <c r="G34" s="261"/>
+      <c r="E34" s="223"/>
+      <c r="F34" s="223"/>
+      <c r="G34" s="224"/>
     </row>
     <row r="35" spans="1:7" ht="15.75">
       <c r="A35" s="99"/>
-      <c r="B35" s="257" t="s">
+      <c r="B35" s="221" t="s">
         <v>921</v>
       </c>
-      <c r="C35" s="258"/>
-      <c r="D35" s="260" t="s">
+      <c r="C35" s="222"/>
+      <c r="D35" s="223" t="s">
         <v>926</v>
       </c>
-      <c r="E35" s="260"/>
-      <c r="F35" s="260"/>
-      <c r="G35" s="261"/>
+      <c r="E35" s="223"/>
+      <c r="F35" s="223"/>
+      <c r="G35" s="224"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" thickBot="1">
       <c r="A36" s="99"/>
-      <c r="B36" s="257" t="s">
+      <c r="B36" s="221" t="s">
         <v>922</v>
       </c>
-      <c r="C36" s="258"/>
-      <c r="D36" s="260" t="s">
+      <c r="C36" s="222"/>
+      <c r="D36" s="223" t="s">
         <v>927</v>
       </c>
-      <c r="E36" s="260"/>
-      <c r="F36" s="260"/>
-      <c r="G36" s="261"/>
+      <c r="E36" s="223"/>
+      <c r="F36" s="223"/>
+      <c r="G36" s="224"/>
     </row>
     <row r="37" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="A37" s="98" t="s">
         <v>923</v>
       </c>
-      <c r="B37" s="238" t="s">
+      <c r="B37" s="227" t="s">
         <v>924</v>
       </c>
-      <c r="C37" s="239"/>
-      <c r="D37" s="239"/>
-      <c r="E37" s="239"/>
-      <c r="F37" s="239"/>
-      <c r="G37" s="240"/>
+      <c r="C37" s="228"/>
+      <c r="D37" s="228"/>
+      <c r="E37" s="228"/>
+      <c r="F37" s="228"/>
+      <c r="G37" s="229"/>
     </row>
     <row r="38" spans="1:7" ht="29.1" customHeight="1">
-      <c r="A38" s="235" t="s">
+      <c r="A38" s="248" t="s">
         <v>517</v>
       </c>
-      <c r="B38" s="238" t="s">
+      <c r="B38" s="227" t="s">
         <v>490</v>
       </c>
-      <c r="C38" s="239"/>
-      <c r="D38" s="239"/>
-      <c r="E38" s="239"/>
-      <c r="F38" s="239"/>
-      <c r="G38" s="240"/>
+      <c r="C38" s="228"/>
+      <c r="D38" s="228"/>
+      <c r="E38" s="228"/>
+      <c r="F38" s="228"/>
+      <c r="G38" s="229"/>
     </row>
     <row r="39" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A39" s="236"/>
-      <c r="B39" s="241"/>
-      <c r="C39" s="242"/>
-      <c r="D39" s="242"/>
-      <c r="E39" s="242"/>
-      <c r="F39" s="242"/>
-      <c r="G39" s="243"/>
+      <c r="A39" s="249"/>
+      <c r="B39" s="251"/>
+      <c r="C39" s="252"/>
+      <c r="D39" s="252"/>
+      <c r="E39" s="252"/>
+      <c r="F39" s="252"/>
+      <c r="G39" s="253"/>
     </row>
     <row r="40" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A40" s="236"/>
-      <c r="B40" s="244" t="s">
+      <c r="A40" s="249"/>
+      <c r="B40" s="254" t="s">
         <v>491</v>
       </c>
-      <c r="C40" s="245"/>
-      <c r="D40" s="245"/>
-      <c r="E40" s="245"/>
-      <c r="F40" s="245"/>
-      <c r="G40" s="246"/>
+      <c r="C40" s="255"/>
+      <c r="D40" s="255"/>
+      <c r="E40" s="255"/>
+      <c r="F40" s="255"/>
+      <c r="G40" s="256"/>
     </row>
     <row r="41" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A41" s="236"/>
-      <c r="B41" s="224" t="s">
+      <c r="A41" s="249"/>
+      <c r="B41" s="257" t="s">
         <v>492</v>
       </c>
       <c r="C41" s="225"/>
       <c r="D41" s="225"/>
       <c r="E41" s="225"/>
       <c r="F41" s="225"/>
-      <c r="G41" s="226"/>
+      <c r="G41" s="258"/>
     </row>
     <row r="42" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A42" s="236"/>
-      <c r="B42" s="241"/>
-      <c r="C42" s="242"/>
-      <c r="D42" s="242"/>
-      <c r="E42" s="242"/>
-      <c r="F42" s="242"/>
-      <c r="G42" s="243"/>
+      <c r="A42" s="249"/>
+      <c r="B42" s="251"/>
+      <c r="C42" s="252"/>
+      <c r="D42" s="252"/>
+      <c r="E42" s="252"/>
+      <c r="F42" s="252"/>
+      <c r="G42" s="253"/>
     </row>
     <row r="43" spans="1:7" ht="42.95" customHeight="1">
-      <c r="A43" s="236"/>
-      <c r="B43" s="224" t="s">
+      <c r="A43" s="249"/>
+      <c r="B43" s="257" t="s">
         <v>493</v>
       </c>
       <c r="C43" s="225"/>
       <c r="D43" s="225"/>
       <c r="E43" s="225"/>
       <c r="F43" s="225"/>
-      <c r="G43" s="226"/>
+      <c r="G43" s="258"/>
     </row>
     <row r="44" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A44" s="236"/>
-      <c r="B44" s="241"/>
-      <c r="C44" s="242"/>
-      <c r="D44" s="242"/>
-      <c r="E44" s="242"/>
-      <c r="F44" s="242"/>
-      <c r="G44" s="243"/>
+      <c r="A44" s="249"/>
+      <c r="B44" s="251"/>
+      <c r="C44" s="252"/>
+      <c r="D44" s="252"/>
+      <c r="E44" s="252"/>
+      <c r="F44" s="252"/>
+      <c r="G44" s="253"/>
     </row>
     <row r="45" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A45" s="236"/>
-      <c r="B45" s="224" t="s">
+      <c r="A45" s="249"/>
+      <c r="B45" s="257" t="s">
         <v>494</v>
       </c>
       <c r="C45" s="225"/>
       <c r="D45" s="225"/>
       <c r="E45" s="225"/>
       <c r="F45" s="225"/>
-      <c r="G45" s="226"/>
+      <c r="G45" s="258"/>
     </row>
     <row r="46" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A46" s="236"/>
-      <c r="B46" s="224" t="s">
+      <c r="A46" s="249"/>
+      <c r="B46" s="257" t="s">
         <v>495</v>
       </c>
       <c r="C46" s="225"/>
       <c r="D46" s="225"/>
       <c r="E46" s="225"/>
       <c r="F46" s="225"/>
-      <c r="G46" s="226"/>
+      <c r="G46" s="258"/>
     </row>
     <row r="47" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A47" s="236"/>
-      <c r="B47" s="224" t="s">
+      <c r="A47" s="249"/>
+      <c r="B47" s="257" t="s">
         <v>496</v>
       </c>
       <c r="C47" s="225"/>
       <c r="D47" s="225"/>
       <c r="E47" s="225"/>
       <c r="F47" s="225"/>
-      <c r="G47" s="226"/>
+      <c r="G47" s="258"/>
     </row>
     <row r="48" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A48" s="236"/>
-      <c r="B48" s="224" t="s">
+      <c r="A48" s="249"/>
+      <c r="B48" s="257" t="s">
         <v>497</v>
       </c>
       <c r="C48" s="225"/>
       <c r="D48" s="225"/>
       <c r="E48" s="225"/>
       <c r="F48" s="225"/>
-      <c r="G48" s="226"/>
+      <c r="G48" s="258"/>
     </row>
     <row r="49" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A49" s="236"/>
-      <c r="B49" s="224" t="s">
+      <c r="A49" s="249"/>
+      <c r="B49" s="257" t="s">
         <v>498</v>
       </c>
       <c r="C49" s="225"/>
       <c r="D49" s="225"/>
       <c r="E49" s="225"/>
       <c r="F49" s="225"/>
-      <c r="G49" s="226"/>
+      <c r="G49" s="258"/>
     </row>
     <row r="50" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A50" s="236"/>
-      <c r="B50" s="224" t="s">
+      <c r="A50" s="249"/>
+      <c r="B50" s="257" t="s">
         <v>499</v>
       </c>
       <c r="C50" s="225"/>
       <c r="D50" s="225"/>
       <c r="E50" s="225"/>
       <c r="F50" s="225"/>
-      <c r="G50" s="226"/>
+      <c r="G50" s="258"/>
     </row>
     <row r="51" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A51" s="236"/>
-      <c r="B51" s="224" t="s">
+      <c r="A51" s="249"/>
+      <c r="B51" s="257" t="s">
         <v>500</v>
       </c>
       <c r="C51" s="225"/>
       <c r="D51" s="225"/>
       <c r="E51" s="225"/>
       <c r="F51" s="225"/>
-      <c r="G51" s="226"/>
+      <c r="G51" s="258"/>
     </row>
     <row r="52" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A52" s="237"/>
-      <c r="B52" s="227" t="s">
+      <c r="A52" s="250"/>
+      <c r="B52" s="259" t="s">
         <v>501</v>
       </c>
-      <c r="C52" s="228"/>
-      <c r="D52" s="228"/>
-      <c r="E52" s="228"/>
-      <c r="F52" s="228"/>
-      <c r="G52" s="229"/>
+      <c r="C52" s="260"/>
+      <c r="D52" s="260"/>
+      <c r="E52" s="260"/>
+      <c r="F52" s="260"/>
+      <c r="G52" s="261"/>
     </row>
     <row r="53" spans="1:7" ht="57.95" customHeight="1" thickBot="1">
       <c r="A53" s="10" t="s">
         <v>516</v>
       </c>
-      <c r="B53" s="221" t="s">
+      <c r="B53" s="230" t="s">
         <v>581</v>
       </c>
-      <c r="C53" s="222"/>
-      <c r="D53" s="222"/>
-      <c r="E53" s="222"/>
-      <c r="F53" s="222"/>
-      <c r="G53" s="223"/>
+      <c r="C53" s="231"/>
+      <c r="D53" s="231"/>
+      <c r="E53" s="231"/>
+      <c r="F53" s="231"/>
+      <c r="G53" s="232"/>
     </row>
     <row r="54" spans="1:7" ht="57.95" customHeight="1" thickBot="1">
       <c r="A54" s="10" t="s">
         <v>515</v>
       </c>
-      <c r="B54" s="221" t="s">
+      <c r="B54" s="230" t="s">
         <v>502</v>
       </c>
-      <c r="C54" s="222"/>
-      <c r="D54" s="222"/>
-      <c r="E54" s="222"/>
-      <c r="F54" s="222"/>
-      <c r="G54" s="223"/>
+      <c r="C54" s="231"/>
+      <c r="D54" s="231"/>
+      <c r="E54" s="231"/>
+      <c r="F54" s="231"/>
+      <c r="G54" s="232"/>
     </row>
     <row r="55" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A55" s="10" t="s">
         <v>514</v>
       </c>
-      <c r="B55" s="221" t="s">
+      <c r="B55" s="230" t="s">
         <v>503</v>
       </c>
-      <c r="C55" s="222"/>
-      <c r="D55" s="222"/>
-      <c r="E55" s="222"/>
-      <c r="F55" s="222"/>
-      <c r="G55" s="223"/>
+      <c r="C55" s="231"/>
+      <c r="D55" s="231"/>
+      <c r="E55" s="231"/>
+      <c r="F55" s="231"/>
+      <c r="G55" s="232"/>
     </row>
     <row r="56" spans="1:7" ht="42.95" customHeight="1" thickBot="1">
       <c r="A56" s="11" t="s">
         <v>508</v>
       </c>
-      <c r="B56" s="221" t="s">
+      <c r="B56" s="230" t="s">
         <v>504</v>
       </c>
-      <c r="C56" s="222"/>
-      <c r="D56" s="222"/>
-      <c r="E56" s="222"/>
-      <c r="F56" s="222"/>
-      <c r="G56" s="223"/>
+      <c r="C56" s="231"/>
+      <c r="D56" s="231"/>
+      <c r="E56" s="231"/>
+      <c r="F56" s="231"/>
+      <c r="G56" s="232"/>
     </row>
     <row r="57" spans="1:7" ht="29.1" customHeight="1" thickBot="1">
       <c r="A57" s="10" t="s">
         <v>513</v>
       </c>
-      <c r="B57" s="221" t="s">
+      <c r="B57" s="230" t="s">
         <v>505</v>
       </c>
-      <c r="C57" s="222"/>
-      <c r="D57" s="222"/>
-      <c r="E57" s="222"/>
-      <c r="F57" s="222"/>
-      <c r="G57" s="223"/>
+      <c r="C57" s="231"/>
+      <c r="D57" s="231"/>
+      <c r="E57" s="231"/>
+      <c r="F57" s="231"/>
+      <c r="G57" s="232"/>
     </row>
     <row r="58" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A58" s="10" t="s">
         <v>512</v>
       </c>
-      <c r="B58" s="221" t="s">
+      <c r="B58" s="230" t="s">
         <v>506</v>
       </c>
-      <c r="C58" s="222"/>
-      <c r="D58" s="222"/>
-      <c r="E58" s="222"/>
-      <c r="F58" s="222"/>
-      <c r="G58" s="223"/>
+      <c r="C58" s="231"/>
+      <c r="D58" s="231"/>
+      <c r="E58" s="231"/>
+      <c r="F58" s="231"/>
+      <c r="G58" s="232"/>
     </row>
     <row r="59" spans="1:7" ht="42.95" customHeight="1" thickBot="1">
       <c r="A59" s="11" t="s">
         <v>509</v>
       </c>
-      <c r="B59" s="221" t="s">
+      <c r="B59" s="230" t="s">
         <v>510</v>
       </c>
-      <c r="C59" s="222"/>
-      <c r="D59" s="222"/>
-      <c r="E59" s="222"/>
-      <c r="F59" s="222"/>
-      <c r="G59" s="223"/>
+      <c r="C59" s="231"/>
+      <c r="D59" s="231"/>
+      <c r="E59" s="231"/>
+      <c r="F59" s="231"/>
+      <c r="G59" s="232"/>
     </row>
     <row r="60" spans="1:7" ht="29.1" customHeight="1" thickBot="1">
       <c r="A60" s="10" t="s">
         <v>511</v>
       </c>
-      <c r="B60" s="221" t="s">
+      <c r="B60" s="230" t="s">
         <v>507</v>
       </c>
-      <c r="C60" s="222"/>
-      <c r="D60" s="222"/>
-      <c r="E60" s="222"/>
-      <c r="F60" s="222"/>
-      <c r="G60" s="223"/>
+      <c r="C60" s="231"/>
+      <c r="D60" s="231"/>
+      <c r="E60" s="231"/>
+      <c r="F60" s="231"/>
+      <c r="G60" s="232"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="A38:A52"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="B37:G37"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="D29:G29"/>
@@ -41799,49 +41828,17 @@
     <mergeCell ref="D34:G34"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="D35:G35"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="A38:A52"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="B43:G43"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B53:G53"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:G28"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -41852,8 +41849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="E113" sqref="E113"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -42065,10 +42062,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>485</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -42314,10 +42311,10 @@
       <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A23" s="232" t="s">
+      <c r="A23" s="235" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="234"/>
+      <c r="B23" s="237"/>
       <c r="C23" s="4" t="s">
         <v>63</v>
       </c>
@@ -42620,10 +42617,10 @@
       <c r="G38" s="11"/>
     </row>
     <row r="39" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A39" s="232" t="s">
+      <c r="A39" s="235" t="s">
         <v>524</v>
       </c>
-      <c r="B39" s="234"/>
+      <c r="B39" s="237"/>
       <c r="C39" s="4" t="s">
         <v>63</v>
       </c>
@@ -42736,10 +42733,10 @@
       <c r="G44" s="11"/>
     </row>
     <row r="45" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A45" s="232" t="s">
+      <c r="A45" s="235" t="s">
         <v>529</v>
       </c>
-      <c r="B45" s="234"/>
+      <c r="B45" s="237"/>
       <c r="C45" s="4" t="s">
         <v>63</v>
       </c>
@@ -42871,10 +42868,10 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A52" s="232" t="s">
+      <c r="A52" s="235" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="234"/>
+      <c r="B52" s="237"/>
       <c r="C52" s="4" t="s">
         <v>63</v>
       </c>
@@ -43044,10 +43041,10 @@
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A61" s="232" t="s">
+      <c r="A61" s="235" t="s">
         <v>111</v>
       </c>
-      <c r="B61" s="234"/>
+      <c r="B61" s="237"/>
       <c r="C61" s="4" t="s">
         <v>63</v>
       </c>
@@ -43141,10 +43138,10 @@
       <c r="G65" s="11"/>
     </row>
     <row r="66" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A66" s="232" t="s">
+      <c r="A66" s="235" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="234"/>
+      <c r="B66" s="237"/>
       <c r="C66" s="4" t="s">
         <v>63</v>
       </c>
@@ -43434,10 +43431,10 @@
       <c r="G80" s="11"/>
     </row>
     <row r="81" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A81" s="232" t="s">
+      <c r="A81" s="235" t="s">
         <v>133</v>
       </c>
-      <c r="B81" s="234"/>
+      <c r="B81" s="237"/>
       <c r="C81" s="4" t="s">
         <v>63</v>
       </c>
@@ -43571,10 +43568,10 @@
       <c r="G87" s="11"/>
     </row>
     <row r="88" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A88" s="232" t="s">
+      <c r="A88" s="235" t="s">
         <v>558</v>
       </c>
-      <c r="B88" s="234"/>
+      <c r="B88" s="237"/>
       <c r="C88" s="4" t="s">
         <v>63</v>
       </c>
@@ -43602,7 +43599,7 @@
         <v>743</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>58</v>
@@ -43623,7 +43620,7 @@
         <v>741</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>58</v>
@@ -43691,10 +43688,10 @@
       <c r="G93" s="11"/>
     </row>
     <row r="94" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A94" s="232" t="s">
+      <c r="A94" s="235" t="s">
         <v>156</v>
       </c>
-      <c r="B94" s="234"/>
+      <c r="B94" s="237"/>
       <c r="C94" s="4" t="s">
         <v>63</v>
       </c>
@@ -43769,10 +43766,10 @@
       <c r="G97" s="11"/>
     </row>
     <row r="98" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A98" s="232" t="s">
+      <c r="A98" s="235" t="s">
         <v>150</v>
       </c>
-      <c r="B98" s="234"/>
+      <c r="B98" s="237"/>
       <c r="C98" s="4" t="s">
         <v>63</v>
       </c>
@@ -43847,10 +43844,10 @@
       <c r="G101" s="11"/>
     </row>
     <row r="102" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A102" s="232" t="s">
+      <c r="A102" s="235" t="s">
         <v>547</v>
       </c>
-      <c r="B102" s="234"/>
+      <c r="B102" s="237"/>
       <c r="C102" s="4" t="s">
         <v>63</v>
       </c>
@@ -43916,7 +43913,7 @@
         <v>737</v>
       </c>
       <c r="D105" s="11" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E105" s="4" t="s">
         <v>56</v>
@@ -43946,10 +43943,10 @@
       <c r="G106" s="11"/>
     </row>
     <row r="107" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A107" s="232" t="s">
+      <c r="A107" s="235" t="s">
         <v>140</v>
       </c>
-      <c r="B107" s="234"/>
+      <c r="B107" s="237"/>
       <c r="C107" s="4" t="s">
         <v>63</v>
       </c>
@@ -44100,10 +44097,10 @@
       <c r="G114" s="11"/>
     </row>
     <row r="115" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A115" s="232" t="s">
+      <c r="A115" s="235" t="s">
         <v>161</v>
       </c>
-      <c r="B115" s="234"/>
+      <c r="B115" s="237"/>
       <c r="C115" s="4" t="s">
         <v>453</v>
       </c>
@@ -44274,6 +44271,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A88:B88"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="C2:D9"/>
@@ -44283,14 +44288,6 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A88:B88"/>
   </mergeCells>
   <conditionalFormatting sqref="A11:A18 A107:A109 A81:A85 A115:A248 A52:A57 A40 A33:A37 A42:A43 A112 A94:A100 A61:A69 A59 A20:A29">
     <cfRule type="beginsWith" dxfId="2421" priority="1148" stopIfTrue="1" operator="beginsWith" text="Exceptional">
@@ -46526,8 +46523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -46739,10 +46736,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>701</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -46979,7 +46976,7 @@
         <v>685</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>58</v>
@@ -47028,10 +47025,10 @@
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A25" s="232" t="s">
+      <c r="A25" s="235" t="s">
         <v>688</v>
       </c>
-      <c r="B25" s="234"/>
+      <c r="B25" s="237"/>
       <c r="C25" s="4" t="s">
         <v>63</v>
       </c>
@@ -47173,7 +47170,7 @@
         <v>695</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>58</v>
@@ -47241,10 +47238,10 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A36" s="232" t="s">
+      <c r="A36" s="235" t="s">
         <v>612</v>
       </c>
-      <c r="B36" s="234"/>
+      <c r="B36" s="237"/>
       <c r="C36" s="4" t="s">
         <v>63</v>
       </c>
@@ -47663,10 +47660,10 @@
       <c r="G57" s="11"/>
     </row>
     <row r="58" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A58" s="232" t="s">
+      <c r="A58" s="235" t="s">
         <v>627</v>
       </c>
-      <c r="B58" s="234"/>
+      <c r="B58" s="237"/>
       <c r="C58" s="4" t="s">
         <v>63</v>
       </c>
@@ -47884,7 +47881,7 @@
         <v>478</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>56</v>
@@ -47971,10 +47968,10 @@
       <c r="G73" s="11"/>
     </row>
     <row r="74" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A74" s="232" t="s">
+      <c r="A74" s="235" t="s">
         <v>651</v>
       </c>
-      <c r="B74" s="234"/>
+      <c r="B74" s="237"/>
       <c r="C74" s="4" t="s">
         <v>63</v>
       </c>
@@ -48163,10 +48160,10 @@
       <c r="G83" s="11"/>
     </row>
     <row r="84" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A84" s="232" t="s">
+      <c r="A84" s="235" t="s">
         <v>663</v>
       </c>
-      <c r="B84" s="234"/>
+      <c r="B84" s="237"/>
       <c r="C84" s="21" t="s">
         <v>456</v>
       </c>
@@ -48526,10 +48523,10 @@
       <c r="G102" s="11"/>
     </row>
     <row r="103" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A103" s="232" t="s">
+      <c r="A103" s="235" t="s">
         <v>677</v>
       </c>
-      <c r="B103" s="234"/>
+      <c r="B103" s="237"/>
       <c r="C103" s="4" t="s">
         <v>63</v>
       </c>
@@ -48728,7 +48725,7 @@
         <v>675</v>
       </c>
       <c r="D113" s="11" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="E113" s="4" t="s">
         <v>58</v>
@@ -48827,7 +48824,7 @@
         <v>460</v>
       </c>
       <c r="D118" s="11" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E118" s="4" t="s">
         <v>58</v>
@@ -51490,8 +51487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -51703,10 +51700,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>291</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -52066,10 +52063,10 @@
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A29" s="232" t="s">
+      <c r="A29" s="235" t="s">
         <v>564</v>
       </c>
-      <c r="B29" s="234"/>
+      <c r="B29" s="237"/>
       <c r="C29" s="4" t="s">
         <v>451</v>
       </c>
@@ -52298,10 +52295,10 @@
       <c r="G40" s="11"/>
     </row>
     <row r="41" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A41" s="232" t="s">
+      <c r="A41" s="235" t="s">
         <v>334</v>
       </c>
-      <c r="B41" s="234"/>
+      <c r="B41" s="237"/>
       <c r="C41" s="4" t="s">
         <v>63</v>
       </c>
@@ -52407,7 +52404,7 @@
         <v>343</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>58</v>
@@ -52515,10 +52512,10 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" s="7" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A52" s="232" t="s">
+      <c r="A52" s="235" t="s">
         <v>84</v>
       </c>
-      <c r="B52" s="234"/>
+      <c r="B52" s="237"/>
       <c r="C52" s="4" t="s">
         <v>63</v>
       </c>
@@ -52688,10 +52685,10 @@
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" s="7" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A61" s="232" t="s">
+      <c r="A61" s="235" t="s">
         <v>370</v>
       </c>
-      <c r="B61" s="234"/>
+      <c r="B61" s="237"/>
       <c r="C61" s="21" t="s">
         <v>452</v>
       </c>
@@ -53828,7 +53825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
@@ -54041,10 +54038,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>810</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -54347,10 +54344,10 @@
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A26" s="232" t="s">
+      <c r="A26" s="235" t="s">
         <v>390</v>
       </c>
-      <c r="B26" s="234"/>
+      <c r="B26" s="237"/>
       <c r="C26" s="4" t="s">
         <v>855</v>
       </c>
@@ -54617,10 +54614,10 @@
       <c r="G39" s="11"/>
     </row>
     <row r="40" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A40" s="232" t="s">
+      <c r="A40" s="235" t="s">
         <v>448</v>
       </c>
-      <c r="B40" s="234"/>
+      <c r="B40" s="237"/>
       <c r="C40" s="102" t="s">
         <v>856</v>
       </c>
@@ -54885,10 +54882,10 @@
       <c r="G53" s="11"/>
     </row>
     <row r="54" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A54" s="232" t="s">
+      <c r="A54" s="235" t="s">
         <v>412</v>
       </c>
-      <c r="B54" s="234"/>
+      <c r="B54" s="237"/>
       <c r="C54" s="4" t="s">
         <v>63</v>
       </c>
@@ -54956,7 +54953,7 @@
         <v>417</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>58</v>
@@ -56538,8 +56535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -56751,10 +56748,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>239</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -56848,10 +56845,10 @@
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A15" s="232" t="s">
+      <c r="A15" s="235" t="s">
         <v>246</v>
       </c>
-      <c r="B15" s="234"/>
+      <c r="B15" s="237"/>
       <c r="C15" s="4" t="s">
         <v>874</v>
       </c>
@@ -56964,10 +56961,10 @@
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A21" s="232" t="s">
+      <c r="A21" s="235" t="s">
         <v>878</v>
       </c>
-      <c r="B21" s="234"/>
+      <c r="B21" s="237"/>
       <c r="C21" s="4" t="s">
         <v>63</v>
       </c>
@@ -57099,10 +57096,10 @@
       <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A28" s="232" t="s">
+      <c r="A28" s="235" t="s">
         <v>254</v>
       </c>
-      <c r="B28" s="234"/>
+      <c r="B28" s="237"/>
       <c r="C28" s="4" t="s">
         <v>875</v>
       </c>
@@ -57205,9 +57202,7 @@
       <c r="C33" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="D33" s="11" t="s">
-        <v>967</v>
-      </c>
+      <c r="D33" s="11"/>
       <c r="E33" s="4" t="s">
         <v>58</v>
       </c>
@@ -57255,10 +57250,10 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A36" s="232" t="s">
+      <c r="A36" s="235" t="s">
         <v>891</v>
       </c>
-      <c r="B36" s="234"/>
+      <c r="B36" s="237"/>
       <c r="C36" s="4" t="s">
         <v>454</v>
       </c>
@@ -57390,10 +57385,10 @@
       <c r="G42" s="11"/>
     </row>
     <row r="43" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A43" s="232" t="s">
+      <c r="A43" s="235" t="s">
         <v>275</v>
       </c>
-      <c r="B43" s="234"/>
+      <c r="B43" s="237"/>
       <c r="C43" s="4" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Fixed some issues caused by mismatched tags set meta files back to text rather than binary.
</commit_message>
<xml_diff>
--- a/GameDocuments/gam352_papercut_rubric.xlsx
+++ b/GameDocuments/gam352_papercut_rubric.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Game Data" sheetId="1" r:id="rId1"/>
@@ -5759,90 +5759,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -5876,6 +5792,18 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -5933,6 +5861,99 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="4" borderId="16" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="4" borderId="18" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="9" fontId="26" fillId="3" borderId="21" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5943,12 +5964,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="26" fillId="3" borderId="26" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6017,37 +6032,55 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="4" borderId="16" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="4" borderId="18" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6059,28 +6092,28 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6107,52 +6140,19 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -38689,54 +38689,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A1" s="144" t="s">
+      <c r="A1" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="146"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="178"/>
       <c r="E1" s="103"/>
-      <c r="F1" s="144" t="s">
+      <c r="F1" s="176" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
-      <c r="J1" s="146"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="178"/>
       <c r="K1" s="104"/>
       <c r="L1" s="104"/>
       <c r="M1" s="105"/>
     </row>
     <row r="2" spans="1:13" ht="14.1" customHeight="1">
-      <c r="A2" s="147" t="s">
+      <c r="A2" s="182" t="s">
         <v>951</v>
       </c>
-      <c r="B2" s="148"/>
-      <c r="C2" s="148"/>
-      <c r="D2" s="149"/>
+      <c r="B2" s="183"/>
+      <c r="C2" s="183"/>
+      <c r="D2" s="184"/>
       <c r="E2" s="103"/>
-      <c r="F2" s="147" t="s">
+      <c r="F2" s="182" t="s">
         <v>954</v>
       </c>
-      <c r="G2" s="148"/>
-      <c r="H2" s="148"/>
-      <c r="I2" s="148"/>
-      <c r="J2" s="149"/>
+      <c r="G2" s="183"/>
+      <c r="H2" s="183"/>
+      <c r="I2" s="183"/>
+      <c r="J2" s="184"/>
       <c r="K2" s="104"/>
       <c r="L2" s="104"/>
       <c r="M2" s="105"/>
     </row>
     <row r="3" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A3" s="150"/>
-      <c r="B3" s="151"/>
-      <c r="C3" s="151"/>
-      <c r="D3" s="152"/>
+      <c r="A3" s="185"/>
+      <c r="B3" s="186"/>
+      <c r="C3" s="186"/>
+      <c r="D3" s="187"/>
       <c r="E3" s="103"/>
-      <c r="F3" s="150"/>
-      <c r="G3" s="151"/>
-      <c r="H3" s="151"/>
-      <c r="I3" s="151"/>
-      <c r="J3" s="152"/>
+      <c r="F3" s="185"/>
+      <c r="G3" s="186"/>
+      <c r="H3" s="186"/>
+      <c r="I3" s="186"/>
+      <c r="J3" s="187"/>
       <c r="K3" s="104"/>
       <c r="L3" s="104"/>
       <c r="M3" s="105"/>
@@ -38757,41 +38757,41 @@
       <c r="M4" s="105"/>
     </row>
     <row r="5" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A5" s="144" t="s">
+      <c r="A5" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="145"/>
-      <c r="C5" s="145"/>
-      <c r="D5" s="146"/>
+      <c r="B5" s="177"/>
+      <c r="C5" s="177"/>
+      <c r="D5" s="178"/>
       <c r="E5" s="103"/>
-      <c r="F5" s="144" t="s">
+      <c r="F5" s="176" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="145"/>
-      <c r="H5" s="145"/>
-      <c r="I5" s="145"/>
-      <c r="J5" s="146"/>
+      <c r="G5" s="177"/>
+      <c r="H5" s="177"/>
+      <c r="I5" s="177"/>
+      <c r="J5" s="178"/>
       <c r="K5" s="104"/>
       <c r="L5" s="107"/>
       <c r="M5" s="105"/>
     </row>
     <row r="6" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A6" s="156" t="s">
+      <c r="A6" s="173" t="s">
         <v>952</v>
       </c>
-      <c r="B6" s="157"/>
-      <c r="C6" s="157"/>
-      <c r="D6" s="158"/>
+      <c r="B6" s="174"/>
+      <c r="C6" s="174"/>
+      <c r="D6" s="175"/>
       <c r="E6" s="103"/>
-      <c r="F6" s="156" t="s">
+      <c r="F6" s="173" t="s">
         <v>955</v>
       </c>
-      <c r="G6" s="157"/>
-      <c r="H6" s="157"/>
-      <c r="I6" s="157"/>
-      <c r="J6" s="158"/>
+      <c r="G6" s="174"/>
+      <c r="H6" s="174"/>
+      <c r="I6" s="174"/>
+      <c r="J6" s="175"/>
       <c r="K6" s="104"/>
-      <c r="L6" s="153" t="s">
+      <c r="L6" s="170" t="s">
         <v>24</v>
       </c>
       <c r="M6" s="105"/>
@@ -38802,47 +38802,47 @@
       <c r="C7" s="108"/>
       <c r="D7" s="109"/>
       <c r="E7" s="103"/>
-      <c r="F7" s="156"/>
-      <c r="G7" s="157"/>
-      <c r="H7" s="157"/>
-      <c r="I7" s="157"/>
-      <c r="J7" s="158"/>
+      <c r="F7" s="173"/>
+      <c r="G7" s="174"/>
+      <c r="H7" s="174"/>
+      <c r="I7" s="174"/>
+      <c r="J7" s="175"/>
       <c r="K7" s="104"/>
-      <c r="L7" s="154"/>
+      <c r="L7" s="171"/>
       <c r="M7" s="105"/>
     </row>
     <row r="8" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A8" s="144" t="s">
+      <c r="A8" s="176" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="145"/>
-      <c r="C8" s="145"/>
-      <c r="D8" s="146"/>
+      <c r="B8" s="177"/>
+      <c r="C8" s="177"/>
+      <c r="D8" s="178"/>
       <c r="E8" s="103"/>
-      <c r="F8" s="156"/>
-      <c r="G8" s="157"/>
-      <c r="H8" s="157"/>
-      <c r="I8" s="157"/>
-      <c r="J8" s="158"/>
+      <c r="F8" s="173"/>
+      <c r="G8" s="174"/>
+      <c r="H8" s="174"/>
+      <c r="I8" s="174"/>
+      <c r="J8" s="175"/>
       <c r="K8" s="104"/>
-      <c r="L8" s="154"/>
+      <c r="L8" s="171"/>
       <c r="M8" s="105"/>
     </row>
     <row r="9" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A9" s="156" t="s">
+      <c r="A9" s="173" t="s">
         <v>953</v>
       </c>
-      <c r="B9" s="157"/>
-      <c r="C9" s="157"/>
-      <c r="D9" s="158"/>
+      <c r="B9" s="174"/>
+      <c r="C9" s="174"/>
+      <c r="D9" s="175"/>
       <c r="E9" s="103"/>
-      <c r="F9" s="156"/>
-      <c r="G9" s="157"/>
-      <c r="H9" s="157"/>
-      <c r="I9" s="157"/>
-      <c r="J9" s="158"/>
+      <c r="F9" s="173"/>
+      <c r="G9" s="174"/>
+      <c r="H9" s="174"/>
+      <c r="I9" s="174"/>
+      <c r="J9" s="175"/>
       <c r="K9" s="104"/>
-      <c r="L9" s="155"/>
+      <c r="L9" s="172"/>
       <c r="M9" s="105"/>
     </row>
     <row r="10" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -38861,18 +38861,18 @@
       <c r="M10" s="105"/>
     </row>
     <row r="11" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A11" s="144" t="s">
+      <c r="A11" s="176" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="145"/>
-      <c r="C11" s="145"/>
-      <c r="D11" s="146"/>
+      <c r="B11" s="177"/>
+      <c r="C11" s="177"/>
+      <c r="D11" s="178"/>
       <c r="E11" s="103"/>
-      <c r="F11" s="144" t="s">
+      <c r="F11" s="176" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="145"/>
-      <c r="H11" s="146"/>
+      <c r="G11" s="177"/>
+      <c r="H11" s="178"/>
       <c r="I11" s="134" t="s">
         <v>7</v>
       </c>
@@ -38912,7 +38912,7 @@
         <v>-0.12</v>
       </c>
       <c r="K12" s="104"/>
-      <c r="L12" s="153" t="s">
+      <c r="L12" s="170" t="s">
         <v>8</v>
       </c>
       <c r="M12" s="105"/>
@@ -38945,7 +38945,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="120"/>
-      <c r="L13" s="154"/>
+      <c r="L13" s="171"/>
       <c r="M13" s="121"/>
     </row>
     <row r="14" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -38975,7 +38975,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="124"/>
-      <c r="L14" s="155"/>
+      <c r="L14" s="172"/>
       <c r="M14" s="125"/>
     </row>
     <row r="15" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39043,11 +39043,11 @@
         <v>939</v>
       </c>
       <c r="E17" s="104"/>
-      <c r="F17" s="144" t="s">
+      <c r="F17" s="176" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="145"/>
-      <c r="H17" s="146"/>
+      <c r="G17" s="177"/>
+      <c r="H17" s="178"/>
       <c r="I17" s="111"/>
       <c r="J17" s="135">
         <v>0.75</v>
@@ -39073,17 +39073,17 @@
       <c r="F18" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="159" t="s">
+      <c r="G18" s="179" t="s">
         <v>956</v>
       </c>
-      <c r="H18" s="160"/>
-      <c r="I18" s="161"/>
+      <c r="H18" s="180"/>
+      <c r="I18" s="181"/>
       <c r="J18" s="137">
         <f>IF(LEFT(G18,6)="Entire",0,IF(LEFT(G18,6)="Custom",-0.05,-0.1))</f>
         <v>-0.1</v>
       </c>
       <c r="K18" s="128"/>
-      <c r="L18" s="153" t="s">
+      <c r="L18" s="170" t="s">
         <v>18</v>
       </c>
       <c r="M18" s="105"/>
@@ -39103,17 +39103,17 @@
       <c r="F19" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="162" t="s">
+      <c r="G19" s="153" t="s">
         <v>957</v>
       </c>
-      <c r="H19" s="163"/>
-      <c r="I19" s="164"/>
+      <c r="H19" s="154"/>
+      <c r="I19" s="155"/>
       <c r="J19" s="139">
         <f>IF(G19="2D Graphics and 2D Gameplay",IF(J11=0.15,-0.05,0),IF(G19="3D Graphics but 2D Gameplay",IF(J11=0.15,-0.02,-0.3),IF(J11=0.15,0,-0.3)))</f>
         <v>0</v>
       </c>
       <c r="K19" s="104"/>
-      <c r="L19" s="155"/>
+      <c r="L19" s="172"/>
       <c r="M19" s="105"/>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39163,22 +39163,22 @@
       <c r="C22" s="118"/>
       <c r="D22" s="119"/>
       <c r="E22" s="104"/>
-      <c r="F22" s="186" t="s">
+      <c r="F22" s="168" t="s">
         <v>713</v>
       </c>
-      <c r="G22" s="184" t="s">
+      <c r="G22" s="166" t="s">
         <v>714</v>
       </c>
-      <c r="H22" s="183"/>
+      <c r="H22" s="165"/>
       <c r="I22" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="181">
+      <c r="J22" s="163">
         <f>J20+J15</f>
         <v>0.68</v>
       </c>
       <c r="K22" s="104"/>
-      <c r="L22" s="165" t="s">
+      <c r="L22" s="144" t="s">
         <v>725</v>
       </c>
       <c r="M22" s="105"/>
@@ -39189,15 +39189,15 @@
       <c r="C23" s="118"/>
       <c r="D23" s="119"/>
       <c r="E23" s="104"/>
-      <c r="F23" s="187"/>
-      <c r="G23" s="185"/>
-      <c r="H23" s="183"/>
+      <c r="F23" s="169"/>
+      <c r="G23" s="167"/>
+      <c r="H23" s="165"/>
       <c r="I23" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="182"/>
+      <c r="J23" s="164"/>
       <c r="K23" s="104"/>
-      <c r="L23" s="166"/>
+      <c r="L23" s="145"/>
       <c r="M23" s="105"/>
     </row>
     <row r="24" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39221,13 +39221,13 @@
       <c r="C25" s="118"/>
       <c r="D25" s="119"/>
       <c r="E25" s="104"/>
-      <c r="F25" s="175" t="s">
+      <c r="F25" s="157" t="s">
         <v>932</v>
       </c>
-      <c r="G25" s="176"/>
-      <c r="H25" s="176"/>
-      <c r="I25" s="176"/>
-      <c r="J25" s="177"/>
+      <c r="G25" s="158"/>
+      <c r="H25" s="158"/>
+      <c r="I25" s="158"/>
+      <c r="J25" s="159"/>
       <c r="K25" s="104"/>
       <c r="L25" s="104"/>
       <c r="M25" s="105"/>
@@ -39238,11 +39238,11 @@
       <c r="C26" s="118"/>
       <c r="D26" s="119"/>
       <c r="E26" s="103"/>
-      <c r="F26" s="178"/>
-      <c r="G26" s="179"/>
-      <c r="H26" s="179"/>
-      <c r="I26" s="179"/>
-      <c r="J26" s="180"/>
+      <c r="F26" s="160"/>
+      <c r="G26" s="161"/>
+      <c r="H26" s="161"/>
+      <c r="I26" s="161"/>
+      <c r="J26" s="162"/>
       <c r="K26" s="104"/>
       <c r="L26" s="104"/>
       <c r="M26" s="105"/>
@@ -39268,13 +39268,13 @@
       <c r="C28" s="118"/>
       <c r="D28" s="119"/>
       <c r="E28" s="103"/>
-      <c r="F28" s="174" t="s">
+      <c r="F28" s="156" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="174"/>
-      <c r="H28" s="174"/>
-      <c r="I28" s="174"/>
-      <c r="J28" s="174"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
       <c r="K28" s="104"/>
       <c r="L28" s="104"/>
       <c r="M28" s="105"/>
@@ -39285,13 +39285,13 @@
       <c r="C29" s="118"/>
       <c r="D29" s="119"/>
       <c r="E29" s="103"/>
-      <c r="F29" s="171" t="s">
+      <c r="F29" s="150" t="s">
         <v>933</v>
       </c>
-      <c r="G29" s="172"/>
-      <c r="H29" s="172"/>
-      <c r="I29" s="172"/>
-      <c r="J29" s="173"/>
+      <c r="G29" s="151"/>
+      <c r="H29" s="151"/>
+      <c r="I29" s="151"/>
+      <c r="J29" s="152"/>
       <c r="K29" s="104"/>
       <c r="L29" s="104"/>
       <c r="M29" s="105"/>
@@ -39302,30 +39302,30 @@
       <c r="C30" s="118"/>
       <c r="D30" s="119"/>
       <c r="E30" s="103"/>
-      <c r="F30" s="171"/>
-      <c r="G30" s="172"/>
-      <c r="H30" s="172"/>
-      <c r="I30" s="172"/>
-      <c r="J30" s="173"/>
+      <c r="F30" s="150"/>
+      <c r="G30" s="151"/>
+      <c r="H30" s="151"/>
+      <c r="I30" s="151"/>
+      <c r="J30" s="152"/>
       <c r="K30" s="104"/>
       <c r="L30" s="104"/>
       <c r="M30" s="105"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A31" s="167" t="s">
+      <c r="A31" s="146" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="168"/>
-      <c r="C31" s="169" t="s">
+      <c r="B31" s="147"/>
+      <c r="C31" s="148" t="s">
         <v>950</v>
       </c>
-      <c r="D31" s="170"/>
+      <c r="D31" s="149"/>
       <c r="E31" s="104"/>
-      <c r="F31" s="162"/>
-      <c r="G31" s="163"/>
-      <c r="H31" s="163"/>
-      <c r="I31" s="163"/>
-      <c r="J31" s="164"/>
+      <c r="F31" s="153"/>
+      <c r="G31" s="154"/>
+      <c r="H31" s="154"/>
+      <c r="I31" s="154"/>
+      <c r="J31" s="155"/>
       <c r="K31" s="104"/>
       <c r="L31" s="104"/>
       <c r="M31" s="105"/>
@@ -39348,16 +39348,12 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0"/>
   <mergeCells count="31">
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F29:J31"/>
-    <mergeCell ref="F28:J28"/>
-    <mergeCell ref="F25:J26"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A2:D3"/>
+    <mergeCell ref="F2:J3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:J5"/>
     <mergeCell ref="L12:L14"/>
     <mergeCell ref="L18:L19"/>
     <mergeCell ref="A6:D6"/>
@@ -39373,12 +39369,16 @@
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="G18:I18"/>
     <mergeCell ref="G19:I19"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="A2:D3"/>
-    <mergeCell ref="F2:J3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F29:J31"/>
+    <mergeCell ref="F28:J28"/>
+    <mergeCell ref="F25:J26"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F22:F23"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6:D6">
@@ -39421,7 +39421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -39446,57 +39446,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A1" s="194" t="s">
+      <c r="A1" s="199" t="s">
         <v>556</v>
       </c>
-      <c r="B1" s="195"/>
-      <c r="C1" s="195"/>
-      <c r="D1" s="195"/>
-      <c r="E1" s="195"/>
-      <c r="F1" s="195"/>
-      <c r="G1" s="195"/>
-      <c r="H1" s="195"/>
-      <c r="J1" s="205" t="s">
+      <c r="B1" s="200"/>
+      <c r="C1" s="200"/>
+      <c r="D1" s="200"/>
+      <c r="E1" s="200"/>
+      <c r="F1" s="200"/>
+      <c r="G1" s="200"/>
+      <c r="H1" s="200"/>
+      <c r="J1" s="210" t="s">
         <v>482</v>
       </c>
-      <c r="K1" s="206"/>
-      <c r="L1" s="207"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="212"/>
       <c r="M1" s="79"/>
       <c r="N1" s="24" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A2" s="194"/>
-      <c r="B2" s="195"/>
-      <c r="C2" s="195"/>
-      <c r="D2" s="195"/>
-      <c r="E2" s="195"/>
-      <c r="F2" s="195"/>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
-      <c r="J2" s="208" t="s">
+      <c r="A2" s="199"/>
+      <c r="B2" s="200"/>
+      <c r="C2" s="200"/>
+      <c r="D2" s="200"/>
+      <c r="E2" s="200"/>
+      <c r="F2" s="200"/>
+      <c r="G2" s="200"/>
+      <c r="H2" s="200"/>
+      <c r="J2" s="213" t="s">
         <v>706</v>
       </c>
-      <c r="K2" s="209"/>
-      <c r="L2" s="210"/>
+      <c r="K2" s="214"/>
+      <c r="L2" s="215"/>
       <c r="M2" s="23"/>
       <c r="N2" s="26" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A3" s="194"/>
-      <c r="B3" s="195"/>
-      <c r="C3" s="195"/>
-      <c r="D3" s="195"/>
-      <c r="E3" s="195"/>
-      <c r="F3" s="195"/>
-      <c r="G3" s="195"/>
-      <c r="H3" s="195"/>
-      <c r="J3" s="208"/>
-      <c r="K3" s="209"/>
-      <c r="L3" s="210"/>
+      <c r="A3" s="199"/>
+      <c r="B3" s="200"/>
+      <c r="C3" s="200"/>
+      <c r="D3" s="200"/>
+      <c r="E3" s="200"/>
+      <c r="F3" s="200"/>
+      <c r="G3" s="200"/>
+      <c r="H3" s="200"/>
+      <c r="J3" s="213"/>
+      <c r="K3" s="214"/>
+      <c r="L3" s="215"/>
       <c r="M3" s="23"/>
       <c r="N3" s="26" t="s">
         <v>431</v>
@@ -39506,14 +39506,14 @@
       <c r="A4" s="2"/>
       <c r="B4" s="5"/>
       <c r="C4" s="8"/>
-      <c r="D4" s="193"/>
-      <c r="E4" s="193"/>
+      <c r="D4" s="192"/>
+      <c r="E4" s="192"/>
       <c r="F4" s="43"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="193"/>
-      <c r="J4" s="208"/>
-      <c r="K4" s="209"/>
-      <c r="L4" s="210"/>
+      <c r="G4" s="192"/>
+      <c r="H4" s="192"/>
+      <c r="J4" s="213"/>
+      <c r="K4" s="214"/>
+      <c r="L4" s="215"/>
       <c r="M4" s="34"/>
       <c r="N4" s="26" t="s">
         <v>432</v>
@@ -39521,24 +39521,24 @@
       <c r="O4" s="81"/>
     </row>
     <row r="5" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A5" s="196" t="s">
+      <c r="A5" s="201" t="s">
         <v>425</v>
       </c>
-      <c r="B5" s="197"/>
+      <c r="B5" s="202"/>
       <c r="C5" s="8"/>
-      <c r="D5" s="200" t="s">
+      <c r="D5" s="205" t="s">
         <v>717</v>
       </c>
-      <c r="E5" s="201"/>
-      <c r="F5" s="202"/>
-      <c r="G5" s="203">
+      <c r="E5" s="206"/>
+      <c r="F5" s="207"/>
+      <c r="G5" s="208">
         <f>Submission!$E$17</f>
         <v>0</v>
       </c>
-      <c r="H5" s="204"/>
-      <c r="J5" s="208"/>
-      <c r="K5" s="209"/>
-      <c r="L5" s="210"/>
+      <c r="H5" s="209"/>
+      <c r="J5" s="213"/>
+      <c r="K5" s="214"/>
+      <c r="L5" s="215"/>
       <c r="M5" s="34"/>
       <c r="N5" s="26" t="s">
         <v>433</v>
@@ -39546,21 +39546,21 @@
       <c r="O5" s="81"/>
     </row>
     <row r="6" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A6" s="198"/>
-      <c r="B6" s="199"/>
+      <c r="A6" s="203"/>
+      <c r="B6" s="204"/>
       <c r="C6" s="43"/>
-      <c r="D6" s="193" t="s">
+      <c r="D6" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="193"/>
+      <c r="E6" s="192"/>
       <c r="F6" s="43"/>
-      <c r="G6" s="193" t="s">
+      <c r="G6" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="193"/>
-      <c r="J6" s="208"/>
-      <c r="K6" s="209"/>
-      <c r="L6" s="210"/>
+      <c r="H6" s="192"/>
+      <c r="J6" s="213"/>
+      <c r="K6" s="214"/>
+      <c r="L6" s="215"/>
       <c r="M6" s="34"/>
       <c r="N6" s="26" t="s">
         <v>434</v>
@@ -39568,24 +39568,24 @@
       <c r="O6" s="81"/>
     </row>
     <row r="7" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A7" s="188">
+      <c r="A7" s="195">
         <f>'Game Data'!$J$22</f>
         <v>0.68</v>
       </c>
-      <c r="B7" s="189"/>
+      <c r="B7" s="196"/>
       <c r="C7" s="43"/>
-      <c r="D7" s="216" t="s">
+      <c r="D7" s="193" t="s">
         <v>724</v>
       </c>
-      <c r="E7" s="217"/>
+      <c r="E7" s="194"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="216" t="s">
+      <c r="G7" s="193" t="s">
         <v>724</v>
       </c>
-      <c r="H7" s="217"/>
-      <c r="J7" s="208"/>
-      <c r="K7" s="209"/>
-      <c r="L7" s="210"/>
+      <c r="H7" s="194"/>
+      <c r="J7" s="213"/>
+      <c r="K7" s="214"/>
+      <c r="L7" s="215"/>
       <c r="M7" s="33"/>
       <c r="N7" s="26" t="s">
         <v>435</v>
@@ -39593,23 +39593,23 @@
       <c r="O7" s="81"/>
     </row>
     <row r="8" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A8" s="190"/>
-      <c r="B8" s="191"/>
+      <c r="A8" s="197"/>
+      <c r="B8" s="198"/>
       <c r="C8" s="97"/>
-      <c r="D8" s="214">
+      <c r="D8" s="219">
         <f>E17+E26+E35+E44+E53</f>
         <v>0.28000000000000003</v>
       </c>
-      <c r="E8" s="215"/>
+      <c r="E8" s="220"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="214">
+      <c r="G8" s="219">
         <f>H17+H26+H35+H44+H53</f>
         <v>0</v>
       </c>
-      <c r="H8" s="215"/>
-      <c r="J8" s="211"/>
-      <c r="K8" s="212"/>
-      <c r="L8" s="213"/>
+      <c r="H8" s="220"/>
+      <c r="J8" s="216"/>
+      <c r="K8" s="217"/>
+      <c r="L8" s="218"/>
       <c r="M8" s="80"/>
       <c r="N8" s="25" t="s">
         <v>436</v>
@@ -39620,15 +39620,15 @@
       <c r="A9" s="2"/>
       <c r="B9" s="5"/>
       <c r="C9" s="43"/>
-      <c r="D9" s="193" t="s">
+      <c r="D9" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="193"/>
+      <c r="E9" s="192"/>
       <c r="F9" s="43"/>
-      <c r="G9" s="193" t="s">
+      <c r="G9" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="193"/>
+      <c r="H9" s="192"/>
       <c r="J9" s="82"/>
       <c r="K9" s="82"/>
       <c r="L9" s="82"/>
@@ -39655,11 +39655,11 @@
       <c r="H10" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="192" t="s">
+      <c r="J10" s="191" t="s">
         <v>707</v>
       </c>
-      <c r="K10" s="192"/>
-      <c r="L10" s="192"/>
+      <c r="K10" s="191"/>
+      <c r="L10" s="191"/>
       <c r="O10" s="84"/>
     </row>
     <row r="11" spans="1:15" ht="14.1" customHeight="1">
@@ -39688,11 +39688,11 @@
         <f t="shared" ref="H11:H16" si="1">$B11*G11</f>
         <v>0</v>
       </c>
-      <c r="J11" s="220" t="s">
+      <c r="J11" s="190" t="s">
         <v>792</v>
       </c>
-      <c r="K11" s="220"/>
-      <c r="L11" s="220"/>
+      <c r="K11" s="190"/>
+      <c r="L11" s="190"/>
       <c r="M11" s="82"/>
       <c r="O11" s="84"/>
     </row>
@@ -39722,9 +39722,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J12" s="220"/>
-      <c r="K12" s="220"/>
-      <c r="L12" s="220"/>
+      <c r="J12" s="190"/>
+      <c r="K12" s="190"/>
+      <c r="L12" s="190"/>
       <c r="M12" s="82"/>
       <c r="O12" s="84"/>
     </row>
@@ -39754,9 +39754,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="220"/>
-      <c r="K13" s="220"/>
-      <c r="L13" s="220"/>
+      <c r="J13" s="190"/>
+      <c r="K13" s="190"/>
+      <c r="L13" s="190"/>
       <c r="M13" s="82"/>
       <c r="O13" s="84"/>
     </row>
@@ -39822,11 +39822,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J15" s="218">
+      <c r="J15" s="188">
         <f>MAX(0,MIN(1,IF($J17 &lt;= 0.95, ROUND($J17,2), FLOOR((0.95+($J17-0.95)/5),0.01))))</f>
         <v>0.83</v>
       </c>
-      <c r="L15" s="218">
+      <c r="L15" s="188">
         <f>MAX(0,MIN(1,IF($L17 &lt;= 0.95, ROUND($L17,2), FLOOR((0.95+($L17-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -39859,8 +39859,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J16" s="219"/>
-      <c r="L16" s="219"/>
+      <c r="J16" s="189"/>
+      <c r="L16" s="189"/>
       <c r="M16" s="82"/>
       <c r="O16" s="84"/>
     </row>
@@ -39897,15 +39897,15 @@
       <c r="A18" s="2"/>
       <c r="B18" s="5"/>
       <c r="C18" s="43"/>
-      <c r="D18" s="193" t="s">
+      <c r="D18" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="193"/>
+      <c r="E18" s="192"/>
       <c r="F18" s="43"/>
-      <c r="G18" s="193" t="s">
+      <c r="G18" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="193"/>
+      <c r="H18" s="192"/>
       <c r="J18" s="88"/>
       <c r="M18" s="78"/>
     </row>
@@ -39930,11 +39930,11 @@
       <c r="H19" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="192" t="s">
+      <c r="J19" s="191" t="s">
         <v>715</v>
       </c>
-      <c r="K19" s="192"/>
-      <c r="L19" s="192"/>
+      <c r="K19" s="191"/>
+      <c r="L19" s="191"/>
       <c r="M19" s="83"/>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1">
@@ -39963,11 +39963,11 @@
         <f t="shared" ref="H20:H25" si="3">$B20*G20</f>
         <v>0</v>
       </c>
-      <c r="J20" s="220" t="s">
+      <c r="J20" s="190" t="s">
         <v>722</v>
       </c>
-      <c r="K20" s="220"/>
-      <c r="L20" s="220"/>
+      <c r="K20" s="190"/>
+      <c r="L20" s="190"/>
       <c r="M20" s="84"/>
     </row>
     <row r="21" spans="1:13" ht="14.1" customHeight="1">
@@ -39996,9 +39996,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J21" s="220"/>
-      <c r="K21" s="220"/>
-      <c r="L21" s="220"/>
+      <c r="J21" s="190"/>
+      <c r="K21" s="190"/>
+      <c r="L21" s="190"/>
       <c r="M21" s="84"/>
     </row>
     <row r="22" spans="1:13" ht="14.1" customHeight="1">
@@ -40027,9 +40027,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J22" s="220"/>
-      <c r="K22" s="220"/>
-      <c r="L22" s="220"/>
+      <c r="J22" s="190"/>
+      <c r="K22" s="190"/>
+      <c r="L22" s="190"/>
       <c r="M22" s="84"/>
     </row>
     <row r="23" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40093,11 +40093,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J24" s="218">
+      <c r="J24" s="188">
         <f>MAX(0,MIN(1,IF($J26 &lt;= 0.95, ROUND($J26,2), FLOOR((0.95+($J26-0.95)/5),0.01))))</f>
         <v>0.86</v>
       </c>
-      <c r="L24" s="218">
+      <c r="L24" s="188">
         <f>MAX(0,MIN(1,IF($L26 &lt;= 0.95, ROUND($L26,2), FLOOR((0.95+($L26-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40129,8 +40129,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J25" s="219"/>
-      <c r="L25" s="219"/>
+      <c r="J25" s="189"/>
+      <c r="L25" s="189"/>
       <c r="M25" s="84"/>
     </row>
     <row r="26" spans="1:13" ht="14.1" customHeight="1">
@@ -40166,15 +40166,15 @@
       <c r="A27" s="2"/>
       <c r="B27" s="5"/>
       <c r="C27" s="43"/>
-      <c r="D27" s="193" t="s">
+      <c r="D27" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="193"/>
+      <c r="E27" s="192"/>
       <c r="F27" s="43"/>
-      <c r="G27" s="193" t="s">
+      <c r="G27" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H27" s="193"/>
+      <c r="H27" s="192"/>
     </row>
     <row r="28" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
       <c r="A28" s="1" t="s">
@@ -40197,11 +40197,11 @@
       <c r="H28" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J28" s="192" t="s">
+      <c r="J28" s="191" t="s">
         <v>709</v>
       </c>
-      <c r="K28" s="192"/>
-      <c r="L28" s="192"/>
+      <c r="K28" s="191"/>
+      <c r="L28" s="191"/>
     </row>
     <row r="29" spans="1:13" ht="14.1" customHeight="1">
       <c r="A29" s="57" t="str">
@@ -40229,11 +40229,11 @@
         <f t="shared" ref="H29:H34" si="5">$B29*G29</f>
         <v>0</v>
       </c>
-      <c r="J29" s="220" t="s">
+      <c r="J29" s="190" t="s">
         <v>710</v>
       </c>
-      <c r="K29" s="220"/>
-      <c r="L29" s="220"/>
+      <c r="K29" s="190"/>
+      <c r="L29" s="190"/>
     </row>
     <row r="30" spans="1:13" ht="14.1" customHeight="1">
       <c r="A30" s="58" t="str">
@@ -40261,9 +40261,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J30" s="220"/>
-      <c r="K30" s="220"/>
-      <c r="L30" s="220"/>
+      <c r="J30" s="190"/>
+      <c r="K30" s="190"/>
+      <c r="L30" s="190"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1">
       <c r="A31" s="58" t="str">
@@ -40291,9 +40291,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J31" s="220"/>
-      <c r="K31" s="220"/>
-      <c r="L31" s="220"/>
+      <c r="J31" s="190"/>
+      <c r="K31" s="190"/>
+      <c r="L31" s="190"/>
     </row>
     <row r="32" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
       <c r="A32" s="58" t="str">
@@ -40355,11 +40355,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J33" s="218">
+      <c r="J33" s="188">
         <f>MAX(0,MIN(1,IF($J35 &lt;= 0.95, ROUND($J35,2), FLOOR((0.95+($J35-0.95)/5),0.01))))</f>
         <v>0.88</v>
       </c>
-      <c r="L33" s="218">
+      <c r="L33" s="188">
         <f>MAX(0,MIN(1,IF($L35 &lt;= 0.95, ROUND($L35,2), FLOOR((0.95+($L35-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40390,8 +40390,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J34" s="219"/>
-      <c r="L34" s="219"/>
+      <c r="J34" s="189"/>
+      <c r="L34" s="189"/>
     </row>
     <row r="35" spans="1:12" ht="14.1" customHeight="1">
       <c r="A35" s="2"/>
@@ -40425,15 +40425,15 @@
       <c r="A36" s="2"/>
       <c r="B36" s="5"/>
       <c r="C36" s="43"/>
-      <c r="D36" s="193" t="s">
+      <c r="D36" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="193"/>
+      <c r="E36" s="192"/>
       <c r="F36" s="43"/>
-      <c r="G36" s="193" t="s">
+      <c r="G36" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H36" s="193"/>
+      <c r="H36" s="192"/>
     </row>
     <row r="37" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A37" s="1" t="s">
@@ -40456,11 +40456,11 @@
       <c r="H37" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J37" s="192" t="s">
+      <c r="J37" s="191" t="s">
         <v>711</v>
       </c>
-      <c r="K37" s="192"/>
-      <c r="L37" s="192"/>
+      <c r="K37" s="191"/>
+      <c r="L37" s="191"/>
     </row>
     <row r="38" spans="1:12" ht="14.1" customHeight="1">
       <c r="A38" s="57" t="str">
@@ -40488,11 +40488,11 @@
         <f t="shared" ref="H38:H43" si="7">$B38*G38</f>
         <v>0</v>
       </c>
-      <c r="J38" s="220" t="s">
+      <c r="J38" s="190" t="s">
         <v>712</v>
       </c>
-      <c r="K38" s="220"/>
-      <c r="L38" s="220"/>
+      <c r="K38" s="190"/>
+      <c r="L38" s="190"/>
     </row>
     <row r="39" spans="1:12" ht="14.1" customHeight="1">
       <c r="A39" s="58" t="str">
@@ -40520,9 +40520,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J39" s="220"/>
-      <c r="K39" s="220"/>
-      <c r="L39" s="220"/>
+      <c r="J39" s="190"/>
+      <c r="K39" s="190"/>
+      <c r="L39" s="190"/>
     </row>
     <row r="40" spans="1:12" ht="14.1" customHeight="1">
       <c r="A40" s="58" t="str">
@@ -40550,9 +40550,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J40" s="220"/>
-      <c r="K40" s="220"/>
-      <c r="L40" s="220"/>
+      <c r="J40" s="190"/>
+      <c r="K40" s="190"/>
+      <c r="L40" s="190"/>
     </row>
     <row r="41" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A41" s="58" t="str">
@@ -40614,11 +40614,11 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J42" s="218">
+      <c r="J42" s="188">
         <f>MAX(0,MIN(1,IF($J44 &lt;= 0.95, ROUND($J44,2), FLOOR((0.95+($J44-0.95)/5),0.01))))</f>
         <v>0.73</v>
       </c>
-      <c r="L42" s="218">
+      <c r="L42" s="188">
         <f>MAX(0,MIN(1,IF($L44 &lt;= 0.95, ROUND($L44,2), FLOOR((0.95+($L44-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40649,8 +40649,8 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J43" s="219"/>
-      <c r="L43" s="219"/>
+      <c r="J43" s="189"/>
+      <c r="L43" s="189"/>
     </row>
     <row r="44" spans="1:12" ht="14.1" customHeight="1">
       <c r="A44" s="2"/>
@@ -40684,15 +40684,15 @@
       <c r="A45" s="2"/>
       <c r="B45" s="5"/>
       <c r="C45" s="43"/>
-      <c r="D45" s="193" t="s">
+      <c r="D45" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="193"/>
+      <c r="E45" s="192"/>
       <c r="F45" s="43"/>
-      <c r="G45" s="193" t="s">
+      <c r="G45" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="193"/>
+      <c r="H45" s="192"/>
     </row>
     <row r="46" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A46" s="1" t="s">
@@ -40900,34 +40900,6 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="L42:L43"/>
-    <mergeCell ref="J29:L31"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="L33:L34"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="J38:L40"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="J11:L13"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J20:L22"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G36:H36"/>
     <mergeCell ref="A7:B8"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="D6:E6"/>
@@ -40941,6 +40913,34 @@
     <mergeCell ref="J2:L8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G8:H8"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="J11:L13"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J20:L22"/>
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="J29:L31"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="L33:L34"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="J38:L40"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -40951,7 +40951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -40968,59 +40968,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A1" s="235" t="s">
+      <c r="A1" s="232" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="237"/>
+      <c r="B1" s="233"/>
+      <c r="C1" s="233"/>
+      <c r="D1" s="233"/>
+      <c r="E1" s="233"/>
+      <c r="F1" s="233"/>
+      <c r="G1" s="234"/>
     </row>
     <row r="2" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A2" s="230" t="s">
+      <c r="A2" s="221" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="231"/>
-      <c r="C2" s="231"/>
-      <c r="D2" s="231"/>
-      <c r="E2" s="231"/>
-      <c r="F2" s="231"/>
-      <c r="G2" s="232"/>
+      <c r="B2" s="222"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="223"/>
     </row>
     <row r="3" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A3" s="227" t="s">
+      <c r="A3" s="238" t="s">
         <v>930</v>
       </c>
-      <c r="B3" s="228"/>
-      <c r="C3" s="228"/>
-      <c r="D3" s="228"/>
-      <c r="E3" s="228"/>
-      <c r="F3" s="228"/>
-      <c r="G3" s="229"/>
+      <c r="B3" s="239"/>
+      <c r="C3" s="239"/>
+      <c r="D3" s="239"/>
+      <c r="E3" s="239"/>
+      <c r="F3" s="239"/>
+      <c r="G3" s="240"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A4" s="230" t="s">
+      <c r="A4" s="221" t="s">
         <v>438</v>
       </c>
-      <c r="B4" s="231"/>
-      <c r="C4" s="231"/>
-      <c r="D4" s="231"/>
-      <c r="E4" s="231"/>
-      <c r="F4" s="231"/>
-      <c r="G4" s="232"/>
+      <c r="B4" s="222"/>
+      <c r="C4" s="222"/>
+      <c r="D4" s="222"/>
+      <c r="E4" s="222"/>
+      <c r="F4" s="222"/>
+      <c r="G4" s="223"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A5" s="238" t="s">
+      <c r="A5" s="249" t="s">
         <v>580</v>
       </c>
-      <c r="B5" s="239"/>
-      <c r="C5" s="239"/>
-      <c r="D5" s="239"/>
-      <c r="E5" s="239"/>
-      <c r="F5" s="239"/>
-      <c r="G5" s="240"/>
+      <c r="B5" s="250"/>
+      <c r="C5" s="250"/>
+      <c r="D5" s="250"/>
+      <c r="E5" s="250"/>
+      <c r="F5" s="250"/>
+      <c r="G5" s="251"/>
     </row>
     <row r="6" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
       <c r="A6" s="2"/>
@@ -41053,10 +41053,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75">
-      <c r="A8" s="233" t="s">
+      <c r="A8" s="247" t="s">
         <v>718</v>
       </c>
-      <c r="B8" s="234"/>
+      <c r="B8" s="248"/>
       <c r="C8" s="65">
         <v>0</v>
       </c>
@@ -41073,10 +41073,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75">
-      <c r="A9" s="242" t="s">
+      <c r="A9" s="253" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="243"/>
+      <c r="B9" s="254"/>
       <c r="C9" s="92">
         <v>0</v>
       </c>
@@ -41093,10 +41093,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75">
-      <c r="A10" s="244" t="s">
+      <c r="A10" s="255" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="245"/>
+      <c r="B10" s="256"/>
       <c r="C10" s="69">
         <v>0</v>
       </c>
@@ -41113,10 +41113,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75">
-      <c r="A11" s="245" t="s">
+      <c r="A11" s="256" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="245"/>
+      <c r="B11" s="256"/>
       <c r="C11" s="69">
         <v>0</v>
       </c>
@@ -41133,10 +41133,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75">
-      <c r="A12" s="245" t="s">
+      <c r="A12" s="256" t="s">
         <v>716</v>
       </c>
-      <c r="B12" s="245"/>
+      <c r="B12" s="256"/>
       <c r="C12" s="69">
         <v>0</v>
       </c>
@@ -41153,10 +41153,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75">
-      <c r="A13" s="245" t="s">
+      <c r="A13" s="256" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="245"/>
+      <c r="B13" s="256"/>
       <c r="C13" s="69">
         <v>0</v>
       </c>
@@ -41173,10 +41173,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75">
-      <c r="A14" s="244" t="s">
+      <c r="A14" s="255" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="245"/>
+      <c r="B14" s="256"/>
       <c r="C14" s="69">
         <v>0</v>
       </c>
@@ -41193,10 +41193,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75">
-      <c r="A15" s="244" t="s">
+      <c r="A15" s="255" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="245"/>
+      <c r="B15" s="256"/>
       <c r="C15" s="69">
         <v>0</v>
       </c>
@@ -41213,10 +41213,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A16" s="246" t="s">
+      <c r="A16" s="230" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="247"/>
+      <c r="B16" s="231"/>
       <c r="C16" s="73">
         <v>0</v>
       </c>
@@ -41234,11 +41234,11 @@
     </row>
     <row r="17" spans="1:7" ht="14.1" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="241" t="s">
+      <c r="B17" s="252" t="s">
         <v>721</v>
       </c>
-      <c r="C17" s="241"/>
-      <c r="D17" s="241"/>
+      <c r="C17" s="252"/>
+      <c r="D17" s="252"/>
       <c r="E17" s="63">
         <f>SUM(E9:E16)</f>
         <v>0</v>
@@ -41259,527 +41259,559 @@
       <c r="A19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="235" t="s">
+      <c r="B19" s="232" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="236"/>
-      <c r="D19" s="236"/>
-      <c r="E19" s="236"/>
-      <c r="F19" s="236"/>
-      <c r="G19" s="237"/>
+      <c r="C19" s="233"/>
+      <c r="D19" s="233"/>
+      <c r="E19" s="233"/>
+      <c r="F19" s="233"/>
+      <c r="G19" s="234"/>
     </row>
     <row r="20" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="A20" s="10" t="s">
         <v>582</v>
       </c>
-      <c r="B20" s="230" t="s">
+      <c r="B20" s="221" t="s">
         <v>931</v>
       </c>
-      <c r="C20" s="231"/>
-      <c r="D20" s="231"/>
-      <c r="E20" s="231"/>
-      <c r="F20" s="231"/>
-      <c r="G20" s="232"/>
+      <c r="C20" s="222"/>
+      <c r="D20" s="222"/>
+      <c r="E20" s="222"/>
+      <c r="F20" s="222"/>
+      <c r="G20" s="223"/>
     </row>
     <row r="21" spans="1:7" ht="60" customHeight="1" thickBot="1">
       <c r="A21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="230" t="s">
+      <c r="B21" s="221" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="231"/>
-      <c r="D21" s="231"/>
-      <c r="E21" s="231"/>
-      <c r="F21" s="231"/>
-      <c r="G21" s="232"/>
+      <c r="C21" s="222"/>
+      <c r="D21" s="222"/>
+      <c r="E21" s="222"/>
+      <c r="F21" s="222"/>
+      <c r="G21" s="223"/>
     </row>
     <row r="22" spans="1:7" ht="45.95" customHeight="1" thickBot="1">
       <c r="A22" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="230" t="s">
+      <c r="B22" s="221" t="s">
         <v>917</v>
       </c>
-      <c r="C22" s="231"/>
-      <c r="D22" s="231"/>
-      <c r="E22" s="231"/>
-      <c r="F22" s="231"/>
-      <c r="G22" s="232"/>
+      <c r="C22" s="222"/>
+      <c r="D22" s="222"/>
+      <c r="E22" s="222"/>
+      <c r="F22" s="222"/>
+      <c r="G22" s="223"/>
     </row>
     <row r="23" spans="1:7" ht="32.1" customHeight="1">
       <c r="A23" s="98" t="s">
         <v>899</v>
       </c>
-      <c r="B23" s="227" t="s">
+      <c r="B23" s="238" t="s">
         <v>916</v>
       </c>
-      <c r="C23" s="228"/>
-      <c r="D23" s="228"/>
-      <c r="E23" s="228"/>
-      <c r="F23" s="228"/>
-      <c r="G23" s="229"/>
+      <c r="C23" s="239"/>
+      <c r="D23" s="239"/>
+      <c r="E23" s="239"/>
+      <c r="F23" s="239"/>
+      <c r="G23" s="240"/>
     </row>
     <row r="24" spans="1:7" ht="15.75">
       <c r="A24" s="99"/>
-      <c r="B24" s="221" t="s">
+      <c r="B24" s="257" t="s">
         <v>900</v>
       </c>
-      <c r="C24" s="222"/>
-      <c r="D24" s="223" t="s">
+      <c r="C24" s="258"/>
+      <c r="D24" s="260" t="s">
         <v>901</v>
       </c>
-      <c r="E24" s="223"/>
-      <c r="F24" s="223"/>
-      <c r="G24" s="224"/>
+      <c r="E24" s="260"/>
+      <c r="F24" s="260"/>
+      <c r="G24" s="261"/>
     </row>
     <row r="25" spans="1:7" ht="15.75">
       <c r="A25" s="99"/>
-      <c r="B25" s="221" t="s">
+      <c r="B25" s="257" t="s">
         <v>902</v>
       </c>
-      <c r="C25" s="222"/>
-      <c r="D25" s="223" t="s">
+      <c r="C25" s="258"/>
+      <c r="D25" s="260" t="s">
         <v>903</v>
       </c>
-      <c r="E25" s="223"/>
-      <c r="F25" s="223"/>
-      <c r="G25" s="224"/>
+      <c r="E25" s="260"/>
+      <c r="F25" s="260"/>
+      <c r="G25" s="261"/>
     </row>
     <row r="26" spans="1:7" ht="15.75">
       <c r="A26" s="99"/>
-      <c r="B26" s="221" t="s">
+      <c r="B26" s="257" t="s">
         <v>904</v>
       </c>
-      <c r="C26" s="222"/>
-      <c r="D26" s="223" t="s">
+      <c r="C26" s="258"/>
+      <c r="D26" s="260" t="s">
         <v>905</v>
       </c>
-      <c r="E26" s="223"/>
-      <c r="F26" s="223"/>
-      <c r="G26" s="224"/>
+      <c r="E26" s="260"/>
+      <c r="F26" s="260"/>
+      <c r="G26" s="261"/>
     </row>
     <row r="27" spans="1:7" ht="15.75">
       <c r="A27" s="99"/>
-      <c r="B27" s="221" t="s">
+      <c r="B27" s="257" t="s">
         <v>906</v>
       </c>
-      <c r="C27" s="222"/>
+      <c r="C27" s="258"/>
       <c r="D27" s="225" t="s">
         <v>907</v>
       </c>
       <c r="E27" s="225"/>
       <c r="F27" s="225"/>
-      <c r="G27" s="226"/>
+      <c r="G27" s="259"/>
     </row>
     <row r="28" spans="1:7" ht="15.75">
       <c r="A28" s="99"/>
-      <c r="B28" s="221" t="s">
+      <c r="B28" s="257" t="s">
         <v>908</v>
       </c>
-      <c r="C28" s="222"/>
-      <c r="D28" s="223" t="s">
+      <c r="C28" s="258"/>
+      <c r="D28" s="260" t="s">
         <v>909</v>
       </c>
-      <c r="E28" s="223"/>
-      <c r="F28" s="223"/>
-      <c r="G28" s="224"/>
+      <c r="E28" s="260"/>
+      <c r="F28" s="260"/>
+      <c r="G28" s="261"/>
     </row>
     <row r="29" spans="1:7" ht="15.75">
       <c r="A29" s="99"/>
-      <c r="B29" s="221" t="s">
+      <c r="B29" s="257" t="s">
         <v>910</v>
       </c>
-      <c r="C29" s="222"/>
+      <c r="C29" s="258"/>
       <c r="D29" s="225" t="s">
         <v>911</v>
       </c>
       <c r="E29" s="225"/>
       <c r="F29" s="225"/>
-      <c r="G29" s="226"/>
+      <c r="G29" s="259"/>
     </row>
     <row r="30" spans="1:7" ht="15.75">
       <c r="A30" s="99"/>
-      <c r="B30" s="221" t="s">
+      <c r="B30" s="257" t="s">
         <v>914</v>
       </c>
-      <c r="C30" s="222"/>
-      <c r="D30" s="223" t="s">
+      <c r="C30" s="258"/>
+      <c r="D30" s="260" t="s">
         <v>915</v>
       </c>
-      <c r="E30" s="223"/>
-      <c r="F30" s="223"/>
-      <c r="G30" s="224"/>
+      <c r="E30" s="260"/>
+      <c r="F30" s="260"/>
+      <c r="G30" s="261"/>
     </row>
     <row r="31" spans="1:7" ht="15.75">
       <c r="A31" s="99"/>
-      <c r="B31" s="221" t="s">
+      <c r="B31" s="257" t="s">
         <v>912</v>
       </c>
-      <c r="C31" s="222"/>
+      <c r="C31" s="258"/>
       <c r="D31" s="225" t="s">
         <v>913</v>
       </c>
       <c r="E31" s="225"/>
       <c r="F31" s="225"/>
-      <c r="G31" s="226"/>
+      <c r="G31" s="259"/>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickBot="1">
       <c r="A32" s="99"/>
-      <c r="B32" s="221" t="s">
+      <c r="B32" s="257" t="s">
         <v>928</v>
       </c>
-      <c r="C32" s="222"/>
+      <c r="C32" s="258"/>
       <c r="D32" s="225" t="s">
         <v>929</v>
       </c>
       <c r="E32" s="225"/>
       <c r="F32" s="225"/>
-      <c r="G32" s="226"/>
+      <c r="G32" s="259"/>
     </row>
     <row r="33" spans="1:7" ht="15.75">
       <c r="A33" s="98" t="s">
         <v>918</v>
       </c>
-      <c r="B33" s="227" t="s">
+      <c r="B33" s="238" t="s">
         <v>919</v>
       </c>
-      <c r="C33" s="228"/>
-      <c r="D33" s="228"/>
-      <c r="E33" s="228"/>
-      <c r="F33" s="228"/>
-      <c r="G33" s="229"/>
+      <c r="C33" s="239"/>
+      <c r="D33" s="239"/>
+      <c r="E33" s="239"/>
+      <c r="F33" s="239"/>
+      <c r="G33" s="240"/>
     </row>
     <row r="34" spans="1:7" ht="15.75">
       <c r="A34" s="99"/>
-      <c r="B34" s="221" t="s">
+      <c r="B34" s="257" t="s">
         <v>920</v>
       </c>
-      <c r="C34" s="222"/>
-      <c r="D34" s="223" t="s">
+      <c r="C34" s="258"/>
+      <c r="D34" s="260" t="s">
         <v>925</v>
       </c>
-      <c r="E34" s="223"/>
-      <c r="F34" s="223"/>
-      <c r="G34" s="224"/>
+      <c r="E34" s="260"/>
+      <c r="F34" s="260"/>
+      <c r="G34" s="261"/>
     </row>
     <row r="35" spans="1:7" ht="15.75">
       <c r="A35" s="99"/>
-      <c r="B35" s="221" t="s">
+      <c r="B35" s="257" t="s">
         <v>921</v>
       </c>
-      <c r="C35" s="222"/>
-      <c r="D35" s="223" t="s">
+      <c r="C35" s="258"/>
+      <c r="D35" s="260" t="s">
         <v>926</v>
       </c>
-      <c r="E35" s="223"/>
-      <c r="F35" s="223"/>
-      <c r="G35" s="224"/>
+      <c r="E35" s="260"/>
+      <c r="F35" s="260"/>
+      <c r="G35" s="261"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" thickBot="1">
       <c r="A36" s="99"/>
-      <c r="B36" s="221" t="s">
+      <c r="B36" s="257" t="s">
         <v>922</v>
       </c>
-      <c r="C36" s="222"/>
-      <c r="D36" s="223" t="s">
+      <c r="C36" s="258"/>
+      <c r="D36" s="260" t="s">
         <v>927</v>
       </c>
-      <c r="E36" s="223"/>
-      <c r="F36" s="223"/>
-      <c r="G36" s="224"/>
+      <c r="E36" s="260"/>
+      <c r="F36" s="260"/>
+      <c r="G36" s="261"/>
     </row>
     <row r="37" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="A37" s="98" t="s">
         <v>923</v>
       </c>
-      <c r="B37" s="227" t="s">
+      <c r="B37" s="238" t="s">
         <v>924</v>
       </c>
-      <c r="C37" s="228"/>
-      <c r="D37" s="228"/>
-      <c r="E37" s="228"/>
-      <c r="F37" s="228"/>
-      <c r="G37" s="229"/>
+      <c r="C37" s="239"/>
+      <c r="D37" s="239"/>
+      <c r="E37" s="239"/>
+      <c r="F37" s="239"/>
+      <c r="G37" s="240"/>
     </row>
     <row r="38" spans="1:7" ht="29.1" customHeight="1">
-      <c r="A38" s="248" t="s">
+      <c r="A38" s="235" t="s">
         <v>517</v>
       </c>
-      <c r="B38" s="227" t="s">
+      <c r="B38" s="238" t="s">
         <v>490</v>
       </c>
-      <c r="C38" s="228"/>
-      <c r="D38" s="228"/>
-      <c r="E38" s="228"/>
-      <c r="F38" s="228"/>
-      <c r="G38" s="229"/>
+      <c r="C38" s="239"/>
+      <c r="D38" s="239"/>
+      <c r="E38" s="239"/>
+      <c r="F38" s="239"/>
+      <c r="G38" s="240"/>
     </row>
     <row r="39" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A39" s="249"/>
-      <c r="B39" s="251"/>
-      <c r="C39" s="252"/>
-      <c r="D39" s="252"/>
-      <c r="E39" s="252"/>
-      <c r="F39" s="252"/>
-      <c r="G39" s="253"/>
+      <c r="A39" s="236"/>
+      <c r="B39" s="241"/>
+      <c r="C39" s="242"/>
+      <c r="D39" s="242"/>
+      <c r="E39" s="242"/>
+      <c r="F39" s="242"/>
+      <c r="G39" s="243"/>
     </row>
     <row r="40" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A40" s="249"/>
-      <c r="B40" s="254" t="s">
+      <c r="A40" s="236"/>
+      <c r="B40" s="244" t="s">
         <v>491</v>
       </c>
-      <c r="C40" s="255"/>
-      <c r="D40" s="255"/>
-      <c r="E40" s="255"/>
-      <c r="F40" s="255"/>
-      <c r="G40" s="256"/>
+      <c r="C40" s="245"/>
+      <c r="D40" s="245"/>
+      <c r="E40" s="245"/>
+      <c r="F40" s="245"/>
+      <c r="G40" s="246"/>
     </row>
     <row r="41" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A41" s="249"/>
-      <c r="B41" s="257" t="s">
+      <c r="A41" s="236"/>
+      <c r="B41" s="224" t="s">
         <v>492</v>
       </c>
       <c r="C41" s="225"/>
       <c r="D41" s="225"/>
       <c r="E41" s="225"/>
       <c r="F41" s="225"/>
-      <c r="G41" s="258"/>
+      <c r="G41" s="226"/>
     </row>
     <row r="42" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A42" s="249"/>
-      <c r="B42" s="251"/>
-      <c r="C42" s="252"/>
-      <c r="D42" s="252"/>
-      <c r="E42" s="252"/>
-      <c r="F42" s="252"/>
-      <c r="G42" s="253"/>
+      <c r="A42" s="236"/>
+      <c r="B42" s="241"/>
+      <c r="C42" s="242"/>
+      <c r="D42" s="242"/>
+      <c r="E42" s="242"/>
+      <c r="F42" s="242"/>
+      <c r="G42" s="243"/>
     </row>
     <row r="43" spans="1:7" ht="42.95" customHeight="1">
-      <c r="A43" s="249"/>
-      <c r="B43" s="257" t="s">
+      <c r="A43" s="236"/>
+      <c r="B43" s="224" t="s">
         <v>493</v>
       </c>
       <c r="C43" s="225"/>
       <c r="D43" s="225"/>
       <c r="E43" s="225"/>
       <c r="F43" s="225"/>
-      <c r="G43" s="258"/>
+      <c r="G43" s="226"/>
     </row>
     <row r="44" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A44" s="249"/>
-      <c r="B44" s="251"/>
-      <c r="C44" s="252"/>
-      <c r="D44" s="252"/>
-      <c r="E44" s="252"/>
-      <c r="F44" s="252"/>
-      <c r="G44" s="253"/>
+      <c r="A44" s="236"/>
+      <c r="B44" s="241"/>
+      <c r="C44" s="242"/>
+      <c r="D44" s="242"/>
+      <c r="E44" s="242"/>
+      <c r="F44" s="242"/>
+      <c r="G44" s="243"/>
     </row>
     <row r="45" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A45" s="249"/>
-      <c r="B45" s="257" t="s">
+      <c r="A45" s="236"/>
+      <c r="B45" s="224" t="s">
         <v>494</v>
       </c>
       <c r="C45" s="225"/>
       <c r="D45" s="225"/>
       <c r="E45" s="225"/>
       <c r="F45" s="225"/>
-      <c r="G45" s="258"/>
+      <c r="G45" s="226"/>
     </row>
     <row r="46" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A46" s="249"/>
-      <c r="B46" s="257" t="s">
+      <c r="A46" s="236"/>
+      <c r="B46" s="224" t="s">
         <v>495</v>
       </c>
       <c r="C46" s="225"/>
       <c r="D46" s="225"/>
       <c r="E46" s="225"/>
       <c r="F46" s="225"/>
-      <c r="G46" s="258"/>
+      <c r="G46" s="226"/>
     </row>
     <row r="47" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A47" s="249"/>
-      <c r="B47" s="257" t="s">
+      <c r="A47" s="236"/>
+      <c r="B47" s="224" t="s">
         <v>496</v>
       </c>
       <c r="C47" s="225"/>
       <c r="D47" s="225"/>
       <c r="E47" s="225"/>
       <c r="F47" s="225"/>
-      <c r="G47" s="258"/>
+      <c r="G47" s="226"/>
     </row>
     <row r="48" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A48" s="249"/>
-      <c r="B48" s="257" t="s">
+      <c r="A48" s="236"/>
+      <c r="B48" s="224" t="s">
         <v>497</v>
       </c>
       <c r="C48" s="225"/>
       <c r="D48" s="225"/>
       <c r="E48" s="225"/>
       <c r="F48" s="225"/>
-      <c r="G48" s="258"/>
+      <c r="G48" s="226"/>
     </row>
     <row r="49" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A49" s="249"/>
-      <c r="B49" s="257" t="s">
+      <c r="A49" s="236"/>
+      <c r="B49" s="224" t="s">
         <v>498</v>
       </c>
       <c r="C49" s="225"/>
       <c r="D49" s="225"/>
       <c r="E49" s="225"/>
       <c r="F49" s="225"/>
-      <c r="G49" s="258"/>
+      <c r="G49" s="226"/>
     </row>
     <row r="50" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A50" s="249"/>
-      <c r="B50" s="257" t="s">
+      <c r="A50" s="236"/>
+      <c r="B50" s="224" t="s">
         <v>499</v>
       </c>
       <c r="C50" s="225"/>
       <c r="D50" s="225"/>
       <c r="E50" s="225"/>
       <c r="F50" s="225"/>
-      <c r="G50" s="258"/>
+      <c r="G50" s="226"/>
     </row>
     <row r="51" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A51" s="249"/>
-      <c r="B51" s="257" t="s">
+      <c r="A51" s="236"/>
+      <c r="B51" s="224" t="s">
         <v>500</v>
       </c>
       <c r="C51" s="225"/>
       <c r="D51" s="225"/>
       <c r="E51" s="225"/>
       <c r="F51" s="225"/>
-      <c r="G51" s="258"/>
+      <c r="G51" s="226"/>
     </row>
     <row r="52" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A52" s="250"/>
-      <c r="B52" s="259" t="s">
+      <c r="A52" s="237"/>
+      <c r="B52" s="227" t="s">
         <v>501</v>
       </c>
-      <c r="C52" s="260"/>
-      <c r="D52" s="260"/>
-      <c r="E52" s="260"/>
-      <c r="F52" s="260"/>
-      <c r="G52" s="261"/>
+      <c r="C52" s="228"/>
+      <c r="D52" s="228"/>
+      <c r="E52" s="228"/>
+      <c r="F52" s="228"/>
+      <c r="G52" s="229"/>
     </row>
     <row r="53" spans="1:7" ht="57.95" customHeight="1" thickBot="1">
       <c r="A53" s="10" t="s">
         <v>516</v>
       </c>
-      <c r="B53" s="230" t="s">
+      <c r="B53" s="221" t="s">
         <v>581</v>
       </c>
-      <c r="C53" s="231"/>
-      <c r="D53" s="231"/>
-      <c r="E53" s="231"/>
-      <c r="F53" s="231"/>
-      <c r="G53" s="232"/>
+      <c r="C53" s="222"/>
+      <c r="D53" s="222"/>
+      <c r="E53" s="222"/>
+      <c r="F53" s="222"/>
+      <c r="G53" s="223"/>
     </row>
     <row r="54" spans="1:7" ht="57.95" customHeight="1" thickBot="1">
       <c r="A54" s="10" t="s">
         <v>515</v>
       </c>
-      <c r="B54" s="230" t="s">
+      <c r="B54" s="221" t="s">
         <v>502</v>
       </c>
-      <c r="C54" s="231"/>
-      <c r="D54" s="231"/>
-      <c r="E54" s="231"/>
-      <c r="F54" s="231"/>
-      <c r="G54" s="232"/>
+      <c r="C54" s="222"/>
+      <c r="D54" s="222"/>
+      <c r="E54" s="222"/>
+      <c r="F54" s="222"/>
+      <c r="G54" s="223"/>
     </row>
     <row r="55" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A55" s="10" t="s">
         <v>514</v>
       </c>
-      <c r="B55" s="230" t="s">
+      <c r="B55" s="221" t="s">
         <v>503</v>
       </c>
-      <c r="C55" s="231"/>
-      <c r="D55" s="231"/>
-      <c r="E55" s="231"/>
-      <c r="F55" s="231"/>
-      <c r="G55" s="232"/>
+      <c r="C55" s="222"/>
+      <c r="D55" s="222"/>
+      <c r="E55" s="222"/>
+      <c r="F55" s="222"/>
+      <c r="G55" s="223"/>
     </row>
     <row r="56" spans="1:7" ht="42.95" customHeight="1" thickBot="1">
       <c r="A56" s="11" t="s">
         <v>508</v>
       </c>
-      <c r="B56" s="230" t="s">
+      <c r="B56" s="221" t="s">
         <v>504</v>
       </c>
-      <c r="C56" s="231"/>
-      <c r="D56" s="231"/>
-      <c r="E56" s="231"/>
-      <c r="F56" s="231"/>
-      <c r="G56" s="232"/>
+      <c r="C56" s="222"/>
+      <c r="D56" s="222"/>
+      <c r="E56" s="222"/>
+      <c r="F56" s="222"/>
+      <c r="G56" s="223"/>
     </row>
     <row r="57" spans="1:7" ht="29.1" customHeight="1" thickBot="1">
       <c r="A57" s="10" t="s">
         <v>513</v>
       </c>
-      <c r="B57" s="230" t="s">
+      <c r="B57" s="221" t="s">
         <v>505</v>
       </c>
-      <c r="C57" s="231"/>
-      <c r="D57" s="231"/>
-      <c r="E57" s="231"/>
-      <c r="F57" s="231"/>
-      <c r="G57" s="232"/>
+      <c r="C57" s="222"/>
+      <c r="D57" s="222"/>
+      <c r="E57" s="222"/>
+      <c r="F57" s="222"/>
+      <c r="G57" s="223"/>
     </row>
     <row r="58" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A58" s="10" t="s">
         <v>512</v>
       </c>
-      <c r="B58" s="230" t="s">
+      <c r="B58" s="221" t="s">
         <v>506</v>
       </c>
-      <c r="C58" s="231"/>
-      <c r="D58" s="231"/>
-      <c r="E58" s="231"/>
-      <c r="F58" s="231"/>
-      <c r="G58" s="232"/>
+      <c r="C58" s="222"/>
+      <c r="D58" s="222"/>
+      <c r="E58" s="222"/>
+      <c r="F58" s="222"/>
+      <c r="G58" s="223"/>
     </row>
     <row r="59" spans="1:7" ht="42.95" customHeight="1" thickBot="1">
       <c r="A59" s="11" t="s">
         <v>509</v>
       </c>
-      <c r="B59" s="230" t="s">
+      <c r="B59" s="221" t="s">
         <v>510</v>
       </c>
-      <c r="C59" s="231"/>
-      <c r="D59" s="231"/>
-      <c r="E59" s="231"/>
-      <c r="F59" s="231"/>
-      <c r="G59" s="232"/>
+      <c r="C59" s="222"/>
+      <c r="D59" s="222"/>
+      <c r="E59" s="222"/>
+      <c r="F59" s="222"/>
+      <c r="G59" s="223"/>
     </row>
     <row r="60" spans="1:7" ht="29.1" customHeight="1" thickBot="1">
       <c r="A60" s="10" t="s">
         <v>511</v>
       </c>
-      <c r="B60" s="230" t="s">
+      <c r="B60" s="221" t="s">
         <v>507</v>
       </c>
-      <c r="C60" s="231"/>
-      <c r="D60" s="231"/>
-      <c r="E60" s="231"/>
-      <c r="F60" s="231"/>
-      <c r="G60" s="232"/>
+      <c r="C60" s="222"/>
+      <c r="D60" s="222"/>
+      <c r="E60" s="222"/>
+      <c r="F60" s="222"/>
+      <c r="G60" s="223"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:G59"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B53:G53"/>
-    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B20:G20"/>
@@ -41796,49 +41828,17 @@
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="B48:G48"/>
     <mergeCell ref="B49:G49"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:G36"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:G35"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B59:G59"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -41849,7 +41849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -42062,10 +42062,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="232" t="s">
         <v>485</v>
       </c>
-      <c r="B10" s="237"/>
+      <c r="B10" s="234"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -42311,10 +42311,10 @@
       <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A23" s="235" t="s">
+      <c r="A23" s="232" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="237"/>
+      <c r="B23" s="234"/>
       <c r="C23" s="4" t="s">
         <v>63</v>
       </c>
@@ -42617,10 +42617,10 @@
       <c r="G38" s="11"/>
     </row>
     <row r="39" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A39" s="235" t="s">
+      <c r="A39" s="232" t="s">
         <v>524</v>
       </c>
-      <c r="B39" s="237"/>
+      <c r="B39" s="234"/>
       <c r="C39" s="4" t="s">
         <v>63</v>
       </c>
@@ -42733,10 +42733,10 @@
       <c r="G44" s="11"/>
     </row>
     <row r="45" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A45" s="235" t="s">
+      <c r="A45" s="232" t="s">
         <v>529</v>
       </c>
-      <c r="B45" s="237"/>
+      <c r="B45" s="234"/>
       <c r="C45" s="4" t="s">
         <v>63</v>
       </c>
@@ -42868,10 +42868,10 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A52" s="235" t="s">
+      <c r="A52" s="232" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="237"/>
+      <c r="B52" s="234"/>
       <c r="C52" s="4" t="s">
         <v>63</v>
       </c>
@@ -43041,10 +43041,10 @@
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A61" s="235" t="s">
+      <c r="A61" s="232" t="s">
         <v>111</v>
       </c>
-      <c r="B61" s="237"/>
+      <c r="B61" s="234"/>
       <c r="C61" s="4" t="s">
         <v>63</v>
       </c>
@@ -43138,10 +43138,10 @@
       <c r="G65" s="11"/>
     </row>
     <row r="66" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A66" s="235" t="s">
+      <c r="A66" s="232" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="237"/>
+      <c r="B66" s="234"/>
       <c r="C66" s="4" t="s">
         <v>63</v>
       </c>
@@ -43431,10 +43431,10 @@
       <c r="G80" s="11"/>
     </row>
     <row r="81" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A81" s="235" t="s">
+      <c r="A81" s="232" t="s">
         <v>133</v>
       </c>
-      <c r="B81" s="237"/>
+      <c r="B81" s="234"/>
       <c r="C81" s="4" t="s">
         <v>63</v>
       </c>
@@ -43568,10 +43568,10 @@
       <c r="G87" s="11"/>
     </row>
     <row r="88" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A88" s="235" t="s">
+      <c r="A88" s="232" t="s">
         <v>558</v>
       </c>
-      <c r="B88" s="237"/>
+      <c r="B88" s="234"/>
       <c r="C88" s="4" t="s">
         <v>63</v>
       </c>
@@ -43688,10 +43688,10 @@
       <c r="G93" s="11"/>
     </row>
     <row r="94" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A94" s="235" t="s">
+      <c r="A94" s="232" t="s">
         <v>156</v>
       </c>
-      <c r="B94" s="237"/>
+      <c r="B94" s="234"/>
       <c r="C94" s="4" t="s">
         <v>63</v>
       </c>
@@ -43766,10 +43766,10 @@
       <c r="G97" s="11"/>
     </row>
     <row r="98" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A98" s="235" t="s">
+      <c r="A98" s="232" t="s">
         <v>150</v>
       </c>
-      <c r="B98" s="237"/>
+      <c r="B98" s="234"/>
       <c r="C98" s="4" t="s">
         <v>63</v>
       </c>
@@ -43844,10 +43844,10 @@
       <c r="G101" s="11"/>
     </row>
     <row r="102" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A102" s="235" t="s">
+      <c r="A102" s="232" t="s">
         <v>547</v>
       </c>
-      <c r="B102" s="237"/>
+      <c r="B102" s="234"/>
       <c r="C102" s="4" t="s">
         <v>63</v>
       </c>
@@ -43943,10 +43943,10 @@
       <c r="G106" s="11"/>
     </row>
     <row r="107" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A107" s="235" t="s">
+      <c r="A107" s="232" t="s">
         <v>140</v>
       </c>
-      <c r="B107" s="237"/>
+      <c r="B107" s="234"/>
       <c r="C107" s="4" t="s">
         <v>63</v>
       </c>
@@ -44097,10 +44097,10 @@
       <c r="G114" s="11"/>
     </row>
     <row r="115" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A115" s="235" t="s">
+      <c r="A115" s="232" t="s">
         <v>161</v>
       </c>
-      <c r="B115" s="237"/>
+      <c r="B115" s="234"/>
       <c r="C115" s="4" t="s">
         <v>453</v>
       </c>
@@ -44271,14 +44271,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A88:B88"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="C2:D9"/>
@@ -44288,6 +44280,14 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A88:B88"/>
   </mergeCells>
   <conditionalFormatting sqref="A11:A18 A107:A109 A81:A85 A115:A248 A52:A57 A40 A33:A37 A42:A43 A112 A94:A100 A61:A69 A59 A20:A29">
     <cfRule type="beginsWith" dxfId="2421" priority="1148" stopIfTrue="1" operator="beginsWith" text="Exceptional">
@@ -46736,10 +46736,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="232" t="s">
         <v>701</v>
       </c>
-      <c r="B10" s="237"/>
+      <c r="B10" s="234"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -47025,10 +47025,10 @@
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A25" s="235" t="s">
+      <c r="A25" s="232" t="s">
         <v>688</v>
       </c>
-      <c r="B25" s="237"/>
+      <c r="B25" s="234"/>
       <c r="C25" s="4" t="s">
         <v>63</v>
       </c>
@@ -47238,10 +47238,10 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A36" s="235" t="s">
+      <c r="A36" s="232" t="s">
         <v>612</v>
       </c>
-      <c r="B36" s="237"/>
+      <c r="B36" s="234"/>
       <c r="C36" s="4" t="s">
         <v>63</v>
       </c>
@@ -47660,10 +47660,10 @@
       <c r="G57" s="11"/>
     </row>
     <row r="58" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A58" s="235" t="s">
+      <c r="A58" s="232" t="s">
         <v>627</v>
       </c>
-      <c r="B58" s="237"/>
+      <c r="B58" s="234"/>
       <c r="C58" s="4" t="s">
         <v>63</v>
       </c>
@@ -47968,10 +47968,10 @@
       <c r="G73" s="11"/>
     </row>
     <row r="74" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A74" s="235" t="s">
+      <c r="A74" s="232" t="s">
         <v>651</v>
       </c>
-      <c r="B74" s="237"/>
+      <c r="B74" s="234"/>
       <c r="C74" s="4" t="s">
         <v>63</v>
       </c>
@@ -48160,10 +48160,10 @@
       <c r="G83" s="11"/>
     </row>
     <row r="84" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A84" s="235" t="s">
+      <c r="A84" s="232" t="s">
         <v>663</v>
       </c>
-      <c r="B84" s="237"/>
+      <c r="B84" s="234"/>
       <c r="C84" s="21" t="s">
         <v>456</v>
       </c>
@@ -48523,10 +48523,10 @@
       <c r="G102" s="11"/>
     </row>
     <row r="103" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A103" s="235" t="s">
+      <c r="A103" s="232" t="s">
         <v>677</v>
       </c>
-      <c r="B103" s="237"/>
+      <c r="B103" s="234"/>
       <c r="C103" s="4" t="s">
         <v>63</v>
       </c>
@@ -51700,10 +51700,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="232" t="s">
         <v>291</v>
       </c>
-      <c r="B10" s="237"/>
+      <c r="B10" s="234"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -52063,10 +52063,10 @@
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A29" s="235" t="s">
+      <c r="A29" s="232" t="s">
         <v>564</v>
       </c>
-      <c r="B29" s="237"/>
+      <c r="B29" s="234"/>
       <c r="C29" s="4" t="s">
         <v>451</v>
       </c>
@@ -52295,10 +52295,10 @@
       <c r="G40" s="11"/>
     </row>
     <row r="41" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A41" s="235" t="s">
+      <c r="A41" s="232" t="s">
         <v>334</v>
       </c>
-      <c r="B41" s="237"/>
+      <c r="B41" s="234"/>
       <c r="C41" s="4" t="s">
         <v>63</v>
       </c>
@@ -52512,10 +52512,10 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" s="7" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A52" s="235" t="s">
+      <c r="A52" s="232" t="s">
         <v>84</v>
       </c>
-      <c r="B52" s="237"/>
+      <c r="B52" s="234"/>
       <c r="C52" s="4" t="s">
         <v>63</v>
       </c>
@@ -52685,10 +52685,10 @@
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" s="7" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A61" s="235" t="s">
+      <c r="A61" s="232" t="s">
         <v>370</v>
       </c>
-      <c r="B61" s="237"/>
+      <c r="B61" s="234"/>
       <c r="C61" s="21" t="s">
         <v>452</v>
       </c>
@@ -54038,10 +54038,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="232" t="s">
         <v>810</v>
       </c>
-      <c r="B10" s="237"/>
+      <c r="B10" s="234"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -54344,10 +54344,10 @@
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A26" s="235" t="s">
+      <c r="A26" s="232" t="s">
         <v>390</v>
       </c>
-      <c r="B26" s="237"/>
+      <c r="B26" s="234"/>
       <c r="C26" s="4" t="s">
         <v>855</v>
       </c>
@@ -54614,10 +54614,10 @@
       <c r="G39" s="11"/>
     </row>
     <row r="40" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A40" s="235" t="s">
+      <c r="A40" s="232" t="s">
         <v>448</v>
       </c>
-      <c r="B40" s="237"/>
+      <c r="B40" s="234"/>
       <c r="C40" s="102" t="s">
         <v>856</v>
       </c>
@@ -54882,10 +54882,10 @@
       <c r="G53" s="11"/>
     </row>
     <row r="54" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A54" s="235" t="s">
+      <c r="A54" s="232" t="s">
         <v>412</v>
       </c>
-      <c r="B54" s="237"/>
+      <c r="B54" s="234"/>
       <c r="C54" s="4" t="s">
         <v>63</v>
       </c>
@@ -56748,10 +56748,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="232" t="s">
         <v>239</v>
       </c>
-      <c r="B10" s="237"/>
+      <c r="B10" s="234"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -56845,10 +56845,10 @@
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A15" s="235" t="s">
+      <c r="A15" s="232" t="s">
         <v>246</v>
       </c>
-      <c r="B15" s="237"/>
+      <c r="B15" s="234"/>
       <c r="C15" s="4" t="s">
         <v>874</v>
       </c>
@@ -56961,10 +56961,10 @@
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A21" s="235" t="s">
+      <c r="A21" s="232" t="s">
         <v>878</v>
       </c>
-      <c r="B21" s="237"/>
+      <c r="B21" s="234"/>
       <c r="C21" s="4" t="s">
         <v>63</v>
       </c>
@@ -57096,10 +57096,10 @@
       <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A28" s="235" t="s">
+      <c r="A28" s="232" t="s">
         <v>254</v>
       </c>
-      <c r="B28" s="237"/>
+      <c r="B28" s="234"/>
       <c r="C28" s="4" t="s">
         <v>875</v>
       </c>
@@ -57250,10 +57250,10 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A36" s="235" t="s">
+      <c r="A36" s="232" t="s">
         <v>891</v>
       </c>
-      <c r="B36" s="237"/>
+      <c r="B36" s="234"/>
       <c r="C36" s="4" t="s">
         <v>454</v>
       </c>
@@ -57385,10 +57385,10 @@
       <c r="G42" s="11"/>
     </row>
     <row r="43" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A43" s="235" t="s">
+      <c r="A43" s="232" t="s">
         <v>275</v>
       </c>
-      <c r="B43" s="237"/>
+      <c r="B43" s="234"/>
       <c r="C43" s="4" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Fixed restart to reset on the main menu properly.  Updated the player settings because they were reset to defaults.
</commit_message>
<xml_diff>
--- a/GameDocuments/gam352_papercut_rubric.xlsx
+++ b/GameDocuments/gam352_papercut_rubric.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Game Data" sheetId="1" r:id="rId1"/>
@@ -5759,6 +5759,90 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -5792,18 +5876,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -5861,99 +5933,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="4" borderId="16" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="4" borderId="18" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="26" fillId="3" borderId="21" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5964,6 +5943,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="26" fillId="3" borderId="26" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6032,55 +6017,37 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="4" borderId="16" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="4" borderId="18" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6092,28 +6059,28 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6140,19 +6107,52 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -38689,54 +38689,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="178"/>
+      <c r="B1" s="145"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="146"/>
       <c r="E1" s="103"/>
-      <c r="F1" s="176" t="s">
+      <c r="F1" s="144" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="177"/>
-      <c r="H1" s="177"/>
-      <c r="I1" s="177"/>
-      <c r="J1" s="178"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
+      <c r="J1" s="146"/>
       <c r="K1" s="104"/>
       <c r="L1" s="104"/>
       <c r="M1" s="105"/>
     </row>
     <row r="2" spans="1:13" ht="14.1" customHeight="1">
-      <c r="A2" s="182" t="s">
+      <c r="A2" s="147" t="s">
         <v>951</v>
       </c>
-      <c r="B2" s="183"/>
-      <c r="C2" s="183"/>
-      <c r="D2" s="184"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="149"/>
       <c r="E2" s="103"/>
-      <c r="F2" s="182" t="s">
+      <c r="F2" s="147" t="s">
         <v>954</v>
       </c>
-      <c r="G2" s="183"/>
-      <c r="H2" s="183"/>
-      <c r="I2" s="183"/>
-      <c r="J2" s="184"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="149"/>
       <c r="K2" s="104"/>
       <c r="L2" s="104"/>
       <c r="M2" s="105"/>
     </row>
     <row r="3" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A3" s="185"/>
-      <c r="B3" s="186"/>
-      <c r="C3" s="186"/>
-      <c r="D3" s="187"/>
+      <c r="A3" s="150"/>
+      <c r="B3" s="151"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="103"/>
-      <c r="F3" s="185"/>
-      <c r="G3" s="186"/>
-      <c r="H3" s="186"/>
-      <c r="I3" s="186"/>
-      <c r="J3" s="187"/>
+      <c r="F3" s="150"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="151"/>
+      <c r="J3" s="152"/>
       <c r="K3" s="104"/>
       <c r="L3" s="104"/>
       <c r="M3" s="105"/>
@@ -38757,41 +38757,41 @@
       <c r="M4" s="105"/>
     </row>
     <row r="5" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="144" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="177"/>
-      <c r="C5" s="177"/>
-      <c r="D5" s="178"/>
+      <c r="B5" s="145"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="146"/>
       <c r="E5" s="103"/>
-      <c r="F5" s="176" t="s">
+      <c r="F5" s="144" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="177"/>
-      <c r="H5" s="177"/>
-      <c r="I5" s="177"/>
-      <c r="J5" s="178"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="145"/>
+      <c r="I5" s="145"/>
+      <c r="J5" s="146"/>
       <c r="K5" s="104"/>
       <c r="L5" s="107"/>
       <c r="M5" s="105"/>
     </row>
     <row r="6" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="156" t="s">
         <v>952</v>
       </c>
-      <c r="B6" s="174"/>
-      <c r="C6" s="174"/>
-      <c r="D6" s="175"/>
+      <c r="B6" s="157"/>
+      <c r="C6" s="157"/>
+      <c r="D6" s="158"/>
       <c r="E6" s="103"/>
-      <c r="F6" s="173" t="s">
+      <c r="F6" s="156" t="s">
         <v>955</v>
       </c>
-      <c r="G6" s="174"/>
-      <c r="H6" s="174"/>
-      <c r="I6" s="174"/>
-      <c r="J6" s="175"/>
+      <c r="G6" s="157"/>
+      <c r="H6" s="157"/>
+      <c r="I6" s="157"/>
+      <c r="J6" s="158"/>
       <c r="K6" s="104"/>
-      <c r="L6" s="170" t="s">
+      <c r="L6" s="153" t="s">
         <v>24</v>
       </c>
       <c r="M6" s="105"/>
@@ -38802,47 +38802,47 @@
       <c r="C7" s="108"/>
       <c r="D7" s="109"/>
       <c r="E7" s="103"/>
-      <c r="F7" s="173"/>
-      <c r="G7" s="174"/>
-      <c r="H7" s="174"/>
-      <c r="I7" s="174"/>
-      <c r="J7" s="175"/>
+      <c r="F7" s="156"/>
+      <c r="G7" s="157"/>
+      <c r="H7" s="157"/>
+      <c r="I7" s="157"/>
+      <c r="J7" s="158"/>
       <c r="K7" s="104"/>
-      <c r="L7" s="171"/>
+      <c r="L7" s="154"/>
       <c r="M7" s="105"/>
     </row>
     <row r="8" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="144" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="177"/>
-      <c r="C8" s="177"/>
-      <c r="D8" s="178"/>
+      <c r="B8" s="145"/>
+      <c r="C8" s="145"/>
+      <c r="D8" s="146"/>
       <c r="E8" s="103"/>
-      <c r="F8" s="173"/>
-      <c r="G8" s="174"/>
-      <c r="H8" s="174"/>
-      <c r="I8" s="174"/>
-      <c r="J8" s="175"/>
+      <c r="F8" s="156"/>
+      <c r="G8" s="157"/>
+      <c r="H8" s="157"/>
+      <c r="I8" s="157"/>
+      <c r="J8" s="158"/>
       <c r="K8" s="104"/>
-      <c r="L8" s="171"/>
+      <c r="L8" s="154"/>
       <c r="M8" s="105"/>
     </row>
     <row r="9" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="156" t="s">
         <v>953</v>
       </c>
-      <c r="B9" s="174"/>
-      <c r="C9" s="174"/>
-      <c r="D9" s="175"/>
+      <c r="B9" s="157"/>
+      <c r="C9" s="157"/>
+      <c r="D9" s="158"/>
       <c r="E9" s="103"/>
-      <c r="F9" s="173"/>
-      <c r="G9" s="174"/>
-      <c r="H9" s="174"/>
-      <c r="I9" s="174"/>
-      <c r="J9" s="175"/>
+      <c r="F9" s="156"/>
+      <c r="G9" s="157"/>
+      <c r="H9" s="157"/>
+      <c r="I9" s="157"/>
+      <c r="J9" s="158"/>
       <c r="K9" s="104"/>
-      <c r="L9" s="172"/>
+      <c r="L9" s="155"/>
       <c r="M9" s="105"/>
     </row>
     <row r="10" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -38861,18 +38861,18 @@
       <c r="M10" s="105"/>
     </row>
     <row r="11" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="144" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="177"/>
-      <c r="C11" s="177"/>
-      <c r="D11" s="178"/>
+      <c r="B11" s="145"/>
+      <c r="C11" s="145"/>
+      <c r="D11" s="146"/>
       <c r="E11" s="103"/>
-      <c r="F11" s="176" t="s">
+      <c r="F11" s="144" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="177"/>
-      <c r="H11" s="178"/>
+      <c r="G11" s="145"/>
+      <c r="H11" s="146"/>
       <c r="I11" s="134" t="s">
         <v>7</v>
       </c>
@@ -38912,7 +38912,7 @@
         <v>-0.12</v>
       </c>
       <c r="K12" s="104"/>
-      <c r="L12" s="170" t="s">
+      <c r="L12" s="153" t="s">
         <v>8</v>
       </c>
       <c r="M12" s="105"/>
@@ -38945,7 +38945,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="120"/>
-      <c r="L13" s="171"/>
+      <c r="L13" s="154"/>
       <c r="M13" s="121"/>
     </row>
     <row r="14" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -38975,7 +38975,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="124"/>
-      <c r="L14" s="172"/>
+      <c r="L14" s="155"/>
       <c r="M14" s="125"/>
     </row>
     <row r="15" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39043,11 +39043,11 @@
         <v>939</v>
       </c>
       <c r="E17" s="104"/>
-      <c r="F17" s="176" t="s">
+      <c r="F17" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="177"/>
-      <c r="H17" s="178"/>
+      <c r="G17" s="145"/>
+      <c r="H17" s="146"/>
       <c r="I17" s="111"/>
       <c r="J17" s="135">
         <v>0.75</v>
@@ -39073,17 +39073,17 @@
       <c r="F18" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="179" t="s">
+      <c r="G18" s="159" t="s">
         <v>956</v>
       </c>
-      <c r="H18" s="180"/>
-      <c r="I18" s="181"/>
+      <c r="H18" s="160"/>
+      <c r="I18" s="161"/>
       <c r="J18" s="137">
         <f>IF(LEFT(G18,6)="Entire",0,IF(LEFT(G18,6)="Custom",-0.05,-0.1))</f>
         <v>-0.1</v>
       </c>
       <c r="K18" s="128"/>
-      <c r="L18" s="170" t="s">
+      <c r="L18" s="153" t="s">
         <v>18</v>
       </c>
       <c r="M18" s="105"/>
@@ -39103,17 +39103,17 @@
       <c r="F19" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="153" t="s">
+      <c r="G19" s="162" t="s">
         <v>957</v>
       </c>
-      <c r="H19" s="154"/>
-      <c r="I19" s="155"/>
+      <c r="H19" s="163"/>
+      <c r="I19" s="164"/>
       <c r="J19" s="139">
         <f>IF(G19="2D Graphics and 2D Gameplay",IF(J11=0.15,-0.05,0),IF(G19="3D Graphics but 2D Gameplay",IF(J11=0.15,-0.02,-0.3),IF(J11=0.15,0,-0.3)))</f>
         <v>0</v>
       </c>
       <c r="K19" s="104"/>
-      <c r="L19" s="172"/>
+      <c r="L19" s="155"/>
       <c r="M19" s="105"/>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39163,22 +39163,22 @@
       <c r="C22" s="118"/>
       <c r="D22" s="119"/>
       <c r="E22" s="104"/>
-      <c r="F22" s="168" t="s">
+      <c r="F22" s="186" t="s">
         <v>713</v>
       </c>
-      <c r="G22" s="166" t="s">
+      <c r="G22" s="184" t="s">
         <v>714</v>
       </c>
-      <c r="H22" s="165"/>
+      <c r="H22" s="183"/>
       <c r="I22" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="163">
+      <c r="J22" s="181">
         <f>J20+J15</f>
         <v>0.68</v>
       </c>
       <c r="K22" s="104"/>
-      <c r="L22" s="144" t="s">
+      <c r="L22" s="165" t="s">
         <v>725</v>
       </c>
       <c r="M22" s="105"/>
@@ -39189,15 +39189,15 @@
       <c r="C23" s="118"/>
       <c r="D23" s="119"/>
       <c r="E23" s="104"/>
-      <c r="F23" s="169"/>
-      <c r="G23" s="167"/>
-      <c r="H23" s="165"/>
+      <c r="F23" s="187"/>
+      <c r="G23" s="185"/>
+      <c r="H23" s="183"/>
       <c r="I23" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="164"/>
+      <c r="J23" s="182"/>
       <c r="K23" s="104"/>
-      <c r="L23" s="145"/>
+      <c r="L23" s="166"/>
       <c r="M23" s="105"/>
     </row>
     <row r="24" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39221,13 +39221,13 @@
       <c r="C25" s="118"/>
       <c r="D25" s="119"/>
       <c r="E25" s="104"/>
-      <c r="F25" s="157" t="s">
+      <c r="F25" s="175" t="s">
         <v>932</v>
       </c>
-      <c r="G25" s="158"/>
-      <c r="H25" s="158"/>
-      <c r="I25" s="158"/>
-      <c r="J25" s="159"/>
+      <c r="G25" s="176"/>
+      <c r="H25" s="176"/>
+      <c r="I25" s="176"/>
+      <c r="J25" s="177"/>
       <c r="K25" s="104"/>
       <c r="L25" s="104"/>
       <c r="M25" s="105"/>
@@ -39238,11 +39238,11 @@
       <c r="C26" s="118"/>
       <c r="D26" s="119"/>
       <c r="E26" s="103"/>
-      <c r="F26" s="160"/>
-      <c r="G26" s="161"/>
-      <c r="H26" s="161"/>
-      <c r="I26" s="161"/>
-      <c r="J26" s="162"/>
+      <c r="F26" s="178"/>
+      <c r="G26" s="179"/>
+      <c r="H26" s="179"/>
+      <c r="I26" s="179"/>
+      <c r="J26" s="180"/>
       <c r="K26" s="104"/>
       <c r="L26" s="104"/>
       <c r="M26" s="105"/>
@@ -39268,13 +39268,13 @@
       <c r="C28" s="118"/>
       <c r="D28" s="119"/>
       <c r="E28" s="103"/>
-      <c r="F28" s="156" t="s">
+      <c r="F28" s="174" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="156"/>
-      <c r="H28" s="156"/>
-      <c r="I28" s="156"/>
-      <c r="J28" s="156"/>
+      <c r="G28" s="174"/>
+      <c r="H28" s="174"/>
+      <c r="I28" s="174"/>
+      <c r="J28" s="174"/>
       <c r="K28" s="104"/>
       <c r="L28" s="104"/>
       <c r="M28" s="105"/>
@@ -39285,13 +39285,13 @@
       <c r="C29" s="118"/>
       <c r="D29" s="119"/>
       <c r="E29" s="103"/>
-      <c r="F29" s="150" t="s">
+      <c r="F29" s="171" t="s">
         <v>933</v>
       </c>
-      <c r="G29" s="151"/>
-      <c r="H29" s="151"/>
-      <c r="I29" s="151"/>
-      <c r="J29" s="152"/>
+      <c r="G29" s="172"/>
+      <c r="H29" s="172"/>
+      <c r="I29" s="172"/>
+      <c r="J29" s="173"/>
       <c r="K29" s="104"/>
       <c r="L29" s="104"/>
       <c r="M29" s="105"/>
@@ -39302,30 +39302,30 @@
       <c r="C30" s="118"/>
       <c r="D30" s="119"/>
       <c r="E30" s="103"/>
-      <c r="F30" s="150"/>
-      <c r="G30" s="151"/>
-      <c r="H30" s="151"/>
-      <c r="I30" s="151"/>
-      <c r="J30" s="152"/>
+      <c r="F30" s="171"/>
+      <c r="G30" s="172"/>
+      <c r="H30" s="172"/>
+      <c r="I30" s="172"/>
+      <c r="J30" s="173"/>
       <c r="K30" s="104"/>
       <c r="L30" s="104"/>
       <c r="M30" s="105"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A31" s="146" t="s">
+      <c r="A31" s="167" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="147"/>
-      <c r="C31" s="148" t="s">
+      <c r="B31" s="168"/>
+      <c r="C31" s="169" t="s">
         <v>950</v>
       </c>
-      <c r="D31" s="149"/>
+      <c r="D31" s="170"/>
       <c r="E31" s="104"/>
-      <c r="F31" s="153"/>
-      <c r="G31" s="154"/>
-      <c r="H31" s="154"/>
-      <c r="I31" s="154"/>
-      <c r="J31" s="155"/>
+      <c r="F31" s="162"/>
+      <c r="G31" s="163"/>
+      <c r="H31" s="163"/>
+      <c r="I31" s="163"/>
+      <c r="J31" s="164"/>
       <c r="K31" s="104"/>
       <c r="L31" s="104"/>
       <c r="M31" s="105"/>
@@ -39348,12 +39348,16 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0"/>
   <mergeCells count="31">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="A2:D3"/>
-    <mergeCell ref="F2:J3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F29:J31"/>
+    <mergeCell ref="F28:J28"/>
+    <mergeCell ref="F25:J26"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F22:F23"/>
     <mergeCell ref="L12:L14"/>
     <mergeCell ref="L18:L19"/>
     <mergeCell ref="A6:D6"/>
@@ -39369,16 +39373,12 @@
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="G18:I18"/>
     <mergeCell ref="G19:I19"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F29:J31"/>
-    <mergeCell ref="F28:J28"/>
-    <mergeCell ref="F25:J26"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A2:D3"/>
+    <mergeCell ref="F2:J3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:J5"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6:D6">
@@ -39446,57 +39446,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="194" t="s">
         <v>556</v>
       </c>
-      <c r="B1" s="200"/>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
-      <c r="E1" s="200"/>
-      <c r="F1" s="200"/>
-      <c r="G1" s="200"/>
-      <c r="H1" s="200"/>
-      <c r="J1" s="210" t="s">
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
+      <c r="F1" s="195"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="195"/>
+      <c r="J1" s="205" t="s">
         <v>482</v>
       </c>
-      <c r="K1" s="211"/>
-      <c r="L1" s="212"/>
+      <c r="K1" s="206"/>
+      <c r="L1" s="207"/>
       <c r="M1" s="79"/>
       <c r="N1" s="24" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A2" s="199"/>
-      <c r="B2" s="200"/>
-      <c r="C2" s="200"/>
-      <c r="D2" s="200"/>
-      <c r="E2" s="200"/>
-      <c r="F2" s="200"/>
-      <c r="G2" s="200"/>
-      <c r="H2" s="200"/>
-      <c r="J2" s="213" t="s">
+      <c r="A2" s="194"/>
+      <c r="B2" s="195"/>
+      <c r="C2" s="195"/>
+      <c r="D2" s="195"/>
+      <c r="E2" s="195"/>
+      <c r="F2" s="195"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="195"/>
+      <c r="J2" s="208" t="s">
         <v>706</v>
       </c>
-      <c r="K2" s="214"/>
-      <c r="L2" s="215"/>
+      <c r="K2" s="209"/>
+      <c r="L2" s="210"/>
       <c r="M2" s="23"/>
       <c r="N2" s="26" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A3" s="199"/>
-      <c r="B3" s="200"/>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200"/>
-      <c r="E3" s="200"/>
-      <c r="F3" s="200"/>
-      <c r="G3" s="200"/>
-      <c r="H3" s="200"/>
-      <c r="J3" s="213"/>
-      <c r="K3" s="214"/>
-      <c r="L3" s="215"/>
+      <c r="A3" s="194"/>
+      <c r="B3" s="195"/>
+      <c r="C3" s="195"/>
+      <c r="D3" s="195"/>
+      <c r="E3" s="195"/>
+      <c r="F3" s="195"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="195"/>
+      <c r="J3" s="208"/>
+      <c r="K3" s="209"/>
+      <c r="L3" s="210"/>
       <c r="M3" s="23"/>
       <c r="N3" s="26" t="s">
         <v>431</v>
@@ -39506,14 +39506,14 @@
       <c r="A4" s="2"/>
       <c r="B4" s="5"/>
       <c r="C4" s="8"/>
-      <c r="D4" s="192"/>
-      <c r="E4" s="192"/>
+      <c r="D4" s="193"/>
+      <c r="E4" s="193"/>
       <c r="F4" s="43"/>
-      <c r="G4" s="192"/>
-      <c r="H4" s="192"/>
-      <c r="J4" s="213"/>
-      <c r="K4" s="214"/>
-      <c r="L4" s="215"/>
+      <c r="G4" s="193"/>
+      <c r="H4" s="193"/>
+      <c r="J4" s="208"/>
+      <c r="K4" s="209"/>
+      <c r="L4" s="210"/>
       <c r="M4" s="34"/>
       <c r="N4" s="26" t="s">
         <v>432</v>
@@ -39521,24 +39521,24 @@
       <c r="O4" s="81"/>
     </row>
     <row r="5" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A5" s="201" t="s">
+      <c r="A5" s="196" t="s">
         <v>425</v>
       </c>
-      <c r="B5" s="202"/>
+      <c r="B5" s="197"/>
       <c r="C5" s="8"/>
-      <c r="D5" s="205" t="s">
+      <c r="D5" s="200" t="s">
         <v>717</v>
       </c>
-      <c r="E5" s="206"/>
-      <c r="F5" s="207"/>
-      <c r="G5" s="208">
+      <c r="E5" s="201"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="203">
         <f>Submission!$E$17</f>
         <v>0</v>
       </c>
-      <c r="H5" s="209"/>
-      <c r="J5" s="213"/>
-      <c r="K5" s="214"/>
-      <c r="L5" s="215"/>
+      <c r="H5" s="204"/>
+      <c r="J5" s="208"/>
+      <c r="K5" s="209"/>
+      <c r="L5" s="210"/>
       <c r="M5" s="34"/>
       <c r="N5" s="26" t="s">
         <v>433</v>
@@ -39546,21 +39546,21 @@
       <c r="O5" s="81"/>
     </row>
     <row r="6" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A6" s="203"/>
-      <c r="B6" s="204"/>
+      <c r="A6" s="198"/>
+      <c r="B6" s="199"/>
       <c r="C6" s="43"/>
-      <c r="D6" s="192" t="s">
+      <c r="D6" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="192"/>
+      <c r="E6" s="193"/>
       <c r="F6" s="43"/>
-      <c r="G6" s="192" t="s">
+      <c r="G6" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="192"/>
-      <c r="J6" s="213"/>
-      <c r="K6" s="214"/>
-      <c r="L6" s="215"/>
+      <c r="H6" s="193"/>
+      <c r="J6" s="208"/>
+      <c r="K6" s="209"/>
+      <c r="L6" s="210"/>
       <c r="M6" s="34"/>
       <c r="N6" s="26" t="s">
         <v>434</v>
@@ -39568,24 +39568,24 @@
       <c r="O6" s="81"/>
     </row>
     <row r="7" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A7" s="195">
+      <c r="A7" s="188">
         <f>'Game Data'!$J$22</f>
         <v>0.68</v>
       </c>
-      <c r="B7" s="196"/>
+      <c r="B7" s="189"/>
       <c r="C7" s="43"/>
-      <c r="D7" s="193" t="s">
+      <c r="D7" s="216" t="s">
         <v>724</v>
       </c>
-      <c r="E7" s="194"/>
+      <c r="E7" s="217"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="193" t="s">
+      <c r="G7" s="216" t="s">
         <v>724</v>
       </c>
-      <c r="H7" s="194"/>
-      <c r="J7" s="213"/>
-      <c r="K7" s="214"/>
-      <c r="L7" s="215"/>
+      <c r="H7" s="217"/>
+      <c r="J7" s="208"/>
+      <c r="K7" s="209"/>
+      <c r="L7" s="210"/>
       <c r="M7" s="33"/>
       <c r="N7" s="26" t="s">
         <v>435</v>
@@ -39593,23 +39593,23 @@
       <c r="O7" s="81"/>
     </row>
     <row r="8" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A8" s="197"/>
-      <c r="B8" s="198"/>
+      <c r="A8" s="190"/>
+      <c r="B8" s="191"/>
       <c r="C8" s="97"/>
-      <c r="D8" s="219">
+      <c r="D8" s="214">
         <f>E17+E26+E35+E44+E53</f>
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="E8" s="220"/>
+        <v>0.29000000000000004</v>
+      </c>
+      <c r="E8" s="215"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="219">
+      <c r="G8" s="214">
         <f>H17+H26+H35+H44+H53</f>
         <v>0</v>
       </c>
-      <c r="H8" s="220"/>
-      <c r="J8" s="216"/>
-      <c r="K8" s="217"/>
-      <c r="L8" s="218"/>
+      <c r="H8" s="215"/>
+      <c r="J8" s="211"/>
+      <c r="K8" s="212"/>
+      <c r="L8" s="213"/>
       <c r="M8" s="80"/>
       <c r="N8" s="25" t="s">
         <v>436</v>
@@ -39620,15 +39620,15 @@
       <c r="A9" s="2"/>
       <c r="B9" s="5"/>
       <c r="C9" s="43"/>
-      <c r="D9" s="192" t="s">
+      <c r="D9" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="192"/>
+      <c r="E9" s="193"/>
       <c r="F9" s="43"/>
-      <c r="G9" s="192" t="s">
+      <c r="G9" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="192"/>
+      <c r="H9" s="193"/>
       <c r="J9" s="82"/>
       <c r="K9" s="82"/>
       <c r="L9" s="82"/>
@@ -39655,11 +39655,11 @@
       <c r="H10" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="191" t="s">
+      <c r="J10" s="192" t="s">
         <v>707</v>
       </c>
-      <c r="K10" s="191"/>
-      <c r="L10" s="191"/>
+      <c r="K10" s="192"/>
+      <c r="L10" s="192"/>
       <c r="O10" s="84"/>
     </row>
     <row r="11" spans="1:15" ht="14.1" customHeight="1">
@@ -39688,11 +39688,11 @@
         <f t="shared" ref="H11:H16" si="1">$B11*G11</f>
         <v>0</v>
       </c>
-      <c r="J11" s="190" t="s">
+      <c r="J11" s="220" t="s">
         <v>792</v>
       </c>
-      <c r="K11" s="190"/>
-      <c r="L11" s="190"/>
+      <c r="K11" s="220"/>
+      <c r="L11" s="220"/>
       <c r="M11" s="82"/>
       <c r="O11" s="84"/>
     </row>
@@ -39722,9 +39722,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J12" s="190"/>
-      <c r="K12" s="190"/>
-      <c r="L12" s="190"/>
+      <c r="J12" s="220"/>
+      <c r="K12" s="220"/>
+      <c r="L12" s="220"/>
       <c r="M12" s="82"/>
       <c r="O12" s="84"/>
     </row>
@@ -39739,11 +39739,11 @@
       <c r="C13" s="35"/>
       <c r="D13" s="39">
         <f>TECH!$E$4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="47">
         <f t="shared" si="0"/>
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="F13" s="43"/>
       <c r="G13" s="39">
@@ -39754,9 +39754,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="190"/>
-      <c r="K13" s="190"/>
-      <c r="L13" s="190"/>
+      <c r="J13" s="220"/>
+      <c r="K13" s="220"/>
+      <c r="L13" s="220"/>
       <c r="M13" s="82"/>
       <c r="O13" s="84"/>
     </row>
@@ -39822,11 +39822,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J15" s="188">
+      <c r="J15" s="218">
         <f>MAX(0,MIN(1,IF($J17 &lt;= 0.95, ROUND($J17,2), FLOOR((0.95+($J17-0.95)/5),0.01))))</f>
-        <v>0.83</v>
-      </c>
-      <c r="L15" s="188">
+        <v>0.84</v>
+      </c>
+      <c r="L15" s="218">
         <f>MAX(0,MIN(1,IF($L17 &lt;= 0.95, ROUND($L17,2), FLOOR((0.95+($L17-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -39859,8 +39859,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J16" s="189"/>
-      <c r="L16" s="189"/>
+      <c r="J16" s="219"/>
+      <c r="L16" s="219"/>
       <c r="M16" s="82"/>
       <c r="O16" s="84"/>
     </row>
@@ -39873,7 +39873,7 @@
       </c>
       <c r="E17" s="41">
         <f>SUM(E11:E16)</f>
-        <v>2.3749999999999997E-2</v>
+        <v>3.3750000000000002E-2</v>
       </c>
       <c r="F17" s="43"/>
       <c r="G17" s="22" t="s">
@@ -39885,7 +39885,7 @@
       </c>
       <c r="J17" s="87">
         <f>$A$7+$E17+IF($D$8-$E17 &gt; 0, ($D$8-$E17)/2, $D$8-$E17)+$G$5</f>
-        <v>0.83187500000000014</v>
+        <v>0.84187500000000015</v>
       </c>
       <c r="L17" s="87">
         <f>$A$7+$H17+IF($G$8 &gt; 0, ($G$8-$H17)/2, $G$8-$H17)+$G$5</f>
@@ -39897,15 +39897,15 @@
       <c r="A18" s="2"/>
       <c r="B18" s="5"/>
       <c r="C18" s="43"/>
-      <c r="D18" s="192" t="s">
+      <c r="D18" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="192"/>
+      <c r="E18" s="193"/>
       <c r="F18" s="43"/>
-      <c r="G18" s="192" t="s">
+      <c r="G18" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="192"/>
+      <c r="H18" s="193"/>
       <c r="J18" s="88"/>
       <c r="M18" s="78"/>
     </row>
@@ -39930,11 +39930,11 @@
       <c r="H19" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="191" t="s">
+      <c r="J19" s="192" t="s">
         <v>715</v>
       </c>
-      <c r="K19" s="191"/>
-      <c r="L19" s="191"/>
+      <c r="K19" s="192"/>
+      <c r="L19" s="192"/>
       <c r="M19" s="83"/>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1">
@@ -39963,11 +39963,11 @@
         <f t="shared" ref="H20:H25" si="3">$B20*G20</f>
         <v>0</v>
       </c>
-      <c r="J20" s="190" t="s">
+      <c r="J20" s="220" t="s">
         <v>722</v>
       </c>
-      <c r="K20" s="190"/>
-      <c r="L20" s="190"/>
+      <c r="K20" s="220"/>
+      <c r="L20" s="220"/>
       <c r="M20" s="84"/>
     </row>
     <row r="21" spans="1:13" ht="14.1" customHeight="1">
@@ -39996,9 +39996,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J21" s="190"/>
-      <c r="K21" s="190"/>
-      <c r="L21" s="190"/>
+      <c r="J21" s="220"/>
+      <c r="K21" s="220"/>
+      <c r="L21" s="220"/>
       <c r="M21" s="84"/>
     </row>
     <row r="22" spans="1:13" ht="14.1" customHeight="1">
@@ -40027,9 +40027,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J22" s="190"/>
-      <c r="K22" s="190"/>
-      <c r="L22" s="190"/>
+      <c r="J22" s="220"/>
+      <c r="K22" s="220"/>
+      <c r="L22" s="220"/>
       <c r="M22" s="84"/>
     </row>
     <row r="23" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40093,11 +40093,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J24" s="188">
+      <c r="J24" s="218">
         <f>MAX(0,MIN(1,IF($J26 &lt;= 0.95, ROUND($J26,2), FLOOR((0.95+($J26-0.95)/5),0.01))))</f>
         <v>0.86</v>
       </c>
-      <c r="L24" s="188">
+      <c r="L24" s="218">
         <f>MAX(0,MIN(1,IF($L26 &lt;= 0.95, ROUND($L26,2), FLOOR((0.95+($L26-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40129,8 +40129,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J25" s="189"/>
-      <c r="L25" s="189"/>
+      <c r="J25" s="219"/>
+      <c r="L25" s="219"/>
       <c r="M25" s="84"/>
     </row>
     <row r="26" spans="1:13" ht="14.1" customHeight="1">
@@ -40166,15 +40166,15 @@
       <c r="A27" s="2"/>
       <c r="B27" s="5"/>
       <c r="C27" s="43"/>
-      <c r="D27" s="192" t="s">
+      <c r="D27" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="192"/>
+      <c r="E27" s="193"/>
       <c r="F27" s="43"/>
-      <c r="G27" s="192" t="s">
+      <c r="G27" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H27" s="192"/>
+      <c r="H27" s="193"/>
     </row>
     <row r="28" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
       <c r="A28" s="1" t="s">
@@ -40197,11 +40197,11 @@
       <c r="H28" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J28" s="191" t="s">
+      <c r="J28" s="192" t="s">
         <v>709</v>
       </c>
-      <c r="K28" s="191"/>
-      <c r="L28" s="191"/>
+      <c r="K28" s="192"/>
+      <c r="L28" s="192"/>
     </row>
     <row r="29" spans="1:13" ht="14.1" customHeight="1">
       <c r="A29" s="57" t="str">
@@ -40229,11 +40229,11 @@
         <f t="shared" ref="H29:H34" si="5">$B29*G29</f>
         <v>0</v>
       </c>
-      <c r="J29" s="190" t="s">
+      <c r="J29" s="220" t="s">
         <v>710</v>
       </c>
-      <c r="K29" s="190"/>
-      <c r="L29" s="190"/>
+      <c r="K29" s="220"/>
+      <c r="L29" s="220"/>
     </row>
     <row r="30" spans="1:13" ht="14.1" customHeight="1">
       <c r="A30" s="58" t="str">
@@ -40261,9 +40261,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J30" s="190"/>
-      <c r="K30" s="190"/>
-      <c r="L30" s="190"/>
+      <c r="J30" s="220"/>
+      <c r="K30" s="220"/>
+      <c r="L30" s="220"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1">
       <c r="A31" s="58" t="str">
@@ -40291,9 +40291,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J31" s="190"/>
-      <c r="K31" s="190"/>
-      <c r="L31" s="190"/>
+      <c r="J31" s="220"/>
+      <c r="K31" s="220"/>
+      <c r="L31" s="220"/>
     </row>
     <row r="32" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
       <c r="A32" s="58" t="str">
@@ -40355,11 +40355,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J33" s="188">
+      <c r="J33" s="218">
         <f>MAX(0,MIN(1,IF($J35 &lt;= 0.95, ROUND($J35,2), FLOOR((0.95+($J35-0.95)/5),0.01))))</f>
         <v>0.88</v>
       </c>
-      <c r="L33" s="188">
+      <c r="L33" s="218">
         <f>MAX(0,MIN(1,IF($L35 &lt;= 0.95, ROUND($L35,2), FLOOR((0.95+($L35-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40390,8 +40390,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J34" s="189"/>
-      <c r="L34" s="189"/>
+      <c r="J34" s="219"/>
+      <c r="L34" s="219"/>
     </row>
     <row r="35" spans="1:12" ht="14.1" customHeight="1">
       <c r="A35" s="2"/>
@@ -40425,15 +40425,15 @@
       <c r="A36" s="2"/>
       <c r="B36" s="5"/>
       <c r="C36" s="43"/>
-      <c r="D36" s="192" t="s">
+      <c r="D36" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="192"/>
+      <c r="E36" s="193"/>
       <c r="F36" s="43"/>
-      <c r="G36" s="192" t="s">
+      <c r="G36" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H36" s="192"/>
+      <c r="H36" s="193"/>
     </row>
     <row r="37" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A37" s="1" t="s">
@@ -40456,11 +40456,11 @@
       <c r="H37" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J37" s="191" t="s">
+      <c r="J37" s="192" t="s">
         <v>711</v>
       </c>
-      <c r="K37" s="191"/>
-      <c r="L37" s="191"/>
+      <c r="K37" s="192"/>
+      <c r="L37" s="192"/>
     </row>
     <row r="38" spans="1:12" ht="14.1" customHeight="1">
       <c r="A38" s="57" t="str">
@@ -40488,11 +40488,11 @@
         <f t="shared" ref="H38:H43" si="7">$B38*G38</f>
         <v>0</v>
       </c>
-      <c r="J38" s="190" t="s">
+      <c r="J38" s="220" t="s">
         <v>712</v>
       </c>
-      <c r="K38" s="190"/>
-      <c r="L38" s="190"/>
+      <c r="K38" s="220"/>
+      <c r="L38" s="220"/>
     </row>
     <row r="39" spans="1:12" ht="14.1" customHeight="1">
       <c r="A39" s="58" t="str">
@@ -40520,9 +40520,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J39" s="190"/>
-      <c r="K39" s="190"/>
-      <c r="L39" s="190"/>
+      <c r="J39" s="220"/>
+      <c r="K39" s="220"/>
+      <c r="L39" s="220"/>
     </row>
     <row r="40" spans="1:12" ht="14.1" customHeight="1">
       <c r="A40" s="58" t="str">
@@ -40550,9 +40550,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J40" s="190"/>
-      <c r="K40" s="190"/>
-      <c r="L40" s="190"/>
+      <c r="J40" s="220"/>
+      <c r="K40" s="220"/>
+      <c r="L40" s="220"/>
     </row>
     <row r="41" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A41" s="58" t="str">
@@ -40614,11 +40614,11 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J42" s="188">
+      <c r="J42" s="218">
         <f>MAX(0,MIN(1,IF($J44 &lt;= 0.95, ROUND($J44,2), FLOOR((0.95+($J44-0.95)/5),0.01))))</f>
         <v>0.73</v>
       </c>
-      <c r="L42" s="188">
+      <c r="L42" s="218">
         <f>MAX(0,MIN(1,IF($L44 &lt;= 0.95, ROUND($L44,2), FLOOR((0.95+($L44-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40649,8 +40649,8 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J43" s="189"/>
-      <c r="L43" s="189"/>
+      <c r="J43" s="219"/>
+      <c r="L43" s="219"/>
     </row>
     <row r="44" spans="1:12" ht="14.1" customHeight="1">
       <c r="A44" s="2"/>
@@ -40684,15 +40684,15 @@
       <c r="A45" s="2"/>
       <c r="B45" s="5"/>
       <c r="C45" s="43"/>
-      <c r="D45" s="192" t="s">
+      <c r="D45" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="192"/>
+      <c r="E45" s="193"/>
       <c r="F45" s="43"/>
-      <c r="G45" s="192" t="s">
+      <c r="G45" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="192"/>
+      <c r="H45" s="193"/>
     </row>
     <row r="46" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A46" s="1" t="s">
@@ -40900,6 +40900,34 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="J29:L31"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="L33:L34"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="J38:L40"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="J11:L13"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J20:L22"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G36:H36"/>
     <mergeCell ref="A7:B8"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="D6:E6"/>
@@ -40913,34 +40941,6 @@
     <mergeCell ref="J2:L8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="J11:L13"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J20:L22"/>
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="L42:L43"/>
-    <mergeCell ref="J29:L31"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="L33:L34"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="J38:L40"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -40951,7 +40951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -40968,59 +40968,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="235" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="233"/>
-      <c r="C1" s="233"/>
-      <c r="D1" s="233"/>
-      <c r="E1" s="233"/>
-      <c r="F1" s="233"/>
-      <c r="G1" s="234"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="237"/>
     </row>
     <row r="2" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A2" s="221" t="s">
+      <c r="A2" s="230" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="222"/>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
-      <c r="G2" s="223"/>
+      <c r="B2" s="231"/>
+      <c r="C2" s="231"/>
+      <c r="D2" s="231"/>
+      <c r="E2" s="231"/>
+      <c r="F2" s="231"/>
+      <c r="G2" s="232"/>
     </row>
     <row r="3" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A3" s="238" t="s">
+      <c r="A3" s="227" t="s">
         <v>930</v>
       </c>
-      <c r="B3" s="239"/>
-      <c r="C3" s="239"/>
-      <c r="D3" s="239"/>
-      <c r="E3" s="239"/>
-      <c r="F3" s="239"/>
-      <c r="G3" s="240"/>
+      <c r="B3" s="228"/>
+      <c r="C3" s="228"/>
+      <c r="D3" s="228"/>
+      <c r="E3" s="228"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="229"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A4" s="221" t="s">
+      <c r="A4" s="230" t="s">
         <v>438</v>
       </c>
-      <c r="B4" s="222"/>
-      <c r="C4" s="222"/>
-      <c r="D4" s="222"/>
-      <c r="E4" s="222"/>
-      <c r="F4" s="222"/>
-      <c r="G4" s="223"/>
+      <c r="B4" s="231"/>
+      <c r="C4" s="231"/>
+      <c r="D4" s="231"/>
+      <c r="E4" s="231"/>
+      <c r="F4" s="231"/>
+      <c r="G4" s="232"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A5" s="249" t="s">
+      <c r="A5" s="238" t="s">
         <v>580</v>
       </c>
-      <c r="B5" s="250"/>
-      <c r="C5" s="250"/>
-      <c r="D5" s="250"/>
-      <c r="E5" s="250"/>
-      <c r="F5" s="250"/>
-      <c r="G5" s="251"/>
+      <c r="B5" s="239"/>
+      <c r="C5" s="239"/>
+      <c r="D5" s="239"/>
+      <c r="E5" s="239"/>
+      <c r="F5" s="239"/>
+      <c r="G5" s="240"/>
     </row>
     <row r="6" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
       <c r="A6" s="2"/>
@@ -41053,10 +41053,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75">
-      <c r="A8" s="247" t="s">
+      <c r="A8" s="233" t="s">
         <v>718</v>
       </c>
-      <c r="B8" s="248"/>
+      <c r="B8" s="234"/>
       <c r="C8" s="65">
         <v>0</v>
       </c>
@@ -41073,10 +41073,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75">
-      <c r="A9" s="253" t="s">
+      <c r="A9" s="242" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="254"/>
+      <c r="B9" s="243"/>
       <c r="C9" s="92">
         <v>0</v>
       </c>
@@ -41093,10 +41093,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75">
-      <c r="A10" s="255" t="s">
+      <c r="A10" s="244" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="256"/>
+      <c r="B10" s="245"/>
       <c r="C10" s="69">
         <v>0</v>
       </c>
@@ -41113,10 +41113,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75">
-      <c r="A11" s="256" t="s">
+      <c r="A11" s="245" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="256"/>
+      <c r="B11" s="245"/>
       <c r="C11" s="69">
         <v>0</v>
       </c>
@@ -41133,10 +41133,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75">
-      <c r="A12" s="256" t="s">
+      <c r="A12" s="245" t="s">
         <v>716</v>
       </c>
-      <c r="B12" s="256"/>
+      <c r="B12" s="245"/>
       <c r="C12" s="69">
         <v>0</v>
       </c>
@@ -41153,10 +41153,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75">
-      <c r="A13" s="256" t="s">
+      <c r="A13" s="245" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="256"/>
+      <c r="B13" s="245"/>
       <c r="C13" s="69">
         <v>0</v>
       </c>
@@ -41173,10 +41173,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75">
-      <c r="A14" s="255" t="s">
+      <c r="A14" s="244" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="256"/>
+      <c r="B14" s="245"/>
       <c r="C14" s="69">
         <v>0</v>
       </c>
@@ -41193,10 +41193,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75">
-      <c r="A15" s="255" t="s">
+      <c r="A15" s="244" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="256"/>
+      <c r="B15" s="245"/>
       <c r="C15" s="69">
         <v>0</v>
       </c>
@@ -41213,10 +41213,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A16" s="230" t="s">
+      <c r="A16" s="246" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="231"/>
+      <c r="B16" s="247"/>
       <c r="C16" s="73">
         <v>0</v>
       </c>
@@ -41234,11 +41234,11 @@
     </row>
     <row r="17" spans="1:7" ht="14.1" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="252" t="s">
+      <c r="B17" s="241" t="s">
         <v>721</v>
       </c>
-      <c r="C17" s="252"/>
-      <c r="D17" s="252"/>
+      <c r="C17" s="241"/>
+      <c r="D17" s="241"/>
       <c r="E17" s="63">
         <f>SUM(E9:E16)</f>
         <v>0</v>
@@ -41259,527 +41259,559 @@
       <c r="A19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="232" t="s">
+      <c r="B19" s="235" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="233"/>
-      <c r="D19" s="233"/>
-      <c r="E19" s="233"/>
-      <c r="F19" s="233"/>
-      <c r="G19" s="234"/>
+      <c r="C19" s="236"/>
+      <c r="D19" s="236"/>
+      <c r="E19" s="236"/>
+      <c r="F19" s="236"/>
+      <c r="G19" s="237"/>
     </row>
     <row r="20" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="A20" s="10" t="s">
         <v>582</v>
       </c>
-      <c r="B20" s="221" t="s">
+      <c r="B20" s="230" t="s">
         <v>931</v>
       </c>
-      <c r="C20" s="222"/>
-      <c r="D20" s="222"/>
-      <c r="E20" s="222"/>
-      <c r="F20" s="222"/>
-      <c r="G20" s="223"/>
+      <c r="C20" s="231"/>
+      <c r="D20" s="231"/>
+      <c r="E20" s="231"/>
+      <c r="F20" s="231"/>
+      <c r="G20" s="232"/>
     </row>
     <row r="21" spans="1:7" ht="60" customHeight="1" thickBot="1">
       <c r="A21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="221" t="s">
+      <c r="B21" s="230" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="222"/>
-      <c r="D21" s="222"/>
-      <c r="E21" s="222"/>
-      <c r="F21" s="222"/>
-      <c r="G21" s="223"/>
+      <c r="C21" s="231"/>
+      <c r="D21" s="231"/>
+      <c r="E21" s="231"/>
+      <c r="F21" s="231"/>
+      <c r="G21" s="232"/>
     </row>
     <row r="22" spans="1:7" ht="45.95" customHeight="1" thickBot="1">
       <c r="A22" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="221" t="s">
+      <c r="B22" s="230" t="s">
         <v>917</v>
       </c>
-      <c r="C22" s="222"/>
-      <c r="D22" s="222"/>
-      <c r="E22" s="222"/>
-      <c r="F22" s="222"/>
-      <c r="G22" s="223"/>
+      <c r="C22" s="231"/>
+      <c r="D22" s="231"/>
+      <c r="E22" s="231"/>
+      <c r="F22" s="231"/>
+      <c r="G22" s="232"/>
     </row>
     <row r="23" spans="1:7" ht="32.1" customHeight="1">
       <c r="A23" s="98" t="s">
         <v>899</v>
       </c>
-      <c r="B23" s="238" t="s">
+      <c r="B23" s="227" t="s">
         <v>916</v>
       </c>
-      <c r="C23" s="239"/>
-      <c r="D23" s="239"/>
-      <c r="E23" s="239"/>
-      <c r="F23" s="239"/>
-      <c r="G23" s="240"/>
+      <c r="C23" s="228"/>
+      <c r="D23" s="228"/>
+      <c r="E23" s="228"/>
+      <c r="F23" s="228"/>
+      <c r="G23" s="229"/>
     </row>
     <row r="24" spans="1:7" ht="15.75">
       <c r="A24" s="99"/>
-      <c r="B24" s="257" t="s">
+      <c r="B24" s="221" t="s">
         <v>900</v>
       </c>
-      <c r="C24" s="258"/>
-      <c r="D24" s="260" t="s">
+      <c r="C24" s="222"/>
+      <c r="D24" s="223" t="s">
         <v>901</v>
       </c>
-      <c r="E24" s="260"/>
-      <c r="F24" s="260"/>
-      <c r="G24" s="261"/>
+      <c r="E24" s="223"/>
+      <c r="F24" s="223"/>
+      <c r="G24" s="224"/>
     </row>
     <row r="25" spans="1:7" ht="15.75">
       <c r="A25" s="99"/>
-      <c r="B25" s="257" t="s">
+      <c r="B25" s="221" t="s">
         <v>902</v>
       </c>
-      <c r="C25" s="258"/>
-      <c r="D25" s="260" t="s">
+      <c r="C25" s="222"/>
+      <c r="D25" s="223" t="s">
         <v>903</v>
       </c>
-      <c r="E25" s="260"/>
-      <c r="F25" s="260"/>
-      <c r="G25" s="261"/>
+      <c r="E25" s="223"/>
+      <c r="F25" s="223"/>
+      <c r="G25" s="224"/>
     </row>
     <row r="26" spans="1:7" ht="15.75">
       <c r="A26" s="99"/>
-      <c r="B26" s="257" t="s">
+      <c r="B26" s="221" t="s">
         <v>904</v>
       </c>
-      <c r="C26" s="258"/>
-      <c r="D26" s="260" t="s">
+      <c r="C26" s="222"/>
+      <c r="D26" s="223" t="s">
         <v>905</v>
       </c>
-      <c r="E26" s="260"/>
-      <c r="F26" s="260"/>
-      <c r="G26" s="261"/>
+      <c r="E26" s="223"/>
+      <c r="F26" s="223"/>
+      <c r="G26" s="224"/>
     </row>
     <row r="27" spans="1:7" ht="15.75">
       <c r="A27" s="99"/>
-      <c r="B27" s="257" t="s">
+      <c r="B27" s="221" t="s">
         <v>906</v>
       </c>
-      <c r="C27" s="258"/>
+      <c r="C27" s="222"/>
       <c r="D27" s="225" t="s">
         <v>907</v>
       </c>
       <c r="E27" s="225"/>
       <c r="F27" s="225"/>
-      <c r="G27" s="259"/>
+      <c r="G27" s="226"/>
     </row>
     <row r="28" spans="1:7" ht="15.75">
       <c r="A28" s="99"/>
-      <c r="B28" s="257" t="s">
+      <c r="B28" s="221" t="s">
         <v>908</v>
       </c>
-      <c r="C28" s="258"/>
-      <c r="D28" s="260" t="s">
+      <c r="C28" s="222"/>
+      <c r="D28" s="223" t="s">
         <v>909</v>
       </c>
-      <c r="E28" s="260"/>
-      <c r="F28" s="260"/>
-      <c r="G28" s="261"/>
+      <c r="E28" s="223"/>
+      <c r="F28" s="223"/>
+      <c r="G28" s="224"/>
     </row>
     <row r="29" spans="1:7" ht="15.75">
       <c r="A29" s="99"/>
-      <c r="B29" s="257" t="s">
+      <c r="B29" s="221" t="s">
         <v>910</v>
       </c>
-      <c r="C29" s="258"/>
+      <c r="C29" s="222"/>
       <c r="D29" s="225" t="s">
         <v>911</v>
       </c>
       <c r="E29" s="225"/>
       <c r="F29" s="225"/>
-      <c r="G29" s="259"/>
+      <c r="G29" s="226"/>
     </row>
     <row r="30" spans="1:7" ht="15.75">
       <c r="A30" s="99"/>
-      <c r="B30" s="257" t="s">
+      <c r="B30" s="221" t="s">
         <v>914</v>
       </c>
-      <c r="C30" s="258"/>
-      <c r="D30" s="260" t="s">
+      <c r="C30" s="222"/>
+      <c r="D30" s="223" t="s">
         <v>915</v>
       </c>
-      <c r="E30" s="260"/>
-      <c r="F30" s="260"/>
-      <c r="G30" s="261"/>
+      <c r="E30" s="223"/>
+      <c r="F30" s="223"/>
+      <c r="G30" s="224"/>
     </row>
     <row r="31" spans="1:7" ht="15.75">
       <c r="A31" s="99"/>
-      <c r="B31" s="257" t="s">
+      <c r="B31" s="221" t="s">
         <v>912</v>
       </c>
-      <c r="C31" s="258"/>
+      <c r="C31" s="222"/>
       <c r="D31" s="225" t="s">
         <v>913</v>
       </c>
       <c r="E31" s="225"/>
       <c r="F31" s="225"/>
-      <c r="G31" s="259"/>
+      <c r="G31" s="226"/>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickBot="1">
       <c r="A32" s="99"/>
-      <c r="B32" s="257" t="s">
+      <c r="B32" s="221" t="s">
         <v>928</v>
       </c>
-      <c r="C32" s="258"/>
+      <c r="C32" s="222"/>
       <c r="D32" s="225" t="s">
         <v>929</v>
       </c>
       <c r="E32" s="225"/>
       <c r="F32" s="225"/>
-      <c r="G32" s="259"/>
+      <c r="G32" s="226"/>
     </row>
     <row r="33" spans="1:7" ht="15.75">
       <c r="A33" s="98" t="s">
         <v>918</v>
       </c>
-      <c r="B33" s="238" t="s">
+      <c r="B33" s="227" t="s">
         <v>919</v>
       </c>
-      <c r="C33" s="239"/>
-      <c r="D33" s="239"/>
-      <c r="E33" s="239"/>
-      <c r="F33" s="239"/>
-      <c r="G33" s="240"/>
+      <c r="C33" s="228"/>
+      <c r="D33" s="228"/>
+      <c r="E33" s="228"/>
+      <c r="F33" s="228"/>
+      <c r="G33" s="229"/>
     </row>
     <row r="34" spans="1:7" ht="15.75">
       <c r="A34" s="99"/>
-      <c r="B34" s="257" t="s">
+      <c r="B34" s="221" t="s">
         <v>920</v>
       </c>
-      <c r="C34" s="258"/>
-      <c r="D34" s="260" t="s">
+      <c r="C34" s="222"/>
+      <c r="D34" s="223" t="s">
         <v>925</v>
       </c>
-      <c r="E34" s="260"/>
-      <c r="F34" s="260"/>
-      <c r="G34" s="261"/>
+      <c r="E34" s="223"/>
+      <c r="F34" s="223"/>
+      <c r="G34" s="224"/>
     </row>
     <row r="35" spans="1:7" ht="15.75">
       <c r="A35" s="99"/>
-      <c r="B35" s="257" t="s">
+      <c r="B35" s="221" t="s">
         <v>921</v>
       </c>
-      <c r="C35" s="258"/>
-      <c r="D35" s="260" t="s">
+      <c r="C35" s="222"/>
+      <c r="D35" s="223" t="s">
         <v>926</v>
       </c>
-      <c r="E35" s="260"/>
-      <c r="F35" s="260"/>
-      <c r="G35" s="261"/>
+      <c r="E35" s="223"/>
+      <c r="F35" s="223"/>
+      <c r="G35" s="224"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" thickBot="1">
       <c r="A36" s="99"/>
-      <c r="B36" s="257" t="s">
+      <c r="B36" s="221" t="s">
         <v>922</v>
       </c>
-      <c r="C36" s="258"/>
-      <c r="D36" s="260" t="s">
+      <c r="C36" s="222"/>
+      <c r="D36" s="223" t="s">
         <v>927</v>
       </c>
-      <c r="E36" s="260"/>
-      <c r="F36" s="260"/>
-      <c r="G36" s="261"/>
+      <c r="E36" s="223"/>
+      <c r="F36" s="223"/>
+      <c r="G36" s="224"/>
     </row>
     <row r="37" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="A37" s="98" t="s">
         <v>923</v>
       </c>
-      <c r="B37" s="238" t="s">
+      <c r="B37" s="227" t="s">
         <v>924</v>
       </c>
-      <c r="C37" s="239"/>
-      <c r="D37" s="239"/>
-      <c r="E37" s="239"/>
-      <c r="F37" s="239"/>
-      <c r="G37" s="240"/>
+      <c r="C37" s="228"/>
+      <c r="D37" s="228"/>
+      <c r="E37" s="228"/>
+      <c r="F37" s="228"/>
+      <c r="G37" s="229"/>
     </row>
     <row r="38" spans="1:7" ht="29.1" customHeight="1">
-      <c r="A38" s="235" t="s">
+      <c r="A38" s="248" t="s">
         <v>517</v>
       </c>
-      <c r="B38" s="238" t="s">
+      <c r="B38" s="227" t="s">
         <v>490</v>
       </c>
-      <c r="C38" s="239"/>
-      <c r="D38" s="239"/>
-      <c r="E38" s="239"/>
-      <c r="F38" s="239"/>
-      <c r="G38" s="240"/>
+      <c r="C38" s="228"/>
+      <c r="D38" s="228"/>
+      <c r="E38" s="228"/>
+      <c r="F38" s="228"/>
+      <c r="G38" s="229"/>
     </row>
     <row r="39" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A39" s="236"/>
-      <c r="B39" s="241"/>
-      <c r="C39" s="242"/>
-      <c r="D39" s="242"/>
-      <c r="E39" s="242"/>
-      <c r="F39" s="242"/>
-      <c r="G39" s="243"/>
+      <c r="A39" s="249"/>
+      <c r="B39" s="251"/>
+      <c r="C39" s="252"/>
+      <c r="D39" s="252"/>
+      <c r="E39" s="252"/>
+      <c r="F39" s="252"/>
+      <c r="G39" s="253"/>
     </row>
     <row r="40" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A40" s="236"/>
-      <c r="B40" s="244" t="s">
+      <c r="A40" s="249"/>
+      <c r="B40" s="254" t="s">
         <v>491</v>
       </c>
-      <c r="C40" s="245"/>
-      <c r="D40" s="245"/>
-      <c r="E40" s="245"/>
-      <c r="F40" s="245"/>
-      <c r="G40" s="246"/>
+      <c r="C40" s="255"/>
+      <c r="D40" s="255"/>
+      <c r="E40" s="255"/>
+      <c r="F40" s="255"/>
+      <c r="G40" s="256"/>
     </row>
     <row r="41" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A41" s="236"/>
-      <c r="B41" s="224" t="s">
+      <c r="A41" s="249"/>
+      <c r="B41" s="257" t="s">
         <v>492</v>
       </c>
       <c r="C41" s="225"/>
       <c r="D41" s="225"/>
       <c r="E41" s="225"/>
       <c r="F41" s="225"/>
-      <c r="G41" s="226"/>
+      <c r="G41" s="258"/>
     </row>
     <row r="42" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A42" s="236"/>
-      <c r="B42" s="241"/>
-      <c r="C42" s="242"/>
-      <c r="D42" s="242"/>
-      <c r="E42" s="242"/>
-      <c r="F42" s="242"/>
-      <c r="G42" s="243"/>
+      <c r="A42" s="249"/>
+      <c r="B42" s="251"/>
+      <c r="C42" s="252"/>
+      <c r="D42" s="252"/>
+      <c r="E42" s="252"/>
+      <c r="F42" s="252"/>
+      <c r="G42" s="253"/>
     </row>
     <row r="43" spans="1:7" ht="42.95" customHeight="1">
-      <c r="A43" s="236"/>
-      <c r="B43" s="224" t="s">
+      <c r="A43" s="249"/>
+      <c r="B43" s="257" t="s">
         <v>493</v>
       </c>
       <c r="C43" s="225"/>
       <c r="D43" s="225"/>
       <c r="E43" s="225"/>
       <c r="F43" s="225"/>
-      <c r="G43" s="226"/>
+      <c r="G43" s="258"/>
     </row>
     <row r="44" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A44" s="236"/>
-      <c r="B44" s="241"/>
-      <c r="C44" s="242"/>
-      <c r="D44" s="242"/>
-      <c r="E44" s="242"/>
-      <c r="F44" s="242"/>
-      <c r="G44" s="243"/>
+      <c r="A44" s="249"/>
+      <c r="B44" s="251"/>
+      <c r="C44" s="252"/>
+      <c r="D44" s="252"/>
+      <c r="E44" s="252"/>
+      <c r="F44" s="252"/>
+      <c r="G44" s="253"/>
     </row>
     <row r="45" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A45" s="236"/>
-      <c r="B45" s="224" t="s">
+      <c r="A45" s="249"/>
+      <c r="B45" s="257" t="s">
         <v>494</v>
       </c>
       <c r="C45" s="225"/>
       <c r="D45" s="225"/>
       <c r="E45" s="225"/>
       <c r="F45" s="225"/>
-      <c r="G45" s="226"/>
+      <c r="G45" s="258"/>
     </row>
     <row r="46" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A46" s="236"/>
-      <c r="B46" s="224" t="s">
+      <c r="A46" s="249"/>
+      <c r="B46" s="257" t="s">
         <v>495</v>
       </c>
       <c r="C46" s="225"/>
       <c r="D46" s="225"/>
       <c r="E46" s="225"/>
       <c r="F46" s="225"/>
-      <c r="G46" s="226"/>
+      <c r="G46" s="258"/>
     </row>
     <row r="47" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A47" s="236"/>
-      <c r="B47" s="224" t="s">
+      <c r="A47" s="249"/>
+      <c r="B47" s="257" t="s">
         <v>496</v>
       </c>
       <c r="C47" s="225"/>
       <c r="D47" s="225"/>
       <c r="E47" s="225"/>
       <c r="F47" s="225"/>
-      <c r="G47" s="226"/>
+      <c r="G47" s="258"/>
     </row>
     <row r="48" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A48" s="236"/>
-      <c r="B48" s="224" t="s">
+      <c r="A48" s="249"/>
+      <c r="B48" s="257" t="s">
         <v>497</v>
       </c>
       <c r="C48" s="225"/>
       <c r="D48" s="225"/>
       <c r="E48" s="225"/>
       <c r="F48" s="225"/>
-      <c r="G48" s="226"/>
+      <c r="G48" s="258"/>
     </row>
     <row r="49" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A49" s="236"/>
-      <c r="B49" s="224" t="s">
+      <c r="A49" s="249"/>
+      <c r="B49" s="257" t="s">
         <v>498</v>
       </c>
       <c r="C49" s="225"/>
       <c r="D49" s="225"/>
       <c r="E49" s="225"/>
       <c r="F49" s="225"/>
-      <c r="G49" s="226"/>
+      <c r="G49" s="258"/>
     </row>
     <row r="50" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A50" s="236"/>
-      <c r="B50" s="224" t="s">
+      <c r="A50" s="249"/>
+      <c r="B50" s="257" t="s">
         <v>499</v>
       </c>
       <c r="C50" s="225"/>
       <c r="D50" s="225"/>
       <c r="E50" s="225"/>
       <c r="F50" s="225"/>
-      <c r="G50" s="226"/>
+      <c r="G50" s="258"/>
     </row>
     <row r="51" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A51" s="236"/>
-      <c r="B51" s="224" t="s">
+      <c r="A51" s="249"/>
+      <c r="B51" s="257" t="s">
         <v>500</v>
       </c>
       <c r="C51" s="225"/>
       <c r="D51" s="225"/>
       <c r="E51" s="225"/>
       <c r="F51" s="225"/>
-      <c r="G51" s="226"/>
+      <c r="G51" s="258"/>
     </row>
     <row r="52" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A52" s="237"/>
-      <c r="B52" s="227" t="s">
+      <c r="A52" s="250"/>
+      <c r="B52" s="259" t="s">
         <v>501</v>
       </c>
-      <c r="C52" s="228"/>
-      <c r="D52" s="228"/>
-      <c r="E52" s="228"/>
-      <c r="F52" s="228"/>
-      <c r="G52" s="229"/>
+      <c r="C52" s="260"/>
+      <c r="D52" s="260"/>
+      <c r="E52" s="260"/>
+      <c r="F52" s="260"/>
+      <c r="G52" s="261"/>
     </row>
     <row r="53" spans="1:7" ht="57.95" customHeight="1" thickBot="1">
       <c r="A53" s="10" t="s">
         <v>516</v>
       </c>
-      <c r="B53" s="221" t="s">
+      <c r="B53" s="230" t="s">
         <v>581</v>
       </c>
-      <c r="C53" s="222"/>
-      <c r="D53" s="222"/>
-      <c r="E53" s="222"/>
-      <c r="F53" s="222"/>
-      <c r="G53" s="223"/>
+      <c r="C53" s="231"/>
+      <c r="D53" s="231"/>
+      <c r="E53" s="231"/>
+      <c r="F53" s="231"/>
+      <c r="G53" s="232"/>
     </row>
     <row r="54" spans="1:7" ht="57.95" customHeight="1" thickBot="1">
       <c r="A54" s="10" t="s">
         <v>515</v>
       </c>
-      <c r="B54" s="221" t="s">
+      <c r="B54" s="230" t="s">
         <v>502</v>
       </c>
-      <c r="C54" s="222"/>
-      <c r="D54" s="222"/>
-      <c r="E54" s="222"/>
-      <c r="F54" s="222"/>
-      <c r="G54" s="223"/>
+      <c r="C54" s="231"/>
+      <c r="D54" s="231"/>
+      <c r="E54" s="231"/>
+      <c r="F54" s="231"/>
+      <c r="G54" s="232"/>
     </row>
     <row r="55" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A55" s="10" t="s">
         <v>514</v>
       </c>
-      <c r="B55" s="221" t="s">
+      <c r="B55" s="230" t="s">
         <v>503</v>
       </c>
-      <c r="C55" s="222"/>
-      <c r="D55" s="222"/>
-      <c r="E55" s="222"/>
-      <c r="F55" s="222"/>
-      <c r="G55" s="223"/>
+      <c r="C55" s="231"/>
+      <c r="D55" s="231"/>
+      <c r="E55" s="231"/>
+      <c r="F55" s="231"/>
+      <c r="G55" s="232"/>
     </row>
     <row r="56" spans="1:7" ht="42.95" customHeight="1" thickBot="1">
       <c r="A56" s="11" t="s">
         <v>508</v>
       </c>
-      <c r="B56" s="221" t="s">
+      <c r="B56" s="230" t="s">
         <v>504</v>
       </c>
-      <c r="C56" s="222"/>
-      <c r="D56" s="222"/>
-      <c r="E56" s="222"/>
-      <c r="F56" s="222"/>
-      <c r="G56" s="223"/>
+      <c r="C56" s="231"/>
+      <c r="D56" s="231"/>
+      <c r="E56" s="231"/>
+      <c r="F56" s="231"/>
+      <c r="G56" s="232"/>
     </row>
     <row r="57" spans="1:7" ht="29.1" customHeight="1" thickBot="1">
       <c r="A57" s="10" t="s">
         <v>513</v>
       </c>
-      <c r="B57" s="221" t="s">
+      <c r="B57" s="230" t="s">
         <v>505</v>
       </c>
-      <c r="C57" s="222"/>
-      <c r="D57" s="222"/>
-      <c r="E57" s="222"/>
-      <c r="F57" s="222"/>
-      <c r="G57" s="223"/>
+      <c r="C57" s="231"/>
+      <c r="D57" s="231"/>
+      <c r="E57" s="231"/>
+      <c r="F57" s="231"/>
+      <c r="G57" s="232"/>
     </row>
     <row r="58" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A58" s="10" t="s">
         <v>512</v>
       </c>
-      <c r="B58" s="221" t="s">
+      <c r="B58" s="230" t="s">
         <v>506</v>
       </c>
-      <c r="C58" s="222"/>
-      <c r="D58" s="222"/>
-      <c r="E58" s="222"/>
-      <c r="F58" s="222"/>
-      <c r="G58" s="223"/>
+      <c r="C58" s="231"/>
+      <c r="D58" s="231"/>
+      <c r="E58" s="231"/>
+      <c r="F58" s="231"/>
+      <c r="G58" s="232"/>
     </row>
     <row r="59" spans="1:7" ht="42.95" customHeight="1" thickBot="1">
       <c r="A59" s="11" t="s">
         <v>509</v>
       </c>
-      <c r="B59" s="221" t="s">
+      <c r="B59" s="230" t="s">
         <v>510</v>
       </c>
-      <c r="C59" s="222"/>
-      <c r="D59" s="222"/>
-      <c r="E59" s="222"/>
-      <c r="F59" s="222"/>
-      <c r="G59" s="223"/>
+      <c r="C59" s="231"/>
+      <c r="D59" s="231"/>
+      <c r="E59" s="231"/>
+      <c r="F59" s="231"/>
+      <c r="G59" s="232"/>
     </row>
     <row r="60" spans="1:7" ht="29.1" customHeight="1" thickBot="1">
       <c r="A60" s="10" t="s">
         <v>511</v>
       </c>
-      <c r="B60" s="221" t="s">
+      <c r="B60" s="230" t="s">
         <v>507</v>
       </c>
-      <c r="C60" s="222"/>
-      <c r="D60" s="222"/>
-      <c r="E60" s="222"/>
-      <c r="F60" s="222"/>
-      <c r="G60" s="223"/>
+      <c r="C60" s="231"/>
+      <c r="D60" s="231"/>
+      <c r="E60" s="231"/>
+      <c r="F60" s="231"/>
+      <c r="G60" s="232"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="A38:A52"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="B37:G37"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="D29:G29"/>
@@ -41796,49 +41828,17 @@
     <mergeCell ref="D34:G34"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="D35:G35"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="A38:A52"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="B43:G43"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B53:G53"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:G28"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -41849,8 +41849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -41944,7 +41944,7 @@
       <c r="D4" s="265"/>
       <c r="E4" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Intermediate")*(E$10:E$247="Missing"))+0.5*SUMPRODUCT(($A$10:$A$247="Intermediate")*(E$10:E$247="Partial"))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Intermediate")*(F$10:F$247="Missing"))+0.5*SUMPRODUCT(($A$10:$A$247="Intermediate")*(F$10:F$247="Partial"))</f>
@@ -41966,7 +41966,7 @@
       <c r="D5" s="265"/>
       <c r="E5" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Intermediate")*(E$10:E$247="Completed"))+SUMPRODUCT(($A$10:$A$247="Intermediate")*(E$10:E$247="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$247="Intermediate")*(E$10:E$247="Partial"))</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Intermediate")*(F$10:F$247="Completed"))+SUMPRODUCT(($A$10:$A$247="Intermediate")*(F$10:F$247="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$247="Intermediate")*(F$10:F$247="Partial"))</f>
@@ -42062,10 +42062,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>485</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -42311,10 +42311,10 @@
       <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A23" s="232" t="s">
+      <c r="A23" s="235" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="234"/>
+      <c r="B23" s="237"/>
       <c r="C23" s="4" t="s">
         <v>63</v>
       </c>
@@ -42617,10 +42617,10 @@
       <c r="G38" s="11"/>
     </row>
     <row r="39" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A39" s="232" t="s">
+      <c r="A39" s="235" t="s">
         <v>524</v>
       </c>
-      <c r="B39" s="234"/>
+      <c r="B39" s="237"/>
       <c r="C39" s="4" t="s">
         <v>63</v>
       </c>
@@ -42733,10 +42733,10 @@
       <c r="G44" s="11"/>
     </row>
     <row r="45" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A45" s="232" t="s">
+      <c r="A45" s="235" t="s">
         <v>529</v>
       </c>
-      <c r="B45" s="234"/>
+      <c r="B45" s="237"/>
       <c r="C45" s="4" t="s">
         <v>63</v>
       </c>
@@ -42868,10 +42868,10 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A52" s="232" t="s">
+      <c r="A52" s="235" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="234"/>
+      <c r="B52" s="237"/>
       <c r="C52" s="4" t="s">
         <v>63</v>
       </c>
@@ -43041,10 +43041,10 @@
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A61" s="232" t="s">
+      <c r="A61" s="235" t="s">
         <v>111</v>
       </c>
-      <c r="B61" s="234"/>
+      <c r="B61" s="237"/>
       <c r="C61" s="4" t="s">
         <v>63</v>
       </c>
@@ -43138,10 +43138,10 @@
       <c r="G65" s="11"/>
     </row>
     <row r="66" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A66" s="232" t="s">
+      <c r="A66" s="235" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="234"/>
+      <c r="B66" s="237"/>
       <c r="C66" s="4" t="s">
         <v>63</v>
       </c>
@@ -43431,10 +43431,10 @@
       <c r="G80" s="11"/>
     </row>
     <row r="81" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A81" s="232" t="s">
+      <c r="A81" s="235" t="s">
         <v>133</v>
       </c>
-      <c r="B81" s="234"/>
+      <c r="B81" s="237"/>
       <c r="C81" s="4" t="s">
         <v>63</v>
       </c>
@@ -43568,10 +43568,10 @@
       <c r="G87" s="11"/>
     </row>
     <row r="88" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A88" s="232" t="s">
+      <c r="A88" s="235" t="s">
         <v>558</v>
       </c>
-      <c r="B88" s="234"/>
+      <c r="B88" s="237"/>
       <c r="C88" s="4" t="s">
         <v>63</v>
       </c>
@@ -43688,10 +43688,10 @@
       <c r="G93" s="11"/>
     </row>
     <row r="94" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A94" s="232" t="s">
+      <c r="A94" s="235" t="s">
         <v>156</v>
       </c>
-      <c r="B94" s="234"/>
+      <c r="B94" s="237"/>
       <c r="C94" s="4" t="s">
         <v>63</v>
       </c>
@@ -43766,10 +43766,10 @@
       <c r="G97" s="11"/>
     </row>
     <row r="98" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A98" s="232" t="s">
+      <c r="A98" s="235" t="s">
         <v>150</v>
       </c>
-      <c r="B98" s="234"/>
+      <c r="B98" s="237"/>
       <c r="C98" s="4" t="s">
         <v>63</v>
       </c>
@@ -43844,10 +43844,10 @@
       <c r="G101" s="11"/>
     </row>
     <row r="102" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A102" s="232" t="s">
+      <c r="A102" s="235" t="s">
         <v>547</v>
       </c>
-      <c r="B102" s="234"/>
+      <c r="B102" s="237"/>
       <c r="C102" s="4" t="s">
         <v>63</v>
       </c>
@@ -43943,10 +43943,10 @@
       <c r="G106" s="11"/>
     </row>
     <row r="107" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A107" s="232" t="s">
+      <c r="A107" s="235" t="s">
         <v>140</v>
       </c>
-      <c r="B107" s="234"/>
+      <c r="B107" s="237"/>
       <c r="C107" s="4" t="s">
         <v>63</v>
       </c>
@@ -44070,7 +44070,7 @@
       </c>
       <c r="D113" s="11"/>
       <c r="E113" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F113" s="4" t="s">
         <v>52</v>
@@ -44097,10 +44097,10 @@
       <c r="G114" s="11"/>
     </row>
     <row r="115" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A115" s="232" t="s">
+      <c r="A115" s="235" t="s">
         <v>161</v>
       </c>
-      <c r="B115" s="234"/>
+      <c r="B115" s="237"/>
       <c r="C115" s="4" t="s">
         <v>453</v>
       </c>
@@ -44271,6 +44271,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A88:B88"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="C2:D9"/>
@@ -44280,14 +44288,6 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A88:B88"/>
   </mergeCells>
   <conditionalFormatting sqref="A11:A18 A107:A109 A81:A85 A115:A248 A52:A57 A40 A33:A37 A42:A43 A112 A94:A100 A61:A69 A59 A20:A29">
     <cfRule type="beginsWith" dxfId="2421" priority="1148" stopIfTrue="1" operator="beginsWith" text="Exceptional">
@@ -46736,10 +46736,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>701</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -47025,10 +47025,10 @@
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A25" s="232" t="s">
+      <c r="A25" s="235" t="s">
         <v>688</v>
       </c>
-      <c r="B25" s="234"/>
+      <c r="B25" s="237"/>
       <c r="C25" s="4" t="s">
         <v>63</v>
       </c>
@@ -47238,10 +47238,10 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A36" s="232" t="s">
+      <c r="A36" s="235" t="s">
         <v>612</v>
       </c>
-      <c r="B36" s="234"/>
+      <c r="B36" s="237"/>
       <c r="C36" s="4" t="s">
         <v>63</v>
       </c>
@@ -47660,10 +47660,10 @@
       <c r="G57" s="11"/>
     </row>
     <row r="58" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A58" s="232" t="s">
+      <c r="A58" s="235" t="s">
         <v>627</v>
       </c>
-      <c r="B58" s="234"/>
+      <c r="B58" s="237"/>
       <c r="C58" s="4" t="s">
         <v>63</v>
       </c>
@@ -47968,10 +47968,10 @@
       <c r="G73" s="11"/>
     </row>
     <row r="74" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A74" s="232" t="s">
+      <c r="A74" s="235" t="s">
         <v>651</v>
       </c>
-      <c r="B74" s="234"/>
+      <c r="B74" s="237"/>
       <c r="C74" s="4" t="s">
         <v>63</v>
       </c>
@@ -48160,10 +48160,10 @@
       <c r="G83" s="11"/>
     </row>
     <row r="84" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A84" s="232" t="s">
+      <c r="A84" s="235" t="s">
         <v>663</v>
       </c>
-      <c r="B84" s="234"/>
+      <c r="B84" s="237"/>
       <c r="C84" s="21" t="s">
         <v>456</v>
       </c>
@@ -48523,10 +48523,10 @@
       <c r="G102" s="11"/>
     </row>
     <row r="103" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A103" s="232" t="s">
+      <c r="A103" s="235" t="s">
         <v>677</v>
       </c>
-      <c r="B103" s="234"/>
+      <c r="B103" s="237"/>
       <c r="C103" s="4" t="s">
         <v>63</v>
       </c>
@@ -51700,10 +51700,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>291</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -52063,10 +52063,10 @@
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A29" s="232" t="s">
+      <c r="A29" s="235" t="s">
         <v>564</v>
       </c>
-      <c r="B29" s="234"/>
+      <c r="B29" s="237"/>
       <c r="C29" s="4" t="s">
         <v>451</v>
       </c>
@@ -52295,10 +52295,10 @@
       <c r="G40" s="11"/>
     </row>
     <row r="41" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A41" s="232" t="s">
+      <c r="A41" s="235" t="s">
         <v>334</v>
       </c>
-      <c r="B41" s="234"/>
+      <c r="B41" s="237"/>
       <c r="C41" s="4" t="s">
         <v>63</v>
       </c>
@@ -52512,10 +52512,10 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" s="7" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A52" s="232" t="s">
+      <c r="A52" s="235" t="s">
         <v>84</v>
       </c>
-      <c r="B52" s="234"/>
+      <c r="B52" s="237"/>
       <c r="C52" s="4" t="s">
         <v>63</v>
       </c>
@@ -52685,10 +52685,10 @@
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" s="7" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A61" s="232" t="s">
+      <c r="A61" s="235" t="s">
         <v>370</v>
       </c>
-      <c r="B61" s="234"/>
+      <c r="B61" s="237"/>
       <c r="C61" s="21" t="s">
         <v>452</v>
       </c>
@@ -54038,10 +54038,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>810</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -54344,10 +54344,10 @@
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A26" s="232" t="s">
+      <c r="A26" s="235" t="s">
         <v>390</v>
       </c>
-      <c r="B26" s="234"/>
+      <c r="B26" s="237"/>
       <c r="C26" s="4" t="s">
         <v>855</v>
       </c>
@@ -54614,10 +54614,10 @@
       <c r="G39" s="11"/>
     </row>
     <row r="40" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A40" s="232" t="s">
+      <c r="A40" s="235" t="s">
         <v>448</v>
       </c>
-      <c r="B40" s="234"/>
+      <c r="B40" s="237"/>
       <c r="C40" s="102" t="s">
         <v>856</v>
       </c>
@@ -54882,10 +54882,10 @@
       <c r="G53" s="11"/>
     </row>
     <row r="54" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A54" s="232" t="s">
+      <c r="A54" s="235" t="s">
         <v>412</v>
       </c>
-      <c r="B54" s="234"/>
+      <c r="B54" s="237"/>
       <c r="C54" s="4" t="s">
         <v>63</v>
       </c>
@@ -56748,10 +56748,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>239</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -56845,10 +56845,10 @@
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A15" s="232" t="s">
+      <c r="A15" s="235" t="s">
         <v>246</v>
       </c>
-      <c r="B15" s="234"/>
+      <c r="B15" s="237"/>
       <c r="C15" s="4" t="s">
         <v>874</v>
       </c>
@@ -56961,10 +56961,10 @@
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A21" s="232" t="s">
+      <c r="A21" s="235" t="s">
         <v>878</v>
       </c>
-      <c r="B21" s="234"/>
+      <c r="B21" s="237"/>
       <c r="C21" s="4" t="s">
         <v>63</v>
       </c>
@@ -57096,10 +57096,10 @@
       <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A28" s="232" t="s">
+      <c r="A28" s="235" t="s">
         <v>254</v>
       </c>
-      <c r="B28" s="234"/>
+      <c r="B28" s="237"/>
       <c r="C28" s="4" t="s">
         <v>875</v>
       </c>
@@ -57250,10 +57250,10 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A36" s="232" t="s">
+      <c r="A36" s="235" t="s">
         <v>891</v>
       </c>
-      <c r="B36" s="234"/>
+      <c r="B36" s="237"/>
       <c r="C36" s="4" t="s">
         <v>454</v>
       </c>
@@ -57385,10 +57385,10 @@
       <c r="G42" s="11"/>
     </row>
     <row r="43" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A43" s="232" t="s">
+      <c r="A43" s="235" t="s">
         <v>275</v>
       </c>
-      <c r="B43" s="234"/>
+      <c r="B43" s="237"/>
       <c r="C43" s="4" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Fixed cheat code to properly set bools when triggered.  Updated rubric.
</commit_message>
<xml_diff>
--- a/GameDocuments/gam352_papercut_rubric.xlsx
+++ b/GameDocuments/gam352_papercut_rubric.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2317" uniqueCount="977">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2318" uniqueCount="978">
   <si>
     <t>GAME NAME</t>
   </si>
@@ -3717,6 +3717,9 @@
   </si>
   <si>
     <t>Presented in humerous way</t>
+  </si>
+  <si>
+    <t>Two member of the team use multiple monitors and the game functions properly.  Unity</t>
   </si>
 </sst>
 </file>
@@ -5759,90 +5762,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -5876,6 +5795,18 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -5933,6 +5864,99 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="4" borderId="16" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="4" borderId="18" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="9" fontId="26" fillId="3" borderId="21" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5943,12 +5967,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="26" fillId="3" borderId="26" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6017,37 +6035,55 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="4" borderId="16" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="4" borderId="18" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6059,28 +6095,28 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6107,52 +6143,19 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -38689,54 +38692,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A1" s="144" t="s">
+      <c r="A1" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="146"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="178"/>
       <c r="E1" s="103"/>
-      <c r="F1" s="144" t="s">
+      <c r="F1" s="176" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
-      <c r="J1" s="146"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="178"/>
       <c r="K1" s="104"/>
       <c r="L1" s="104"/>
       <c r="M1" s="105"/>
     </row>
     <row r="2" spans="1:13" ht="14.1" customHeight="1">
-      <c r="A2" s="147" t="s">
+      <c r="A2" s="182" t="s">
         <v>951</v>
       </c>
-      <c r="B2" s="148"/>
-      <c r="C2" s="148"/>
-      <c r="D2" s="149"/>
+      <c r="B2" s="183"/>
+      <c r="C2" s="183"/>
+      <c r="D2" s="184"/>
       <c r="E2" s="103"/>
-      <c r="F2" s="147" t="s">
+      <c r="F2" s="182" t="s">
         <v>954</v>
       </c>
-      <c r="G2" s="148"/>
-      <c r="H2" s="148"/>
-      <c r="I2" s="148"/>
-      <c r="J2" s="149"/>
+      <c r="G2" s="183"/>
+      <c r="H2" s="183"/>
+      <c r="I2" s="183"/>
+      <c r="J2" s="184"/>
       <c r="K2" s="104"/>
       <c r="L2" s="104"/>
       <c r="M2" s="105"/>
     </row>
     <row r="3" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A3" s="150"/>
-      <c r="B3" s="151"/>
-      <c r="C3" s="151"/>
-      <c r="D3" s="152"/>
+      <c r="A3" s="185"/>
+      <c r="B3" s="186"/>
+      <c r="C3" s="186"/>
+      <c r="D3" s="187"/>
       <c r="E3" s="103"/>
-      <c r="F3" s="150"/>
-      <c r="G3" s="151"/>
-      <c r="H3" s="151"/>
-      <c r="I3" s="151"/>
-      <c r="J3" s="152"/>
+      <c r="F3" s="185"/>
+      <c r="G3" s="186"/>
+      <c r="H3" s="186"/>
+      <c r="I3" s="186"/>
+      <c r="J3" s="187"/>
       <c r="K3" s="104"/>
       <c r="L3" s="104"/>
       <c r="M3" s="105"/>
@@ -38757,41 +38760,41 @@
       <c r="M4" s="105"/>
     </row>
     <row r="5" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A5" s="144" t="s">
+      <c r="A5" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="145"/>
-      <c r="C5" s="145"/>
-      <c r="D5" s="146"/>
+      <c r="B5" s="177"/>
+      <c r="C5" s="177"/>
+      <c r="D5" s="178"/>
       <c r="E5" s="103"/>
-      <c r="F5" s="144" t="s">
+      <c r="F5" s="176" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="145"/>
-      <c r="H5" s="145"/>
-      <c r="I5" s="145"/>
-      <c r="J5" s="146"/>
+      <c r="G5" s="177"/>
+      <c r="H5" s="177"/>
+      <c r="I5" s="177"/>
+      <c r="J5" s="178"/>
       <c r="K5" s="104"/>
       <c r="L5" s="107"/>
       <c r="M5" s="105"/>
     </row>
     <row r="6" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A6" s="156" t="s">
+      <c r="A6" s="173" t="s">
         <v>952</v>
       </c>
-      <c r="B6" s="157"/>
-      <c r="C6" s="157"/>
-      <c r="D6" s="158"/>
+      <c r="B6" s="174"/>
+      <c r="C6" s="174"/>
+      <c r="D6" s="175"/>
       <c r="E6" s="103"/>
-      <c r="F6" s="156" t="s">
+      <c r="F6" s="173" t="s">
         <v>955</v>
       </c>
-      <c r="G6" s="157"/>
-      <c r="H6" s="157"/>
-      <c r="I6" s="157"/>
-      <c r="J6" s="158"/>
+      <c r="G6" s="174"/>
+      <c r="H6" s="174"/>
+      <c r="I6" s="174"/>
+      <c r="J6" s="175"/>
       <c r="K6" s="104"/>
-      <c r="L6" s="153" t="s">
+      <c r="L6" s="170" t="s">
         <v>24</v>
       </c>
       <c r="M6" s="105"/>
@@ -38802,47 +38805,47 @@
       <c r="C7" s="108"/>
       <c r="D7" s="109"/>
       <c r="E7" s="103"/>
-      <c r="F7" s="156"/>
-      <c r="G7" s="157"/>
-      <c r="H7" s="157"/>
-      <c r="I7" s="157"/>
-      <c r="J7" s="158"/>
+      <c r="F7" s="173"/>
+      <c r="G7" s="174"/>
+      <c r="H7" s="174"/>
+      <c r="I7" s="174"/>
+      <c r="J7" s="175"/>
       <c r="K7" s="104"/>
-      <c r="L7" s="154"/>
+      <c r="L7" s="171"/>
       <c r="M7" s="105"/>
     </row>
     <row r="8" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A8" s="144" t="s">
+      <c r="A8" s="176" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="145"/>
-      <c r="C8" s="145"/>
-      <c r="D8" s="146"/>
+      <c r="B8" s="177"/>
+      <c r="C8" s="177"/>
+      <c r="D8" s="178"/>
       <c r="E8" s="103"/>
-      <c r="F8" s="156"/>
-      <c r="G8" s="157"/>
-      <c r="H8" s="157"/>
-      <c r="I8" s="157"/>
-      <c r="J8" s="158"/>
+      <c r="F8" s="173"/>
+      <c r="G8" s="174"/>
+      <c r="H8" s="174"/>
+      <c r="I8" s="174"/>
+      <c r="J8" s="175"/>
       <c r="K8" s="104"/>
-      <c r="L8" s="154"/>
+      <c r="L8" s="171"/>
       <c r="M8" s="105"/>
     </row>
     <row r="9" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A9" s="156" t="s">
+      <c r="A9" s="173" t="s">
         <v>953</v>
       </c>
-      <c r="B9" s="157"/>
-      <c r="C9" s="157"/>
-      <c r="D9" s="158"/>
+      <c r="B9" s="174"/>
+      <c r="C9" s="174"/>
+      <c r="D9" s="175"/>
       <c r="E9" s="103"/>
-      <c r="F9" s="156"/>
-      <c r="G9" s="157"/>
-      <c r="H9" s="157"/>
-      <c r="I9" s="157"/>
-      <c r="J9" s="158"/>
+      <c r="F9" s="173"/>
+      <c r="G9" s="174"/>
+      <c r="H9" s="174"/>
+      <c r="I9" s="174"/>
+      <c r="J9" s="175"/>
       <c r="K9" s="104"/>
-      <c r="L9" s="155"/>
+      <c r="L9" s="172"/>
       <c r="M9" s="105"/>
     </row>
     <row r="10" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -38861,18 +38864,18 @@
       <c r="M10" s="105"/>
     </row>
     <row r="11" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A11" s="144" t="s">
+      <c r="A11" s="176" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="145"/>
-      <c r="C11" s="145"/>
-      <c r="D11" s="146"/>
+      <c r="B11" s="177"/>
+      <c r="C11" s="177"/>
+      <c r="D11" s="178"/>
       <c r="E11" s="103"/>
-      <c r="F11" s="144" t="s">
+      <c r="F11" s="176" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="145"/>
-      <c r="H11" s="146"/>
+      <c r="G11" s="177"/>
+      <c r="H11" s="178"/>
       <c r="I11" s="134" t="s">
         <v>7</v>
       </c>
@@ -38912,7 +38915,7 @@
         <v>-0.12</v>
       </c>
       <c r="K12" s="104"/>
-      <c r="L12" s="153" t="s">
+      <c r="L12" s="170" t="s">
         <v>8</v>
       </c>
       <c r="M12" s="105"/>
@@ -38945,7 +38948,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="120"/>
-      <c r="L13" s="154"/>
+      <c r="L13" s="171"/>
       <c r="M13" s="121"/>
     </row>
     <row r="14" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -38975,7 +38978,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="124"/>
-      <c r="L14" s="155"/>
+      <c r="L14" s="172"/>
       <c r="M14" s="125"/>
     </row>
     <row r="15" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39043,11 +39046,11 @@
         <v>939</v>
       </c>
       <c r="E17" s="104"/>
-      <c r="F17" s="144" t="s">
+      <c r="F17" s="176" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="145"/>
-      <c r="H17" s="146"/>
+      <c r="G17" s="177"/>
+      <c r="H17" s="178"/>
       <c r="I17" s="111"/>
       <c r="J17" s="135">
         <v>0.75</v>
@@ -39073,17 +39076,17 @@
       <c r="F18" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="159" t="s">
+      <c r="G18" s="179" t="s">
         <v>956</v>
       </c>
-      <c r="H18" s="160"/>
-      <c r="I18" s="161"/>
+      <c r="H18" s="180"/>
+      <c r="I18" s="181"/>
       <c r="J18" s="137">
         <f>IF(LEFT(G18,6)="Entire",0,IF(LEFT(G18,6)="Custom",-0.05,-0.1))</f>
         <v>-0.1</v>
       </c>
       <c r="K18" s="128"/>
-      <c r="L18" s="153" t="s">
+      <c r="L18" s="170" t="s">
         <v>18</v>
       </c>
       <c r="M18" s="105"/>
@@ -39103,17 +39106,17 @@
       <c r="F19" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="162" t="s">
+      <c r="G19" s="153" t="s">
         <v>957</v>
       </c>
-      <c r="H19" s="163"/>
-      <c r="I19" s="164"/>
+      <c r="H19" s="154"/>
+      <c r="I19" s="155"/>
       <c r="J19" s="139">
         <f>IF(G19="2D Graphics and 2D Gameplay",IF(J11=0.15,-0.05,0),IF(G19="3D Graphics but 2D Gameplay",IF(J11=0.15,-0.02,-0.3),IF(J11=0.15,0,-0.3)))</f>
         <v>0</v>
       </c>
       <c r="K19" s="104"/>
-      <c r="L19" s="155"/>
+      <c r="L19" s="172"/>
       <c r="M19" s="105"/>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39163,22 +39166,22 @@
       <c r="C22" s="118"/>
       <c r="D22" s="119"/>
       <c r="E22" s="104"/>
-      <c r="F22" s="186" t="s">
+      <c r="F22" s="168" t="s">
         <v>713</v>
       </c>
-      <c r="G22" s="184" t="s">
+      <c r="G22" s="166" t="s">
         <v>714</v>
       </c>
-      <c r="H22" s="183"/>
+      <c r="H22" s="165"/>
       <c r="I22" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="181">
+      <c r="J22" s="163">
         <f>J20+J15</f>
         <v>0.68</v>
       </c>
       <c r="K22" s="104"/>
-      <c r="L22" s="165" t="s">
+      <c r="L22" s="144" t="s">
         <v>725</v>
       </c>
       <c r="M22" s="105"/>
@@ -39189,15 +39192,15 @@
       <c r="C23" s="118"/>
       <c r="D23" s="119"/>
       <c r="E23" s="104"/>
-      <c r="F23" s="187"/>
-      <c r="G23" s="185"/>
-      <c r="H23" s="183"/>
+      <c r="F23" s="169"/>
+      <c r="G23" s="167"/>
+      <c r="H23" s="165"/>
       <c r="I23" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="182"/>
+      <c r="J23" s="164"/>
       <c r="K23" s="104"/>
-      <c r="L23" s="166"/>
+      <c r="L23" s="145"/>
       <c r="M23" s="105"/>
     </row>
     <row r="24" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -39221,13 +39224,13 @@
       <c r="C25" s="118"/>
       <c r="D25" s="119"/>
       <c r="E25" s="104"/>
-      <c r="F25" s="175" t="s">
+      <c r="F25" s="157" t="s">
         <v>932</v>
       </c>
-      <c r="G25" s="176"/>
-      <c r="H25" s="176"/>
-      <c r="I25" s="176"/>
-      <c r="J25" s="177"/>
+      <c r="G25" s="158"/>
+      <c r="H25" s="158"/>
+      <c r="I25" s="158"/>
+      <c r="J25" s="159"/>
       <c r="K25" s="104"/>
       <c r="L25" s="104"/>
       <c r="M25" s="105"/>
@@ -39238,11 +39241,11 @@
       <c r="C26" s="118"/>
       <c r="D26" s="119"/>
       <c r="E26" s="103"/>
-      <c r="F26" s="178"/>
-      <c r="G26" s="179"/>
-      <c r="H26" s="179"/>
-      <c r="I26" s="179"/>
-      <c r="J26" s="180"/>
+      <c r="F26" s="160"/>
+      <c r="G26" s="161"/>
+      <c r="H26" s="161"/>
+      <c r="I26" s="161"/>
+      <c r="J26" s="162"/>
       <c r="K26" s="104"/>
       <c r="L26" s="104"/>
       <c r="M26" s="105"/>
@@ -39268,13 +39271,13 @@
       <c r="C28" s="118"/>
       <c r="D28" s="119"/>
       <c r="E28" s="103"/>
-      <c r="F28" s="174" t="s">
+      <c r="F28" s="156" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="174"/>
-      <c r="H28" s="174"/>
-      <c r="I28" s="174"/>
-      <c r="J28" s="174"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
       <c r="K28" s="104"/>
       <c r="L28" s="104"/>
       <c r="M28" s="105"/>
@@ -39285,13 +39288,13 @@
       <c r="C29" s="118"/>
       <c r="D29" s="119"/>
       <c r="E29" s="103"/>
-      <c r="F29" s="171" t="s">
+      <c r="F29" s="150" t="s">
         <v>933</v>
       </c>
-      <c r="G29" s="172"/>
-      <c r="H29" s="172"/>
-      <c r="I29" s="172"/>
-      <c r="J29" s="173"/>
+      <c r="G29" s="151"/>
+      <c r="H29" s="151"/>
+      <c r="I29" s="151"/>
+      <c r="J29" s="152"/>
       <c r="K29" s="104"/>
       <c r="L29" s="104"/>
       <c r="M29" s="105"/>
@@ -39302,30 +39305,30 @@
       <c r="C30" s="118"/>
       <c r="D30" s="119"/>
       <c r="E30" s="103"/>
-      <c r="F30" s="171"/>
-      <c r="G30" s="172"/>
-      <c r="H30" s="172"/>
-      <c r="I30" s="172"/>
-      <c r="J30" s="173"/>
+      <c r="F30" s="150"/>
+      <c r="G30" s="151"/>
+      <c r="H30" s="151"/>
+      <c r="I30" s="151"/>
+      <c r="J30" s="152"/>
       <c r="K30" s="104"/>
       <c r="L30" s="104"/>
       <c r="M30" s="105"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A31" s="167" t="s">
+      <c r="A31" s="146" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="168"/>
-      <c r="C31" s="169" t="s">
+      <c r="B31" s="147"/>
+      <c r="C31" s="148" t="s">
         <v>950</v>
       </c>
-      <c r="D31" s="170"/>
+      <c r="D31" s="149"/>
       <c r="E31" s="104"/>
-      <c r="F31" s="162"/>
-      <c r="G31" s="163"/>
-      <c r="H31" s="163"/>
-      <c r="I31" s="163"/>
-      <c r="J31" s="164"/>
+      <c r="F31" s="153"/>
+      <c r="G31" s="154"/>
+      <c r="H31" s="154"/>
+      <c r="I31" s="154"/>
+      <c r="J31" s="155"/>
       <c r="K31" s="104"/>
       <c r="L31" s="104"/>
       <c r="M31" s="105"/>
@@ -39348,16 +39351,12 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0"/>
   <mergeCells count="31">
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F29:J31"/>
-    <mergeCell ref="F28:J28"/>
-    <mergeCell ref="F25:J26"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A2:D3"/>
+    <mergeCell ref="F2:J3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:J5"/>
     <mergeCell ref="L12:L14"/>
     <mergeCell ref="L18:L19"/>
     <mergeCell ref="A6:D6"/>
@@ -39373,12 +39372,16 @@
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="G18:I18"/>
     <mergeCell ref="G19:I19"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="A2:D3"/>
-    <mergeCell ref="F2:J3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F29:J31"/>
+    <mergeCell ref="F28:J28"/>
+    <mergeCell ref="F25:J26"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F22:F23"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6:D6">
@@ -39446,57 +39449,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A1" s="194" t="s">
+      <c r="A1" s="199" t="s">
         <v>556</v>
       </c>
-      <c r="B1" s="195"/>
-      <c r="C1" s="195"/>
-      <c r="D1" s="195"/>
-      <c r="E1" s="195"/>
-      <c r="F1" s="195"/>
-      <c r="G1" s="195"/>
-      <c r="H1" s="195"/>
-      <c r="J1" s="205" t="s">
+      <c r="B1" s="200"/>
+      <c r="C1" s="200"/>
+      <c r="D1" s="200"/>
+      <c r="E1" s="200"/>
+      <c r="F1" s="200"/>
+      <c r="G1" s="200"/>
+      <c r="H1" s="200"/>
+      <c r="J1" s="210" t="s">
         <v>482</v>
       </c>
-      <c r="K1" s="206"/>
-      <c r="L1" s="207"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="212"/>
       <c r="M1" s="79"/>
       <c r="N1" s="24" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A2" s="194"/>
-      <c r="B2" s="195"/>
-      <c r="C2" s="195"/>
-      <c r="D2" s="195"/>
-      <c r="E2" s="195"/>
-      <c r="F2" s="195"/>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
-      <c r="J2" s="208" t="s">
+      <c r="A2" s="199"/>
+      <c r="B2" s="200"/>
+      <c r="C2" s="200"/>
+      <c r="D2" s="200"/>
+      <c r="E2" s="200"/>
+      <c r="F2" s="200"/>
+      <c r="G2" s="200"/>
+      <c r="H2" s="200"/>
+      <c r="J2" s="213" t="s">
         <v>706</v>
       </c>
-      <c r="K2" s="209"/>
-      <c r="L2" s="210"/>
+      <c r="K2" s="214"/>
+      <c r="L2" s="215"/>
       <c r="M2" s="23"/>
       <c r="N2" s="26" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A3" s="194"/>
-      <c r="B3" s="195"/>
-      <c r="C3" s="195"/>
-      <c r="D3" s="195"/>
-      <c r="E3" s="195"/>
-      <c r="F3" s="195"/>
-      <c r="G3" s="195"/>
-      <c r="H3" s="195"/>
-      <c r="J3" s="208"/>
-      <c r="K3" s="209"/>
-      <c r="L3" s="210"/>
+      <c r="A3" s="199"/>
+      <c r="B3" s="200"/>
+      <c r="C3" s="200"/>
+      <c r="D3" s="200"/>
+      <c r="E3" s="200"/>
+      <c r="F3" s="200"/>
+      <c r="G3" s="200"/>
+      <c r="H3" s="200"/>
+      <c r="J3" s="213"/>
+      <c r="K3" s="214"/>
+      <c r="L3" s="215"/>
       <c r="M3" s="23"/>
       <c r="N3" s="26" t="s">
         <v>431</v>
@@ -39506,14 +39509,14 @@
       <c r="A4" s="2"/>
       <c r="B4" s="5"/>
       <c r="C4" s="8"/>
-      <c r="D4" s="193"/>
-      <c r="E4" s="193"/>
+      <c r="D4" s="192"/>
+      <c r="E4" s="192"/>
       <c r="F4" s="43"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="193"/>
-      <c r="J4" s="208"/>
-      <c r="K4" s="209"/>
-      <c r="L4" s="210"/>
+      <c r="G4" s="192"/>
+      <c r="H4" s="192"/>
+      <c r="J4" s="213"/>
+      <c r="K4" s="214"/>
+      <c r="L4" s="215"/>
       <c r="M4" s="34"/>
       <c r="N4" s="26" t="s">
         <v>432</v>
@@ -39521,24 +39524,24 @@
       <c r="O4" s="81"/>
     </row>
     <row r="5" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A5" s="196" t="s">
+      <c r="A5" s="201" t="s">
         <v>425</v>
       </c>
-      <c r="B5" s="197"/>
+      <c r="B5" s="202"/>
       <c r="C5" s="8"/>
-      <c r="D5" s="200" t="s">
+      <c r="D5" s="205" t="s">
         <v>717</v>
       </c>
-      <c r="E5" s="201"/>
-      <c r="F5" s="202"/>
-      <c r="G5" s="203">
+      <c r="E5" s="206"/>
+      <c r="F5" s="207"/>
+      <c r="G5" s="208">
         <f>Submission!$E$17</f>
         <v>0</v>
       </c>
-      <c r="H5" s="204"/>
-      <c r="J5" s="208"/>
-      <c r="K5" s="209"/>
-      <c r="L5" s="210"/>
+      <c r="H5" s="209"/>
+      <c r="J5" s="213"/>
+      <c r="K5" s="214"/>
+      <c r="L5" s="215"/>
       <c r="M5" s="34"/>
       <c r="N5" s="26" t="s">
         <v>433</v>
@@ -39546,21 +39549,21 @@
       <c r="O5" s="81"/>
     </row>
     <row r="6" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A6" s="198"/>
-      <c r="B6" s="199"/>
+      <c r="A6" s="203"/>
+      <c r="B6" s="204"/>
       <c r="C6" s="43"/>
-      <c r="D6" s="193" t="s">
+      <c r="D6" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="193"/>
+      <c r="E6" s="192"/>
       <c r="F6" s="43"/>
-      <c r="G6" s="193" t="s">
+      <c r="G6" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="193"/>
-      <c r="J6" s="208"/>
-      <c r="K6" s="209"/>
-      <c r="L6" s="210"/>
+      <c r="H6" s="192"/>
+      <c r="J6" s="213"/>
+      <c r="K6" s="214"/>
+      <c r="L6" s="215"/>
       <c r="M6" s="34"/>
       <c r="N6" s="26" t="s">
         <v>434</v>
@@ -39568,24 +39571,24 @@
       <c r="O6" s="81"/>
     </row>
     <row r="7" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A7" s="188">
+      <c r="A7" s="195">
         <f>'Game Data'!$J$22</f>
         <v>0.68</v>
       </c>
-      <c r="B7" s="189"/>
+      <c r="B7" s="196"/>
       <c r="C7" s="43"/>
-      <c r="D7" s="216" t="s">
+      <c r="D7" s="193" t="s">
         <v>724</v>
       </c>
-      <c r="E7" s="217"/>
+      <c r="E7" s="194"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="216" t="s">
+      <c r="G7" s="193" t="s">
         <v>724</v>
       </c>
-      <c r="H7" s="217"/>
-      <c r="J7" s="208"/>
-      <c r="K7" s="209"/>
-      <c r="L7" s="210"/>
+      <c r="H7" s="194"/>
+      <c r="J7" s="213"/>
+      <c r="K7" s="214"/>
+      <c r="L7" s="215"/>
       <c r="M7" s="33"/>
       <c r="N7" s="26" t="s">
         <v>435</v>
@@ -39593,23 +39596,23 @@
       <c r="O7" s="81"/>
     </row>
     <row r="8" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A8" s="190"/>
-      <c r="B8" s="191"/>
+      <c r="A8" s="197"/>
+      <c r="B8" s="198"/>
       <c r="C8" s="97"/>
-      <c r="D8" s="214">
+      <c r="D8" s="219">
         <f>E17+E26+E35+E44+E53</f>
-        <v>0.29000000000000004</v>
-      </c>
-      <c r="E8" s="215"/>
+        <v>0.29749999999999999</v>
+      </c>
+      <c r="E8" s="220"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="214">
+      <c r="G8" s="219">
         <f>H17+H26+H35+H44+H53</f>
         <v>0</v>
       </c>
-      <c r="H8" s="215"/>
-      <c r="J8" s="211"/>
-      <c r="K8" s="212"/>
-      <c r="L8" s="213"/>
+      <c r="H8" s="220"/>
+      <c r="J8" s="216"/>
+      <c r="K8" s="217"/>
+      <c r="L8" s="218"/>
       <c r="M8" s="80"/>
       <c r="N8" s="25" t="s">
         <v>436</v>
@@ -39620,15 +39623,15 @@
       <c r="A9" s="2"/>
       <c r="B9" s="5"/>
       <c r="C9" s="43"/>
-      <c r="D9" s="193" t="s">
+      <c r="D9" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="193"/>
+      <c r="E9" s="192"/>
       <c r="F9" s="43"/>
-      <c r="G9" s="193" t="s">
+      <c r="G9" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="193"/>
+      <c r="H9" s="192"/>
       <c r="J9" s="82"/>
       <c r="K9" s="82"/>
       <c r="L9" s="82"/>
@@ -39655,11 +39658,11 @@
       <c r="H10" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="192" t="s">
+      <c r="J10" s="191" t="s">
         <v>707</v>
       </c>
-      <c r="K10" s="192"/>
-      <c r="L10" s="192"/>
+      <c r="K10" s="191"/>
+      <c r="L10" s="191"/>
       <c r="O10" s="84"/>
     </row>
     <row r="11" spans="1:15" ht="14.1" customHeight="1">
@@ -39688,11 +39691,11 @@
         <f t="shared" ref="H11:H16" si="1">$B11*G11</f>
         <v>0</v>
       </c>
-      <c r="J11" s="220" t="s">
+      <c r="J11" s="190" t="s">
         <v>792</v>
       </c>
-      <c r="K11" s="220"/>
-      <c r="L11" s="220"/>
+      <c r="K11" s="190"/>
+      <c r="L11" s="190"/>
       <c r="M11" s="82"/>
       <c r="O11" s="84"/>
     </row>
@@ -39722,9 +39725,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J12" s="220"/>
-      <c r="K12" s="220"/>
-      <c r="L12" s="220"/>
+      <c r="J12" s="190"/>
+      <c r="K12" s="190"/>
+      <c r="L12" s="190"/>
       <c r="M12" s="82"/>
       <c r="O12" s="84"/>
     </row>
@@ -39754,9 +39757,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="220"/>
-      <c r="K13" s="220"/>
-      <c r="L13" s="220"/>
+      <c r="J13" s="190"/>
+      <c r="K13" s="190"/>
+      <c r="L13" s="190"/>
       <c r="M13" s="82"/>
       <c r="O13" s="84"/>
     </row>
@@ -39807,11 +39810,11 @@
       <c r="C15" s="37"/>
       <c r="D15" s="39">
         <f>TECH!$E$8</f>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="E15" s="47">
         <f t="shared" si="0"/>
-        <v>3.7499999999999999E-3</v>
+        <v>1.125E-2</v>
       </c>
       <c r="F15" s="43"/>
       <c r="G15" s="39">
@@ -39822,11 +39825,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J15" s="218">
+      <c r="J15" s="188">
         <f>MAX(0,MIN(1,IF($J17 &lt;= 0.95, ROUND($J17,2), FLOOR((0.95+($J17-0.95)/5),0.01))))</f>
-        <v>0.84</v>
-      </c>
-      <c r="L15" s="218">
+        <v>0.85</v>
+      </c>
+      <c r="L15" s="188">
         <f>MAX(0,MIN(1,IF($L17 &lt;= 0.95, ROUND($L17,2), FLOOR((0.95+($L17-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -39859,8 +39862,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J16" s="219"/>
-      <c r="L16" s="219"/>
+      <c r="J16" s="189"/>
+      <c r="L16" s="189"/>
       <c r="M16" s="82"/>
       <c r="O16" s="84"/>
     </row>
@@ -39873,7 +39876,7 @@
       </c>
       <c r="E17" s="41">
         <f>SUM(E11:E16)</f>
-        <v>3.3750000000000002E-2</v>
+        <v>4.1249999999999995E-2</v>
       </c>
       <c r="F17" s="43"/>
       <c r="G17" s="22" t="s">
@@ -39885,7 +39888,7 @@
       </c>
       <c r="J17" s="87">
         <f>$A$7+$E17+IF($D$8-$E17 &gt; 0, ($D$8-$E17)/2, $D$8-$E17)+$G$5</f>
-        <v>0.84187500000000015</v>
+        <v>0.84937499999999999</v>
       </c>
       <c r="L17" s="87">
         <f>$A$7+$H17+IF($G$8 &gt; 0, ($G$8-$H17)/2, $G$8-$H17)+$G$5</f>
@@ -39897,15 +39900,15 @@
       <c r="A18" s="2"/>
       <c r="B18" s="5"/>
       <c r="C18" s="43"/>
-      <c r="D18" s="193" t="s">
+      <c r="D18" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="193"/>
+      <c r="E18" s="192"/>
       <c r="F18" s="43"/>
-      <c r="G18" s="193" t="s">
+      <c r="G18" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="193"/>
+      <c r="H18" s="192"/>
       <c r="J18" s="88"/>
       <c r="M18" s="78"/>
     </row>
@@ -39930,11 +39933,11 @@
       <c r="H19" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="192" t="s">
+      <c r="J19" s="191" t="s">
         <v>715</v>
       </c>
-      <c r="K19" s="192"/>
-      <c r="L19" s="192"/>
+      <c r="K19" s="191"/>
+      <c r="L19" s="191"/>
       <c r="M19" s="83"/>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1">
@@ -39963,11 +39966,11 @@
         <f t="shared" ref="H20:H25" si="3">$B20*G20</f>
         <v>0</v>
       </c>
-      <c r="J20" s="220" t="s">
+      <c r="J20" s="190" t="s">
         <v>722</v>
       </c>
-      <c r="K20" s="220"/>
-      <c r="L20" s="220"/>
+      <c r="K20" s="190"/>
+      <c r="L20" s="190"/>
       <c r="M20" s="84"/>
     </row>
     <row r="21" spans="1:13" ht="14.1" customHeight="1">
@@ -39996,9 +39999,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J21" s="220"/>
-      <c r="K21" s="220"/>
-      <c r="L21" s="220"/>
+      <c r="J21" s="190"/>
+      <c r="K21" s="190"/>
+      <c r="L21" s="190"/>
       <c r="M21" s="84"/>
     </row>
     <row r="22" spans="1:13" ht="14.1" customHeight="1">
@@ -40027,9 +40030,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J22" s="220"/>
-      <c r="K22" s="220"/>
-      <c r="L22" s="220"/>
+      <c r="J22" s="190"/>
+      <c r="K22" s="190"/>
+      <c r="L22" s="190"/>
       <c r="M22" s="84"/>
     </row>
     <row r="23" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40093,11 +40096,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J24" s="218">
+      <c r="J24" s="188">
         <f>MAX(0,MIN(1,IF($J26 &lt;= 0.95, ROUND($J26,2), FLOOR((0.95+($J26-0.95)/5),0.01))))</f>
         <v>0.86</v>
       </c>
-      <c r="L24" s="218">
+      <c r="L24" s="188">
         <f>MAX(0,MIN(1,IF($L26 &lt;= 0.95, ROUND($L26,2), FLOOR((0.95+($L26-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40129,8 +40132,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J25" s="219"/>
-      <c r="L25" s="219"/>
+      <c r="J25" s="189"/>
+      <c r="L25" s="189"/>
       <c r="M25" s="84"/>
     </row>
     <row r="26" spans="1:13" ht="14.1" customHeight="1">
@@ -40166,15 +40169,15 @@
       <c r="A27" s="2"/>
       <c r="B27" s="5"/>
       <c r="C27" s="43"/>
-      <c r="D27" s="193" t="s">
+      <c r="D27" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="193"/>
+      <c r="E27" s="192"/>
       <c r="F27" s="43"/>
-      <c r="G27" s="193" t="s">
+      <c r="G27" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H27" s="193"/>
+      <c r="H27" s="192"/>
     </row>
     <row r="28" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
       <c r="A28" s="1" t="s">
@@ -40197,11 +40200,11 @@
       <c r="H28" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J28" s="192" t="s">
+      <c r="J28" s="191" t="s">
         <v>709</v>
       </c>
-      <c r="K28" s="192"/>
-      <c r="L28" s="192"/>
+      <c r="K28" s="191"/>
+      <c r="L28" s="191"/>
     </row>
     <row r="29" spans="1:13" ht="14.1" customHeight="1">
       <c r="A29" s="57" t="str">
@@ -40229,11 +40232,11 @@
         <f t="shared" ref="H29:H34" si="5">$B29*G29</f>
         <v>0</v>
       </c>
-      <c r="J29" s="220" t="s">
+      <c r="J29" s="190" t="s">
         <v>710</v>
       </c>
-      <c r="K29" s="220"/>
-      <c r="L29" s="220"/>
+      <c r="K29" s="190"/>
+      <c r="L29" s="190"/>
     </row>
     <row r="30" spans="1:13" ht="14.1" customHeight="1">
       <c r="A30" s="58" t="str">
@@ -40261,9 +40264,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J30" s="220"/>
-      <c r="K30" s="220"/>
-      <c r="L30" s="220"/>
+      <c r="J30" s="190"/>
+      <c r="K30" s="190"/>
+      <c r="L30" s="190"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1">
       <c r="A31" s="58" t="str">
@@ -40291,9 +40294,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J31" s="220"/>
-      <c r="K31" s="220"/>
-      <c r="L31" s="220"/>
+      <c r="J31" s="190"/>
+      <c r="K31" s="190"/>
+      <c r="L31" s="190"/>
     </row>
     <row r="32" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
       <c r="A32" s="58" t="str">
@@ -40355,11 +40358,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J33" s="218">
+      <c r="J33" s="188">
         <f>MAX(0,MIN(1,IF($J35 &lt;= 0.95, ROUND($J35,2), FLOOR((0.95+($J35-0.95)/5),0.01))))</f>
         <v>0.88</v>
       </c>
-      <c r="L33" s="218">
+      <c r="L33" s="188">
         <f>MAX(0,MIN(1,IF($L35 &lt;= 0.95, ROUND($L35,2), FLOOR((0.95+($L35-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40390,8 +40393,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J34" s="219"/>
-      <c r="L34" s="219"/>
+      <c r="J34" s="189"/>
+      <c r="L34" s="189"/>
     </row>
     <row r="35" spans="1:12" ht="14.1" customHeight="1">
       <c r="A35" s="2"/>
@@ -40425,15 +40428,15 @@
       <c r="A36" s="2"/>
       <c r="B36" s="5"/>
       <c r="C36" s="43"/>
-      <c r="D36" s="193" t="s">
+      <c r="D36" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="193"/>
+      <c r="E36" s="192"/>
       <c r="F36" s="43"/>
-      <c r="G36" s="193" t="s">
+      <c r="G36" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H36" s="193"/>
+      <c r="H36" s="192"/>
     </row>
     <row r="37" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A37" s="1" t="s">
@@ -40456,11 +40459,11 @@
       <c r="H37" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J37" s="192" t="s">
+      <c r="J37" s="191" t="s">
         <v>711</v>
       </c>
-      <c r="K37" s="192"/>
-      <c r="L37" s="192"/>
+      <c r="K37" s="191"/>
+      <c r="L37" s="191"/>
     </row>
     <row r="38" spans="1:12" ht="14.1" customHeight="1">
       <c r="A38" s="57" t="str">
@@ -40488,11 +40491,11 @@
         <f t="shared" ref="H38:H43" si="7">$B38*G38</f>
         <v>0</v>
       </c>
-      <c r="J38" s="220" t="s">
+      <c r="J38" s="190" t="s">
         <v>712</v>
       </c>
-      <c r="K38" s="220"/>
-      <c r="L38" s="220"/>
+      <c r="K38" s="190"/>
+      <c r="L38" s="190"/>
     </row>
     <row r="39" spans="1:12" ht="14.1" customHeight="1">
       <c r="A39" s="58" t="str">
@@ -40520,9 +40523,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J39" s="220"/>
-      <c r="K39" s="220"/>
-      <c r="L39" s="220"/>
+      <c r="J39" s="190"/>
+      <c r="K39" s="190"/>
+      <c r="L39" s="190"/>
     </row>
     <row r="40" spans="1:12" ht="14.1" customHeight="1">
       <c r="A40" s="58" t="str">
@@ -40550,9 +40553,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J40" s="220"/>
-      <c r="K40" s="220"/>
-      <c r="L40" s="220"/>
+      <c r="J40" s="190"/>
+      <c r="K40" s="190"/>
+      <c r="L40" s="190"/>
     </row>
     <row r="41" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A41" s="58" t="str">
@@ -40614,11 +40617,11 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J42" s="218">
+      <c r="J42" s="188">
         <f>MAX(0,MIN(1,IF($J44 &lt;= 0.95, ROUND($J44,2), FLOOR((0.95+($J44-0.95)/5),0.01))))</f>
         <v>0.73</v>
       </c>
-      <c r="L42" s="218">
+      <c r="L42" s="188">
         <f>MAX(0,MIN(1,IF($L44 &lt;= 0.95, ROUND($L44,2), FLOOR((0.95+($L44-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -40649,8 +40652,8 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J43" s="219"/>
-      <c r="L43" s="219"/>
+      <c r="J43" s="189"/>
+      <c r="L43" s="189"/>
     </row>
     <row r="44" spans="1:12" ht="14.1" customHeight="1">
       <c r="A44" s="2"/>
@@ -40684,15 +40687,15 @@
       <c r="A45" s="2"/>
       <c r="B45" s="5"/>
       <c r="C45" s="43"/>
-      <c r="D45" s="193" t="s">
+      <c r="D45" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="193"/>
+      <c r="E45" s="192"/>
       <c r="F45" s="43"/>
-      <c r="G45" s="193" t="s">
+      <c r="G45" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="193"/>
+      <c r="H45" s="192"/>
     </row>
     <row r="46" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A46" s="1" t="s">
@@ -40900,34 +40903,6 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="L42:L43"/>
-    <mergeCell ref="J29:L31"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="L33:L34"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="J38:L40"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="J11:L13"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J20:L22"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G36:H36"/>
     <mergeCell ref="A7:B8"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="D6:E6"/>
@@ -40941,6 +40916,34 @@
     <mergeCell ref="J2:L8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G8:H8"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="J11:L13"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J20:L22"/>
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="J29:L31"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="L33:L34"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="J38:L40"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -40968,59 +40971,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A1" s="235" t="s">
+      <c r="A1" s="232" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="237"/>
+      <c r="B1" s="233"/>
+      <c r="C1" s="233"/>
+      <c r="D1" s="233"/>
+      <c r="E1" s="233"/>
+      <c r="F1" s="233"/>
+      <c r="G1" s="234"/>
     </row>
     <row r="2" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A2" s="230" t="s">
+      <c r="A2" s="221" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="231"/>
-      <c r="C2" s="231"/>
-      <c r="D2" s="231"/>
-      <c r="E2" s="231"/>
-      <c r="F2" s="231"/>
-      <c r="G2" s="232"/>
+      <c r="B2" s="222"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="223"/>
     </row>
     <row r="3" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A3" s="227" t="s">
+      <c r="A3" s="238" t="s">
         <v>930</v>
       </c>
-      <c r="B3" s="228"/>
-      <c r="C3" s="228"/>
-      <c r="D3" s="228"/>
-      <c r="E3" s="228"/>
-      <c r="F3" s="228"/>
-      <c r="G3" s="229"/>
+      <c r="B3" s="239"/>
+      <c r="C3" s="239"/>
+      <c r="D3" s="239"/>
+      <c r="E3" s="239"/>
+      <c r="F3" s="239"/>
+      <c r="G3" s="240"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A4" s="230" t="s">
+      <c r="A4" s="221" t="s">
         <v>438</v>
       </c>
-      <c r="B4" s="231"/>
-      <c r="C4" s="231"/>
-      <c r="D4" s="231"/>
-      <c r="E4" s="231"/>
-      <c r="F4" s="231"/>
-      <c r="G4" s="232"/>
+      <c r="B4" s="222"/>
+      <c r="C4" s="222"/>
+      <c r="D4" s="222"/>
+      <c r="E4" s="222"/>
+      <c r="F4" s="222"/>
+      <c r="G4" s="223"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A5" s="238" t="s">
+      <c r="A5" s="249" t="s">
         <v>580</v>
       </c>
-      <c r="B5" s="239"/>
-      <c r="C5" s="239"/>
-      <c r="D5" s="239"/>
-      <c r="E5" s="239"/>
-      <c r="F5" s="239"/>
-      <c r="G5" s="240"/>
+      <c r="B5" s="250"/>
+      <c r="C5" s="250"/>
+      <c r="D5" s="250"/>
+      <c r="E5" s="250"/>
+      <c r="F5" s="250"/>
+      <c r="G5" s="251"/>
     </row>
     <row r="6" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
       <c r="A6" s="2"/>
@@ -41053,10 +41056,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75">
-      <c r="A8" s="233" t="s">
+      <c r="A8" s="247" t="s">
         <v>718</v>
       </c>
-      <c r="B8" s="234"/>
+      <c r="B8" s="248"/>
       <c r="C8" s="65">
         <v>0</v>
       </c>
@@ -41073,10 +41076,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75">
-      <c r="A9" s="242" t="s">
+      <c r="A9" s="253" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="243"/>
+      <c r="B9" s="254"/>
       <c r="C9" s="92">
         <v>0</v>
       </c>
@@ -41093,10 +41096,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75">
-      <c r="A10" s="244" t="s">
+      <c r="A10" s="255" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="245"/>
+      <c r="B10" s="256"/>
       <c r="C10" s="69">
         <v>0</v>
       </c>
@@ -41113,10 +41116,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75">
-      <c r="A11" s="245" t="s">
+      <c r="A11" s="256" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="245"/>
+      <c r="B11" s="256"/>
       <c r="C11" s="69">
         <v>0</v>
       </c>
@@ -41133,10 +41136,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75">
-      <c r="A12" s="245" t="s">
+      <c r="A12" s="256" t="s">
         <v>716</v>
       </c>
-      <c r="B12" s="245"/>
+      <c r="B12" s="256"/>
       <c r="C12" s="69">
         <v>0</v>
       </c>
@@ -41153,10 +41156,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75">
-      <c r="A13" s="245" t="s">
+      <c r="A13" s="256" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="245"/>
+      <c r="B13" s="256"/>
       <c r="C13" s="69">
         <v>0</v>
       </c>
@@ -41173,10 +41176,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75">
-      <c r="A14" s="244" t="s">
+      <c r="A14" s="255" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="245"/>
+      <c r="B14" s="256"/>
       <c r="C14" s="69">
         <v>0</v>
       </c>
@@ -41193,10 +41196,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75">
-      <c r="A15" s="244" t="s">
+      <c r="A15" s="255" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="245"/>
+      <c r="B15" s="256"/>
       <c r="C15" s="69">
         <v>0</v>
       </c>
@@ -41213,10 +41216,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A16" s="246" t="s">
+      <c r="A16" s="230" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="247"/>
+      <c r="B16" s="231"/>
       <c r="C16" s="73">
         <v>0</v>
       </c>
@@ -41234,11 +41237,11 @@
     </row>
     <row r="17" spans="1:7" ht="14.1" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="241" t="s">
+      <c r="B17" s="252" t="s">
         <v>721</v>
       </c>
-      <c r="C17" s="241"/>
-      <c r="D17" s="241"/>
+      <c r="C17" s="252"/>
+      <c r="D17" s="252"/>
       <c r="E17" s="63">
         <f>SUM(E9:E16)</f>
         <v>0</v>
@@ -41259,527 +41262,559 @@
       <c r="A19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="235" t="s">
+      <c r="B19" s="232" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="236"/>
-      <c r="D19" s="236"/>
-      <c r="E19" s="236"/>
-      <c r="F19" s="236"/>
-      <c r="G19" s="237"/>
+      <c r="C19" s="233"/>
+      <c r="D19" s="233"/>
+      <c r="E19" s="233"/>
+      <c r="F19" s="233"/>
+      <c r="G19" s="234"/>
     </row>
     <row r="20" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="A20" s="10" t="s">
         <v>582</v>
       </c>
-      <c r="B20" s="230" t="s">
+      <c r="B20" s="221" t="s">
         <v>931</v>
       </c>
-      <c r="C20" s="231"/>
-      <c r="D20" s="231"/>
-      <c r="E20" s="231"/>
-      <c r="F20" s="231"/>
-      <c r="G20" s="232"/>
+      <c r="C20" s="222"/>
+      <c r="D20" s="222"/>
+      <c r="E20" s="222"/>
+      <c r="F20" s="222"/>
+      <c r="G20" s="223"/>
     </row>
     <row r="21" spans="1:7" ht="60" customHeight="1" thickBot="1">
       <c r="A21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="230" t="s">
+      <c r="B21" s="221" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="231"/>
-      <c r="D21" s="231"/>
-      <c r="E21" s="231"/>
-      <c r="F21" s="231"/>
-      <c r="G21" s="232"/>
+      <c r="C21" s="222"/>
+      <c r="D21" s="222"/>
+      <c r="E21" s="222"/>
+      <c r="F21" s="222"/>
+      <c r="G21" s="223"/>
     </row>
     <row r="22" spans="1:7" ht="45.95" customHeight="1" thickBot="1">
       <c r="A22" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="230" t="s">
+      <c r="B22" s="221" t="s">
         <v>917</v>
       </c>
-      <c r="C22" s="231"/>
-      <c r="D22" s="231"/>
-      <c r="E22" s="231"/>
-      <c r="F22" s="231"/>
-      <c r="G22" s="232"/>
+      <c r="C22" s="222"/>
+      <c r="D22" s="222"/>
+      <c r="E22" s="222"/>
+      <c r="F22" s="222"/>
+      <c r="G22" s="223"/>
     </row>
     <row r="23" spans="1:7" ht="32.1" customHeight="1">
       <c r="A23" s="98" t="s">
         <v>899</v>
       </c>
-      <c r="B23" s="227" t="s">
+      <c r="B23" s="238" t="s">
         <v>916</v>
       </c>
-      <c r="C23" s="228"/>
-      <c r="D23" s="228"/>
-      <c r="E23" s="228"/>
-      <c r="F23" s="228"/>
-      <c r="G23" s="229"/>
+      <c r="C23" s="239"/>
+      <c r="D23" s="239"/>
+      <c r="E23" s="239"/>
+      <c r="F23" s="239"/>
+      <c r="G23" s="240"/>
     </row>
     <row r="24" spans="1:7" ht="15.75">
       <c r="A24" s="99"/>
-      <c r="B24" s="221" t="s">
+      <c r="B24" s="257" t="s">
         <v>900</v>
       </c>
-      <c r="C24" s="222"/>
-      <c r="D24" s="223" t="s">
+      <c r="C24" s="258"/>
+      <c r="D24" s="260" t="s">
         <v>901</v>
       </c>
-      <c r="E24" s="223"/>
-      <c r="F24" s="223"/>
-      <c r="G24" s="224"/>
+      <c r="E24" s="260"/>
+      <c r="F24" s="260"/>
+      <c r="G24" s="261"/>
     </row>
     <row r="25" spans="1:7" ht="15.75">
       <c r="A25" s="99"/>
-      <c r="B25" s="221" t="s">
+      <c r="B25" s="257" t="s">
         <v>902</v>
       </c>
-      <c r="C25" s="222"/>
-      <c r="D25" s="223" t="s">
+      <c r="C25" s="258"/>
+      <c r="D25" s="260" t="s">
         <v>903</v>
       </c>
-      <c r="E25" s="223"/>
-      <c r="F25" s="223"/>
-      <c r="G25" s="224"/>
+      <c r="E25" s="260"/>
+      <c r="F25" s="260"/>
+      <c r="G25" s="261"/>
     </row>
     <row r="26" spans="1:7" ht="15.75">
       <c r="A26" s="99"/>
-      <c r="B26" s="221" t="s">
+      <c r="B26" s="257" t="s">
         <v>904</v>
       </c>
-      <c r="C26" s="222"/>
-      <c r="D26" s="223" t="s">
+      <c r="C26" s="258"/>
+      <c r="D26" s="260" t="s">
         <v>905</v>
       </c>
-      <c r="E26" s="223"/>
-      <c r="F26" s="223"/>
-      <c r="G26" s="224"/>
+      <c r="E26" s="260"/>
+      <c r="F26" s="260"/>
+      <c r="G26" s="261"/>
     </row>
     <row r="27" spans="1:7" ht="15.75">
       <c r="A27" s="99"/>
-      <c r="B27" s="221" t="s">
+      <c r="B27" s="257" t="s">
         <v>906</v>
       </c>
-      <c r="C27" s="222"/>
+      <c r="C27" s="258"/>
       <c r="D27" s="225" t="s">
         <v>907</v>
       </c>
       <c r="E27" s="225"/>
       <c r="F27" s="225"/>
-      <c r="G27" s="226"/>
+      <c r="G27" s="259"/>
     </row>
     <row r="28" spans="1:7" ht="15.75">
       <c r="A28" s="99"/>
-      <c r="B28" s="221" t="s">
+      <c r="B28" s="257" t="s">
         <v>908</v>
       </c>
-      <c r="C28" s="222"/>
-      <c r="D28" s="223" t="s">
+      <c r="C28" s="258"/>
+      <c r="D28" s="260" t="s">
         <v>909</v>
       </c>
-      <c r="E28" s="223"/>
-      <c r="F28" s="223"/>
-      <c r="G28" s="224"/>
+      <c r="E28" s="260"/>
+      <c r="F28" s="260"/>
+      <c r="G28" s="261"/>
     </row>
     <row r="29" spans="1:7" ht="15.75">
       <c r="A29" s="99"/>
-      <c r="B29" s="221" t="s">
+      <c r="B29" s="257" t="s">
         <v>910</v>
       </c>
-      <c r="C29" s="222"/>
+      <c r="C29" s="258"/>
       <c r="D29" s="225" t="s">
         <v>911</v>
       </c>
       <c r="E29" s="225"/>
       <c r="F29" s="225"/>
-      <c r="G29" s="226"/>
+      <c r="G29" s="259"/>
     </row>
     <row r="30" spans="1:7" ht="15.75">
       <c r="A30" s="99"/>
-      <c r="B30" s="221" t="s">
+      <c r="B30" s="257" t="s">
         <v>914</v>
       </c>
-      <c r="C30" s="222"/>
-      <c r="D30" s="223" t="s">
+      <c r="C30" s="258"/>
+      <c r="D30" s="260" t="s">
         <v>915</v>
       </c>
-      <c r="E30" s="223"/>
-      <c r="F30" s="223"/>
-      <c r="G30" s="224"/>
+      <c r="E30" s="260"/>
+      <c r="F30" s="260"/>
+      <c r="G30" s="261"/>
     </row>
     <row r="31" spans="1:7" ht="15.75">
       <c r="A31" s="99"/>
-      <c r="B31" s="221" t="s">
+      <c r="B31" s="257" t="s">
         <v>912</v>
       </c>
-      <c r="C31" s="222"/>
+      <c r="C31" s="258"/>
       <c r="D31" s="225" t="s">
         <v>913</v>
       </c>
       <c r="E31" s="225"/>
       <c r="F31" s="225"/>
-      <c r="G31" s="226"/>
+      <c r="G31" s="259"/>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickBot="1">
       <c r="A32" s="99"/>
-      <c r="B32" s="221" t="s">
+      <c r="B32" s="257" t="s">
         <v>928</v>
       </c>
-      <c r="C32" s="222"/>
+      <c r="C32" s="258"/>
       <c r="D32" s="225" t="s">
         <v>929</v>
       </c>
       <c r="E32" s="225"/>
       <c r="F32" s="225"/>
-      <c r="G32" s="226"/>
+      <c r="G32" s="259"/>
     </row>
     <row r="33" spans="1:7" ht="15.75">
       <c r="A33" s="98" t="s">
         <v>918</v>
       </c>
-      <c r="B33" s="227" t="s">
+      <c r="B33" s="238" t="s">
         <v>919</v>
       </c>
-      <c r="C33" s="228"/>
-      <c r="D33" s="228"/>
-      <c r="E33" s="228"/>
-      <c r="F33" s="228"/>
-      <c r="G33" s="229"/>
+      <c r="C33" s="239"/>
+      <c r="D33" s="239"/>
+      <c r="E33" s="239"/>
+      <c r="F33" s="239"/>
+      <c r="G33" s="240"/>
     </row>
     <row r="34" spans="1:7" ht="15.75">
       <c r="A34" s="99"/>
-      <c r="B34" s="221" t="s">
+      <c r="B34" s="257" t="s">
         <v>920</v>
       </c>
-      <c r="C34" s="222"/>
-      <c r="D34" s="223" t="s">
+      <c r="C34" s="258"/>
+      <c r="D34" s="260" t="s">
         <v>925</v>
       </c>
-      <c r="E34" s="223"/>
-      <c r="F34" s="223"/>
-      <c r="G34" s="224"/>
+      <c r="E34" s="260"/>
+      <c r="F34" s="260"/>
+      <c r="G34" s="261"/>
     </row>
     <row r="35" spans="1:7" ht="15.75">
       <c r="A35" s="99"/>
-      <c r="B35" s="221" t="s">
+      <c r="B35" s="257" t="s">
         <v>921</v>
       </c>
-      <c r="C35" s="222"/>
-      <c r="D35" s="223" t="s">
+      <c r="C35" s="258"/>
+      <c r="D35" s="260" t="s">
         <v>926</v>
       </c>
-      <c r="E35" s="223"/>
-      <c r="F35" s="223"/>
-      <c r="G35" s="224"/>
+      <c r="E35" s="260"/>
+      <c r="F35" s="260"/>
+      <c r="G35" s="261"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" thickBot="1">
       <c r="A36" s="99"/>
-      <c r="B36" s="221" t="s">
+      <c r="B36" s="257" t="s">
         <v>922</v>
       </c>
-      <c r="C36" s="222"/>
-      <c r="D36" s="223" t="s">
+      <c r="C36" s="258"/>
+      <c r="D36" s="260" t="s">
         <v>927</v>
       </c>
-      <c r="E36" s="223"/>
-      <c r="F36" s="223"/>
-      <c r="G36" s="224"/>
+      <c r="E36" s="260"/>
+      <c r="F36" s="260"/>
+      <c r="G36" s="261"/>
     </row>
     <row r="37" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="A37" s="98" t="s">
         <v>923</v>
       </c>
-      <c r="B37" s="227" t="s">
+      <c r="B37" s="238" t="s">
         <v>924</v>
       </c>
-      <c r="C37" s="228"/>
-      <c r="D37" s="228"/>
-      <c r="E37" s="228"/>
-      <c r="F37" s="228"/>
-      <c r="G37" s="229"/>
+      <c r="C37" s="239"/>
+      <c r="D37" s="239"/>
+      <c r="E37" s="239"/>
+      <c r="F37" s="239"/>
+      <c r="G37" s="240"/>
     </row>
     <row r="38" spans="1:7" ht="29.1" customHeight="1">
-      <c r="A38" s="248" t="s">
+      <c r="A38" s="235" t="s">
         <v>517</v>
       </c>
-      <c r="B38" s="227" t="s">
+      <c r="B38" s="238" t="s">
         <v>490</v>
       </c>
-      <c r="C38" s="228"/>
-      <c r="D38" s="228"/>
-      <c r="E38" s="228"/>
-      <c r="F38" s="228"/>
-      <c r="G38" s="229"/>
+      <c r="C38" s="239"/>
+      <c r="D38" s="239"/>
+      <c r="E38" s="239"/>
+      <c r="F38" s="239"/>
+      <c r="G38" s="240"/>
     </row>
     <row r="39" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A39" s="249"/>
-      <c r="B39" s="251"/>
-      <c r="C39" s="252"/>
-      <c r="D39" s="252"/>
-      <c r="E39" s="252"/>
-      <c r="F39" s="252"/>
-      <c r="G39" s="253"/>
+      <c r="A39" s="236"/>
+      <c r="B39" s="241"/>
+      <c r="C39" s="242"/>
+      <c r="D39" s="242"/>
+      <c r="E39" s="242"/>
+      <c r="F39" s="242"/>
+      <c r="G39" s="243"/>
     </row>
     <row r="40" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A40" s="249"/>
-      <c r="B40" s="254" t="s">
+      <c r="A40" s="236"/>
+      <c r="B40" s="244" t="s">
         <v>491</v>
       </c>
-      <c r="C40" s="255"/>
-      <c r="D40" s="255"/>
-      <c r="E40" s="255"/>
-      <c r="F40" s="255"/>
-      <c r="G40" s="256"/>
+      <c r="C40" s="245"/>
+      <c r="D40" s="245"/>
+      <c r="E40" s="245"/>
+      <c r="F40" s="245"/>
+      <c r="G40" s="246"/>
     </row>
     <row r="41" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A41" s="249"/>
-      <c r="B41" s="257" t="s">
+      <c r="A41" s="236"/>
+      <c r="B41" s="224" t="s">
         <v>492</v>
       </c>
       <c r="C41" s="225"/>
       <c r="D41" s="225"/>
       <c r="E41" s="225"/>
       <c r="F41" s="225"/>
-      <c r="G41" s="258"/>
+      <c r="G41" s="226"/>
     </row>
     <row r="42" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A42" s="249"/>
-      <c r="B42" s="251"/>
-      <c r="C42" s="252"/>
-      <c r="D42" s="252"/>
-      <c r="E42" s="252"/>
-      <c r="F42" s="252"/>
-      <c r="G42" s="253"/>
+      <c r="A42" s="236"/>
+      <c r="B42" s="241"/>
+      <c r="C42" s="242"/>
+      <c r="D42" s="242"/>
+      <c r="E42" s="242"/>
+      <c r="F42" s="242"/>
+      <c r="G42" s="243"/>
     </row>
     <row r="43" spans="1:7" ht="42.95" customHeight="1">
-      <c r="A43" s="249"/>
-      <c r="B43" s="257" t="s">
+      <c r="A43" s="236"/>
+      <c r="B43" s="224" t="s">
         <v>493</v>
       </c>
       <c r="C43" s="225"/>
       <c r="D43" s="225"/>
       <c r="E43" s="225"/>
       <c r="F43" s="225"/>
-      <c r="G43" s="258"/>
+      <c r="G43" s="226"/>
     </row>
     <row r="44" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A44" s="249"/>
-      <c r="B44" s="251"/>
-      <c r="C44" s="252"/>
-      <c r="D44" s="252"/>
-      <c r="E44" s="252"/>
-      <c r="F44" s="252"/>
-      <c r="G44" s="253"/>
+      <c r="A44" s="236"/>
+      <c r="B44" s="241"/>
+      <c r="C44" s="242"/>
+      <c r="D44" s="242"/>
+      <c r="E44" s="242"/>
+      <c r="F44" s="242"/>
+      <c r="G44" s="243"/>
     </row>
     <row r="45" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A45" s="249"/>
-      <c r="B45" s="257" t="s">
+      <c r="A45" s="236"/>
+      <c r="B45" s="224" t="s">
         <v>494</v>
       </c>
       <c r="C45" s="225"/>
       <c r="D45" s="225"/>
       <c r="E45" s="225"/>
       <c r="F45" s="225"/>
-      <c r="G45" s="258"/>
+      <c r="G45" s="226"/>
     </row>
     <row r="46" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A46" s="249"/>
-      <c r="B46" s="257" t="s">
+      <c r="A46" s="236"/>
+      <c r="B46" s="224" t="s">
         <v>495</v>
       </c>
       <c r="C46" s="225"/>
       <c r="D46" s="225"/>
       <c r="E46" s="225"/>
       <c r="F46" s="225"/>
-      <c r="G46" s="258"/>
+      <c r="G46" s="226"/>
     </row>
     <row r="47" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A47" s="249"/>
-      <c r="B47" s="257" t="s">
+      <c r="A47" s="236"/>
+      <c r="B47" s="224" t="s">
         <v>496</v>
       </c>
       <c r="C47" s="225"/>
       <c r="D47" s="225"/>
       <c r="E47" s="225"/>
       <c r="F47" s="225"/>
-      <c r="G47" s="258"/>
+      <c r="G47" s="226"/>
     </row>
     <row r="48" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A48" s="249"/>
-      <c r="B48" s="257" t="s">
+      <c r="A48" s="236"/>
+      <c r="B48" s="224" t="s">
         <v>497</v>
       </c>
       <c r="C48" s="225"/>
       <c r="D48" s="225"/>
       <c r="E48" s="225"/>
       <c r="F48" s="225"/>
-      <c r="G48" s="258"/>
+      <c r="G48" s="226"/>
     </row>
     <row r="49" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A49" s="249"/>
-      <c r="B49" s="257" t="s">
+      <c r="A49" s="236"/>
+      <c r="B49" s="224" t="s">
         <v>498</v>
       </c>
       <c r="C49" s="225"/>
       <c r="D49" s="225"/>
       <c r="E49" s="225"/>
       <c r="F49" s="225"/>
-      <c r="G49" s="258"/>
+      <c r="G49" s="226"/>
     </row>
     <row r="50" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A50" s="249"/>
-      <c r="B50" s="257" t="s">
+      <c r="A50" s="236"/>
+      <c r="B50" s="224" t="s">
         <v>499</v>
       </c>
       <c r="C50" s="225"/>
       <c r="D50" s="225"/>
       <c r="E50" s="225"/>
       <c r="F50" s="225"/>
-      <c r="G50" s="258"/>
+      <c r="G50" s="226"/>
     </row>
     <row r="51" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A51" s="249"/>
-      <c r="B51" s="257" t="s">
+      <c r="A51" s="236"/>
+      <c r="B51" s="224" t="s">
         <v>500</v>
       </c>
       <c r="C51" s="225"/>
       <c r="D51" s="225"/>
       <c r="E51" s="225"/>
       <c r="F51" s="225"/>
-      <c r="G51" s="258"/>
+      <c r="G51" s="226"/>
     </row>
     <row r="52" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A52" s="250"/>
-      <c r="B52" s="259" t="s">
+      <c r="A52" s="237"/>
+      <c r="B52" s="227" t="s">
         <v>501</v>
       </c>
-      <c r="C52" s="260"/>
-      <c r="D52" s="260"/>
-      <c r="E52" s="260"/>
-      <c r="F52" s="260"/>
-      <c r="G52" s="261"/>
+      <c r="C52" s="228"/>
+      <c r="D52" s="228"/>
+      <c r="E52" s="228"/>
+      <c r="F52" s="228"/>
+      <c r="G52" s="229"/>
     </row>
     <row r="53" spans="1:7" ht="57.95" customHeight="1" thickBot="1">
       <c r="A53" s="10" t="s">
         <v>516</v>
       </c>
-      <c r="B53" s="230" t="s">
+      <c r="B53" s="221" t="s">
         <v>581</v>
       </c>
-      <c r="C53" s="231"/>
-      <c r="D53" s="231"/>
-      <c r="E53" s="231"/>
-      <c r="F53" s="231"/>
-      <c r="G53" s="232"/>
+      <c r="C53" s="222"/>
+      <c r="D53" s="222"/>
+      <c r="E53" s="222"/>
+      <c r="F53" s="222"/>
+      <c r="G53" s="223"/>
     </row>
     <row r="54" spans="1:7" ht="57.95" customHeight="1" thickBot="1">
       <c r="A54" s="10" t="s">
         <v>515</v>
       </c>
-      <c r="B54" s="230" t="s">
+      <c r="B54" s="221" t="s">
         <v>502</v>
       </c>
-      <c r="C54" s="231"/>
-      <c r="D54" s="231"/>
-      <c r="E54" s="231"/>
-      <c r="F54" s="231"/>
-      <c r="G54" s="232"/>
+      <c r="C54" s="222"/>
+      <c r="D54" s="222"/>
+      <c r="E54" s="222"/>
+      <c r="F54" s="222"/>
+      <c r="G54" s="223"/>
     </row>
     <row r="55" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A55" s="10" t="s">
         <v>514</v>
       </c>
-      <c r="B55" s="230" t="s">
+      <c r="B55" s="221" t="s">
         <v>503</v>
       </c>
-      <c r="C55" s="231"/>
-      <c r="D55" s="231"/>
-      <c r="E55" s="231"/>
-      <c r="F55" s="231"/>
-      <c r="G55" s="232"/>
+      <c r="C55" s="222"/>
+      <c r="D55" s="222"/>
+      <c r="E55" s="222"/>
+      <c r="F55" s="222"/>
+      <c r="G55" s="223"/>
     </row>
     <row r="56" spans="1:7" ht="42.95" customHeight="1" thickBot="1">
       <c r="A56" s="11" t="s">
         <v>508</v>
       </c>
-      <c r="B56" s="230" t="s">
+      <c r="B56" s="221" t="s">
         <v>504</v>
       </c>
-      <c r="C56" s="231"/>
-      <c r="D56" s="231"/>
-      <c r="E56" s="231"/>
-      <c r="F56" s="231"/>
-      <c r="G56" s="232"/>
+      <c r="C56" s="222"/>
+      <c r="D56" s="222"/>
+      <c r="E56" s="222"/>
+      <c r="F56" s="222"/>
+      <c r="G56" s="223"/>
     </row>
     <row r="57" spans="1:7" ht="29.1" customHeight="1" thickBot="1">
       <c r="A57" s="10" t="s">
         <v>513</v>
       </c>
-      <c r="B57" s="230" t="s">
+      <c r="B57" s="221" t="s">
         <v>505</v>
       </c>
-      <c r="C57" s="231"/>
-      <c r="D57" s="231"/>
-      <c r="E57" s="231"/>
-      <c r="F57" s="231"/>
-      <c r="G57" s="232"/>
+      <c r="C57" s="222"/>
+      <c r="D57" s="222"/>
+      <c r="E57" s="222"/>
+      <c r="F57" s="222"/>
+      <c r="G57" s="223"/>
     </row>
     <row r="58" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A58" s="10" t="s">
         <v>512</v>
       </c>
-      <c r="B58" s="230" t="s">
+      <c r="B58" s="221" t="s">
         <v>506</v>
       </c>
-      <c r="C58" s="231"/>
-      <c r="D58" s="231"/>
-      <c r="E58" s="231"/>
-      <c r="F58" s="231"/>
-      <c r="G58" s="232"/>
+      <c r="C58" s="222"/>
+      <c r="D58" s="222"/>
+      <c r="E58" s="222"/>
+      <c r="F58" s="222"/>
+      <c r="G58" s="223"/>
     </row>
     <row r="59" spans="1:7" ht="42.95" customHeight="1" thickBot="1">
       <c r="A59" s="11" t="s">
         <v>509</v>
       </c>
-      <c r="B59" s="230" t="s">
+      <c r="B59" s="221" t="s">
         <v>510</v>
       </c>
-      <c r="C59" s="231"/>
-      <c r="D59" s="231"/>
-      <c r="E59" s="231"/>
-      <c r="F59" s="231"/>
-      <c r="G59" s="232"/>
+      <c r="C59" s="222"/>
+      <c r="D59" s="222"/>
+      <c r="E59" s="222"/>
+      <c r="F59" s="222"/>
+      <c r="G59" s="223"/>
     </row>
     <row r="60" spans="1:7" ht="29.1" customHeight="1" thickBot="1">
       <c r="A60" s="10" t="s">
         <v>511</v>
       </c>
-      <c r="B60" s="230" t="s">
+      <c r="B60" s="221" t="s">
         <v>507</v>
       </c>
-      <c r="C60" s="231"/>
-      <c r="D60" s="231"/>
-      <c r="E60" s="231"/>
-      <c r="F60" s="231"/>
-      <c r="G60" s="232"/>
+      <c r="C60" s="222"/>
+      <c r="D60" s="222"/>
+      <c r="E60" s="222"/>
+      <c r="F60" s="222"/>
+      <c r="G60" s="223"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:G59"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B53:G53"/>
-    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B20:G20"/>
@@ -41796,49 +41831,17 @@
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="B48:G48"/>
     <mergeCell ref="B49:G49"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:G36"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:G35"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B59:G59"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -41849,8 +41852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E113" sqref="E113"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -42030,7 +42033,7 @@
       <c r="D8" s="265"/>
       <c r="E8" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Professional")*(E$10:E$247="Completed"))+SUMPRODUCT(($A$10:$A$247="Professional")*(E$10:E$247="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$247="Professional")*(E$10:E$247="Partial"))</f>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="F8" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Professional")*(F$10:F$247="Completed"))+SUMPRODUCT(($A$10:$A$247="Professional")*(F$10:F$247="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$247="Professional")*(F$10:F$247="Partial"))</f>
@@ -42062,10 +42065,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="232" t="s">
         <v>485</v>
       </c>
-      <c r="B10" s="237"/>
+      <c r="B10" s="234"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -42311,10 +42314,10 @@
       <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A23" s="235" t="s">
+      <c r="A23" s="232" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="237"/>
+      <c r="B23" s="234"/>
       <c r="C23" s="4" t="s">
         <v>63</v>
       </c>
@@ -42617,10 +42620,10 @@
       <c r="G38" s="11"/>
     </row>
     <row r="39" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A39" s="235" t="s">
+      <c r="A39" s="232" t="s">
         <v>524</v>
       </c>
-      <c r="B39" s="237"/>
+      <c r="B39" s="234"/>
       <c r="C39" s="4" t="s">
         <v>63</v>
       </c>
@@ -42733,10 +42736,10 @@
       <c r="G44" s="11"/>
     </row>
     <row r="45" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A45" s="235" t="s">
+      <c r="A45" s="232" t="s">
         <v>529</v>
       </c>
-      <c r="B45" s="237"/>
+      <c r="B45" s="234"/>
       <c r="C45" s="4" t="s">
         <v>63</v>
       </c>
@@ -42868,10 +42871,10 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A52" s="235" t="s">
+      <c r="A52" s="232" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="237"/>
+      <c r="B52" s="234"/>
       <c r="C52" s="4" t="s">
         <v>63</v>
       </c>
@@ -43041,10 +43044,10 @@
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A61" s="235" t="s">
+      <c r="A61" s="232" t="s">
         <v>111</v>
       </c>
-      <c r="B61" s="237"/>
+      <c r="B61" s="234"/>
       <c r="C61" s="4" t="s">
         <v>63</v>
       </c>
@@ -43138,10 +43141,10 @@
       <c r="G65" s="11"/>
     </row>
     <row r="66" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A66" s="235" t="s">
+      <c r="A66" s="232" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="237"/>
+      <c r="B66" s="234"/>
       <c r="C66" s="4" t="s">
         <v>63</v>
       </c>
@@ -43421,9 +43424,11 @@
       <c r="C80" s="11" t="s">
         <v>749</v>
       </c>
-      <c r="D80" s="11"/>
+      <c r="D80" s="11" t="s">
+        <v>977</v>
+      </c>
       <c r="E80" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F80" s="4" t="s">
         <v>52</v>
@@ -43431,10 +43436,10 @@
       <c r="G80" s="11"/>
     </row>
     <row r="81" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A81" s="235" t="s">
+      <c r="A81" s="232" t="s">
         <v>133</v>
       </c>
-      <c r="B81" s="237"/>
+      <c r="B81" s="234"/>
       <c r="C81" s="4" t="s">
         <v>63</v>
       </c>
@@ -43568,10 +43573,10 @@
       <c r="G87" s="11"/>
     </row>
     <row r="88" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A88" s="235" t="s">
+      <c r="A88" s="232" t="s">
         <v>558</v>
       </c>
-      <c r="B88" s="237"/>
+      <c r="B88" s="234"/>
       <c r="C88" s="4" t="s">
         <v>63</v>
       </c>
@@ -43688,10 +43693,10 @@
       <c r="G93" s="11"/>
     </row>
     <row r="94" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A94" s="235" t="s">
+      <c r="A94" s="232" t="s">
         <v>156</v>
       </c>
-      <c r="B94" s="237"/>
+      <c r="B94" s="234"/>
       <c r="C94" s="4" t="s">
         <v>63</v>
       </c>
@@ -43766,10 +43771,10 @@
       <c r="G97" s="11"/>
     </row>
     <row r="98" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A98" s="235" t="s">
+      <c r="A98" s="232" t="s">
         <v>150</v>
       </c>
-      <c r="B98" s="237"/>
+      <c r="B98" s="234"/>
       <c r="C98" s="4" t="s">
         <v>63</v>
       </c>
@@ -43844,10 +43849,10 @@
       <c r="G101" s="11"/>
     </row>
     <row r="102" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A102" s="235" t="s">
+      <c r="A102" s="232" t="s">
         <v>547</v>
       </c>
-      <c r="B102" s="237"/>
+      <c r="B102" s="234"/>
       <c r="C102" s="4" t="s">
         <v>63</v>
       </c>
@@ -43943,10 +43948,10 @@
       <c r="G106" s="11"/>
     </row>
     <row r="107" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A107" s="235" t="s">
+      <c r="A107" s="232" t="s">
         <v>140</v>
       </c>
-      <c r="B107" s="237"/>
+      <c r="B107" s="234"/>
       <c r="C107" s="4" t="s">
         <v>63</v>
       </c>
@@ -44097,10 +44102,10 @@
       <c r="G114" s="11"/>
     </row>
     <row r="115" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A115" s="235" t="s">
+      <c r="A115" s="232" t="s">
         <v>161</v>
       </c>
-      <c r="B115" s="237"/>
+      <c r="B115" s="234"/>
       <c r="C115" s="4" t="s">
         <v>453</v>
       </c>
@@ -44271,14 +44276,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A88:B88"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="C2:D9"/>
@@ -44288,6 +44285,14 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A88:B88"/>
   </mergeCells>
   <conditionalFormatting sqref="A11:A18 A107:A109 A81:A85 A115:A248 A52:A57 A40 A33:A37 A42:A43 A112 A94:A100 A61:A69 A59 A20:A29">
     <cfRule type="beginsWith" dxfId="2421" priority="1148" stopIfTrue="1" operator="beginsWith" text="Exceptional">
@@ -46736,10 +46741,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="232" t="s">
         <v>701</v>
       </c>
-      <c r="B10" s="237"/>
+      <c r="B10" s="234"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -47025,10 +47030,10 @@
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A25" s="235" t="s">
+      <c r="A25" s="232" t="s">
         <v>688</v>
       </c>
-      <c r="B25" s="237"/>
+      <c r="B25" s="234"/>
       <c r="C25" s="4" t="s">
         <v>63</v>
       </c>
@@ -47238,10 +47243,10 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A36" s="235" t="s">
+      <c r="A36" s="232" t="s">
         <v>612</v>
       </c>
-      <c r="B36" s="237"/>
+      <c r="B36" s="234"/>
       <c r="C36" s="4" t="s">
         <v>63</v>
       </c>
@@ -47660,10 +47665,10 @@
       <c r="G57" s="11"/>
     </row>
     <row r="58" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A58" s="235" t="s">
+      <c r="A58" s="232" t="s">
         <v>627</v>
       </c>
-      <c r="B58" s="237"/>
+      <c r="B58" s="234"/>
       <c r="C58" s="4" t="s">
         <v>63</v>
       </c>
@@ -47968,10 +47973,10 @@
       <c r="G73" s="11"/>
     </row>
     <row r="74" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A74" s="235" t="s">
+      <c r="A74" s="232" t="s">
         <v>651</v>
       </c>
-      <c r="B74" s="237"/>
+      <c r="B74" s="234"/>
       <c r="C74" s="4" t="s">
         <v>63</v>
       </c>
@@ -48160,10 +48165,10 @@
       <c r="G83" s="11"/>
     </row>
     <row r="84" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A84" s="235" t="s">
+      <c r="A84" s="232" t="s">
         <v>663</v>
       </c>
-      <c r="B84" s="237"/>
+      <c r="B84" s="234"/>
       <c r="C84" s="21" t="s">
         <v>456</v>
       </c>
@@ -48523,10 +48528,10 @@
       <c r="G102" s="11"/>
     </row>
     <row r="103" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A103" s="235" t="s">
+      <c r="A103" s="232" t="s">
         <v>677</v>
       </c>
-      <c r="B103" s="237"/>
+      <c r="B103" s="234"/>
       <c r="C103" s="4" t="s">
         <v>63</v>
       </c>
@@ -51700,10 +51705,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="232" t="s">
         <v>291</v>
       </c>
-      <c r="B10" s="237"/>
+      <c r="B10" s="234"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -52063,10 +52068,10 @@
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A29" s="235" t="s">
+      <c r="A29" s="232" t="s">
         <v>564</v>
       </c>
-      <c r="B29" s="237"/>
+      <c r="B29" s="234"/>
       <c r="C29" s="4" t="s">
         <v>451</v>
       </c>
@@ -52295,10 +52300,10 @@
       <c r="G40" s="11"/>
     </row>
     <row r="41" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A41" s="235" t="s">
+      <c r="A41" s="232" t="s">
         <v>334</v>
       </c>
-      <c r="B41" s="237"/>
+      <c r="B41" s="234"/>
       <c r="C41" s="4" t="s">
         <v>63</v>
       </c>
@@ -52512,10 +52517,10 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" s="7" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A52" s="235" t="s">
+      <c r="A52" s="232" t="s">
         <v>84</v>
       </c>
-      <c r="B52" s="237"/>
+      <c r="B52" s="234"/>
       <c r="C52" s="4" t="s">
         <v>63</v>
       </c>
@@ -52685,10 +52690,10 @@
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" s="7" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A61" s="235" t="s">
+      <c r="A61" s="232" t="s">
         <v>370</v>
       </c>
-      <c r="B61" s="237"/>
+      <c r="B61" s="234"/>
       <c r="C61" s="21" t="s">
         <v>452</v>
       </c>
@@ -54038,10 +54043,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="232" t="s">
         <v>810</v>
       </c>
-      <c r="B10" s="237"/>
+      <c r="B10" s="234"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -54344,10 +54349,10 @@
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A26" s="235" t="s">
+      <c r="A26" s="232" t="s">
         <v>390</v>
       </c>
-      <c r="B26" s="237"/>
+      <c r="B26" s="234"/>
       <c r="C26" s="4" t="s">
         <v>855</v>
       </c>
@@ -54614,10 +54619,10 @@
       <c r="G39" s="11"/>
     </row>
     <row r="40" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A40" s="235" t="s">
+      <c r="A40" s="232" t="s">
         <v>448</v>
       </c>
-      <c r="B40" s="237"/>
+      <c r="B40" s="234"/>
       <c r="C40" s="102" t="s">
         <v>856</v>
       </c>
@@ -54882,10 +54887,10 @@
       <c r="G53" s="11"/>
     </row>
     <row r="54" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A54" s="235" t="s">
+      <c r="A54" s="232" t="s">
         <v>412</v>
       </c>
-      <c r="B54" s="237"/>
+      <c r="B54" s="234"/>
       <c r="C54" s="4" t="s">
         <v>63</v>
       </c>
@@ -56748,10 +56753,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="232" t="s">
         <v>239</v>
       </c>
-      <c r="B10" s="237"/>
+      <c r="B10" s="234"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -56845,10 +56850,10 @@
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A15" s="235" t="s">
+      <c r="A15" s="232" t="s">
         <v>246</v>
       </c>
-      <c r="B15" s="237"/>
+      <c r="B15" s="234"/>
       <c r="C15" s="4" t="s">
         <v>874</v>
       </c>
@@ -56961,10 +56966,10 @@
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A21" s="235" t="s">
+      <c r="A21" s="232" t="s">
         <v>878</v>
       </c>
-      <c r="B21" s="237"/>
+      <c r="B21" s="234"/>
       <c r="C21" s="4" t="s">
         <v>63</v>
       </c>
@@ -57096,10 +57101,10 @@
       <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A28" s="235" t="s">
+      <c r="A28" s="232" t="s">
         <v>254</v>
       </c>
-      <c r="B28" s="237"/>
+      <c r="B28" s="234"/>
       <c r="C28" s="4" t="s">
         <v>875</v>
       </c>
@@ -57250,10 +57255,10 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A36" s="235" t="s">
+      <c r="A36" s="232" t="s">
         <v>891</v>
       </c>
-      <c r="B36" s="237"/>
+      <c r="B36" s="234"/>
       <c r="C36" s="4" t="s">
         <v>454</v>
       </c>
@@ -57385,10 +57390,10 @@
       <c r="G42" s="11"/>
     </row>
     <row r="43" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A43" s="235" t="s">
+      <c r="A43" s="232" t="s">
         <v>275</v>
       </c>
-      <c r="B43" s="237"/>
+      <c r="B43" s="234"/>
       <c r="C43" s="4" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Updated rubric, moved the XInputInterface.dll to the root so controllers function properly on the installed version.
</commit_message>
<xml_diff>
--- a/GameDocuments/gam352_papercut_rubric.xlsx
+++ b/GameDocuments/gam352_papercut_rubric.xlsx
@@ -41852,8 +41852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>

</xml_diff>

<commit_message>
Fixed the splash screen skip to work with all required buttons.
</commit_message>
<xml_diff>
--- a/GameDocuments/gam352_papercut_rubric.xlsx
+++ b/GameDocuments/gam352_papercut_rubric.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Game Data" sheetId="1" r:id="rId1"/>
@@ -5780,6 +5780,90 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -5813,18 +5897,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -5882,99 +5954,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="4" borderId="16" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="4" borderId="18" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="26" fillId="3" borderId="21" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5985,6 +5964,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="26" fillId="3" borderId="26" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6053,55 +6038,37 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="4" borderId="16" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="4" borderId="18" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6113,28 +6080,28 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6161,19 +6128,52 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -39834,7 +39834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -39854,54 +39854,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="178"/>
+      <c r="B1" s="145"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="146"/>
       <c r="E1" s="103"/>
-      <c r="F1" s="176" t="s">
+      <c r="F1" s="144" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="177"/>
-      <c r="H1" s="177"/>
-      <c r="I1" s="177"/>
-      <c r="J1" s="178"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
+      <c r="J1" s="146"/>
       <c r="K1" s="104"/>
       <c r="L1" s="104"/>
       <c r="M1" s="105"/>
     </row>
     <row r="2" spans="1:13" ht="14.1" customHeight="1">
-      <c r="A2" s="182" t="s">
+      <c r="A2" s="147" t="s">
         <v>951</v>
       </c>
-      <c r="B2" s="183"/>
-      <c r="C2" s="183"/>
-      <c r="D2" s="184"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="149"/>
       <c r="E2" s="103"/>
-      <c r="F2" s="182" t="s">
+      <c r="F2" s="147" t="s">
         <v>954</v>
       </c>
-      <c r="G2" s="183"/>
-      <c r="H2" s="183"/>
-      <c r="I2" s="183"/>
-      <c r="J2" s="184"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="149"/>
       <c r="K2" s="104"/>
       <c r="L2" s="104"/>
       <c r="M2" s="105"/>
     </row>
     <row r="3" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A3" s="185"/>
-      <c r="B3" s="186"/>
-      <c r="C3" s="186"/>
-      <c r="D3" s="187"/>
+      <c r="A3" s="150"/>
+      <c r="B3" s="151"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="103"/>
-      <c r="F3" s="185"/>
-      <c r="G3" s="186"/>
-      <c r="H3" s="186"/>
-      <c r="I3" s="186"/>
-      <c r="J3" s="187"/>
+      <c r="F3" s="150"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="151"/>
+      <c r="J3" s="152"/>
       <c r="K3" s="104"/>
       <c r="L3" s="104"/>
       <c r="M3" s="105"/>
@@ -39922,41 +39922,41 @@
       <c r="M4" s="105"/>
     </row>
     <row r="5" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="144" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="177"/>
-      <c r="C5" s="177"/>
-      <c r="D5" s="178"/>
+      <c r="B5" s="145"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="146"/>
       <c r="E5" s="103"/>
-      <c r="F5" s="176" t="s">
+      <c r="F5" s="144" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="177"/>
-      <c r="H5" s="177"/>
-      <c r="I5" s="177"/>
-      <c r="J5" s="178"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="145"/>
+      <c r="I5" s="145"/>
+      <c r="J5" s="146"/>
       <c r="K5" s="104"/>
       <c r="L5" s="107"/>
       <c r="M5" s="105"/>
     </row>
     <row r="6" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="156" t="s">
         <v>952</v>
       </c>
-      <c r="B6" s="174"/>
-      <c r="C6" s="174"/>
-      <c r="D6" s="175"/>
+      <c r="B6" s="157"/>
+      <c r="C6" s="157"/>
+      <c r="D6" s="158"/>
       <c r="E6" s="103"/>
-      <c r="F6" s="173" t="s">
+      <c r="F6" s="156" t="s">
         <v>955</v>
       </c>
-      <c r="G6" s="174"/>
-      <c r="H6" s="174"/>
-      <c r="I6" s="174"/>
-      <c r="J6" s="175"/>
+      <c r="G6" s="157"/>
+      <c r="H6" s="157"/>
+      <c r="I6" s="157"/>
+      <c r="J6" s="158"/>
       <c r="K6" s="104"/>
-      <c r="L6" s="170" t="s">
+      <c r="L6" s="153" t="s">
         <v>24</v>
       </c>
       <c r="M6" s="105"/>
@@ -39967,51 +39967,51 @@
       <c r="C7" s="108"/>
       <c r="D7" s="109"/>
       <c r="E7" s="103"/>
-      <c r="F7" s="173" t="s">
+      <c r="F7" s="156" t="s">
         <v>979</v>
       </c>
-      <c r="G7" s="174"/>
-      <c r="H7" s="174"/>
-      <c r="I7" s="174"/>
-      <c r="J7" s="175"/>
+      <c r="G7" s="157"/>
+      <c r="H7" s="157"/>
+      <c r="I7" s="157"/>
+      <c r="J7" s="158"/>
       <c r="K7" s="104"/>
-      <c r="L7" s="171"/>
+      <c r="L7" s="154"/>
       <c r="M7" s="105"/>
     </row>
     <row r="8" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="144" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="177"/>
-      <c r="C8" s="177"/>
-      <c r="D8" s="178"/>
+      <c r="B8" s="145"/>
+      <c r="C8" s="145"/>
+      <c r="D8" s="146"/>
       <c r="E8" s="103"/>
-      <c r="F8" s="173" t="s">
+      <c r="F8" s="156" t="s">
         <v>978</v>
       </c>
-      <c r="G8" s="174"/>
-      <c r="H8" s="174"/>
-      <c r="I8" s="174"/>
-      <c r="J8" s="175"/>
+      <c r="G8" s="157"/>
+      <c r="H8" s="157"/>
+      <c r="I8" s="157"/>
+      <c r="J8" s="158"/>
       <c r="K8" s="104"/>
-      <c r="L8" s="171"/>
+      <c r="L8" s="154"/>
       <c r="M8" s="105"/>
     </row>
     <row r="9" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="156" t="s">
         <v>953</v>
       </c>
-      <c r="B9" s="174"/>
-      <c r="C9" s="174"/>
-      <c r="D9" s="175"/>
+      <c r="B9" s="157"/>
+      <c r="C9" s="157"/>
+      <c r="D9" s="158"/>
       <c r="E9" s="103"/>
-      <c r="F9" s="173"/>
-      <c r="G9" s="174"/>
-      <c r="H9" s="174"/>
-      <c r="I9" s="174"/>
-      <c r="J9" s="175"/>
+      <c r="F9" s="156"/>
+      <c r="G9" s="157"/>
+      <c r="H9" s="157"/>
+      <c r="I9" s="157"/>
+      <c r="J9" s="158"/>
       <c r="K9" s="104"/>
-      <c r="L9" s="172"/>
+      <c r="L9" s="155"/>
       <c r="M9" s="105"/>
     </row>
     <row r="10" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40030,18 +40030,18 @@
       <c r="M10" s="105"/>
     </row>
     <row r="11" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="144" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="177"/>
-      <c r="C11" s="177"/>
-      <c r="D11" s="178"/>
+      <c r="B11" s="145"/>
+      <c r="C11" s="145"/>
+      <c r="D11" s="146"/>
       <c r="E11" s="103"/>
-      <c r="F11" s="176" t="s">
+      <c r="F11" s="144" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="177"/>
-      <c r="H11" s="178"/>
+      <c r="G11" s="145"/>
+      <c r="H11" s="146"/>
       <c r="I11" s="134" t="s">
         <v>7</v>
       </c>
@@ -40081,7 +40081,7 @@
         <v>-0.12</v>
       </c>
       <c r="K12" s="104"/>
-      <c r="L12" s="170" t="s">
+      <c r="L12" s="153" t="s">
         <v>8</v>
       </c>
       <c r="M12" s="105"/>
@@ -40114,7 +40114,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="120"/>
-      <c r="L13" s="171"/>
+      <c r="L13" s="154"/>
       <c r="M13" s="121"/>
     </row>
     <row r="14" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40144,7 +40144,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="124"/>
-      <c r="L14" s="172"/>
+      <c r="L14" s="155"/>
       <c r="M14" s="125"/>
     </row>
     <row r="15" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40212,11 +40212,11 @@
         <v>939</v>
       </c>
       <c r="E17" s="104"/>
-      <c r="F17" s="176" t="s">
+      <c r="F17" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="177"/>
-      <c r="H17" s="178"/>
+      <c r="G17" s="145"/>
+      <c r="H17" s="146"/>
       <c r="I17" s="111"/>
       <c r="J17" s="135">
         <v>0.75</v>
@@ -40242,17 +40242,17 @@
       <c r="F18" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="179" t="s">
+      <c r="G18" s="159" t="s">
         <v>956</v>
       </c>
-      <c r="H18" s="180"/>
-      <c r="I18" s="181"/>
+      <c r="H18" s="160"/>
+      <c r="I18" s="161"/>
       <c r="J18" s="137">
         <f>IF(LEFT(G18,6)="Entire",0,IF(LEFT(G18,6)="Custom",-0.05,-0.1))</f>
         <v>-0.1</v>
       </c>
       <c r="K18" s="128"/>
-      <c r="L18" s="170" t="s">
+      <c r="L18" s="153" t="s">
         <v>18</v>
       </c>
       <c r="M18" s="105"/>
@@ -40274,17 +40274,17 @@
       <c r="F19" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="153" t="s">
+      <c r="G19" s="162" t="s">
         <v>957</v>
       </c>
-      <c r="H19" s="154"/>
-      <c r="I19" s="155"/>
+      <c r="H19" s="163"/>
+      <c r="I19" s="164"/>
       <c r="J19" s="139">
         <f>IF(G19="2D Graphics and 2D Gameplay",IF(J11=0.15,-0.05,0),IF(G19="3D Graphics but 2D Gameplay",IF(J11=0.15,-0.02,-0.3),IF(J11=0.15,0,-0.3)))</f>
         <v>0</v>
       </c>
       <c r="K19" s="104"/>
-      <c r="L19" s="172"/>
+      <c r="L19" s="155"/>
       <c r="M19" s="105"/>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40336,22 +40336,22 @@
       <c r="C22" s="118"/>
       <c r="D22" s="119"/>
       <c r="E22" s="104"/>
-      <c r="F22" s="168" t="s">
+      <c r="F22" s="186" t="s">
         <v>713</v>
       </c>
-      <c r="G22" s="166" t="s">
+      <c r="G22" s="184" t="s">
         <v>714</v>
       </c>
-      <c r="H22" s="165"/>
+      <c r="H22" s="183"/>
       <c r="I22" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="163">
+      <c r="J22" s="181">
         <f>J20+J15</f>
         <v>0.68</v>
       </c>
       <c r="K22" s="104"/>
-      <c r="L22" s="144" t="s">
+      <c r="L22" s="165" t="s">
         <v>725</v>
       </c>
       <c r="M22" s="105"/>
@@ -40362,15 +40362,15 @@
       <c r="C23" s="118"/>
       <c r="D23" s="119"/>
       <c r="E23" s="104"/>
-      <c r="F23" s="169"/>
-      <c r="G23" s="167"/>
-      <c r="H23" s="165"/>
+      <c r="F23" s="187"/>
+      <c r="G23" s="185"/>
+      <c r="H23" s="183"/>
       <c r="I23" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="164"/>
+      <c r="J23" s="182"/>
       <c r="K23" s="104"/>
-      <c r="L23" s="145"/>
+      <c r="L23" s="166"/>
       <c r="M23" s="105"/>
     </row>
     <row r="24" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40394,13 +40394,13 @@
       <c r="C25" s="118"/>
       <c r="D25" s="119"/>
       <c r="E25" s="104"/>
-      <c r="F25" s="157" t="s">
+      <c r="F25" s="175" t="s">
         <v>932</v>
       </c>
-      <c r="G25" s="158"/>
-      <c r="H25" s="158"/>
-      <c r="I25" s="158"/>
-      <c r="J25" s="159"/>
+      <c r="G25" s="176"/>
+      <c r="H25" s="176"/>
+      <c r="I25" s="176"/>
+      <c r="J25" s="177"/>
       <c r="K25" s="104"/>
       <c r="L25" s="104"/>
       <c r="M25" s="105"/>
@@ -40411,11 +40411,11 @@
       <c r="C26" s="118"/>
       <c r="D26" s="119"/>
       <c r="E26" s="103"/>
-      <c r="F26" s="160"/>
-      <c r="G26" s="161"/>
-      <c r="H26" s="161"/>
-      <c r="I26" s="161"/>
-      <c r="J26" s="162"/>
+      <c r="F26" s="178"/>
+      <c r="G26" s="179"/>
+      <c r="H26" s="179"/>
+      <c r="I26" s="179"/>
+      <c r="J26" s="180"/>
       <c r="K26" s="104"/>
       <c r="L26" s="104"/>
       <c r="M26" s="105"/>
@@ -40441,13 +40441,13 @@
       <c r="C28" s="118"/>
       <c r="D28" s="119"/>
       <c r="E28" s="103"/>
-      <c r="F28" s="156" t="s">
+      <c r="F28" s="174" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="156"/>
-      <c r="H28" s="156"/>
-      <c r="I28" s="156"/>
-      <c r="J28" s="156"/>
+      <c r="G28" s="174"/>
+      <c r="H28" s="174"/>
+      <c r="I28" s="174"/>
+      <c r="J28" s="174"/>
       <c r="K28" s="104"/>
       <c r="L28" s="104"/>
       <c r="M28" s="105"/>
@@ -40458,13 +40458,13 @@
       <c r="C29" s="118"/>
       <c r="D29" s="119"/>
       <c r="E29" s="103"/>
-      <c r="F29" s="150" t="s">
+      <c r="F29" s="171" t="s">
         <v>933</v>
       </c>
-      <c r="G29" s="151"/>
-      <c r="H29" s="151"/>
-      <c r="I29" s="151"/>
-      <c r="J29" s="152"/>
+      <c r="G29" s="172"/>
+      <c r="H29" s="172"/>
+      <c r="I29" s="172"/>
+      <c r="J29" s="173"/>
       <c r="K29" s="104"/>
       <c r="L29" s="104"/>
       <c r="M29" s="105"/>
@@ -40475,30 +40475,30 @@
       <c r="C30" s="118"/>
       <c r="D30" s="119"/>
       <c r="E30" s="103"/>
-      <c r="F30" s="150"/>
-      <c r="G30" s="151"/>
-      <c r="H30" s="151"/>
-      <c r="I30" s="151"/>
-      <c r="J30" s="152"/>
+      <c r="F30" s="171"/>
+      <c r="G30" s="172"/>
+      <c r="H30" s="172"/>
+      <c r="I30" s="172"/>
+      <c r="J30" s="173"/>
       <c r="K30" s="104"/>
       <c r="L30" s="104"/>
       <c r="M30" s="105"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A31" s="146" t="s">
+      <c r="A31" s="167" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="147"/>
-      <c r="C31" s="148" t="s">
+      <c r="B31" s="168"/>
+      <c r="C31" s="169" t="s">
         <v>950</v>
       </c>
-      <c r="D31" s="149"/>
+      <c r="D31" s="170"/>
       <c r="E31" s="104"/>
-      <c r="F31" s="153"/>
-      <c r="G31" s="154"/>
-      <c r="H31" s="154"/>
-      <c r="I31" s="154"/>
-      <c r="J31" s="155"/>
+      <c r="F31" s="162"/>
+      <c r="G31" s="163"/>
+      <c r="H31" s="163"/>
+      <c r="I31" s="163"/>
+      <c r="J31" s="164"/>
       <c r="K31" s="104"/>
       <c r="L31" s="104"/>
       <c r="M31" s="105"/>
@@ -40521,12 +40521,16 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0"/>
   <mergeCells count="31">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="A2:D3"/>
-    <mergeCell ref="F2:J3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F29:J31"/>
+    <mergeCell ref="F28:J28"/>
+    <mergeCell ref="F25:J26"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F22:F23"/>
     <mergeCell ref="L12:L14"/>
     <mergeCell ref="L18:L19"/>
     <mergeCell ref="A6:D6"/>
@@ -40542,16 +40546,12 @@
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="G18:I18"/>
     <mergeCell ref="G19:I19"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F29:J31"/>
-    <mergeCell ref="F28:J28"/>
-    <mergeCell ref="F25:J26"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A2:D3"/>
+    <mergeCell ref="F2:J3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:J5"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6:D6">
@@ -40619,57 +40619,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="194" t="s">
         <v>556</v>
       </c>
-      <c r="B1" s="200"/>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
-      <c r="E1" s="200"/>
-      <c r="F1" s="200"/>
-      <c r="G1" s="200"/>
-      <c r="H1" s="200"/>
-      <c r="J1" s="210" t="s">
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
+      <c r="F1" s="195"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="195"/>
+      <c r="J1" s="205" t="s">
         <v>482</v>
       </c>
-      <c r="K1" s="211"/>
-      <c r="L1" s="212"/>
+      <c r="K1" s="206"/>
+      <c r="L1" s="207"/>
       <c r="M1" s="79"/>
       <c r="N1" s="24" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A2" s="199"/>
-      <c r="B2" s="200"/>
-      <c r="C2" s="200"/>
-      <c r="D2" s="200"/>
-      <c r="E2" s="200"/>
-      <c r="F2" s="200"/>
-      <c r="G2" s="200"/>
-      <c r="H2" s="200"/>
-      <c r="J2" s="213" t="s">
+      <c r="A2" s="194"/>
+      <c r="B2" s="195"/>
+      <c r="C2" s="195"/>
+      <c r="D2" s="195"/>
+      <c r="E2" s="195"/>
+      <c r="F2" s="195"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="195"/>
+      <c r="J2" s="208" t="s">
         <v>706</v>
       </c>
-      <c r="K2" s="214"/>
-      <c r="L2" s="215"/>
+      <c r="K2" s="209"/>
+      <c r="L2" s="210"/>
       <c r="M2" s="23"/>
       <c r="N2" s="26" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A3" s="199"/>
-      <c r="B3" s="200"/>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200"/>
-      <c r="E3" s="200"/>
-      <c r="F3" s="200"/>
-      <c r="G3" s="200"/>
-      <c r="H3" s="200"/>
-      <c r="J3" s="213"/>
-      <c r="K3" s="214"/>
-      <c r="L3" s="215"/>
+      <c r="A3" s="194"/>
+      <c r="B3" s="195"/>
+      <c r="C3" s="195"/>
+      <c r="D3" s="195"/>
+      <c r="E3" s="195"/>
+      <c r="F3" s="195"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="195"/>
+      <c r="J3" s="208"/>
+      <c r="K3" s="209"/>
+      <c r="L3" s="210"/>
       <c r="M3" s="23"/>
       <c r="N3" s="26" t="s">
         <v>431</v>
@@ -40679,14 +40679,14 @@
       <c r="A4" s="2"/>
       <c r="B4" s="5"/>
       <c r="C4" s="8"/>
-      <c r="D4" s="192"/>
-      <c r="E4" s="192"/>
+      <c r="D4" s="193"/>
+      <c r="E4" s="193"/>
       <c r="F4" s="43"/>
-      <c r="G4" s="192"/>
-      <c r="H4" s="192"/>
-      <c r="J4" s="213"/>
-      <c r="K4" s="214"/>
-      <c r="L4" s="215"/>
+      <c r="G4" s="193"/>
+      <c r="H4" s="193"/>
+      <c r="J4" s="208"/>
+      <c r="K4" s="209"/>
+      <c r="L4" s="210"/>
       <c r="M4" s="34"/>
       <c r="N4" s="26" t="s">
         <v>432</v>
@@ -40694,24 +40694,24 @@
       <c r="O4" s="81"/>
     </row>
     <row r="5" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A5" s="201" t="s">
+      <c r="A5" s="196" t="s">
         <v>425</v>
       </c>
-      <c r="B5" s="202"/>
+      <c r="B5" s="197"/>
       <c r="C5" s="8"/>
-      <c r="D5" s="205" t="s">
+      <c r="D5" s="200" t="s">
         <v>717</v>
       </c>
-      <c r="E5" s="206"/>
-      <c r="F5" s="207"/>
-      <c r="G5" s="208">
+      <c r="E5" s="201"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="203">
         <f>Submission!$E$17</f>
         <v>0</v>
       </c>
-      <c r="H5" s="209"/>
-      <c r="J5" s="213"/>
-      <c r="K5" s="214"/>
-      <c r="L5" s="215"/>
+      <c r="H5" s="204"/>
+      <c r="J5" s="208"/>
+      <c r="K5" s="209"/>
+      <c r="L5" s="210"/>
       <c r="M5" s="34"/>
       <c r="N5" s="26" t="s">
         <v>433</v>
@@ -40719,21 +40719,21 @@
       <c r="O5" s="81"/>
     </row>
     <row r="6" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A6" s="203"/>
-      <c r="B6" s="204"/>
+      <c r="A6" s="198"/>
+      <c r="B6" s="199"/>
       <c r="C6" s="43"/>
-      <c r="D6" s="192" t="s">
+      <c r="D6" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="192"/>
+      <c r="E6" s="193"/>
       <c r="F6" s="43"/>
-      <c r="G6" s="192" t="s">
+      <c r="G6" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="192"/>
-      <c r="J6" s="213"/>
-      <c r="K6" s="214"/>
-      <c r="L6" s="215"/>
+      <c r="H6" s="193"/>
+      <c r="J6" s="208"/>
+      <c r="K6" s="209"/>
+      <c r="L6" s="210"/>
       <c r="M6" s="34"/>
       <c r="N6" s="26" t="s">
         <v>434</v>
@@ -40741,24 +40741,24 @@
       <c r="O6" s="81"/>
     </row>
     <row r="7" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A7" s="195">
+      <c r="A7" s="188">
         <f>'Game Data'!$J$22</f>
         <v>0.68</v>
       </c>
-      <c r="B7" s="196"/>
+      <c r="B7" s="189"/>
       <c r="C7" s="43"/>
-      <c r="D7" s="193" t="s">
+      <c r="D7" s="216" t="s">
         <v>724</v>
       </c>
-      <c r="E7" s="194"/>
+      <c r="E7" s="217"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="193" t="s">
+      <c r="G7" s="216" t="s">
         <v>724</v>
       </c>
-      <c r="H7" s="194"/>
-      <c r="J7" s="213"/>
-      <c r="K7" s="214"/>
-      <c r="L7" s="215"/>
+      <c r="H7" s="217"/>
+      <c r="J7" s="208"/>
+      <c r="K7" s="209"/>
+      <c r="L7" s="210"/>
       <c r="M7" s="33"/>
       <c r="N7" s="26" t="s">
         <v>435</v>
@@ -40766,23 +40766,23 @@
       <c r="O7" s="81"/>
     </row>
     <row r="8" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A8" s="197"/>
-      <c r="B8" s="198"/>
+      <c r="A8" s="190"/>
+      <c r="B8" s="191"/>
       <c r="C8" s="97"/>
-      <c r="D8" s="219">
+      <c r="D8" s="214">
         <f>E17+E26+E35+E44+E53</f>
         <v>0.30125000000000002</v>
       </c>
-      <c r="E8" s="220"/>
+      <c r="E8" s="215"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="219">
+      <c r="G8" s="214">
         <f>H17+H26+H35+H44+H53</f>
         <v>4.9999999999999975E-3</v>
       </c>
-      <c r="H8" s="220"/>
-      <c r="J8" s="216"/>
-      <c r="K8" s="217"/>
-      <c r="L8" s="218"/>
+      <c r="H8" s="215"/>
+      <c r="J8" s="211"/>
+      <c r="K8" s="212"/>
+      <c r="L8" s="213"/>
       <c r="M8" s="80"/>
       <c r="N8" s="25" t="s">
         <v>436</v>
@@ -40793,15 +40793,15 @@
       <c r="A9" s="2"/>
       <c r="B9" s="5"/>
       <c r="C9" s="43"/>
-      <c r="D9" s="192" t="s">
+      <c r="D9" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="192"/>
+      <c r="E9" s="193"/>
       <c r="F9" s="43"/>
-      <c r="G9" s="192" t="s">
+      <c r="G9" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="192"/>
+      <c r="H9" s="193"/>
       <c r="J9" s="82"/>
       <c r="K9" s="82"/>
       <c r="L9" s="82"/>
@@ -40828,11 +40828,11 @@
       <c r="H10" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="191" t="s">
+      <c r="J10" s="192" t="s">
         <v>707</v>
       </c>
-      <c r="K10" s="191"/>
-      <c r="L10" s="191"/>
+      <c r="K10" s="192"/>
+      <c r="L10" s="192"/>
       <c r="O10" s="84"/>
     </row>
     <row r="11" spans="1:15" ht="14.1" customHeight="1">
@@ -40861,11 +40861,11 @@
         <f t="shared" ref="H11:H16" si="1">$B11*G11</f>
         <v>0</v>
       </c>
-      <c r="J11" s="190" t="s">
+      <c r="J11" s="220" t="s">
         <v>792</v>
       </c>
-      <c r="K11" s="190"/>
-      <c r="L11" s="190"/>
+      <c r="K11" s="220"/>
+      <c r="L11" s="220"/>
       <c r="M11" s="82"/>
       <c r="O11" s="84"/>
     </row>
@@ -40895,9 +40895,9 @@
         <f t="shared" si="1"/>
         <v>-0.04</v>
       </c>
-      <c r="J12" s="190"/>
-      <c r="K12" s="190"/>
-      <c r="L12" s="190"/>
+      <c r="J12" s="220"/>
+      <c r="K12" s="220"/>
+      <c r="L12" s="220"/>
       <c r="M12" s="82"/>
       <c r="O12" s="84"/>
     </row>
@@ -40927,9 +40927,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="190"/>
-      <c r="K13" s="190"/>
-      <c r="L13" s="190"/>
+      <c r="J13" s="220"/>
+      <c r="K13" s="220"/>
+      <c r="L13" s="220"/>
       <c r="M13" s="82"/>
       <c r="O13" s="84"/>
     </row>
@@ -40995,11 +40995,11 @@
         <f t="shared" si="1"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J15" s="188">
+      <c r="J15" s="218">
         <f>MAX(0,MIN(1,IF($J17 &lt;= 0.95, ROUND($J17,2), FLOOR((0.95+($J17-0.95)/5),0.01))))</f>
         <v>0.85</v>
       </c>
-      <c r="L15" s="188">
+      <c r="L15" s="218">
         <f>MAX(0,MIN(1,IF($L17 &lt;= 0.95, ROUND($L17,2), FLOOR((0.95+($L17-0.95)/5),0.01))))</f>
         <v>0.69</v>
       </c>
@@ -41032,8 +41032,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J16" s="189"/>
-      <c r="L16" s="189"/>
+      <c r="J16" s="219"/>
+      <c r="L16" s="219"/>
       <c r="M16" s="82"/>
       <c r="O16" s="84"/>
     </row>
@@ -41070,15 +41070,15 @@
       <c r="A18" s="2"/>
       <c r="B18" s="5"/>
       <c r="C18" s="43"/>
-      <c r="D18" s="192" t="s">
+      <c r="D18" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="192"/>
+      <c r="E18" s="193"/>
       <c r="F18" s="43"/>
-      <c r="G18" s="192" t="s">
+      <c r="G18" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="192"/>
+      <c r="H18" s="193"/>
       <c r="J18" s="88"/>
       <c r="M18" s="78"/>
     </row>
@@ -41103,11 +41103,11 @@
       <c r="H19" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="191" t="s">
+      <c r="J19" s="192" t="s">
         <v>715</v>
       </c>
-      <c r="K19" s="191"/>
-      <c r="L19" s="191"/>
+      <c r="K19" s="192"/>
+      <c r="L19" s="192"/>
       <c r="M19" s="83"/>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1">
@@ -41136,11 +41136,11 @@
         <f t="shared" ref="H20:H25" si="3">$B20*G20</f>
         <v>0</v>
       </c>
-      <c r="J20" s="190" t="s">
+      <c r="J20" s="220" t="s">
         <v>722</v>
       </c>
-      <c r="K20" s="190"/>
-      <c r="L20" s="190"/>
+      <c r="K20" s="220"/>
+      <c r="L20" s="220"/>
       <c r="M20" s="84"/>
     </row>
     <row r="21" spans="1:13" ht="14.1" customHeight="1">
@@ -41169,9 +41169,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J21" s="190"/>
-      <c r="K21" s="190"/>
-      <c r="L21" s="190"/>
+      <c r="J21" s="220"/>
+      <c r="K21" s="220"/>
+      <c r="L21" s="220"/>
       <c r="M21" s="84"/>
     </row>
     <row r="22" spans="1:13" ht="14.1" customHeight="1">
@@ -41200,9 +41200,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J22" s="190"/>
-      <c r="K22" s="190"/>
-      <c r="L22" s="190"/>
+      <c r="J22" s="220"/>
+      <c r="K22" s="220"/>
+      <c r="L22" s="220"/>
       <c r="M22" s="84"/>
     </row>
     <row r="23" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -41266,11 +41266,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J24" s="188">
+      <c r="J24" s="218">
         <f>MAX(0,MIN(1,IF($J26 &lt;= 0.95, ROUND($J26,2), FLOOR((0.95+($J26-0.95)/5),0.01))))</f>
         <v>0.86</v>
       </c>
-      <c r="L24" s="188">
+      <c r="L24" s="218">
         <f>MAX(0,MIN(1,IF($L26 &lt;= 0.95, ROUND($L26,2), FLOOR((0.95+($L26-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -41302,8 +41302,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J25" s="189"/>
-      <c r="L25" s="189"/>
+      <c r="J25" s="219"/>
+      <c r="L25" s="219"/>
       <c r="M25" s="84"/>
     </row>
     <row r="26" spans="1:13" ht="14.1" customHeight="1">
@@ -41339,15 +41339,15 @@
       <c r="A27" s="2"/>
       <c r="B27" s="5"/>
       <c r="C27" s="43"/>
-      <c r="D27" s="192" t="s">
+      <c r="D27" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="192"/>
+      <c r="E27" s="193"/>
       <c r="F27" s="43"/>
-      <c r="G27" s="192" t="s">
+      <c r="G27" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H27" s="192"/>
+      <c r="H27" s="193"/>
     </row>
     <row r="28" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
       <c r="A28" s="1" t="s">
@@ -41370,11 +41370,11 @@
       <c r="H28" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J28" s="191" t="s">
+      <c r="J28" s="192" t="s">
         <v>709</v>
       </c>
-      <c r="K28" s="191"/>
-      <c r="L28" s="191"/>
+      <c r="K28" s="192"/>
+      <c r="L28" s="192"/>
     </row>
     <row r="29" spans="1:13" ht="14.1" customHeight="1">
       <c r="A29" s="57" t="str">
@@ -41402,11 +41402,11 @@
         <f t="shared" ref="H29:H34" si="5">$B29*G29</f>
         <v>0</v>
       </c>
-      <c r="J29" s="190" t="s">
+      <c r="J29" s="220" t="s">
         <v>710</v>
       </c>
-      <c r="K29" s="190"/>
-      <c r="L29" s="190"/>
+      <c r="K29" s="220"/>
+      <c r="L29" s="220"/>
     </row>
     <row r="30" spans="1:13" ht="14.1" customHeight="1">
       <c r="A30" s="58" t="str">
@@ -41434,9 +41434,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J30" s="190"/>
-      <c r="K30" s="190"/>
-      <c r="L30" s="190"/>
+      <c r="J30" s="220"/>
+      <c r="K30" s="220"/>
+      <c r="L30" s="220"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1">
       <c r="A31" s="58" t="str">
@@ -41464,9 +41464,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J31" s="190"/>
-      <c r="K31" s="190"/>
-      <c r="L31" s="190"/>
+      <c r="J31" s="220"/>
+      <c r="K31" s="220"/>
+      <c r="L31" s="220"/>
     </row>
     <row r="32" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
       <c r="A32" s="58" t="str">
@@ -41528,11 +41528,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J33" s="188">
+      <c r="J33" s="218">
         <f>MAX(0,MIN(1,IF($J35 &lt;= 0.95, ROUND($J35,2), FLOOR((0.95+($J35-0.95)/5),0.01))))</f>
         <v>0.88</v>
       </c>
-      <c r="L33" s="188">
+      <c r="L33" s="218">
         <f>MAX(0,MIN(1,IF($L35 &lt;= 0.95, ROUND($L35,2), FLOOR((0.95+($L35-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -41563,8 +41563,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J34" s="189"/>
-      <c r="L34" s="189"/>
+      <c r="J34" s="219"/>
+      <c r="L34" s="219"/>
     </row>
     <row r="35" spans="1:12" ht="14.1" customHeight="1">
       <c r="A35" s="2"/>
@@ -41598,15 +41598,15 @@
       <c r="A36" s="2"/>
       <c r="B36" s="5"/>
       <c r="C36" s="43"/>
-      <c r="D36" s="192" t="s">
+      <c r="D36" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="192"/>
+      <c r="E36" s="193"/>
       <c r="F36" s="43"/>
-      <c r="G36" s="192" t="s">
+      <c r="G36" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H36" s="192"/>
+      <c r="H36" s="193"/>
     </row>
     <row r="37" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A37" s="1" t="s">
@@ -41629,11 +41629,11 @@
       <c r="H37" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J37" s="191" t="s">
+      <c r="J37" s="192" t="s">
         <v>711</v>
       </c>
-      <c r="K37" s="191"/>
-      <c r="L37" s="191"/>
+      <c r="K37" s="192"/>
+      <c r="L37" s="192"/>
     </row>
     <row r="38" spans="1:12" ht="14.1" customHeight="1">
       <c r="A38" s="57" t="str">
@@ -41661,11 +41661,11 @@
         <f t="shared" ref="H38:H43" si="7">$B38*G38</f>
         <v>0</v>
       </c>
-      <c r="J38" s="190" t="s">
+      <c r="J38" s="220" t="s">
         <v>712</v>
       </c>
-      <c r="K38" s="190"/>
-      <c r="L38" s="190"/>
+      <c r="K38" s="220"/>
+      <c r="L38" s="220"/>
     </row>
     <row r="39" spans="1:12" ht="14.1" customHeight="1">
       <c r="A39" s="58" t="str">
@@ -41693,9 +41693,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J39" s="190"/>
-      <c r="K39" s="190"/>
-      <c r="L39" s="190"/>
+      <c r="J39" s="220"/>
+      <c r="K39" s="220"/>
+      <c r="L39" s="220"/>
     </row>
     <row r="40" spans="1:12" ht="14.1" customHeight="1">
       <c r="A40" s="58" t="str">
@@ -41723,9 +41723,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J40" s="190"/>
-      <c r="K40" s="190"/>
-      <c r="L40" s="190"/>
+      <c r="J40" s="220"/>
+      <c r="K40" s="220"/>
+      <c r="L40" s="220"/>
     </row>
     <row r="41" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A41" s="58" t="str">
@@ -41787,11 +41787,11 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J42" s="188">
+      <c r="J42" s="218">
         <f>MAX(0,MIN(1,IF($J44 &lt;= 0.95, ROUND($J44,2), FLOOR((0.95+($J44-0.95)/5),0.01))))</f>
         <v>0.73</v>
       </c>
-      <c r="L42" s="188">
+      <c r="L42" s="218">
         <f>MAX(0,MIN(1,IF($L44 &lt;= 0.95, ROUND($L44,2), FLOOR((0.95+($L44-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -41822,8 +41822,8 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J43" s="189"/>
-      <c r="L43" s="189"/>
+      <c r="J43" s="219"/>
+      <c r="L43" s="219"/>
     </row>
     <row r="44" spans="1:12" ht="14.1" customHeight="1">
       <c r="A44" s="2"/>
@@ -41857,15 +41857,15 @@
       <c r="A45" s="2"/>
       <c r="B45" s="5"/>
       <c r="C45" s="43"/>
-      <c r="D45" s="192" t="s">
+      <c r="D45" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="192"/>
+      <c r="E45" s="193"/>
       <c r="F45" s="43"/>
-      <c r="G45" s="192" t="s">
+      <c r="G45" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="192"/>
+      <c r="H45" s="193"/>
     </row>
     <row r="46" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A46" s="1" t="s">
@@ -42073,6 +42073,34 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="J29:L31"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="L33:L34"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="J38:L40"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="J11:L13"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J20:L22"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G36:H36"/>
     <mergeCell ref="A7:B8"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="D6:E6"/>
@@ -42086,34 +42114,6 @@
     <mergeCell ref="J2:L8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="J11:L13"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J20:L22"/>
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="L42:L43"/>
-    <mergeCell ref="J29:L31"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="L33:L34"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="J38:L40"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -42141,59 +42141,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="235" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="233"/>
-      <c r="C1" s="233"/>
-      <c r="D1" s="233"/>
-      <c r="E1" s="233"/>
-      <c r="F1" s="233"/>
-      <c r="G1" s="234"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="237"/>
     </row>
     <row r="2" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A2" s="221" t="s">
+      <c r="A2" s="230" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="222"/>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
-      <c r="G2" s="223"/>
+      <c r="B2" s="231"/>
+      <c r="C2" s="231"/>
+      <c r="D2" s="231"/>
+      <c r="E2" s="231"/>
+      <c r="F2" s="231"/>
+      <c r="G2" s="232"/>
     </row>
     <row r="3" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A3" s="238" t="s">
+      <c r="A3" s="227" t="s">
         <v>930</v>
       </c>
-      <c r="B3" s="239"/>
-      <c r="C3" s="239"/>
-      <c r="D3" s="239"/>
-      <c r="E3" s="239"/>
-      <c r="F3" s="239"/>
-      <c r="G3" s="240"/>
+      <c r="B3" s="228"/>
+      <c r="C3" s="228"/>
+      <c r="D3" s="228"/>
+      <c r="E3" s="228"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="229"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A4" s="221" t="s">
+      <c r="A4" s="230" t="s">
         <v>438</v>
       </c>
-      <c r="B4" s="222"/>
-      <c r="C4" s="222"/>
-      <c r="D4" s="222"/>
-      <c r="E4" s="222"/>
-      <c r="F4" s="222"/>
-      <c r="G4" s="223"/>
+      <c r="B4" s="231"/>
+      <c r="C4" s="231"/>
+      <c r="D4" s="231"/>
+      <c r="E4" s="231"/>
+      <c r="F4" s="231"/>
+      <c r="G4" s="232"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A5" s="249" t="s">
+      <c r="A5" s="238" t="s">
         <v>580</v>
       </c>
-      <c r="B5" s="250"/>
-      <c r="C5" s="250"/>
-      <c r="D5" s="250"/>
-      <c r="E5" s="250"/>
-      <c r="F5" s="250"/>
-      <c r="G5" s="251"/>
+      <c r="B5" s="239"/>
+      <c r="C5" s="239"/>
+      <c r="D5" s="239"/>
+      <c r="E5" s="239"/>
+      <c r="F5" s="239"/>
+      <c r="G5" s="240"/>
     </row>
     <row r="6" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
       <c r="A6" s="2"/>
@@ -42226,10 +42226,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75">
-      <c r="A8" s="247" t="s">
+      <c r="A8" s="233" t="s">
         <v>718</v>
       </c>
-      <c r="B8" s="248"/>
+      <c r="B8" s="234"/>
       <c r="C8" s="65">
         <v>0</v>
       </c>
@@ -42246,10 +42246,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75">
-      <c r="A9" s="253" t="s">
+      <c r="A9" s="242" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="254"/>
+      <c r="B9" s="243"/>
       <c r="C9" s="92">
         <v>0</v>
       </c>
@@ -42266,10 +42266,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75">
-      <c r="A10" s="255" t="s">
+      <c r="A10" s="244" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="256"/>
+      <c r="B10" s="245"/>
       <c r="C10" s="69">
         <v>0</v>
       </c>
@@ -42286,10 +42286,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75">
-      <c r="A11" s="256" t="s">
+      <c r="A11" s="245" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="256"/>
+      <c r="B11" s="245"/>
       <c r="C11" s="69">
         <v>0</v>
       </c>
@@ -42306,10 +42306,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75">
-      <c r="A12" s="256" t="s">
+      <c r="A12" s="245" t="s">
         <v>716</v>
       </c>
-      <c r="B12" s="256"/>
+      <c r="B12" s="245"/>
       <c r="C12" s="69">
         <v>0</v>
       </c>
@@ -42326,10 +42326,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75">
-      <c r="A13" s="256" t="s">
+      <c r="A13" s="245" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="256"/>
+      <c r="B13" s="245"/>
       <c r="C13" s="69">
         <v>0</v>
       </c>
@@ -42346,10 +42346,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75">
-      <c r="A14" s="255" t="s">
+      <c r="A14" s="244" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="256"/>
+      <c r="B14" s="245"/>
       <c r="C14" s="69">
         <v>0</v>
       </c>
@@ -42366,10 +42366,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75">
-      <c r="A15" s="255" t="s">
+      <c r="A15" s="244" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="256"/>
+      <c r="B15" s="245"/>
       <c r="C15" s="69">
         <v>0</v>
       </c>
@@ -42386,10 +42386,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A16" s="230" t="s">
+      <c r="A16" s="246" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="231"/>
+      <c r="B16" s="247"/>
       <c r="C16" s="73">
         <v>0</v>
       </c>
@@ -42407,11 +42407,11 @@
     </row>
     <row r="17" spans="1:7" ht="14.1" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="252" t="s">
+      <c r="B17" s="241" t="s">
         <v>721</v>
       </c>
-      <c r="C17" s="252"/>
-      <c r="D17" s="252"/>
+      <c r="C17" s="241"/>
+      <c r="D17" s="241"/>
       <c r="E17" s="63">
         <f>SUM(E9:E16)</f>
         <v>0</v>
@@ -42432,527 +42432,559 @@
       <c r="A19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="232" t="s">
+      <c r="B19" s="235" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="233"/>
-      <c r="D19" s="233"/>
-      <c r="E19" s="233"/>
-      <c r="F19" s="233"/>
-      <c r="G19" s="234"/>
+      <c r="C19" s="236"/>
+      <c r="D19" s="236"/>
+      <c r="E19" s="236"/>
+      <c r="F19" s="236"/>
+      <c r="G19" s="237"/>
     </row>
     <row r="20" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="A20" s="10" t="s">
         <v>582</v>
       </c>
-      <c r="B20" s="221" t="s">
+      <c r="B20" s="230" t="s">
         <v>931</v>
       </c>
-      <c r="C20" s="222"/>
-      <c r="D20" s="222"/>
-      <c r="E20" s="222"/>
-      <c r="F20" s="222"/>
-      <c r="G20" s="223"/>
+      <c r="C20" s="231"/>
+      <c r="D20" s="231"/>
+      <c r="E20" s="231"/>
+      <c r="F20" s="231"/>
+      <c r="G20" s="232"/>
     </row>
     <row r="21" spans="1:7" ht="60" customHeight="1" thickBot="1">
       <c r="A21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="221" t="s">
+      <c r="B21" s="230" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="222"/>
-      <c r="D21" s="222"/>
-      <c r="E21" s="222"/>
-      <c r="F21" s="222"/>
-      <c r="G21" s="223"/>
+      <c r="C21" s="231"/>
+      <c r="D21" s="231"/>
+      <c r="E21" s="231"/>
+      <c r="F21" s="231"/>
+      <c r="G21" s="232"/>
     </row>
     <row r="22" spans="1:7" ht="45.95" customHeight="1" thickBot="1">
       <c r="A22" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="221" t="s">
+      <c r="B22" s="230" t="s">
         <v>917</v>
       </c>
-      <c r="C22" s="222"/>
-      <c r="D22" s="222"/>
-      <c r="E22" s="222"/>
-      <c r="F22" s="222"/>
-      <c r="G22" s="223"/>
+      <c r="C22" s="231"/>
+      <c r="D22" s="231"/>
+      <c r="E22" s="231"/>
+      <c r="F22" s="231"/>
+      <c r="G22" s="232"/>
     </row>
     <row r="23" spans="1:7" ht="32.1" customHeight="1">
       <c r="A23" s="98" t="s">
         <v>899</v>
       </c>
-      <c r="B23" s="238" t="s">
+      <c r="B23" s="227" t="s">
         <v>916</v>
       </c>
-      <c r="C23" s="239"/>
-      <c r="D23" s="239"/>
-      <c r="E23" s="239"/>
-      <c r="F23" s="239"/>
-      <c r="G23" s="240"/>
+      <c r="C23" s="228"/>
+      <c r="D23" s="228"/>
+      <c r="E23" s="228"/>
+      <c r="F23" s="228"/>
+      <c r="G23" s="229"/>
     </row>
     <row r="24" spans="1:7" ht="15.75">
       <c r="A24" s="99"/>
-      <c r="B24" s="257" t="s">
+      <c r="B24" s="221" t="s">
         <v>900</v>
       </c>
-      <c r="C24" s="258"/>
-      <c r="D24" s="260" t="s">
+      <c r="C24" s="222"/>
+      <c r="D24" s="223" t="s">
         <v>901</v>
       </c>
-      <c r="E24" s="260"/>
-      <c r="F24" s="260"/>
-      <c r="G24" s="261"/>
+      <c r="E24" s="223"/>
+      <c r="F24" s="223"/>
+      <c r="G24" s="224"/>
     </row>
     <row r="25" spans="1:7" ht="15.75">
       <c r="A25" s="99"/>
-      <c r="B25" s="257" t="s">
+      <c r="B25" s="221" t="s">
         <v>902</v>
       </c>
-      <c r="C25" s="258"/>
-      <c r="D25" s="260" t="s">
+      <c r="C25" s="222"/>
+      <c r="D25" s="223" t="s">
         <v>903</v>
       </c>
-      <c r="E25" s="260"/>
-      <c r="F25" s="260"/>
-      <c r="G25" s="261"/>
+      <c r="E25" s="223"/>
+      <c r="F25" s="223"/>
+      <c r="G25" s="224"/>
     </row>
     <row r="26" spans="1:7" ht="15.75">
       <c r="A26" s="99"/>
-      <c r="B26" s="257" t="s">
+      <c r="B26" s="221" t="s">
         <v>904</v>
       </c>
-      <c r="C26" s="258"/>
-      <c r="D26" s="260" t="s">
+      <c r="C26" s="222"/>
+      <c r="D26" s="223" t="s">
         <v>905</v>
       </c>
-      <c r="E26" s="260"/>
-      <c r="F26" s="260"/>
-      <c r="G26" s="261"/>
+      <c r="E26" s="223"/>
+      <c r="F26" s="223"/>
+      <c r="G26" s="224"/>
     </row>
     <row r="27" spans="1:7" ht="15.75">
       <c r="A27" s="99"/>
-      <c r="B27" s="257" t="s">
+      <c r="B27" s="221" t="s">
         <v>906</v>
       </c>
-      <c r="C27" s="258"/>
+      <c r="C27" s="222"/>
       <c r="D27" s="225" t="s">
         <v>907</v>
       </c>
       <c r="E27" s="225"/>
       <c r="F27" s="225"/>
-      <c r="G27" s="259"/>
+      <c r="G27" s="226"/>
     </row>
     <row r="28" spans="1:7" ht="15.75">
       <c r="A28" s="99"/>
-      <c r="B28" s="257" t="s">
+      <c r="B28" s="221" t="s">
         <v>908</v>
       </c>
-      <c r="C28" s="258"/>
-      <c r="D28" s="260" t="s">
+      <c r="C28" s="222"/>
+      <c r="D28" s="223" t="s">
         <v>909</v>
       </c>
-      <c r="E28" s="260"/>
-      <c r="F28" s="260"/>
-      <c r="G28" s="261"/>
+      <c r="E28" s="223"/>
+      <c r="F28" s="223"/>
+      <c r="G28" s="224"/>
     </row>
     <row r="29" spans="1:7" ht="15.75">
       <c r="A29" s="99"/>
-      <c r="B29" s="257" t="s">
+      <c r="B29" s="221" t="s">
         <v>910</v>
       </c>
-      <c r="C29" s="258"/>
+      <c r="C29" s="222"/>
       <c r="D29" s="225" t="s">
         <v>911</v>
       </c>
       <c r="E29" s="225"/>
       <c r="F29" s="225"/>
-      <c r="G29" s="259"/>
+      <c r="G29" s="226"/>
     </row>
     <row r="30" spans="1:7" ht="15.75">
       <c r="A30" s="99"/>
-      <c r="B30" s="257" t="s">
+      <c r="B30" s="221" t="s">
         <v>914</v>
       </c>
-      <c r="C30" s="258"/>
-      <c r="D30" s="260" t="s">
+      <c r="C30" s="222"/>
+      <c r="D30" s="223" t="s">
         <v>915</v>
       </c>
-      <c r="E30" s="260"/>
-      <c r="F30" s="260"/>
-      <c r="G30" s="261"/>
+      <c r="E30" s="223"/>
+      <c r="F30" s="223"/>
+      <c r="G30" s="224"/>
     </row>
     <row r="31" spans="1:7" ht="15.75">
       <c r="A31" s="99"/>
-      <c r="B31" s="257" t="s">
+      <c r="B31" s="221" t="s">
         <v>912</v>
       </c>
-      <c r="C31" s="258"/>
+      <c r="C31" s="222"/>
       <c r="D31" s="225" t="s">
         <v>913</v>
       </c>
       <c r="E31" s="225"/>
       <c r="F31" s="225"/>
-      <c r="G31" s="259"/>
+      <c r="G31" s="226"/>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickBot="1">
       <c r="A32" s="99"/>
-      <c r="B32" s="257" t="s">
+      <c r="B32" s="221" t="s">
         <v>928</v>
       </c>
-      <c r="C32" s="258"/>
+      <c r="C32" s="222"/>
       <c r="D32" s="225" t="s">
         <v>929</v>
       </c>
       <c r="E32" s="225"/>
       <c r="F32" s="225"/>
-      <c r="G32" s="259"/>
+      <c r="G32" s="226"/>
     </row>
     <row r="33" spans="1:7" ht="15.75">
       <c r="A33" s="98" t="s">
         <v>918</v>
       </c>
-      <c r="B33" s="238" t="s">
+      <c r="B33" s="227" t="s">
         <v>919</v>
       </c>
-      <c r="C33" s="239"/>
-      <c r="D33" s="239"/>
-      <c r="E33" s="239"/>
-      <c r="F33" s="239"/>
-      <c r="G33" s="240"/>
+      <c r="C33" s="228"/>
+      <c r="D33" s="228"/>
+      <c r="E33" s="228"/>
+      <c r="F33" s="228"/>
+      <c r="G33" s="229"/>
     </row>
     <row r="34" spans="1:7" ht="15.75">
       <c r="A34" s="99"/>
-      <c r="B34" s="257" t="s">
+      <c r="B34" s="221" t="s">
         <v>920</v>
       </c>
-      <c r="C34" s="258"/>
-      <c r="D34" s="260" t="s">
+      <c r="C34" s="222"/>
+      <c r="D34" s="223" t="s">
         <v>925</v>
       </c>
-      <c r="E34" s="260"/>
-      <c r="F34" s="260"/>
-      <c r="G34" s="261"/>
+      <c r="E34" s="223"/>
+      <c r="F34" s="223"/>
+      <c r="G34" s="224"/>
     </row>
     <row r="35" spans="1:7" ht="15.75">
       <c r="A35" s="99"/>
-      <c r="B35" s="257" t="s">
+      <c r="B35" s="221" t="s">
         <v>921</v>
       </c>
-      <c r="C35" s="258"/>
-      <c r="D35" s="260" t="s">
+      <c r="C35" s="222"/>
+      <c r="D35" s="223" t="s">
         <v>926</v>
       </c>
-      <c r="E35" s="260"/>
-      <c r="F35" s="260"/>
-      <c r="G35" s="261"/>
+      <c r="E35" s="223"/>
+      <c r="F35" s="223"/>
+      <c r="G35" s="224"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" thickBot="1">
       <c r="A36" s="99"/>
-      <c r="B36" s="257" t="s">
+      <c r="B36" s="221" t="s">
         <v>922</v>
       </c>
-      <c r="C36" s="258"/>
-      <c r="D36" s="260" t="s">
+      <c r="C36" s="222"/>
+      <c r="D36" s="223" t="s">
         <v>927</v>
       </c>
-      <c r="E36" s="260"/>
-      <c r="F36" s="260"/>
-      <c r="G36" s="261"/>
+      <c r="E36" s="223"/>
+      <c r="F36" s="223"/>
+      <c r="G36" s="224"/>
     </row>
     <row r="37" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="A37" s="98" t="s">
         <v>923</v>
       </c>
-      <c r="B37" s="238" t="s">
+      <c r="B37" s="227" t="s">
         <v>924</v>
       </c>
-      <c r="C37" s="239"/>
-      <c r="D37" s="239"/>
-      <c r="E37" s="239"/>
-      <c r="F37" s="239"/>
-      <c r="G37" s="240"/>
+      <c r="C37" s="228"/>
+      <c r="D37" s="228"/>
+      <c r="E37" s="228"/>
+      <c r="F37" s="228"/>
+      <c r="G37" s="229"/>
     </row>
     <row r="38" spans="1:7" ht="29.1" customHeight="1">
-      <c r="A38" s="235" t="s">
+      <c r="A38" s="248" t="s">
         <v>517</v>
       </c>
-      <c r="B38" s="238" t="s">
+      <c r="B38" s="227" t="s">
         <v>490</v>
       </c>
-      <c r="C38" s="239"/>
-      <c r="D38" s="239"/>
-      <c r="E38" s="239"/>
-      <c r="F38" s="239"/>
-      <c r="G38" s="240"/>
+      <c r="C38" s="228"/>
+      <c r="D38" s="228"/>
+      <c r="E38" s="228"/>
+      <c r="F38" s="228"/>
+      <c r="G38" s="229"/>
     </row>
     <row r="39" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A39" s="236"/>
-      <c r="B39" s="241"/>
-      <c r="C39" s="242"/>
-      <c r="D39" s="242"/>
-      <c r="E39" s="242"/>
-      <c r="F39" s="242"/>
-      <c r="G39" s="243"/>
+      <c r="A39" s="249"/>
+      <c r="B39" s="251"/>
+      <c r="C39" s="252"/>
+      <c r="D39" s="252"/>
+      <c r="E39" s="252"/>
+      <c r="F39" s="252"/>
+      <c r="G39" s="253"/>
     </row>
     <row r="40" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A40" s="236"/>
-      <c r="B40" s="244" t="s">
+      <c r="A40" s="249"/>
+      <c r="B40" s="254" t="s">
         <v>491</v>
       </c>
-      <c r="C40" s="245"/>
-      <c r="D40" s="245"/>
-      <c r="E40" s="245"/>
-      <c r="F40" s="245"/>
-      <c r="G40" s="246"/>
+      <c r="C40" s="255"/>
+      <c r="D40" s="255"/>
+      <c r="E40" s="255"/>
+      <c r="F40" s="255"/>
+      <c r="G40" s="256"/>
     </row>
     <row r="41" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A41" s="236"/>
-      <c r="B41" s="224" t="s">
+      <c r="A41" s="249"/>
+      <c r="B41" s="257" t="s">
         <v>492</v>
       </c>
       <c r="C41" s="225"/>
       <c r="D41" s="225"/>
       <c r="E41" s="225"/>
       <c r="F41" s="225"/>
-      <c r="G41" s="226"/>
+      <c r="G41" s="258"/>
     </row>
     <row r="42" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A42" s="236"/>
-      <c r="B42" s="241"/>
-      <c r="C42" s="242"/>
-      <c r="D42" s="242"/>
-      <c r="E42" s="242"/>
-      <c r="F42" s="242"/>
-      <c r="G42" s="243"/>
+      <c r="A42" s="249"/>
+      <c r="B42" s="251"/>
+      <c r="C42" s="252"/>
+      <c r="D42" s="252"/>
+      <c r="E42" s="252"/>
+      <c r="F42" s="252"/>
+      <c r="G42" s="253"/>
     </row>
     <row r="43" spans="1:7" ht="42.95" customHeight="1">
-      <c r="A43" s="236"/>
-      <c r="B43" s="224" t="s">
+      <c r="A43" s="249"/>
+      <c r="B43" s="257" t="s">
         <v>493</v>
       </c>
       <c r="C43" s="225"/>
       <c r="D43" s="225"/>
       <c r="E43" s="225"/>
       <c r="F43" s="225"/>
-      <c r="G43" s="226"/>
+      <c r="G43" s="258"/>
     </row>
     <row r="44" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A44" s="236"/>
-      <c r="B44" s="241"/>
-      <c r="C44" s="242"/>
-      <c r="D44" s="242"/>
-      <c r="E44" s="242"/>
-      <c r="F44" s="242"/>
-      <c r="G44" s="243"/>
+      <c r="A44" s="249"/>
+      <c r="B44" s="251"/>
+      <c r="C44" s="252"/>
+      <c r="D44" s="252"/>
+      <c r="E44" s="252"/>
+      <c r="F44" s="252"/>
+      <c r="G44" s="253"/>
     </row>
     <row r="45" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A45" s="236"/>
-      <c r="B45" s="224" t="s">
+      <c r="A45" s="249"/>
+      <c r="B45" s="257" t="s">
         <v>494</v>
       </c>
       <c r="C45" s="225"/>
       <c r="D45" s="225"/>
       <c r="E45" s="225"/>
       <c r="F45" s="225"/>
-      <c r="G45" s="226"/>
+      <c r="G45" s="258"/>
     </row>
     <row r="46" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A46" s="236"/>
-      <c r="B46" s="224" t="s">
+      <c r="A46" s="249"/>
+      <c r="B46" s="257" t="s">
         <v>495</v>
       </c>
       <c r="C46" s="225"/>
       <c r="D46" s="225"/>
       <c r="E46" s="225"/>
       <c r="F46" s="225"/>
-      <c r="G46" s="226"/>
+      <c r="G46" s="258"/>
     </row>
     <row r="47" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A47" s="236"/>
-      <c r="B47" s="224" t="s">
+      <c r="A47" s="249"/>
+      <c r="B47" s="257" t="s">
         <v>496</v>
       </c>
       <c r="C47" s="225"/>
       <c r="D47" s="225"/>
       <c r="E47" s="225"/>
       <c r="F47" s="225"/>
-      <c r="G47" s="226"/>
+      <c r="G47" s="258"/>
     </row>
     <row r="48" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A48" s="236"/>
-      <c r="B48" s="224" t="s">
+      <c r="A48" s="249"/>
+      <c r="B48" s="257" t="s">
         <v>497</v>
       </c>
       <c r="C48" s="225"/>
       <c r="D48" s="225"/>
       <c r="E48" s="225"/>
       <c r="F48" s="225"/>
-      <c r="G48" s="226"/>
+      <c r="G48" s="258"/>
     </row>
     <row r="49" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A49" s="236"/>
-      <c r="B49" s="224" t="s">
+      <c r="A49" s="249"/>
+      <c r="B49" s="257" t="s">
         <v>498</v>
       </c>
       <c r="C49" s="225"/>
       <c r="D49" s="225"/>
       <c r="E49" s="225"/>
       <c r="F49" s="225"/>
-      <c r="G49" s="226"/>
+      <c r="G49" s="258"/>
     </row>
     <row r="50" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A50" s="236"/>
-      <c r="B50" s="224" t="s">
+      <c r="A50" s="249"/>
+      <c r="B50" s="257" t="s">
         <v>499</v>
       </c>
       <c r="C50" s="225"/>
       <c r="D50" s="225"/>
       <c r="E50" s="225"/>
       <c r="F50" s="225"/>
-      <c r="G50" s="226"/>
+      <c r="G50" s="258"/>
     </row>
     <row r="51" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A51" s="236"/>
-      <c r="B51" s="224" t="s">
+      <c r="A51" s="249"/>
+      <c r="B51" s="257" t="s">
         <v>500</v>
       </c>
       <c r="C51" s="225"/>
       <c r="D51" s="225"/>
       <c r="E51" s="225"/>
       <c r="F51" s="225"/>
-      <c r="G51" s="226"/>
+      <c r="G51" s="258"/>
     </row>
     <row r="52" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A52" s="237"/>
-      <c r="B52" s="227" t="s">
+      <c r="A52" s="250"/>
+      <c r="B52" s="259" t="s">
         <v>501</v>
       </c>
-      <c r="C52" s="228"/>
-      <c r="D52" s="228"/>
-      <c r="E52" s="228"/>
-      <c r="F52" s="228"/>
-      <c r="G52" s="229"/>
+      <c r="C52" s="260"/>
+      <c r="D52" s="260"/>
+      <c r="E52" s="260"/>
+      <c r="F52" s="260"/>
+      <c r="G52" s="261"/>
     </row>
     <row r="53" spans="1:7" ht="57.95" customHeight="1" thickBot="1">
       <c r="A53" s="10" t="s">
         <v>516</v>
       </c>
-      <c r="B53" s="221" t="s">
+      <c r="B53" s="230" t="s">
         <v>581</v>
       </c>
-      <c r="C53" s="222"/>
-      <c r="D53" s="222"/>
-      <c r="E53" s="222"/>
-      <c r="F53" s="222"/>
-      <c r="G53" s="223"/>
+      <c r="C53" s="231"/>
+      <c r="D53" s="231"/>
+      <c r="E53" s="231"/>
+      <c r="F53" s="231"/>
+      <c r="G53" s="232"/>
     </row>
     <row r="54" spans="1:7" ht="57.95" customHeight="1" thickBot="1">
       <c r="A54" s="10" t="s">
         <v>515</v>
       </c>
-      <c r="B54" s="221" t="s">
+      <c r="B54" s="230" t="s">
         <v>502</v>
       </c>
-      <c r="C54" s="222"/>
-      <c r="D54" s="222"/>
-      <c r="E54" s="222"/>
-      <c r="F54" s="222"/>
-      <c r="G54" s="223"/>
+      <c r="C54" s="231"/>
+      <c r="D54" s="231"/>
+      <c r="E54" s="231"/>
+      <c r="F54" s="231"/>
+      <c r="G54" s="232"/>
     </row>
     <row r="55" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A55" s="10" t="s">
         <v>514</v>
       </c>
-      <c r="B55" s="221" t="s">
+      <c r="B55" s="230" t="s">
         <v>503</v>
       </c>
-      <c r="C55" s="222"/>
-      <c r="D55" s="222"/>
-      <c r="E55" s="222"/>
-      <c r="F55" s="222"/>
-      <c r="G55" s="223"/>
+      <c r="C55" s="231"/>
+      <c r="D55" s="231"/>
+      <c r="E55" s="231"/>
+      <c r="F55" s="231"/>
+      <c r="G55" s="232"/>
     </row>
     <row r="56" spans="1:7" ht="42.95" customHeight="1" thickBot="1">
       <c r="A56" s="11" t="s">
         <v>508</v>
       </c>
-      <c r="B56" s="221" t="s">
+      <c r="B56" s="230" t="s">
         <v>504</v>
       </c>
-      <c r="C56" s="222"/>
-      <c r="D56" s="222"/>
-      <c r="E56" s="222"/>
-      <c r="F56" s="222"/>
-      <c r="G56" s="223"/>
+      <c r="C56" s="231"/>
+      <c r="D56" s="231"/>
+      <c r="E56" s="231"/>
+      <c r="F56" s="231"/>
+      <c r="G56" s="232"/>
     </row>
     <row r="57" spans="1:7" ht="29.1" customHeight="1" thickBot="1">
       <c r="A57" s="10" t="s">
         <v>513</v>
       </c>
-      <c r="B57" s="221" t="s">
+      <c r="B57" s="230" t="s">
         <v>505</v>
       </c>
-      <c r="C57" s="222"/>
-      <c r="D57" s="222"/>
-      <c r="E57" s="222"/>
-      <c r="F57" s="222"/>
-      <c r="G57" s="223"/>
+      <c r="C57" s="231"/>
+      <c r="D57" s="231"/>
+      <c r="E57" s="231"/>
+      <c r="F57" s="231"/>
+      <c r="G57" s="232"/>
     </row>
     <row r="58" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A58" s="10" t="s">
         <v>512</v>
       </c>
-      <c r="B58" s="221" t="s">
+      <c r="B58" s="230" t="s">
         <v>506</v>
       </c>
-      <c r="C58" s="222"/>
-      <c r="D58" s="222"/>
-      <c r="E58" s="222"/>
-      <c r="F58" s="222"/>
-      <c r="G58" s="223"/>
+      <c r="C58" s="231"/>
+      <c r="D58" s="231"/>
+      <c r="E58" s="231"/>
+      <c r="F58" s="231"/>
+      <c r="G58" s="232"/>
     </row>
     <row r="59" spans="1:7" ht="42.95" customHeight="1" thickBot="1">
       <c r="A59" s="11" t="s">
         <v>509</v>
       </c>
-      <c r="B59" s="221" t="s">
+      <c r="B59" s="230" t="s">
         <v>510</v>
       </c>
-      <c r="C59" s="222"/>
-      <c r="D59" s="222"/>
-      <c r="E59" s="222"/>
-      <c r="F59" s="222"/>
-      <c r="G59" s="223"/>
+      <c r="C59" s="231"/>
+      <c r="D59" s="231"/>
+      <c r="E59" s="231"/>
+      <c r="F59" s="231"/>
+      <c r="G59" s="232"/>
     </row>
     <row r="60" spans="1:7" ht="29.1" customHeight="1" thickBot="1">
       <c r="A60" s="10" t="s">
         <v>511</v>
       </c>
-      <c r="B60" s="221" t="s">
+      <c r="B60" s="230" t="s">
         <v>507</v>
       </c>
-      <c r="C60" s="222"/>
-      <c r="D60" s="222"/>
-      <c r="E60" s="222"/>
-      <c r="F60" s="222"/>
-      <c r="G60" s="223"/>
+      <c r="C60" s="231"/>
+      <c r="D60" s="231"/>
+      <c r="E60" s="231"/>
+      <c r="F60" s="231"/>
+      <c r="G60" s="232"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="A38:A52"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="B37:G37"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="D29:G29"/>
@@ -42969,49 +43001,17 @@
     <mergeCell ref="D34:G34"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="D35:G35"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="A38:A52"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="B43:G43"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B53:G53"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:G28"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -43022,7 +43022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
@@ -43235,10 +43235,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>485</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -43255,7 +43255,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="77.25" thickBot="1">
+    <row r="11" spans="1:7" ht="64.5" thickBot="1">
       <c r="A11" s="15" t="s">
         <v>66</v>
       </c>
@@ -43402,7 +43402,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="102.75" thickBot="1">
+    <row r="18" spans="1:7" ht="90" thickBot="1">
       <c r="A18" s="16" t="s">
         <v>68</v>
       </c>
@@ -43465,7 +43465,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="77.25" thickBot="1">
+    <row r="21" spans="1:7" ht="64.5" thickBot="1">
       <c r="A21" s="18" t="s">
         <v>80</v>
       </c>
@@ -43508,10 +43508,10 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A23" s="232" t="s">
+      <c r="A23" s="235" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="234"/>
+      <c r="B23" s="237"/>
       <c r="C23" s="4" t="s">
         <v>63</v>
       </c>
@@ -43844,10 +43844,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A39" s="232" t="s">
+      <c r="A39" s="235" t="s">
         <v>524</v>
       </c>
-      <c r="B39" s="234"/>
+      <c r="B39" s="237"/>
       <c r="C39" s="4" t="s">
         <v>63</v>
       </c>
@@ -43970,10 +43970,10 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A45" s="232" t="s">
+      <c r="A45" s="235" t="s">
         <v>529</v>
       </c>
-      <c r="B45" s="234"/>
+      <c r="B45" s="237"/>
       <c r="C45" s="4" t="s">
         <v>63</v>
       </c>
@@ -44119,10 +44119,10 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A52" s="232" t="s">
+      <c r="A52" s="235" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="234"/>
+      <c r="B52" s="237"/>
       <c r="C52" s="4" t="s">
         <v>63</v>
       </c>
@@ -44310,10 +44310,10 @@
       </c>
     </row>
     <row r="61" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A61" s="232" t="s">
+      <c r="A61" s="235" t="s">
         <v>111</v>
       </c>
-      <c r="B61" s="234"/>
+      <c r="B61" s="237"/>
       <c r="C61" s="4" t="s">
         <v>63</v>
       </c>
@@ -44415,10 +44415,10 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A66" s="232" t="s">
+      <c r="A66" s="235" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="234"/>
+      <c r="B66" s="237"/>
       <c r="C66" s="4" t="s">
         <v>63</v>
       </c>
@@ -44738,10 +44738,10 @@
       </c>
     </row>
     <row r="81" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A81" s="232" t="s">
+      <c r="A81" s="235" t="s">
         <v>133</v>
       </c>
-      <c r="B81" s="234"/>
+      <c r="B81" s="237"/>
       <c r="C81" s="4" t="s">
         <v>63</v>
       </c>
@@ -44758,7 +44758,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="26.25" thickBot="1">
+    <row r="82" spans="1:7" ht="16.5" thickBot="1">
       <c r="A82" s="15" t="s">
         <v>66</v>
       </c>
@@ -44887,10 +44887,10 @@
       </c>
     </row>
     <row r="88" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A88" s="232" t="s">
+      <c r="A88" s="235" t="s">
         <v>558</v>
       </c>
-      <c r="B88" s="234"/>
+      <c r="B88" s="237"/>
       <c r="C88" s="4" t="s">
         <v>63</v>
       </c>
@@ -44930,7 +44930,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="39" thickBot="1">
+    <row r="90" spans="1:7" ht="26.25" thickBot="1">
       <c r="A90" s="16" t="s">
         <v>68</v>
       </c>
@@ -45017,10 +45017,10 @@
       </c>
     </row>
     <row r="94" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A94" s="232" t="s">
+      <c r="A94" s="235" t="s">
         <v>156</v>
       </c>
-      <c r="B94" s="234"/>
+      <c r="B94" s="237"/>
       <c r="C94" s="4" t="s">
         <v>63</v>
       </c>
@@ -45101,10 +45101,10 @@
       </c>
     </row>
     <row r="98" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A98" s="232" t="s">
+      <c r="A98" s="235" t="s">
         <v>150</v>
       </c>
-      <c r="B98" s="234"/>
+      <c r="B98" s="237"/>
       <c r="C98" s="4" t="s">
         <v>63</v>
       </c>
@@ -45185,10 +45185,10 @@
       </c>
     </row>
     <row r="102" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A102" s="232" t="s">
+      <c r="A102" s="235" t="s">
         <v>547</v>
       </c>
-      <c r="B102" s="234"/>
+      <c r="B102" s="237"/>
       <c r="C102" s="4" t="s">
         <v>63</v>
       </c>
@@ -45292,10 +45292,10 @@
       </c>
     </row>
     <row r="107" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A107" s="232" t="s">
+      <c r="A107" s="235" t="s">
         <v>140</v>
       </c>
-      <c r="B107" s="234"/>
+      <c r="B107" s="237"/>
       <c r="C107" s="4" t="s">
         <v>63</v>
       </c>
@@ -45460,10 +45460,10 @@
       </c>
     </row>
     <row r="115" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A115" s="232" t="s">
+      <c r="A115" s="235" t="s">
         <v>161</v>
       </c>
-      <c r="B115" s="234"/>
+      <c r="B115" s="237"/>
       <c r="C115" s="4" t="s">
         <v>453</v>
       </c>
@@ -45636,6 +45636,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A88:B88"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="C2:D9"/>
@@ -45645,14 +45653,6 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A88:B88"/>
   </mergeCells>
   <conditionalFormatting sqref="A11:A18 A107:A109 A81:A85 A115:A248 A52:A57 A40 A33:A37 A42:A43 A112 A94:A100 A61:A69 A59 A20:A29">
     <cfRule type="beginsWith" dxfId="2509" priority="1308" stopIfTrue="1" operator="beginsWith" text="Exceptional">
@@ -48387,10 +48387,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>701</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -48676,10 +48676,10 @@
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A25" s="232" t="s">
+      <c r="A25" s="235" t="s">
         <v>688</v>
       </c>
-      <c r="B25" s="234"/>
+      <c r="B25" s="237"/>
       <c r="C25" s="4" t="s">
         <v>63</v>
       </c>
@@ -48889,10 +48889,10 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A36" s="232" t="s">
+      <c r="A36" s="235" t="s">
         <v>612</v>
       </c>
-      <c r="B36" s="234"/>
+      <c r="B36" s="237"/>
       <c r="C36" s="4" t="s">
         <v>63</v>
       </c>
@@ -49311,10 +49311,10 @@
       <c r="G57" s="11"/>
     </row>
     <row r="58" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A58" s="232" t="s">
+      <c r="A58" s="235" t="s">
         <v>627</v>
       </c>
-      <c r="B58" s="234"/>
+      <c r="B58" s="237"/>
       <c r="C58" s="4" t="s">
         <v>63</v>
       </c>
@@ -49619,10 +49619,10 @@
       <c r="G73" s="11"/>
     </row>
     <row r="74" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A74" s="232" t="s">
+      <c r="A74" s="235" t="s">
         <v>651</v>
       </c>
-      <c r="B74" s="234"/>
+      <c r="B74" s="237"/>
       <c r="C74" s="4" t="s">
         <v>63</v>
       </c>
@@ -49811,10 +49811,10 @@
       <c r="G83" s="11"/>
     </row>
     <row r="84" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A84" s="232" t="s">
+      <c r="A84" s="235" t="s">
         <v>663</v>
       </c>
-      <c r="B84" s="234"/>
+      <c r="B84" s="237"/>
       <c r="C84" s="21" t="s">
         <v>456</v>
       </c>
@@ -50174,10 +50174,10 @@
       <c r="G102" s="11"/>
     </row>
     <row r="103" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A103" s="232" t="s">
+      <c r="A103" s="235" t="s">
         <v>677</v>
       </c>
-      <c r="B103" s="234"/>
+      <c r="B103" s="237"/>
       <c r="C103" s="4" t="s">
         <v>63</v>
       </c>
@@ -53351,10 +53351,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>291</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -53714,10 +53714,10 @@
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A29" s="232" t="s">
+      <c r="A29" s="235" t="s">
         <v>564</v>
       </c>
-      <c r="B29" s="234"/>
+      <c r="B29" s="237"/>
       <c r="C29" s="4" t="s">
         <v>451</v>
       </c>
@@ -53946,10 +53946,10 @@
       <c r="G40" s="11"/>
     </row>
     <row r="41" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A41" s="232" t="s">
+      <c r="A41" s="235" t="s">
         <v>334</v>
       </c>
-      <c r="B41" s="234"/>
+      <c r="B41" s="237"/>
       <c r="C41" s="4" t="s">
         <v>63</v>
       </c>
@@ -54163,10 +54163,10 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" s="7" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A52" s="232" t="s">
+      <c r="A52" s="235" t="s">
         <v>84</v>
       </c>
-      <c r="B52" s="234"/>
+      <c r="B52" s="237"/>
       <c r="C52" s="4" t="s">
         <v>63</v>
       </c>
@@ -54336,10 +54336,10 @@
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" s="7" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A61" s="232" t="s">
+      <c r="A61" s="235" t="s">
         <v>370</v>
       </c>
-      <c r="B61" s="234"/>
+      <c r="B61" s="237"/>
       <c r="C61" s="21" t="s">
         <v>452</v>
       </c>
@@ -55689,10 +55689,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>810</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -55995,10 +55995,10 @@
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A26" s="232" t="s">
+      <c r="A26" s="235" t="s">
         <v>390</v>
       </c>
-      <c r="B26" s="234"/>
+      <c r="B26" s="237"/>
       <c r="C26" s="4" t="s">
         <v>855</v>
       </c>
@@ -56265,10 +56265,10 @@
       <c r="G39" s="11"/>
     </row>
     <row r="40" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A40" s="232" t="s">
+      <c r="A40" s="235" t="s">
         <v>448</v>
       </c>
-      <c r="B40" s="234"/>
+      <c r="B40" s="237"/>
       <c r="C40" s="102" t="s">
         <v>856</v>
       </c>
@@ -56533,10 +56533,10 @@
       <c r="G53" s="11"/>
     </row>
     <row r="54" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A54" s="232" t="s">
+      <c r="A54" s="235" t="s">
         <v>412</v>
       </c>
-      <c r="B54" s="234"/>
+      <c r="B54" s="237"/>
       <c r="C54" s="4" t="s">
         <v>63</v>
       </c>
@@ -58399,10 +58399,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>239</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -58496,10 +58496,10 @@
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A15" s="232" t="s">
+      <c r="A15" s="235" t="s">
         <v>246</v>
       </c>
-      <c r="B15" s="234"/>
+      <c r="B15" s="237"/>
       <c r="C15" s="4" t="s">
         <v>874</v>
       </c>
@@ -58612,10 +58612,10 @@
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A21" s="232" t="s">
+      <c r="A21" s="235" t="s">
         <v>878</v>
       </c>
-      <c r="B21" s="234"/>
+      <c r="B21" s="237"/>
       <c r="C21" s="4" t="s">
         <v>63</v>
       </c>
@@ -58747,10 +58747,10 @@
       <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A28" s="232" t="s">
+      <c r="A28" s="235" t="s">
         <v>254</v>
       </c>
-      <c r="B28" s="234"/>
+      <c r="B28" s="237"/>
       <c r="C28" s="4" t="s">
         <v>875</v>
       </c>
@@ -58901,10 +58901,10 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A36" s="232" t="s">
+      <c r="A36" s="235" t="s">
         <v>891</v>
       </c>
-      <c r="B36" s="234"/>
+      <c r="B36" s="237"/>
       <c r="C36" s="4" t="s">
         <v>454</v>
       </c>
@@ -59036,10 +59036,10 @@
       <c r="G42" s="11"/>
     </row>
     <row r="43" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A43" s="232" t="s">
+      <c r="A43" s="235" t="s">
         <v>275</v>
       </c>
-      <c r="B43" s="234"/>
+      <c r="B43" s="237"/>
       <c r="C43" s="4" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Updated rubric, TCR complete.
</commit_message>
<xml_diff>
--- a/GameDocuments/gam352_papercut_rubric.xlsx
+++ b/GameDocuments/gam352_papercut_rubric.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Game Data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2417" uniqueCount="984">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2424" uniqueCount="983">
   <si>
     <t>GAME NAME</t>
   </si>
@@ -3704,9 +3704,6 @@
 Windows 10 laptop</t>
   </si>
   <si>
-    <t>Ending</t>
-  </si>
-  <si>
     <t xml:space="preserve">Discovery, Catharsis, Sensation </t>
   </si>
   <si>
@@ -3731,13 +3728,13 @@
     <t>Graded by Douglas</t>
   </si>
   <si>
-    <t>Spacebar, Enter and Start button not supported, yet.  Graded by Douglas</t>
-  </si>
-  <si>
     <t>Fade in and out</t>
   </si>
   <si>
     <t>No pause</t>
+  </si>
+  <si>
+    <t>Rocket Ending</t>
   </si>
 </sst>
 </file>
@@ -5780,90 +5777,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -5897,6 +5810,18 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -5954,6 +5879,99 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="4" borderId="16" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="4" borderId="18" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="9" fontId="26" fillId="3" borderId="21" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5964,12 +5982,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="26" fillId="3" borderId="26" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6038,37 +6050,55 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="4" borderId="16" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="4" borderId="18" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6080,28 +6110,28 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6128,52 +6158,19 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -39834,7 +39831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -39854,54 +39851,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A1" s="144" t="s">
+      <c r="A1" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="146"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="178"/>
       <c r="E1" s="103"/>
-      <c r="F1" s="144" t="s">
+      <c r="F1" s="176" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
-      <c r="J1" s="146"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="178"/>
       <c r="K1" s="104"/>
       <c r="L1" s="104"/>
       <c r="M1" s="105"/>
     </row>
     <row r="2" spans="1:13" ht="14.1" customHeight="1">
-      <c r="A2" s="147" t="s">
+      <c r="A2" s="182" t="s">
         <v>951</v>
       </c>
-      <c r="B2" s="148"/>
-      <c r="C2" s="148"/>
-      <c r="D2" s="149"/>
+      <c r="B2" s="183"/>
+      <c r="C2" s="183"/>
+      <c r="D2" s="184"/>
       <c r="E2" s="103"/>
-      <c r="F2" s="147" t="s">
+      <c r="F2" s="182" t="s">
         <v>954</v>
       </c>
-      <c r="G2" s="148"/>
-      <c r="H2" s="148"/>
-      <c r="I2" s="148"/>
-      <c r="J2" s="149"/>
+      <c r="G2" s="183"/>
+      <c r="H2" s="183"/>
+      <c r="I2" s="183"/>
+      <c r="J2" s="184"/>
       <c r="K2" s="104"/>
       <c r="L2" s="104"/>
       <c r="M2" s="105"/>
     </row>
     <row r="3" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A3" s="150"/>
-      <c r="B3" s="151"/>
-      <c r="C3" s="151"/>
-      <c r="D3" s="152"/>
+      <c r="A3" s="185"/>
+      <c r="B3" s="186"/>
+      <c r="C3" s="186"/>
+      <c r="D3" s="187"/>
       <c r="E3" s="103"/>
-      <c r="F3" s="150"/>
-      <c r="G3" s="151"/>
-      <c r="H3" s="151"/>
-      <c r="I3" s="151"/>
-      <c r="J3" s="152"/>
+      <c r="F3" s="185"/>
+      <c r="G3" s="186"/>
+      <c r="H3" s="186"/>
+      <c r="I3" s="186"/>
+      <c r="J3" s="187"/>
       <c r="K3" s="104"/>
       <c r="L3" s="104"/>
       <c r="M3" s="105"/>
@@ -39922,41 +39919,41 @@
       <c r="M4" s="105"/>
     </row>
     <row r="5" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A5" s="144" t="s">
+      <c r="A5" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="145"/>
-      <c r="C5" s="145"/>
-      <c r="D5" s="146"/>
+      <c r="B5" s="177"/>
+      <c r="C5" s="177"/>
+      <c r="D5" s="178"/>
       <c r="E5" s="103"/>
-      <c r="F5" s="144" t="s">
+      <c r="F5" s="176" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="145"/>
-      <c r="H5" s="145"/>
-      <c r="I5" s="145"/>
-      <c r="J5" s="146"/>
+      <c r="G5" s="177"/>
+      <c r="H5" s="177"/>
+      <c r="I5" s="177"/>
+      <c r="J5" s="178"/>
       <c r="K5" s="104"/>
       <c r="L5" s="107"/>
       <c r="M5" s="105"/>
     </row>
     <row r="6" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A6" s="156" t="s">
+      <c r="A6" s="173" t="s">
         <v>952</v>
       </c>
-      <c r="B6" s="157"/>
-      <c r="C6" s="157"/>
-      <c r="D6" s="158"/>
+      <c r="B6" s="174"/>
+      <c r="C6" s="174"/>
+      <c r="D6" s="175"/>
       <c r="E6" s="103"/>
-      <c r="F6" s="156" t="s">
+      <c r="F6" s="173" t="s">
         <v>955</v>
       </c>
-      <c r="G6" s="157"/>
-      <c r="H6" s="157"/>
-      <c r="I6" s="157"/>
-      <c r="J6" s="158"/>
+      <c r="G6" s="174"/>
+      <c r="H6" s="174"/>
+      <c r="I6" s="174"/>
+      <c r="J6" s="175"/>
       <c r="K6" s="104"/>
-      <c r="L6" s="153" t="s">
+      <c r="L6" s="170" t="s">
         <v>24</v>
       </c>
       <c r="M6" s="105"/>
@@ -39967,51 +39964,51 @@
       <c r="C7" s="108"/>
       <c r="D7" s="109"/>
       <c r="E7" s="103"/>
-      <c r="F7" s="156" t="s">
-        <v>979</v>
-      </c>
-      <c r="G7" s="157"/>
-      <c r="H7" s="157"/>
-      <c r="I7" s="157"/>
-      <c r="J7" s="158"/>
+      <c r="F7" s="173" t="s">
+        <v>978</v>
+      </c>
+      <c r="G7" s="174"/>
+      <c r="H7" s="174"/>
+      <c r="I7" s="174"/>
+      <c r="J7" s="175"/>
       <c r="K7" s="104"/>
-      <c r="L7" s="154"/>
+      <c r="L7" s="171"/>
       <c r="M7" s="105"/>
     </row>
     <row r="8" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A8" s="144" t="s">
+      <c r="A8" s="176" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="145"/>
-      <c r="C8" s="145"/>
-      <c r="D8" s="146"/>
+      <c r="B8" s="177"/>
+      <c r="C8" s="177"/>
+      <c r="D8" s="178"/>
       <c r="E8" s="103"/>
-      <c r="F8" s="156" t="s">
-        <v>978</v>
-      </c>
-      <c r="G8" s="157"/>
-      <c r="H8" s="157"/>
-      <c r="I8" s="157"/>
-      <c r="J8" s="158"/>
+      <c r="F8" s="173" t="s">
+        <v>977</v>
+      </c>
+      <c r="G8" s="174"/>
+      <c r="H8" s="174"/>
+      <c r="I8" s="174"/>
+      <c r="J8" s="175"/>
       <c r="K8" s="104"/>
-      <c r="L8" s="154"/>
+      <c r="L8" s="171"/>
       <c r="M8" s="105"/>
     </row>
     <row r="9" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A9" s="156" t="s">
+      <c r="A9" s="173" t="s">
         <v>953</v>
       </c>
-      <c r="B9" s="157"/>
-      <c r="C9" s="157"/>
-      <c r="D9" s="158"/>
+      <c r="B9" s="174"/>
+      <c r="C9" s="174"/>
+      <c r="D9" s="175"/>
       <c r="E9" s="103"/>
-      <c r="F9" s="156"/>
-      <c r="G9" s="157"/>
-      <c r="H9" s="157"/>
-      <c r="I9" s="157"/>
-      <c r="J9" s="158"/>
+      <c r="F9" s="173"/>
+      <c r="G9" s="174"/>
+      <c r="H9" s="174"/>
+      <c r="I9" s="174"/>
+      <c r="J9" s="175"/>
       <c r="K9" s="104"/>
-      <c r="L9" s="155"/>
+      <c r="L9" s="172"/>
       <c r="M9" s="105"/>
     </row>
     <row r="10" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40030,18 +40027,18 @@
       <c r="M10" s="105"/>
     </row>
     <row r="11" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A11" s="144" t="s">
+      <c r="A11" s="176" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="145"/>
-      <c r="C11" s="145"/>
-      <c r="D11" s="146"/>
+      <c r="B11" s="177"/>
+      <c r="C11" s="177"/>
+      <c r="D11" s="178"/>
       <c r="E11" s="103"/>
-      <c r="F11" s="144" t="s">
+      <c r="F11" s="176" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="145"/>
-      <c r="H11" s="146"/>
+      <c r="G11" s="177"/>
+      <c r="H11" s="178"/>
       <c r="I11" s="134" t="s">
         <v>7</v>
       </c>
@@ -40081,7 +40078,7 @@
         <v>-0.12</v>
       </c>
       <c r="K12" s="104"/>
-      <c r="L12" s="153" t="s">
+      <c r="L12" s="170" t="s">
         <v>8</v>
       </c>
       <c r="M12" s="105"/>
@@ -40114,7 +40111,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="120"/>
-      <c r="L13" s="154"/>
+      <c r="L13" s="171"/>
       <c r="M13" s="121"/>
     </row>
     <row r="14" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40144,7 +40141,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="124"/>
-      <c r="L14" s="155"/>
+      <c r="L14" s="172"/>
       <c r="M14" s="125"/>
     </row>
     <row r="15" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40212,11 +40209,11 @@
         <v>939</v>
       </c>
       <c r="E17" s="104"/>
-      <c r="F17" s="144" t="s">
+      <c r="F17" s="176" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="145"/>
-      <c r="H17" s="146"/>
+      <c r="G17" s="177"/>
+      <c r="H17" s="178"/>
       <c r="I17" s="111"/>
       <c r="J17" s="135">
         <v>0.75</v>
@@ -40242,17 +40239,17 @@
       <c r="F18" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="159" t="s">
+      <c r="G18" s="179" t="s">
         <v>956</v>
       </c>
-      <c r="H18" s="160"/>
-      <c r="I18" s="161"/>
+      <c r="H18" s="180"/>
+      <c r="I18" s="181"/>
       <c r="J18" s="137">
         <f>IF(LEFT(G18,6)="Entire",0,IF(LEFT(G18,6)="Custom",-0.05,-0.1))</f>
         <v>-0.1</v>
       </c>
       <c r="K18" s="128"/>
-      <c r="L18" s="153" t="s">
+      <c r="L18" s="170" t="s">
         <v>18</v>
       </c>
       <c r="M18" s="105"/>
@@ -40274,17 +40271,17 @@
       <c r="F19" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="162" t="s">
+      <c r="G19" s="153" t="s">
         <v>957</v>
       </c>
-      <c r="H19" s="163"/>
-      <c r="I19" s="164"/>
+      <c r="H19" s="154"/>
+      <c r="I19" s="155"/>
       <c r="J19" s="139">
         <f>IF(G19="2D Graphics and 2D Gameplay",IF(J11=0.15,-0.05,0),IF(G19="3D Graphics but 2D Gameplay",IF(J11=0.15,-0.02,-0.3),IF(J11=0.15,0,-0.3)))</f>
         <v>0</v>
       </c>
       <c r="K19" s="104"/>
-      <c r="L19" s="155"/>
+      <c r="L19" s="172"/>
       <c r="M19" s="105"/>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40336,22 +40333,22 @@
       <c r="C22" s="118"/>
       <c r="D22" s="119"/>
       <c r="E22" s="104"/>
-      <c r="F22" s="186" t="s">
+      <c r="F22" s="168" t="s">
         <v>713</v>
       </c>
-      <c r="G22" s="184" t="s">
+      <c r="G22" s="166" t="s">
         <v>714</v>
       </c>
-      <c r="H22" s="183"/>
+      <c r="H22" s="165"/>
       <c r="I22" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="181">
+      <c r="J22" s="163">
         <f>J20+J15</f>
         <v>0.68</v>
       </c>
       <c r="K22" s="104"/>
-      <c r="L22" s="165" t="s">
+      <c r="L22" s="144" t="s">
         <v>725</v>
       </c>
       <c r="M22" s="105"/>
@@ -40362,15 +40359,15 @@
       <c r="C23" s="118"/>
       <c r="D23" s="119"/>
       <c r="E23" s="104"/>
-      <c r="F23" s="187"/>
-      <c r="G23" s="185"/>
-      <c r="H23" s="183"/>
+      <c r="F23" s="169"/>
+      <c r="G23" s="167"/>
+      <c r="H23" s="165"/>
       <c r="I23" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="182"/>
+      <c r="J23" s="164"/>
       <c r="K23" s="104"/>
-      <c r="L23" s="166"/>
+      <c r="L23" s="145"/>
       <c r="M23" s="105"/>
     </row>
     <row r="24" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40394,13 +40391,13 @@
       <c r="C25" s="118"/>
       <c r="D25" s="119"/>
       <c r="E25" s="104"/>
-      <c r="F25" s="175" t="s">
+      <c r="F25" s="157" t="s">
         <v>932</v>
       </c>
-      <c r="G25" s="176"/>
-      <c r="H25" s="176"/>
-      <c r="I25" s="176"/>
-      <c r="J25" s="177"/>
+      <c r="G25" s="158"/>
+      <c r="H25" s="158"/>
+      <c r="I25" s="158"/>
+      <c r="J25" s="159"/>
       <c r="K25" s="104"/>
       <c r="L25" s="104"/>
       <c r="M25" s="105"/>
@@ -40411,11 +40408,11 @@
       <c r="C26" s="118"/>
       <c r="D26" s="119"/>
       <c r="E26" s="103"/>
-      <c r="F26" s="178"/>
-      <c r="G26" s="179"/>
-      <c r="H26" s="179"/>
-      <c r="I26" s="179"/>
-      <c r="J26" s="180"/>
+      <c r="F26" s="160"/>
+      <c r="G26" s="161"/>
+      <c r="H26" s="161"/>
+      <c r="I26" s="161"/>
+      <c r="J26" s="162"/>
       <c r="K26" s="104"/>
       <c r="L26" s="104"/>
       <c r="M26" s="105"/>
@@ -40441,13 +40438,13 @@
       <c r="C28" s="118"/>
       <c r="D28" s="119"/>
       <c r="E28" s="103"/>
-      <c r="F28" s="174" t="s">
+      <c r="F28" s="156" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="174"/>
-      <c r="H28" s="174"/>
-      <c r="I28" s="174"/>
-      <c r="J28" s="174"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
       <c r="K28" s="104"/>
       <c r="L28" s="104"/>
       <c r="M28" s="105"/>
@@ -40458,13 +40455,13 @@
       <c r="C29" s="118"/>
       <c r="D29" s="119"/>
       <c r="E29" s="103"/>
-      <c r="F29" s="171" t="s">
+      <c r="F29" s="150" t="s">
         <v>933</v>
       </c>
-      <c r="G29" s="172"/>
-      <c r="H29" s="172"/>
-      <c r="I29" s="172"/>
-      <c r="J29" s="173"/>
+      <c r="G29" s="151"/>
+      <c r="H29" s="151"/>
+      <c r="I29" s="151"/>
+      <c r="J29" s="152"/>
       <c r="K29" s="104"/>
       <c r="L29" s="104"/>
       <c r="M29" s="105"/>
@@ -40475,30 +40472,30 @@
       <c r="C30" s="118"/>
       <c r="D30" s="119"/>
       <c r="E30" s="103"/>
-      <c r="F30" s="171"/>
-      <c r="G30" s="172"/>
-      <c r="H30" s="172"/>
-      <c r="I30" s="172"/>
-      <c r="J30" s="173"/>
+      <c r="F30" s="150"/>
+      <c r="G30" s="151"/>
+      <c r="H30" s="151"/>
+      <c r="I30" s="151"/>
+      <c r="J30" s="152"/>
       <c r="K30" s="104"/>
       <c r="L30" s="104"/>
       <c r="M30" s="105"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A31" s="167" t="s">
+      <c r="A31" s="146" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="168"/>
-      <c r="C31" s="169" t="s">
+      <c r="B31" s="147"/>
+      <c r="C31" s="148" t="s">
         <v>950</v>
       </c>
-      <c r="D31" s="170"/>
+      <c r="D31" s="149"/>
       <c r="E31" s="104"/>
-      <c r="F31" s="162"/>
-      <c r="G31" s="163"/>
-      <c r="H31" s="163"/>
-      <c r="I31" s="163"/>
-      <c r="J31" s="164"/>
+      <c r="F31" s="153"/>
+      <c r="G31" s="154"/>
+      <c r="H31" s="154"/>
+      <c r="I31" s="154"/>
+      <c r="J31" s="155"/>
       <c r="K31" s="104"/>
       <c r="L31" s="104"/>
       <c r="M31" s="105"/>
@@ -40521,16 +40518,12 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0"/>
   <mergeCells count="31">
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F29:J31"/>
-    <mergeCell ref="F28:J28"/>
-    <mergeCell ref="F25:J26"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A2:D3"/>
+    <mergeCell ref="F2:J3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:J5"/>
     <mergeCell ref="L12:L14"/>
     <mergeCell ref="L18:L19"/>
     <mergeCell ref="A6:D6"/>
@@ -40546,12 +40539,16 @@
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="G18:I18"/>
     <mergeCell ref="G19:I19"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="A2:D3"/>
-    <mergeCell ref="F2:J3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F29:J31"/>
+    <mergeCell ref="F28:J28"/>
+    <mergeCell ref="F25:J26"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F22:F23"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6:D6">
@@ -40595,7 +40592,7 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -40619,57 +40616,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A1" s="194" t="s">
+      <c r="A1" s="199" t="s">
         <v>556</v>
       </c>
-      <c r="B1" s="195"/>
-      <c r="C1" s="195"/>
-      <c r="D1" s="195"/>
-      <c r="E1" s="195"/>
-      <c r="F1" s="195"/>
-      <c r="G1" s="195"/>
-      <c r="H1" s="195"/>
-      <c r="J1" s="205" t="s">
+      <c r="B1" s="200"/>
+      <c r="C1" s="200"/>
+      <c r="D1" s="200"/>
+      <c r="E1" s="200"/>
+      <c r="F1" s="200"/>
+      <c r="G1" s="200"/>
+      <c r="H1" s="200"/>
+      <c r="J1" s="210" t="s">
         <v>482</v>
       </c>
-      <c r="K1" s="206"/>
-      <c r="L1" s="207"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="212"/>
       <c r="M1" s="79"/>
       <c r="N1" s="24" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A2" s="194"/>
-      <c r="B2" s="195"/>
-      <c r="C2" s="195"/>
-      <c r="D2" s="195"/>
-      <c r="E2" s="195"/>
-      <c r="F2" s="195"/>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
-      <c r="J2" s="208" t="s">
+      <c r="A2" s="199"/>
+      <c r="B2" s="200"/>
+      <c r="C2" s="200"/>
+      <c r="D2" s="200"/>
+      <c r="E2" s="200"/>
+      <c r="F2" s="200"/>
+      <c r="G2" s="200"/>
+      <c r="H2" s="200"/>
+      <c r="J2" s="213" t="s">
         <v>706</v>
       </c>
-      <c r="K2" s="209"/>
-      <c r="L2" s="210"/>
+      <c r="K2" s="214"/>
+      <c r="L2" s="215"/>
       <c r="M2" s="23"/>
       <c r="N2" s="26" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A3" s="194"/>
-      <c r="B3" s="195"/>
-      <c r="C3" s="195"/>
-      <c r="D3" s="195"/>
-      <c r="E3" s="195"/>
-      <c r="F3" s="195"/>
-      <c r="G3" s="195"/>
-      <c r="H3" s="195"/>
-      <c r="J3" s="208"/>
-      <c r="K3" s="209"/>
-      <c r="L3" s="210"/>
+      <c r="A3" s="199"/>
+      <c r="B3" s="200"/>
+      <c r="C3" s="200"/>
+      <c r="D3" s="200"/>
+      <c r="E3" s="200"/>
+      <c r="F3" s="200"/>
+      <c r="G3" s="200"/>
+      <c r="H3" s="200"/>
+      <c r="J3" s="213"/>
+      <c r="K3" s="214"/>
+      <c r="L3" s="215"/>
       <c r="M3" s="23"/>
       <c r="N3" s="26" t="s">
         <v>431</v>
@@ -40679,14 +40676,14 @@
       <c r="A4" s="2"/>
       <c r="B4" s="5"/>
       <c r="C4" s="8"/>
-      <c r="D4" s="193"/>
-      <c r="E4" s="193"/>
+      <c r="D4" s="192"/>
+      <c r="E4" s="192"/>
       <c r="F4" s="43"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="193"/>
-      <c r="J4" s="208"/>
-      <c r="K4" s="209"/>
-      <c r="L4" s="210"/>
+      <c r="G4" s="192"/>
+      <c r="H4" s="192"/>
+      <c r="J4" s="213"/>
+      <c r="K4" s="214"/>
+      <c r="L4" s="215"/>
       <c r="M4" s="34"/>
       <c r="N4" s="26" t="s">
         <v>432</v>
@@ -40694,24 +40691,24 @@
       <c r="O4" s="81"/>
     </row>
     <row r="5" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A5" s="196" t="s">
+      <c r="A5" s="201" t="s">
         <v>425</v>
       </c>
-      <c r="B5" s="197"/>
+      <c r="B5" s="202"/>
       <c r="C5" s="8"/>
-      <c r="D5" s="200" t="s">
+      <c r="D5" s="205" t="s">
         <v>717</v>
       </c>
-      <c r="E5" s="201"/>
-      <c r="F5" s="202"/>
-      <c r="G5" s="203">
+      <c r="E5" s="206"/>
+      <c r="F5" s="207"/>
+      <c r="G5" s="208">
         <f>Submission!$E$17</f>
         <v>0</v>
       </c>
-      <c r="H5" s="204"/>
-      <c r="J5" s="208"/>
-      <c r="K5" s="209"/>
-      <c r="L5" s="210"/>
+      <c r="H5" s="209"/>
+      <c r="J5" s="213"/>
+      <c r="K5" s="214"/>
+      <c r="L5" s="215"/>
       <c r="M5" s="34"/>
       <c r="N5" s="26" t="s">
         <v>433</v>
@@ -40719,21 +40716,21 @@
       <c r="O5" s="81"/>
     </row>
     <row r="6" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A6" s="198"/>
-      <c r="B6" s="199"/>
+      <c r="A6" s="203"/>
+      <c r="B6" s="204"/>
       <c r="C6" s="43"/>
-      <c r="D6" s="193" t="s">
+      <c r="D6" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="193"/>
+      <c r="E6" s="192"/>
       <c r="F6" s="43"/>
-      <c r="G6" s="193" t="s">
+      <c r="G6" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="193"/>
-      <c r="J6" s="208"/>
-      <c r="K6" s="209"/>
-      <c r="L6" s="210"/>
+      <c r="H6" s="192"/>
+      <c r="J6" s="213"/>
+      <c r="K6" s="214"/>
+      <c r="L6" s="215"/>
       <c r="M6" s="34"/>
       <c r="N6" s="26" t="s">
         <v>434</v>
@@ -40741,24 +40738,24 @@
       <c r="O6" s="81"/>
     </row>
     <row r="7" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A7" s="188">
+      <c r="A7" s="195">
         <f>'Game Data'!$J$22</f>
         <v>0.68</v>
       </c>
-      <c r="B7" s="189"/>
+      <c r="B7" s="196"/>
       <c r="C7" s="43"/>
-      <c r="D7" s="216" t="s">
+      <c r="D7" s="193" t="s">
         <v>724</v>
       </c>
-      <c r="E7" s="217"/>
+      <c r="E7" s="194"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="216" t="s">
+      <c r="G7" s="193" t="s">
         <v>724</v>
       </c>
-      <c r="H7" s="217"/>
-      <c r="J7" s="208"/>
-      <c r="K7" s="209"/>
-      <c r="L7" s="210"/>
+      <c r="H7" s="194"/>
+      <c r="J7" s="213"/>
+      <c r="K7" s="214"/>
+      <c r="L7" s="215"/>
       <c r="M7" s="33"/>
       <c r="N7" s="26" t="s">
         <v>435</v>
@@ -40766,23 +40763,23 @@
       <c r="O7" s="81"/>
     </row>
     <row r="8" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A8" s="190"/>
-      <c r="B8" s="191"/>
+      <c r="A8" s="197"/>
+      <c r="B8" s="198"/>
       <c r="C8" s="97"/>
-      <c r="D8" s="214">
+      <c r="D8" s="219">
         <f>E17+E26+E35+E44+E53</f>
-        <v>0.30125000000000002</v>
-      </c>
-      <c r="E8" s="215"/>
+        <v>0.31124999999999997</v>
+      </c>
+      <c r="E8" s="220"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="214">
+      <c r="G8" s="219">
         <f>H17+H26+H35+H44+H53</f>
-        <v>4.9999999999999975E-3</v>
-      </c>
-      <c r="H8" s="215"/>
-      <c r="J8" s="211"/>
-      <c r="K8" s="212"/>
-      <c r="L8" s="213"/>
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="H8" s="220"/>
+      <c r="J8" s="216"/>
+      <c r="K8" s="217"/>
+      <c r="L8" s="218"/>
       <c r="M8" s="80"/>
       <c r="N8" s="25" t="s">
         <v>436</v>
@@ -40793,15 +40790,15 @@
       <c r="A9" s="2"/>
       <c r="B9" s="5"/>
       <c r="C9" s="43"/>
-      <c r="D9" s="193" t="s">
+      <c r="D9" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="193"/>
+      <c r="E9" s="192"/>
       <c r="F9" s="43"/>
-      <c r="G9" s="193" t="s">
+      <c r="G9" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="193"/>
+      <c r="H9" s="192"/>
       <c r="J9" s="82"/>
       <c r="K9" s="82"/>
       <c r="L9" s="82"/>
@@ -40828,11 +40825,11 @@
       <c r="H10" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="192" t="s">
+      <c r="J10" s="191" t="s">
         <v>707</v>
       </c>
-      <c r="K10" s="192"/>
-      <c r="L10" s="192"/>
+      <c r="K10" s="191"/>
+      <c r="L10" s="191"/>
       <c r="O10" s="84"/>
     </row>
     <row r="11" spans="1:15" ht="14.1" customHeight="1">
@@ -40861,11 +40858,11 @@
         <f t="shared" ref="H11:H16" si="1">$B11*G11</f>
         <v>0</v>
       </c>
-      <c r="J11" s="220" t="s">
+      <c r="J11" s="190" t="s">
         <v>792</v>
       </c>
-      <c r="K11" s="220"/>
-      <c r="L11" s="220"/>
+      <c r="K11" s="190"/>
+      <c r="L11" s="190"/>
       <c r="M11" s="82"/>
       <c r="O11" s="84"/>
     </row>
@@ -40889,15 +40886,15 @@
       <c r="F12" s="43"/>
       <c r="G12" s="39">
         <f>TECH!$F$3</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H12" s="47">
         <f t="shared" si="1"/>
-        <v>-0.04</v>
-      </c>
-      <c r="J12" s="220"/>
-      <c r="K12" s="220"/>
-      <c r="L12" s="220"/>
+        <v>-0.02</v>
+      </c>
+      <c r="J12" s="190"/>
+      <c r="K12" s="190"/>
+      <c r="L12" s="190"/>
       <c r="M12" s="82"/>
       <c r="O12" s="84"/>
     </row>
@@ -40927,9 +40924,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="220"/>
-      <c r="K13" s="220"/>
-      <c r="L13" s="220"/>
+      <c r="J13" s="190"/>
+      <c r="K13" s="190"/>
+      <c r="L13" s="190"/>
       <c r="M13" s="82"/>
       <c r="O13" s="84"/>
     </row>
@@ -40995,13 +40992,13 @@
         <f t="shared" si="1"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J15" s="218">
+      <c r="J15" s="188">
         <f>MAX(0,MIN(1,IF($J17 &lt;= 0.95, ROUND($J17,2), FLOOR((0.95+($J17-0.95)/5),0.01))))</f>
-        <v>0.85</v>
-      </c>
-      <c r="L15" s="218">
+        <v>0.86</v>
+      </c>
+      <c r="L15" s="188">
         <f>MAX(0,MIN(1,IF($L17 &lt;= 0.95, ROUND($L17,2), FLOOR((0.95+($L17-0.95)/5),0.01))))</f>
-        <v>0.69</v>
+        <v>0.71</v>
       </c>
       <c r="M15" s="82"/>
       <c r="O15" s="84"/>
@@ -41032,8 +41029,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J16" s="219"/>
-      <c r="L16" s="219"/>
+      <c r="J16" s="189"/>
+      <c r="L16" s="189"/>
       <c r="M16" s="82"/>
       <c r="O16" s="84"/>
     </row>
@@ -41054,15 +41051,15 @@
       </c>
       <c r="H17" s="41">
         <f>SUM(H11:H16)</f>
-        <v>4.9999999999999975E-3</v>
+        <v>2.4999999999999998E-2</v>
       </c>
       <c r="J17" s="87">
         <f>$A$7+$E17+IF($D$8-$E17 &gt; 0, ($D$8-$E17)/2, $D$8-$E17)+$G$5</f>
-        <v>0.85312500000000013</v>
+        <v>0.85812500000000003</v>
       </c>
       <c r="L17" s="87">
         <f>$A$7+$H17+IF($G$8 &gt; 0, ($G$8-$H17)/2, $G$8-$H17)+$G$5</f>
-        <v>0.68500000000000005</v>
+        <v>0.70500000000000007</v>
       </c>
       <c r="M17" s="82"/>
     </row>
@@ -41070,15 +41067,15 @@
       <c r="A18" s="2"/>
       <c r="B18" s="5"/>
       <c r="C18" s="43"/>
-      <c r="D18" s="193" t="s">
+      <c r="D18" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="193"/>
+      <c r="E18" s="192"/>
       <c r="F18" s="43"/>
-      <c r="G18" s="193" t="s">
+      <c r="G18" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="193"/>
+      <c r="H18" s="192"/>
       <c r="J18" s="88"/>
       <c r="M18" s="78"/>
     </row>
@@ -41103,11 +41100,11 @@
       <c r="H19" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="192" t="s">
+      <c r="J19" s="191" t="s">
         <v>715</v>
       </c>
-      <c r="K19" s="192"/>
-      <c r="L19" s="192"/>
+      <c r="K19" s="191"/>
+      <c r="L19" s="191"/>
       <c r="M19" s="83"/>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1">
@@ -41136,11 +41133,11 @@
         <f t="shared" ref="H20:H25" si="3">$B20*G20</f>
         <v>0</v>
       </c>
-      <c r="J20" s="220" t="s">
+      <c r="J20" s="190" t="s">
         <v>722</v>
       </c>
-      <c r="K20" s="220"/>
-      <c r="L20" s="220"/>
+      <c r="K20" s="190"/>
+      <c r="L20" s="190"/>
       <c r="M20" s="84"/>
     </row>
     <row r="21" spans="1:13" ht="14.1" customHeight="1">
@@ -41169,9 +41166,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J21" s="220"/>
-      <c r="K21" s="220"/>
-      <c r="L21" s="220"/>
+      <c r="J21" s="190"/>
+      <c r="K21" s="190"/>
+      <c r="L21" s="190"/>
       <c r="M21" s="84"/>
     </row>
     <row r="22" spans="1:13" ht="14.1" customHeight="1">
@@ -41200,9 +41197,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J22" s="220"/>
-      <c r="K22" s="220"/>
-      <c r="L22" s="220"/>
+      <c r="J22" s="190"/>
+      <c r="K22" s="190"/>
+      <c r="L22" s="190"/>
       <c r="M22" s="84"/>
     </row>
     <row r="23" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -41216,11 +41213,11 @@
       <c r="C23" s="36"/>
       <c r="D23" s="39">
         <f>DESIGN!$E$7</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E23" s="47">
         <f t="shared" si="2"/>
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="F23" s="43"/>
       <c r="G23" s="39">
@@ -41266,11 +41263,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J24" s="218">
+      <c r="J24" s="188">
         <f>MAX(0,MIN(1,IF($J26 &lt;= 0.95, ROUND($J26,2), FLOOR((0.95+($J26-0.95)/5),0.01))))</f>
-        <v>0.86</v>
-      </c>
-      <c r="L24" s="218">
+        <v>0.88</v>
+      </c>
+      <c r="L24" s="188">
         <f>MAX(0,MIN(1,IF($L26 &lt;= 0.95, ROUND($L26,2), FLOOR((0.95+($L26-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -41302,8 +41299,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J25" s="219"/>
-      <c r="L25" s="219"/>
+      <c r="J25" s="189"/>
+      <c r="L25" s="189"/>
       <c r="M25" s="84"/>
     </row>
     <row r="26" spans="1:13" ht="14.1" customHeight="1">
@@ -41315,7 +41312,7 @@
       </c>
       <c r="E26" s="41">
         <f>SUM(E20:E25)</f>
-        <v>8.8750000000000009E-2</v>
+        <v>9.8750000000000004E-2</v>
       </c>
       <c r="F26" s="43"/>
       <c r="G26" s="22" t="s">
@@ -41327,7 +41324,7 @@
       </c>
       <c r="J26" s="87">
         <f>$A$7+MIN(MAX($E26*2,$E26),$D$8)</f>
-        <v>0.85750000000000004</v>
+        <v>0.87750000000000006</v>
       </c>
       <c r="L26" s="87">
         <f>$A$7+MIN(MAX($H26*2,$H26),$G$8)+$G$5</f>
@@ -41339,15 +41336,15 @@
       <c r="A27" s="2"/>
       <c r="B27" s="5"/>
       <c r="C27" s="43"/>
-      <c r="D27" s="193" t="s">
+      <c r="D27" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="193"/>
+      <c r="E27" s="192"/>
       <c r="F27" s="43"/>
-      <c r="G27" s="193" t="s">
+      <c r="G27" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H27" s="193"/>
+      <c r="H27" s="192"/>
     </row>
     <row r="28" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
       <c r="A28" s="1" t="s">
@@ -41370,11 +41367,11 @@
       <c r="H28" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J28" s="192" t="s">
+      <c r="J28" s="191" t="s">
         <v>709</v>
       </c>
-      <c r="K28" s="192"/>
-      <c r="L28" s="192"/>
+      <c r="K28" s="191"/>
+      <c r="L28" s="191"/>
     </row>
     <row r="29" spans="1:13" ht="14.1" customHeight="1">
       <c r="A29" s="57" t="str">
@@ -41402,11 +41399,11 @@
         <f t="shared" ref="H29:H34" si="5">$B29*G29</f>
         <v>0</v>
       </c>
-      <c r="J29" s="220" t="s">
+      <c r="J29" s="190" t="s">
         <v>710</v>
       </c>
-      <c r="K29" s="220"/>
-      <c r="L29" s="220"/>
+      <c r="K29" s="190"/>
+      <c r="L29" s="190"/>
     </row>
     <row r="30" spans="1:13" ht="14.1" customHeight="1">
       <c r="A30" s="58" t="str">
@@ -41434,9 +41431,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J30" s="220"/>
-      <c r="K30" s="220"/>
-      <c r="L30" s="220"/>
+      <c r="J30" s="190"/>
+      <c r="K30" s="190"/>
+      <c r="L30" s="190"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1">
       <c r="A31" s="58" t="str">
@@ -41464,9 +41461,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J31" s="220"/>
-      <c r="K31" s="220"/>
-      <c r="L31" s="220"/>
+      <c r="J31" s="190"/>
+      <c r="K31" s="190"/>
+      <c r="L31" s="190"/>
     </row>
     <row r="32" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
       <c r="A32" s="58" t="str">
@@ -41528,11 +41525,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J33" s="218">
+      <c r="J33" s="188">
         <f>MAX(0,MIN(1,IF($J35 &lt;= 0.95, ROUND($J35,2), FLOOR((0.95+($J35-0.95)/5),0.01))))</f>
         <v>0.88</v>
       </c>
-      <c r="L33" s="218">
+      <c r="L33" s="188">
         <f>MAX(0,MIN(1,IF($L35 &lt;= 0.95, ROUND($L35,2), FLOOR((0.95+($L35-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -41563,8 +41560,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J34" s="219"/>
-      <c r="L34" s="219"/>
+      <c r="J34" s="189"/>
+      <c r="L34" s="189"/>
     </row>
     <row r="35" spans="1:12" ht="14.1" customHeight="1">
       <c r="A35" s="2"/>
@@ -41598,15 +41595,15 @@
       <c r="A36" s="2"/>
       <c r="B36" s="5"/>
       <c r="C36" s="43"/>
-      <c r="D36" s="193" t="s">
+      <c r="D36" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="193"/>
+      <c r="E36" s="192"/>
       <c r="F36" s="43"/>
-      <c r="G36" s="193" t="s">
+      <c r="G36" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H36" s="193"/>
+      <c r="H36" s="192"/>
     </row>
     <row r="37" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A37" s="1" t="s">
@@ -41629,11 +41626,11 @@
       <c r="H37" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J37" s="192" t="s">
+      <c r="J37" s="191" t="s">
         <v>711</v>
       </c>
-      <c r="K37" s="192"/>
-      <c r="L37" s="192"/>
+      <c r="K37" s="191"/>
+      <c r="L37" s="191"/>
     </row>
     <row r="38" spans="1:12" ht="14.1" customHeight="1">
       <c r="A38" s="57" t="str">
@@ -41661,11 +41658,11 @@
         <f t="shared" ref="H38:H43" si="7">$B38*G38</f>
         <v>0</v>
       </c>
-      <c r="J38" s="220" t="s">
+      <c r="J38" s="190" t="s">
         <v>712</v>
       </c>
-      <c r="K38" s="220"/>
-      <c r="L38" s="220"/>
+      <c r="K38" s="190"/>
+      <c r="L38" s="190"/>
     </row>
     <row r="39" spans="1:12" ht="14.1" customHeight="1">
       <c r="A39" s="58" t="str">
@@ -41693,9 +41690,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J39" s="220"/>
-      <c r="K39" s="220"/>
-      <c r="L39" s="220"/>
+      <c r="J39" s="190"/>
+      <c r="K39" s="190"/>
+      <c r="L39" s="190"/>
     </row>
     <row r="40" spans="1:12" ht="14.1" customHeight="1">
       <c r="A40" s="58" t="str">
@@ -41723,9 +41720,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J40" s="220"/>
-      <c r="K40" s="220"/>
-      <c r="L40" s="220"/>
+      <c r="J40" s="190"/>
+      <c r="K40" s="190"/>
+      <c r="L40" s="190"/>
     </row>
     <row r="41" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A41" s="58" t="str">
@@ -41787,11 +41784,11 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J42" s="218">
+      <c r="J42" s="188">
         <f>MAX(0,MIN(1,IF($J44 &lt;= 0.95, ROUND($J44,2), FLOOR((0.95+($J44-0.95)/5),0.01))))</f>
         <v>0.73</v>
       </c>
-      <c r="L42" s="218">
+      <c r="L42" s="188">
         <f>MAX(0,MIN(1,IF($L44 &lt;= 0.95, ROUND($L44,2), FLOOR((0.95+($L44-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -41822,8 +41819,8 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J43" s="219"/>
-      <c r="L43" s="219"/>
+      <c r="J43" s="189"/>
+      <c r="L43" s="189"/>
     </row>
     <row r="44" spans="1:12" ht="14.1" customHeight="1">
       <c r="A44" s="2"/>
@@ -41857,15 +41854,15 @@
       <c r="A45" s="2"/>
       <c r="B45" s="5"/>
       <c r="C45" s="43"/>
-      <c r="D45" s="193" t="s">
+      <c r="D45" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="193"/>
+      <c r="E45" s="192"/>
       <c r="F45" s="43"/>
-      <c r="G45" s="193" t="s">
+      <c r="G45" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="193"/>
+      <c r="H45" s="192"/>
     </row>
     <row r="46" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A46" s="1" t="s">
@@ -42073,34 +42070,6 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="L42:L43"/>
-    <mergeCell ref="J29:L31"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="L33:L34"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="J38:L40"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="J11:L13"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J20:L22"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G36:H36"/>
     <mergeCell ref="A7:B8"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="D6:E6"/>
@@ -42114,6 +42083,34 @@
     <mergeCell ref="J2:L8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G8:H8"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="J11:L13"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J20:L22"/>
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="J29:L31"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="L33:L34"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="J38:L40"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -42124,8 +42121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -42141,59 +42138,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A1" s="235" t="s">
+      <c r="A1" s="232" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="237"/>
+      <c r="B1" s="233"/>
+      <c r="C1" s="233"/>
+      <c r="D1" s="233"/>
+      <c r="E1" s="233"/>
+      <c r="F1" s="233"/>
+      <c r="G1" s="234"/>
     </row>
     <row r="2" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A2" s="230" t="s">
+      <c r="A2" s="221" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="231"/>
-      <c r="C2" s="231"/>
-      <c r="D2" s="231"/>
-      <c r="E2" s="231"/>
-      <c r="F2" s="231"/>
-      <c r="G2" s="232"/>
+      <c r="B2" s="222"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="223"/>
     </row>
     <row r="3" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A3" s="227" t="s">
+      <c r="A3" s="238" t="s">
         <v>930</v>
       </c>
-      <c r="B3" s="228"/>
-      <c r="C3" s="228"/>
-      <c r="D3" s="228"/>
-      <c r="E3" s="228"/>
-      <c r="F3" s="228"/>
-      <c r="G3" s="229"/>
+      <c r="B3" s="239"/>
+      <c r="C3" s="239"/>
+      <c r="D3" s="239"/>
+      <c r="E3" s="239"/>
+      <c r="F3" s="239"/>
+      <c r="G3" s="240"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A4" s="230" t="s">
+      <c r="A4" s="221" t="s">
         <v>438</v>
       </c>
-      <c r="B4" s="231"/>
-      <c r="C4" s="231"/>
-      <c r="D4" s="231"/>
-      <c r="E4" s="231"/>
-      <c r="F4" s="231"/>
-      <c r="G4" s="232"/>
+      <c r="B4" s="222"/>
+      <c r="C4" s="222"/>
+      <c r="D4" s="222"/>
+      <c r="E4" s="222"/>
+      <c r="F4" s="222"/>
+      <c r="G4" s="223"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A5" s="238" t="s">
+      <c r="A5" s="249" t="s">
         <v>580</v>
       </c>
-      <c r="B5" s="239"/>
-      <c r="C5" s="239"/>
-      <c r="D5" s="239"/>
-      <c r="E5" s="239"/>
-      <c r="F5" s="239"/>
-      <c r="G5" s="240"/>
+      <c r="B5" s="250"/>
+      <c r="C5" s="250"/>
+      <c r="D5" s="250"/>
+      <c r="E5" s="250"/>
+      <c r="F5" s="250"/>
+      <c r="G5" s="251"/>
     </row>
     <row r="6" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
       <c r="A6" s="2"/>
@@ -42226,10 +42223,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75">
-      <c r="A8" s="233" t="s">
+      <c r="A8" s="247" t="s">
         <v>718</v>
       </c>
-      <c r="B8" s="234"/>
+      <c r="B8" s="248"/>
       <c r="C8" s="65">
         <v>0</v>
       </c>
@@ -42246,10 +42243,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75">
-      <c r="A9" s="242" t="s">
+      <c r="A9" s="253" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="243"/>
+      <c r="B9" s="254"/>
       <c r="C9" s="92">
         <v>0</v>
       </c>
@@ -42266,10 +42263,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75">
-      <c r="A10" s="244" t="s">
+      <c r="A10" s="255" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="245"/>
+      <c r="B10" s="256"/>
       <c r="C10" s="69">
         <v>0</v>
       </c>
@@ -42286,10 +42283,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75">
-      <c r="A11" s="245" t="s">
+      <c r="A11" s="256" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="245"/>
+      <c r="B11" s="256"/>
       <c r="C11" s="69">
         <v>0</v>
       </c>
@@ -42306,10 +42303,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75">
-      <c r="A12" s="245" t="s">
+      <c r="A12" s="256" t="s">
         <v>716</v>
       </c>
-      <c r="B12" s="245"/>
+      <c r="B12" s="256"/>
       <c r="C12" s="69">
         <v>0</v>
       </c>
@@ -42326,10 +42323,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75">
-      <c r="A13" s="245" t="s">
+      <c r="A13" s="256" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="245"/>
+      <c r="B13" s="256"/>
       <c r="C13" s="69">
         <v>0</v>
       </c>
@@ -42346,10 +42343,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75">
-      <c r="A14" s="244" t="s">
+      <c r="A14" s="255" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="245"/>
+      <c r="B14" s="256"/>
       <c r="C14" s="69">
         <v>0</v>
       </c>
@@ -42366,10 +42363,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75">
-      <c r="A15" s="244" t="s">
+      <c r="A15" s="255" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="245"/>
+      <c r="B15" s="256"/>
       <c r="C15" s="69">
         <v>0</v>
       </c>
@@ -42386,10 +42383,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A16" s="246" t="s">
+      <c r="A16" s="230" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="247"/>
+      <c r="B16" s="231"/>
       <c r="C16" s="73">
         <v>0</v>
       </c>
@@ -42407,11 +42404,11 @@
     </row>
     <row r="17" spans="1:7" ht="14.1" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="241" t="s">
+      <c r="B17" s="252" t="s">
         <v>721</v>
       </c>
-      <c r="C17" s="241"/>
-      <c r="D17" s="241"/>
+      <c r="C17" s="252"/>
+      <c r="D17" s="252"/>
       <c r="E17" s="63">
         <f>SUM(E9:E16)</f>
         <v>0</v>
@@ -42432,527 +42429,559 @@
       <c r="A19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="235" t="s">
+      <c r="B19" s="232" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="236"/>
-      <c r="D19" s="236"/>
-      <c r="E19" s="236"/>
-      <c r="F19" s="236"/>
-      <c r="G19" s="237"/>
+      <c r="C19" s="233"/>
+      <c r="D19" s="233"/>
+      <c r="E19" s="233"/>
+      <c r="F19" s="233"/>
+      <c r="G19" s="234"/>
     </row>
     <row r="20" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="A20" s="10" t="s">
         <v>582</v>
       </c>
-      <c r="B20" s="230" t="s">
+      <c r="B20" s="221" t="s">
         <v>931</v>
       </c>
-      <c r="C20" s="231"/>
-      <c r="D20" s="231"/>
-      <c r="E20" s="231"/>
-      <c r="F20" s="231"/>
-      <c r="G20" s="232"/>
+      <c r="C20" s="222"/>
+      <c r="D20" s="222"/>
+      <c r="E20" s="222"/>
+      <c r="F20" s="222"/>
+      <c r="G20" s="223"/>
     </row>
     <row r="21" spans="1:7" ht="60" customHeight="1" thickBot="1">
       <c r="A21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="230" t="s">
+      <c r="B21" s="221" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="231"/>
-      <c r="D21" s="231"/>
-      <c r="E21" s="231"/>
-      <c r="F21" s="231"/>
-      <c r="G21" s="232"/>
+      <c r="C21" s="222"/>
+      <c r="D21" s="222"/>
+      <c r="E21" s="222"/>
+      <c r="F21" s="222"/>
+      <c r="G21" s="223"/>
     </row>
     <row r="22" spans="1:7" ht="45.95" customHeight="1" thickBot="1">
       <c r="A22" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="230" t="s">
+      <c r="B22" s="221" t="s">
         <v>917</v>
       </c>
-      <c r="C22" s="231"/>
-      <c r="D22" s="231"/>
-      <c r="E22" s="231"/>
-      <c r="F22" s="231"/>
-      <c r="G22" s="232"/>
+      <c r="C22" s="222"/>
+      <c r="D22" s="222"/>
+      <c r="E22" s="222"/>
+      <c r="F22" s="222"/>
+      <c r="G22" s="223"/>
     </row>
     <row r="23" spans="1:7" ht="32.1" customHeight="1">
       <c r="A23" s="98" t="s">
         <v>899</v>
       </c>
-      <c r="B23" s="227" t="s">
+      <c r="B23" s="238" t="s">
         <v>916</v>
       </c>
-      <c r="C23" s="228"/>
-      <c r="D23" s="228"/>
-      <c r="E23" s="228"/>
-      <c r="F23" s="228"/>
-      <c r="G23" s="229"/>
+      <c r="C23" s="239"/>
+      <c r="D23" s="239"/>
+      <c r="E23" s="239"/>
+      <c r="F23" s="239"/>
+      <c r="G23" s="240"/>
     </row>
     <row r="24" spans="1:7" ht="15.75">
       <c r="A24" s="99"/>
-      <c r="B24" s="221" t="s">
+      <c r="B24" s="257" t="s">
         <v>900</v>
       </c>
-      <c r="C24" s="222"/>
-      <c r="D24" s="223" t="s">
+      <c r="C24" s="258"/>
+      <c r="D24" s="260" t="s">
         <v>901</v>
       </c>
-      <c r="E24" s="223"/>
-      <c r="F24" s="223"/>
-      <c r="G24" s="224"/>
+      <c r="E24" s="260"/>
+      <c r="F24" s="260"/>
+      <c r="G24" s="261"/>
     </row>
     <row r="25" spans="1:7" ht="15.75">
       <c r="A25" s="99"/>
-      <c r="B25" s="221" t="s">
+      <c r="B25" s="257" t="s">
         <v>902</v>
       </c>
-      <c r="C25" s="222"/>
-      <c r="D25" s="223" t="s">
+      <c r="C25" s="258"/>
+      <c r="D25" s="260" t="s">
         <v>903</v>
       </c>
-      <c r="E25" s="223"/>
-      <c r="F25" s="223"/>
-      <c r="G25" s="224"/>
+      <c r="E25" s="260"/>
+      <c r="F25" s="260"/>
+      <c r="G25" s="261"/>
     </row>
     <row r="26" spans="1:7" ht="15.75">
       <c r="A26" s="99"/>
-      <c r="B26" s="221" t="s">
+      <c r="B26" s="257" t="s">
         <v>904</v>
       </c>
-      <c r="C26" s="222"/>
-      <c r="D26" s="223" t="s">
+      <c r="C26" s="258"/>
+      <c r="D26" s="260" t="s">
         <v>905</v>
       </c>
-      <c r="E26" s="223"/>
-      <c r="F26" s="223"/>
-      <c r="G26" s="224"/>
+      <c r="E26" s="260"/>
+      <c r="F26" s="260"/>
+      <c r="G26" s="261"/>
     </row>
     <row r="27" spans="1:7" ht="15.75">
       <c r="A27" s="99"/>
-      <c r="B27" s="221" t="s">
+      <c r="B27" s="257" t="s">
         <v>906</v>
       </c>
-      <c r="C27" s="222"/>
+      <c r="C27" s="258"/>
       <c r="D27" s="225" t="s">
         <v>907</v>
       </c>
       <c r="E27" s="225"/>
       <c r="F27" s="225"/>
-      <c r="G27" s="226"/>
+      <c r="G27" s="259"/>
     </row>
     <row r="28" spans="1:7" ht="15.75">
       <c r="A28" s="99"/>
-      <c r="B28" s="221" t="s">
+      <c r="B28" s="257" t="s">
         <v>908</v>
       </c>
-      <c r="C28" s="222"/>
-      <c r="D28" s="223" t="s">
+      <c r="C28" s="258"/>
+      <c r="D28" s="260" t="s">
         <v>909</v>
       </c>
-      <c r="E28" s="223"/>
-      <c r="F28" s="223"/>
-      <c r="G28" s="224"/>
+      <c r="E28" s="260"/>
+      <c r="F28" s="260"/>
+      <c r="G28" s="261"/>
     </row>
     <row r="29" spans="1:7" ht="15.75">
       <c r="A29" s="99"/>
-      <c r="B29" s="221" t="s">
+      <c r="B29" s="257" t="s">
         <v>910</v>
       </c>
-      <c r="C29" s="222"/>
+      <c r="C29" s="258"/>
       <c r="D29" s="225" t="s">
         <v>911</v>
       </c>
       <c r="E29" s="225"/>
       <c r="F29" s="225"/>
-      <c r="G29" s="226"/>
+      <c r="G29" s="259"/>
     </row>
     <row r="30" spans="1:7" ht="15.75">
       <c r="A30" s="99"/>
-      <c r="B30" s="221" t="s">
+      <c r="B30" s="257" t="s">
         <v>914</v>
       </c>
-      <c r="C30" s="222"/>
-      <c r="D30" s="223" t="s">
+      <c r="C30" s="258"/>
+      <c r="D30" s="260" t="s">
         <v>915</v>
       </c>
-      <c r="E30" s="223"/>
-      <c r="F30" s="223"/>
-      <c r="G30" s="224"/>
+      <c r="E30" s="260"/>
+      <c r="F30" s="260"/>
+      <c r="G30" s="261"/>
     </row>
     <row r="31" spans="1:7" ht="15.75">
       <c r="A31" s="99"/>
-      <c r="B31" s="221" t="s">
+      <c r="B31" s="257" t="s">
         <v>912</v>
       </c>
-      <c r="C31" s="222"/>
+      <c r="C31" s="258"/>
       <c r="D31" s="225" t="s">
         <v>913</v>
       </c>
       <c r="E31" s="225"/>
       <c r="F31" s="225"/>
-      <c r="G31" s="226"/>
+      <c r="G31" s="259"/>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickBot="1">
       <c r="A32" s="99"/>
-      <c r="B32" s="221" t="s">
+      <c r="B32" s="257" t="s">
         <v>928</v>
       </c>
-      <c r="C32" s="222"/>
+      <c r="C32" s="258"/>
       <c r="D32" s="225" t="s">
         <v>929</v>
       </c>
       <c r="E32" s="225"/>
       <c r="F32" s="225"/>
-      <c r="G32" s="226"/>
+      <c r="G32" s="259"/>
     </row>
     <row r="33" spans="1:7" ht="15.75">
       <c r="A33" s="98" t="s">
         <v>918</v>
       </c>
-      <c r="B33" s="227" t="s">
+      <c r="B33" s="238" t="s">
         <v>919</v>
       </c>
-      <c r="C33" s="228"/>
-      <c r="D33" s="228"/>
-      <c r="E33" s="228"/>
-      <c r="F33" s="228"/>
-      <c r="G33" s="229"/>
+      <c r="C33" s="239"/>
+      <c r="D33" s="239"/>
+      <c r="E33" s="239"/>
+      <c r="F33" s="239"/>
+      <c r="G33" s="240"/>
     </row>
     <row r="34" spans="1:7" ht="15.75">
       <c r="A34" s="99"/>
-      <c r="B34" s="221" t="s">
+      <c r="B34" s="257" t="s">
         <v>920</v>
       </c>
-      <c r="C34" s="222"/>
-      <c r="D34" s="223" t="s">
+      <c r="C34" s="258"/>
+      <c r="D34" s="260" t="s">
         <v>925</v>
       </c>
-      <c r="E34" s="223"/>
-      <c r="F34" s="223"/>
-      <c r="G34" s="224"/>
+      <c r="E34" s="260"/>
+      <c r="F34" s="260"/>
+      <c r="G34" s="261"/>
     </row>
     <row r="35" spans="1:7" ht="15.75">
       <c r="A35" s="99"/>
-      <c r="B35" s="221" t="s">
+      <c r="B35" s="257" t="s">
         <v>921</v>
       </c>
-      <c r="C35" s="222"/>
-      <c r="D35" s="223" t="s">
+      <c r="C35" s="258"/>
+      <c r="D35" s="260" t="s">
         <v>926</v>
       </c>
-      <c r="E35" s="223"/>
-      <c r="F35" s="223"/>
-      <c r="G35" s="224"/>
+      <c r="E35" s="260"/>
+      <c r="F35" s="260"/>
+      <c r="G35" s="261"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" thickBot="1">
       <c r="A36" s="99"/>
-      <c r="B36" s="221" t="s">
+      <c r="B36" s="257" t="s">
         <v>922</v>
       </c>
-      <c r="C36" s="222"/>
-      <c r="D36" s="223" t="s">
+      <c r="C36" s="258"/>
+      <c r="D36" s="260" t="s">
         <v>927</v>
       </c>
-      <c r="E36" s="223"/>
-      <c r="F36" s="223"/>
-      <c r="G36" s="224"/>
+      <c r="E36" s="260"/>
+      <c r="F36" s="260"/>
+      <c r="G36" s="261"/>
     </row>
     <row r="37" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="A37" s="98" t="s">
         <v>923</v>
       </c>
-      <c r="B37" s="227" t="s">
+      <c r="B37" s="238" t="s">
         <v>924</v>
       </c>
-      <c r="C37" s="228"/>
-      <c r="D37" s="228"/>
-      <c r="E37" s="228"/>
-      <c r="F37" s="228"/>
-      <c r="G37" s="229"/>
+      <c r="C37" s="239"/>
+      <c r="D37" s="239"/>
+      <c r="E37" s="239"/>
+      <c r="F37" s="239"/>
+      <c r="G37" s="240"/>
     </row>
     <row r="38" spans="1:7" ht="29.1" customHeight="1">
-      <c r="A38" s="248" t="s">
+      <c r="A38" s="235" t="s">
         <v>517</v>
       </c>
-      <c r="B38" s="227" t="s">
+      <c r="B38" s="238" t="s">
         <v>490</v>
       </c>
-      <c r="C38" s="228"/>
-      <c r="D38" s="228"/>
-      <c r="E38" s="228"/>
-      <c r="F38" s="228"/>
-      <c r="G38" s="229"/>
+      <c r="C38" s="239"/>
+      <c r="D38" s="239"/>
+      <c r="E38" s="239"/>
+      <c r="F38" s="239"/>
+      <c r="G38" s="240"/>
     </row>
     <row r="39" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A39" s="249"/>
-      <c r="B39" s="251"/>
-      <c r="C39" s="252"/>
-      <c r="D39" s="252"/>
-      <c r="E39" s="252"/>
-      <c r="F39" s="252"/>
-      <c r="G39" s="253"/>
+      <c r="A39" s="236"/>
+      <c r="B39" s="241"/>
+      <c r="C39" s="242"/>
+      <c r="D39" s="242"/>
+      <c r="E39" s="242"/>
+      <c r="F39" s="242"/>
+      <c r="G39" s="243"/>
     </row>
     <row r="40" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A40" s="249"/>
-      <c r="B40" s="254" t="s">
+      <c r="A40" s="236"/>
+      <c r="B40" s="244" t="s">
         <v>491</v>
       </c>
-      <c r="C40" s="255"/>
-      <c r="D40" s="255"/>
-      <c r="E40" s="255"/>
-      <c r="F40" s="255"/>
-      <c r="G40" s="256"/>
+      <c r="C40" s="245"/>
+      <c r="D40" s="245"/>
+      <c r="E40" s="245"/>
+      <c r="F40" s="245"/>
+      <c r="G40" s="246"/>
     </row>
     <row r="41" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A41" s="249"/>
-      <c r="B41" s="257" t="s">
+      <c r="A41" s="236"/>
+      <c r="B41" s="224" t="s">
         <v>492</v>
       </c>
       <c r="C41" s="225"/>
       <c r="D41" s="225"/>
       <c r="E41" s="225"/>
       <c r="F41" s="225"/>
-      <c r="G41" s="258"/>
+      <c r="G41" s="226"/>
     </row>
     <row r="42" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A42" s="249"/>
-      <c r="B42" s="251"/>
-      <c r="C42" s="252"/>
-      <c r="D42" s="252"/>
-      <c r="E42" s="252"/>
-      <c r="F42" s="252"/>
-      <c r="G42" s="253"/>
+      <c r="A42" s="236"/>
+      <c r="B42" s="241"/>
+      <c r="C42" s="242"/>
+      <c r="D42" s="242"/>
+      <c r="E42" s="242"/>
+      <c r="F42" s="242"/>
+      <c r="G42" s="243"/>
     </row>
     <row r="43" spans="1:7" ht="42.95" customHeight="1">
-      <c r="A43" s="249"/>
-      <c r="B43" s="257" t="s">
+      <c r="A43" s="236"/>
+      <c r="B43" s="224" t="s">
         <v>493</v>
       </c>
       <c r="C43" s="225"/>
       <c r="D43" s="225"/>
       <c r="E43" s="225"/>
       <c r="F43" s="225"/>
-      <c r="G43" s="258"/>
+      <c r="G43" s="226"/>
     </row>
     <row r="44" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A44" s="249"/>
-      <c r="B44" s="251"/>
-      <c r="C44" s="252"/>
-      <c r="D44" s="252"/>
-      <c r="E44" s="252"/>
-      <c r="F44" s="252"/>
-      <c r="G44" s="253"/>
+      <c r="A44" s="236"/>
+      <c r="B44" s="241"/>
+      <c r="C44" s="242"/>
+      <c r="D44" s="242"/>
+      <c r="E44" s="242"/>
+      <c r="F44" s="242"/>
+      <c r="G44" s="243"/>
     </row>
     <row r="45" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A45" s="249"/>
-      <c r="B45" s="257" t="s">
+      <c r="A45" s="236"/>
+      <c r="B45" s="224" t="s">
         <v>494</v>
       </c>
       <c r="C45" s="225"/>
       <c r="D45" s="225"/>
       <c r="E45" s="225"/>
       <c r="F45" s="225"/>
-      <c r="G45" s="258"/>
+      <c r="G45" s="226"/>
     </row>
     <row r="46" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A46" s="249"/>
-      <c r="B46" s="257" t="s">
+      <c r="A46" s="236"/>
+      <c r="B46" s="224" t="s">
         <v>495</v>
       </c>
       <c r="C46" s="225"/>
       <c r="D46" s="225"/>
       <c r="E46" s="225"/>
       <c r="F46" s="225"/>
-      <c r="G46" s="258"/>
+      <c r="G46" s="226"/>
     </row>
     <row r="47" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A47" s="249"/>
-      <c r="B47" s="257" t="s">
+      <c r="A47" s="236"/>
+      <c r="B47" s="224" t="s">
         <v>496</v>
       </c>
       <c r="C47" s="225"/>
       <c r="D47" s="225"/>
       <c r="E47" s="225"/>
       <c r="F47" s="225"/>
-      <c r="G47" s="258"/>
+      <c r="G47" s="226"/>
     </row>
     <row r="48" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A48" s="249"/>
-      <c r="B48" s="257" t="s">
+      <c r="A48" s="236"/>
+      <c r="B48" s="224" t="s">
         <v>497</v>
       </c>
       <c r="C48" s="225"/>
       <c r="D48" s="225"/>
       <c r="E48" s="225"/>
       <c r="F48" s="225"/>
-      <c r="G48" s="258"/>
+      <c r="G48" s="226"/>
     </row>
     <row r="49" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A49" s="249"/>
-      <c r="B49" s="257" t="s">
+      <c r="A49" s="236"/>
+      <c r="B49" s="224" t="s">
         <v>498</v>
       </c>
       <c r="C49" s="225"/>
       <c r="D49" s="225"/>
       <c r="E49" s="225"/>
       <c r="F49" s="225"/>
-      <c r="G49" s="258"/>
+      <c r="G49" s="226"/>
     </row>
     <row r="50" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A50" s="249"/>
-      <c r="B50" s="257" t="s">
+      <c r="A50" s="236"/>
+      <c r="B50" s="224" t="s">
         <v>499</v>
       </c>
       <c r="C50" s="225"/>
       <c r="D50" s="225"/>
       <c r="E50" s="225"/>
       <c r="F50" s="225"/>
-      <c r="G50" s="258"/>
+      <c r="G50" s="226"/>
     </row>
     <row r="51" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A51" s="249"/>
-      <c r="B51" s="257" t="s">
+      <c r="A51" s="236"/>
+      <c r="B51" s="224" t="s">
         <v>500</v>
       </c>
       <c r="C51" s="225"/>
       <c r="D51" s="225"/>
       <c r="E51" s="225"/>
       <c r="F51" s="225"/>
-      <c r="G51" s="258"/>
+      <c r="G51" s="226"/>
     </row>
     <row r="52" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A52" s="250"/>
-      <c r="B52" s="259" t="s">
+      <c r="A52" s="237"/>
+      <c r="B52" s="227" t="s">
         <v>501</v>
       </c>
-      <c r="C52" s="260"/>
-      <c r="D52" s="260"/>
-      <c r="E52" s="260"/>
-      <c r="F52" s="260"/>
-      <c r="G52" s="261"/>
+      <c r="C52" s="228"/>
+      <c r="D52" s="228"/>
+      <c r="E52" s="228"/>
+      <c r="F52" s="228"/>
+      <c r="G52" s="229"/>
     </row>
     <row r="53" spans="1:7" ht="57.95" customHeight="1" thickBot="1">
       <c r="A53" s="10" t="s">
         <v>516</v>
       </c>
-      <c r="B53" s="230" t="s">
+      <c r="B53" s="221" t="s">
         <v>581</v>
       </c>
-      <c r="C53" s="231"/>
-      <c r="D53" s="231"/>
-      <c r="E53" s="231"/>
-      <c r="F53" s="231"/>
-      <c r="G53" s="232"/>
+      <c r="C53" s="222"/>
+      <c r="D53" s="222"/>
+      <c r="E53" s="222"/>
+      <c r="F53" s="222"/>
+      <c r="G53" s="223"/>
     </row>
     <row r="54" spans="1:7" ht="57.95" customHeight="1" thickBot="1">
       <c r="A54" s="10" t="s">
         <v>515</v>
       </c>
-      <c r="B54" s="230" t="s">
+      <c r="B54" s="221" t="s">
         <v>502</v>
       </c>
-      <c r="C54" s="231"/>
-      <c r="D54" s="231"/>
-      <c r="E54" s="231"/>
-      <c r="F54" s="231"/>
-      <c r="G54" s="232"/>
+      <c r="C54" s="222"/>
+      <c r="D54" s="222"/>
+      <c r="E54" s="222"/>
+      <c r="F54" s="222"/>
+      <c r="G54" s="223"/>
     </row>
     <row r="55" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A55" s="10" t="s">
         <v>514</v>
       </c>
-      <c r="B55" s="230" t="s">
+      <c r="B55" s="221" t="s">
         <v>503</v>
       </c>
-      <c r="C55" s="231"/>
-      <c r="D55" s="231"/>
-      <c r="E55" s="231"/>
-      <c r="F55" s="231"/>
-      <c r="G55" s="232"/>
+      <c r="C55" s="222"/>
+      <c r="D55" s="222"/>
+      <c r="E55" s="222"/>
+      <c r="F55" s="222"/>
+      <c r="G55" s="223"/>
     </row>
     <row r="56" spans="1:7" ht="42.95" customHeight="1" thickBot="1">
       <c r="A56" s="11" t="s">
         <v>508</v>
       </c>
-      <c r="B56" s="230" t="s">
+      <c r="B56" s="221" t="s">
         <v>504</v>
       </c>
-      <c r="C56" s="231"/>
-      <c r="D56" s="231"/>
-      <c r="E56" s="231"/>
-      <c r="F56" s="231"/>
-      <c r="G56" s="232"/>
+      <c r="C56" s="222"/>
+      <c r="D56" s="222"/>
+      <c r="E56" s="222"/>
+      <c r="F56" s="222"/>
+      <c r="G56" s="223"/>
     </row>
     <row r="57" spans="1:7" ht="29.1" customHeight="1" thickBot="1">
       <c r="A57" s="10" t="s">
         <v>513</v>
       </c>
-      <c r="B57" s="230" t="s">
+      <c r="B57" s="221" t="s">
         <v>505</v>
       </c>
-      <c r="C57" s="231"/>
-      <c r="D57" s="231"/>
-      <c r="E57" s="231"/>
-      <c r="F57" s="231"/>
-      <c r="G57" s="232"/>
+      <c r="C57" s="222"/>
+      <c r="D57" s="222"/>
+      <c r="E57" s="222"/>
+      <c r="F57" s="222"/>
+      <c r="G57" s="223"/>
     </row>
     <row r="58" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A58" s="10" t="s">
         <v>512</v>
       </c>
-      <c r="B58" s="230" t="s">
+      <c r="B58" s="221" t="s">
         <v>506</v>
       </c>
-      <c r="C58" s="231"/>
-      <c r="D58" s="231"/>
-      <c r="E58" s="231"/>
-      <c r="F58" s="231"/>
-      <c r="G58" s="232"/>
+      <c r="C58" s="222"/>
+      <c r="D58" s="222"/>
+      <c r="E58" s="222"/>
+      <c r="F58" s="222"/>
+      <c r="G58" s="223"/>
     </row>
     <row r="59" spans="1:7" ht="42.95" customHeight="1" thickBot="1">
       <c r="A59" s="11" t="s">
         <v>509</v>
       </c>
-      <c r="B59" s="230" t="s">
+      <c r="B59" s="221" t="s">
         <v>510</v>
       </c>
-      <c r="C59" s="231"/>
-      <c r="D59" s="231"/>
-      <c r="E59" s="231"/>
-      <c r="F59" s="231"/>
-      <c r="G59" s="232"/>
+      <c r="C59" s="222"/>
+      <c r="D59" s="222"/>
+      <c r="E59" s="222"/>
+      <c r="F59" s="222"/>
+      <c r="G59" s="223"/>
     </row>
     <row r="60" spans="1:7" ht="29.1" customHeight="1" thickBot="1">
       <c r="A60" s="10" t="s">
         <v>511</v>
       </c>
-      <c r="B60" s="230" t="s">
+      <c r="B60" s="221" t="s">
         <v>507</v>
       </c>
-      <c r="C60" s="231"/>
-      <c r="D60" s="231"/>
-      <c r="E60" s="231"/>
-      <c r="F60" s="231"/>
-      <c r="G60" s="232"/>
+      <c r="C60" s="222"/>
+      <c r="D60" s="222"/>
+      <c r="E60" s="222"/>
+      <c r="F60" s="222"/>
+      <c r="G60" s="223"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:G59"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B53:G53"/>
-    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B20:G20"/>
@@ -42969,49 +42998,17 @@
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="B48:G48"/>
     <mergeCell ref="B49:G49"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:G36"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:G35"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B59:G59"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -43022,8 +43019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -43099,7 +43096,7 @@
       </c>
       <c r="F3" s="14">
         <f>SUMPRODUCT(($A$10:$A$247="Basic")*(F$10:F$247="Missing"))+0.5*SUMPRODUCT(($A$10:$A$247="Basic")*(F$10:F$247="Partial"))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="11" t="str">
         <f>"Basic "&amp;$G$1&amp;"s "&amp;A3</f>
@@ -43235,10 +43232,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="232" t="s">
         <v>485</v>
       </c>
-      <c r="B10" s="237"/>
+      <c r="B10" s="234"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -43273,7 +43270,7 @@
         <v>58</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="39" thickBot="1">
@@ -43294,7 +43291,7 @@
         <v>58</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="16.5" thickBot="1">
@@ -43315,7 +43312,7 @@
         <v>58</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="16.5" thickBot="1">
@@ -43336,7 +43333,7 @@
         <v>58</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="26.25" thickBot="1">
@@ -43357,7 +43354,7 @@
         <v>58</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="39" thickBot="1">
@@ -43378,7 +43375,7 @@
         <v>58</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="39" thickBot="1">
@@ -43399,7 +43396,7 @@
         <v>58</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="90" thickBot="1">
@@ -43420,7 +43417,7 @@
         <v>58</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="39" thickBot="1">
@@ -43441,7 +43438,7 @@
         <v>58</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="39" thickBot="1">
@@ -43462,7 +43459,7 @@
         <v>58</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="64.5" thickBot="1">
@@ -43483,7 +43480,7 @@
         <v>58</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="26.25" thickBot="1">
@@ -43504,14 +43501,14 @@
         <v>58</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A23" s="235" t="s">
+      <c r="A23" s="232" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="237"/>
+      <c r="B23" s="234"/>
       <c r="C23" s="4" t="s">
         <v>63</v>
       </c>
@@ -43546,7 +43543,7 @@
         <v>58</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="64.5" thickBot="1">
@@ -43567,7 +43564,7 @@
         <v>58</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="39" thickBot="1">
@@ -43588,7 +43585,7 @@
         <v>58</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="77.25" thickBot="1">
@@ -43609,7 +43606,7 @@
         <v>58</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="39" thickBot="1">
@@ -43630,7 +43627,7 @@
         <v>58</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="99" customHeight="1" thickBot="1">
@@ -43651,7 +43648,7 @@
         <v>58</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="51.75" thickBot="1">
@@ -43672,7 +43669,7 @@
         <v>58</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="64.5" thickBot="1">
@@ -43693,7 +43690,7 @@
         <v>58</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="141" thickBot="1">
@@ -43714,7 +43711,7 @@
         <v>58</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="39" thickBot="1">
@@ -43735,7 +43732,7 @@
         <v>58</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="64.5" thickBot="1">
@@ -43756,7 +43753,7 @@
         <v>58</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="16.5" thickBot="1">
@@ -43777,7 +43774,7 @@
         <v>58</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="39" thickBot="1">
@@ -43798,7 +43795,7 @@
         <v>58</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="90" thickBot="1">
@@ -43819,7 +43816,7 @@
         <v>58</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="39" thickBot="1">
@@ -43840,14 +43837,14 @@
         <v>58</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A39" s="235" t="s">
+      <c r="A39" s="232" t="s">
         <v>524</v>
       </c>
-      <c r="B39" s="237"/>
+      <c r="B39" s="234"/>
       <c r="C39" s="4" t="s">
         <v>63</v>
       </c>
@@ -43882,7 +43879,7 @@
         <v>58</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="64.5" thickBot="1">
@@ -43903,7 +43900,7 @@
         <v>58</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="26.25" thickBot="1">
@@ -43924,7 +43921,7 @@
         <v>58</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="26.25" thickBot="1">
@@ -43945,7 +43942,7 @@
         <v>58</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="128.25" thickBot="1">
@@ -43963,17 +43960,17 @@
         <v>58</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A45" s="235" t="s">
+      <c r="A45" s="232" t="s">
         <v>529</v>
       </c>
-      <c r="B45" s="237"/>
+      <c r="B45" s="234"/>
       <c r="C45" s="4" t="s">
         <v>63</v>
       </c>
@@ -44008,7 +44005,7 @@
         <v>58</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="16.5" thickBot="1">
@@ -44029,7 +44026,7 @@
         <v>58</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="90" thickBot="1">
@@ -44050,7 +44047,7 @@
         <v>58</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="39" thickBot="1">
@@ -44064,7 +44061,7 @@
         <v>769</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>61</v>
@@ -44073,7 +44070,7 @@
         <v>61</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="26.25" thickBot="1">
@@ -44094,7 +44091,7 @@
         <v>54</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="51.75" thickBot="1">
@@ -44115,14 +44112,14 @@
         <v>54</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A52" s="235" t="s">
+      <c r="A52" s="232" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="237"/>
+      <c r="B52" s="234"/>
       <c r="C52" s="4" t="s">
         <v>63</v>
       </c>
@@ -44157,7 +44154,7 @@
         <v>58</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="39" thickBot="1">
@@ -44178,7 +44175,7 @@
         <v>58</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="77.25" thickBot="1">
@@ -44199,7 +44196,7 @@
         <v>58</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="77.25" thickBot="1">
@@ -44220,7 +44217,7 @@
         <v>58</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="26.25" thickBot="1">
@@ -44234,7 +44231,7 @@
         <v>107</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>61</v>
@@ -44243,7 +44240,7 @@
         <v>61</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="51.75" thickBot="1">
@@ -44264,7 +44261,7 @@
         <v>58</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="26.25" thickBot="1">
@@ -44285,7 +44282,7 @@
         <v>58</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="77.25" thickBot="1">
@@ -44306,14 +44303,14 @@
         <v>54</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A61" s="235" t="s">
+      <c r="A61" s="232" t="s">
         <v>111</v>
       </c>
-      <c r="B61" s="237"/>
+      <c r="B61" s="234"/>
       <c r="C61" s="4" t="s">
         <v>63</v>
       </c>
@@ -44348,7 +44345,7 @@
         <v>58</v>
       </c>
       <c r="G62" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="39" thickBot="1">
@@ -44369,7 +44366,7 @@
         <v>58</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="16.5" thickBot="1">
@@ -44390,7 +44387,7 @@
         <v>58</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="16.5" thickBot="1">
@@ -44411,14 +44408,14 @@
         <v>58</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A66" s="235" t="s">
+      <c r="A66" s="232" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="237"/>
+      <c r="B66" s="234"/>
       <c r="C66" s="4" t="s">
         <v>63</v>
       </c>
@@ -44453,7 +44450,7 @@
         <v>58</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="16.5" thickBot="1">
@@ -44474,7 +44471,7 @@
         <v>58</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="26.25" thickBot="1">
@@ -44495,7 +44492,7 @@
         <v>58</v>
       </c>
       <c r="G69" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="39" thickBot="1">
@@ -44516,7 +44513,7 @@
         <v>58</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="51.75" thickBot="1">
@@ -44537,7 +44534,7 @@
         <v>58</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="39" thickBot="1">
@@ -44558,7 +44555,7 @@
         <v>58</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="64.5" thickBot="1">
@@ -44579,7 +44576,7 @@
         <v>58</v>
       </c>
       <c r="G73" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="51.75" thickBot="1">
@@ -44600,7 +44597,7 @@
         <v>58</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="51.75" thickBot="1">
@@ -44621,7 +44618,7 @@
         <v>58</v>
       </c>
       <c r="G75" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="39" thickBot="1">
@@ -44642,7 +44639,7 @@
         <v>58</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="77.25" thickBot="1">
@@ -44665,7 +44662,7 @@
         <v>58</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="115.5" thickBot="1">
@@ -44688,7 +44685,7 @@
         <v>58</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="51.75" thickBot="1">
@@ -44711,7 +44708,7 @@
         <v>58</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="39" thickBot="1">
@@ -44725,7 +44722,7 @@
         <v>749</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>58</v>
@@ -44734,14 +44731,14 @@
         <v>58</v>
       </c>
       <c r="G80" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A81" s="235" t="s">
+      <c r="A81" s="232" t="s">
         <v>133</v>
       </c>
-      <c r="B81" s="237"/>
+      <c r="B81" s="234"/>
       <c r="C81" s="4" t="s">
         <v>63</v>
       </c>
@@ -44776,7 +44773,7 @@
         <v>58</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="16.5" thickBot="1">
@@ -44797,7 +44794,7 @@
         <v>58</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="26.25" thickBot="1">
@@ -44818,7 +44815,7 @@
         <v>58</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="26.25" thickBot="1">
@@ -44839,7 +44836,7 @@
         <v>58</v>
       </c>
       <c r="G85" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="51.75" thickBot="1">
@@ -44862,7 +44859,7 @@
         <v>58</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="39" thickBot="1">
@@ -44883,14 +44880,14 @@
         <v>54</v>
       </c>
       <c r="G87" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A88" s="235" t="s">
+      <c r="A88" s="232" t="s">
         <v>558</v>
       </c>
-      <c r="B88" s="237"/>
+      <c r="B88" s="234"/>
       <c r="C88" s="4" t="s">
         <v>63</v>
       </c>
@@ -44927,7 +44924,7 @@
         <v>58</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="26.25" thickBot="1">
@@ -44950,7 +44947,7 @@
         <v>58</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="26.25" thickBot="1">
@@ -44971,7 +44968,7 @@
         <v>54</v>
       </c>
       <c r="G91" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="26.25" thickBot="1">
@@ -44992,7 +44989,7 @@
         <v>54</v>
       </c>
       <c r="G92" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="26.25" thickBot="1">
@@ -45013,14 +45010,14 @@
         <v>54</v>
       </c>
       <c r="G93" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A94" s="235" t="s">
+      <c r="A94" s="232" t="s">
         <v>156</v>
       </c>
-      <c r="B94" s="237"/>
+      <c r="B94" s="234"/>
       <c r="C94" s="4" t="s">
         <v>63</v>
       </c>
@@ -45055,7 +45052,7 @@
         <v>58</v>
       </c>
       <c r="G95" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="16.5" thickBot="1">
@@ -45076,7 +45073,7 @@
         <v>58</v>
       </c>
       <c r="G96" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="111.95" customHeight="1" thickBot="1">
@@ -45097,14 +45094,14 @@
         <v>54</v>
       </c>
       <c r="G97" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A98" s="235" t="s">
+      <c r="A98" s="232" t="s">
         <v>150</v>
       </c>
-      <c r="B98" s="237"/>
+      <c r="B98" s="234"/>
       <c r="C98" s="4" t="s">
         <v>63</v>
       </c>
@@ -45139,7 +45136,7 @@
         <v>58</v>
       </c>
       <c r="G99" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="39" thickBot="1">
@@ -45160,7 +45157,7 @@
         <v>58</v>
       </c>
       <c r="G100" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="26.25" thickBot="1">
@@ -45181,14 +45178,14 @@
         <v>58</v>
       </c>
       <c r="G101" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A102" s="235" t="s">
+      <c r="A102" s="232" t="s">
         <v>547</v>
       </c>
-      <c r="B102" s="237"/>
+      <c r="B102" s="234"/>
       <c r="C102" s="4" t="s">
         <v>63</v>
       </c>
@@ -45223,7 +45220,7 @@
         <v>58</v>
       </c>
       <c r="G103" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="26.25" thickBot="1">
@@ -45244,7 +45241,7 @@
         <v>58</v>
       </c>
       <c r="G104" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="51.75" thickBot="1">
@@ -45267,7 +45264,7 @@
         <v>58</v>
       </c>
       <c r="G105" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="39" thickBot="1">
@@ -45288,14 +45285,14 @@
         <v>54</v>
       </c>
       <c r="G106" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A107" s="235" t="s">
+      <c r="A107" s="232" t="s">
         <v>140</v>
       </c>
-      <c r="B107" s="237"/>
+      <c r="B107" s="234"/>
       <c r="C107" s="4" t="s">
         <v>63</v>
       </c>
@@ -45330,7 +45327,7 @@
         <v>58</v>
       </c>
       <c r="G108" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="16.5" thickBot="1">
@@ -45351,7 +45348,7 @@
         <v>58</v>
       </c>
       <c r="G109" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="51.75" thickBot="1">
@@ -45372,7 +45369,7 @@
         <v>58</v>
       </c>
       <c r="G110" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="51.75" thickBot="1">
@@ -45393,7 +45390,7 @@
         <v>58</v>
       </c>
       <c r="G111" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="39" thickBot="1">
@@ -45414,7 +45411,7 @@
         <v>58</v>
       </c>
       <c r="G112" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="26.25" thickBot="1">
@@ -45435,7 +45432,7 @@
         <v>58</v>
       </c>
       <c r="G113" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="26.25" thickBot="1">
@@ -45456,14 +45453,14 @@
         <v>58</v>
       </c>
       <c r="G114" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A115" s="235" t="s">
+      <c r="A115" s="232" t="s">
         <v>161</v>
       </c>
-      <c r="B115" s="237"/>
+      <c r="B115" s="234"/>
       <c r="C115" s="4" t="s">
         <v>453</v>
       </c>
@@ -45498,7 +45495,7 @@
         <v>61</v>
       </c>
       <c r="G116" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="26.25" thickBot="1">
@@ -45518,7 +45515,9 @@
       <c r="F117" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G117" s="11"/>
+      <c r="G117" s="11" t="s">
+        <v>979</v>
+      </c>
     </row>
     <row r="118" spans="1:7" ht="16.5" thickBot="1">
       <c r="A118" s="16" t="s">
@@ -45537,7 +45536,9 @@
       <c r="F118" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G118" s="11"/>
+      <c r="G118" s="11" t="s">
+        <v>979</v>
+      </c>
     </row>
     <row r="119" spans="1:7" ht="26.25" thickBot="1">
       <c r="A119" s="18" t="s">
@@ -45556,7 +45557,9 @@
       <c r="F119" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G119" s="11"/>
+      <c r="G119" s="11" t="s">
+        <v>979</v>
+      </c>
     </row>
     <row r="120" spans="1:7" ht="16.5" thickBot="1">
       <c r="A120" s="17" t="s">
@@ -45575,7 +45578,9 @@
       <c r="F120" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G120" s="11"/>
+      <c r="G120" s="11" t="s">
+        <v>979</v>
+      </c>
     </row>
     <row r="121" spans="1:7" ht="26.25" thickBot="1">
       <c r="A121" s="17" t="s">
@@ -45594,7 +45599,9 @@
       <c r="F121" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G121" s="11"/>
+      <c r="G121" s="11" t="s">
+        <v>979</v>
+      </c>
     </row>
     <row r="122" spans="1:7" ht="26.25" thickBot="1">
       <c r="A122" s="19" t="s">
@@ -45613,7 +45620,9 @@
       <c r="F122" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G122" s="11"/>
+      <c r="G122" s="11" t="s">
+        <v>979</v>
+      </c>
     </row>
     <row r="123" spans="1:7" ht="16.5" thickBot="1">
       <c r="A123" s="17" t="s">
@@ -45632,18 +45641,12 @@
       <c r="F123" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G123" s="11"/>
+      <c r="G123" s="11" t="s">
+        <v>979</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A88:B88"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="C2:D9"/>
@@ -45653,6 +45656,14 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A88:B88"/>
   </mergeCells>
   <conditionalFormatting sqref="A11:A18 A107:A109 A81:A85 A115:A248 A52:A57 A40 A33:A37 A42:A43 A112 A94:A100 A61:A69 A59 A20:A29">
     <cfRule type="beginsWith" dxfId="2509" priority="1308" stopIfTrue="1" operator="beginsWith" text="Exceptional">
@@ -48174,8 +48185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -48313,7 +48324,7 @@
       <c r="D6" s="265"/>
       <c r="E6" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Advanced")*(E$10:E$209="Missing"))+0.5*SUMPRODUCT(($A$10:$A$209="Advanced")*(E$10:E$209="Partial"))</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F6" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Advanced")*(F$10:F$209="Missing"))+0.5*SUMPRODUCT(($A$10:$A$209="Advanced")*(F$10:F$209="Partial"))</f>
@@ -48335,7 +48346,7 @@
       <c r="D7" s="265"/>
       <c r="E7" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Advanced")*(E$10:E$209="Completed"))+SUMPRODUCT(($A$10:$A$209="Advanced")*(E$10:E$209="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$209="Advanced")*(E$10:E$209="Partial"))</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F7" s="14">
         <f>SUMPRODUCT(($A$10:$A$209="Advanced")*(F$10:F$209="Completed"))+SUMPRODUCT(($A$10:$A$209="Advanced")*(F$10:F$209="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$209="Advanced")*(F$10:F$209="Partial"))</f>
@@ -48387,10 +48398,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="232" t="s">
         <v>701</v>
       </c>
-      <c r="B10" s="237"/>
+      <c r="B10" s="234"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -48676,10 +48687,10 @@
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A25" s="235" t="s">
+      <c r="A25" s="232" t="s">
         <v>688</v>
       </c>
-      <c r="B25" s="237"/>
+      <c r="B25" s="234"/>
       <c r="C25" s="4" t="s">
         <v>63</v>
       </c>
@@ -48862,7 +48873,7 @@
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>52</v>
@@ -48889,10 +48900,10 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A36" s="235" t="s">
+      <c r="A36" s="232" t="s">
         <v>612</v>
       </c>
-      <c r="B36" s="237"/>
+      <c r="B36" s="234"/>
       <c r="C36" s="4" t="s">
         <v>63</v>
       </c>
@@ -49311,10 +49322,10 @@
       <c r="G57" s="11"/>
     </row>
     <row r="58" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A58" s="235" t="s">
+      <c r="A58" s="232" t="s">
         <v>627</v>
       </c>
-      <c r="B58" s="237"/>
+      <c r="B58" s="234"/>
       <c r="C58" s="4" t="s">
         <v>63</v>
       </c>
@@ -49532,7 +49543,7 @@
         <v>478</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>56</v>
@@ -49619,10 +49630,10 @@
       <c r="G73" s="11"/>
     </row>
     <row r="74" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A74" s="235" t="s">
+      <c r="A74" s="232" t="s">
         <v>651</v>
       </c>
-      <c r="B74" s="237"/>
+      <c r="B74" s="234"/>
       <c r="C74" s="4" t="s">
         <v>63</v>
       </c>
@@ -49811,10 +49822,10 @@
       <c r="G83" s="11"/>
     </row>
     <row r="84" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A84" s="235" t="s">
+      <c r="A84" s="232" t="s">
         <v>663</v>
       </c>
-      <c r="B84" s="237"/>
+      <c r="B84" s="234"/>
       <c r="C84" s="21" t="s">
         <v>456</v>
       </c>
@@ -50052,7 +50063,7 @@
       </c>
       <c r="D96" s="11"/>
       <c r="E96" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F96" s="4" t="s">
         <v>52</v>
@@ -50174,10 +50185,10 @@
       <c r="G102" s="11"/>
     </row>
     <row r="103" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A103" s="235" t="s">
+      <c r="A103" s="232" t="s">
         <v>677</v>
       </c>
-      <c r="B103" s="237"/>
+      <c r="B103" s="234"/>
       <c r="C103" s="4" t="s">
         <v>63</v>
       </c>
@@ -50376,7 +50387,7 @@
         <v>675</v>
       </c>
       <c r="D113" s="11" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E113" s="4" t="s">
         <v>58</v>
@@ -50475,7 +50486,7 @@
         <v>460</v>
       </c>
       <c r="D118" s="11" t="s">
-        <v>972</v>
+        <v>982</v>
       </c>
       <c r="E118" s="4" t="s">
         <v>58</v>
@@ -53351,10 +53362,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="232" t="s">
         <v>291</v>
       </c>
-      <c r="B10" s="237"/>
+      <c r="B10" s="234"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -53714,10 +53725,10 @@
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A29" s="235" t="s">
+      <c r="A29" s="232" t="s">
         <v>564</v>
       </c>
-      <c r="B29" s="237"/>
+      <c r="B29" s="234"/>
       <c r="C29" s="4" t="s">
         <v>451</v>
       </c>
@@ -53946,10 +53957,10 @@
       <c r="G40" s="11"/>
     </row>
     <row r="41" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A41" s="235" t="s">
+      <c r="A41" s="232" t="s">
         <v>334</v>
       </c>
-      <c r="B41" s="237"/>
+      <c r="B41" s="234"/>
       <c r="C41" s="4" t="s">
         <v>63</v>
       </c>
@@ -54055,7 +54066,7 @@
         <v>343</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>58</v>
@@ -54163,10 +54174,10 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" s="7" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A52" s="235" t="s">
+      <c r="A52" s="232" t="s">
         <v>84</v>
       </c>
-      <c r="B52" s="237"/>
+      <c r="B52" s="234"/>
       <c r="C52" s="4" t="s">
         <v>63</v>
       </c>
@@ -54336,10 +54347,10 @@
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" s="7" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A61" s="235" t="s">
+      <c r="A61" s="232" t="s">
         <v>370</v>
       </c>
-      <c r="B61" s="237"/>
+      <c r="B61" s="234"/>
       <c r="C61" s="21" t="s">
         <v>452</v>
       </c>
@@ -55689,10 +55700,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="232" t="s">
         <v>810</v>
       </c>
-      <c r="B10" s="237"/>
+      <c r="B10" s="234"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -55995,10 +56006,10 @@
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A26" s="235" t="s">
+      <c r="A26" s="232" t="s">
         <v>390</v>
       </c>
-      <c r="B26" s="237"/>
+      <c r="B26" s="234"/>
       <c r="C26" s="4" t="s">
         <v>855</v>
       </c>
@@ -56265,10 +56276,10 @@
       <c r="G39" s="11"/>
     </row>
     <row r="40" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A40" s="235" t="s">
+      <c r="A40" s="232" t="s">
         <v>448</v>
       </c>
-      <c r="B40" s="237"/>
+      <c r="B40" s="234"/>
       <c r="C40" s="102" t="s">
         <v>856</v>
       </c>
@@ -56533,10 +56544,10 @@
       <c r="G53" s="11"/>
     </row>
     <row r="54" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A54" s="235" t="s">
+      <c r="A54" s="232" t="s">
         <v>412</v>
       </c>
-      <c r="B54" s="237"/>
+      <c r="B54" s="234"/>
       <c r="C54" s="4" t="s">
         <v>63</v>
       </c>
@@ -56604,7 +56615,7 @@
         <v>417</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>58</v>
@@ -58399,10 +58410,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="232" t="s">
         <v>239</v>
       </c>
-      <c r="B10" s="237"/>
+      <c r="B10" s="234"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -58496,10 +58507,10 @@
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A15" s="235" t="s">
+      <c r="A15" s="232" t="s">
         <v>246</v>
       </c>
-      <c r="B15" s="237"/>
+      <c r="B15" s="234"/>
       <c r="C15" s="4" t="s">
         <v>874</v>
       </c>
@@ -58612,10 +58623,10 @@
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A21" s="235" t="s">
+      <c r="A21" s="232" t="s">
         <v>878</v>
       </c>
-      <c r="B21" s="237"/>
+      <c r="B21" s="234"/>
       <c r="C21" s="4" t="s">
         <v>63</v>
       </c>
@@ -58747,10 +58758,10 @@
       <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A28" s="235" t="s">
+      <c r="A28" s="232" t="s">
         <v>254</v>
       </c>
-      <c r="B28" s="237"/>
+      <c r="B28" s="234"/>
       <c r="C28" s="4" t="s">
         <v>875</v>
       </c>
@@ -58901,10 +58912,10 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A36" s="235" t="s">
+      <c r="A36" s="232" t="s">
         <v>891</v>
       </c>
-      <c r="B36" s="237"/>
+      <c r="B36" s="234"/>
       <c r="C36" s="4" t="s">
         <v>454</v>
       </c>
@@ -59036,10 +59047,10 @@
       <c r="G42" s="11"/>
     </row>
     <row r="43" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A43" s="235" t="s">
+      <c r="A43" s="232" t="s">
         <v>275</v>
       </c>
-      <c r="B43" s="237"/>
+      <c r="B43" s="234"/>
       <c r="C43" s="4" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Fixed an issue with pulltab highlights appearing at the wrong time.  Changed the scientist's dialog at the duckpond.
</commit_message>
<xml_diff>
--- a/GameDocuments/gam352_papercut_rubric.xlsx
+++ b/GameDocuments/gam352_papercut_rubric.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Game Data" sheetId="1" r:id="rId1"/>
@@ -5777,6 +5777,90 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -5810,18 +5894,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -5879,99 +5951,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="4" borderId="16" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="4" borderId="18" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="26" fillId="3" borderId="21" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5982,6 +5961,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="26" fillId="3" borderId="26" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6050,55 +6035,37 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="4" borderId="16" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="4" borderId="18" xfId="653" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6110,28 +6077,28 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6158,19 +6125,52 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -39831,7 +39831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -39851,54 +39851,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="178"/>
+      <c r="B1" s="145"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="146"/>
       <c r="E1" s="103"/>
-      <c r="F1" s="176" t="s">
+      <c r="F1" s="144" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="177"/>
-      <c r="H1" s="177"/>
-      <c r="I1" s="177"/>
-      <c r="J1" s="178"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
+      <c r="J1" s="146"/>
       <c r="K1" s="104"/>
       <c r="L1" s="104"/>
       <c r="M1" s="105"/>
     </row>
     <row r="2" spans="1:13" ht="14.1" customHeight="1">
-      <c r="A2" s="182" t="s">
+      <c r="A2" s="147" t="s">
         <v>951</v>
       </c>
-      <c r="B2" s="183"/>
-      <c r="C2" s="183"/>
-      <c r="D2" s="184"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="149"/>
       <c r="E2" s="103"/>
-      <c r="F2" s="182" t="s">
+      <c r="F2" s="147" t="s">
         <v>954</v>
       </c>
-      <c r="G2" s="183"/>
-      <c r="H2" s="183"/>
-      <c r="I2" s="183"/>
-      <c r="J2" s="184"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="149"/>
       <c r="K2" s="104"/>
       <c r="L2" s="104"/>
       <c r="M2" s="105"/>
     </row>
     <row r="3" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A3" s="185"/>
-      <c r="B3" s="186"/>
-      <c r="C3" s="186"/>
-      <c r="D3" s="187"/>
+      <c r="A3" s="150"/>
+      <c r="B3" s="151"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="103"/>
-      <c r="F3" s="185"/>
-      <c r="G3" s="186"/>
-      <c r="H3" s="186"/>
-      <c r="I3" s="186"/>
-      <c r="J3" s="187"/>
+      <c r="F3" s="150"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="151"/>
+      <c r="J3" s="152"/>
       <c r="K3" s="104"/>
       <c r="L3" s="104"/>
       <c r="M3" s="105"/>
@@ -39919,41 +39919,41 @@
       <c r="M4" s="105"/>
     </row>
     <row r="5" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="144" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="177"/>
-      <c r="C5" s="177"/>
-      <c r="D5" s="178"/>
+      <c r="B5" s="145"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="146"/>
       <c r="E5" s="103"/>
-      <c r="F5" s="176" t="s">
+      <c r="F5" s="144" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="177"/>
-      <c r="H5" s="177"/>
-      <c r="I5" s="177"/>
-      <c r="J5" s="178"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="145"/>
+      <c r="I5" s="145"/>
+      <c r="J5" s="146"/>
       <c r="K5" s="104"/>
       <c r="L5" s="107"/>
       <c r="M5" s="105"/>
     </row>
     <row r="6" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="156" t="s">
         <v>952</v>
       </c>
-      <c r="B6" s="174"/>
-      <c r="C6" s="174"/>
-      <c r="D6" s="175"/>
+      <c r="B6" s="157"/>
+      <c r="C6" s="157"/>
+      <c r="D6" s="158"/>
       <c r="E6" s="103"/>
-      <c r="F6" s="173" t="s">
+      <c r="F6" s="156" t="s">
         <v>955</v>
       </c>
-      <c r="G6" s="174"/>
-      <c r="H6" s="174"/>
-      <c r="I6" s="174"/>
-      <c r="J6" s="175"/>
+      <c r="G6" s="157"/>
+      <c r="H6" s="157"/>
+      <c r="I6" s="157"/>
+      <c r="J6" s="158"/>
       <c r="K6" s="104"/>
-      <c r="L6" s="170" t="s">
+      <c r="L6" s="153" t="s">
         <v>24</v>
       </c>
       <c r="M6" s="105"/>
@@ -39964,51 +39964,51 @@
       <c r="C7" s="108"/>
       <c r="D7" s="109"/>
       <c r="E7" s="103"/>
-      <c r="F7" s="173" t="s">
+      <c r="F7" s="156" t="s">
         <v>978</v>
       </c>
-      <c r="G7" s="174"/>
-      <c r="H7" s="174"/>
-      <c r="I7" s="174"/>
-      <c r="J7" s="175"/>
+      <c r="G7" s="157"/>
+      <c r="H7" s="157"/>
+      <c r="I7" s="157"/>
+      <c r="J7" s="158"/>
       <c r="K7" s="104"/>
-      <c r="L7" s="171"/>
+      <c r="L7" s="154"/>
       <c r="M7" s="105"/>
     </row>
     <row r="8" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="144" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="177"/>
-      <c r="C8" s="177"/>
-      <c r="D8" s="178"/>
+      <c r="B8" s="145"/>
+      <c r="C8" s="145"/>
+      <c r="D8" s="146"/>
       <c r="E8" s="103"/>
-      <c r="F8" s="173" t="s">
+      <c r="F8" s="156" t="s">
         <v>977</v>
       </c>
-      <c r="G8" s="174"/>
-      <c r="H8" s="174"/>
-      <c r="I8" s="174"/>
-      <c r="J8" s="175"/>
+      <c r="G8" s="157"/>
+      <c r="H8" s="157"/>
+      <c r="I8" s="157"/>
+      <c r="J8" s="158"/>
       <c r="K8" s="104"/>
-      <c r="L8" s="171"/>
+      <c r="L8" s="154"/>
       <c r="M8" s="105"/>
     </row>
     <row r="9" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="156" t="s">
         <v>953</v>
       </c>
-      <c r="B9" s="174"/>
-      <c r="C9" s="174"/>
-      <c r="D9" s="175"/>
+      <c r="B9" s="157"/>
+      <c r="C9" s="157"/>
+      <c r="D9" s="158"/>
       <c r="E9" s="103"/>
-      <c r="F9" s="173"/>
-      <c r="G9" s="174"/>
-      <c r="H9" s="174"/>
-      <c r="I9" s="174"/>
-      <c r="J9" s="175"/>
+      <c r="F9" s="156"/>
+      <c r="G9" s="157"/>
+      <c r="H9" s="157"/>
+      <c r="I9" s="157"/>
+      <c r="J9" s="158"/>
       <c r="K9" s="104"/>
-      <c r="L9" s="172"/>
+      <c r="L9" s="155"/>
       <c r="M9" s="105"/>
     </row>
     <row r="10" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40027,18 +40027,18 @@
       <c r="M10" s="105"/>
     </row>
     <row r="11" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="144" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="177"/>
-      <c r="C11" s="177"/>
-      <c r="D11" s="178"/>
+      <c r="B11" s="145"/>
+      <c r="C11" s="145"/>
+      <c r="D11" s="146"/>
       <c r="E11" s="103"/>
-      <c r="F11" s="176" t="s">
+      <c r="F11" s="144" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="177"/>
-      <c r="H11" s="178"/>
+      <c r="G11" s="145"/>
+      <c r="H11" s="146"/>
       <c r="I11" s="134" t="s">
         <v>7</v>
       </c>
@@ -40078,7 +40078,7 @@
         <v>-0.12</v>
       </c>
       <c r="K12" s="104"/>
-      <c r="L12" s="170" t="s">
+      <c r="L12" s="153" t="s">
         <v>8</v>
       </c>
       <c r="M12" s="105"/>
@@ -40111,7 +40111,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="120"/>
-      <c r="L13" s="171"/>
+      <c r="L13" s="154"/>
       <c r="M13" s="121"/>
     </row>
     <row r="14" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40141,7 +40141,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="124"/>
-      <c r="L14" s="172"/>
+      <c r="L14" s="155"/>
       <c r="M14" s="125"/>
     </row>
     <row r="15" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40209,11 +40209,11 @@
         <v>939</v>
       </c>
       <c r="E17" s="104"/>
-      <c r="F17" s="176" t="s">
+      <c r="F17" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="177"/>
-      <c r="H17" s="178"/>
+      <c r="G17" s="145"/>
+      <c r="H17" s="146"/>
       <c r="I17" s="111"/>
       <c r="J17" s="135">
         <v>0.75</v>
@@ -40239,17 +40239,17 @@
       <c r="F18" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="179" t="s">
+      <c r="G18" s="159" t="s">
         <v>956</v>
       </c>
-      <c r="H18" s="180"/>
-      <c r="I18" s="181"/>
+      <c r="H18" s="160"/>
+      <c r="I18" s="161"/>
       <c r="J18" s="137">
         <f>IF(LEFT(G18,6)="Entire",0,IF(LEFT(G18,6)="Custom",-0.05,-0.1))</f>
         <v>-0.1</v>
       </c>
       <c r="K18" s="128"/>
-      <c r="L18" s="170" t="s">
+      <c r="L18" s="153" t="s">
         <v>18</v>
       </c>
       <c r="M18" s="105"/>
@@ -40271,17 +40271,17 @@
       <c r="F19" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="153" t="s">
+      <c r="G19" s="162" t="s">
         <v>957</v>
       </c>
-      <c r="H19" s="154"/>
-      <c r="I19" s="155"/>
+      <c r="H19" s="163"/>
+      <c r="I19" s="164"/>
       <c r="J19" s="139">
         <f>IF(G19="2D Graphics and 2D Gameplay",IF(J11=0.15,-0.05,0),IF(G19="3D Graphics but 2D Gameplay",IF(J11=0.15,-0.02,-0.3),IF(J11=0.15,0,-0.3)))</f>
         <v>0</v>
       </c>
       <c r="K19" s="104"/>
-      <c r="L19" s="172"/>
+      <c r="L19" s="155"/>
       <c r="M19" s="105"/>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40333,22 +40333,22 @@
       <c r="C22" s="118"/>
       <c r="D22" s="119"/>
       <c r="E22" s="104"/>
-      <c r="F22" s="168" t="s">
+      <c r="F22" s="186" t="s">
         <v>713</v>
       </c>
-      <c r="G22" s="166" t="s">
+      <c r="G22" s="184" t="s">
         <v>714</v>
       </c>
-      <c r="H22" s="165"/>
+      <c r="H22" s="183"/>
       <c r="I22" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="163">
+      <c r="J22" s="181">
         <f>J20+J15</f>
         <v>0.68</v>
       </c>
       <c r="K22" s="104"/>
-      <c r="L22" s="144" t="s">
+      <c r="L22" s="165" t="s">
         <v>725</v>
       </c>
       <c r="M22" s="105"/>
@@ -40359,15 +40359,15 @@
       <c r="C23" s="118"/>
       <c r="D23" s="119"/>
       <c r="E23" s="104"/>
-      <c r="F23" s="169"/>
-      <c r="G23" s="167"/>
-      <c r="H23" s="165"/>
+      <c r="F23" s="187"/>
+      <c r="G23" s="185"/>
+      <c r="H23" s="183"/>
       <c r="I23" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="164"/>
+      <c r="J23" s="182"/>
       <c r="K23" s="104"/>
-      <c r="L23" s="145"/>
+      <c r="L23" s="166"/>
       <c r="M23" s="105"/>
     </row>
     <row r="24" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -40391,13 +40391,13 @@
       <c r="C25" s="118"/>
       <c r="D25" s="119"/>
       <c r="E25" s="104"/>
-      <c r="F25" s="157" t="s">
+      <c r="F25" s="175" t="s">
         <v>932</v>
       </c>
-      <c r="G25" s="158"/>
-      <c r="H25" s="158"/>
-      <c r="I25" s="158"/>
-      <c r="J25" s="159"/>
+      <c r="G25" s="176"/>
+      <c r="H25" s="176"/>
+      <c r="I25" s="176"/>
+      <c r="J25" s="177"/>
       <c r="K25" s="104"/>
       <c r="L25" s="104"/>
       <c r="M25" s="105"/>
@@ -40408,11 +40408,11 @@
       <c r="C26" s="118"/>
       <c r="D26" s="119"/>
       <c r="E26" s="103"/>
-      <c r="F26" s="160"/>
-      <c r="G26" s="161"/>
-      <c r="H26" s="161"/>
-      <c r="I26" s="161"/>
-      <c r="J26" s="162"/>
+      <c r="F26" s="178"/>
+      <c r="G26" s="179"/>
+      <c r="H26" s="179"/>
+      <c r="I26" s="179"/>
+      <c r="J26" s="180"/>
       <c r="K26" s="104"/>
       <c r="L26" s="104"/>
       <c r="M26" s="105"/>
@@ -40438,13 +40438,13 @@
       <c r="C28" s="118"/>
       <c r="D28" s="119"/>
       <c r="E28" s="103"/>
-      <c r="F28" s="156" t="s">
+      <c r="F28" s="174" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="156"/>
-      <c r="H28" s="156"/>
-      <c r="I28" s="156"/>
-      <c r="J28" s="156"/>
+      <c r="G28" s="174"/>
+      <c r="H28" s="174"/>
+      <c r="I28" s="174"/>
+      <c r="J28" s="174"/>
       <c r="K28" s="104"/>
       <c r="L28" s="104"/>
       <c r="M28" s="105"/>
@@ -40455,13 +40455,13 @@
       <c r="C29" s="118"/>
       <c r="D29" s="119"/>
       <c r="E29" s="103"/>
-      <c r="F29" s="150" t="s">
+      <c r="F29" s="171" t="s">
         <v>933</v>
       </c>
-      <c r="G29" s="151"/>
-      <c r="H29" s="151"/>
-      <c r="I29" s="151"/>
-      <c r="J29" s="152"/>
+      <c r="G29" s="172"/>
+      <c r="H29" s="172"/>
+      <c r="I29" s="172"/>
+      <c r="J29" s="173"/>
       <c r="K29" s="104"/>
       <c r="L29" s="104"/>
       <c r="M29" s="105"/>
@@ -40472,30 +40472,30 @@
       <c r="C30" s="118"/>
       <c r="D30" s="119"/>
       <c r="E30" s="103"/>
-      <c r="F30" s="150"/>
-      <c r="G30" s="151"/>
-      <c r="H30" s="151"/>
-      <c r="I30" s="151"/>
-      <c r="J30" s="152"/>
+      <c r="F30" s="171"/>
+      <c r="G30" s="172"/>
+      <c r="H30" s="172"/>
+      <c r="I30" s="172"/>
+      <c r="J30" s="173"/>
       <c r="K30" s="104"/>
       <c r="L30" s="104"/>
       <c r="M30" s="105"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A31" s="146" t="s">
+      <c r="A31" s="167" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="147"/>
-      <c r="C31" s="148" t="s">
+      <c r="B31" s="168"/>
+      <c r="C31" s="169" t="s">
         <v>950</v>
       </c>
-      <c r="D31" s="149"/>
+      <c r="D31" s="170"/>
       <c r="E31" s="104"/>
-      <c r="F31" s="153"/>
-      <c r="G31" s="154"/>
-      <c r="H31" s="154"/>
-      <c r="I31" s="154"/>
-      <c r="J31" s="155"/>
+      <c r="F31" s="162"/>
+      <c r="G31" s="163"/>
+      <c r="H31" s="163"/>
+      <c r="I31" s="163"/>
+      <c r="J31" s="164"/>
       <c r="K31" s="104"/>
       <c r="L31" s="104"/>
       <c r="M31" s="105"/>
@@ -40518,12 +40518,16 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0"/>
   <mergeCells count="31">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="A2:D3"/>
-    <mergeCell ref="F2:J3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F29:J31"/>
+    <mergeCell ref="F28:J28"/>
+    <mergeCell ref="F25:J26"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F22:F23"/>
     <mergeCell ref="L12:L14"/>
     <mergeCell ref="L18:L19"/>
     <mergeCell ref="A6:D6"/>
@@ -40539,16 +40543,12 @@
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="G18:I18"/>
     <mergeCell ref="G19:I19"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F29:J31"/>
-    <mergeCell ref="F28:J28"/>
-    <mergeCell ref="F25:J26"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A2:D3"/>
+    <mergeCell ref="F2:J3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:J5"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6:D6">
@@ -40616,57 +40616,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="194" t="s">
         <v>556</v>
       </c>
-      <c r="B1" s="200"/>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
-      <c r="E1" s="200"/>
-      <c r="F1" s="200"/>
-      <c r="G1" s="200"/>
-      <c r="H1" s="200"/>
-      <c r="J1" s="210" t="s">
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
+      <c r="F1" s="195"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="195"/>
+      <c r="J1" s="205" t="s">
         <v>482</v>
       </c>
-      <c r="K1" s="211"/>
-      <c r="L1" s="212"/>
+      <c r="K1" s="206"/>
+      <c r="L1" s="207"/>
       <c r="M1" s="79"/>
       <c r="N1" s="24" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A2" s="199"/>
-      <c r="B2" s="200"/>
-      <c r="C2" s="200"/>
-      <c r="D2" s="200"/>
-      <c r="E2" s="200"/>
-      <c r="F2" s="200"/>
-      <c r="G2" s="200"/>
-      <c r="H2" s="200"/>
-      <c r="J2" s="213" t="s">
+      <c r="A2" s="194"/>
+      <c r="B2" s="195"/>
+      <c r="C2" s="195"/>
+      <c r="D2" s="195"/>
+      <c r="E2" s="195"/>
+      <c r="F2" s="195"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="195"/>
+      <c r="J2" s="208" t="s">
         <v>706</v>
       </c>
-      <c r="K2" s="214"/>
-      <c r="L2" s="215"/>
+      <c r="K2" s="209"/>
+      <c r="L2" s="210"/>
       <c r="M2" s="23"/>
       <c r="N2" s="26" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="14.1" customHeight="1">
-      <c r="A3" s="199"/>
-      <c r="B3" s="200"/>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200"/>
-      <c r="E3" s="200"/>
-      <c r="F3" s="200"/>
-      <c r="G3" s="200"/>
-      <c r="H3" s="200"/>
-      <c r="J3" s="213"/>
-      <c r="K3" s="214"/>
-      <c r="L3" s="215"/>
+      <c r="A3" s="194"/>
+      <c r="B3" s="195"/>
+      <c r="C3" s="195"/>
+      <c r="D3" s="195"/>
+      <c r="E3" s="195"/>
+      <c r="F3" s="195"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="195"/>
+      <c r="J3" s="208"/>
+      <c r="K3" s="209"/>
+      <c r="L3" s="210"/>
       <c r="M3" s="23"/>
       <c r="N3" s="26" t="s">
         <v>431</v>
@@ -40676,14 +40676,14 @@
       <c r="A4" s="2"/>
       <c r="B4" s="5"/>
       <c r="C4" s="8"/>
-      <c r="D4" s="192"/>
-      <c r="E4" s="192"/>
+      <c r="D4" s="193"/>
+      <c r="E4" s="193"/>
       <c r="F4" s="43"/>
-      <c r="G4" s="192"/>
-      <c r="H4" s="192"/>
-      <c r="J4" s="213"/>
-      <c r="K4" s="214"/>
-      <c r="L4" s="215"/>
+      <c r="G4" s="193"/>
+      <c r="H4" s="193"/>
+      <c r="J4" s="208"/>
+      <c r="K4" s="209"/>
+      <c r="L4" s="210"/>
       <c r="M4" s="34"/>
       <c r="N4" s="26" t="s">
         <v>432</v>
@@ -40691,24 +40691,24 @@
       <c r="O4" s="81"/>
     </row>
     <row r="5" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A5" s="201" t="s">
+      <c r="A5" s="196" t="s">
         <v>425</v>
       </c>
-      <c r="B5" s="202"/>
+      <c r="B5" s="197"/>
       <c r="C5" s="8"/>
-      <c r="D5" s="205" t="s">
+      <c r="D5" s="200" t="s">
         <v>717</v>
       </c>
-      <c r="E5" s="206"/>
-      <c r="F5" s="207"/>
-      <c r="G5" s="208">
+      <c r="E5" s="201"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="203">
         <f>Submission!$E$17</f>
         <v>0</v>
       </c>
-      <c r="H5" s="209"/>
-      <c r="J5" s="213"/>
-      <c r="K5" s="214"/>
-      <c r="L5" s="215"/>
+      <c r="H5" s="204"/>
+      <c r="J5" s="208"/>
+      <c r="K5" s="209"/>
+      <c r="L5" s="210"/>
       <c r="M5" s="34"/>
       <c r="N5" s="26" t="s">
         <v>433</v>
@@ -40716,21 +40716,21 @@
       <c r="O5" s="81"/>
     </row>
     <row r="6" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A6" s="203"/>
-      <c r="B6" s="204"/>
+      <c r="A6" s="198"/>
+      <c r="B6" s="199"/>
       <c r="C6" s="43"/>
-      <c r="D6" s="192" t="s">
+      <c r="D6" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="192"/>
+      <c r="E6" s="193"/>
       <c r="F6" s="43"/>
-      <c r="G6" s="192" t="s">
+      <c r="G6" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="192"/>
-      <c r="J6" s="213"/>
-      <c r="K6" s="214"/>
-      <c r="L6" s="215"/>
+      <c r="H6" s="193"/>
+      <c r="J6" s="208"/>
+      <c r="K6" s="209"/>
+      <c r="L6" s="210"/>
       <c r="M6" s="34"/>
       <c r="N6" s="26" t="s">
         <v>434</v>
@@ -40738,24 +40738,24 @@
       <c r="O6" s="81"/>
     </row>
     <row r="7" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A7" s="195">
+      <c r="A7" s="188">
         <f>'Game Data'!$J$22</f>
         <v>0.68</v>
       </c>
-      <c r="B7" s="196"/>
+      <c r="B7" s="189"/>
       <c r="C7" s="43"/>
-      <c r="D7" s="193" t="s">
+      <c r="D7" s="216" t="s">
         <v>724</v>
       </c>
-      <c r="E7" s="194"/>
+      <c r="E7" s="217"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="193" t="s">
+      <c r="G7" s="216" t="s">
         <v>724</v>
       </c>
-      <c r="H7" s="194"/>
-      <c r="J7" s="213"/>
-      <c r="K7" s="214"/>
-      <c r="L7" s="215"/>
+      <c r="H7" s="217"/>
+      <c r="J7" s="208"/>
+      <c r="K7" s="209"/>
+      <c r="L7" s="210"/>
       <c r="M7" s="33"/>
       <c r="N7" s="26" t="s">
         <v>435</v>
@@ -40763,23 +40763,23 @@
       <c r="O7" s="81"/>
     </row>
     <row r="8" spans="1:15" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A8" s="197"/>
-      <c r="B8" s="198"/>
+      <c r="A8" s="190"/>
+      <c r="B8" s="191"/>
       <c r="C8" s="97"/>
-      <c r="D8" s="219">
+      <c r="D8" s="214">
         <f>E17+E26+E35+E44+E53</f>
         <v>0.31124999999999997</v>
       </c>
-      <c r="E8" s="220"/>
+      <c r="E8" s="215"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="219">
+      <c r="G8" s="214">
         <f>H17+H26+H35+H44+H53</f>
         <v>2.4999999999999998E-2</v>
       </c>
-      <c r="H8" s="220"/>
-      <c r="J8" s="216"/>
-      <c r="K8" s="217"/>
-      <c r="L8" s="218"/>
+      <c r="H8" s="215"/>
+      <c r="J8" s="211"/>
+      <c r="K8" s="212"/>
+      <c r="L8" s="213"/>
       <c r="M8" s="80"/>
       <c r="N8" s="25" t="s">
         <v>436</v>
@@ -40790,15 +40790,15 @@
       <c r="A9" s="2"/>
       <c r="B9" s="5"/>
       <c r="C9" s="43"/>
-      <c r="D9" s="192" t="s">
+      <c r="D9" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="192"/>
+      <c r="E9" s="193"/>
       <c r="F9" s="43"/>
-      <c r="G9" s="192" t="s">
+      <c r="G9" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="192"/>
+      <c r="H9" s="193"/>
       <c r="J9" s="82"/>
       <c r="K9" s="82"/>
       <c r="L9" s="82"/>
@@ -40825,11 +40825,11 @@
       <c r="H10" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="191" t="s">
+      <c r="J10" s="192" t="s">
         <v>707</v>
       </c>
-      <c r="K10" s="191"/>
-      <c r="L10" s="191"/>
+      <c r="K10" s="192"/>
+      <c r="L10" s="192"/>
       <c r="O10" s="84"/>
     </row>
     <row r="11" spans="1:15" ht="14.1" customHeight="1">
@@ -40858,11 +40858,11 @@
         <f t="shared" ref="H11:H16" si="1">$B11*G11</f>
         <v>0</v>
       </c>
-      <c r="J11" s="190" t="s">
+      <c r="J11" s="220" t="s">
         <v>792</v>
       </c>
-      <c r="K11" s="190"/>
-      <c r="L11" s="190"/>
+      <c r="K11" s="220"/>
+      <c r="L11" s="220"/>
       <c r="M11" s="82"/>
       <c r="O11" s="84"/>
     </row>
@@ -40892,9 +40892,9 @@
         <f t="shared" si="1"/>
         <v>-0.02</v>
       </c>
-      <c r="J12" s="190"/>
-      <c r="K12" s="190"/>
-      <c r="L12" s="190"/>
+      <c r="J12" s="220"/>
+      <c r="K12" s="220"/>
+      <c r="L12" s="220"/>
       <c r="M12" s="82"/>
       <c r="O12" s="84"/>
     </row>
@@ -40924,9 +40924,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="190"/>
-      <c r="K13" s="190"/>
-      <c r="L13" s="190"/>
+      <c r="J13" s="220"/>
+      <c r="K13" s="220"/>
+      <c r="L13" s="220"/>
       <c r="M13" s="82"/>
       <c r="O13" s="84"/>
     </row>
@@ -40992,11 +40992,11 @@
         <f t="shared" si="1"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J15" s="188">
+      <c r="J15" s="218">
         <f>MAX(0,MIN(1,IF($J17 &lt;= 0.95, ROUND($J17,2), FLOOR((0.95+($J17-0.95)/5),0.01))))</f>
         <v>0.86</v>
       </c>
-      <c r="L15" s="188">
+      <c r="L15" s="218">
         <f>MAX(0,MIN(1,IF($L17 &lt;= 0.95, ROUND($L17,2), FLOOR((0.95+($L17-0.95)/5),0.01))))</f>
         <v>0.71</v>
       </c>
@@ -41029,8 +41029,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J16" s="189"/>
-      <c r="L16" s="189"/>
+      <c r="J16" s="219"/>
+      <c r="L16" s="219"/>
       <c r="M16" s="82"/>
       <c r="O16" s="84"/>
     </row>
@@ -41067,15 +41067,15 @@
       <c r="A18" s="2"/>
       <c r="B18" s="5"/>
       <c r="C18" s="43"/>
-      <c r="D18" s="192" t="s">
+      <c r="D18" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="192"/>
+      <c r="E18" s="193"/>
       <c r="F18" s="43"/>
-      <c r="G18" s="192" t="s">
+      <c r="G18" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="192"/>
+      <c r="H18" s="193"/>
       <c r="J18" s="88"/>
       <c r="M18" s="78"/>
     </row>
@@ -41100,11 +41100,11 @@
       <c r="H19" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="191" t="s">
+      <c r="J19" s="192" t="s">
         <v>715</v>
       </c>
-      <c r="K19" s="191"/>
-      <c r="L19" s="191"/>
+      <c r="K19" s="192"/>
+      <c r="L19" s="192"/>
       <c r="M19" s="83"/>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1">
@@ -41133,11 +41133,11 @@
         <f t="shared" ref="H20:H25" si="3">$B20*G20</f>
         <v>0</v>
       </c>
-      <c r="J20" s="190" t="s">
+      <c r="J20" s="220" t="s">
         <v>722</v>
       </c>
-      <c r="K20" s="190"/>
-      <c r="L20" s="190"/>
+      <c r="K20" s="220"/>
+      <c r="L20" s="220"/>
       <c r="M20" s="84"/>
     </row>
     <row r="21" spans="1:13" ht="14.1" customHeight="1">
@@ -41166,9 +41166,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J21" s="190"/>
-      <c r="K21" s="190"/>
-      <c r="L21" s="190"/>
+      <c r="J21" s="220"/>
+      <c r="K21" s="220"/>
+      <c r="L21" s="220"/>
       <c r="M21" s="84"/>
     </row>
     <row r="22" spans="1:13" ht="14.1" customHeight="1">
@@ -41197,9 +41197,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J22" s="190"/>
-      <c r="K22" s="190"/>
-      <c r="L22" s="190"/>
+      <c r="J22" s="220"/>
+      <c r="K22" s="220"/>
+      <c r="L22" s="220"/>
       <c r="M22" s="84"/>
     </row>
     <row r="23" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
@@ -41263,11 +41263,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J24" s="188">
+      <c r="J24" s="218">
         <f>MAX(0,MIN(1,IF($J26 &lt;= 0.95, ROUND($J26,2), FLOOR((0.95+($J26-0.95)/5),0.01))))</f>
         <v>0.88</v>
       </c>
-      <c r="L24" s="188">
+      <c r="L24" s="218">
         <f>MAX(0,MIN(1,IF($L26 &lt;= 0.95, ROUND($L26,2), FLOOR((0.95+($L26-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -41299,8 +41299,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J25" s="189"/>
-      <c r="L25" s="189"/>
+      <c r="J25" s="219"/>
+      <c r="L25" s="219"/>
       <c r="M25" s="84"/>
     </row>
     <row r="26" spans="1:13" ht="14.1" customHeight="1">
@@ -41336,15 +41336,15 @@
       <c r="A27" s="2"/>
       <c r="B27" s="5"/>
       <c r="C27" s="43"/>
-      <c r="D27" s="192" t="s">
+      <c r="D27" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="192"/>
+      <c r="E27" s="193"/>
       <c r="F27" s="43"/>
-      <c r="G27" s="192" t="s">
+      <c r="G27" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H27" s="192"/>
+      <c r="H27" s="193"/>
     </row>
     <row r="28" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
       <c r="A28" s="1" t="s">
@@ -41367,11 +41367,11 @@
       <c r="H28" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J28" s="191" t="s">
+      <c r="J28" s="192" t="s">
         <v>709</v>
       </c>
-      <c r="K28" s="191"/>
-      <c r="L28" s="191"/>
+      <c r="K28" s="192"/>
+      <c r="L28" s="192"/>
     </row>
     <row r="29" spans="1:13" ht="14.1" customHeight="1">
       <c r="A29" s="57" t="str">
@@ -41399,11 +41399,11 @@
         <f t="shared" ref="H29:H34" si="5">$B29*G29</f>
         <v>0</v>
       </c>
-      <c r="J29" s="190" t="s">
+      <c r="J29" s="220" t="s">
         <v>710</v>
       </c>
-      <c r="K29" s="190"/>
-      <c r="L29" s="190"/>
+      <c r="K29" s="220"/>
+      <c r="L29" s="220"/>
     </row>
     <row r="30" spans="1:13" ht="14.1" customHeight="1">
       <c r="A30" s="58" t="str">
@@ -41431,9 +41431,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J30" s="190"/>
-      <c r="K30" s="190"/>
-      <c r="L30" s="190"/>
+      <c r="J30" s="220"/>
+      <c r="K30" s="220"/>
+      <c r="L30" s="220"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1">
       <c r="A31" s="58" t="str">
@@ -41461,9 +41461,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J31" s="190"/>
-      <c r="K31" s="190"/>
-      <c r="L31" s="190"/>
+      <c r="J31" s="220"/>
+      <c r="K31" s="220"/>
+      <c r="L31" s="220"/>
     </row>
     <row r="32" spans="1:13" ht="14.1" customHeight="1" thickBot="1">
       <c r="A32" s="58" t="str">
@@ -41525,11 +41525,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J33" s="188">
+      <c r="J33" s="218">
         <f>MAX(0,MIN(1,IF($J35 &lt;= 0.95, ROUND($J35,2), FLOOR((0.95+($J35-0.95)/5),0.01))))</f>
         <v>0.88</v>
       </c>
-      <c r="L33" s="188">
+      <c r="L33" s="218">
         <f>MAX(0,MIN(1,IF($L35 &lt;= 0.95, ROUND($L35,2), FLOOR((0.95+($L35-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -41560,8 +41560,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J34" s="189"/>
-      <c r="L34" s="189"/>
+      <c r="J34" s="219"/>
+      <c r="L34" s="219"/>
     </row>
     <row r="35" spans="1:12" ht="14.1" customHeight="1">
       <c r="A35" s="2"/>
@@ -41595,15 +41595,15 @@
       <c r="A36" s="2"/>
       <c r="B36" s="5"/>
       <c r="C36" s="43"/>
-      <c r="D36" s="192" t="s">
+      <c r="D36" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="192"/>
+      <c r="E36" s="193"/>
       <c r="F36" s="43"/>
-      <c r="G36" s="192" t="s">
+      <c r="G36" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H36" s="192"/>
+      <c r="H36" s="193"/>
     </row>
     <row r="37" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A37" s="1" t="s">
@@ -41626,11 +41626,11 @@
       <c r="H37" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J37" s="191" t="s">
+      <c r="J37" s="192" t="s">
         <v>711</v>
       </c>
-      <c r="K37" s="191"/>
-      <c r="L37" s="191"/>
+      <c r="K37" s="192"/>
+      <c r="L37" s="192"/>
     </row>
     <row r="38" spans="1:12" ht="14.1" customHeight="1">
       <c r="A38" s="57" t="str">
@@ -41658,11 +41658,11 @@
         <f t="shared" ref="H38:H43" si="7">$B38*G38</f>
         <v>0</v>
       </c>
-      <c r="J38" s="190" t="s">
+      <c r="J38" s="220" t="s">
         <v>712</v>
       </c>
-      <c r="K38" s="190"/>
-      <c r="L38" s="190"/>
+      <c r="K38" s="220"/>
+      <c r="L38" s="220"/>
     </row>
     <row r="39" spans="1:12" ht="14.1" customHeight="1">
       <c r="A39" s="58" t="str">
@@ -41690,9 +41690,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J39" s="190"/>
-      <c r="K39" s="190"/>
-      <c r="L39" s="190"/>
+      <c r="J39" s="220"/>
+      <c r="K39" s="220"/>
+      <c r="L39" s="220"/>
     </row>
     <row r="40" spans="1:12" ht="14.1" customHeight="1">
       <c r="A40" s="58" t="str">
@@ -41720,9 +41720,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J40" s="190"/>
-      <c r="K40" s="190"/>
-      <c r="L40" s="190"/>
+      <c r="J40" s="220"/>
+      <c r="K40" s="220"/>
+      <c r="L40" s="220"/>
     </row>
     <row r="41" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A41" s="58" t="str">
@@ -41784,11 +41784,11 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J42" s="188">
+      <c r="J42" s="218">
         <f>MAX(0,MIN(1,IF($J44 &lt;= 0.95, ROUND($J44,2), FLOOR((0.95+($J44-0.95)/5),0.01))))</f>
         <v>0.73</v>
       </c>
-      <c r="L42" s="188">
+      <c r="L42" s="218">
         <f>MAX(0,MIN(1,IF($L44 &lt;= 0.95, ROUND($L44,2), FLOOR((0.95+($L44-0.95)/5),0.01))))</f>
         <v>0.68</v>
       </c>
@@ -41819,8 +41819,8 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J43" s="189"/>
-      <c r="L43" s="189"/>
+      <c r="J43" s="219"/>
+      <c r="L43" s="219"/>
     </row>
     <row r="44" spans="1:12" ht="14.1" customHeight="1">
       <c r="A44" s="2"/>
@@ -41854,15 +41854,15 @@
       <c r="A45" s="2"/>
       <c r="B45" s="5"/>
       <c r="C45" s="43"/>
-      <c r="D45" s="192" t="s">
+      <c r="D45" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="192"/>
+      <c r="E45" s="193"/>
       <c r="F45" s="43"/>
-      <c r="G45" s="192" t="s">
+      <c r="G45" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="192"/>
+      <c r="H45" s="193"/>
     </row>
     <row r="46" spans="1:12" ht="14.1" customHeight="1" thickBot="1">
       <c r="A46" s="1" t="s">
@@ -42070,6 +42070,34 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="J29:L31"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="L33:L34"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="J38:L40"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="J11:L13"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J20:L22"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G36:H36"/>
     <mergeCell ref="A7:B8"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="D6:E6"/>
@@ -42083,34 +42111,6 @@
     <mergeCell ref="J2:L8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="J11:L13"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J20:L22"/>
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="L42:L43"/>
-    <mergeCell ref="J29:L31"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="L33:L34"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="J38:L40"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -42121,8 +42121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -42138,59 +42138,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="235" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="233"/>
-      <c r="C1" s="233"/>
-      <c r="D1" s="233"/>
-      <c r="E1" s="233"/>
-      <c r="F1" s="233"/>
-      <c r="G1" s="234"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="237"/>
     </row>
     <row r="2" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A2" s="221" t="s">
+      <c r="A2" s="230" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="222"/>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
-      <c r="G2" s="223"/>
+      <c r="B2" s="231"/>
+      <c r="C2" s="231"/>
+      <c r="D2" s="231"/>
+      <c r="E2" s="231"/>
+      <c r="F2" s="231"/>
+      <c r="G2" s="232"/>
     </row>
     <row r="3" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A3" s="238" t="s">
+      <c r="A3" s="227" t="s">
         <v>930</v>
       </c>
-      <c r="B3" s="239"/>
-      <c r="C3" s="239"/>
-      <c r="D3" s="239"/>
-      <c r="E3" s="239"/>
-      <c r="F3" s="239"/>
-      <c r="G3" s="240"/>
+      <c r="B3" s="228"/>
+      <c r="C3" s="228"/>
+      <c r="D3" s="228"/>
+      <c r="E3" s="228"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="229"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A4" s="221" t="s">
+      <c r="A4" s="230" t="s">
         <v>438</v>
       </c>
-      <c r="B4" s="222"/>
-      <c r="C4" s="222"/>
-      <c r="D4" s="222"/>
-      <c r="E4" s="222"/>
-      <c r="F4" s="222"/>
-      <c r="G4" s="223"/>
+      <c r="B4" s="231"/>
+      <c r="C4" s="231"/>
+      <c r="D4" s="231"/>
+      <c r="E4" s="231"/>
+      <c r="F4" s="231"/>
+      <c r="G4" s="232"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A5" s="249" t="s">
+      <c r="A5" s="238" t="s">
         <v>580</v>
       </c>
-      <c r="B5" s="250"/>
-      <c r="C5" s="250"/>
-      <c r="D5" s="250"/>
-      <c r="E5" s="250"/>
-      <c r="F5" s="250"/>
-      <c r="G5" s="251"/>
+      <c r="B5" s="239"/>
+      <c r="C5" s="239"/>
+      <c r="D5" s="239"/>
+      <c r="E5" s="239"/>
+      <c r="F5" s="239"/>
+      <c r="G5" s="240"/>
     </row>
     <row r="6" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
       <c r="A6" s="2"/>
@@ -42223,10 +42223,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75">
-      <c r="A8" s="247" t="s">
+      <c r="A8" s="233" t="s">
         <v>718</v>
       </c>
-      <c r="B8" s="248"/>
+      <c r="B8" s="234"/>
       <c r="C8" s="65">
         <v>0</v>
       </c>
@@ -42243,10 +42243,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75">
-      <c r="A9" s="253" t="s">
+      <c r="A9" s="242" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="254"/>
+      <c r="B9" s="243"/>
       <c r="C9" s="92">
         <v>0</v>
       </c>
@@ -42263,10 +42263,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75">
-      <c r="A10" s="255" t="s">
+      <c r="A10" s="244" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="256"/>
+      <c r="B10" s="245"/>
       <c r="C10" s="69">
         <v>0</v>
       </c>
@@ -42283,10 +42283,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75">
-      <c r="A11" s="256" t="s">
+      <c r="A11" s="245" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="256"/>
+      <c r="B11" s="245"/>
       <c r="C11" s="69">
         <v>0</v>
       </c>
@@ -42303,10 +42303,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75">
-      <c r="A12" s="256" t="s">
+      <c r="A12" s="245" t="s">
         <v>716</v>
       </c>
-      <c r="B12" s="256"/>
+      <c r="B12" s="245"/>
       <c r="C12" s="69">
         <v>0</v>
       </c>
@@ -42323,10 +42323,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75">
-      <c r="A13" s="256" t="s">
+      <c r="A13" s="245" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="256"/>
+      <c r="B13" s="245"/>
       <c r="C13" s="69">
         <v>0</v>
       </c>
@@ -42343,10 +42343,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75">
-      <c r="A14" s="255" t="s">
+      <c r="A14" s="244" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="256"/>
+      <c r="B14" s="245"/>
       <c r="C14" s="69">
         <v>0</v>
       </c>
@@ -42363,10 +42363,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75">
-      <c r="A15" s="255" t="s">
+      <c r="A15" s="244" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="256"/>
+      <c r="B15" s="245"/>
       <c r="C15" s="69">
         <v>0</v>
       </c>
@@ -42383,10 +42383,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A16" s="230" t="s">
+      <c r="A16" s="246" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="231"/>
+      <c r="B16" s="247"/>
       <c r="C16" s="73">
         <v>0</v>
       </c>
@@ -42404,11 +42404,11 @@
     </row>
     <row r="17" spans="1:7" ht="14.1" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="252" t="s">
+      <c r="B17" s="241" t="s">
         <v>721</v>
       </c>
-      <c r="C17" s="252"/>
-      <c r="D17" s="252"/>
+      <c r="C17" s="241"/>
+      <c r="D17" s="241"/>
       <c r="E17" s="63">
         <f>SUM(E9:E16)</f>
         <v>0</v>
@@ -42429,527 +42429,559 @@
       <c r="A19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="232" t="s">
+      <c r="B19" s="235" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="233"/>
-      <c r="D19" s="233"/>
-      <c r="E19" s="233"/>
-      <c r="F19" s="233"/>
-      <c r="G19" s="234"/>
+      <c r="C19" s="236"/>
+      <c r="D19" s="236"/>
+      <c r="E19" s="236"/>
+      <c r="F19" s="236"/>
+      <c r="G19" s="237"/>
     </row>
     <row r="20" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="A20" s="10" t="s">
         <v>582</v>
       </c>
-      <c r="B20" s="221" t="s">
+      <c r="B20" s="230" t="s">
         <v>931</v>
       </c>
-      <c r="C20" s="222"/>
-      <c r="D20" s="222"/>
-      <c r="E20" s="222"/>
-      <c r="F20" s="222"/>
-      <c r="G20" s="223"/>
+      <c r="C20" s="231"/>
+      <c r="D20" s="231"/>
+      <c r="E20" s="231"/>
+      <c r="F20" s="231"/>
+      <c r="G20" s="232"/>
     </row>
     <row r="21" spans="1:7" ht="60" customHeight="1" thickBot="1">
       <c r="A21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="221" t="s">
+      <c r="B21" s="230" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="222"/>
-      <c r="D21" s="222"/>
-      <c r="E21" s="222"/>
-      <c r="F21" s="222"/>
-      <c r="G21" s="223"/>
+      <c r="C21" s="231"/>
+      <c r="D21" s="231"/>
+      <c r="E21" s="231"/>
+      <c r="F21" s="231"/>
+      <c r="G21" s="232"/>
     </row>
     <row r="22" spans="1:7" ht="45.95" customHeight="1" thickBot="1">
       <c r="A22" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="221" t="s">
+      <c r="B22" s="230" t="s">
         <v>917</v>
       </c>
-      <c r="C22" s="222"/>
-      <c r="D22" s="222"/>
-      <c r="E22" s="222"/>
-      <c r="F22" s="222"/>
-      <c r="G22" s="223"/>
+      <c r="C22" s="231"/>
+      <c r="D22" s="231"/>
+      <c r="E22" s="231"/>
+      <c r="F22" s="231"/>
+      <c r="G22" s="232"/>
     </row>
     <row r="23" spans="1:7" ht="32.1" customHeight="1">
       <c r="A23" s="98" t="s">
         <v>899</v>
       </c>
-      <c r="B23" s="238" t="s">
+      <c r="B23" s="227" t="s">
         <v>916</v>
       </c>
-      <c r="C23" s="239"/>
-      <c r="D23" s="239"/>
-      <c r="E23" s="239"/>
-      <c r="F23" s="239"/>
-      <c r="G23" s="240"/>
+      <c r="C23" s="228"/>
+      <c r="D23" s="228"/>
+      <c r="E23" s="228"/>
+      <c r="F23" s="228"/>
+      <c r="G23" s="229"/>
     </row>
     <row r="24" spans="1:7" ht="15.75">
       <c r="A24" s="99"/>
-      <c r="B24" s="257" t="s">
+      <c r="B24" s="221" t="s">
         <v>900</v>
       </c>
-      <c r="C24" s="258"/>
-      <c r="D24" s="260" t="s">
+      <c r="C24" s="222"/>
+      <c r="D24" s="223" t="s">
         <v>901</v>
       </c>
-      <c r="E24" s="260"/>
-      <c r="F24" s="260"/>
-      <c r="G24" s="261"/>
+      <c r="E24" s="223"/>
+      <c r="F24" s="223"/>
+      <c r="G24" s="224"/>
     </row>
     <row r="25" spans="1:7" ht="15.75">
       <c r="A25" s="99"/>
-      <c r="B25" s="257" t="s">
+      <c r="B25" s="221" t="s">
         <v>902</v>
       </c>
-      <c r="C25" s="258"/>
-      <c r="D25" s="260" t="s">
+      <c r="C25" s="222"/>
+      <c r="D25" s="223" t="s">
         <v>903</v>
       </c>
-      <c r="E25" s="260"/>
-      <c r="F25" s="260"/>
-      <c r="G25" s="261"/>
+      <c r="E25" s="223"/>
+      <c r="F25" s="223"/>
+      <c r="G25" s="224"/>
     </row>
     <row r="26" spans="1:7" ht="15.75">
       <c r="A26" s="99"/>
-      <c r="B26" s="257" t="s">
+      <c r="B26" s="221" t="s">
         <v>904</v>
       </c>
-      <c r="C26" s="258"/>
-      <c r="D26" s="260" t="s">
+      <c r="C26" s="222"/>
+      <c r="D26" s="223" t="s">
         <v>905</v>
       </c>
-      <c r="E26" s="260"/>
-      <c r="F26" s="260"/>
-      <c r="G26" s="261"/>
+      <c r="E26" s="223"/>
+      <c r="F26" s="223"/>
+      <c r="G26" s="224"/>
     </row>
     <row r="27" spans="1:7" ht="15.75">
       <c r="A27" s="99"/>
-      <c r="B27" s="257" t="s">
+      <c r="B27" s="221" t="s">
         <v>906</v>
       </c>
-      <c r="C27" s="258"/>
+      <c r="C27" s="222"/>
       <c r="D27" s="225" t="s">
         <v>907</v>
       </c>
       <c r="E27" s="225"/>
       <c r="F27" s="225"/>
-      <c r="G27" s="259"/>
+      <c r="G27" s="226"/>
     </row>
     <row r="28" spans="1:7" ht="15.75">
       <c r="A28" s="99"/>
-      <c r="B28" s="257" t="s">
+      <c r="B28" s="221" t="s">
         <v>908</v>
       </c>
-      <c r="C28" s="258"/>
-      <c r="D28" s="260" t="s">
+      <c r="C28" s="222"/>
+      <c r="D28" s="223" t="s">
         <v>909</v>
       </c>
-      <c r="E28" s="260"/>
-      <c r="F28" s="260"/>
-      <c r="G28" s="261"/>
+      <c r="E28" s="223"/>
+      <c r="F28" s="223"/>
+      <c r="G28" s="224"/>
     </row>
     <row r="29" spans="1:7" ht="15.75">
       <c r="A29" s="99"/>
-      <c r="B29" s="257" t="s">
+      <c r="B29" s="221" t="s">
         <v>910</v>
       </c>
-      <c r="C29" s="258"/>
+      <c r="C29" s="222"/>
       <c r="D29" s="225" t="s">
         <v>911</v>
       </c>
       <c r="E29" s="225"/>
       <c r="F29" s="225"/>
-      <c r="G29" s="259"/>
+      <c r="G29" s="226"/>
     </row>
     <row r="30" spans="1:7" ht="15.75">
       <c r="A30" s="99"/>
-      <c r="B30" s="257" t="s">
+      <c r="B30" s="221" t="s">
         <v>914</v>
       </c>
-      <c r="C30" s="258"/>
-      <c r="D30" s="260" t="s">
+      <c r="C30" s="222"/>
+      <c r="D30" s="223" t="s">
         <v>915</v>
       </c>
-      <c r="E30" s="260"/>
-      <c r="F30" s="260"/>
-      <c r="G30" s="261"/>
+      <c r="E30" s="223"/>
+      <c r="F30" s="223"/>
+      <c r="G30" s="224"/>
     </row>
     <row r="31" spans="1:7" ht="15.75">
       <c r="A31" s="99"/>
-      <c r="B31" s="257" t="s">
+      <c r="B31" s="221" t="s">
         <v>912</v>
       </c>
-      <c r="C31" s="258"/>
+      <c r="C31" s="222"/>
       <c r="D31" s="225" t="s">
         <v>913</v>
       </c>
       <c r="E31" s="225"/>
       <c r="F31" s="225"/>
-      <c r="G31" s="259"/>
+      <c r="G31" s="226"/>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickBot="1">
       <c r="A32" s="99"/>
-      <c r="B32" s="257" t="s">
+      <c r="B32" s="221" t="s">
         <v>928</v>
       </c>
-      <c r="C32" s="258"/>
+      <c r="C32" s="222"/>
       <c r="D32" s="225" t="s">
         <v>929</v>
       </c>
       <c r="E32" s="225"/>
       <c r="F32" s="225"/>
-      <c r="G32" s="259"/>
+      <c r="G32" s="226"/>
     </row>
     <row r="33" spans="1:7" ht="15.75">
       <c r="A33" s="98" t="s">
         <v>918</v>
       </c>
-      <c r="B33" s="238" t="s">
+      <c r="B33" s="227" t="s">
         <v>919</v>
       </c>
-      <c r="C33" s="239"/>
-      <c r="D33" s="239"/>
-      <c r="E33" s="239"/>
-      <c r="F33" s="239"/>
-      <c r="G33" s="240"/>
+      <c r="C33" s="228"/>
+      <c r="D33" s="228"/>
+      <c r="E33" s="228"/>
+      <c r="F33" s="228"/>
+      <c r="G33" s="229"/>
     </row>
     <row r="34" spans="1:7" ht="15.75">
       <c r="A34" s="99"/>
-      <c r="B34" s="257" t="s">
+      <c r="B34" s="221" t="s">
         <v>920</v>
       </c>
-      <c r="C34" s="258"/>
-      <c r="D34" s="260" t="s">
+      <c r="C34" s="222"/>
+      <c r="D34" s="223" t="s">
         <v>925</v>
       </c>
-      <c r="E34" s="260"/>
-      <c r="F34" s="260"/>
-      <c r="G34" s="261"/>
+      <c r="E34" s="223"/>
+      <c r="F34" s="223"/>
+      <c r="G34" s="224"/>
     </row>
     <row r="35" spans="1:7" ht="15.75">
       <c r="A35" s="99"/>
-      <c r="B35" s="257" t="s">
+      <c r="B35" s="221" t="s">
         <v>921</v>
       </c>
-      <c r="C35" s="258"/>
-      <c r="D35" s="260" t="s">
+      <c r="C35" s="222"/>
+      <c r="D35" s="223" t="s">
         <v>926</v>
       </c>
-      <c r="E35" s="260"/>
-      <c r="F35" s="260"/>
-      <c r="G35" s="261"/>
+      <c r="E35" s="223"/>
+      <c r="F35" s="223"/>
+      <c r="G35" s="224"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" thickBot="1">
       <c r="A36" s="99"/>
-      <c r="B36" s="257" t="s">
+      <c r="B36" s="221" t="s">
         <v>922</v>
       </c>
-      <c r="C36" s="258"/>
-      <c r="D36" s="260" t="s">
+      <c r="C36" s="222"/>
+      <c r="D36" s="223" t="s">
         <v>927</v>
       </c>
-      <c r="E36" s="260"/>
-      <c r="F36" s="260"/>
-      <c r="G36" s="261"/>
+      <c r="E36" s="223"/>
+      <c r="F36" s="223"/>
+      <c r="G36" s="224"/>
     </row>
     <row r="37" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="A37" s="98" t="s">
         <v>923</v>
       </c>
-      <c r="B37" s="238" t="s">
+      <c r="B37" s="227" t="s">
         <v>924</v>
       </c>
-      <c r="C37" s="239"/>
-      <c r="D37" s="239"/>
-      <c r="E37" s="239"/>
-      <c r="F37" s="239"/>
-      <c r="G37" s="240"/>
+      <c r="C37" s="228"/>
+      <c r="D37" s="228"/>
+      <c r="E37" s="228"/>
+      <c r="F37" s="228"/>
+      <c r="G37" s="229"/>
     </row>
     <row r="38" spans="1:7" ht="29.1" customHeight="1">
-      <c r="A38" s="235" t="s">
+      <c r="A38" s="248" t="s">
         <v>517</v>
       </c>
-      <c r="B38" s="238" t="s">
+      <c r="B38" s="227" t="s">
         <v>490</v>
       </c>
-      <c r="C38" s="239"/>
-      <c r="D38" s="239"/>
-      <c r="E38" s="239"/>
-      <c r="F38" s="239"/>
-      <c r="G38" s="240"/>
+      <c r="C38" s="228"/>
+      <c r="D38" s="228"/>
+      <c r="E38" s="228"/>
+      <c r="F38" s="228"/>
+      <c r="G38" s="229"/>
     </row>
     <row r="39" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A39" s="236"/>
-      <c r="B39" s="241"/>
-      <c r="C39" s="242"/>
-      <c r="D39" s="242"/>
-      <c r="E39" s="242"/>
-      <c r="F39" s="242"/>
-      <c r="G39" s="243"/>
+      <c r="A39" s="249"/>
+      <c r="B39" s="251"/>
+      <c r="C39" s="252"/>
+      <c r="D39" s="252"/>
+      <c r="E39" s="252"/>
+      <c r="F39" s="252"/>
+      <c r="G39" s="253"/>
     </row>
     <row r="40" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A40" s="236"/>
-      <c r="B40" s="244" t="s">
+      <c r="A40" s="249"/>
+      <c r="B40" s="254" t="s">
         <v>491</v>
       </c>
-      <c r="C40" s="245"/>
-      <c r="D40" s="245"/>
-      <c r="E40" s="245"/>
-      <c r="F40" s="245"/>
-      <c r="G40" s="246"/>
+      <c r="C40" s="255"/>
+      <c r="D40" s="255"/>
+      <c r="E40" s="255"/>
+      <c r="F40" s="255"/>
+      <c r="G40" s="256"/>
     </row>
     <row r="41" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A41" s="236"/>
-      <c r="B41" s="224" t="s">
+      <c r="A41" s="249"/>
+      <c r="B41" s="257" t="s">
         <v>492</v>
       </c>
       <c r="C41" s="225"/>
       <c r="D41" s="225"/>
       <c r="E41" s="225"/>
       <c r="F41" s="225"/>
-      <c r="G41" s="226"/>
+      <c r="G41" s="258"/>
     </row>
     <row r="42" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A42" s="236"/>
-      <c r="B42" s="241"/>
-      <c r="C42" s="242"/>
-      <c r="D42" s="242"/>
-      <c r="E42" s="242"/>
-      <c r="F42" s="242"/>
-      <c r="G42" s="243"/>
+      <c r="A42" s="249"/>
+      <c r="B42" s="251"/>
+      <c r="C42" s="252"/>
+      <c r="D42" s="252"/>
+      <c r="E42" s="252"/>
+      <c r="F42" s="252"/>
+      <c r="G42" s="253"/>
     </row>
     <row r="43" spans="1:7" ht="42.95" customHeight="1">
-      <c r="A43" s="236"/>
-      <c r="B43" s="224" t="s">
+      <c r="A43" s="249"/>
+      <c r="B43" s="257" t="s">
         <v>493</v>
       </c>
       <c r="C43" s="225"/>
       <c r="D43" s="225"/>
       <c r="E43" s="225"/>
       <c r="F43" s="225"/>
-      <c r="G43" s="226"/>
+      <c r="G43" s="258"/>
     </row>
     <row r="44" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A44" s="236"/>
-      <c r="B44" s="241"/>
-      <c r="C44" s="242"/>
-      <c r="D44" s="242"/>
-      <c r="E44" s="242"/>
-      <c r="F44" s="242"/>
-      <c r="G44" s="243"/>
+      <c r="A44" s="249"/>
+      <c r="B44" s="251"/>
+      <c r="C44" s="252"/>
+      <c r="D44" s="252"/>
+      <c r="E44" s="252"/>
+      <c r="F44" s="252"/>
+      <c r="G44" s="253"/>
     </row>
     <row r="45" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A45" s="236"/>
-      <c r="B45" s="224" t="s">
+      <c r="A45" s="249"/>
+      <c r="B45" s="257" t="s">
         <v>494</v>
       </c>
       <c r="C45" s="225"/>
       <c r="D45" s="225"/>
       <c r="E45" s="225"/>
       <c r="F45" s="225"/>
-      <c r="G45" s="226"/>
+      <c r="G45" s="258"/>
     </row>
     <row r="46" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A46" s="236"/>
-      <c r="B46" s="224" t="s">
+      <c r="A46" s="249"/>
+      <c r="B46" s="257" t="s">
         <v>495</v>
       </c>
       <c r="C46" s="225"/>
       <c r="D46" s="225"/>
       <c r="E46" s="225"/>
       <c r="F46" s="225"/>
-      <c r="G46" s="226"/>
+      <c r="G46" s="258"/>
     </row>
     <row r="47" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A47" s="236"/>
-      <c r="B47" s="224" t="s">
+      <c r="A47" s="249"/>
+      <c r="B47" s="257" t="s">
         <v>496</v>
       </c>
       <c r="C47" s="225"/>
       <c r="D47" s="225"/>
       <c r="E47" s="225"/>
       <c r="F47" s="225"/>
-      <c r="G47" s="226"/>
+      <c r="G47" s="258"/>
     </row>
     <row r="48" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A48" s="236"/>
-      <c r="B48" s="224" t="s">
+      <c r="A48" s="249"/>
+      <c r="B48" s="257" t="s">
         <v>497</v>
       </c>
       <c r="C48" s="225"/>
       <c r="D48" s="225"/>
       <c r="E48" s="225"/>
       <c r="F48" s="225"/>
-      <c r="G48" s="226"/>
+      <c r="G48" s="258"/>
     </row>
     <row r="49" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A49" s="236"/>
-      <c r="B49" s="224" t="s">
+      <c r="A49" s="249"/>
+      <c r="B49" s="257" t="s">
         <v>498</v>
       </c>
       <c r="C49" s="225"/>
       <c r="D49" s="225"/>
       <c r="E49" s="225"/>
       <c r="F49" s="225"/>
-      <c r="G49" s="226"/>
+      <c r="G49" s="258"/>
     </row>
     <row r="50" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A50" s="236"/>
-      <c r="B50" s="224" t="s">
+      <c r="A50" s="249"/>
+      <c r="B50" s="257" t="s">
         <v>499</v>
       </c>
       <c r="C50" s="225"/>
       <c r="D50" s="225"/>
       <c r="E50" s="225"/>
       <c r="F50" s="225"/>
-      <c r="G50" s="226"/>
+      <c r="G50" s="258"/>
     </row>
     <row r="51" spans="1:7" ht="15.95" customHeight="1">
-      <c r="A51" s="236"/>
-      <c r="B51" s="224" t="s">
+      <c r="A51" s="249"/>
+      <c r="B51" s="257" t="s">
         <v>500</v>
       </c>
       <c r="C51" s="225"/>
       <c r="D51" s="225"/>
       <c r="E51" s="225"/>
       <c r="F51" s="225"/>
-      <c r="G51" s="226"/>
+      <c r="G51" s="258"/>
     </row>
     <row r="52" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A52" s="237"/>
-      <c r="B52" s="227" t="s">
+      <c r="A52" s="250"/>
+      <c r="B52" s="259" t="s">
         <v>501</v>
       </c>
-      <c r="C52" s="228"/>
-      <c r="D52" s="228"/>
-      <c r="E52" s="228"/>
-      <c r="F52" s="228"/>
-      <c r="G52" s="229"/>
+      <c r="C52" s="260"/>
+      <c r="D52" s="260"/>
+      <c r="E52" s="260"/>
+      <c r="F52" s="260"/>
+      <c r="G52" s="261"/>
     </row>
     <row r="53" spans="1:7" ht="57.95" customHeight="1" thickBot="1">
       <c r="A53" s="10" t="s">
         <v>516</v>
       </c>
-      <c r="B53" s="221" t="s">
+      <c r="B53" s="230" t="s">
         <v>581</v>
       </c>
-      <c r="C53" s="222"/>
-      <c r="D53" s="222"/>
-      <c r="E53" s="222"/>
-      <c r="F53" s="222"/>
-      <c r="G53" s="223"/>
+      <c r="C53" s="231"/>
+      <c r="D53" s="231"/>
+      <c r="E53" s="231"/>
+      <c r="F53" s="231"/>
+      <c r="G53" s="232"/>
     </row>
     <row r="54" spans="1:7" ht="57.95" customHeight="1" thickBot="1">
       <c r="A54" s="10" t="s">
         <v>515</v>
       </c>
-      <c r="B54" s="221" t="s">
+      <c r="B54" s="230" t="s">
         <v>502</v>
       </c>
-      <c r="C54" s="222"/>
-      <c r="D54" s="222"/>
-      <c r="E54" s="222"/>
-      <c r="F54" s="222"/>
-      <c r="G54" s="223"/>
+      <c r="C54" s="231"/>
+      <c r="D54" s="231"/>
+      <c r="E54" s="231"/>
+      <c r="F54" s="231"/>
+      <c r="G54" s="232"/>
     </row>
     <row r="55" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A55" s="10" t="s">
         <v>514</v>
       </c>
-      <c r="B55" s="221" t="s">
+      <c r="B55" s="230" t="s">
         <v>503</v>
       </c>
-      <c r="C55" s="222"/>
-      <c r="D55" s="222"/>
-      <c r="E55" s="222"/>
-      <c r="F55" s="222"/>
-      <c r="G55" s="223"/>
+      <c r="C55" s="231"/>
+      <c r="D55" s="231"/>
+      <c r="E55" s="231"/>
+      <c r="F55" s="231"/>
+      <c r="G55" s="232"/>
     </row>
     <row r="56" spans="1:7" ht="42.95" customHeight="1" thickBot="1">
       <c r="A56" s="11" t="s">
         <v>508</v>
       </c>
-      <c r="B56" s="221" t="s">
+      <c r="B56" s="230" t="s">
         <v>504</v>
       </c>
-      <c r="C56" s="222"/>
-      <c r="D56" s="222"/>
-      <c r="E56" s="222"/>
-      <c r="F56" s="222"/>
-      <c r="G56" s="223"/>
+      <c r="C56" s="231"/>
+      <c r="D56" s="231"/>
+      <c r="E56" s="231"/>
+      <c r="F56" s="231"/>
+      <c r="G56" s="232"/>
     </row>
     <row r="57" spans="1:7" ht="29.1" customHeight="1" thickBot="1">
       <c r="A57" s="10" t="s">
         <v>513</v>
       </c>
-      <c r="B57" s="221" t="s">
+      <c r="B57" s="230" t="s">
         <v>505</v>
       </c>
-      <c r="C57" s="222"/>
-      <c r="D57" s="222"/>
-      <c r="E57" s="222"/>
-      <c r="F57" s="222"/>
-      <c r="G57" s="223"/>
+      <c r="C57" s="231"/>
+      <c r="D57" s="231"/>
+      <c r="E57" s="231"/>
+      <c r="F57" s="231"/>
+      <c r="G57" s="232"/>
     </row>
     <row r="58" spans="1:7" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A58" s="10" t="s">
         <v>512</v>
       </c>
-      <c r="B58" s="221" t="s">
+      <c r="B58" s="230" t="s">
         <v>506</v>
       </c>
-      <c r="C58" s="222"/>
-      <c r="D58" s="222"/>
-      <c r="E58" s="222"/>
-      <c r="F58" s="222"/>
-      <c r="G58" s="223"/>
+      <c r="C58" s="231"/>
+      <c r="D58" s="231"/>
+      <c r="E58" s="231"/>
+      <c r="F58" s="231"/>
+      <c r="G58" s="232"/>
     </row>
     <row r="59" spans="1:7" ht="42.95" customHeight="1" thickBot="1">
       <c r="A59" s="11" t="s">
         <v>509</v>
       </c>
-      <c r="B59" s="221" t="s">
+      <c r="B59" s="230" t="s">
         <v>510</v>
       </c>
-      <c r="C59" s="222"/>
-      <c r="D59" s="222"/>
-      <c r="E59" s="222"/>
-      <c r="F59" s="222"/>
-      <c r="G59" s="223"/>
+      <c r="C59" s="231"/>
+      <c r="D59" s="231"/>
+      <c r="E59" s="231"/>
+      <c r="F59" s="231"/>
+      <c r="G59" s="232"/>
     </row>
     <row r="60" spans="1:7" ht="29.1" customHeight="1" thickBot="1">
       <c r="A60" s="10" t="s">
         <v>511</v>
       </c>
-      <c r="B60" s="221" t="s">
+      <c r="B60" s="230" t="s">
         <v>507</v>
       </c>
-      <c r="C60" s="222"/>
-      <c r="D60" s="222"/>
-      <c r="E60" s="222"/>
-      <c r="F60" s="222"/>
-      <c r="G60" s="223"/>
+      <c r="C60" s="231"/>
+      <c r="D60" s="231"/>
+      <c r="E60" s="231"/>
+      <c r="F60" s="231"/>
+      <c r="G60" s="232"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="A38:A52"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="B37:G37"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="D29:G29"/>
@@ -42966,49 +42998,17 @@
     <mergeCell ref="D34:G34"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="D35:G35"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="A38:A52"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="B43:G43"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B53:G53"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:G28"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -43232,10 +43232,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>485</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -43505,10 +43505,10 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A23" s="232" t="s">
+      <c r="A23" s="235" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="234"/>
+      <c r="B23" s="237"/>
       <c r="C23" s="4" t="s">
         <v>63</v>
       </c>
@@ -43841,10 +43841,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A39" s="232" t="s">
+      <c r="A39" s="235" t="s">
         <v>524</v>
       </c>
-      <c r="B39" s="234"/>
+      <c r="B39" s="237"/>
       <c r="C39" s="4" t="s">
         <v>63</v>
       </c>
@@ -43967,10 +43967,10 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A45" s="232" t="s">
+      <c r="A45" s="235" t="s">
         <v>529</v>
       </c>
-      <c r="B45" s="234"/>
+      <c r="B45" s="237"/>
       <c r="C45" s="4" t="s">
         <v>63</v>
       </c>
@@ -44116,10 +44116,10 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A52" s="232" t="s">
+      <c r="A52" s="235" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="234"/>
+      <c r="B52" s="237"/>
       <c r="C52" s="4" t="s">
         <v>63</v>
       </c>
@@ -44307,10 +44307,10 @@
       </c>
     </row>
     <row r="61" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A61" s="232" t="s">
+      <c r="A61" s="235" t="s">
         <v>111</v>
       </c>
-      <c r="B61" s="234"/>
+      <c r="B61" s="237"/>
       <c r="C61" s="4" t="s">
         <v>63</v>
       </c>
@@ -44412,10 +44412,10 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A66" s="232" t="s">
+      <c r="A66" s="235" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="234"/>
+      <c r="B66" s="237"/>
       <c r="C66" s="4" t="s">
         <v>63</v>
       </c>
@@ -44735,10 +44735,10 @@
       </c>
     </row>
     <row r="81" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A81" s="232" t="s">
+      <c r="A81" s="235" t="s">
         <v>133</v>
       </c>
-      <c r="B81" s="234"/>
+      <c r="B81" s="237"/>
       <c r="C81" s="4" t="s">
         <v>63</v>
       </c>
@@ -44884,10 +44884,10 @@
       </c>
     </row>
     <row r="88" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A88" s="232" t="s">
+      <c r="A88" s="235" t="s">
         <v>558</v>
       </c>
-      <c r="B88" s="234"/>
+      <c r="B88" s="237"/>
       <c r="C88" s="4" t="s">
         <v>63</v>
       </c>
@@ -45014,10 +45014,10 @@
       </c>
     </row>
     <row r="94" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A94" s="232" t="s">
+      <c r="A94" s="235" t="s">
         <v>156</v>
       </c>
-      <c r="B94" s="234"/>
+      <c r="B94" s="237"/>
       <c r="C94" s="4" t="s">
         <v>63</v>
       </c>
@@ -45098,10 +45098,10 @@
       </c>
     </row>
     <row r="98" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A98" s="232" t="s">
+      <c r="A98" s="235" t="s">
         <v>150</v>
       </c>
-      <c r="B98" s="234"/>
+      <c r="B98" s="237"/>
       <c r="C98" s="4" t="s">
         <v>63</v>
       </c>
@@ -45182,10 +45182,10 @@
       </c>
     </row>
     <row r="102" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A102" s="232" t="s">
+      <c r="A102" s="235" t="s">
         <v>547</v>
       </c>
-      <c r="B102" s="234"/>
+      <c r="B102" s="237"/>
       <c r="C102" s="4" t="s">
         <v>63</v>
       </c>
@@ -45289,10 +45289,10 @@
       </c>
     </row>
     <row r="107" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A107" s="232" t="s">
+      <c r="A107" s="235" t="s">
         <v>140</v>
       </c>
-      <c r="B107" s="234"/>
+      <c r="B107" s="237"/>
       <c r="C107" s="4" t="s">
         <v>63</v>
       </c>
@@ -45457,10 +45457,10 @@
       </c>
     </row>
     <row r="115" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A115" s="232" t="s">
+      <c r="A115" s="235" t="s">
         <v>161</v>
       </c>
-      <c r="B115" s="234"/>
+      <c r="B115" s="237"/>
       <c r="C115" s="4" t="s">
         <v>453</v>
       </c>
@@ -45647,6 +45647,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A88:B88"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="C2:D9"/>
@@ -45656,14 +45664,6 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A88:B88"/>
   </mergeCells>
   <conditionalFormatting sqref="A11:A18 A107:A109 A81:A85 A115:A248 A52:A57 A40 A33:A37 A42:A43 A112 A94:A100 A61:A69 A59 A20:A29">
     <cfRule type="beginsWith" dxfId="2509" priority="1308" stopIfTrue="1" operator="beginsWith" text="Exceptional">
@@ -48185,8 +48185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.1" customHeight="1"/>
@@ -48398,10 +48398,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>701</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -48687,10 +48687,10 @@
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A25" s="232" t="s">
+      <c r="A25" s="235" t="s">
         <v>688</v>
       </c>
-      <c r="B25" s="234"/>
+      <c r="B25" s="237"/>
       <c r="C25" s="4" t="s">
         <v>63</v>
       </c>
@@ -48900,10 +48900,10 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A36" s="232" t="s">
+      <c r="A36" s="235" t="s">
         <v>612</v>
       </c>
-      <c r="B36" s="234"/>
+      <c r="B36" s="237"/>
       <c r="C36" s="4" t="s">
         <v>63</v>
       </c>
@@ -49322,10 +49322,10 @@
       <c r="G57" s="11"/>
     </row>
     <row r="58" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A58" s="232" t="s">
+      <c r="A58" s="235" t="s">
         <v>627</v>
       </c>
-      <c r="B58" s="234"/>
+      <c r="B58" s="237"/>
       <c r="C58" s="4" t="s">
         <v>63</v>
       </c>
@@ -49630,10 +49630,10 @@
       <c r="G73" s="11"/>
     </row>
     <row r="74" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A74" s="232" t="s">
+      <c r="A74" s="235" t="s">
         <v>651</v>
       </c>
-      <c r="B74" s="234"/>
+      <c r="B74" s="237"/>
       <c r="C74" s="4" t="s">
         <v>63</v>
       </c>
@@ -49822,10 +49822,10 @@
       <c r="G83" s="11"/>
     </row>
     <row r="84" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A84" s="232" t="s">
+      <c r="A84" s="235" t="s">
         <v>663</v>
       </c>
-      <c r="B84" s="234"/>
+      <c r="B84" s="237"/>
       <c r="C84" s="21" t="s">
         <v>456</v>
       </c>
@@ -50185,10 +50185,10 @@
       <c r="G102" s="11"/>
     </row>
     <row r="103" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A103" s="232" t="s">
+      <c r="A103" s="235" t="s">
         <v>677</v>
       </c>
-      <c r="B103" s="234"/>
+      <c r="B103" s="237"/>
       <c r="C103" s="4" t="s">
         <v>63</v>
       </c>
@@ -53362,10 +53362,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>291</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -53725,10 +53725,10 @@
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A29" s="232" t="s">
+      <c r="A29" s="235" t="s">
         <v>564</v>
       </c>
-      <c r="B29" s="234"/>
+      <c r="B29" s="237"/>
       <c r="C29" s="4" t="s">
         <v>451</v>
       </c>
@@ -53957,10 +53957,10 @@
       <c r="G40" s="11"/>
     </row>
     <row r="41" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A41" s="232" t="s">
+      <c r="A41" s="235" t="s">
         <v>334</v>
       </c>
-      <c r="B41" s="234"/>
+      <c r="B41" s="237"/>
       <c r="C41" s="4" t="s">
         <v>63</v>
       </c>
@@ -54174,10 +54174,10 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" s="7" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A52" s="232" t="s">
+      <c r="A52" s="235" t="s">
         <v>84</v>
       </c>
-      <c r="B52" s="234"/>
+      <c r="B52" s="237"/>
       <c r="C52" s="4" t="s">
         <v>63</v>
       </c>
@@ -54347,10 +54347,10 @@
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" s="7" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A61" s="232" t="s">
+      <c r="A61" s="235" t="s">
         <v>370</v>
       </c>
-      <c r="B61" s="234"/>
+      <c r="B61" s="237"/>
       <c r="C61" s="21" t="s">
         <v>452</v>
       </c>
@@ -55700,10 +55700,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>810</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -56006,10 +56006,10 @@
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A26" s="232" t="s">
+      <c r="A26" s="235" t="s">
         <v>390</v>
       </c>
-      <c r="B26" s="234"/>
+      <c r="B26" s="237"/>
       <c r="C26" s="4" t="s">
         <v>855</v>
       </c>
@@ -56276,10 +56276,10 @@
       <c r="G39" s="11"/>
     </row>
     <row r="40" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A40" s="232" t="s">
+      <c r="A40" s="235" t="s">
         <v>448</v>
       </c>
-      <c r="B40" s="234"/>
+      <c r="B40" s="237"/>
       <c r="C40" s="102" t="s">
         <v>856</v>
       </c>
@@ -56544,10 +56544,10 @@
       <c r="G53" s="11"/>
     </row>
     <row r="54" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A54" s="232" t="s">
+      <c r="A54" s="235" t="s">
         <v>412</v>
       </c>
-      <c r="B54" s="234"/>
+      <c r="B54" s="237"/>
       <c r="C54" s="4" t="s">
         <v>63</v>
       </c>
@@ -58410,10 +58410,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A10" s="232" t="s">
+      <c r="A10" s="235" t="s">
         <v>239</v>
       </c>
-      <c r="B10" s="234"/>
+      <c r="B10" s="237"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -58507,10 +58507,10 @@
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A15" s="232" t="s">
+      <c r="A15" s="235" t="s">
         <v>246</v>
       </c>
-      <c r="B15" s="234"/>
+      <c r="B15" s="237"/>
       <c r="C15" s="4" t="s">
         <v>874</v>
       </c>
@@ -58623,10 +58623,10 @@
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A21" s="232" t="s">
+      <c r="A21" s="235" t="s">
         <v>878</v>
       </c>
-      <c r="B21" s="234"/>
+      <c r="B21" s="237"/>
       <c r="C21" s="4" t="s">
         <v>63</v>
       </c>
@@ -58758,10 +58758,10 @@
       <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A28" s="232" t="s">
+      <c r="A28" s="235" t="s">
         <v>254</v>
       </c>
-      <c r="B28" s="234"/>
+      <c r="B28" s="237"/>
       <c r="C28" s="4" t="s">
         <v>875</v>
       </c>
@@ -58912,10 +58912,10 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A36" s="232" t="s">
+      <c r="A36" s="235" t="s">
         <v>891</v>
       </c>
-      <c r="B36" s="234"/>
+      <c r="B36" s="237"/>
       <c r="C36" s="4" t="s">
         <v>454</v>
       </c>
@@ -59047,10 +59047,10 @@
       <c r="G42" s="11"/>
     </row>
     <row r="43" spans="1:7" ht="14.1" customHeight="1" thickBot="1">
-      <c r="A43" s="232" t="s">
+      <c r="A43" s="235" t="s">
         <v>275</v>
       </c>
-      <c r="B43" s="234"/>
+      <c r="B43" s="237"/>
       <c r="C43" s="4" t="s">
         <v>63</v>
       </c>

</xml_diff>